<commit_message>
Added more material_analyzed fields and a note saying to send an email to mosaic if there is a field missing
</commit_message>
<xml_diff>
--- a/Excel_templates/MOSAIC_input_excel_file_2022.xlsx
+++ b/Excel_templates/MOSAIC_input_excel_file_2022.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sparadis\Documents\ETH\MOSAIC\MOSAIC_Client\Excel_templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A89B41A-EF40-4DA9-A061-E6520DD25C2E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F275883-6895-4E7A-A93A-B275039E8ACA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30204" yWindow="10044" windowWidth="40020" windowHeight="22296" tabRatio="694" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30204" yWindow="10044" windowWidth="40020" windowHeight="22296" tabRatio="694" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ARTICLE_AUTHOR" sheetId="3" r:id="rId1"/>
@@ -57,7 +57,7 @@
     <definedName name="Lebanon">SET_VARIABLES!$AK$2:$AK$4</definedName>
     <definedName name="MAR_model">SET_VARIABLES!$BK$2:$BK$9</definedName>
     <definedName name="MAR_tracer">SET_VARIABLES!$BJ$2:$BJ$12</definedName>
-    <definedName name="material_analyzed">SET_VARIABLES!$CL$2:$CL$16</definedName>
+    <definedName name="material_analyzed">SET_VARIABLES!$CL$2:$CL$29</definedName>
     <definedName name="Mauritania">SET_VARIABLES!$AL$2:$AL$7</definedName>
     <definedName name="Mixing_rate_tracer">SET_VARIABLES!$BO$3:$BO$13</definedName>
     <definedName name="Netherlands">SET_VARIABLES!$AM$2:$AM$13</definedName>
@@ -132,7 +132,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3562" uniqueCount="2925">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3575" uniqueCount="2938">
   <si>
     <t>sample_name</t>
   </si>
@@ -8907,6 +8907,45 @@
   </si>
   <si>
     <t>grab corer (type: Shipek, van Veen, Soutar, Ponar, Peterson, Smith and McIntyre)</t>
+  </si>
+  <si>
+    <t>black_carbon</t>
+  </si>
+  <si>
+    <t>&gt;2.5 g/cm3</t>
+  </si>
+  <si>
+    <t>2-2.5 g/cm3</t>
+  </si>
+  <si>
+    <t>1.6-2 g/cm3</t>
+  </si>
+  <si>
+    <t>&lt;1.6 g/cm3</t>
+  </si>
+  <si>
+    <t>&gt;0.5 mm</t>
+  </si>
+  <si>
+    <t>0.25-0.5 mm</t>
+  </si>
+  <si>
+    <t>0.125-0.25 mm</t>
+  </si>
+  <si>
+    <t>0.063-0.125 mm</t>
+  </si>
+  <si>
+    <t>0.032-0.063 mm</t>
+  </si>
+  <si>
+    <t>0.020-0.032 mm</t>
+  </si>
+  <si>
+    <t>&lt;0.020 mm</t>
+  </si>
+  <si>
+    <t>&gt;0.250 mm</t>
   </si>
 </sst>
 </file>
@@ -9921,7 +9960,7 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -11745,7 +11784,7 @@
       <pane xSplit="3" ySplit="4" topLeftCell="F5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="J17" sqref="J17"/>
+      <selection pane="bottomRight" activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -14225,7 +14264,7 @@
     <mergeCell ref="D2:D4"/>
     <mergeCell ref="E2:E4"/>
   </mergeCells>
-  <dataValidations xWindow="389" yWindow="346" count="10">
+  <dataValidations xWindow="389" yWindow="346" count="11">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Write the core_name or select from the drop-down menu the cores you have in the Workbook._x000a_Make sure that the core name matches with its metadata given in GEOPOINTS_CORES sheet" sqref="B2" xr:uid="{6685FF74-A7F2-42C2-901B-99DBBBFECDB4}"/>
     <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Sample analysis category" prompt="Choose from the drop-down list the analysis category the variable belongs to" sqref="L1:CB1" xr:uid="{2372D2F3-EE0C-4296-AC86-BA3569CC20EF}">
       <formula1>Sample_analyses_types</formula1>
@@ -14247,7 +14286,10 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Sample analysis" prompt="Choose from the drop-down menu the variable to be added" sqref="L2:CB2" xr:uid="{ADED0455-8DDC-445F-B013-7A6BE4A4748B}">
       <formula1>INDIRECT(L1)</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Material analyzed" prompt="Choose from the drop-down menu the material analyzed (i.e. bulk, OC, sand, etc.). If left blank, the default material analyzed (bulk) will be used. " sqref="M3:CB3 L3" xr:uid="{B3206B9A-BD85-4C2B-B436-B08F0FC71300}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Material analyzed" prompt="Choose from the drop-down menu the material analyzed (i.e. bulk, OC, sand, etc.). If left blank, the default material analyzed (bulk) will be used. If there's a material_analyzed that is missing, please let us know sending an email to mosaic@erdw.eth.ch." sqref="M3:CB3" xr:uid="{B3206B9A-BD85-4C2B-B436-B08F0FC71300}">
+      <formula1>material_analyzed</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Material analyzed" prompt="Choose from the drop-down menu the material analyzed (i.e. bulk, OC, sand, etc.). If left blank, the default material analyzed (bulk) will be used. If there's a material_analyzed that is missing, please let us know sending an email to mosaic@erdw.eth.ch." sqref="L3" xr:uid="{EE584956-CBED-4592-9CF0-B13DC6BA795C}">
       <formula1>material_analyzed</formula1>
     </dataValidation>
   </dataValidations>
@@ -14303,8 +14345,8 @@
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:ET277"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+    <sheetView topLeftCell="CK1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="CM25" sqref="CM25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -19468,6 +19510,9 @@
       <c r="CK17" s="20">
         <v>16</v>
       </c>
+      <c r="CL17" s="14" t="s">
+        <v>2925</v>
+      </c>
       <c r="CM17" s="10" t="s">
         <v>2102</v>
       </c>
@@ -19641,6 +19686,9 @@
       <c r="CK18" s="20">
         <v>17</v>
       </c>
+      <c r="CL18" s="14" t="s">
+        <v>2926</v>
+      </c>
       <c r="CM18" s="10" t="s">
         <v>2141</v>
       </c>
@@ -19796,6 +19844,9 @@
       <c r="CK19" s="20">
         <v>18</v>
       </c>
+      <c r="CL19" s="14" t="s">
+        <v>2927</v>
+      </c>
       <c r="CM19" s="10" t="s">
         <v>2262</v>
       </c>
@@ -19951,6 +20002,9 @@
       <c r="CK20" s="20">
         <v>19</v>
       </c>
+      <c r="CL20" s="14" t="s">
+        <v>2928</v>
+      </c>
       <c r="CP20" s="11" t="s">
         <v>2425</v>
       </c>
@@ -20083,6 +20137,9 @@
       <c r="CH21" s="20" t="s">
         <v>2586</v>
       </c>
+      <c r="CL21" s="14" t="s">
+        <v>2929</v>
+      </c>
       <c r="CP21" s="11" t="s">
         <v>2429</v>
       </c>
@@ -20182,6 +20239,9 @@
       <c r="CH22" s="20" t="s">
         <v>2831</v>
       </c>
+      <c r="CL22" s="14" t="s">
+        <v>2930</v>
+      </c>
       <c r="CP22" s="11" t="s">
         <v>2674</v>
       </c>
@@ -20271,6 +20331,9 @@
       <c r="BZ23" s="10"/>
       <c r="CA23" s="10"/>
       <c r="CB23" s="10"/>
+      <c r="CL23" s="14" t="s">
+        <v>2931</v>
+      </c>
       <c r="CP23" s="11" t="s">
         <v>2675</v>
       </c>
@@ -20362,6 +20425,9 @@
         <v>1943</v>
       </c>
       <c r="BD24" s="17"/>
+      <c r="CL24" s="14" t="s">
+        <v>2932</v>
+      </c>
       <c r="CP24" s="11" t="s">
         <v>2676</v>
       </c>
@@ -20448,6 +20514,9 @@
         <v>1944</v>
       </c>
       <c r="BD25" s="17"/>
+      <c r="CL25" s="14" t="s">
+        <v>2933</v>
+      </c>
       <c r="CP25" s="11" t="s">
         <v>2677</v>
       </c>
@@ -20533,6 +20602,9 @@
         <v>1744</v>
       </c>
       <c r="BD26" s="17"/>
+      <c r="CL26" s="14" t="s">
+        <v>2934</v>
+      </c>
       <c r="CP26" s="11" t="s">
         <v>1769</v>
       </c>
@@ -20611,6 +20683,9 @@
       <c r="BC27" s="6" t="s">
         <v>1945</v>
       </c>
+      <c r="CL27" s="14" t="s">
+        <v>2935</v>
+      </c>
       <c r="CP27" s="11" t="s">
         <v>1779</v>
       </c>
@@ -20689,6 +20764,9 @@
       <c r="BC28" s="6" t="s">
         <v>1656</v>
       </c>
+      <c r="CL28" s="14" t="s">
+        <v>2936</v>
+      </c>
       <c r="CP28" s="11" t="s">
         <v>2835</v>
       </c>
@@ -20763,6 +20841,9 @@
       </c>
       <c r="BC29" s="6" t="s">
         <v>1679</v>
+      </c>
+      <c r="CL29" s="14" t="s">
+        <v>2937</v>
       </c>
       <c r="CP29" s="20" t="s">
         <v>2540</v>
@@ -26586,7 +26667,7 @@
       <c r="DK277" s="45"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="dglLbzSeFlIWNlY5Hd+MsJjnxyWZO0EZiOep6oC48b3evfkcasj438BwkSL6EWMunybmUANMIyWycmqiEW84CQ==" saltValue="1yZBx9+VPyv1Bg54MegX5w==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="ZVWuNvN7OAi1U1mEX5GDiZ25DsPoayYk756mpLdzgzloknW1ST5xtM8nPmjukCr3K0O9xnM5Y7ytecnBHmgkPw==" saltValue="UVFQ9MamL+M104Hz6cWarQ==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="2">
     <mergeCell ref="M27:M28"/>
     <mergeCell ref="M34:M35"/>

</xml_diff>

<commit_message>
Protected the sheet. This time I hope it worked
</commit_message>
<xml_diff>
--- a/Excel_templates/MOSAIC_input_excel_file_2022.xlsx
+++ b/Excel_templates/MOSAIC_input_excel_file_2022.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sparadis\Documents\ETH\MOSAIC\MOSAIC_Client\Excel_templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11658A77-F41C-41AB-9642-584E06019646}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A23367AE-295D-4403-8606-C991340CACFC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="30204" yWindow="10044" windowWidth="40020" windowHeight="22296" tabRatio="694" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -14465,7 +14465,7 @@
   <dimension ref="A1:EU277"/>
   <sheetViews>
     <sheetView topLeftCell="EF1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="EU1" sqref="EU1"/>
+      <selection activeCell="EJ15" sqref="EJ15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Added a new research vessel in the list
</commit_message>
<xml_diff>
--- a/Excel_templates/MOSAIC_input_excel_file_2022.xlsx
+++ b/Excel_templates/MOSAIC_input_excel_file_2022.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sparadis\Documents\ETH\MOSAIC\MOSAIC_Client\Excel_templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A23367AE-295D-4403-8606-C991340CACFC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07D1601D-710B-4298-966F-0FF696F05576}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="30204" yWindow="10044" windowWidth="40020" windowHeight="22296" tabRatio="694" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
     <definedName name="Bermuda">SET_VARIABLES!$T$4</definedName>
     <definedName name="Brazil">SET_VARIABLES!$U$2:$U$12</definedName>
     <definedName name="C_lab">SET_VARIABLES!$G$2:$G$277</definedName>
-    <definedName name="Canada">SET_VARIABLES!$V$2:$V$18</definedName>
+    <definedName name="Canada">SET_VARIABLES!$V$2:$V$19</definedName>
     <definedName name="Chile">SET_VARIABLES!$W$2:$W$5</definedName>
     <definedName name="China">SET_VARIABLES!$X$2:$X$9</definedName>
     <definedName name="Colombia">SET_VARIABLES!$Y$2:$Y$7</definedName>
@@ -133,7 +133,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3575" uniqueCount="2938">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3576" uniqueCount="2939">
   <si>
     <t>sample_name</t>
   </si>
@@ -8947,6 +8947,9 @@
   </si>
   <si>
     <t>elemental analyzer</t>
+  </si>
+  <si>
+    <t>CCGS Wilfrid Laurier</t>
   </si>
 </sst>
 </file>
@@ -9420,7 +9423,7 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="110">
+  <cellXfs count="111">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="13" applyFont="1" applyFill="1" applyAlignment="1"/>
@@ -9546,6 +9549,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="19" fillId="4" borderId="4" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
@@ -9985,15 +9989,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="64" customFormat="1" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="82" t="s">
+      <c r="A1" s="83" t="s">
         <v>2677</v>
       </c>
-      <c r="B1" s="82"/>
-      <c r="C1" s="82"/>
-      <c r="D1" s="82"/>
-      <c r="E1" s="82"/>
-      <c r="F1" s="82"/>
-      <c r="G1" s="82"/>
+      <c r="B1" s="83"/>
+      <c r="C1" s="83"/>
+      <c r="D1" s="83"/>
+      <c r="E1" s="83"/>
+      <c r="F1" s="83"/>
+      <c r="G1" s="83"/>
     </row>
     <row r="2" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="53" t="s">
@@ -10082,25 +10086,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="63" customFormat="1" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="83" t="s">
+      <c r="A1" s="84" t="s">
         <v>2678</v>
       </c>
-      <c r="B1" s="83"/>
-      <c r="C1" s="83"/>
-      <c r="D1" s="83"/>
-      <c r="E1" s="84" t="s">
+      <c r="B1" s="84"/>
+      <c r="C1" s="84"/>
+      <c r="D1" s="84"/>
+      <c r="E1" s="85" t="s">
         <v>2818</v>
       </c>
-      <c r="F1" s="84"/>
-      <c r="G1" s="84"/>
-      <c r="H1" s="84"/>
-      <c r="I1" s="84"/>
-      <c r="J1" s="84"/>
-      <c r="K1" s="84"/>
-      <c r="L1" s="84"/>
-      <c r="M1" s="84"/>
-      <c r="N1" s="84"/>
-      <c r="O1" s="84"/>
+      <c r="F1" s="85"/>
+      <c r="G1" s="85"/>
+      <c r="H1" s="85"/>
+      <c r="I1" s="85"/>
+      <c r="J1" s="85"/>
+      <c r="K1" s="85"/>
+      <c r="L1" s="85"/>
+      <c r="M1" s="85"/>
+      <c r="N1" s="85"/>
+      <c r="O1" s="85"/>
     </row>
     <row r="2" spans="1:15" s="66" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="62" t="s">
@@ -10412,16 +10416,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:34" s="55" customFormat="1" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="85" t="s">
+      <c r="A1" s="86" t="s">
         <v>2680</v>
       </c>
-      <c r="B1" s="85"/>
-      <c r="C1" s="85" t="s">
+      <c r="B1" s="86"/>
+      <c r="C1" s="86" t="s">
         <v>2679</v>
       </c>
-      <c r="D1" s="85"/>
-      <c r="E1" s="85"/>
-      <c r="F1" s="85"/>
+      <c r="D1" s="86"/>
+      <c r="E1" s="86"/>
+      <c r="F1" s="86"/>
       <c r="G1" s="55" t="s">
         <v>2219</v>
       </c>
@@ -10433,22 +10437,22 @@
       </c>
     </row>
     <row r="2" spans="1:34" ht="15.6" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="86" t="s">
+      <c r="A2" s="87" t="s">
         <v>2568</v>
       </c>
-      <c r="B2" s="86" t="s">
+      <c r="B2" s="87" t="s">
         <v>1825</v>
       </c>
-      <c r="C2" s="86" t="s">
+      <c r="C2" s="87" t="s">
         <v>1834</v>
       </c>
-      <c r="D2" s="86" t="s">
+      <c r="D2" s="87" t="s">
         <v>2687</v>
       </c>
-      <c r="E2" s="86" t="s">
+      <c r="E2" s="87" t="s">
         <v>1823</v>
       </c>
-      <c r="F2" s="89" t="s">
+      <c r="F2" s="90" t="s">
         <v>1824</v>
       </c>
       <c r="G2" s="56" t="s">
@@ -10487,12 +10491,12 @@
       <c r="AH2" s="56"/>
     </row>
     <row r="3" spans="1:34" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="87"/>
-      <c r="B3" s="87"/>
-      <c r="C3" s="87"/>
-      <c r="D3" s="87"/>
-      <c r="E3" s="87"/>
-      <c r="F3" s="90"/>
+      <c r="A3" s="88"/>
+      <c r="B3" s="88"/>
+      <c r="C3" s="88"/>
+      <c r="D3" s="88"/>
+      <c r="E3" s="88"/>
+      <c r="F3" s="91"/>
       <c r="G3" s="56"/>
       <c r="H3" s="56"/>
       <c r="I3" s="56"/>
@@ -10523,12 +10527,12 @@
       <c r="AH3" s="56"/>
     </row>
     <row r="4" spans="1:34" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="88"/>
-      <c r="B4" s="88"/>
-      <c r="C4" s="88"/>
-      <c r="D4" s="88"/>
-      <c r="E4" s="88"/>
-      <c r="F4" s="90"/>
+      <c r="A4" s="89"/>
+      <c r="B4" s="89"/>
+      <c r="C4" s="89"/>
+      <c r="D4" s="89"/>
+      <c r="E4" s="89"/>
+      <c r="F4" s="91"/>
       <c r="G4" s="56"/>
       <c r="H4" s="56"/>
       <c r="I4" s="56"/>
@@ -10559,12 +10563,12 @@
       <c r="AH4" s="56"/>
     </row>
     <row r="5" spans="1:34" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="88"/>
-      <c r="B5" s="88"/>
-      <c r="C5" s="88"/>
-      <c r="D5" s="88"/>
-      <c r="E5" s="88"/>
-      <c r="F5" s="90"/>
+      <c r="A5" s="89"/>
+      <c r="B5" s="89"/>
+      <c r="C5" s="89"/>
+      <c r="D5" s="89"/>
+      <c r="E5" s="89"/>
+      <c r="F5" s="91"/>
       <c r="G5" s="56"/>
       <c r="H5" s="56"/>
       <c r="I5" s="56"/>
@@ -11841,23 +11845,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:80" s="79" customFormat="1" ht="20.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="91" t="s">
+      <c r="A1" s="92" t="s">
         <v>2689</v>
       </c>
-      <c r="B1" s="92"/>
-      <c r="C1" s="93"/>
-      <c r="D1" s="91" t="s">
+      <c r="B1" s="93"/>
+      <c r="C1" s="94"/>
+      <c r="D1" s="92" t="s">
         <v>2679</v>
       </c>
-      <c r="E1" s="92"/>
-      <c r="F1" s="92"/>
-      <c r="G1" s="93"/>
-      <c r="H1" s="94" t="s">
+      <c r="E1" s="93"/>
+      <c r="F1" s="93"/>
+      <c r="G1" s="94"/>
+      <c r="H1" s="95" t="s">
         <v>2681</v>
       </c>
-      <c r="I1" s="95"/>
-      <c r="J1" s="95"/>
-      <c r="K1" s="96"/>
+      <c r="I1" s="96"/>
+      <c r="J1" s="96"/>
+      <c r="K1" s="97"/>
       <c r="L1" s="79" t="s">
         <v>1840</v>
       </c>
@@ -11875,37 +11879,37 @@
       </c>
     </row>
     <row r="2" spans="1:80" s="81" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="97" t="s">
+      <c r="A2" s="98" t="s">
         <v>2568</v>
       </c>
-      <c r="B2" s="100" t="s">
+      <c r="B2" s="101" t="s">
         <v>1825</v>
       </c>
-      <c r="C2" s="103" t="s">
+      <c r="C2" s="104" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="98" t="s">
+      <c r="D2" s="99" t="s">
         <v>1834</v>
       </c>
-      <c r="E2" s="101" t="s">
+      <c r="E2" s="102" t="s">
         <v>2687</v>
       </c>
-      <c r="F2" s="101" t="s">
+      <c r="F2" s="102" t="s">
         <v>1823</v>
       </c>
-      <c r="G2" s="104" t="s">
+      <c r="G2" s="105" t="s">
         <v>1824</v>
       </c>
-      <c r="H2" s="97" t="s">
+      <c r="H2" s="98" t="s">
         <v>1835</v>
       </c>
-      <c r="I2" s="100" t="s">
+      <c r="I2" s="101" t="s">
         <v>1836</v>
       </c>
-      <c r="J2" s="100" t="s">
+      <c r="J2" s="101" t="s">
         <v>1837</v>
       </c>
-      <c r="K2" s="106" t="s">
+      <c r="K2" s="107" t="s">
         <v>1838</v>
       </c>
       <c r="L2" s="80" t="s">
@@ -11987,17 +11991,17 @@
       <c r="CB2" s="80"/>
     </row>
     <row r="3" spans="1:80" s="81" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="98"/>
-      <c r="B3" s="101"/>
-      <c r="C3" s="104"/>
-      <c r="D3" s="98"/>
-      <c r="E3" s="101"/>
-      <c r="F3" s="101"/>
-      <c r="G3" s="104"/>
-      <c r="H3" s="98"/>
-      <c r="I3" s="101"/>
-      <c r="J3" s="101"/>
-      <c r="K3" s="107"/>
+      <c r="A3" s="99"/>
+      <c r="B3" s="102"/>
+      <c r="C3" s="105"/>
+      <c r="D3" s="99"/>
+      <c r="E3" s="102"/>
+      <c r="F3" s="102"/>
+      <c r="G3" s="105"/>
+      <c r="H3" s="99"/>
+      <c r="I3" s="102"/>
+      <c r="J3" s="102"/>
+      <c r="K3" s="108"/>
       <c r="L3" s="80"/>
       <c r="M3" s="80"/>
       <c r="N3" s="80"/>
@@ -12069,17 +12073,17 @@
       <c r="CB3" s="80"/>
     </row>
     <row r="4" spans="1:80" s="81" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="98"/>
-      <c r="B4" s="101"/>
-      <c r="C4" s="104"/>
-      <c r="D4" s="98"/>
-      <c r="E4" s="101"/>
-      <c r="F4" s="101"/>
-      <c r="G4" s="104"/>
-      <c r="H4" s="98"/>
-      <c r="I4" s="101"/>
-      <c r="J4" s="101"/>
-      <c r="K4" s="107"/>
+      <c r="A4" s="99"/>
+      <c r="B4" s="102"/>
+      <c r="C4" s="105"/>
+      <c r="D4" s="99"/>
+      <c r="E4" s="102"/>
+      <c r="F4" s="102"/>
+      <c r="G4" s="105"/>
+      <c r="H4" s="99"/>
+      <c r="I4" s="102"/>
+      <c r="J4" s="102"/>
+      <c r="K4" s="108"/>
       <c r="L4" s="80"/>
       <c r="M4" s="80"/>
       <c r="N4" s="80"/>
@@ -12151,17 +12155,17 @@
       <c r="CB4" s="80"/>
     </row>
     <row r="5" spans="1:80" s="81" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="99"/>
-      <c r="B5" s="102"/>
-      <c r="C5" s="105"/>
-      <c r="D5" s="99"/>
-      <c r="E5" s="102"/>
-      <c r="F5" s="102"/>
-      <c r="G5" s="105"/>
-      <c r="H5" s="99"/>
-      <c r="I5" s="102"/>
-      <c r="J5" s="102"/>
-      <c r="K5" s="108"/>
+      <c r="A5" s="100"/>
+      <c r="B5" s="103"/>
+      <c r="C5" s="106"/>
+      <c r="D5" s="100"/>
+      <c r="E5" s="103"/>
+      <c r="F5" s="103"/>
+      <c r="G5" s="106"/>
+      <c r="H5" s="100"/>
+      <c r="I5" s="103"/>
+      <c r="J5" s="103"/>
+      <c r="K5" s="109"/>
       <c r="L5" s="80"/>
       <c r="M5" s="80"/>
       <c r="N5" s="80"/>
@@ -14464,8 +14468,8 @@
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:EU277"/>
   <sheetViews>
-    <sheetView topLeftCell="EF1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="EJ15" sqref="EJ15"/>
+    <sheetView topLeftCell="Q4" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="V9" sqref="V9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -18755,8 +18759,8 @@
         <v>1897</v>
       </c>
       <c r="U13" s="6"/>
-      <c r="V13" s="67" t="s">
-        <v>2806</v>
+      <c r="V13" s="82" t="s">
+        <v>2938</v>
       </c>
       <c r="AB13" s="6" t="s">
         <v>1387</v>
@@ -18971,8 +18975,8 @@
         <v>1898</v>
       </c>
       <c r="U14" s="6"/>
-      <c r="V14" s="6" t="s">
-        <v>1357</v>
+      <c r="V14" s="67" t="s">
+        <v>2806</v>
       </c>
       <c r="AB14" s="6" t="s">
         <v>1394</v>
@@ -19174,7 +19178,7 @@
         <v>1899</v>
       </c>
       <c r="V15" s="6" t="s">
-        <v>1702</v>
+        <v>1357</v>
       </c>
       <c r="AB15" s="6" t="s">
         <v>1382</v>
@@ -19369,7 +19373,7 @@
         <v>1900</v>
       </c>
       <c r="V16" s="6" t="s">
-        <v>1703</v>
+        <v>1702</v>
       </c>
       <c r="AB16" s="6" t="s">
         <v>1383</v>
@@ -19558,7 +19562,7 @@
         <v>1901</v>
       </c>
       <c r="V17" s="6" t="s">
-        <v>1704</v>
+        <v>1703</v>
       </c>
       <c r="AB17" s="6" t="s">
         <v>1391</v>
@@ -19739,7 +19743,7 @@
         <v>1902</v>
       </c>
       <c r="V18" s="6" t="s">
-        <v>1358</v>
+        <v>1704</v>
       </c>
       <c r="AB18" s="6" t="s">
         <v>1384</v>
@@ -19903,6 +19907,9 @@
       <c r="Q19" s="18" t="s">
         <v>1903</v>
       </c>
+      <c r="V19" s="6" t="s">
+        <v>1358</v>
+      </c>
       <c r="AB19" s="6" t="s">
         <v>1392</v>
       </c>
@@ -20786,7 +20793,7 @@
       <c r="L27" t="s">
         <v>228</v>
       </c>
-      <c r="M27" s="109"/>
+      <c r="M27" s="110"/>
       <c r="O27" s="12" t="s">
         <v>822</v>
       </c>
@@ -20867,7 +20874,7 @@
       <c r="L28" t="s">
         <v>235</v>
       </c>
-      <c r="M28" s="109"/>
+      <c r="M28" s="110"/>
       <c r="O28" s="12" t="s">
         <v>1712</v>
       </c>
@@ -21267,7 +21274,7 @@
       <c r="L34" t="s">
         <v>276</v>
       </c>
-      <c r="M34" s="109"/>
+      <c r="M34" s="110"/>
       <c r="O34" s="12" t="s">
         <v>915</v>
       </c>
@@ -21326,7 +21333,7 @@
       <c r="L35" t="s">
         <v>283</v>
       </c>
-      <c r="M35" s="109"/>
+      <c r="M35" s="110"/>
       <c r="O35" s="12" t="s">
         <v>939</v>
       </c>
@@ -26792,7 +26799,7 @@
       <c r="DK277" s="45"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="Gm0W14WDyDRZMPGyz+6p1pFEDMMSD1r1GEzBwhSegGABsHopl8HTTgK3gRlAUWJzUdrZZF5dGD+/lGWmXDo/AQ==" saltValue="TVXjyi7qrPSC01rrrxACog==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="8Y4BpAuCoFcIb0UkWykzR/3+C7ErK0+CUCmVco+eBNsMlH9epISSmC4CRsHNdhRj3m2vxBONpLrvzkGWT3cg2Q==" saltValue="Rbd1v5n+KDJhkwn/N+LsNw==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="2">
     <mergeCell ref="M27:M28"/>
     <mergeCell ref="M34:M35"/>

</xml_diff>

<commit_message>
Added a new sampling method technique
</commit_message>
<xml_diff>
--- a/Excel_templates/MOSAIC_input_excel_file_2022.xlsx
+++ b/Excel_templates/MOSAIC_input_excel_file_2022.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sparadis\Documents\ETH\MOSAIC\MOSAIC_Client\Excel_templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07D1601D-710B-4298-966F-0FF696F05576}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B906316-E663-40A9-83BA-2EF76002E53A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="30204" yWindow="10044" windowWidth="40020" windowHeight="22296" tabRatio="694" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -133,7 +133,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3576" uniqueCount="2939">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3577" uniqueCount="2940">
   <si>
     <t>sample_name</t>
   </si>
@@ -8950,6 +8950,9 @@
   </si>
   <si>
     <t>CCGS Wilfrid Laurier</t>
+  </si>
+  <si>
+    <t>single corer (Niemisto, Kajak corer)</t>
   </si>
 </sst>
 </file>
@@ -10380,7 +10383,7 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please select corer type if relevant. Chosse _unkown if unknown. Otherwise leave blank." prompt="Please select corer type if relevant. Chosse _unkown if unknown. Otherwise leave blank." xr:uid="{89ED9B77-757F-4A56-BFAB-AB1DC0DB17FB}">
           <x14:formula1>
-            <xm:f>SET_VARIABLES!$J$2:$J$12</xm:f>
+            <xm:f>SET_VARIABLES!$J$2:$J$13</xm:f>
           </x14:formula1>
           <xm:sqref>H3:H1048576</xm:sqref>
         </x14:dataValidation>
@@ -14468,8 +14471,8 @@
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:EU277"/>
   <sheetViews>
-    <sheetView topLeftCell="Q4" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="V9" sqref="V9"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -18743,6 +18746,9 @@
       <c r="H13" t="s">
         <v>127</v>
       </c>
+      <c r="J13" t="s">
+        <v>2939</v>
+      </c>
       <c r="K13" s="35" t="s">
         <v>2090</v>
       </c>
@@ -26799,7 +26805,7 @@
       <c r="DK277" s="45"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="8Y4BpAuCoFcIb0UkWykzR/3+C7ErK0+CUCmVco+eBNsMlH9epISSmC4CRsHNdhRj3m2vxBONpLrvzkGWT3cg2Q==" saltValue="Rbd1v5n+KDJhkwn/N+LsNw==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="RB5XeN6hBT90ymVcYN6vejS5i8Ne8+QkfdM3HHvtsdfV/B/flriRE20aphvjt7r7ypfPwAQ63bngC9sWemLP9A==" saltValue="c3mYTNoRf5oN96dwNN34ag==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="2">
     <mergeCell ref="M27:M28"/>
     <mergeCell ref="M34:M35"/>

</xml_diff>

<commit_message>
Added conditional formatting to the core_name of the geopoints, so that the user automatically sees which cores are duplicate
</commit_message>
<xml_diff>
--- a/Excel_templates/MOSAIC_input_excel_file_2022.xlsx
+++ b/Excel_templates/MOSAIC_input_excel_file_2022.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sparadis\Documents\ETH\MOSAIC\MOSAIC_Client\Excel_templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DB2830A-82AF-464E-A4A7-1C54DB5960EA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AA8F87B-E0B3-4828-952E-0D822E3C7DC0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="30204" yWindow="10044" windowWidth="40020" windowHeight="22296" tabRatio="694" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -9662,7 +9662,18 @@
     <cellStyle name="Normal 10" xfId="13" xr:uid="{00000000-0005-0000-0000-00000C000000}"/>
     <cellStyle name="Total" xfId="1" builtinId="25" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -10340,6 +10351,9 @@
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="E1:O1"/>
   </mergeCells>
+  <conditionalFormatting sqref="B1:B1048576">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  </conditionalFormatting>
   <dataValidations count="13">
     <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="WGS 84 decimal degrees" sqref="C28:C1048576" xr:uid="{0D6BC13B-7101-4C34-935E-0FF74090A779}">
       <formula1>-90</formula1>

</xml_diff>

<commit_message>
Changed sedimentation rates and mixing rates to sample variables. Added lists of methods for most of the analyses (on-going!)
</commit_message>
<xml_diff>
--- a/Excel_templates/MOSAIC_input_excel_file_2022.xlsx
+++ b/Excel_templates/MOSAIC_input_excel_file_2022.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20384"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20385"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sparadis\Documents\ETH\MOSAIC\MOSAIC_Client\Excel_templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6203BA1-95BA-4F0B-914B-48BD472F35D8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1D07607-1295-4678-9895-0109438E3F6B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30204" yWindow="10044" windowWidth="40020" windowHeight="22296" tabRatio="694" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30204" yWindow="10044" windowWidth="40020" windowHeight="22296" tabRatio="694" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ARTICLE_AUTHOR" sheetId="3" r:id="rId1"/>
@@ -20,19 +20,24 @@
     <sheet name="SET_VARIABLES" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
+    <definedName name="Age_14C_ybp">SET_VARIABLES!$GZ$2:$GZ$17</definedName>
     <definedName name="Argentina">SET_VARIABLES!$P$2:$P$8</definedName>
     <definedName name="Australia">SET_VARIABLES!$Q$2:$Q$28</definedName>
     <definedName name="Bangladesh">SET_VARIABLES!$R$2:$R$5</definedName>
+    <definedName name="Be7_Bq_kg">SET_VARIABLES!$GU$2:$GU$3</definedName>
     <definedName name="Belgium">SET_VARIABLES!$S$2:$S$6</definedName>
     <definedName name="Bermuda">SET_VARIABLES!$T$4</definedName>
     <definedName name="Brazil">SET_VARIABLES!$U$2:$U$12</definedName>
     <definedName name="C_lab">SET_VARIABLES!$G$2:$G$277</definedName>
+    <definedName name="CaCO3_">SET_VARIABLES!$FZ$2:$FZ$4</definedName>
     <definedName name="Canada">SET_VARIABLES!$V$2:$V$19</definedName>
     <definedName name="Chile">SET_VARIABLES!$W$2:$W$5</definedName>
     <definedName name="China">SET_VARIABLES!$X$2:$X$9</definedName>
+    <definedName name="clay__2microm">SET_VARIABLES!$FO$2:$FO$4</definedName>
+    <definedName name="clay__4microm">SET_VARIABLES!$FN$2:$FN$4</definedName>
     <definedName name="Colombia">SET_VARIABLES!$Y$2:$Y$7</definedName>
     <definedName name="Core_Analyses">SET_VARIABLES!$BQ$2:$BQ$43</definedName>
-    <definedName name="core_analyses_type">SET_VARIABLES!$BF$2:$BF$9</definedName>
+    <definedName name="core_analyses_type">SET_VARIABLES!$BF$2:$BF$7</definedName>
     <definedName name="core_anthropogenic_disturbance">SET_VARIABLES!#REF!</definedName>
     <definedName name="core_biogeochemical_properties">SET_VARIABLES!$CG$2:$CG$22</definedName>
     <definedName name="core_bottom_water">SET_VARIABLES!$CD$2:$CD$12</definedName>
@@ -42,41 +47,74 @@
     <definedName name="core_sediment_mixing">SET_VARIABLES!$BM$2:$BM$7</definedName>
     <definedName name="core_sediment_properties">SET_VARIABLES!$BT$2</definedName>
     <definedName name="core_sedimentation_rate">SET_VARIABLES!$BG$2:$BG$11</definedName>
+    <definedName name="Cs137_Bq_kg">SET_VARIABLES!$GR$2:$GR$4</definedName>
+    <definedName name="cumulative_dry_mass_g_cm2">SET_VARIABLES!$FU$2:$FU$4</definedName>
+    <definedName name="dating_year">SET_VARIABLES!$FV$2:$FV$8</definedName>
+    <definedName name="Delta_13C">SET_VARIABLES!$GM$2:$GM$4</definedName>
+    <definedName name="Delta_14C">SET_VARIABLES!$GJ$2:$GJ$4</definedName>
+    <definedName name="Delta_15N">SET_VARIABLES!$GO$2:$GO$4</definedName>
+    <definedName name="Delta_18O">SET_VARIABLES!$GN$2:$GN$4</definedName>
     <definedName name="Denmark">SET_VARIABLES!$Z$2:$Z$11</definedName>
+    <definedName name="dry_bulk_density_g_cm3">SET_VARIABLES!$FH$2:$FH$4</definedName>
+    <definedName name="Excess_Pb210_Bq_kg">SET_VARIABLES!$GQ$2:$GQ$5</definedName>
+    <definedName name="Excess_Th228_Bq_kg">SET_VARIABLES!$GV$2:$GV$4</definedName>
     <definedName name="Finland">SET_VARIABLES!$AA$2:$AA$12</definedName>
+    <definedName name="Fm_14C">SET_VARIABLES!$GK$2:$GK$4</definedName>
     <definedName name="France">SET_VARIABLES!$AB$2:$AB$20</definedName>
     <definedName name="geomorphological_site">SET_VARIABLES!$K$2:$K$26</definedName>
     <definedName name="Germany">SET_VARIABLES!$AC$2:$AC$29</definedName>
+    <definedName name="gravel_">SET_VARIABLES!$FK$2:$FK$4</definedName>
     <definedName name="Greece">SET_VARIABLES!$AD$2:$AD$8</definedName>
     <definedName name="Iceland">SET_VARIABLES!$AE$2:$AE$5</definedName>
     <definedName name="India">SET_VARIABLES!$AF$2:$AF$25</definedName>
+    <definedName name="inorganic_nitrogen_">SET_VARIABLES!$GB$2:$GB$4</definedName>
     <definedName name="Iran">SET_VARIABLES!$AG$2:$AG$4</definedName>
     <definedName name="Ireland">SET_VARIABLES!$AH$2:$AH$9</definedName>
     <definedName name="Italy">SET_VARIABLES!$AI$2:$AI$29</definedName>
     <definedName name="Japan">SET_VARIABLES!$AJ$2:$AJ$20</definedName>
+    <definedName name="K37_ng_g">SET_VARIABLES!$HC$2:$HC$4</definedName>
+    <definedName name="K38_ng_g">SET_VARIABLES!$HD$2:$HD$4</definedName>
+    <definedName name="K38Et_ng_g">SET_VARIABLES!$HE$2:$HE$4</definedName>
+    <definedName name="K38Me_ng_g">SET_VARIABLES!$HF$2:$HF$4</definedName>
     <definedName name="Lebanon">SET_VARIABLES!$AK$2:$AK$4</definedName>
+    <definedName name="MAR_g_cm2_yr">SET_VARIABLES!$GY$2:$GY$17</definedName>
     <definedName name="MAR_model">SET_VARIABLES!$BL$2:$BL$9</definedName>
     <definedName name="MAR_tracer">SET_VARIABLES!$BJ$2:$BJ$12</definedName>
     <definedName name="material_analyzed">SET_VARIABLES!$CM$2:$CM$29</definedName>
     <definedName name="Mauritania">SET_VARIABLES!$AL$2:$AL$7</definedName>
+    <definedName name="mean_grain_size_microm">SET_VARIABLES!$FQ$2:$FQ$4</definedName>
+    <definedName name="median_grain_size_microm">SET_VARIABLES!$FR$2:$FR$4</definedName>
+    <definedName name="Mixing_rate_cm2_yr">SET_VARIABLES!$HB$2:$HB$13</definedName>
     <definedName name="Mixing_rate_tracer">SET_VARIABLES!$BP$3:$BP$13</definedName>
+    <definedName name="mode_grain_size_microm">SET_VARIABLES!$FS$2:$FS$4</definedName>
+    <definedName name="mud_silt_clay_">SET_VARIABLES!$FP$2:$FP$4</definedName>
     <definedName name="Netherlands">SET_VARIABLES!$AM$2:$AM$13</definedName>
     <definedName name="New_Zealand">SET_VARIABLES!$AN$2:$AN$13</definedName>
     <definedName name="Norway">SET_VARIABLES!$AO$2:$AO$13</definedName>
+    <definedName name="OCON_ratio">SET_VARIABLES!$GD$2:$GD$4</definedName>
+    <definedName name="OCTN_ratio">SET_VARIABLES!$GE$2:$GE$4</definedName>
+    <definedName name="OM_LOI_">SET_VARIABLES!$FX$2:$FX$8</definedName>
+    <definedName name="organic_nitrogen_">SET_VARIABLES!$GA$2:$GA$4</definedName>
+    <definedName name="P_org_">SET_VARIABLES!$GG$2:$GG$4</definedName>
+    <definedName name="P_total_">SET_VARIABLES!$GF$2:$GF$4</definedName>
     <definedName name="Pakistan">SET_VARIABLES!$AP$2:$AP$4</definedName>
     <definedName name="Peru">SET_VARIABLES!$AQ$2:$AQ$7</definedName>
     <definedName name="Philippines">SET_VARIABLES!$AR$2:$AR$7</definedName>
     <definedName name="Poland">SET_VARIABLES!$AS$2:$AS$21</definedName>
+    <definedName name="porosity">SET_VARIABLES!$FI$2:$FI$6</definedName>
     <definedName name="Portugal">SET_VARIABLES!$AT$4:$AT$14</definedName>
+    <definedName name="Ra224_Bq_kg">SET_VARIABLES!$GX$2:$GX$5</definedName>
+    <definedName name="Ra226_Bq_kg">SET_VARIABLES!$GS$2:$GS$5</definedName>
     <definedName name="Republic_of_Korea">SET_VARIABLES!$AV$2:$AV$6</definedName>
     <definedName name="Research_Vessel_Countries">SET_VARIABLES!$O$2:$O$44</definedName>
     <definedName name="Romania">SET_VARIABLES!$AU$2:$AU$4</definedName>
     <definedName name="Russia">SET_VARIABLES!$AW$2:$AW$134</definedName>
+    <definedName name="S_total_">SET_VARIABLES!$GI$2:$GI$4</definedName>
     <definedName name="sample_14C">SET_VARIABLES!$CT$2:$CT$9</definedName>
     <definedName name="sample_aliphatic_carbons">SET_VARIABLES!$DO$2:$DO$32</definedName>
     <definedName name="sample_alkenones">SET_VARIABLES!$DL$2:$DL$11</definedName>
     <definedName name="sample_amino_acids">SET_VARIABLES!$DX$2:$DX$20</definedName>
-    <definedName name="Sample_analyses_types">SET_VARIABLES!$CJ$2:$CJ$20</definedName>
+    <definedName name="Sample_analyses_types">SET_VARIABLES!$CJ$2:$CJ$22</definedName>
     <definedName name="Sample_biomarkers_CuO">SET_VARIABLES!$DI$2:$DI$115</definedName>
     <definedName name="sample_biomarkers_CuO_grouped">SET_VARIABLES!$DF$2:$DF$37</definedName>
     <definedName name="sample_black_carbon">SET_VARIABLES!$EG$2:$EG$5</definedName>
@@ -89,20 +127,35 @@
     <definedName name="sample_pore_water">SET_VARIABLES!$ED$2:$ED$8</definedName>
     <definedName name="Sample_radioisotopes">SET_VARIABLES!$DC$2:$DC$17</definedName>
     <definedName name="sample_rock_eval_pyrolysis">SET_VARIABLES!$EA$2:$EA$7</definedName>
+    <definedName name="sample_sediment_mixing">SET_VARIABLES!$FB$2:$FB$4</definedName>
     <definedName name="Sample_sediment_properties">SET_VARIABLES!$CN$2:$CN$19</definedName>
+    <definedName name="sample_sedimentation_rate">SET_VARIABLES!$EV$2:$EV$5</definedName>
     <definedName name="Sample_sterols">SET_VARIABLES!$DR$2:$DR$10</definedName>
+    <definedName name="sand_">SET_VARIABLES!$FL$2:$FL$4</definedName>
+    <definedName name="SAR_cm_yr">SET_VARIABLES!$GZ$2:$GZ$17</definedName>
     <definedName name="SAR_model">SET_VARIABLES!$BK$2:$BK$9</definedName>
     <definedName name="SAR_tracer">SET_VARIABLES!$BJ$2:$BJ$12</definedName>
+    <definedName name="silt_">SET_VARIABLES!$FM$2:$FM$4</definedName>
+    <definedName name="SiO2_">SET_VARIABLES!$GH$2:$GH$4</definedName>
+    <definedName name="SML_cm">SET_VARIABLES!$HA$2:$HA$13</definedName>
     <definedName name="SML_tracer">SET_VARIABLES!$BP$2:$BP$13</definedName>
     <definedName name="South_Africa">SET_VARIABLES!$AX$2:$AX$6</definedName>
     <definedName name="Spain">SET_VARIABLES!$AY$2:$AY$18</definedName>
     <definedName name="substrate_classification">SET_VARIABLES!$BW$2:$BW$15</definedName>
+    <definedName name="surface_area_m2_g">SET_VARIABLES!$FT$2:$FT$12</definedName>
     <definedName name="Taiwan_Republic_of_China">SET_VARIABLES!$BA$2:$BA$9</definedName>
-    <definedName name="total_organic_carbon">SET_VARIABLES!$EV$2</definedName>
+    <definedName name="Th232_Bq_kg">SET_VARIABLES!$GW$2:$GW$4</definedName>
+    <definedName name="total_carbon_">SET_VARIABLES!$FW$2:$FW$4</definedName>
+    <definedName name="total_inorganic_carbon_">SET_VARIABLES!$FY$2:$FY$4</definedName>
+    <definedName name="total_nitrogen_">SET_VARIABLES!$GC$2:$GC$4</definedName>
+    <definedName name="total_organic_carbon_">SET_VARIABLES!$FG$2:$FG$5</definedName>
+    <definedName name="Total_Pb210_Bq_kg">SET_VARIABLES!$GP$2:$GP$4</definedName>
     <definedName name="Turkey">SET_VARIABLES!$AZ$2:$AZ$14</definedName>
+    <definedName name="UK38Et">SET_VARIABLES!$HI$2:$HI$4</definedName>
     <definedName name="United_Kingdom">SET_VARIABLES!$BB$2:$BB$63</definedName>
     <definedName name="United_States">SET_VARIABLES!$BC$2:$BC$98</definedName>
     <definedName name="Vietnam">SET_VARIABLES!$BD$2:$BD$4</definedName>
+    <definedName name="water_content_">SET_VARIABLES!$FJ$2:$FJ$4</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
 </workbook>
@@ -133,7 +186,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3589" uniqueCount="2941">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3924" uniqueCount="3010">
   <si>
     <t>sample_name</t>
   </si>
@@ -8956,6 +9009,213 @@
   </si>
   <si>
     <t>MAR_dbd</t>
+  </si>
+  <si>
+    <t>Phosphate concentration in porewater</t>
+  </si>
+  <si>
+    <t>Ammonia concentration in porewater</t>
+  </si>
+  <si>
+    <t>Nitrate concentration in porewater</t>
+  </si>
+  <si>
+    <t>Silicate concentration in porewater</t>
+  </si>
+  <si>
+    <t>Iron concentration in porewater</t>
+  </si>
+  <si>
+    <t>Manganese concentration in porewater</t>
+  </si>
+  <si>
+    <t>Chlorophyll concentration in porewater</t>
+  </si>
+  <si>
+    <t>224Ra concentration in sediment sample.</t>
+  </si>
+  <si>
+    <t>Error in the 226Ra concentration in sediment sample.</t>
+  </si>
+  <si>
+    <t>Error in the 224Ra concentration in sediment sample.</t>
+  </si>
+  <si>
+    <t>Ra224_Bq_kg</t>
+  </si>
+  <si>
+    <t>Ra224_Bq_kg_error</t>
+  </si>
+  <si>
+    <t>sample_sedimentation_rate</t>
+  </si>
+  <si>
+    <t>sample_sediment_mixing</t>
+  </si>
+  <si>
+    <t>Sedimentation rate of specific samples</t>
+  </si>
+  <si>
+    <t>Sediment mixing of specific samples</t>
+  </si>
+  <si>
+    <t>Methods</t>
+  </si>
+  <si>
+    <t>alpha</t>
+  </si>
+  <si>
+    <t>gamma (46 keV)</t>
+  </si>
+  <si>
+    <t>gamma (662 keV)</t>
+  </si>
+  <si>
+    <t>gamma (unknown keV)</t>
+  </si>
+  <si>
+    <t>gamma Pb-214 (295 keV)</t>
+  </si>
+  <si>
+    <t>gamma Pb-214 (352 keV)</t>
+  </si>
+  <si>
+    <t>beta</t>
+  </si>
+  <si>
+    <t>gamma (63 keV)</t>
+  </si>
+  <si>
+    <t>gamma (93 keV)</t>
+  </si>
+  <si>
+    <t>wet and dry weight</t>
+  </si>
+  <si>
+    <t>laser</t>
+  </si>
+  <si>
+    <t>sieving</t>
+  </si>
+  <si>
+    <t>350 °C 2 hours</t>
+  </si>
+  <si>
+    <t>500 °C 2 hours</t>
+  </si>
+  <si>
+    <t>650 °C 2 hours</t>
+  </si>
+  <si>
+    <t>350 °C 4 hours</t>
+  </si>
+  <si>
+    <t>500 °C 4 hours</t>
+  </si>
+  <si>
+    <t>650 °C 4 hours</t>
+  </si>
+  <si>
+    <t>Pb-210 CFCS</t>
+  </si>
+  <si>
+    <t>Pb-210 CIC</t>
+  </si>
+  <si>
+    <t>Pb-210 CRS</t>
+  </si>
+  <si>
+    <t>other</t>
+  </si>
+  <si>
+    <t>inorganic carbon 100/12 molecular mass ratio</t>
+  </si>
+  <si>
+    <t>molar mass ratio</t>
+  </si>
+  <si>
+    <t>gamma (478 keV)</t>
+  </si>
+  <si>
+    <t>alpha Po-210</t>
+  </si>
+  <si>
+    <t>gamma Pb-212 (239 keV)</t>
+  </si>
+  <si>
+    <t>gamma Ac-228 (911 keV)</t>
+  </si>
+  <si>
+    <t>Pb-210 Cs-137 CFCS</t>
+  </si>
+  <si>
+    <t>Pb-210 Cs-137 CRS</t>
+  </si>
+  <si>
+    <t>Pb-210 Cs-137 CIC</t>
+  </si>
+  <si>
+    <t>Pb-210 max penetration</t>
+  </si>
+  <si>
+    <t>Cs-137 max penetration</t>
+  </si>
+  <si>
+    <t>SAR x dry bulk density</t>
+  </si>
+  <si>
+    <t>MAR / dry bulk density</t>
+  </si>
+  <si>
+    <t>RadeCC</t>
+  </si>
+  <si>
+    <t>total mass ratio</t>
+  </si>
+  <si>
+    <t>AVS (acidic volatized sulfur)</t>
+  </si>
+  <si>
+    <t>dry volume and volume sampled</t>
+  </si>
+  <si>
+    <t>titration</t>
+  </si>
+  <si>
+    <t>total and organic carbon</t>
+  </si>
+  <si>
+    <t>coulorometry</t>
+  </si>
+  <si>
+    <t>combustion mass loss</t>
+  </si>
+  <si>
+    <t>BET unknown point</t>
+  </si>
+  <si>
+    <t>BET N2 2 point</t>
+  </si>
+  <si>
+    <t>BET N2 1 point</t>
+  </si>
+  <si>
+    <t>BET N2 3 point</t>
+  </si>
+  <si>
+    <t>BET N2 4 point</t>
+  </si>
+  <si>
+    <t>BET N2 5 point</t>
+  </si>
+  <si>
+    <t>BET N2 6 point</t>
+  </si>
+  <si>
+    <t>BET analyser</t>
+  </si>
+  <si>
+    <t>Mercury</t>
   </si>
 </sst>
 </file>
@@ -9429,7 +9689,7 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="112">
+  <cellXfs count="116">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="13" applyFont="1" applyFill="1" applyAlignment="1"/>
@@ -9557,6 +9817,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="19" fillId="4" borderId="4" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
@@ -9643,6 +9905,8 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="16">
     <cellStyle name="20% - Accent1" xfId="3" builtinId="30" customBuiltin="1"/>
@@ -9986,7 +10250,7 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -10007,15 +10271,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="64" customFormat="1" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="84" t="s">
+      <c r="A1" s="86" t="s">
         <v>2676</v>
       </c>
-      <c r="B1" s="84"/>
-      <c r="C1" s="84"/>
-      <c r="D1" s="84"/>
-      <c r="E1" s="84"/>
-      <c r="F1" s="84"/>
-      <c r="G1" s="84"/>
+      <c r="B1" s="86"/>
+      <c r="C1" s="86"/>
+      <c r="D1" s="86"/>
+      <c r="E1" s="86"/>
+      <c r="F1" s="86"/>
+      <c r="G1" s="86"/>
     </row>
     <row r="2" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="53" t="s">
@@ -10104,25 +10368,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="63" customFormat="1" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="85" t="s">
+      <c r="A1" s="87" t="s">
         <v>2677</v>
       </c>
-      <c r="B1" s="85"/>
-      <c r="C1" s="85"/>
-      <c r="D1" s="85"/>
-      <c r="E1" s="86" t="s">
+      <c r="B1" s="87"/>
+      <c r="C1" s="87"/>
+      <c r="D1" s="87"/>
+      <c r="E1" s="88" t="s">
         <v>2817</v>
       </c>
-      <c r="F1" s="86"/>
-      <c r="G1" s="86"/>
-      <c r="H1" s="86"/>
-      <c r="I1" s="86"/>
-      <c r="J1" s="86"/>
-      <c r="K1" s="86"/>
-      <c r="L1" s="86"/>
-      <c r="M1" s="86"/>
-      <c r="N1" s="86"/>
-      <c r="O1" s="86"/>
+      <c r="F1" s="88"/>
+      <c r="G1" s="88"/>
+      <c r="H1" s="88"/>
+      <c r="I1" s="88"/>
+      <c r="J1" s="88"/>
+      <c r="K1" s="88"/>
+      <c r="L1" s="88"/>
+      <c r="M1" s="88"/>
+      <c r="N1" s="88"/>
+      <c r="O1" s="88"/>
     </row>
     <row r="2" spans="1:15" s="66" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="62" t="s">
@@ -10420,7 +10684,7 @@
       <pane xSplit="2" ySplit="5" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="A6" sqref="A6"/>
+      <selection pane="bottomRight" activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -10437,60 +10701,45 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:35" s="55" customFormat="1" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="87" t="s">
+      <c r="A1" s="89" t="s">
         <v>2679</v>
       </c>
-      <c r="B1" s="87"/>
-      <c r="C1" s="87" t="s">
+      <c r="B1" s="89"/>
+      <c r="C1" s="89" t="s">
         <v>2678</v>
       </c>
-      <c r="D1" s="87"/>
-      <c r="E1" s="87"/>
-      <c r="F1" s="87"/>
+      <c r="D1" s="89"/>
+      <c r="E1" s="89"/>
+      <c r="F1" s="89"/>
       <c r="G1" s="55" t="s">
-        <v>2218</v>
-      </c>
-      <c r="H1" s="55" t="s">
-        <v>2217</v>
-      </c>
-      <c r="I1" s="55" t="s">
-        <v>2217</v>
-      </c>
-      <c r="J1" s="55" t="s">
         <v>2832</v>
       </c>
     </row>
     <row r="2" spans="1:35" ht="15.6" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="88" t="s">
+      <c r="A2" s="90" t="s">
         <v>2567</v>
       </c>
-      <c r="B2" s="88" t="s">
+      <c r="B2" s="90" t="s">
         <v>1825</v>
       </c>
-      <c r="C2" s="88" t="s">
+      <c r="C2" s="90" t="s">
         <v>1834</v>
       </c>
-      <c r="D2" s="88" t="s">
+      <c r="D2" s="90" t="s">
         <v>2686</v>
       </c>
-      <c r="E2" s="88" t="s">
+      <c r="E2" s="90" t="s">
         <v>1823</v>
       </c>
-      <c r="F2" s="91" t="s">
+      <c r="F2" s="93" t="s">
         <v>1824</v>
       </c>
       <c r="G2" s="56" t="s">
-        <v>2815</v>
-      </c>
-      <c r="H2" s="56" t="s">
-        <v>2807</v>
-      </c>
-      <c r="I2" s="56" t="s">
-        <v>1757</v>
-      </c>
-      <c r="J2" s="56" t="s">
-        <v>1758</v>
-      </c>
+        <v>2246</v>
+      </c>
+      <c r="H2" s="56"/>
+      <c r="I2" s="56"/>
+      <c r="J2" s="56"/>
       <c r="K2" s="56"/>
       <c r="L2" s="56"/>
       <c r="M2" s="56"/>
@@ -10518,12 +10767,12 @@
       <c r="AI2" s="56"/>
     </row>
     <row r="3" spans="1:35" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="89"/>
-      <c r="B3" s="89"/>
-      <c r="C3" s="89"/>
-      <c r="D3" s="89"/>
-      <c r="E3" s="89"/>
-      <c r="F3" s="92"/>
+      <c r="A3" s="91"/>
+      <c r="B3" s="91"/>
+      <c r="C3" s="91"/>
+      <c r="D3" s="91"/>
+      <c r="E3" s="91"/>
+      <c r="F3" s="94"/>
       <c r="G3" s="56"/>
       <c r="H3" s="56"/>
       <c r="I3" s="56"/>
@@ -10555,12 +10804,12 @@
       <c r="AI3" s="56"/>
     </row>
     <row r="4" spans="1:35" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="90"/>
-      <c r="B4" s="90"/>
-      <c r="C4" s="90"/>
-      <c r="D4" s="90"/>
-      <c r="E4" s="90"/>
-      <c r="F4" s="92"/>
+      <c r="A4" s="92"/>
+      <c r="B4" s="92"/>
+      <c r="C4" s="92"/>
+      <c r="D4" s="92"/>
+      <c r="E4" s="92"/>
+      <c r="F4" s="94"/>
       <c r="G4" s="56"/>
       <c r="H4" s="56"/>
       <c r="I4" s="56"/>
@@ -10592,12 +10841,12 @@
       <c r="AI4" s="56"/>
     </row>
     <row r="5" spans="1:35" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="90"/>
-      <c r="B5" s="90"/>
-      <c r="C5" s="90"/>
-      <c r="D5" s="90"/>
-      <c r="E5" s="90"/>
-      <c r="F5" s="92"/>
+      <c r="A5" s="92"/>
+      <c r="B5" s="92"/>
+      <c r="C5" s="92"/>
+      <c r="D5" s="92"/>
+      <c r="E5" s="92"/>
+      <c r="F5" s="94"/>
       <c r="G5" s="56"/>
       <c r="H5" s="56"/>
       <c r="I5" s="56"/>
@@ -11887,13 +12136,13 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3CFE241-5737-4A2C-8697-F7D7B3FD7C10}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:CB51"/>
+  <dimension ref="A1:CB52"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="3" ySplit="5" topLeftCell="D6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="6" topLeftCell="H7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="A6" sqref="A6"/>
+      <selection pane="bottomRight" activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -11908,91 +12157,94 @@
     <col min="11" max="11" width="16" style="78" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="22.5" style="57" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="24.59765625" style="57" bestFit="1" customWidth="1"/>
-    <col min="14" max="80" width="15.69921875" style="57" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="31.3984375" style="57" bestFit="1" customWidth="1"/>
+    <col min="15" max="80" width="15.69921875" style="57" bestFit="1" customWidth="1"/>
     <col min="81" max="16384" width="15" style="29"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:80" s="79" customFormat="1" ht="20.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="93" t="s">
+      <c r="A1" s="95" t="s">
         <v>2688</v>
       </c>
-      <c r="B1" s="94"/>
-      <c r="C1" s="95"/>
-      <c r="D1" s="93" t="s">
+      <c r="B1" s="96"/>
+      <c r="C1" s="97"/>
+      <c r="D1" s="95" t="s">
         <v>2678</v>
       </c>
-      <c r="E1" s="94"/>
-      <c r="F1" s="94"/>
-      <c r="G1" s="95"/>
-      <c r="H1" s="96" t="s">
+      <c r="E1" s="96"/>
+      <c r="F1" s="96"/>
+      <c r="G1" s="97"/>
+      <c r="H1" s="98" t="s">
         <v>2680</v>
       </c>
-      <c r="I1" s="97"/>
-      <c r="J1" s="97"/>
-      <c r="K1" s="98"/>
+      <c r="I1" s="99"/>
+      <c r="J1" s="99"/>
+      <c r="K1" s="100"/>
       <c r="L1" s="79" t="s">
         <v>1840</v>
       </c>
       <c r="M1" s="79" t="s">
+        <v>1840</v>
+      </c>
+      <c r="N1" s="79" t="s">
         <v>1841</v>
-      </c>
-      <c r="N1" s="79" t="s">
-        <v>2882</v>
       </c>
       <c r="O1" s="79" t="s">
         <v>2898</v>
       </c>
       <c r="P1" s="79" t="s">
-        <v>2112</v>
+        <v>2953</v>
       </c>
     </row>
     <row r="2" spans="1:80" s="81" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="99" t="s">
+      <c r="A2" s="101" t="s">
         <v>2567</v>
       </c>
-      <c r="B2" s="102" t="s">
+      <c r="B2" s="104" t="s">
         <v>1825</v>
       </c>
-      <c r="C2" s="105" t="s">
+      <c r="C2" s="107" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="100" t="s">
+      <c r="D2" s="102" t="s">
         <v>1834</v>
       </c>
-      <c r="E2" s="103" t="s">
+      <c r="E2" s="105" t="s">
         <v>2686</v>
       </c>
-      <c r="F2" s="103" t="s">
+      <c r="F2" s="105" t="s">
         <v>1823</v>
       </c>
-      <c r="G2" s="106" t="s">
+      <c r="G2" s="108" t="s">
         <v>1824</v>
       </c>
-      <c r="H2" s="99" t="s">
+      <c r="H2" s="101" t="s">
         <v>1835</v>
       </c>
-      <c r="I2" s="102" t="s">
+      <c r="I2" s="104" t="s">
         <v>1836</v>
       </c>
-      <c r="J2" s="102" t="s">
+      <c r="J2" s="104" t="s">
         <v>1837</v>
       </c>
-      <c r="K2" s="108" t="s">
+      <c r="K2" s="110" t="s">
         <v>1838</v>
       </c>
       <c r="L2" s="80" t="s">
         <v>2052</v>
       </c>
       <c r="M2" s="80" t="s">
-        <v>2062</v>
+        <v>2193</v>
       </c>
       <c r="N2" s="80" t="s">
-        <v>2887</v>
+        <v>1843</v>
       </c>
       <c r="O2" s="80" t="s">
         <v>2900</v>
       </c>
-      <c r="P2" s="80"/>
+      <c r="P2" s="80" t="s">
+        <v>2807</v>
+      </c>
       <c r="Q2" s="80"/>
       <c r="R2" s="80"/>
       <c r="S2" s="80"/>
@@ -12059,18 +12311,20 @@
       <c r="CB2" s="80"/>
     </row>
     <row r="3" spans="1:80" s="81" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="100"/>
-      <c r="B3" s="103"/>
-      <c r="C3" s="106"/>
-      <c r="D3" s="100"/>
-      <c r="E3" s="103"/>
-      <c r="F3" s="103"/>
-      <c r="G3" s="106"/>
-      <c r="H3" s="100"/>
-      <c r="I3" s="103"/>
-      <c r="J3" s="103"/>
-      <c r="K3" s="109"/>
-      <c r="L3" s="80"/>
+      <c r="A3" s="102"/>
+      <c r="B3" s="105"/>
+      <c r="C3" s="108"/>
+      <c r="D3" s="102"/>
+      <c r="E3" s="105"/>
+      <c r="F3" s="105"/>
+      <c r="G3" s="108"/>
+      <c r="H3" s="102"/>
+      <c r="I3" s="105"/>
+      <c r="J3" s="105"/>
+      <c r="K3" s="111"/>
+      <c r="L3" s="80" t="s">
+        <v>2936</v>
+      </c>
       <c r="M3" s="80"/>
       <c r="N3" s="80"/>
       <c r="O3" s="80"/>
@@ -12141,17 +12395,17 @@
       <c r="CB3" s="80"/>
     </row>
     <row r="4" spans="1:80" s="81" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="100"/>
-      <c r="B4" s="103"/>
-      <c r="C4" s="106"/>
-      <c r="D4" s="100"/>
-      <c r="E4" s="103"/>
-      <c r="F4" s="103"/>
-      <c r="G4" s="106"/>
-      <c r="H4" s="100"/>
-      <c r="I4" s="103"/>
-      <c r="J4" s="103"/>
-      <c r="K4" s="109"/>
+      <c r="A4" s="102"/>
+      <c r="B4" s="105"/>
+      <c r="C4" s="108"/>
+      <c r="D4" s="102"/>
+      <c r="E4" s="105"/>
+      <c r="F4" s="105"/>
+      <c r="G4" s="108"/>
+      <c r="H4" s="102"/>
+      <c r="I4" s="105"/>
+      <c r="J4" s="105"/>
+      <c r="K4" s="111"/>
       <c r="L4" s="80"/>
       <c r="M4" s="80"/>
       <c r="N4" s="80"/>
@@ -12222,18 +12476,18 @@
       <c r="CA4" s="80"/>
       <c r="CB4" s="80"/>
     </row>
-    <row r="5" spans="1:80" s="81" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="101"/>
-      <c r="B5" s="104"/>
-      <c r="C5" s="107"/>
-      <c r="D5" s="101"/>
-      <c r="E5" s="104"/>
-      <c r="F5" s="104"/>
-      <c r="G5" s="107"/>
-      <c r="H5" s="101"/>
-      <c r="I5" s="104"/>
-      <c r="J5" s="104"/>
-      <c r="K5" s="110"/>
+    <row r="5" spans="1:80" s="81" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="102"/>
+      <c r="B5" s="105"/>
+      <c r="C5" s="108"/>
+      <c r="D5" s="102"/>
+      <c r="E5" s="105"/>
+      <c r="F5" s="105"/>
+      <c r="G5" s="108"/>
+      <c r="H5" s="102"/>
+      <c r="I5" s="105"/>
+      <c r="J5" s="105"/>
+      <c r="K5" s="111"/>
       <c r="L5" s="80"/>
       <c r="M5" s="80"/>
       <c r="N5" s="80"/>
@@ -12304,151 +12558,160 @@
       <c r="CA5" s="80"/>
       <c r="CB5" s="80"/>
     </row>
-    <row r="6" spans="1:80" x14ac:dyDescent="0.3">
-      <c r="H6" s="41"/>
-      <c r="I6" s="39"/>
-      <c r="L6" s="58"/>
-      <c r="M6" s="41"/>
-      <c r="N6" s="60"/>
-      <c r="O6" s="60"/>
-      <c r="P6" s="60"/>
-      <c r="Q6" s="58"/>
-      <c r="R6" s="58"/>
-      <c r="S6" s="58"/>
-      <c r="T6" s="58"/>
-      <c r="U6" s="58"/>
-      <c r="V6" s="58"/>
-      <c r="W6" s="58"/>
-      <c r="X6" s="58"/>
-      <c r="Y6" s="58"/>
-      <c r="Z6" s="58"/>
-      <c r="AA6" s="58"/>
-      <c r="AB6" s="58"/>
-      <c r="AC6" s="58"/>
-      <c r="AD6" s="58"/>
-      <c r="AE6" s="58"/>
-      <c r="AF6" s="58"/>
-      <c r="AG6" s="58"/>
-      <c r="AH6" s="58"/>
-      <c r="AI6" s="58"/>
-      <c r="AJ6" s="58"/>
-      <c r="AK6" s="58"/>
-      <c r="AL6" s="58"/>
-      <c r="AM6" s="58"/>
-      <c r="AN6" s="58"/>
-      <c r="AO6" s="58"/>
-      <c r="AP6" s="58"/>
-      <c r="AQ6" s="58"/>
-      <c r="AR6" s="58"/>
-      <c r="AS6" s="58"/>
-      <c r="AT6" s="58"/>
-      <c r="AU6" s="58"/>
-      <c r="AV6" s="58"/>
-      <c r="AW6" s="58"/>
-      <c r="AX6" s="58"/>
-      <c r="AY6" s="58"/>
-      <c r="AZ6" s="58"/>
-      <c r="BA6" s="58"/>
-      <c r="BB6" s="58"/>
-      <c r="BC6" s="58"/>
-      <c r="BD6" s="58"/>
-      <c r="BE6" s="58"/>
-      <c r="BF6" s="58"/>
-      <c r="BG6" s="58"/>
-      <c r="BH6" s="58"/>
-      <c r="BI6" s="58"/>
-      <c r="BJ6" s="58"/>
-      <c r="BK6" s="58"/>
-      <c r="BL6" s="58"/>
-      <c r="BM6" s="58"/>
-      <c r="BN6" s="58"/>
-      <c r="BO6" s="58"/>
-      <c r="BP6" s="58"/>
-      <c r="BQ6" s="58"/>
-      <c r="BR6" s="58"/>
-      <c r="BS6" s="58"/>
-      <c r="BT6" s="58"/>
-      <c r="BU6" s="58"/>
-      <c r="BV6" s="58"/>
-      <c r="BW6" s="58"/>
-      <c r="BX6" s="58"/>
-      <c r="BY6" s="58"/>
-      <c r="BZ6" s="58"/>
-      <c r="CA6" s="58"/>
-      <c r="CB6" s="58"/>
+    <row r="6" spans="1:80" s="81" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="103"/>
+      <c r="B6" s="106"/>
+      <c r="C6" s="109"/>
+      <c r="D6" s="103"/>
+      <c r="E6" s="106"/>
+      <c r="F6" s="106"/>
+      <c r="G6" s="109"/>
+      <c r="H6" s="103"/>
+      <c r="I6" s="106"/>
+      <c r="J6" s="106"/>
+      <c r="K6" s="112"/>
+      <c r="L6" s="80"/>
+      <c r="M6" s="80"/>
+      <c r="N6" s="80"/>
+      <c r="O6" s="80"/>
+      <c r="P6" s="80"/>
+      <c r="Q6" s="80"/>
+      <c r="R6" s="80"/>
+      <c r="S6" s="80"/>
+      <c r="T6" s="80"/>
+      <c r="U6" s="80"/>
+      <c r="V6" s="80"/>
+      <c r="W6" s="80"/>
+      <c r="X6" s="80"/>
+      <c r="Y6" s="80"/>
+      <c r="Z6" s="80"/>
+      <c r="AA6" s="80"/>
+      <c r="AB6" s="80"/>
+      <c r="AC6" s="80"/>
+      <c r="AD6" s="80"/>
+      <c r="AE6" s="80"/>
+      <c r="AF6" s="80"/>
+      <c r="AG6" s="80"/>
+      <c r="AH6" s="80"/>
+      <c r="AI6" s="80"/>
+      <c r="AJ6" s="80"/>
+      <c r="AK6" s="80"/>
+      <c r="AL6" s="80"/>
+      <c r="AM6" s="80"/>
+      <c r="AN6" s="80"/>
+      <c r="AO6" s="80"/>
+      <c r="AP6" s="80"/>
+      <c r="AQ6" s="80"/>
+      <c r="AR6" s="80"/>
+      <c r="AS6" s="80"/>
+      <c r="AT6" s="80"/>
+      <c r="AU6" s="80"/>
+      <c r="AV6" s="80"/>
+      <c r="AW6" s="80"/>
+      <c r="AX6" s="80"/>
+      <c r="AY6" s="80"/>
+      <c r="AZ6" s="80"/>
+      <c r="BA6" s="80"/>
+      <c r="BB6" s="80"/>
+      <c r="BC6" s="80"/>
+      <c r="BD6" s="80"/>
+      <c r="BE6" s="80"/>
+      <c r="BF6" s="80"/>
+      <c r="BG6" s="80"/>
+      <c r="BH6" s="80"/>
+      <c r="BI6" s="80"/>
+      <c r="BJ6" s="80"/>
+      <c r="BK6" s="80"/>
+      <c r="BL6" s="80"/>
+      <c r="BM6" s="80"/>
+      <c r="BN6" s="80"/>
+      <c r="BO6" s="80"/>
+      <c r="BP6" s="80"/>
+      <c r="BQ6" s="80"/>
+      <c r="BR6" s="80"/>
+      <c r="BS6" s="80"/>
+      <c r="BT6" s="80"/>
+      <c r="BU6" s="80"/>
+      <c r="BV6" s="80"/>
+      <c r="BW6" s="80"/>
+      <c r="BX6" s="80"/>
+      <c r="BY6" s="80"/>
+      <c r="BZ6" s="80"/>
+      <c r="CA6" s="80"/>
+      <c r="CB6" s="80"/>
     </row>
     <row r="7" spans="1:80" x14ac:dyDescent="0.3">
       <c r="H7" s="41"/>
-      <c r="I7" s="74"/>
-      <c r="L7" s="59"/>
+      <c r="I7" s="39"/>
+      <c r="L7" s="58"/>
       <c r="M7" s="41"/>
       <c r="N7" s="60"/>
       <c r="O7" s="60"/>
       <c r="P7" s="60"/>
       <c r="Q7" s="58"/>
-      <c r="R7" s="59"/>
-      <c r="S7" s="59"/>
-      <c r="T7" s="59"/>
-      <c r="U7" s="59"/>
-      <c r="V7" s="59"/>
-      <c r="W7" s="59"/>
-      <c r="X7" s="59"/>
-      <c r="Y7" s="59"/>
-      <c r="Z7" s="59"/>
-      <c r="AA7" s="59"/>
-      <c r="AB7" s="59"/>
-      <c r="AC7" s="59"/>
-      <c r="AD7" s="59"/>
-      <c r="AE7" s="59"/>
-      <c r="AF7" s="59"/>
-      <c r="AG7" s="59"/>
-      <c r="AH7" s="59"/>
-      <c r="AI7" s="59"/>
-      <c r="AJ7" s="59"/>
-      <c r="AK7" s="59"/>
-      <c r="AL7" s="59"/>
-      <c r="AM7" s="59"/>
-      <c r="AN7" s="59"/>
-      <c r="AO7" s="59"/>
-      <c r="AP7" s="59"/>
-      <c r="AQ7" s="59"/>
-      <c r="AR7" s="59"/>
-      <c r="AS7" s="59"/>
-      <c r="AT7" s="59"/>
-      <c r="AU7" s="59"/>
-      <c r="AV7" s="59"/>
-      <c r="AW7" s="59"/>
-      <c r="AX7" s="59"/>
-      <c r="AY7" s="59"/>
-      <c r="AZ7" s="59"/>
-      <c r="BA7" s="59"/>
-      <c r="BB7" s="59"/>
-      <c r="BC7" s="59"/>
-      <c r="BD7" s="59"/>
-      <c r="BE7" s="59"/>
-      <c r="BF7" s="59"/>
-      <c r="BG7" s="59"/>
-      <c r="BH7" s="59"/>
-      <c r="BI7" s="59"/>
-      <c r="BJ7" s="59"/>
-      <c r="BK7" s="59"/>
-      <c r="BL7" s="59"/>
-      <c r="BM7" s="59"/>
-      <c r="BN7" s="59"/>
-      <c r="BO7" s="59"/>
-      <c r="BP7" s="59"/>
-      <c r="BQ7" s="59"/>
-      <c r="BR7" s="59"/>
-      <c r="BS7" s="59"/>
-      <c r="BT7" s="59"/>
-      <c r="BU7" s="59"/>
-      <c r="BV7" s="59"/>
-      <c r="BW7" s="59"/>
-      <c r="BX7" s="59"/>
-      <c r="BY7" s="59"/>
-      <c r="BZ7" s="59"/>
-      <c r="CA7" s="59"/>
-      <c r="CB7" s="59"/>
+      <c r="R7" s="58"/>
+      <c r="S7" s="58"/>
+      <c r="T7" s="58"/>
+      <c r="U7" s="58"/>
+      <c r="V7" s="58"/>
+      <c r="W7" s="58"/>
+      <c r="X7" s="58"/>
+      <c r="Y7" s="58"/>
+      <c r="Z7" s="58"/>
+      <c r="AA7" s="58"/>
+      <c r="AB7" s="58"/>
+      <c r="AC7" s="58"/>
+      <c r="AD7" s="58"/>
+      <c r="AE7" s="58"/>
+      <c r="AF7" s="58"/>
+      <c r="AG7" s="58"/>
+      <c r="AH7" s="58"/>
+      <c r="AI7" s="58"/>
+      <c r="AJ7" s="58"/>
+      <c r="AK7" s="58"/>
+      <c r="AL7" s="58"/>
+      <c r="AM7" s="58"/>
+      <c r="AN7" s="58"/>
+      <c r="AO7" s="58"/>
+      <c r="AP7" s="58"/>
+      <c r="AQ7" s="58"/>
+      <c r="AR7" s="58"/>
+      <c r="AS7" s="58"/>
+      <c r="AT7" s="58"/>
+      <c r="AU7" s="58"/>
+      <c r="AV7" s="58"/>
+      <c r="AW7" s="58"/>
+      <c r="AX7" s="58"/>
+      <c r="AY7" s="58"/>
+      <c r="AZ7" s="58"/>
+      <c r="BA7" s="58"/>
+      <c r="BB7" s="58"/>
+      <c r="BC7" s="58"/>
+      <c r="BD7" s="58"/>
+      <c r="BE7" s="58"/>
+      <c r="BF7" s="58"/>
+      <c r="BG7" s="58"/>
+      <c r="BH7" s="58"/>
+      <c r="BI7" s="58"/>
+      <c r="BJ7" s="58"/>
+      <c r="BK7" s="58"/>
+      <c r="BL7" s="58"/>
+      <c r="BM7" s="58"/>
+      <c r="BN7" s="58"/>
+      <c r="BO7" s="58"/>
+      <c r="BP7" s="58"/>
+      <c r="BQ7" s="58"/>
+      <c r="BR7" s="58"/>
+      <c r="BS7" s="58"/>
+      <c r="BT7" s="58"/>
+      <c r="BU7" s="58"/>
+      <c r="BV7" s="58"/>
+      <c r="BW7" s="58"/>
+      <c r="BX7" s="58"/>
+      <c r="BY7" s="58"/>
+      <c r="BZ7" s="58"/>
+      <c r="CA7" s="58"/>
+      <c r="CB7" s="58"/>
     </row>
     <row r="8" spans="1:80" x14ac:dyDescent="0.3">
       <c r="H8" s="41"/>
@@ -12599,9 +12862,9 @@
     <row r="10" spans="1:80" x14ac:dyDescent="0.3">
       <c r="H10" s="41"/>
       <c r="I10" s="74"/>
-      <c r="L10" s="59"/>
+      <c r="L10" s="41"/>
       <c r="M10" s="41"/>
-      <c r="N10" s="60"/>
+      <c r="N10" s="41"/>
       <c r="O10" s="60"/>
       <c r="P10" s="60"/>
       <c r="Q10" s="58"/>
@@ -12674,7 +12937,7 @@
       <c r="I11" s="74"/>
       <c r="L11" s="59"/>
       <c r="M11" s="41"/>
-      <c r="N11" s="60"/>
+      <c r="N11" s="85"/>
       <c r="O11" s="60"/>
       <c r="P11" s="60"/>
       <c r="Q11" s="58"/>
@@ -13842,10 +14105,10 @@
       <c r="I27" s="74"/>
       <c r="L27" s="59"/>
       <c r="M27" s="41"/>
-      <c r="N27" s="59"/>
-      <c r="O27" s="59"/>
-      <c r="P27" s="59"/>
-      <c r="Q27" s="59"/>
+      <c r="N27" s="60"/>
+      <c r="O27" s="60"/>
+      <c r="P27" s="60"/>
+      <c r="Q27" s="58"/>
       <c r="R27" s="59"/>
       <c r="S27" s="59"/>
       <c r="T27" s="59"/>
@@ -14351,7 +14614,75 @@
     <row r="34" spans="8:80" x14ac:dyDescent="0.3">
       <c r="H34" s="41"/>
       <c r="I34" s="74"/>
+      <c r="L34" s="59"/>
       <c r="M34" s="41"/>
+      <c r="N34" s="59"/>
+      <c r="O34" s="59"/>
+      <c r="P34" s="59"/>
+      <c r="Q34" s="59"/>
+      <c r="R34" s="59"/>
+      <c r="S34" s="59"/>
+      <c r="T34" s="59"/>
+      <c r="U34" s="59"/>
+      <c r="V34" s="59"/>
+      <c r="W34" s="59"/>
+      <c r="X34" s="59"/>
+      <c r="Y34" s="59"/>
+      <c r="Z34" s="59"/>
+      <c r="AA34" s="59"/>
+      <c r="AB34" s="59"/>
+      <c r="AC34" s="59"/>
+      <c r="AD34" s="59"/>
+      <c r="AE34" s="59"/>
+      <c r="AF34" s="59"/>
+      <c r="AG34" s="59"/>
+      <c r="AH34" s="59"/>
+      <c r="AI34" s="59"/>
+      <c r="AJ34" s="59"/>
+      <c r="AK34" s="59"/>
+      <c r="AL34" s="59"/>
+      <c r="AM34" s="59"/>
+      <c r="AN34" s="59"/>
+      <c r="AO34" s="59"/>
+      <c r="AP34" s="59"/>
+      <c r="AQ34" s="59"/>
+      <c r="AR34" s="59"/>
+      <c r="AS34" s="59"/>
+      <c r="AT34" s="59"/>
+      <c r="AU34" s="59"/>
+      <c r="AV34" s="59"/>
+      <c r="AW34" s="59"/>
+      <c r="AX34" s="59"/>
+      <c r="AY34" s="59"/>
+      <c r="AZ34" s="59"/>
+      <c r="BA34" s="59"/>
+      <c r="BB34" s="59"/>
+      <c r="BC34" s="59"/>
+      <c r="BD34" s="59"/>
+      <c r="BE34" s="59"/>
+      <c r="BF34" s="59"/>
+      <c r="BG34" s="59"/>
+      <c r="BH34" s="59"/>
+      <c r="BI34" s="59"/>
+      <c r="BJ34" s="59"/>
+      <c r="BK34" s="59"/>
+      <c r="BL34" s="59"/>
+      <c r="BM34" s="59"/>
+      <c r="BN34" s="59"/>
+      <c r="BO34" s="59"/>
+      <c r="BP34" s="59"/>
+      <c r="BQ34" s="59"/>
+      <c r="BR34" s="59"/>
+      <c r="BS34" s="59"/>
+      <c r="BT34" s="59"/>
+      <c r="BU34" s="59"/>
+      <c r="BV34" s="59"/>
+      <c r="BW34" s="59"/>
+      <c r="BX34" s="59"/>
+      <c r="BY34" s="59"/>
+      <c r="BZ34" s="59"/>
+      <c r="CA34" s="59"/>
+      <c r="CB34" s="59"/>
     </row>
     <row r="35" spans="8:80" x14ac:dyDescent="0.3">
       <c r="H35" s="41"/>
@@ -14437,51 +14768,63 @@
       <c r="H51" s="41"/>
       <c r="I51" s="74"/>
       <c r="M51" s="41"/>
+    </row>
+    <row r="52" spans="8:13" x14ac:dyDescent="0.3">
+      <c r="H52" s="41"/>
+      <c r="I52" s="74"/>
+      <c r="M52" s="41"/>
     </row>
   </sheetData>
   <mergeCells count="14">
     <mergeCell ref="D1:G1"/>
     <mergeCell ref="H1:K1"/>
     <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A2:A5"/>
-    <mergeCell ref="B2:B5"/>
-    <mergeCell ref="C2:C5"/>
-    <mergeCell ref="F2:F5"/>
-    <mergeCell ref="G2:G5"/>
-    <mergeCell ref="H2:H5"/>
-    <mergeCell ref="I2:I5"/>
-    <mergeCell ref="J2:J5"/>
-    <mergeCell ref="K2:K5"/>
-    <mergeCell ref="D2:D5"/>
-    <mergeCell ref="E2:E5"/>
+    <mergeCell ref="A2:A6"/>
+    <mergeCell ref="B2:B6"/>
+    <mergeCell ref="C2:C6"/>
+    <mergeCell ref="F2:F6"/>
+    <mergeCell ref="G2:G6"/>
+    <mergeCell ref="H2:H6"/>
+    <mergeCell ref="I2:I6"/>
+    <mergeCell ref="J2:J6"/>
+    <mergeCell ref="K2:K6"/>
+    <mergeCell ref="D2:D6"/>
+    <mergeCell ref="E2:E6"/>
   </mergeCells>
-  <dataValidations xWindow="389" yWindow="346" count="11">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Write the core_name or select from the drop-down menu the cores you have in the Workbook._x000a_Make sure that the core name matches with its metadata given in GEOPOINTS_CORES sheet" sqref="B2:B3" xr:uid="{6685FF74-A7F2-42C2-901B-99DBBBFECDB4}"/>
+  <dataValidations xWindow="389" yWindow="346" count="14">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Write the core_name or select from the drop-down menu the cores you have in the Workbook._x000a_Make sure that the core name matches with its metadata given in GEOPOINTS_CORES sheet" sqref="B2:B4" xr:uid="{6685FF74-A7F2-42C2-901B-99DBBBFECDB4}"/>
     <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Sample analysis category" prompt="Choose from the drop-down list the analysis category the variable belongs to" sqref="L1:CB1" xr:uid="{2372D2F3-EE0C-4296-AC86-BA3569CC20EF}">
       <formula1>Sample_analyses_types</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Specify if the following analyses are open or private (i.e. published or unpublished)" sqref="D2:D3" xr:uid="{2D0E370F-3B05-4238-897F-C6B71BB62191}"/>
-    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Depth should be positive." prompt="Core depth of the upper limit of the sample (i.e. 0 cm)" sqref="H6:H1048576" xr:uid="{BE1F0784-49D8-4BCD-8064-3F609B2CEBBB}">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Specify if the following analyses are open or private (i.e. published or unpublished)" sqref="D2:D4" xr:uid="{2D0E370F-3B05-4238-897F-C6B71BB62191}"/>
+    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Depth should be positive." prompt="Core depth of the upper limit of the sample (i.e. 0 cm)" sqref="H7:H1048576" xr:uid="{BE1F0784-49D8-4BCD-8064-3F609B2CEBBB}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Core depth should be positive." prompt="Core depth of the lower limit of the sample (i.e. 1 cm)" sqref="I6:I1048576" xr:uid="{903AFEB5-EF00-4CC1-B53D-2984DF88687F}">
+    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Core depth should be positive." prompt="Core depth of the lower limit of the sample (i.e. 1 cm)" sqref="I7:I1048576" xr:uid="{903AFEB5-EF00-4CC1-B53D-2984DF88687F}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Core depth should be positive." prompt="Average sample depth of the sample (i.e. 0.5 cm)" sqref="J6:J1048576" xr:uid="{76CC5D1F-1565-4594-B5AF-8B25948B4A60}">
+    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Core depth should be positive." prompt="Average sample depth of the sample (i.e. 0.5 cm)" sqref="J7:J1048576" xr:uid="{76CC5D1F-1565-4594-B5AF-8B25948B4A60}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="Q7:Q26 L6 N6:CB6" xr:uid="{6673B6D2-9563-46FC-8335-F6B94E523361}">
+    <dataValidation type="list" allowBlank="1" sqref="Q8:Q27 L7 N7:CB7" xr:uid="{6673B6D2-9563-46FC-8335-F6B94E523361}">
       <formula1>INDIRECT(L$2)</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Name of user who is entering data" sqref="A6:A1048576" xr:uid="{4BF522A4-2999-4EF9-835E-16C3A98D1BAF}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Name of user who is entering data" sqref="A7:A1048576" xr:uid="{4BF522A4-2999-4EF9-835E-16C3A98D1BAF}"/>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Sample analysis" prompt="Choose from the drop-down menu the variable to be added" sqref="L2:CB2" xr:uid="{ADED0455-8DDC-445F-B013-7A6BE4A4748B}">
       <formula1>INDIRECT(L1)</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Material analyzed" prompt="Choose from the drop-down menu the material analyzed (i.e. bulk, OC, sand, etc.). If left blank, the default material analyzed (bulk) will be used. If there's a material_analyzed that is missing, please let us know sending an email to mosaic@erdw.eth.ch." sqref="L4:CB4" xr:uid="{B3206B9A-BD85-4C2B-B436-B08F0FC71300}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Material analyzed" prompt="Choose from the drop-down menu the material analyzed (i.e. bulk, OC, sand, etc.). If left blank, the default material analyzed (bulk) will be used. If there's a material_analyzed that is missing, please let us know sending an email to mosaic@erdw.eth.ch." sqref="L5:CB5" xr:uid="{B3206B9A-BD85-4C2B-B436-B08F0FC71300}">
       <formula1>material_analyzed</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Method" prompt="Choose from the drop-down menu the method used to analyze the variable. If unknown, choose _unknown. If the method used is not in the drop-down list, please contact mosaic@erdw.ethz.ch" sqref="L3:CB3" xr:uid="{AE24206A-75B4-4703-8A70-F441CD150FA7}">
-      <formula1>INDIRECT(LEFT(L2,LEN(SUBSTITUTE(L2,"_",""))+1))</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Method" prompt="Choose from the drop-down menu the method used to analyze the variable. If unknown, choose _unknown. If the method used is not in the drop-down list, please contact mosaic@erdw.ethz.ch" sqref="L3 O3:CB3" xr:uid="{AE24206A-75B4-4703-8A70-F441CD150FA7}">
+      <formula1>INDIRECT(SUBSTITUTE(SUBSTITUTE(L2,":",""),"%",""))</formula1>
+    </dataValidation>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Method details" prompt="If known, add any additional information about the method used to obtain the variable, such as the model of the analyzer." sqref="L4:CB4" xr:uid="{A2878DFE-8081-4751-8EA1-1B0E764D61E4}"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Method" prompt="Choose from the drop-down menu the method used to analyze the variable. If unknown, choose _unknown. If the method used is not in the drop-down list, please contact mosaic@erdw.ethz.ch" sqref="M3" xr:uid="{F1209CA9-F3B6-443C-9AF8-06621DB14272}">
+      <formula1>INDIRECT(SUBSTITUTE(SUBSTITUTE(M2,":",""),"%",""))</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Method" prompt="Choose from the drop-down menu the method used to analyze the variable. If unknown, choose _unknown. If the method used is not in the drop-down list, please contact mosaic@erdw.ethz.ch" sqref="N3" xr:uid="{FC1DB26B-EA6D-4B32-BCFB-3680E3C8BBD5}">
+      <formula1>INDIRECT(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(N2,"-",""),":",""),"%",""))</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -14493,37 +14836,37 @@
           <x14:formula1>
             <xm:f>ARTICLE_AUTHOR!$F$3:$F$11</xm:f>
           </x14:formula1>
-          <xm:sqref>F6:F1048576</xm:sqref>
+          <xm:sqref>F7:F1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Write the author/contact person of the core, or select from the drop-down menu the authors you have in the Workbook._x000a_Make sure that the author name matches with its metadata given in Article_Author sheet" xr:uid="{0D093603-B7BD-4D12-AE99-C2A1A46AF914}">
           <x14:formula1>
             <xm:f>ARTICLE_AUTHOR!$G$3:$G$11</xm:f>
           </x14:formula1>
-          <xm:sqref>G6:G1048576</xm:sqref>
+          <xm:sqref>G7:G1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Write the article name or select from the drop-down menu the articles you have in the Workbook._x000a_Make sure that the article name matches with its metadata given in Article_Author sheet" xr:uid="{41F1BC95-4CA6-435B-BAD0-642CD7E39391}">
           <x14:formula1>
             <xm:f>ARTICLE_AUTHOR!$B$3:$B$11</xm:f>
           </x14:formula1>
-          <xm:sqref>E6:E1048576</xm:sqref>
+          <xm:sqref>E7:E1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please state wether data is exlusive (unpublished) for eglinton-group only" promptTitle="Exclusive samples?" prompt="Are these samples for internal use only?" xr:uid="{F93D77B0-FE44-4B6E-9566-255830135751}">
           <x14:formula1>
             <xm:f>SET_VARIABLES!$A$2:$A$3</xm:f>
           </x14:formula1>
-          <xm:sqref>D6:D1048576</xm:sqref>
+          <xm:sqref>D7:D1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Write the core name or select from the drop-down menu the cores you have in the Workbook._x000a_Make sure that the core name matches with its metadata given in GEOPOINTS_CORES sheet" xr:uid="{E4FFB722-8CB2-4C84-A9DE-29D8614FBFFB}">
           <x14:formula1>
             <xm:f>GEOPOINTS_CORES!$B$3:$B$1048576</xm:f>
           </x14:formula1>
-          <xm:sqref>B6:B1048576</xm:sqref>
+          <xm:sqref>B7:B1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Raw / calculated data" prompt="Specify if the data provided has been extracted directly from the source (i.e. paper) or is calculated using available data. If left blank, default of &quot;raw data&quot; will be used. " xr:uid="{30C7084F-BEF5-4E01-80B0-5EBF52EBFAA6}">
           <x14:formula1>
             <xm:f>SET_VARIABLES!$BE$2:$BE$3</xm:f>
           </x14:formula1>
-          <xm:sqref>L5:CB5</xm:sqref>
+          <xm:sqref>L6:CB6</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -14534,10 +14877,10 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr codeName="Sheet6"/>
-  <dimension ref="A1:EV277"/>
+  <dimension ref="A1:HL277"/>
   <sheetViews>
-    <sheetView topLeftCell="BB1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="BK10" sqref="BK10"/>
+    <sheetView tabSelected="1" topLeftCell="FF1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="FJ9" sqref="FJ9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -14561,7 +14904,7 @@
     <col min="82" max="87" width="36" style="20" customWidth="1"/>
     <col min="88" max="88" width="36" style="14" customWidth="1"/>
     <col min="89" max="89" width="96.69921875" style="20" customWidth="1"/>
-    <col min="90" max="90" width="36" style="20" customWidth="1"/>
+    <col min="90" max="90" width="36" style="20" hidden="1" customWidth="1"/>
     <col min="91" max="91" width="36" style="14" customWidth="1"/>
     <col min="92" max="92" width="39.3984375" style="10" bestFit="1" customWidth="1"/>
     <col min="93" max="93" width="32" style="10" bestFit="1" customWidth="1"/>
@@ -14593,9 +14936,13 @@
     <col min="134" max="134" width="18.3984375" bestFit="1" customWidth="1"/>
     <col min="135" max="135" width="28" bestFit="1" customWidth="1"/>
     <col min="136" max="136" width="29.3984375" bestFit="1" customWidth="1"/>
+    <col min="162" max="162" width="11.19921875" style="115"/>
+    <col min="163" max="163" width="21.59765625" bestFit="1" customWidth="1"/>
+    <col min="180" max="180" width="13.09765625" bestFit="1" customWidth="1"/>
+    <col min="198" max="198" width="17.8984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:152" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:220" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -15106,10 +15453,218 @@
         <v>sample_strontium_description</v>
       </c>
       <c r="EV1" s="1" t="s">
+        <v>2953</v>
+      </c>
+      <c r="EW1" s="9" t="str">
+        <f>_xlfn.CONCAT(EV1,"_units")</f>
+        <v>sample_sedimentation_rate_units</v>
+      </c>
+      <c r="EX1" s="9" t="str">
+        <f>_xlfn.CONCAT(EV1,"_description")</f>
+        <v>sample_sedimentation_rate_description</v>
+      </c>
+      <c r="EY1" s="1" t="s">
+        <v>2035</v>
+      </c>
+      <c r="EZ1" s="1" t="s">
+        <v>1757</v>
+      </c>
+      <c r="FA1" s="1" t="s">
+        <v>1756</v>
+      </c>
+      <c r="FB1" s="1" t="s">
+        <v>2954</v>
+      </c>
+      <c r="FC1" s="9" t="str">
+        <f>_xlfn.CONCAT(FB1,"_units")</f>
+        <v>sample_sediment_mixing_units</v>
+      </c>
+      <c r="FD1" s="9" t="str">
+        <f>_xlfn.CONCAT(FB1,"_description")</f>
+        <v>sample_sediment_mixing_description</v>
+      </c>
+      <c r="FE1" s="1" t="s">
+        <v>1753</v>
+      </c>
+      <c r="FF1" s="114" t="s">
+        <v>2957</v>
+      </c>
+      <c r="FG1" s="1" t="s">
         <v>2052</v>
       </c>
-    </row>
-    <row r="2" spans="1:152" x14ac:dyDescent="0.3">
+      <c r="FH1" s="1" t="s">
+        <v>1842</v>
+      </c>
+      <c r="FI1" s="1" t="s">
+        <v>1843</v>
+      </c>
+      <c r="FJ1" s="1" t="s">
+        <v>1844</v>
+      </c>
+      <c r="FK1" s="1" t="s">
+        <v>1845</v>
+      </c>
+      <c r="FL1" s="1" t="s">
+        <v>1846</v>
+      </c>
+      <c r="FM1" s="1" t="s">
+        <v>1847</v>
+      </c>
+      <c r="FN1" s="1" t="s">
+        <v>2914</v>
+      </c>
+      <c r="FO1" s="1" t="s">
+        <v>2915</v>
+      </c>
+      <c r="FP1" s="1" t="s">
+        <v>1848</v>
+      </c>
+      <c r="FQ1" s="1" t="s">
+        <v>1849</v>
+      </c>
+      <c r="FR1" s="1" t="s">
+        <v>2852</v>
+      </c>
+      <c r="FS1" s="1" t="s">
+        <v>2917</v>
+      </c>
+      <c r="FT1" s="1" t="s">
+        <v>2062</v>
+      </c>
+      <c r="FU1" s="1" t="s">
+        <v>2100</v>
+      </c>
+      <c r="FV1" s="1" t="s">
+        <v>2139</v>
+      </c>
+      <c r="FW1" s="1" t="s">
+        <v>2050</v>
+      </c>
+      <c r="FX1" s="1" t="s">
+        <v>2193</v>
+      </c>
+      <c r="FY1" s="1" t="s">
+        <v>2054</v>
+      </c>
+      <c r="FZ1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="GA1" s="1" t="s">
+        <v>2056</v>
+      </c>
+      <c r="GB1" s="1" t="s">
+        <v>2058</v>
+      </c>
+      <c r="GC1" s="1" t="s">
+        <v>2060</v>
+      </c>
+      <c r="GD1" s="1" t="s">
+        <v>2422</v>
+      </c>
+      <c r="GE1" s="1" t="s">
+        <v>2423</v>
+      </c>
+      <c r="GF1" s="1" t="s">
+        <v>2672</v>
+      </c>
+      <c r="GG1" s="1" t="s">
+        <v>2674</v>
+      </c>
+      <c r="GH1" s="1" t="s">
+        <v>1768</v>
+      </c>
+      <c r="GI1" s="1" t="s">
+        <v>2833</v>
+      </c>
+      <c r="GJ1" s="1" t="s">
+        <v>1771</v>
+      </c>
+      <c r="GK1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="GL1" s="1" t="s">
+        <v>2250</v>
+      </c>
+      <c r="GM1" s="1" t="s">
+        <v>1769</v>
+      </c>
+      <c r="GN1" s="1" t="s">
+        <v>1773</v>
+      </c>
+      <c r="GO1" s="1" t="s">
+        <v>1779</v>
+      </c>
+      <c r="GP1" s="1" t="s">
+        <v>2835</v>
+      </c>
+      <c r="GQ1" s="1" t="s">
+        <v>1781</v>
+      </c>
+      <c r="GR1" s="1" t="s">
+        <v>1783</v>
+      </c>
+      <c r="GS1" s="1" t="s">
+        <v>1785</v>
+      </c>
+      <c r="GT1" s="1" t="s">
+        <v>1787</v>
+      </c>
+      <c r="GU1" s="1" t="s">
+        <v>1789</v>
+      </c>
+      <c r="GV1" s="1" t="s">
+        <v>1791</v>
+      </c>
+      <c r="GW1" s="1" t="s">
+        <v>1793</v>
+      </c>
+      <c r="GX1" s="1" t="s">
+        <v>2951</v>
+      </c>
+      <c r="GY1" s="1" t="s">
+        <v>2807</v>
+      </c>
+      <c r="GZ1" s="1" t="s">
+        <v>1752</v>
+      </c>
+      <c r="HA1" s="1" t="s">
+        <v>1751</v>
+      </c>
+      <c r="HB1" s="1" t="s">
+        <v>2809</v>
+      </c>
+      <c r="HC1" s="22" t="s">
+        <v>2102</v>
+      </c>
+      <c r="HD1" s="22" t="s">
+        <v>2103</v>
+      </c>
+      <c r="HE1" s="22" t="s">
+        <v>2104</v>
+      </c>
+      <c r="HF1" s="1" t="s">
+        <v>2105</v>
+      </c>
+      <c r="HG1" s="1" t="s">
+        <v>2106</v>
+      </c>
+      <c r="HH1" s="1" t="s">
+        <v>2107</v>
+      </c>
+      <c r="HI1" s="1" t="s">
+        <v>2108</v>
+      </c>
+      <c r="HJ1" s="1" t="s">
+        <v>2109</v>
+      </c>
+      <c r="HK1" s="22" t="s">
+        <v>2111</v>
+      </c>
+      <c r="HL1" s="22" t="s">
+        <v>2110</v>
+      </c>
+    </row>
+    <row r="2" spans="1:220" x14ac:dyDescent="0.3">
       <c r="A2" t="b">
         <v>1</v>
       </c>
@@ -15282,7 +15837,7 @@
         <v>2920</v>
       </c>
       <c r="BF2" s="16" t="s">
-        <v>2217</v>
+        <v>2219</v>
       </c>
       <c r="BG2" s="10" t="s">
         <v>2816</v>
@@ -15538,11 +16093,212 @@
       <c r="EQ2" s="12" t="s">
         <v>2901</v>
       </c>
-      <c r="EV2" t="s">
-        <v>2936</v>
-      </c>
-    </row>
-    <row r="3" spans="1:152" x14ac:dyDescent="0.3">
+      <c r="EV2" s="10" t="s">
+        <v>2807</v>
+      </c>
+      <c r="EW2" s="10" t="s">
+        <v>2585</v>
+      </c>
+      <c r="EX2" s="10" t="s">
+        <v>2592</v>
+      </c>
+      <c r="EY2" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="EZ2" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="FA2" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="FB2" s="10" t="s">
+        <v>1751</v>
+      </c>
+      <c r="FC2" s="10" t="s">
+        <v>2574</v>
+      </c>
+      <c r="FD2" s="10" t="s">
+        <v>2598</v>
+      </c>
+      <c r="FE2" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="FG2" s="85" t="s">
+        <v>5</v>
+      </c>
+      <c r="FH2" s="85" t="s">
+        <v>5</v>
+      </c>
+      <c r="FI2" s="85" t="s">
+        <v>5</v>
+      </c>
+      <c r="FJ2" s="85" t="s">
+        <v>5</v>
+      </c>
+      <c r="FK2" s="85" t="s">
+        <v>5</v>
+      </c>
+      <c r="FL2" s="85" t="s">
+        <v>5</v>
+      </c>
+      <c r="FM2" s="85" t="s">
+        <v>5</v>
+      </c>
+      <c r="FN2" s="85" t="s">
+        <v>5</v>
+      </c>
+      <c r="FO2" s="85" t="s">
+        <v>5</v>
+      </c>
+      <c r="FP2" s="85" t="s">
+        <v>5</v>
+      </c>
+      <c r="FQ2" s="85" t="s">
+        <v>5</v>
+      </c>
+      <c r="FR2" s="85" t="s">
+        <v>5</v>
+      </c>
+      <c r="FS2" s="85" t="s">
+        <v>5</v>
+      </c>
+      <c r="FT2" s="85" t="s">
+        <v>5</v>
+      </c>
+      <c r="FU2" s="85" t="s">
+        <v>5</v>
+      </c>
+      <c r="FV2" s="85" t="s">
+        <v>5</v>
+      </c>
+      <c r="FW2" s="85" t="s">
+        <v>5</v>
+      </c>
+      <c r="FX2" s="85" t="s">
+        <v>5</v>
+      </c>
+      <c r="FY2" s="85" t="s">
+        <v>5</v>
+      </c>
+      <c r="FZ2" s="85" t="s">
+        <v>5</v>
+      </c>
+      <c r="GA2" s="85" t="s">
+        <v>5</v>
+      </c>
+      <c r="GB2" s="85" t="s">
+        <v>5</v>
+      </c>
+      <c r="GC2" s="85" t="s">
+        <v>5</v>
+      </c>
+      <c r="GD2" s="85" t="s">
+        <v>5</v>
+      </c>
+      <c r="GE2" s="85" t="s">
+        <v>5</v>
+      </c>
+      <c r="GF2" s="85" t="s">
+        <v>5</v>
+      </c>
+      <c r="GG2" s="85" t="s">
+        <v>5</v>
+      </c>
+      <c r="GH2" s="85" t="s">
+        <v>5</v>
+      </c>
+      <c r="GI2" s="85" t="s">
+        <v>5</v>
+      </c>
+      <c r="GJ2" s="85" t="s">
+        <v>5</v>
+      </c>
+      <c r="GK2" s="85" t="s">
+        <v>5</v>
+      </c>
+      <c r="GL2" s="85" t="s">
+        <v>5</v>
+      </c>
+      <c r="GM2" s="85" t="s">
+        <v>5</v>
+      </c>
+      <c r="GN2" s="85" t="s">
+        <v>5</v>
+      </c>
+      <c r="GO2" s="85" t="s">
+        <v>5</v>
+      </c>
+      <c r="GP2" t="s">
+        <v>5</v>
+      </c>
+      <c r="GQ2" s="85" t="s">
+        <v>5</v>
+      </c>
+      <c r="GR2" t="s">
+        <v>5</v>
+      </c>
+      <c r="GS2" s="85" t="s">
+        <v>5</v>
+      </c>
+      <c r="GT2" s="85" t="s">
+        <v>5</v>
+      </c>
+      <c r="GU2" s="85" t="s">
+        <v>5</v>
+      </c>
+      <c r="GV2" s="85" t="s">
+        <v>5</v>
+      </c>
+      <c r="GW2" s="85" t="s">
+        <v>5</v>
+      </c>
+      <c r="GX2" s="85" t="s">
+        <v>5</v>
+      </c>
+      <c r="GY2" t="s">
+        <v>5</v>
+      </c>
+      <c r="GZ2" s="85" t="s">
+        <v>5</v>
+      </c>
+      <c r="HA2" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="HB2" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="HC2" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="HD2" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="HE2" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="HF2" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="HG2" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="HH2" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="HI2" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="HJ2" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="HK2" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="HL2" s="10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:220" x14ac:dyDescent="0.3">
       <c r="A3" t="b">
         <v>0</v>
       </c>
@@ -15715,7 +16471,7 @@
         <v>2921</v>
       </c>
       <c r="BF3" s="16" t="s">
-        <v>2218</v>
+        <v>2220</v>
       </c>
       <c r="BG3" s="10" t="s">
         <v>2807</v>
@@ -15970,8 +16726,140 @@
       <c r="EP3" s="12" t="s">
         <v>2900</v>
       </c>
-    </row>
-    <row r="4" spans="1:152" x14ac:dyDescent="0.3">
+      <c r="EV3" s="10" t="s">
+        <v>2808</v>
+      </c>
+      <c r="EW3" s="10" t="s">
+        <v>2585</v>
+      </c>
+      <c r="EX3" s="10" t="s">
+        <v>2588</v>
+      </c>
+      <c r="EY3" s="10" t="s">
+        <v>2028</v>
+      </c>
+      <c r="EZ3" s="10" t="s">
+        <v>2032</v>
+      </c>
+      <c r="FA3" s="10" t="s">
+        <v>2032</v>
+      </c>
+      <c r="FB3" s="10" t="s">
+        <v>2809</v>
+      </c>
+      <c r="FC3" s="10" t="s">
+        <v>2596</v>
+      </c>
+      <c r="FD3" s="10" t="s">
+        <v>2601</v>
+      </c>
+      <c r="FE3" s="10" t="s">
+        <v>2028</v>
+      </c>
+      <c r="FG3" t="s">
+        <v>2936</v>
+      </c>
+      <c r="FH3" t="s">
+        <v>2967</v>
+      </c>
+      <c r="FI3" t="s">
+        <v>2967</v>
+      </c>
+      <c r="FJ3" s="85" t="s">
+        <v>2967</v>
+      </c>
+      <c r="FK3" t="s">
+        <v>2968</v>
+      </c>
+      <c r="FL3" s="85" t="s">
+        <v>2968</v>
+      </c>
+      <c r="FM3" s="85" t="s">
+        <v>2968</v>
+      </c>
+      <c r="FN3" s="85" t="s">
+        <v>2968</v>
+      </c>
+      <c r="FO3" s="85" t="s">
+        <v>2968</v>
+      </c>
+      <c r="FP3" s="85" t="s">
+        <v>2968</v>
+      </c>
+      <c r="FQ3" s="85" t="s">
+        <v>2968</v>
+      </c>
+      <c r="FR3" s="85" t="s">
+        <v>2968</v>
+      </c>
+      <c r="FS3" s="85" t="s">
+        <v>2968</v>
+      </c>
+      <c r="FT3" s="85" t="s">
+        <v>3003</v>
+      </c>
+      <c r="FV3" t="s">
+        <v>2976</v>
+      </c>
+      <c r="FX3" t="s">
+        <v>2970</v>
+      </c>
+      <c r="FY3" t="s">
+        <v>2998</v>
+      </c>
+      <c r="FZ3" t="s">
+        <v>2980</v>
+      </c>
+      <c r="GD3" t="s">
+        <v>2981</v>
+      </c>
+      <c r="GE3" s="85" t="s">
+        <v>2981</v>
+      </c>
+      <c r="GI3" t="s">
+        <v>2995</v>
+      </c>
+      <c r="GP3" t="s">
+        <v>2983</v>
+      </c>
+      <c r="GQ3" s="85" t="s">
+        <v>2983</v>
+      </c>
+      <c r="GR3" s="85" t="s">
+        <v>2960</v>
+      </c>
+      <c r="GS3" s="85" t="s">
+        <v>2961</v>
+      </c>
+      <c r="GT3" s="85" t="s">
+        <v>2961</v>
+      </c>
+      <c r="GU3" t="s">
+        <v>2982</v>
+      </c>
+      <c r="GV3" t="s">
+        <v>2958</v>
+      </c>
+      <c r="GW3" s="85" t="s">
+        <v>2958</v>
+      </c>
+      <c r="GX3" s="85" t="s">
+        <v>2958</v>
+      </c>
+      <c r="GY3" t="s">
+        <v>2976</v>
+      </c>
+      <c r="GZ3" s="85" t="s">
+        <v>2976</v>
+      </c>
+      <c r="HA3" s="10" t="s">
+        <v>2028</v>
+      </c>
+      <c r="HB3" s="10" t="s">
+        <v>2028</v>
+      </c>
+    </row>
+    <row r="4" spans="1:220" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>29</v>
       </c>
@@ -16138,7 +17026,7 @@
         <v>1646</v>
       </c>
       <c r="BF4" s="16" t="s">
-        <v>2219</v>
+        <v>2221</v>
       </c>
       <c r="BG4" s="10" t="s">
         <v>2808</v>
@@ -16381,8 +17269,128 @@
       <c r="EQ4" t="s">
         <v>2904</v>
       </c>
-    </row>
-    <row r="5" spans="1:152" x14ac:dyDescent="0.3">
+      <c r="EV4" s="10" t="s">
+        <v>1752</v>
+      </c>
+      <c r="EW4" s="10" t="s">
+        <v>2586</v>
+      </c>
+      <c r="EX4" s="10" t="s">
+        <v>2591</v>
+      </c>
+      <c r="EY4" s="10" t="s">
+        <v>2029</v>
+      </c>
+      <c r="EZ4" s="10" t="s">
+        <v>2033</v>
+      </c>
+      <c r="FA4" s="10" t="s">
+        <v>2033</v>
+      </c>
+      <c r="FB4" s="10" t="s">
+        <v>2810</v>
+      </c>
+      <c r="FC4" s="10" t="s">
+        <v>2596</v>
+      </c>
+      <c r="FD4" s="10" t="s">
+        <v>2600</v>
+      </c>
+      <c r="FE4" s="85" t="s">
+        <v>2036</v>
+      </c>
+      <c r="FG4" t="s">
+        <v>3000</v>
+      </c>
+      <c r="FH4" t="s">
+        <v>2996</v>
+      </c>
+      <c r="FI4" s="85" t="s">
+        <v>2996</v>
+      </c>
+      <c r="FK4" t="s">
+        <v>2969</v>
+      </c>
+      <c r="FL4" s="85" t="s">
+        <v>2969</v>
+      </c>
+      <c r="FM4" s="85" t="s">
+        <v>2969</v>
+      </c>
+      <c r="FN4" s="85" t="s">
+        <v>2969</v>
+      </c>
+      <c r="FO4" s="85" t="s">
+        <v>2969</v>
+      </c>
+      <c r="FP4" s="85" t="s">
+        <v>2969</v>
+      </c>
+      <c r="FQ4" s="85" t="s">
+        <v>2969</v>
+      </c>
+      <c r="FR4" s="85" t="s">
+        <v>2969</v>
+      </c>
+      <c r="FS4" s="85" t="s">
+        <v>2969</v>
+      </c>
+      <c r="FT4" t="s">
+        <v>3002</v>
+      </c>
+      <c r="FV4" s="85" t="s">
+        <v>2977</v>
+      </c>
+      <c r="FX4" s="85" t="s">
+        <v>2973</v>
+      </c>
+      <c r="FZ4" t="s">
+        <v>2997</v>
+      </c>
+      <c r="GD4" t="s">
+        <v>2994</v>
+      </c>
+      <c r="GE4" s="85" t="s">
+        <v>2994</v>
+      </c>
+      <c r="GI4" t="s">
+        <v>2936</v>
+      </c>
+      <c r="GP4" t="s">
+        <v>2959</v>
+      </c>
+      <c r="GQ4" s="85" t="s">
+        <v>2959</v>
+      </c>
+      <c r="GS4" s="85" t="s">
+        <v>2962</v>
+      </c>
+      <c r="GT4" s="85" t="s">
+        <v>2965</v>
+      </c>
+      <c r="GV4" s="85" t="s">
+        <v>2984</v>
+      </c>
+      <c r="GW4" s="85" t="s">
+        <v>2985</v>
+      </c>
+      <c r="GX4" s="85" t="s">
+        <v>2984</v>
+      </c>
+      <c r="GY4" t="s">
+        <v>2978</v>
+      </c>
+      <c r="GZ4" s="85" t="s">
+        <v>2978</v>
+      </c>
+      <c r="HA4" s="85" t="s">
+        <v>2036</v>
+      </c>
+      <c r="HB4" s="85" t="s">
+        <v>2036</v>
+      </c>
+    </row>
+    <row r="5" spans="1:220" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>40</v>
       </c>
@@ -16531,7 +17539,7 @@
         <v>1661</v>
       </c>
       <c r="BF5" s="16" t="s">
-        <v>2220</v>
+        <v>2832</v>
       </c>
       <c r="BG5" s="10" t="s">
         <v>1754</v>
@@ -16763,8 +17771,68 @@
       <c r="EL5" t="s">
         <v>2894</v>
       </c>
-    </row>
-    <row r="6" spans="1:152" x14ac:dyDescent="0.3">
+      <c r="EV5" s="10" t="s">
+        <v>1777</v>
+      </c>
+      <c r="EW5" s="10" t="s">
+        <v>2586</v>
+      </c>
+      <c r="EX5" s="10" t="s">
+        <v>2593</v>
+      </c>
+      <c r="EY5" s="10" t="s">
+        <v>2216</v>
+      </c>
+      <c r="EZ5" s="10" t="s">
+        <v>2034</v>
+      </c>
+      <c r="FA5" s="10" t="s">
+        <v>2034</v>
+      </c>
+      <c r="FB5" s="85"/>
+      <c r="FC5" s="85"/>
+      <c r="FD5" s="85"/>
+      <c r="FE5" s="85" t="s">
+        <v>2037</v>
+      </c>
+      <c r="FG5" t="s">
+        <v>2999</v>
+      </c>
+      <c r="FI5" t="s">
+        <v>3008</v>
+      </c>
+      <c r="FT5" s="85" t="s">
+        <v>3004</v>
+      </c>
+      <c r="FV5" s="85" t="s">
+        <v>2978</v>
+      </c>
+      <c r="FX5" s="85" t="s">
+        <v>2971</v>
+      </c>
+      <c r="GS5" s="85" t="s">
+        <v>2963</v>
+      </c>
+      <c r="GT5" s="85" t="s">
+        <v>2966</v>
+      </c>
+      <c r="GX5" t="s">
+        <v>2993</v>
+      </c>
+      <c r="GY5" t="s">
+        <v>2977</v>
+      </c>
+      <c r="GZ5" s="85" t="s">
+        <v>2977</v>
+      </c>
+      <c r="HA5" s="85" t="s">
+        <v>2037</v>
+      </c>
+      <c r="HB5" s="85" t="s">
+        <v>2037</v>
+      </c>
+    </row>
+    <row r="6" spans="1:220" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>52</v>
       </c>
@@ -16906,7 +17974,7 @@
         <v>1653</v>
       </c>
       <c r="BF6" s="16" t="s">
-        <v>2221</v>
+        <v>2222</v>
       </c>
       <c r="BG6" s="10" t="s">
         <v>1756</v>
@@ -17127,8 +18195,56 @@
       <c r="EF6" s="12" t="s">
         <v>2566</v>
       </c>
-    </row>
-    <row r="7" spans="1:152" x14ac:dyDescent="0.3">
+      <c r="EV6" s="85"/>
+      <c r="EW6" s="85"/>
+      <c r="EX6" s="85"/>
+      <c r="EY6" s="10" t="s">
+        <v>2880</v>
+      </c>
+      <c r="EZ6" s="10" t="s">
+        <v>2573</v>
+      </c>
+      <c r="FA6" s="10" t="s">
+        <v>2573</v>
+      </c>
+      <c r="FB6" s="85"/>
+      <c r="FC6" s="85"/>
+      <c r="FD6" s="85"/>
+      <c r="FE6" s="85" t="s">
+        <v>2038</v>
+      </c>
+      <c r="FG6" t="s">
+        <v>2997</v>
+      </c>
+      <c r="FI6" t="s">
+        <v>3009</v>
+      </c>
+      <c r="FT6" s="85" t="s">
+        <v>3005</v>
+      </c>
+      <c r="FV6" t="s">
+        <v>2029</v>
+      </c>
+      <c r="FX6" s="85" t="s">
+        <v>2974</v>
+      </c>
+      <c r="GT6" t="s">
+        <v>2964</v>
+      </c>
+      <c r="GY6" t="s">
+        <v>2986</v>
+      </c>
+      <c r="GZ6" s="85" t="s">
+        <v>2986</v>
+      </c>
+      <c r="HA6" s="85" t="s">
+        <v>2038</v>
+      </c>
+      <c r="HB6" s="85" t="s">
+        <v>2038</v>
+      </c>
+    </row>
+    <row r="7" spans="1:220" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>63</v>
       </c>
@@ -17261,7 +18377,7 @@
         <v>1650</v>
       </c>
       <c r="BF7" s="16" t="s">
-        <v>2832</v>
+        <v>2223</v>
       </c>
       <c r="BG7" s="10" t="s">
         <v>2048</v>
@@ -17467,11 +18583,56 @@
       <c r="EC7" s="12" t="s">
         <v>2524</v>
       </c>
-      <c r="ED7" s="12"/>
-      <c r="EE7" s="46"/>
-      <c r="EF7" s="46"/>
-    </row>
-    <row r="8" spans="1:152" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="ED7" s="20" t="s">
+        <v>2247</v>
+      </c>
+      <c r="EE7" s="20" t="s">
+        <v>2661</v>
+      </c>
+      <c r="EF7" s="20" t="s">
+        <v>2941</v>
+      </c>
+      <c r="EV7" s="85"/>
+      <c r="EW7" s="85"/>
+      <c r="EX7" s="85"/>
+      <c r="EY7" s="10" t="s">
+        <v>2030</v>
+      </c>
+      <c r="EZ7" s="10" t="s">
+        <v>2830</v>
+      </c>
+      <c r="FA7" s="10" t="s">
+        <v>2830</v>
+      </c>
+      <c r="FB7" s="85"/>
+      <c r="FC7" s="85"/>
+      <c r="FD7" s="85"/>
+      <c r="FE7" s="85" t="s">
+        <v>2030</v>
+      </c>
+      <c r="FT7" s="85" t="s">
+        <v>3006</v>
+      </c>
+      <c r="FV7" t="s">
+        <v>2030</v>
+      </c>
+      <c r="FX7" s="85" t="s">
+        <v>2972</v>
+      </c>
+      <c r="GY7" s="85" t="s">
+        <v>2987</v>
+      </c>
+      <c r="GZ7" s="85" t="s">
+        <v>2987</v>
+      </c>
+      <c r="HA7" s="85" t="s">
+        <v>2030</v>
+      </c>
+      <c r="HB7" s="85" t="s">
+        <v>2030</v>
+      </c>
+    </row>
+    <row r="8" spans="1:220" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>75</v>
       </c>
@@ -17587,9 +18748,6 @@
       </c>
       <c r="BC8" s="6" t="s">
         <v>1927</v>
-      </c>
-      <c r="BF8" s="16" t="s">
-        <v>2222</v>
       </c>
       <c r="BG8" s="10" t="s">
         <v>1752</v>
@@ -17776,11 +18934,53 @@
       <c r="EA8" s="12"/>
       <c r="EB8" s="12"/>
       <c r="EC8" s="12"/>
-      <c r="ED8" s="12"/>
-      <c r="EE8" s="46"/>
-      <c r="EF8" s="46"/>
-    </row>
-    <row r="9" spans="1:152" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="ED8" s="20" t="s">
+        <v>2248</v>
+      </c>
+      <c r="EE8" s="20" t="s">
+        <v>2661</v>
+      </c>
+      <c r="EF8" s="20" t="s">
+        <v>2942</v>
+      </c>
+      <c r="EY8" s="10" t="s">
+        <v>2038</v>
+      </c>
+      <c r="EZ8" s="10" t="s">
+        <v>2831</v>
+      </c>
+      <c r="FA8" s="10" t="s">
+        <v>2831</v>
+      </c>
+      <c r="FB8" s="85"/>
+      <c r="FC8" s="85"/>
+      <c r="FD8" s="85"/>
+      <c r="FE8" s="85" t="s">
+        <v>2039</v>
+      </c>
+      <c r="FT8" s="85" t="s">
+        <v>3007</v>
+      </c>
+      <c r="FV8" t="s">
+        <v>2979</v>
+      </c>
+      <c r="FX8" s="85" t="s">
+        <v>2975</v>
+      </c>
+      <c r="GY8" s="85" t="s">
+        <v>2988</v>
+      </c>
+      <c r="GZ8" s="85" t="s">
+        <v>2988</v>
+      </c>
+      <c r="HA8" s="85" t="s">
+        <v>2039</v>
+      </c>
+      <c r="HB8" s="85" t="s">
+        <v>2039</v>
+      </c>
+    </row>
+    <row r="9" spans="1:220" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>86</v>
       </c>
@@ -17885,9 +19085,6 @@
         <v>1928</v>
       </c>
       <c r="BD9" s="17"/>
-      <c r="BF9" s="16" t="s">
-        <v>2223</v>
-      </c>
       <c r="BG9" s="10" t="s">
         <v>1777</v>
       </c>
@@ -18013,7 +19210,7 @@
         <v>2320</v>
       </c>
       <c r="DE9" s="45" t="s">
-        <v>2325</v>
+        <v>2949</v>
       </c>
       <c r="DF9" s="12" t="s">
         <v>1802</v>
@@ -18063,11 +19260,47 @@
       <c r="EA9" s="12"/>
       <c r="EB9" s="12"/>
       <c r="EC9" s="12"/>
-      <c r="ED9" s="12"/>
-      <c r="EE9" s="46"/>
-      <c r="EF9" s="46"/>
-    </row>
-    <row r="10" spans="1:152" x14ac:dyDescent="0.3">
+      <c r="ED9" s="20" t="s">
+        <v>2249</v>
+      </c>
+      <c r="EE9" s="20" t="s">
+        <v>2661</v>
+      </c>
+      <c r="EF9" s="20" t="s">
+        <v>2943</v>
+      </c>
+      <c r="EY9" s="10" t="s">
+        <v>2036</v>
+      </c>
+      <c r="EZ9" s="10" t="s">
+        <v>2940</v>
+      </c>
+      <c r="FA9" s="10" t="s">
+        <v>2939</v>
+      </c>
+      <c r="FB9" s="85"/>
+      <c r="FC9" s="85"/>
+      <c r="FD9" s="85"/>
+      <c r="FE9" s="85" t="s">
+        <v>2029</v>
+      </c>
+      <c r="FT9" t="s">
+        <v>3001</v>
+      </c>
+      <c r="GY9" t="s">
+        <v>2989</v>
+      </c>
+      <c r="GZ9" s="85" t="s">
+        <v>2989</v>
+      </c>
+      <c r="HA9" s="85" t="s">
+        <v>2029</v>
+      </c>
+      <c r="HB9" s="85" t="s">
+        <v>2029</v>
+      </c>
+    </row>
+    <row r="10" spans="1:220" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>95</v>
       </c>
@@ -18325,11 +19558,40 @@
       <c r="EA10" s="12"/>
       <c r="EB10" s="12"/>
       <c r="EC10" s="12"/>
-      <c r="ED10" s="12"/>
-      <c r="EE10" s="46"/>
-      <c r="EF10" s="46"/>
-    </row>
-    <row r="11" spans="1:152" x14ac:dyDescent="0.3">
+      <c r="ED10" s="20" t="s">
+        <v>2906</v>
+      </c>
+      <c r="EE10" s="20" t="s">
+        <v>2661</v>
+      </c>
+      <c r="EF10" s="20" t="s">
+        <v>2944</v>
+      </c>
+      <c r="EY10" s="10" t="s">
+        <v>2031</v>
+      </c>
+      <c r="EZ10" s="85"/>
+      <c r="FA10" s="10"/>
+      <c r="FB10" s="85"/>
+      <c r="FC10" s="85"/>
+      <c r="FD10" s="85"/>
+      <c r="FE10" s="85" t="s">
+        <v>2216</v>
+      </c>
+      <c r="GY10" t="s">
+        <v>2990</v>
+      </c>
+      <c r="GZ10" s="85" t="s">
+        <v>2990</v>
+      </c>
+      <c r="HA10" s="85" t="s">
+        <v>2216</v>
+      </c>
+      <c r="HB10" s="85" t="s">
+        <v>2216</v>
+      </c>
+    </row>
+    <row r="11" spans="1:220" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>104</v>
       </c>
@@ -18581,11 +19843,37 @@
       <c r="EA11" s="12"/>
       <c r="EB11" s="12"/>
       <c r="EC11" s="12"/>
-      <c r="ED11" s="12"/>
-      <c r="EE11" s="46"/>
-      <c r="EF11" s="46"/>
-    </row>
-    <row r="12" spans="1:152" x14ac:dyDescent="0.3">
+      <c r="ED11" s="20" t="s">
+        <v>2908</v>
+      </c>
+      <c r="EE11" s="20" t="s">
+        <v>2661</v>
+      </c>
+      <c r="EF11" s="20" t="s">
+        <v>2945</v>
+      </c>
+      <c r="EY11" s="10" t="s">
+        <v>2259</v>
+      </c>
+      <c r="EZ11" s="10"/>
+      <c r="FA11" s="10"/>
+      <c r="FE11" s="85" t="s">
+        <v>2040</v>
+      </c>
+      <c r="GY11" t="s">
+        <v>2029</v>
+      </c>
+      <c r="GZ11" s="85" t="s">
+        <v>2029</v>
+      </c>
+      <c r="HA11" s="85" t="s">
+        <v>2040</v>
+      </c>
+      <c r="HB11" s="85" t="s">
+        <v>2040</v>
+      </c>
+    </row>
+    <row r="12" spans="1:220" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>113</v>
       </c>
@@ -18821,11 +20109,37 @@
       <c r="EA12" s="12"/>
       <c r="EB12" s="12"/>
       <c r="EC12" s="12"/>
-      <c r="ED12" s="12"/>
-      <c r="EE12" s="46"/>
-      <c r="EF12" s="46"/>
-    </row>
-    <row r="13" spans="1:152" x14ac:dyDescent="0.3">
+      <c r="ED12" s="20" t="s">
+        <v>2910</v>
+      </c>
+      <c r="EE12" s="20" t="s">
+        <v>2661</v>
+      </c>
+      <c r="EF12" s="20" t="s">
+        <v>2946</v>
+      </c>
+      <c r="EY12" s="10" t="s">
+        <v>2879</v>
+      </c>
+      <c r="EZ12" s="10"/>
+      <c r="FA12" s="85"/>
+      <c r="FE12" s="85" t="s">
+        <v>2041</v>
+      </c>
+      <c r="GY12" t="s">
+        <v>2030</v>
+      </c>
+      <c r="GZ12" s="85" t="s">
+        <v>2030</v>
+      </c>
+      <c r="HA12" s="85" t="s">
+        <v>2041</v>
+      </c>
+      <c r="HB12" s="85" t="s">
+        <v>2041</v>
+      </c>
+    </row>
+    <row r="13" spans="1:220" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>122</v>
       </c>
@@ -19041,11 +20355,35 @@
       <c r="DZ13" s="46" t="s">
         <v>2469</v>
       </c>
-      <c r="ED13" s="12"/>
-      <c r="EE13" s="46"/>
-      <c r="EF13" s="46"/>
-    </row>
-    <row r="14" spans="1:152" x14ac:dyDescent="0.3">
+      <c r="ED13" s="20" t="s">
+        <v>2875</v>
+      </c>
+      <c r="EE13" s="20" t="s">
+        <v>2876</v>
+      </c>
+      <c r="EF13" s="20" t="s">
+        <v>2947</v>
+      </c>
+      <c r="EY13" s="10"/>
+      <c r="EZ13" s="10"/>
+      <c r="FA13" s="85"/>
+      <c r="FE13" s="85" t="s">
+        <v>2031</v>
+      </c>
+      <c r="GY13" t="s">
+        <v>2031</v>
+      </c>
+      <c r="GZ13" s="85" t="s">
+        <v>2031</v>
+      </c>
+      <c r="HA13" s="85" t="s">
+        <v>2031</v>
+      </c>
+      <c r="HB13" s="85" t="s">
+        <v>2031</v>
+      </c>
+    </row>
+    <row r="14" spans="1:220" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>130</v>
       </c>
@@ -19248,8 +20586,14 @@
       <c r="ED14" s="12"/>
       <c r="EE14" s="46"/>
       <c r="EF14" s="46"/>
-    </row>
-    <row r="15" spans="1:152" x14ac:dyDescent="0.3">
+      <c r="GY14" t="s">
+        <v>2036</v>
+      </c>
+      <c r="GZ14" s="85" t="s">
+        <v>2036</v>
+      </c>
+    </row>
+    <row r="15" spans="1:220" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
         <v>138</v>
       </c>
@@ -19444,8 +20788,14 @@
       <c r="ED15" s="12"/>
       <c r="EE15" s="46"/>
       <c r="EF15" s="46"/>
-    </row>
-    <row r="16" spans="1:152" x14ac:dyDescent="0.3">
+      <c r="GY15" t="s">
+        <v>2991</v>
+      </c>
+      <c r="GZ15" s="85" t="s">
+        <v>2992</v>
+      </c>
+    </row>
+    <row r="16" spans="1:220" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>145</v>
       </c>
@@ -19635,8 +20985,14 @@
       <c r="ED16" s="12"/>
       <c r="EE16" s="46"/>
       <c r="EF16" s="46"/>
-    </row>
-    <row r="17" spans="2:136" x14ac:dyDescent="0.3">
+      <c r="GY16" s="10" t="s">
+        <v>2259</v>
+      </c>
+      <c r="GZ16" s="10" t="s">
+        <v>2259</v>
+      </c>
+    </row>
+    <row r="17" spans="2:208" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>153</v>
       </c>
@@ -19816,8 +21172,14 @@
       <c r="ED17" s="12"/>
       <c r="EE17" s="46"/>
       <c r="EF17" s="46"/>
-    </row>
-    <row r="18" spans="2:136" x14ac:dyDescent="0.3">
+      <c r="GY17" s="10" t="s">
+        <v>2879</v>
+      </c>
+      <c r="GZ17" s="10" t="s">
+        <v>2879</v>
+      </c>
+    </row>
+    <row r="18" spans="2:208" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>160</v>
       </c>
@@ -19944,6 +21306,15 @@
       <c r="CT18" s="11"/>
       <c r="CU18" s="11"/>
       <c r="CV18" s="11"/>
+      <c r="DC18" s="12" t="s">
+        <v>2951</v>
+      </c>
+      <c r="DD18" s="84" t="s">
+        <v>2320</v>
+      </c>
+      <c r="DE18" s="84" t="s">
+        <v>2948</v>
+      </c>
       <c r="DF18" s="12" t="s">
         <v>1805</v>
       </c>
@@ -19982,7 +21353,7 @@
       <c r="EE18" s="46"/>
       <c r="EF18" s="46"/>
     </row>
-    <row r="19" spans="2:136" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:208" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
         <v>167</v>
       </c>
@@ -20104,6 +21475,15 @@
       <c r="CT19" s="11"/>
       <c r="CU19" s="11"/>
       <c r="CV19" s="11"/>
+      <c r="DC19" s="12" t="s">
+        <v>2952</v>
+      </c>
+      <c r="DD19" s="84" t="s">
+        <v>2320</v>
+      </c>
+      <c r="DE19" s="84" t="s">
+        <v>2950</v>
+      </c>
       <c r="DF19" s="12" t="s">
         <v>1806</v>
       </c>
@@ -20142,7 +21522,7 @@
       <c r="EE19" s="46"/>
       <c r="EF19" s="46"/>
     </row>
-    <row r="20" spans="2:136" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:208" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
         <v>174</v>
       </c>
@@ -20292,7 +21672,7 @@
       <c r="EE20" s="46"/>
       <c r="EF20" s="46"/>
     </row>
-    <row r="21" spans="2:136" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:208" ht="16.8" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
         <v>181</v>
       </c>
@@ -20376,6 +21756,12 @@
       <c r="CI21" s="20" t="s">
         <v>2584</v>
       </c>
+      <c r="CJ21" s="14" t="s">
+        <v>2953</v>
+      </c>
+      <c r="CK21" s="20" t="s">
+        <v>2955</v>
+      </c>
       <c r="CM21" s="14" t="s">
         <v>2927</v>
       </c>
@@ -20410,7 +21796,7 @@
         <v>2335</v>
       </c>
     </row>
-    <row r="22" spans="2:136" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:208" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
         <v>188</v>
       </c>
@@ -20478,6 +21864,12 @@
       <c r="CI22" s="20" t="s">
         <v>2829</v>
       </c>
+      <c r="CJ22" s="14" t="s">
+        <v>2954</v>
+      </c>
+      <c r="CK22" s="20" t="s">
+        <v>2956</v>
+      </c>
       <c r="CM22" s="14" t="s">
         <v>2928</v>
       </c>
@@ -20515,7 +21907,7 @@
         <v>2335</v>
       </c>
     </row>
-    <row r="23" spans="2:136" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:208" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
         <v>195</v>
       </c>
@@ -20613,7 +22005,7 @@
         <v>2442</v>
       </c>
     </row>
-    <row r="24" spans="2:136" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:208" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
         <v>202</v>
       </c>
@@ -20702,7 +22094,7 @@
         <v>2445</v>
       </c>
     </row>
-    <row r="25" spans="2:136" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:208" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
         <v>209</v>
       </c>
@@ -20793,7 +22185,7 @@
         <v>2438</v>
       </c>
     </row>
-    <row r="26" spans="2:136" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:208" ht="16.8" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
         <v>216</v>
       </c>
@@ -20878,7 +22270,7 @@
         <v>2439</v>
       </c>
     </row>
-    <row r="27" spans="2:136" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:208" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
         <v>222</v>
       </c>
@@ -20900,7 +22292,7 @@
       <c r="L27" t="s">
         <v>228</v>
       </c>
-      <c r="M27" s="111"/>
+      <c r="M27" s="113"/>
       <c r="O27" s="12" t="s">
         <v>822</v>
       </c>
@@ -20959,7 +22351,7 @@
         <v>2440</v>
       </c>
     </row>
-    <row r="28" spans="2:136" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:208" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
         <v>229</v>
       </c>
@@ -20981,7 +22373,7 @@
       <c r="L28" t="s">
         <v>235</v>
       </c>
-      <c r="M28" s="111"/>
+      <c r="M28" s="113"/>
       <c r="O28" s="12" t="s">
         <v>1712</v>
       </c>
@@ -21040,7 +22432,7 @@
         <v>2441</v>
       </c>
     </row>
-    <row r="29" spans="2:136" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:208" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
         <v>236</v>
       </c>
@@ -21116,7 +22508,7 @@
         <v>2436</v>
       </c>
     </row>
-    <row r="30" spans="2:136" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:208" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
         <v>243</v>
       </c>
@@ -21176,7 +22568,7 @@
         <v>2437</v>
       </c>
     </row>
-    <row r="31" spans="2:136" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:208" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
         <v>249</v>
       </c>
@@ -21237,7 +22629,7 @@
         <v>2537</v>
       </c>
     </row>
-    <row r="32" spans="2:136" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:208" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="B32" t="s">
         <v>256</v>
       </c>
@@ -21381,7 +22773,7 @@
       <c r="L34" t="s">
         <v>276</v>
       </c>
-      <c r="M34" s="111"/>
+      <c r="M34" s="113"/>
       <c r="O34" s="12" t="s">
         <v>915</v>
       </c>
@@ -21440,7 +22832,7 @@
       <c r="L35" t="s">
         <v>283</v>
       </c>
-      <c r="M35" s="111"/>
+      <c r="M35" s="113"/>
       <c r="O35" s="12" t="s">
         <v>939</v>
       </c>
@@ -26906,7 +28298,6 @@
       <c r="DL277" s="45"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="yKpNSaC0wkEyc2CwDSZTJrTqfmhfVYnBVszaCq7RKlAW3n4OH9PSWhdZXf3f2SBg8JPrylJX9lBW95YjjAExFw==" saltValue="+13U7S2ORaK8CrNff9rjOQ==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="2">
     <mergeCell ref="M27:M28"/>
     <mergeCell ref="M34:M35"/>

</xml_diff>

<commit_message>
Protected the variable sheet
</commit_message>
<xml_diff>
--- a/Excel_templates/MOSAIC_input_excel_file_2022.xlsx
+++ b/Excel_templates/MOSAIC_input_excel_file_2022.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sparadis\Documents\ETH\MOSAIC\MOSAIC_Client\Excel_templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1D07607-1295-4678-9895-0109438E3F6B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C7E2560-73D6-490D-B366-40919960394E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30204" yWindow="10044" windowWidth="40020" windowHeight="22296" tabRatio="694" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30204" yWindow="10044" windowWidth="40020" windowHeight="22296" tabRatio="694" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ARTICLE_AUTHOR" sheetId="3" r:id="rId1"/>
@@ -9819,6 +9819,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="19" fillId="4" borderId="4" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
@@ -9905,8 +9907,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="16">
     <cellStyle name="20% - Accent1" xfId="3" builtinId="30" customBuiltin="1"/>
@@ -10250,7 +10250,7 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -10271,15 +10271,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="64" customFormat="1" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="86" t="s">
+      <c r="A1" s="88" t="s">
         <v>2676</v>
       </c>
-      <c r="B1" s="86"/>
-      <c r="C1" s="86"/>
-      <c r="D1" s="86"/>
-      <c r="E1" s="86"/>
-      <c r="F1" s="86"/>
-      <c r="G1" s="86"/>
+      <c r="B1" s="88"/>
+      <c r="C1" s="88"/>
+      <c r="D1" s="88"/>
+      <c r="E1" s="88"/>
+      <c r="F1" s="88"/>
+      <c r="G1" s="88"/>
     </row>
     <row r="2" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="53" t="s">
@@ -10368,25 +10368,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="63" customFormat="1" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="87" t="s">
+      <c r="A1" s="89" t="s">
         <v>2677</v>
       </c>
-      <c r="B1" s="87"/>
-      <c r="C1" s="87"/>
-      <c r="D1" s="87"/>
-      <c r="E1" s="88" t="s">
+      <c r="B1" s="89"/>
+      <c r="C1" s="89"/>
+      <c r="D1" s="89"/>
+      <c r="E1" s="90" t="s">
         <v>2817</v>
       </c>
-      <c r="F1" s="88"/>
-      <c r="G1" s="88"/>
-      <c r="H1" s="88"/>
-      <c r="I1" s="88"/>
-      <c r="J1" s="88"/>
-      <c r="K1" s="88"/>
-      <c r="L1" s="88"/>
-      <c r="M1" s="88"/>
-      <c r="N1" s="88"/>
-      <c r="O1" s="88"/>
+      <c r="F1" s="90"/>
+      <c r="G1" s="90"/>
+      <c r="H1" s="90"/>
+      <c r="I1" s="90"/>
+      <c r="J1" s="90"/>
+      <c r="K1" s="90"/>
+      <c r="L1" s="90"/>
+      <c r="M1" s="90"/>
+      <c r="N1" s="90"/>
+      <c r="O1" s="90"/>
     </row>
     <row r="2" spans="1:15" s="66" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="62" t="s">
@@ -10701,37 +10701,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:35" s="55" customFormat="1" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="89" t="s">
+      <c r="A1" s="91" t="s">
         <v>2679</v>
       </c>
-      <c r="B1" s="89"/>
-      <c r="C1" s="89" t="s">
+      <c r="B1" s="91"/>
+      <c r="C1" s="91" t="s">
         <v>2678</v>
       </c>
-      <c r="D1" s="89"/>
-      <c r="E1" s="89"/>
-      <c r="F1" s="89"/>
+      <c r="D1" s="91"/>
+      <c r="E1" s="91"/>
+      <c r="F1" s="91"/>
       <c r="G1" s="55" t="s">
         <v>2832</v>
       </c>
     </row>
     <row r="2" spans="1:35" ht="15.6" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="90" t="s">
+      <c r="A2" s="92" t="s">
         <v>2567</v>
       </c>
-      <c r="B2" s="90" t="s">
+      <c r="B2" s="92" t="s">
         <v>1825</v>
       </c>
-      <c r="C2" s="90" t="s">
+      <c r="C2" s="92" t="s">
         <v>1834</v>
       </c>
-      <c r="D2" s="90" t="s">
+      <c r="D2" s="92" t="s">
         <v>2686</v>
       </c>
-      <c r="E2" s="90" t="s">
+      <c r="E2" s="92" t="s">
         <v>1823</v>
       </c>
-      <c r="F2" s="93" t="s">
+      <c r="F2" s="95" t="s">
         <v>1824</v>
       </c>
       <c r="G2" s="56" t="s">
@@ -10767,12 +10767,12 @@
       <c r="AI2" s="56"/>
     </row>
     <row r="3" spans="1:35" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="91"/>
-      <c r="B3" s="91"/>
-      <c r="C3" s="91"/>
-      <c r="D3" s="91"/>
-      <c r="E3" s="91"/>
-      <c r="F3" s="94"/>
+      <c r="A3" s="93"/>
+      <c r="B3" s="93"/>
+      <c r="C3" s="93"/>
+      <c r="D3" s="93"/>
+      <c r="E3" s="93"/>
+      <c r="F3" s="96"/>
       <c r="G3" s="56"/>
       <c r="H3" s="56"/>
       <c r="I3" s="56"/>
@@ -10804,12 +10804,12 @@
       <c r="AI3" s="56"/>
     </row>
     <row r="4" spans="1:35" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="92"/>
-      <c r="B4" s="92"/>
-      <c r="C4" s="92"/>
-      <c r="D4" s="92"/>
-      <c r="E4" s="92"/>
-      <c r="F4" s="94"/>
+      <c r="A4" s="94"/>
+      <c r="B4" s="94"/>
+      <c r="C4" s="94"/>
+      <c r="D4" s="94"/>
+      <c r="E4" s="94"/>
+      <c r="F4" s="96"/>
       <c r="G4" s="56"/>
       <c r="H4" s="56"/>
       <c r="I4" s="56"/>
@@ -10841,12 +10841,12 @@
       <c r="AI4" s="56"/>
     </row>
     <row r="5" spans="1:35" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="92"/>
-      <c r="B5" s="92"/>
-      <c r="C5" s="92"/>
-      <c r="D5" s="92"/>
-      <c r="E5" s="92"/>
-      <c r="F5" s="94"/>
+      <c r="A5" s="94"/>
+      <c r="B5" s="94"/>
+      <c r="C5" s="94"/>
+      <c r="D5" s="94"/>
+      <c r="E5" s="94"/>
+      <c r="F5" s="96"/>
       <c r="G5" s="56"/>
       <c r="H5" s="56"/>
       <c r="I5" s="56"/>
@@ -12163,23 +12163,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:80" s="79" customFormat="1" ht="20.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="95" t="s">
+      <c r="A1" s="97" t="s">
         <v>2688</v>
       </c>
-      <c r="B1" s="96"/>
-      <c r="C1" s="97"/>
-      <c r="D1" s="95" t="s">
+      <c r="B1" s="98"/>
+      <c r="C1" s="99"/>
+      <c r="D1" s="97" t="s">
         <v>2678</v>
       </c>
-      <c r="E1" s="96"/>
-      <c r="F1" s="96"/>
-      <c r="G1" s="97"/>
-      <c r="H1" s="98" t="s">
+      <c r="E1" s="98"/>
+      <c r="F1" s="98"/>
+      <c r="G1" s="99"/>
+      <c r="H1" s="100" t="s">
         <v>2680</v>
       </c>
-      <c r="I1" s="99"/>
-      <c r="J1" s="99"/>
-      <c r="K1" s="100"/>
+      <c r="I1" s="101"/>
+      <c r="J1" s="101"/>
+      <c r="K1" s="102"/>
       <c r="L1" s="79" t="s">
         <v>1840</v>
       </c>
@@ -12197,37 +12197,37 @@
       </c>
     </row>
     <row r="2" spans="1:80" s="81" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="101" t="s">
+      <c r="A2" s="103" t="s">
         <v>2567</v>
       </c>
-      <c r="B2" s="104" t="s">
+      <c r="B2" s="106" t="s">
         <v>1825</v>
       </c>
-      <c r="C2" s="107" t="s">
+      <c r="C2" s="109" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="102" t="s">
+      <c r="D2" s="104" t="s">
         <v>1834</v>
       </c>
-      <c r="E2" s="105" t="s">
+      <c r="E2" s="107" t="s">
         <v>2686</v>
       </c>
-      <c r="F2" s="105" t="s">
+      <c r="F2" s="107" t="s">
         <v>1823</v>
       </c>
-      <c r="G2" s="108" t="s">
+      <c r="G2" s="110" t="s">
         <v>1824</v>
       </c>
-      <c r="H2" s="101" t="s">
+      <c r="H2" s="103" t="s">
         <v>1835</v>
       </c>
-      <c r="I2" s="104" t="s">
+      <c r="I2" s="106" t="s">
         <v>1836</v>
       </c>
-      <c r="J2" s="104" t="s">
+      <c r="J2" s="106" t="s">
         <v>1837</v>
       </c>
-      <c r="K2" s="110" t="s">
+      <c r="K2" s="112" t="s">
         <v>1838</v>
       </c>
       <c r="L2" s="80" t="s">
@@ -12311,17 +12311,17 @@
       <c r="CB2" s="80"/>
     </row>
     <row r="3" spans="1:80" s="81" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="102"/>
-      <c r="B3" s="105"/>
-      <c r="C3" s="108"/>
-      <c r="D3" s="102"/>
-      <c r="E3" s="105"/>
-      <c r="F3" s="105"/>
-      <c r="G3" s="108"/>
-      <c r="H3" s="102"/>
-      <c r="I3" s="105"/>
-      <c r="J3" s="105"/>
-      <c r="K3" s="111"/>
+      <c r="A3" s="104"/>
+      <c r="B3" s="107"/>
+      <c r="C3" s="110"/>
+      <c r="D3" s="104"/>
+      <c r="E3" s="107"/>
+      <c r="F3" s="107"/>
+      <c r="G3" s="110"/>
+      <c r="H3" s="104"/>
+      <c r="I3" s="107"/>
+      <c r="J3" s="107"/>
+      <c r="K3" s="113"/>
       <c r="L3" s="80" t="s">
         <v>2936</v>
       </c>
@@ -12395,17 +12395,17 @@
       <c r="CB3" s="80"/>
     </row>
     <row r="4" spans="1:80" s="81" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="102"/>
-      <c r="B4" s="105"/>
-      <c r="C4" s="108"/>
-      <c r="D4" s="102"/>
-      <c r="E4" s="105"/>
-      <c r="F4" s="105"/>
-      <c r="G4" s="108"/>
-      <c r="H4" s="102"/>
-      <c r="I4" s="105"/>
-      <c r="J4" s="105"/>
-      <c r="K4" s="111"/>
+      <c r="A4" s="104"/>
+      <c r="B4" s="107"/>
+      <c r="C4" s="110"/>
+      <c r="D4" s="104"/>
+      <c r="E4" s="107"/>
+      <c r="F4" s="107"/>
+      <c r="G4" s="110"/>
+      <c r="H4" s="104"/>
+      <c r="I4" s="107"/>
+      <c r="J4" s="107"/>
+      <c r="K4" s="113"/>
       <c r="L4" s="80"/>
       <c r="M4" s="80"/>
       <c r="N4" s="80"/>
@@ -12477,17 +12477,17 @@
       <c r="CB4" s="80"/>
     </row>
     <row r="5" spans="1:80" s="81" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="102"/>
-      <c r="B5" s="105"/>
-      <c r="C5" s="108"/>
-      <c r="D5" s="102"/>
-      <c r="E5" s="105"/>
-      <c r="F5" s="105"/>
-      <c r="G5" s="108"/>
-      <c r="H5" s="102"/>
-      <c r="I5" s="105"/>
-      <c r="J5" s="105"/>
-      <c r="K5" s="111"/>
+      <c r="A5" s="104"/>
+      <c r="B5" s="107"/>
+      <c r="C5" s="110"/>
+      <c r="D5" s="104"/>
+      <c r="E5" s="107"/>
+      <c r="F5" s="107"/>
+      <c r="G5" s="110"/>
+      <c r="H5" s="104"/>
+      <c r="I5" s="107"/>
+      <c r="J5" s="107"/>
+      <c r="K5" s="113"/>
       <c r="L5" s="80"/>
       <c r="M5" s="80"/>
       <c r="N5" s="80"/>
@@ -12559,17 +12559,17 @@
       <c r="CB5" s="80"/>
     </row>
     <row r="6" spans="1:80" s="81" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="103"/>
-      <c r="B6" s="106"/>
-      <c r="C6" s="109"/>
-      <c r="D6" s="103"/>
-      <c r="E6" s="106"/>
-      <c r="F6" s="106"/>
-      <c r="G6" s="109"/>
-      <c r="H6" s="103"/>
-      <c r="I6" s="106"/>
-      <c r="J6" s="106"/>
-      <c r="K6" s="112"/>
+      <c r="A6" s="105"/>
+      <c r="B6" s="108"/>
+      <c r="C6" s="111"/>
+      <c r="D6" s="105"/>
+      <c r="E6" s="108"/>
+      <c r="F6" s="108"/>
+      <c r="G6" s="111"/>
+      <c r="H6" s="105"/>
+      <c r="I6" s="108"/>
+      <c r="J6" s="108"/>
+      <c r="K6" s="114"/>
       <c r="L6" s="80"/>
       <c r="M6" s="80"/>
       <c r="N6" s="80"/>
@@ -14791,7 +14791,7 @@
     <mergeCell ref="D2:D6"/>
     <mergeCell ref="E2:E6"/>
   </mergeCells>
-  <dataValidations xWindow="389" yWindow="346" count="14">
+  <dataValidations xWindow="389" yWindow="346" count="13">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Write the core_name or select from the drop-down menu the cores you have in the Workbook._x000a_Make sure that the core name matches with its metadata given in GEOPOINTS_CORES sheet" sqref="B2:B4" xr:uid="{6685FF74-A7F2-42C2-901B-99DBBBFECDB4}"/>
     <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Sample analysis category" prompt="Choose from the drop-down list the analysis category the variable belongs to" sqref="L1:CB1" xr:uid="{2372D2F3-EE0C-4296-AC86-BA3569CC20EF}">
       <formula1>Sample_analyses_types</formula1>
@@ -14816,13 +14816,10 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Material analyzed" prompt="Choose from the drop-down menu the material analyzed (i.e. bulk, OC, sand, etc.). If left blank, the default material analyzed (bulk) will be used. If there's a material_analyzed that is missing, please let us know sending an email to mosaic@erdw.eth.ch." sqref="L5:CB5" xr:uid="{B3206B9A-BD85-4C2B-B436-B08F0FC71300}">
       <formula1>material_analyzed</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Method" prompt="Choose from the drop-down menu the method used to analyze the variable. If unknown, choose _unknown. If the method used is not in the drop-down list, please contact mosaic@erdw.ethz.ch" sqref="L3 O3:CB3" xr:uid="{AE24206A-75B4-4703-8A70-F441CD150FA7}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Method" prompt="Choose from the drop-down menu the method used to analyze the variable. If unknown, choose _unknown. If the method used is not in the drop-down list, please contact mosaic@erdw.ethz.ch" sqref="O3:CB3 L3:M3" xr:uid="{AE24206A-75B4-4703-8A70-F441CD150FA7}">
       <formula1>INDIRECT(SUBSTITUTE(SUBSTITUTE(L2,":",""),"%",""))</formula1>
     </dataValidation>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Method details" prompt="If known, add any additional information about the method used to obtain the variable, such as the model of the analyzer." sqref="L4:CB4" xr:uid="{A2878DFE-8081-4751-8EA1-1B0E764D61E4}"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Method" prompt="Choose from the drop-down menu the method used to analyze the variable. If unknown, choose _unknown. If the method used is not in the drop-down list, please contact mosaic@erdw.ethz.ch" sqref="M3" xr:uid="{F1209CA9-F3B6-443C-9AF8-06621DB14272}">
-      <formula1>INDIRECT(SUBSTITUTE(SUBSTITUTE(M2,":",""),"%",""))</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Method" prompt="Choose from the drop-down menu the method used to analyze the variable. If unknown, choose _unknown. If the method used is not in the drop-down list, please contact mosaic@erdw.ethz.ch" sqref="N3" xr:uid="{FC1DB26B-EA6D-4B32-BCFB-3680E3C8BBD5}">
       <formula1>INDIRECT(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(N2,"-",""),":",""),"%",""))</formula1>
     </dataValidation>
@@ -14879,7 +14876,7 @@
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:HL277"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="FF1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView topLeftCell="FF1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="FJ9" sqref="FJ9"/>
     </sheetView>
   </sheetViews>
@@ -14936,7 +14933,7 @@
     <col min="134" max="134" width="18.3984375" bestFit="1" customWidth="1"/>
     <col min="135" max="135" width="28" bestFit="1" customWidth="1"/>
     <col min="136" max="136" width="29.3984375" bestFit="1" customWidth="1"/>
-    <col min="162" max="162" width="11.19921875" style="115"/>
+    <col min="162" max="162" width="11.19921875" style="87"/>
     <col min="163" max="163" width="21.59765625" bestFit="1" customWidth="1"/>
     <col min="180" max="180" width="13.09765625" bestFit="1" customWidth="1"/>
     <col min="198" max="198" width="17.8984375" bestFit="1" customWidth="1"/>
@@ -15486,7 +15483,7 @@
       <c r="FE1" s="1" t="s">
         <v>1753</v>
       </c>
-      <c r="FF1" s="114" t="s">
+      <c r="FF1" s="86" t="s">
         <v>2957</v>
       </c>
       <c r="FG1" s="1" t="s">
@@ -22292,7 +22289,7 @@
       <c r="L27" t="s">
         <v>228</v>
       </c>
-      <c r="M27" s="113"/>
+      <c r="M27" s="115"/>
       <c r="O27" s="12" t="s">
         <v>822</v>
       </c>
@@ -22373,7 +22370,7 @@
       <c r="L28" t="s">
         <v>235</v>
       </c>
-      <c r="M28" s="113"/>
+      <c r="M28" s="115"/>
       <c r="O28" s="12" t="s">
         <v>1712</v>
       </c>
@@ -22773,7 +22770,7 @@
       <c r="L34" t="s">
         <v>276</v>
       </c>
-      <c r="M34" s="113"/>
+      <c r="M34" s="115"/>
       <c r="O34" s="12" t="s">
         <v>915</v>
       </c>
@@ -22832,7 +22829,7 @@
       <c r="L35" t="s">
         <v>283</v>
       </c>
-      <c r="M35" s="113"/>
+      <c r="M35" s="115"/>
       <c r="O35" s="12" t="s">
         <v>939</v>
       </c>
@@ -28298,6 +28295,7 @@
       <c r="DL277" s="45"/>
     </row>
   </sheetData>
+  <sheetProtection algorithmName="SHA-512" hashValue="Mcatd7Y5thVOYBjly4I5csENk+KJJ2h23IKiVWx9zUm8AA9cQPhjvl1XPQV9gtAqi8w7LMzbopaSaizwttdFRg==" saltValue="93CylD+J8lrbmWSNxRaETA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="2">
     <mergeCell ref="M27:M28"/>
     <mergeCell ref="M34:M35"/>

</xml_diff>

<commit_message>
Eliminated CN_method from variables
</commit_message>
<xml_diff>
--- a/Excel_templates/MOSAIC_input_excel_file_2022.xlsx
+++ b/Excel_templates/MOSAIC_input_excel_file_2022.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sparadis\Documents\ETH\MOSAIC\MOSAIC_Client\Excel_templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C7E2560-73D6-490D-B366-40919960394E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A71EA522-D7C7-4A77-9233-03EF35C924A4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="30204" yWindow="10044" windowWidth="40020" windowHeight="22296" tabRatio="694" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -186,7 +186,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3924" uniqueCount="3010">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3922" uniqueCount="3008">
   <si>
     <t>sample_name</t>
   </si>
@@ -7800,12 +7800,6 @@
   </si>
   <si>
     <t>odd over even predominance (different calculations?)</t>
-  </si>
-  <si>
-    <t>CN_method</t>
-  </si>
-  <si>
-    <t>Description of the method of analysis of elemental data (OC, TN, etc.)</t>
   </si>
   <si>
     <t>Delta notation of 15N</t>
@@ -10272,7 +10266,7 @@
   <sheetData>
     <row r="1" spans="1:8" s="64" customFormat="1" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A1" s="88" t="s">
-        <v>2676</v>
+        <v>2674</v>
       </c>
       <c r="B1" s="88"/>
       <c r="C1" s="88"/>
@@ -10283,10 +10277,10 @@
     </row>
     <row r="2" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="53" t="s">
-        <v>2567</v>
+        <v>2565</v>
       </c>
       <c r="B2" s="53" t="s">
-        <v>2686</v>
+        <v>2684</v>
       </c>
       <c r="C2" s="31" t="s">
         <v>1821</v>
@@ -10295,7 +10289,7 @@
         <v>1822</v>
       </c>
       <c r="E2" s="53" t="s">
-        <v>2687</v>
+        <v>2685</v>
       </c>
       <c r="F2" s="53" t="s">
         <v>1823</v>
@@ -10304,7 +10298,7 @@
         <v>1824</v>
       </c>
       <c r="H2" s="72" t="s">
-        <v>2847</v>
+        <v>2845</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
@@ -10369,13 +10363,13 @@
   <sheetData>
     <row r="1" spans="1:15" s="63" customFormat="1" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A1" s="89" t="s">
-        <v>2677</v>
+        <v>2675</v>
       </c>
       <c r="B1" s="89"/>
       <c r="C1" s="89"/>
       <c r="D1" s="89"/>
       <c r="E1" s="90" t="s">
-        <v>2817</v>
+        <v>2815</v>
       </c>
       <c r="F1" s="90"/>
       <c r="G1" s="90"/>
@@ -10390,7 +10384,7 @@
     </row>
     <row r="2" spans="1:15" s="66" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="62" t="s">
-        <v>2567</v>
+        <v>2565</v>
       </c>
       <c r="B2" s="62" t="s">
         <v>1825</v>
@@ -10702,22 +10696,22 @@
   <sheetData>
     <row r="1" spans="1:35" s="55" customFormat="1" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A1" s="91" t="s">
-        <v>2679</v>
+        <v>2677</v>
       </c>
       <c r="B1" s="91"/>
       <c r="C1" s="91" t="s">
-        <v>2678</v>
+        <v>2676</v>
       </c>
       <c r="D1" s="91"/>
       <c r="E1" s="91"/>
       <c r="F1" s="91"/>
       <c r="G1" s="55" t="s">
-        <v>2832</v>
+        <v>2830</v>
       </c>
     </row>
     <row r="2" spans="1:35" ht="15.6" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A2" s="92" t="s">
-        <v>2567</v>
+        <v>2565</v>
       </c>
       <c r="B2" s="92" t="s">
         <v>1825</v>
@@ -10726,7 +10720,7 @@
         <v>1834</v>
       </c>
       <c r="D2" s="92" t="s">
-        <v>2686</v>
+        <v>2684</v>
       </c>
       <c r="E2" s="92" t="s">
         <v>1823</v>
@@ -12164,18 +12158,18 @@
   <sheetData>
     <row r="1" spans="1:80" s="79" customFormat="1" ht="20.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A1" s="97" t="s">
-        <v>2688</v>
+        <v>2686</v>
       </c>
       <c r="B1" s="98"/>
       <c r="C1" s="99"/>
       <c r="D1" s="97" t="s">
-        <v>2678</v>
+        <v>2676</v>
       </c>
       <c r="E1" s="98"/>
       <c r="F1" s="98"/>
       <c r="G1" s="99"/>
       <c r="H1" s="100" t="s">
-        <v>2680</v>
+        <v>2678</v>
       </c>
       <c r="I1" s="101"/>
       <c r="J1" s="101"/>
@@ -12190,15 +12184,15 @@
         <v>1841</v>
       </c>
       <c r="O1" s="79" t="s">
-        <v>2898</v>
+        <v>2896</v>
       </c>
       <c r="P1" s="79" t="s">
-        <v>2953</v>
+        <v>2951</v>
       </c>
     </row>
     <row r="2" spans="1:80" s="81" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="103" t="s">
-        <v>2567</v>
+        <v>2565</v>
       </c>
       <c r="B2" s="106" t="s">
         <v>1825</v>
@@ -12210,7 +12204,7 @@
         <v>1834</v>
       </c>
       <c r="E2" s="107" t="s">
-        <v>2686</v>
+        <v>2684</v>
       </c>
       <c r="F2" s="107" t="s">
         <v>1823</v>
@@ -12240,10 +12234,10 @@
         <v>1843</v>
       </c>
       <c r="O2" s="80" t="s">
-        <v>2900</v>
+        <v>2898</v>
       </c>
       <c r="P2" s="80" t="s">
-        <v>2807</v>
+        <v>2805</v>
       </c>
       <c r="Q2" s="80"/>
       <c r="R2" s="80"/>
@@ -12323,7 +12317,7 @@
       <c r="J3" s="107"/>
       <c r="K3" s="113"/>
       <c r="L3" s="80" t="s">
-        <v>2936</v>
+        <v>2934</v>
       </c>
       <c r="M3" s="80"/>
       <c r="N3" s="80"/>
@@ -14876,8 +14870,8 @@
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:HL277"/>
   <sheetViews>
-    <sheetView topLeftCell="FF1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="FJ9" sqref="FJ9"/>
+    <sheetView topLeftCell="CP1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="CQ24" sqref="CQ24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -15109,7 +15103,7 @@
         <v>1143</v>
       </c>
       <c r="BE1" s="1" t="s">
-        <v>2919</v>
+        <v>2917</v>
       </c>
       <c r="BF1" s="15" t="s">
         <v>1851</v>
@@ -15196,7 +15190,7 @@
         <v>core_burial_rates_description</v>
       </c>
       <c r="CD1" s="24" t="s">
-        <v>2832</v>
+        <v>2830</v>
       </c>
       <c r="CE1" s="9" t="str">
         <f>_xlfn.CONCAT(CD1,"_units")</f>
@@ -15252,7 +15246,7 @@
         <v>sample_composition_description</v>
       </c>
       <c r="CT1" s="9" t="s">
-        <v>2811</v>
+        <v>2809</v>
       </c>
       <c r="CU1" s="9" t="str">
         <f>_xlfn.CONCAT(CT1,"_units")</f>
@@ -15395,7 +15389,7 @@
         <v>sample_pore_water_description</v>
       </c>
       <c r="EG1" s="9" t="s">
-        <v>2689</v>
+        <v>2687</v>
       </c>
       <c r="EH1" s="9" t="str">
         <f>_xlfn.CONCAT(EG1,"_units")</f>
@@ -15406,7 +15400,7 @@
         <v>sample_black_carbon_description</v>
       </c>
       <c r="EJ1" s="9" t="s">
-        <v>2882</v>
+        <v>2880</v>
       </c>
       <c r="EK1" s="9" t="str">
         <f>_xlfn.CONCAT(EJ1,"_units")</f>
@@ -15417,7 +15411,7 @@
         <v>sample_mineralogy_description</v>
       </c>
       <c r="EM1" s="9" t="s">
-        <v>2885</v>
+        <v>2883</v>
       </c>
       <c r="EN1" s="9" t="str">
         <f>_xlfn.CONCAT(EM1,"_units")</f>
@@ -15428,7 +15422,7 @@
         <v>sample_dating_description</v>
       </c>
       <c r="EP1" s="9" t="s">
-        <v>2898</v>
+        <v>2896</v>
       </c>
       <c r="EQ1" s="9" t="str">
         <f>_xlfn.CONCAT(EP1,"_units")</f>
@@ -15439,7 +15433,7 @@
         <v>sample_neodynium_description</v>
       </c>
       <c r="ES1" s="9" t="s">
-        <v>2903</v>
+        <v>2901</v>
       </c>
       <c r="ET1" s="9" t="str">
         <f>_xlfn.CONCAT(ES1,"_units")</f>
@@ -15450,7 +15444,7 @@
         <v>sample_strontium_description</v>
       </c>
       <c r="EV1" s="1" t="s">
-        <v>2953</v>
+        <v>2951</v>
       </c>
       <c r="EW1" s="9" t="str">
         <f>_xlfn.CONCAT(EV1,"_units")</f>
@@ -15470,7 +15464,7 @@
         <v>1756</v>
       </c>
       <c r="FB1" s="1" t="s">
-        <v>2954</v>
+        <v>2952</v>
       </c>
       <c r="FC1" s="9" t="str">
         <f>_xlfn.CONCAT(FB1,"_units")</f>
@@ -15484,7 +15478,7 @@
         <v>1753</v>
       </c>
       <c r="FF1" s="86" t="s">
-        <v>2957</v>
+        <v>2955</v>
       </c>
       <c r="FG1" s="1" t="s">
         <v>2052</v>
@@ -15508,10 +15502,10 @@
         <v>1847</v>
       </c>
       <c r="FN1" s="1" t="s">
-        <v>2914</v>
+        <v>2912</v>
       </c>
       <c r="FO1" s="1" t="s">
-        <v>2915</v>
+        <v>2913</v>
       </c>
       <c r="FP1" s="1" t="s">
         <v>1848</v>
@@ -15520,10 +15514,10 @@
         <v>1849</v>
       </c>
       <c r="FR1" s="1" t="s">
-        <v>2852</v>
+        <v>2850</v>
       </c>
       <c r="FS1" s="1" t="s">
-        <v>2917</v>
+        <v>2915</v>
       </c>
       <c r="FT1" s="1" t="s">
         <v>2062</v>
@@ -15562,16 +15556,16 @@
         <v>2423</v>
       </c>
       <c r="GF1" s="1" t="s">
+        <v>2670</v>
+      </c>
+      <c r="GG1" s="1" t="s">
         <v>2672</v>
-      </c>
-      <c r="GG1" s="1" t="s">
-        <v>2674</v>
       </c>
       <c r="GH1" s="1" t="s">
         <v>1768</v>
       </c>
       <c r="GI1" s="1" t="s">
-        <v>2833</v>
+        <v>2831</v>
       </c>
       <c r="GJ1" s="1" t="s">
         <v>1771</v>
@@ -15592,7 +15586,7 @@
         <v>1779</v>
       </c>
       <c r="GP1" s="1" t="s">
-        <v>2835</v>
+        <v>2833</v>
       </c>
       <c r="GQ1" s="1" t="s">
         <v>1781</v>
@@ -15616,10 +15610,10 @@
         <v>1793</v>
       </c>
       <c r="GX1" s="1" t="s">
-        <v>2951</v>
+        <v>2949</v>
       </c>
       <c r="GY1" s="1" t="s">
-        <v>2807</v>
+        <v>2805</v>
       </c>
       <c r="GZ1" s="1" t="s">
         <v>1752</v>
@@ -15628,7 +15622,7 @@
         <v>1751</v>
       </c>
       <c r="HB1" s="1" t="s">
-        <v>2809</v>
+        <v>2807</v>
       </c>
       <c r="HC1" s="22" t="s">
         <v>2102</v>
@@ -15831,19 +15825,19 @@
         <v>5</v>
       </c>
       <c r="BE2" s="77" t="s">
-        <v>2920</v>
+        <v>2918</v>
       </c>
       <c r="BF2" s="16" t="s">
         <v>2219</v>
       </c>
       <c r="BG2" s="10" t="s">
-        <v>2816</v>
+        <v>2814</v>
       </c>
       <c r="BH2" s="10" t="s">
         <v>2282</v>
       </c>
       <c r="BI2" s="10" t="s">
-        <v>2587</v>
+        <v>2585</v>
       </c>
       <c r="BJ2" s="10" t="s">
         <v>5</v>
@@ -15855,13 +15849,13 @@
         <v>5</v>
       </c>
       <c r="BM2" s="10" t="s">
-        <v>2815</v>
+        <v>2813</v>
       </c>
       <c r="BN2" s="10" t="s">
         <v>2282</v>
       </c>
       <c r="BO2" s="10" t="s">
-        <v>2597</v>
+        <v>2595</v>
       </c>
       <c r="BP2" s="10" t="s">
         <v>5</v>
@@ -15870,10 +15864,10 @@
         <v>2064</v>
       </c>
       <c r="BR2" s="54" t="s">
-        <v>2603</v>
+        <v>2601</v>
       </c>
       <c r="BS2" s="54" t="s">
-        <v>2604</v>
+        <v>2602</v>
       </c>
       <c r="BT2" s="43" t="s">
         <v>2196</v>
@@ -15882,7 +15876,7 @@
         <v>2282</v>
       </c>
       <c r="BV2" s="54" t="s">
-        <v>2617</v>
+        <v>2615</v>
       </c>
       <c r="BW2" s="43" t="s">
         <v>2199</v>
@@ -15891,37 +15885,37 @@
         <v>1759</v>
       </c>
       <c r="BY2" s="20" t="s">
-        <v>2622</v>
+        <v>2620</v>
       </c>
       <c r="BZ2" s="20" t="s">
-        <v>2626</v>
+        <v>2624</v>
       </c>
       <c r="CA2" s="44" t="s">
         <v>2224</v>
       </c>
       <c r="CB2" s="20" t="s">
-        <v>2646</v>
+        <v>2644</v>
       </c>
       <c r="CC2" s="20" t="s">
-        <v>2647</v>
+        <v>2645</v>
       </c>
       <c r="CD2" s="20" t="s">
         <v>2246</v>
       </c>
       <c r="CE2" s="20" t="s">
-        <v>2661</v>
+        <v>2659</v>
       </c>
       <c r="CF2" s="20" t="s">
-        <v>2665</v>
+        <v>2663</v>
       </c>
       <c r="CG2" s="20" t="s">
         <v>2215</v>
       </c>
       <c r="CH2" s="20" t="s">
+        <v>2572</v>
+      </c>
+      <c r="CI2" s="20" t="s">
         <v>2574</v>
-      </c>
-      <c r="CI2" s="20" t="s">
-        <v>2576</v>
       </c>
       <c r="CJ2" s="14" t="s">
         <v>1841</v>
@@ -15933,7 +15927,7 @@
         <v>1</v>
       </c>
       <c r="CM2" s="14" t="s">
-        <v>2841</v>
+        <v>2839</v>
       </c>
       <c r="CN2" s="10" t="s">
         <v>1842</v>
@@ -15960,7 +15954,7 @@
         <v>2318</v>
       </c>
       <c r="CV2" s="25" t="s">
-        <v>2550</v>
+        <v>2548</v>
       </c>
       <c r="CW2" s="25" t="s">
         <v>1769</v>
@@ -15969,10 +15963,10 @@
         <v>2318</v>
       </c>
       <c r="CY2" s="25" t="s">
-        <v>2547</v>
+        <v>2545</v>
       </c>
       <c r="CZ2" s="23" t="s">
-        <v>2858</v>
+        <v>2856</v>
       </c>
       <c r="DA2" s="73" t="s">
         <v>2498</v>
@@ -15981,13 +15975,13 @@
         <v>2336</v>
       </c>
       <c r="DC2" s="12" t="s">
-        <v>2835</v>
+        <v>2833</v>
       </c>
       <c r="DD2" s="71" t="s">
         <v>2320</v>
       </c>
       <c r="DE2" s="71" t="s">
-        <v>2837</v>
+        <v>2835</v>
       </c>
       <c r="DF2" s="12" t="s">
         <v>1795</v>
@@ -16049,55 +16043,55 @@
       <c r="EB2" s="12"/>
       <c r="EC2" s="12"/>
       <c r="ED2" s="12" t="s">
+        <v>2553</v>
+      </c>
+      <c r="EE2" s="12" t="s">
+        <v>2554</v>
+      </c>
+      <c r="EF2" s="12" t="s">
         <v>2555</v>
       </c>
-      <c r="EE2" s="12" t="s">
-        <v>2556</v>
-      </c>
-      <c r="EF2" s="12" t="s">
-        <v>2557</v>
-      </c>
       <c r="EG2" s="12" t="s">
-        <v>2690</v>
+        <v>2688</v>
       </c>
       <c r="EH2" s="12" t="s">
         <v>2280</v>
       </c>
       <c r="EI2" s="12" t="s">
-        <v>2691</v>
+        <v>2689</v>
       </c>
       <c r="EJ2" s="12" t="s">
-        <v>2887</v>
+        <v>2885</v>
       </c>
       <c r="EK2" s="12" t="s">
         <v>2280</v>
       </c>
       <c r="EL2" s="12" t="s">
-        <v>2891</v>
+        <v>2889</v>
       </c>
       <c r="EM2" s="12" t="s">
         <v>2139</v>
       </c>
       <c r="EN2" s="12" t="s">
-        <v>2896</v>
+        <v>2894</v>
       </c>
       <c r="EO2" s="12" t="s">
         <v>2296</v>
       </c>
       <c r="EP2" s="12" t="s">
+        <v>2897</v>
+      </c>
+      <c r="EQ2" s="12" t="s">
         <v>2899</v>
       </c>
-      <c r="EQ2" s="12" t="s">
-        <v>2901</v>
-      </c>
       <c r="EV2" s="10" t="s">
-        <v>2807</v>
+        <v>2805</v>
       </c>
       <c r="EW2" s="10" t="s">
-        <v>2585</v>
+        <v>2583</v>
       </c>
       <c r="EX2" s="10" t="s">
-        <v>2592</v>
+        <v>2590</v>
       </c>
       <c r="EY2" s="10" t="s">
         <v>5</v>
@@ -16112,10 +16106,10 @@
         <v>1751</v>
       </c>
       <c r="FC2" s="10" t="s">
-        <v>2574</v>
+        <v>2572</v>
       </c>
       <c r="FD2" s="10" t="s">
-        <v>2598</v>
+        <v>2596</v>
       </c>
       <c r="FE2" s="10" t="s">
         <v>5</v>
@@ -16324,7 +16318,7 @@
         <v>19</v>
       </c>
       <c r="J3" t="s">
-        <v>2913</v>
+        <v>2911</v>
       </c>
       <c r="K3" s="35" t="s">
         <v>2080</v>
@@ -16465,19 +16459,19 @@
         <v>20</v>
       </c>
       <c r="BE3" s="77" t="s">
-        <v>2921</v>
+        <v>2919</v>
       </c>
       <c r="BF3" s="16" t="s">
         <v>2220</v>
       </c>
       <c r="BG3" s="10" t="s">
-        <v>2807</v>
+        <v>2805</v>
       </c>
       <c r="BH3" s="10" t="s">
-        <v>2585</v>
+        <v>2583</v>
       </c>
       <c r="BI3" s="10" t="s">
-        <v>2592</v>
+        <v>2590</v>
       </c>
       <c r="BJ3" s="10" t="s">
         <v>2028</v>
@@ -16492,10 +16486,10 @@
         <v>1751</v>
       </c>
       <c r="BN3" s="10" t="s">
-        <v>2574</v>
+        <v>2572</v>
       </c>
       <c r="BO3" s="10" t="s">
-        <v>2598</v>
+        <v>2596</v>
       </c>
       <c r="BP3" s="10" t="s">
         <v>2028</v>
@@ -16504,19 +16498,19 @@
         <v>2065</v>
       </c>
       <c r="BR3" s="54" t="s">
+        <v>2601</v>
+      </c>
+      <c r="BS3" s="54" t="s">
         <v>2603</v>
-      </c>
-      <c r="BS3" s="54" t="s">
-        <v>2605</v>
       </c>
       <c r="BT3" s="43" t="s">
         <v>2211</v>
       </c>
       <c r="BU3" s="54" t="s">
+        <v>2614</v>
+      </c>
+      <c r="BV3" s="54" t="s">
         <v>2616</v>
-      </c>
-      <c r="BV3" s="54" t="s">
-        <v>2618</v>
       </c>
       <c r="BW3" s="43" t="s">
         <v>2209</v>
@@ -16525,37 +16519,37 @@
         <v>1776</v>
       </c>
       <c r="BY3" s="20" t="s">
-        <v>2622</v>
+        <v>2620</v>
       </c>
       <c r="BZ3" s="20" t="s">
-        <v>2627</v>
+        <v>2625</v>
       </c>
       <c r="CA3" s="44" t="s">
         <v>2225</v>
       </c>
       <c r="CB3" s="20" t="s">
+        <v>2644</v>
+      </c>
+      <c r="CC3" s="20" t="s">
         <v>2646</v>
-      </c>
-      <c r="CC3" s="20" t="s">
-        <v>2648</v>
       </c>
       <c r="CD3" s="20" t="s">
         <v>2192</v>
       </c>
       <c r="CE3" s="20" t="s">
-        <v>2662</v>
+        <v>2660</v>
       </c>
       <c r="CF3" s="20" t="s">
-        <v>2666</v>
+        <v>2664</v>
       </c>
       <c r="CG3" s="20" t="s">
+        <v>2840</v>
+      </c>
+      <c r="CH3" s="20" t="s">
+        <v>2573</v>
+      </c>
+      <c r="CI3" s="20" t="s">
         <v>2842</v>
-      </c>
-      <c r="CH3" s="20" t="s">
-        <v>2575</v>
-      </c>
-      <c r="CI3" s="20" t="s">
-        <v>2844</v>
       </c>
       <c r="CJ3" s="14" t="s">
         <v>1840</v>
@@ -16594,7 +16588,7 @@
         <v>2318</v>
       </c>
       <c r="CV3" s="25" t="s">
-        <v>2549</v>
+        <v>2547</v>
       </c>
       <c r="CW3" s="25" t="s">
         <v>1770</v>
@@ -16603,10 +16597,10 @@
         <v>2318</v>
       </c>
       <c r="CY3" s="25" t="s">
-        <v>2548</v>
+        <v>2546</v>
       </c>
       <c r="CZ3" s="23" t="s">
-        <v>2859</v>
+        <v>2857</v>
       </c>
       <c r="DA3" s="73" t="s">
         <v>2498</v>
@@ -16615,13 +16609,13 @@
         <v>2337</v>
       </c>
       <c r="DC3" s="12" t="s">
-        <v>2836</v>
+        <v>2834</v>
       </c>
       <c r="DD3" s="71" t="s">
         <v>2320</v>
       </c>
       <c r="DE3" s="71" t="s">
-        <v>2838</v>
+        <v>2836</v>
       </c>
       <c r="DF3" s="12" t="s">
         <v>1796</v>
@@ -16633,13 +16627,13 @@
         <v>2351</v>
       </c>
       <c r="DI3" s="12" t="s">
-        <v>2694</v>
+        <v>2692</v>
       </c>
       <c r="DJ3" s="61" t="s">
         <v>2334</v>
       </c>
       <c r="DK3" s="12" t="s">
-        <v>2695</v>
+        <v>2693</v>
       </c>
       <c r="DL3" s="12" t="s">
         <v>2103</v>
@@ -16689,48 +16683,48 @@
         <v>2525</v>
       </c>
       <c r="ED3" s="12" t="s">
-        <v>2562</v>
+        <v>2560</v>
       </c>
       <c r="EE3" s="12" t="s">
-        <v>2563</v>
+        <v>2561</v>
       </c>
       <c r="EF3" s="52"/>
       <c r="EG3" s="12" t="s">
-        <v>2692</v>
+        <v>2690</v>
       </c>
       <c r="EH3" s="12"/>
       <c r="EI3" s="12" t="s">
-        <v>2693</v>
+        <v>2691</v>
       </c>
       <c r="EJ3" s="12" t="s">
-        <v>2888</v>
+        <v>2886</v>
       </c>
       <c r="EK3" t="s">
         <v>2280</v>
       </c>
       <c r="EL3" s="12" t="s">
-        <v>2892</v>
+        <v>2890</v>
       </c>
       <c r="EM3" s="12" t="s">
         <v>2260</v>
       </c>
       <c r="EN3" s="12" t="s">
-        <v>2896</v>
+        <v>2894</v>
       </c>
       <c r="EO3" s="12" t="s">
         <v>2297</v>
       </c>
       <c r="EP3" s="12" t="s">
-        <v>2900</v>
+        <v>2898</v>
       </c>
       <c r="EV3" s="10" t="s">
-        <v>2808</v>
+        <v>2806</v>
       </c>
       <c r="EW3" s="10" t="s">
-        <v>2585</v>
+        <v>2583</v>
       </c>
       <c r="EX3" s="10" t="s">
-        <v>2588</v>
+        <v>2586</v>
       </c>
       <c r="EY3" s="10" t="s">
         <v>2028</v>
@@ -16742,112 +16736,112 @@
         <v>2032</v>
       </c>
       <c r="FB3" s="10" t="s">
-        <v>2809</v>
+        <v>2807</v>
       </c>
       <c r="FC3" s="10" t="s">
-        <v>2596</v>
+        <v>2594</v>
       </c>
       <c r="FD3" s="10" t="s">
-        <v>2601</v>
+        <v>2599</v>
       </c>
       <c r="FE3" s="10" t="s">
         <v>2028</v>
       </c>
       <c r="FG3" t="s">
-        <v>2936</v>
+        <v>2934</v>
       </c>
       <c r="FH3" t="s">
-        <v>2967</v>
+        <v>2965</v>
       </c>
       <c r="FI3" t="s">
-        <v>2967</v>
+        <v>2965</v>
       </c>
       <c r="FJ3" s="85" t="s">
-        <v>2967</v>
+        <v>2965</v>
       </c>
       <c r="FK3" t="s">
+        <v>2966</v>
+      </c>
+      <c r="FL3" s="85" t="s">
+        <v>2966</v>
+      </c>
+      <c r="FM3" s="85" t="s">
+        <v>2966</v>
+      </c>
+      <c r="FN3" s="85" t="s">
+        <v>2966</v>
+      </c>
+      <c r="FO3" s="85" t="s">
+        <v>2966</v>
+      </c>
+      <c r="FP3" s="85" t="s">
+        <v>2966</v>
+      </c>
+      <c r="FQ3" s="85" t="s">
+        <v>2966</v>
+      </c>
+      <c r="FR3" s="85" t="s">
+        <v>2966</v>
+      </c>
+      <c r="FS3" s="85" t="s">
+        <v>2966</v>
+      </c>
+      <c r="FT3" s="85" t="s">
+        <v>3001</v>
+      </c>
+      <c r="FV3" t="s">
+        <v>2974</v>
+      </c>
+      <c r="FX3" t="s">
         <v>2968</v>
       </c>
-      <c r="FL3" s="85" t="s">
-        <v>2968</v>
-      </c>
-      <c r="FM3" s="85" t="s">
-        <v>2968</v>
-      </c>
-      <c r="FN3" s="85" t="s">
-        <v>2968</v>
-      </c>
-      <c r="FO3" s="85" t="s">
-        <v>2968</v>
-      </c>
-      <c r="FP3" s="85" t="s">
-        <v>2968</v>
-      </c>
-      <c r="FQ3" s="85" t="s">
-        <v>2968</v>
-      </c>
-      <c r="FR3" s="85" t="s">
-        <v>2968</v>
-      </c>
-      <c r="FS3" s="85" t="s">
-        <v>2968</v>
-      </c>
-      <c r="FT3" s="85" t="s">
-        <v>3003</v>
-      </c>
-      <c r="FV3" t="s">
-        <v>2976</v>
-      </c>
-      <c r="FX3" t="s">
-        <v>2970</v>
-      </c>
       <c r="FY3" t="s">
-        <v>2998</v>
+        <v>2996</v>
       </c>
       <c r="FZ3" t="s">
+        <v>2978</v>
+      </c>
+      <c r="GD3" t="s">
+        <v>2979</v>
+      </c>
+      <c r="GE3" s="85" t="s">
+        <v>2979</v>
+      </c>
+      <c r="GI3" t="s">
+        <v>2993</v>
+      </c>
+      <c r="GP3" t="s">
+        <v>2981</v>
+      </c>
+      <c r="GQ3" s="85" t="s">
+        <v>2981</v>
+      </c>
+      <c r="GR3" s="85" t="s">
+        <v>2958</v>
+      </c>
+      <c r="GS3" s="85" t="s">
+        <v>2959</v>
+      </c>
+      <c r="GT3" s="85" t="s">
+        <v>2959</v>
+      </c>
+      <c r="GU3" t="s">
         <v>2980</v>
       </c>
-      <c r="GD3" t="s">
-        <v>2981</v>
-      </c>
-      <c r="GE3" s="85" t="s">
-        <v>2981</v>
-      </c>
-      <c r="GI3" t="s">
-        <v>2995</v>
-      </c>
-      <c r="GP3" t="s">
-        <v>2983</v>
-      </c>
-      <c r="GQ3" s="85" t="s">
-        <v>2983</v>
-      </c>
-      <c r="GR3" s="85" t="s">
-        <v>2960</v>
-      </c>
-      <c r="GS3" s="85" t="s">
-        <v>2961</v>
-      </c>
-      <c r="GT3" s="85" t="s">
-        <v>2961</v>
-      </c>
-      <c r="GU3" t="s">
-        <v>2982</v>
-      </c>
       <c r="GV3" t="s">
-        <v>2958</v>
+        <v>2956</v>
       </c>
       <c r="GW3" s="85" t="s">
-        <v>2958</v>
+        <v>2956</v>
       </c>
       <c r="GX3" s="85" t="s">
-        <v>2958</v>
+        <v>2956</v>
       </c>
       <c r="GY3" t="s">
-        <v>2976</v>
+        <v>2974</v>
       </c>
       <c r="GZ3" s="85" t="s">
-        <v>2976</v>
+        <v>2974</v>
       </c>
       <c r="HA3" s="10" t="s">
         <v>2028</v>
@@ -17026,13 +17020,13 @@
         <v>2221</v>
       </c>
       <c r="BG4" s="10" t="s">
-        <v>2808</v>
+        <v>2806</v>
       </c>
       <c r="BH4" s="10" t="s">
-        <v>2585</v>
+        <v>2583</v>
       </c>
       <c r="BI4" s="10" t="s">
-        <v>2588</v>
+        <v>2586</v>
       </c>
       <c r="BJ4" s="10" t="s">
         <v>2029</v>
@@ -17050,7 +17044,7 @@
         <v>2282</v>
       </c>
       <c r="BO4" s="10" t="s">
-        <v>2599</v>
+        <v>2597</v>
       </c>
       <c r="BP4" s="17" t="s">
         <v>2036</v>
@@ -17059,19 +17053,19 @@
         <v>2066</v>
       </c>
       <c r="BR4" s="54" t="s">
-        <v>2603</v>
+        <v>2601</v>
       </c>
       <c r="BS4" s="54" t="s">
-        <v>2606</v>
+        <v>2604</v>
       </c>
       <c r="BT4" s="29" t="s">
-        <v>2854</v>
+        <v>2852</v>
       </c>
       <c r="BU4" s="29" t="s">
-        <v>2616</v>
+        <v>2614</v>
       </c>
       <c r="BV4" s="29" t="s">
-        <v>2855</v>
+        <v>2853</v>
       </c>
       <c r="BW4" s="43" t="s">
         <v>2204</v>
@@ -17080,43 +17074,43 @@
         <v>2043</v>
       </c>
       <c r="BY4" s="20" t="s">
-        <v>2574</v>
+        <v>2572</v>
       </c>
       <c r="BZ4" s="20" t="s">
-        <v>2628</v>
+        <v>2626</v>
       </c>
       <c r="CA4" s="44" t="s">
         <v>2226</v>
       </c>
       <c r="CB4" s="20" t="s">
-        <v>2646</v>
+        <v>2644</v>
       </c>
       <c r="CC4" s="20" t="s">
-        <v>2649</v>
+        <v>2647</v>
       </c>
       <c r="CD4" s="20" t="s">
-        <v>2851</v>
+        <v>2849</v>
       </c>
       <c r="CE4" s="20" t="s">
-        <v>2663</v>
+        <v>2661</v>
       </c>
       <c r="CF4" s="20" t="s">
-        <v>2667</v>
+        <v>2665</v>
       </c>
       <c r="CG4" s="20" t="s">
+        <v>2841</v>
+      </c>
+      <c r="CH4" s="20" t="s">
+        <v>2573</v>
+      </c>
+      <c r="CI4" s="20" t="s">
         <v>2843</v>
-      </c>
-      <c r="CH4" s="20" t="s">
-        <v>2575</v>
-      </c>
-      <c r="CI4" s="20" t="s">
-        <v>2845</v>
       </c>
       <c r="CJ4" s="14" t="s">
         <v>1839</v>
       </c>
       <c r="CK4" s="20" t="s">
-        <v>2812</v>
+        <v>2810</v>
       </c>
       <c r="CL4" s="20">
         <v>3</v>
@@ -17147,17 +17141,17 @@
       </c>
       <c r="CU4" s="25"/>
       <c r="CV4" s="25" t="s">
-        <v>2551</v>
+        <v>2549</v>
       </c>
       <c r="CW4" s="25" t="s">
-        <v>2544</v>
+        <v>2542</v>
       </c>
       <c r="CX4" s="25"/>
       <c r="CY4" s="25" t="s">
-        <v>2545</v>
+        <v>2543</v>
       </c>
       <c r="CZ4" s="23" t="s">
-        <v>2860</v>
+        <v>2858</v>
       </c>
       <c r="DA4" s="73" t="s">
         <v>2498</v>
@@ -17234,46 +17228,46 @@
         <v>2517</v>
       </c>
       <c r="ED4" s="12" t="s">
-        <v>2569</v>
+        <v>2567</v>
       </c>
       <c r="EE4" s="52" t="s">
         <v>2318</v>
       </c>
       <c r="EF4" s="52" t="s">
-        <v>2564</v>
+        <v>2562</v>
       </c>
       <c r="EJ4" t="s">
-        <v>2889</v>
+        <v>2887</v>
       </c>
       <c r="EK4" t="s">
         <v>2280</v>
       </c>
       <c r="EL4" t="s">
+        <v>2891</v>
+      </c>
+      <c r="EM4" t="s">
         <v>2893</v>
-      </c>
-      <c r="EM4" t="s">
-        <v>2895</v>
       </c>
       <c r="EN4" t="s">
         <v>2282</v>
       </c>
       <c r="EO4" t="s">
-        <v>2897</v>
+        <v>2895</v>
       </c>
       <c r="EP4" t="s">
+        <v>2900</v>
+      </c>
+      <c r="EQ4" t="s">
         <v>2902</v>
-      </c>
-      <c r="EQ4" t="s">
-        <v>2904</v>
       </c>
       <c r="EV4" s="10" t="s">
         <v>1752</v>
       </c>
       <c r="EW4" s="10" t="s">
-        <v>2586</v>
+        <v>2584</v>
       </c>
       <c r="EX4" s="10" t="s">
-        <v>2591</v>
+        <v>2589</v>
       </c>
       <c r="EY4" s="10" t="s">
         <v>2029</v>
@@ -17285,100 +17279,100 @@
         <v>2033</v>
       </c>
       <c r="FB4" s="10" t="s">
-        <v>2810</v>
+        <v>2808</v>
       </c>
       <c r="FC4" s="10" t="s">
-        <v>2596</v>
+        <v>2594</v>
       </c>
       <c r="FD4" s="10" t="s">
-        <v>2600</v>
+        <v>2598</v>
       </c>
       <c r="FE4" s="85" t="s">
         <v>2036</v>
       </c>
       <c r="FG4" t="s">
+        <v>2998</v>
+      </c>
+      <c r="FH4" t="s">
+        <v>2994</v>
+      </c>
+      <c r="FI4" s="85" t="s">
+        <v>2994</v>
+      </c>
+      <c r="FK4" t="s">
+        <v>2967</v>
+      </c>
+      <c r="FL4" s="85" t="s">
+        <v>2967</v>
+      </c>
+      <c r="FM4" s="85" t="s">
+        <v>2967</v>
+      </c>
+      <c r="FN4" s="85" t="s">
+        <v>2967</v>
+      </c>
+      <c r="FO4" s="85" t="s">
+        <v>2967</v>
+      </c>
+      <c r="FP4" s="85" t="s">
+        <v>2967</v>
+      </c>
+      <c r="FQ4" s="85" t="s">
+        <v>2967</v>
+      </c>
+      <c r="FR4" s="85" t="s">
+        <v>2967</v>
+      </c>
+      <c r="FS4" s="85" t="s">
+        <v>2967</v>
+      </c>
+      <c r="FT4" t="s">
         <v>3000</v>
       </c>
-      <c r="FH4" t="s">
-        <v>2996</v>
-      </c>
-      <c r="FI4" s="85" t="s">
-        <v>2996</v>
-      </c>
-      <c r="FK4" t="s">
-        <v>2969</v>
-      </c>
-      <c r="FL4" s="85" t="s">
-        <v>2969</v>
-      </c>
-      <c r="FM4" s="85" t="s">
-        <v>2969</v>
-      </c>
-      <c r="FN4" s="85" t="s">
-        <v>2969</v>
-      </c>
-      <c r="FO4" s="85" t="s">
-        <v>2969</v>
-      </c>
-      <c r="FP4" s="85" t="s">
-        <v>2969</v>
-      </c>
-      <c r="FQ4" s="85" t="s">
-        <v>2969</v>
-      </c>
-      <c r="FR4" s="85" t="s">
-        <v>2969</v>
-      </c>
-      <c r="FS4" s="85" t="s">
-        <v>2969</v>
-      </c>
-      <c r="FT4" t="s">
-        <v>3002</v>
-      </c>
       <c r="FV4" s="85" t="s">
-        <v>2977</v>
+        <v>2975</v>
       </c>
       <c r="FX4" s="85" t="s">
-        <v>2973</v>
+        <v>2971</v>
       </c>
       <c r="FZ4" t="s">
-        <v>2997</v>
+        <v>2995</v>
       </c>
       <c r="GD4" t="s">
-        <v>2994</v>
+        <v>2992</v>
       </c>
       <c r="GE4" s="85" t="s">
-        <v>2994</v>
+        <v>2992</v>
       </c>
       <c r="GI4" t="s">
-        <v>2936</v>
+        <v>2934</v>
       </c>
       <c r="GP4" t="s">
-        <v>2959</v>
+        <v>2957</v>
       </c>
       <c r="GQ4" s="85" t="s">
-        <v>2959</v>
+        <v>2957</v>
       </c>
       <c r="GS4" s="85" t="s">
-        <v>2962</v>
+        <v>2960</v>
       </c>
       <c r="GT4" s="85" t="s">
-        <v>2965</v>
+        <v>2963</v>
       </c>
       <c r="GV4" s="85" t="s">
-        <v>2984</v>
+        <v>2982</v>
       </c>
       <c r="GW4" s="85" t="s">
-        <v>2985</v>
+        <v>2983</v>
       </c>
       <c r="GX4" s="85" t="s">
-        <v>2984</v>
+        <v>2982</v>
       </c>
       <c r="GY4" t="s">
-        <v>2978</v>
+        <v>2976</v>
       </c>
       <c r="GZ4" s="85" t="s">
-        <v>2978</v>
+        <v>2976</v>
       </c>
       <c r="HA4" s="85" t="s">
         <v>2036</v>
@@ -17449,7 +17443,7 @@
         <v>1348</v>
       </c>
       <c r="W5" t="s">
-        <v>2682</v>
+        <v>2680</v>
       </c>
       <c r="X5" s="6" t="s">
         <v>1361</v>
@@ -17536,7 +17530,7 @@
         <v>1661</v>
       </c>
       <c r="BF5" s="16" t="s">
-        <v>2832</v>
+        <v>2830</v>
       </c>
       <c r="BG5" s="10" t="s">
         <v>1754</v>
@@ -17545,7 +17539,7 @@
         <v>2282</v>
       </c>
       <c r="BI5" s="10" t="s">
-        <v>2589</v>
+        <v>2587</v>
       </c>
       <c r="BJ5" s="10" t="s">
         <v>2216</v>
@@ -17557,13 +17551,13 @@
         <v>2034</v>
       </c>
       <c r="BM5" s="10" t="s">
-        <v>2809</v>
+        <v>2807</v>
       </c>
       <c r="BN5" s="10" t="s">
-        <v>2596</v>
+        <v>2594</v>
       </c>
       <c r="BO5" s="10" t="s">
-        <v>2601</v>
+        <v>2599</v>
       </c>
       <c r="BP5" s="17" t="s">
         <v>2037</v>
@@ -17572,10 +17566,10 @@
         <v>2067</v>
       </c>
       <c r="BR5" s="54" t="s">
-        <v>2603</v>
+        <v>2601</v>
       </c>
       <c r="BS5" s="54" t="s">
-        <v>2607</v>
+        <v>2605</v>
       </c>
       <c r="BT5" s="43" t="s">
         <v>2212</v>
@@ -17584,7 +17578,7 @@
         <v>2280</v>
       </c>
       <c r="BV5" s="54" t="s">
-        <v>2619</v>
+        <v>2617</v>
       </c>
       <c r="BW5" s="43" t="s">
         <v>2207</v>
@@ -17593,43 +17587,43 @@
         <v>2044</v>
       </c>
       <c r="BY5" s="20" t="s">
-        <v>2624</v>
+        <v>2622</v>
       </c>
       <c r="BZ5" s="20" t="s">
-        <v>2629</v>
+        <v>2627</v>
       </c>
       <c r="CA5" s="44" t="s">
         <v>2227</v>
       </c>
       <c r="CB5" s="20" t="s">
-        <v>2646</v>
+        <v>2644</v>
       </c>
       <c r="CC5" s="20" t="s">
-        <v>2650</v>
+        <v>2648</v>
       </c>
       <c r="CD5" s="20" t="s">
         <v>2141</v>
       </c>
       <c r="CE5" s="20" t="s">
-        <v>2664</v>
+        <v>2662</v>
       </c>
       <c r="CF5" s="20" t="s">
-        <v>2668</v>
+        <v>2666</v>
       </c>
       <c r="CG5" s="20" t="s">
-        <v>2819</v>
+        <v>2817</v>
       </c>
       <c r="CH5" s="20" t="s">
-        <v>2575</v>
+        <v>2573</v>
       </c>
       <c r="CI5" s="20" t="s">
-        <v>2820</v>
+        <v>2818</v>
       </c>
       <c r="CJ5" s="14" t="s">
+        <v>2809</v>
+      </c>
+      <c r="CK5" s="20" t="s">
         <v>2811</v>
-      </c>
-      <c r="CK5" s="20" t="s">
-        <v>2813</v>
       </c>
       <c r="CL5" s="20">
         <v>4</v>
@@ -17660,7 +17654,7 @@
       </c>
       <c r="CU5" s="25"/>
       <c r="CV5" s="25" t="s">
-        <v>2552</v>
+        <v>2550</v>
       </c>
       <c r="CW5" s="25" t="s">
         <v>1773</v>
@@ -17669,10 +17663,10 @@
         <v>2318</v>
       </c>
       <c r="CY5" s="25" t="s">
-        <v>2541</v>
+        <v>2539</v>
       </c>
       <c r="CZ5" s="23" t="s">
-        <v>2861</v>
+        <v>2859</v>
       </c>
       <c r="DA5" s="73" t="s">
         <v>2498</v>
@@ -17696,13 +17690,13 @@
         <v>2334</v>
       </c>
       <c r="DI5" s="12" t="s">
-        <v>2696</v>
+        <v>2694</v>
       </c>
       <c r="DJ5" s="61" t="s">
         <v>2334</v>
       </c>
       <c r="DK5" s="12" t="s">
-        <v>2697</v>
+        <v>2695</v>
       </c>
       <c r="DL5" s="36" t="s">
         <v>2105</v>
@@ -17751,31 +17745,31 @@
         <v>2521</v>
       </c>
       <c r="ED5" s="12" t="s">
-        <v>2570</v>
+        <v>2568</v>
       </c>
       <c r="EE5" s="52" t="s">
         <v>2318</v>
       </c>
       <c r="EF5" s="12" t="s">
-        <v>2565</v>
+        <v>2563</v>
       </c>
       <c r="EJ5" t="s">
-        <v>2890</v>
+        <v>2888</v>
       </c>
       <c r="EK5" t="s">
         <v>2280</v>
       </c>
       <c r="EL5" t="s">
-        <v>2894</v>
+        <v>2892</v>
       </c>
       <c r="EV5" s="10" t="s">
         <v>1777</v>
       </c>
       <c r="EW5" s="10" t="s">
-        <v>2586</v>
+        <v>2584</v>
       </c>
       <c r="EX5" s="10" t="s">
-        <v>2593</v>
+        <v>2591</v>
       </c>
       <c r="EY5" s="10" t="s">
         <v>2216</v>
@@ -17793,34 +17787,34 @@
         <v>2037</v>
       </c>
       <c r="FG5" t="s">
-        <v>2999</v>
+        <v>2997</v>
       </c>
       <c r="FI5" t="s">
-        <v>3008</v>
+        <v>3006</v>
       </c>
       <c r="FT5" s="85" t="s">
-        <v>3004</v>
+        <v>3002</v>
       </c>
       <c r="FV5" s="85" t="s">
-        <v>2978</v>
+        <v>2976</v>
       </c>
       <c r="FX5" s="85" t="s">
-        <v>2971</v>
+        <v>2969</v>
       </c>
       <c r="GS5" s="85" t="s">
-        <v>2963</v>
+        <v>2961</v>
       </c>
       <c r="GT5" s="85" t="s">
-        <v>2966</v>
+        <v>2964</v>
       </c>
       <c r="GX5" t="s">
-        <v>2993</v>
+        <v>2991</v>
       </c>
       <c r="GY5" t="s">
-        <v>2977</v>
+        <v>2975</v>
       </c>
       <c r="GZ5" s="85" t="s">
-        <v>2977</v>
+        <v>2975</v>
       </c>
       <c r="HA5" s="85" t="s">
         <v>2037</v>
@@ -17855,7 +17849,7 @@
         <v>59</v>
       </c>
       <c r="J6" t="s">
-        <v>2922</v>
+        <v>2920</v>
       </c>
       <c r="K6" s="35" t="s">
         <v>2083</v>
@@ -17888,7 +17882,7 @@
         <v>1349</v>
       </c>
       <c r="X6" t="s">
-        <v>2683</v>
+        <v>2681</v>
       </c>
       <c r="Y6" s="6" t="s">
         <v>1364</v>
@@ -17980,25 +17974,25 @@
         <v>2282</v>
       </c>
       <c r="BI6" s="10" t="s">
-        <v>2590</v>
+        <v>2588</v>
       </c>
       <c r="BJ6" s="10" t="s">
-        <v>2880</v>
+        <v>2878</v>
       </c>
       <c r="BK6" s="10" t="s">
-        <v>2573</v>
+        <v>2571</v>
       </c>
       <c r="BL6" s="10" t="s">
-        <v>2573</v>
+        <v>2571</v>
       </c>
       <c r="BM6" s="10" t="s">
-        <v>2810</v>
+        <v>2808</v>
       </c>
       <c r="BN6" s="10" t="s">
-        <v>2596</v>
+        <v>2594</v>
       </c>
       <c r="BO6" s="10" t="s">
-        <v>2600</v>
+        <v>2598</v>
       </c>
       <c r="BP6" s="17" t="s">
         <v>2038</v>
@@ -18007,10 +18001,10 @@
         <v>2068</v>
       </c>
       <c r="BR6" s="54" t="s">
-        <v>2603</v>
+        <v>2601</v>
       </c>
       <c r="BS6" s="54" t="s">
-        <v>2608</v>
+        <v>2606</v>
       </c>
       <c r="BT6" s="43" t="s">
         <v>2213</v>
@@ -18019,7 +18013,7 @@
         <v>2280</v>
       </c>
       <c r="BV6" s="54" t="s">
-        <v>2620</v>
+        <v>2618</v>
       </c>
       <c r="BW6" s="43" t="s">
         <v>2197</v>
@@ -18028,38 +18022,38 @@
         <v>2045</v>
       </c>
       <c r="BY6" s="20" t="s">
-        <v>2624</v>
+        <v>2622</v>
       </c>
       <c r="BZ6" s="20" t="s">
-        <v>2630</v>
+        <v>2628</v>
       </c>
       <c r="CA6" s="44" t="s">
         <v>2228</v>
       </c>
       <c r="CB6" s="20" t="s">
-        <v>2646</v>
+        <v>2644</v>
       </c>
       <c r="CC6" s="20" t="s">
-        <v>2651</v>
+        <v>2649</v>
       </c>
       <c r="CD6" s="20" t="s">
         <v>2247</v>
       </c>
       <c r="CE6" s="20" t="s">
-        <v>2661</v>
+        <v>2659</v>
       </c>
       <c r="CF6" s="20" t="s">
-        <v>2669</v>
+        <v>2667</v>
       </c>
       <c r="CG6" s="20" t="str">
         <f>_xlfn.CONCAT(CG5,"_error")</f>
         <v>CO2_flux_mmol_m2_d_error</v>
       </c>
       <c r="CH6" s="20" t="s">
-        <v>2575</v>
+        <v>2573</v>
       </c>
       <c r="CI6" s="20" t="s">
-        <v>2821</v>
+        <v>2819</v>
       </c>
       <c r="CJ6" s="14" t="s">
         <v>1818</v>
@@ -18098,7 +18092,7 @@
         <v>2319</v>
       </c>
       <c r="CV6" s="25" t="s">
-        <v>2553</v>
+        <v>2551</v>
       </c>
       <c r="CW6" s="25" t="s">
         <v>1774</v>
@@ -18110,7 +18104,7 @@
         <v>2340</v>
       </c>
       <c r="CZ6" s="23" t="s">
-        <v>2862</v>
+        <v>2860</v>
       </c>
       <c r="DA6" s="73" t="s">
         <v>2498</v>
@@ -18186,23 +18180,23 @@
         <v>2523</v>
       </c>
       <c r="ED6" s="12" t="s">
-        <v>2571</v>
+        <v>2569</v>
       </c>
       <c r="EE6" s="52"/>
       <c r="EF6" s="12" t="s">
-        <v>2566</v>
+        <v>2564</v>
       </c>
       <c r="EV6" s="85"/>
       <c r="EW6" s="85"/>
       <c r="EX6" s="85"/>
       <c r="EY6" s="10" t="s">
-        <v>2880</v>
+        <v>2878</v>
       </c>
       <c r="EZ6" s="10" t="s">
-        <v>2573</v>
+        <v>2571</v>
       </c>
       <c r="FA6" s="10" t="s">
-        <v>2573</v>
+        <v>2571</v>
       </c>
       <c r="FB6" s="85"/>
       <c r="FC6" s="85"/>
@@ -18211,28 +18205,28 @@
         <v>2038</v>
       </c>
       <c r="FG6" t="s">
-        <v>2997</v>
+        <v>2995</v>
       </c>
       <c r="FI6" t="s">
-        <v>3009</v>
+        <v>3007</v>
       </c>
       <c r="FT6" s="85" t="s">
-        <v>3005</v>
+        <v>3003</v>
       </c>
       <c r="FV6" t="s">
         <v>2029</v>
       </c>
       <c r="FX6" s="85" t="s">
-        <v>2974</v>
+        <v>2972</v>
       </c>
       <c r="GT6" t="s">
-        <v>2964</v>
+        <v>2962</v>
       </c>
       <c r="GY6" t="s">
-        <v>2986</v>
+        <v>2984</v>
       </c>
       <c r="GZ6" s="85" t="s">
-        <v>2986</v>
+        <v>2984</v>
       </c>
       <c r="HA6" s="85" t="s">
         <v>2038</v>
@@ -18297,7 +18291,7 @@
         <v>1350</v>
       </c>
       <c r="X7" s="70" t="s">
-        <v>2818</v>
+        <v>2816</v>
       </c>
       <c r="Y7" s="6" t="s">
         <v>1365</v>
@@ -18380,16 +18374,16 @@
         <v>2048</v>
       </c>
       <c r="BH7" s="10" t="s">
-        <v>2586</v>
+        <v>2584</v>
       </c>
       <c r="BJ7" s="10" t="s">
         <v>2030</v>
       </c>
       <c r="BK7" s="10" t="s">
-        <v>2830</v>
+        <v>2828</v>
       </c>
       <c r="BL7" s="10" t="s">
-        <v>2830</v>
+        <v>2828</v>
       </c>
       <c r="BM7" s="10" t="s">
         <v>1758</v>
@@ -18398,7 +18392,7 @@
         <v>2282</v>
       </c>
       <c r="BO7" s="10" t="s">
-        <v>2602</v>
+        <v>2600</v>
       </c>
       <c r="BP7" s="17" t="s">
         <v>2030</v>
@@ -18407,10 +18401,10 @@
         <v>2069</v>
       </c>
       <c r="BR7" s="54" t="s">
-        <v>2603</v>
+        <v>2601</v>
       </c>
       <c r="BS7" s="54" t="s">
-        <v>2609</v>
+        <v>2607</v>
       </c>
       <c r="BT7" s="43" t="s">
         <v>2214</v>
@@ -18419,7 +18413,7 @@
         <v>2280</v>
       </c>
       <c r="BV7" s="54" t="s">
-        <v>2621</v>
+        <v>2619</v>
       </c>
       <c r="BW7" s="43" t="s">
         <v>2206</v>
@@ -18428,43 +18422,43 @@
         <v>2046</v>
       </c>
       <c r="BY7" s="20" t="s">
-        <v>2623</v>
+        <v>2621</v>
       </c>
       <c r="BZ7" s="20" t="s">
-        <v>2631</v>
+        <v>2629</v>
       </c>
       <c r="CA7" s="44" t="s">
         <v>2229</v>
       </c>
       <c r="CB7" s="20" t="s">
-        <v>2646</v>
+        <v>2644</v>
       </c>
       <c r="CC7" s="20" t="s">
-        <v>2652</v>
+        <v>2650</v>
       </c>
       <c r="CD7" s="20" t="s">
         <v>2248</v>
       </c>
       <c r="CE7" s="20" t="s">
-        <v>2661</v>
+        <v>2659</v>
       </c>
       <c r="CF7" s="20" t="s">
-        <v>2670</v>
+        <v>2668</v>
       </c>
       <c r="CG7" s="20" t="s">
         <v>2238</v>
       </c>
       <c r="CH7" s="20" t="s">
+        <v>2573</v>
+      </c>
+      <c r="CI7" s="20" t="s">
         <v>2575</v>
-      </c>
-      <c r="CI7" s="20" t="s">
-        <v>2577</v>
       </c>
       <c r="CJ7" s="14" t="s">
         <v>1819</v>
       </c>
       <c r="CK7" s="20" t="s">
-        <v>2558</v>
+        <v>2556</v>
       </c>
       <c r="CL7" s="20">
         <v>6</v>
@@ -18497,7 +18491,7 @@
         <v>2319</v>
       </c>
       <c r="CV7" s="25" t="s">
-        <v>2554</v>
+        <v>2552</v>
       </c>
       <c r="CW7" s="20" t="s">
         <v>1779</v>
@@ -18506,10 +18500,10 @@
         <v>2318</v>
       </c>
       <c r="CY7" s="20" t="s">
-        <v>2540</v>
+        <v>2538</v>
       </c>
       <c r="CZ7" s="23" t="s">
-        <v>2863</v>
+        <v>2861</v>
       </c>
       <c r="DA7" s="73" t="s">
         <v>2498</v>
@@ -18533,13 +18527,13 @@
         <v>2334</v>
       </c>
       <c r="DI7" s="12" t="s">
-        <v>2698</v>
+        <v>2696</v>
       </c>
       <c r="DJ7" s="61" t="s">
         <v>2334</v>
       </c>
       <c r="DK7" s="12" t="s">
-        <v>2699</v>
+        <v>2697</v>
       </c>
       <c r="DL7" s="36" t="s">
         <v>2107</v>
@@ -18584,10 +18578,10 @@
         <v>2247</v>
       </c>
       <c r="EE7" s="20" t="s">
-        <v>2661</v>
+        <v>2659</v>
       </c>
       <c r="EF7" s="20" t="s">
-        <v>2941</v>
+        <v>2939</v>
       </c>
       <c r="EV7" s="85"/>
       <c r="EW7" s="85"/>
@@ -18596,10 +18590,10 @@
         <v>2030</v>
       </c>
       <c r="EZ7" s="10" t="s">
-        <v>2830</v>
+        <v>2828</v>
       </c>
       <c r="FA7" s="10" t="s">
-        <v>2830</v>
+        <v>2828</v>
       </c>
       <c r="FB7" s="85"/>
       <c r="FC7" s="85"/>
@@ -18608,19 +18602,19 @@
         <v>2030</v>
       </c>
       <c r="FT7" s="85" t="s">
-        <v>3006</v>
+        <v>3004</v>
       </c>
       <c r="FV7" t="s">
         <v>2030</v>
       </c>
       <c r="FX7" s="85" t="s">
-        <v>2972</v>
+        <v>2970</v>
       </c>
       <c r="GY7" s="85" t="s">
-        <v>2987</v>
+        <v>2985</v>
       </c>
       <c r="GZ7" s="85" t="s">
-        <v>2987</v>
+        <v>2985</v>
       </c>
       <c r="HA7" s="85" t="s">
         <v>2030</v>
@@ -18658,7 +18652,7 @@
         <v>83</v>
       </c>
       <c r="K8" s="75" t="s">
-        <v>2881</v>
+        <v>2879</v>
       </c>
       <c r="L8" t="s">
         <v>84</v>
@@ -18682,7 +18676,7 @@
         <v>1355</v>
       </c>
       <c r="X8" t="s">
-        <v>2684</v>
+        <v>2682</v>
       </c>
       <c r="Z8" s="6" t="s">
         <v>1371</v>
@@ -18720,7 +18714,7 @@
         <v>1971</v>
       </c>
       <c r="AO8" s="6" t="s">
-        <v>2572</v>
+        <v>2570</v>
       </c>
       <c r="AS8" s="6" t="s">
         <v>1916</v>
@@ -18750,19 +18744,19 @@
         <v>1752</v>
       </c>
       <c r="BH8" s="10" t="s">
-        <v>2586</v>
+        <v>2584</v>
       </c>
       <c r="BI8" s="10" t="s">
-        <v>2591</v>
+        <v>2589</v>
       </c>
       <c r="BJ8" s="10" t="s">
         <v>2038</v>
       </c>
       <c r="BK8" s="10" t="s">
-        <v>2831</v>
+        <v>2829</v>
       </c>
       <c r="BL8" s="10" t="s">
-        <v>2831</v>
+        <v>2829</v>
       </c>
       <c r="BP8" s="17" t="s">
         <v>2039</v>
@@ -18771,10 +18765,10 @@
         <v>2070</v>
       </c>
       <c r="BR8" s="54" t="s">
-        <v>2603</v>
+        <v>2601</v>
       </c>
       <c r="BS8" s="54" t="s">
-        <v>2610</v>
+        <v>2608</v>
       </c>
       <c r="BT8" s="43"/>
       <c r="BU8" s="54"/>
@@ -18786,38 +18780,38 @@
         <v>2047</v>
       </c>
       <c r="BY8" s="20" t="s">
-        <v>2623</v>
+        <v>2621</v>
       </c>
       <c r="BZ8" s="20" t="s">
-        <v>2632</v>
+        <v>2630</v>
       </c>
       <c r="CA8" s="44" t="s">
         <v>2230</v>
       </c>
       <c r="CB8" s="20" t="s">
-        <v>2646</v>
+        <v>2644</v>
       </c>
       <c r="CC8" s="20" t="s">
-        <v>2653</v>
+        <v>2651</v>
       </c>
       <c r="CD8" s="20" t="s">
         <v>2249</v>
       </c>
       <c r="CE8" s="20" t="s">
-        <v>2661</v>
+        <v>2659</v>
       </c>
       <c r="CF8" s="20" t="s">
-        <v>2671</v>
+        <v>2669</v>
       </c>
       <c r="CG8" s="20" t="str">
         <f>_xlfn.CONCAT(CG7,"_error")</f>
         <v>DIC_flux_mmol_m2_d_error</v>
       </c>
       <c r="CH8" s="20" t="s">
-        <v>2575</v>
+        <v>2573</v>
       </c>
       <c r="CI8" s="20" t="s">
-        <v>2822</v>
+        <v>2820</v>
       </c>
       <c r="CJ8" s="14" t="s">
         <v>2144</v>
@@ -18832,7 +18826,7 @@
         <v>2257</v>
       </c>
       <c r="CN8" s="10" t="s">
-        <v>2914</v>
+        <v>2912</v>
       </c>
       <c r="CO8" s="13" t="s">
         <v>2280</v>
@@ -18850,7 +18844,7 @@
         <v>2304</v>
       </c>
       <c r="CT8" s="12" t="s">
-        <v>2543</v>
+        <v>2541</v>
       </c>
       <c r="CU8" s="12"/>
       <c r="CV8" s="12" t="s">
@@ -18866,7 +18860,7 @@
         <v>2341</v>
       </c>
       <c r="CZ8" s="12" t="s">
-        <v>2864</v>
+        <v>2862</v>
       </c>
       <c r="DA8" s="73" t="s">
         <v>2498</v>
@@ -18935,19 +18929,19 @@
         <v>2248</v>
       </c>
       <c r="EE8" s="20" t="s">
-        <v>2661</v>
+        <v>2659</v>
       </c>
       <c r="EF8" s="20" t="s">
-        <v>2942</v>
+        <v>2940</v>
       </c>
       <c r="EY8" s="10" t="s">
         <v>2038</v>
       </c>
       <c r="EZ8" s="10" t="s">
-        <v>2831</v>
+        <v>2829</v>
       </c>
       <c r="FA8" s="10" t="s">
-        <v>2831</v>
+        <v>2829</v>
       </c>
       <c r="FB8" s="85"/>
       <c r="FC8" s="85"/>
@@ -18956,19 +18950,19 @@
         <v>2039</v>
       </c>
       <c r="FT8" s="85" t="s">
-        <v>3007</v>
+        <v>3005</v>
       </c>
       <c r="FV8" t="s">
-        <v>2979</v>
+        <v>2977</v>
       </c>
       <c r="FX8" s="85" t="s">
-        <v>2975</v>
+        <v>2973</v>
       </c>
       <c r="GY8" s="85" t="s">
-        <v>2988</v>
+        <v>2986</v>
       </c>
       <c r="GZ8" s="85" t="s">
-        <v>2988</v>
+        <v>2986</v>
       </c>
       <c r="HA8" s="85" t="s">
         <v>2039</v>
@@ -19021,7 +19015,7 @@
         <v>1351</v>
       </c>
       <c r="X9" t="s">
-        <v>2685</v>
+        <v>2683</v>
       </c>
       <c r="Z9" s="6" t="s">
         <v>1372</v>
@@ -19089,16 +19083,16 @@
         <v>2282</v>
       </c>
       <c r="BI9" s="10" t="s">
-        <v>2593</v>
+        <v>2591</v>
       </c>
       <c r="BJ9" s="10" t="s">
         <v>2036</v>
       </c>
       <c r="BK9" s="10" t="s">
-        <v>2940</v>
+        <v>2938</v>
       </c>
       <c r="BL9" s="10" t="s">
-        <v>2939</v>
+        <v>2937</v>
       </c>
       <c r="BP9" s="17" t="s">
         <v>2029</v>
@@ -19107,10 +19101,10 @@
         <v>2071</v>
       </c>
       <c r="BR9" s="54" t="s">
-        <v>2603</v>
+        <v>2601</v>
       </c>
       <c r="BS9" s="54" t="s">
-        <v>2611</v>
+        <v>2609</v>
       </c>
       <c r="BT9" s="43"/>
       <c r="BU9" s="54"/>
@@ -19122,37 +19116,37 @@
         <v>1760</v>
       </c>
       <c r="BY9" s="20" t="s">
-        <v>2622</v>
+        <v>2620</v>
       </c>
       <c r="BZ9" s="20" t="s">
-        <v>2633</v>
+        <v>2631</v>
       </c>
       <c r="CA9" s="44" t="s">
         <v>2231</v>
       </c>
       <c r="CB9" s="20" t="s">
-        <v>2646</v>
+        <v>2644</v>
       </c>
       <c r="CC9" s="20" t="s">
-        <v>2654</v>
+        <v>2652</v>
       </c>
       <c r="CD9" s="20" t="s">
-        <v>2906</v>
+        <v>2904</v>
       </c>
       <c r="CE9" s="20" t="s">
-        <v>2661</v>
+        <v>2659</v>
       </c>
       <c r="CF9" s="20" t="s">
-        <v>2907</v>
+        <v>2905</v>
       </c>
       <c r="CG9" s="20" t="s">
         <v>2239</v>
       </c>
       <c r="CH9" s="20" t="s">
-        <v>2575</v>
+        <v>2573</v>
       </c>
       <c r="CI9" s="20" t="s">
-        <v>2582</v>
+        <v>2580</v>
       </c>
       <c r="CJ9" s="14" t="s">
         <v>2101</v>
@@ -19167,13 +19161,13 @@
         <v>2253</v>
       </c>
       <c r="CN9" s="10" t="s">
-        <v>2915</v>
+        <v>2913</v>
       </c>
       <c r="CO9" s="13" t="s">
         <v>2280</v>
       </c>
       <c r="CP9" s="10" t="s">
-        <v>2916</v>
+        <v>2914</v>
       </c>
       <c r="CQ9" s="11" t="s">
         <v>2055</v>
@@ -19185,14 +19179,14 @@
         <v>2305</v>
       </c>
       <c r="CT9" s="12" t="s">
-        <v>2542</v>
+        <v>2540</v>
       </c>
       <c r="CU9" s="12"/>
       <c r="CV9" s="12" t="s">
-        <v>2546</v>
+        <v>2544</v>
       </c>
       <c r="CZ9" s="12" t="s">
-        <v>2865</v>
+        <v>2863</v>
       </c>
       <c r="DA9" s="73" t="s">
         <v>2498</v>
@@ -19207,7 +19201,7 @@
         <v>2320</v>
       </c>
       <c r="DE9" s="45" t="s">
-        <v>2949</v>
+        <v>2947</v>
       </c>
       <c r="DF9" s="12" t="s">
         <v>1802</v>
@@ -19216,13 +19210,13 @@
         <v>2334</v>
       </c>
       <c r="DI9" s="12" t="s">
-        <v>2700</v>
+        <v>2698</v>
       </c>
       <c r="DJ9" s="61" t="s">
         <v>2334</v>
       </c>
       <c r="DK9" s="12" t="s">
-        <v>2701</v>
+        <v>2699</v>
       </c>
       <c r="DL9" s="36" t="s">
         <v>2109</v>
@@ -19261,19 +19255,19 @@
         <v>2249</v>
       </c>
       <c r="EE9" s="20" t="s">
-        <v>2661</v>
+        <v>2659</v>
       </c>
       <c r="EF9" s="20" t="s">
-        <v>2943</v>
+        <v>2941</v>
       </c>
       <c r="EY9" s="10" t="s">
         <v>2036</v>
       </c>
       <c r="EZ9" s="10" t="s">
-        <v>2940</v>
+        <v>2938</v>
       </c>
       <c r="FA9" s="10" t="s">
-        <v>2939</v>
+        <v>2937</v>
       </c>
       <c r="FB9" s="85"/>
       <c r="FC9" s="85"/>
@@ -19282,13 +19276,13 @@
         <v>2029</v>
       </c>
       <c r="FT9" t="s">
-        <v>3001</v>
+        <v>2999</v>
       </c>
       <c r="GY9" t="s">
-        <v>2989</v>
+        <v>2987</v>
       </c>
       <c r="GZ9" s="85" t="s">
-        <v>2989</v>
+        <v>2987</v>
       </c>
       <c r="HA9" s="85" t="s">
         <v>2029</v>
@@ -19401,7 +19395,7 @@
         <v>2282</v>
       </c>
       <c r="BI10" s="10" t="s">
-        <v>2594</v>
+        <v>2592</v>
       </c>
       <c r="BJ10" s="10" t="s">
         <v>2031</v>
@@ -19414,10 +19408,10 @@
         <v>2072</v>
       </c>
       <c r="BR10" s="54" t="s">
-        <v>2603</v>
+        <v>2601</v>
       </c>
       <c r="BS10" s="54" t="s">
-        <v>2612</v>
+        <v>2610</v>
       </c>
       <c r="BT10" s="43"/>
       <c r="BU10" s="54"/>
@@ -19429,38 +19423,38 @@
         <v>1775</v>
       </c>
       <c r="BY10" s="20" t="s">
-        <v>2622</v>
+        <v>2620</v>
       </c>
       <c r="BZ10" s="20" t="s">
-        <v>2634</v>
+        <v>2632</v>
       </c>
       <c r="CA10" s="44" t="s">
         <v>2232</v>
       </c>
       <c r="CB10" s="20" t="s">
-        <v>2646</v>
+        <v>2644</v>
       </c>
       <c r="CC10" s="20" t="s">
-        <v>2655</v>
+        <v>2653</v>
       </c>
       <c r="CD10" s="20" t="s">
-        <v>2908</v>
+        <v>2906</v>
       </c>
       <c r="CE10" s="20" t="s">
-        <v>2661</v>
+        <v>2659</v>
       </c>
       <c r="CF10" s="20" t="s">
-        <v>2909</v>
+        <v>2907</v>
       </c>
       <c r="CG10" s="20" t="str">
         <f>_xlfn.CONCAT(CG9,"_error")</f>
         <v>NH4_flux_mmol_m2_d_error</v>
       </c>
       <c r="CH10" s="20" t="s">
-        <v>2575</v>
+        <v>2573</v>
       </c>
       <c r="CI10" s="20" t="s">
-        <v>2823</v>
+        <v>2821</v>
       </c>
       <c r="CJ10" s="14" t="s">
         <v>2112</v>
@@ -19496,7 +19490,7 @@
       <c r="CU10" s="68"/>
       <c r="CV10" s="68"/>
       <c r="CZ10" s="12" t="s">
-        <v>2866</v>
+        <v>2864</v>
       </c>
       <c r="DA10" s="73" t="s">
         <v>2498</v>
@@ -19556,13 +19550,13 @@
       <c r="EB10" s="12"/>
       <c r="EC10" s="12"/>
       <c r="ED10" s="20" t="s">
-        <v>2906</v>
+        <v>2904</v>
       </c>
       <c r="EE10" s="20" t="s">
-        <v>2661</v>
+        <v>2659</v>
       </c>
       <c r="EF10" s="20" t="s">
-        <v>2944</v>
+        <v>2942</v>
       </c>
       <c r="EY10" s="10" t="s">
         <v>2031</v>
@@ -19576,10 +19570,10 @@
         <v>2216</v>
       </c>
       <c r="GY10" t="s">
-        <v>2990</v>
+        <v>2988</v>
       </c>
       <c r="GZ10" s="85" t="s">
-        <v>2990</v>
+        <v>2988</v>
       </c>
       <c r="HA10" s="85" t="s">
         <v>2216</v>
@@ -19688,7 +19682,7 @@
         <v>1757</v>
       </c>
       <c r="BI11" s="10" t="s">
-        <v>2595</v>
+        <v>2593</v>
       </c>
       <c r="BJ11" s="10" t="s">
         <v>2259</v>
@@ -19702,10 +19696,10 @@
         <v>2073</v>
       </c>
       <c r="BR11" s="54" t="s">
-        <v>2603</v>
+        <v>2601</v>
       </c>
       <c r="BS11" s="54" t="s">
-        <v>2613</v>
+        <v>2611</v>
       </c>
       <c r="BT11" s="43"/>
       <c r="BU11" s="54"/>
@@ -19714,46 +19708,46 @@
         <v>2208</v>
       </c>
       <c r="BX11" s="20" t="s">
-        <v>2625</v>
+        <v>2623</v>
       </c>
       <c r="BY11" s="20" t="s">
-        <v>2574</v>
+        <v>2572</v>
       </c>
       <c r="BZ11" s="20" t="s">
-        <v>2635</v>
+        <v>2633</v>
       </c>
       <c r="CA11" s="44" t="s">
         <v>2233</v>
       </c>
       <c r="CB11" s="20" t="s">
-        <v>2646</v>
+        <v>2644</v>
       </c>
       <c r="CC11" s="20" t="s">
-        <v>2656</v>
+        <v>2654</v>
       </c>
       <c r="CD11" s="20" t="s">
-        <v>2910</v>
+        <v>2908</v>
       </c>
       <c r="CE11" s="20" t="s">
-        <v>2661</v>
+        <v>2659</v>
       </c>
       <c r="CF11" s="20" t="s">
-        <v>2911</v>
+        <v>2909</v>
       </c>
       <c r="CG11" s="20" t="s">
         <v>2240</v>
       </c>
       <c r="CH11" s="20" t="s">
-        <v>2575</v>
+        <v>2573</v>
       </c>
       <c r="CI11" s="20" t="s">
-        <v>2581</v>
+        <v>2579</v>
       </c>
       <c r="CJ11" s="14" t="s">
         <v>2449</v>
       </c>
       <c r="CK11" s="20" t="s">
-        <v>2559</v>
+        <v>2557</v>
       </c>
       <c r="CL11" s="20">
         <v>10</v>
@@ -19783,7 +19777,7 @@
       <c r="CU11" s="68"/>
       <c r="CV11" s="68"/>
       <c r="CZ11" s="12" t="s">
-        <v>2867</v>
+        <v>2865</v>
       </c>
       <c r="DA11" s="73" t="s">
         <v>2498</v>
@@ -19807,13 +19801,13 @@
         <v>2334</v>
       </c>
       <c r="DI11" s="12" t="s">
-        <v>2702</v>
+        <v>2700</v>
       </c>
       <c r="DJ11" s="61" t="s">
         <v>2334</v>
       </c>
       <c r="DK11" s="12" t="s">
-        <v>2703</v>
+        <v>2701</v>
       </c>
       <c r="DL11" s="12" t="s">
         <v>2110</v>
@@ -19841,13 +19835,13 @@
       <c r="EB11" s="12"/>
       <c r="EC11" s="12"/>
       <c r="ED11" s="20" t="s">
-        <v>2908</v>
+        <v>2906</v>
       </c>
       <c r="EE11" s="20" t="s">
-        <v>2661</v>
+        <v>2659</v>
       </c>
       <c r="EF11" s="20" t="s">
-        <v>2945</v>
+        <v>2943</v>
       </c>
       <c r="EY11" s="10" t="s">
         <v>2259</v>
@@ -19927,7 +19921,7 @@
       </c>
       <c r="AG12" s="17"/>
       <c r="AI12" s="69" t="s">
-        <v>2814</v>
+        <v>2812</v>
       </c>
       <c r="AJ12" s="6" t="s">
         <v>1461</v>
@@ -19964,7 +19958,7 @@
       </c>
       <c r="BD12" s="17"/>
       <c r="BJ12" s="10" t="s">
-        <v>2879</v>
+        <v>2877</v>
       </c>
       <c r="BK12" s="10"/>
       <c r="BP12" s="17" t="s">
@@ -19974,10 +19968,10 @@
         <v>2074</v>
       </c>
       <c r="BR12" s="54" t="s">
-        <v>2603</v>
+        <v>2601</v>
       </c>
       <c r="BS12" s="54" t="s">
-        <v>2614</v>
+        <v>2612</v>
       </c>
       <c r="BT12" s="43"/>
       <c r="BU12" s="54"/>
@@ -19989,38 +19983,38 @@
         <v>1761</v>
       </c>
       <c r="BY12" s="20" t="s">
-        <v>2622</v>
+        <v>2620</v>
       </c>
       <c r="BZ12" s="20" t="s">
-        <v>2636</v>
+        <v>2634</v>
       </c>
       <c r="CA12" s="44" t="s">
         <v>2234</v>
       </c>
       <c r="CB12" s="20" t="s">
-        <v>2646</v>
+        <v>2644</v>
       </c>
       <c r="CC12" s="20" t="s">
-        <v>2657</v>
+        <v>2655</v>
       </c>
       <c r="CD12" s="20" t="s">
+        <v>2873</v>
+      </c>
+      <c r="CE12" s="20" t="s">
+        <v>2874</v>
+      </c>
+      <c r="CF12" s="20" t="s">
         <v>2875</v>
-      </c>
-      <c r="CE12" s="20" t="s">
-        <v>2876</v>
-      </c>
-      <c r="CF12" s="20" t="s">
-        <v>2877</v>
       </c>
       <c r="CG12" s="20" t="str">
         <f>_xlfn.CONCAT(CG11,"_error")</f>
         <v>Fe_flux_mmol_m2_d_error</v>
       </c>
       <c r="CH12" s="20" t="s">
-        <v>2575</v>
+        <v>2573</v>
       </c>
       <c r="CI12" s="20" t="s">
-        <v>2824</v>
+        <v>2822</v>
       </c>
       <c r="CJ12" s="14" t="s">
         <v>2457</v>
@@ -20035,13 +20029,13 @@
         <v>2265</v>
       </c>
       <c r="CN12" s="10" t="s">
-        <v>2839</v>
+        <v>2837</v>
       </c>
       <c r="CO12" s="13" t="s">
         <v>2281</v>
       </c>
       <c r="CP12" s="10" t="s">
-        <v>2840</v>
+        <v>2838</v>
       </c>
       <c r="CQ12" s="11" t="s">
         <v>2056</v>
@@ -20056,7 +20050,7 @@
       <c r="CU12" s="68"/>
       <c r="CV12" s="68"/>
       <c r="CZ12" s="12" t="s">
-        <v>2868</v>
+        <v>2866</v>
       </c>
       <c r="DA12" s="73" t="s">
         <v>2498</v>
@@ -20107,16 +20101,16 @@
       <c r="EB12" s="12"/>
       <c r="EC12" s="12"/>
       <c r="ED12" s="20" t="s">
-        <v>2910</v>
+        <v>2908</v>
       </c>
       <c r="EE12" s="20" t="s">
-        <v>2661</v>
+        <v>2659</v>
       </c>
       <c r="EF12" s="20" t="s">
-        <v>2946</v>
+        <v>2944</v>
       </c>
       <c r="EY12" s="10" t="s">
-        <v>2879</v>
+        <v>2877</v>
       </c>
       <c r="EZ12" s="10"/>
       <c r="FA12" s="85"/>
@@ -20156,7 +20150,7 @@
         <v>127</v>
       </c>
       <c r="J13" t="s">
-        <v>2938</v>
+        <v>2936</v>
       </c>
       <c r="K13" s="35" t="s">
         <v>2089</v>
@@ -20175,7 +20169,7 @@
       </c>
       <c r="U13" s="6"/>
       <c r="V13" s="82" t="s">
-        <v>2937</v>
+        <v>2935</v>
       </c>
       <c r="AB13" s="6" t="s">
         <v>1387</v>
@@ -20233,10 +20227,10 @@
         <v>2075</v>
       </c>
       <c r="BR13" s="54" t="s">
-        <v>2603</v>
+        <v>2601</v>
       </c>
       <c r="BS13" s="54" t="s">
-        <v>2615</v>
+        <v>2613</v>
       </c>
       <c r="BT13" s="43"/>
       <c r="BU13" s="54"/>
@@ -20248,34 +20242,34 @@
         <v>2042</v>
       </c>
       <c r="BY13" s="20" t="s">
-        <v>2622</v>
+        <v>2620</v>
       </c>
       <c r="BZ13" s="20" t="s">
-        <v>2637</v>
+        <v>2635</v>
       </c>
       <c r="CA13" s="44" t="s">
         <v>2235</v>
       </c>
       <c r="CB13" s="20" t="s">
-        <v>2646</v>
+        <v>2644</v>
       </c>
       <c r="CC13" s="20" t="s">
-        <v>2658</v>
+        <v>2656</v>
       </c>
       <c r="CG13" s="20" t="s">
         <v>2241</v>
       </c>
       <c r="CH13" s="20" t="s">
-        <v>2575</v>
+        <v>2573</v>
       </c>
       <c r="CI13" s="20" t="s">
-        <v>2580</v>
+        <v>2578</v>
       </c>
       <c r="CJ13" s="14" t="s">
         <v>2530</v>
       </c>
       <c r="CK13" s="20" t="s">
-        <v>2561</v>
+        <v>2559</v>
       </c>
       <c r="CL13" s="20">
         <v>12</v>
@@ -20284,13 +20278,13 @@
         <v>2266</v>
       </c>
       <c r="CN13" s="10" t="s">
-        <v>2852</v>
+        <v>2850</v>
       </c>
       <c r="CO13" s="13" t="s">
         <v>2281</v>
       </c>
       <c r="CP13" s="10" t="s">
-        <v>2853</v>
+        <v>2851</v>
       </c>
       <c r="CQ13" s="11" t="s">
         <v>2057</v>
@@ -20305,7 +20299,7 @@
       <c r="CU13" s="68"/>
       <c r="CV13" s="68"/>
       <c r="CZ13" s="12" t="s">
-        <v>2869</v>
+        <v>2867</v>
       </c>
       <c r="DA13" s="73" t="s">
         <v>2498</v>
@@ -20329,13 +20323,13 @@
         <v>2334</v>
       </c>
       <c r="DI13" s="12" t="s">
-        <v>2704</v>
+        <v>2702</v>
       </c>
       <c r="DJ13" s="61" t="s">
         <v>2334</v>
       </c>
       <c r="DK13" s="12" t="s">
-        <v>2705</v>
+        <v>2703</v>
       </c>
       <c r="DO13" s="37" t="s">
         <v>2126</v>
@@ -20353,13 +20347,13 @@
         <v>2469</v>
       </c>
       <c r="ED13" s="20" t="s">
-        <v>2875</v>
+        <v>2873</v>
       </c>
       <c r="EE13" s="20" t="s">
-        <v>2876</v>
+        <v>2874</v>
       </c>
       <c r="EF13" s="20" t="s">
-        <v>2947</v>
+        <v>2945</v>
       </c>
       <c r="EY13" s="10"/>
       <c r="EZ13" s="10"/>
@@ -20400,7 +20394,7 @@
         <v>135</v>
       </c>
       <c r="K14" s="76" t="s">
-        <v>2912</v>
+        <v>2910</v>
       </c>
       <c r="L14" t="s">
         <v>136</v>
@@ -20416,7 +20410,7 @@
       </c>
       <c r="U14" s="6"/>
       <c r="V14" s="67" t="s">
-        <v>2805</v>
+        <v>2803</v>
       </c>
       <c r="AB14" s="6" t="s">
         <v>1394</v>
@@ -20471,29 +20465,29 @@
         <v>1762</v>
       </c>
       <c r="BY14" s="20" t="s">
-        <v>2574</v>
+        <v>2572</v>
       </c>
       <c r="BZ14" s="20" t="s">
-        <v>2638</v>
+        <v>2636</v>
       </c>
       <c r="CA14" s="10" t="s">
+        <v>2844</v>
+      </c>
+      <c r="CB14" s="20" t="s">
+        <v>2644</v>
+      </c>
+      <c r="CC14" s="20" t="s">
         <v>2846</v>
-      </c>
-      <c r="CB14" s="20" t="s">
-        <v>2646</v>
-      </c>
-      <c r="CC14" s="20" t="s">
-        <v>2848</v>
       </c>
       <c r="CG14" s="20" t="str">
         <f>_xlfn.CONCAT(CG13,"_error")</f>
         <v>Mn_flux_mmol_m2_d_error</v>
       </c>
       <c r="CH14" s="20" t="s">
-        <v>2575</v>
+        <v>2573</v>
       </c>
       <c r="CI14" s="20" t="s">
-        <v>2825</v>
+        <v>2823</v>
       </c>
       <c r="CJ14" s="14" t="s">
         <v>2140</v>
@@ -20508,13 +20502,13 @@
         <v>2267</v>
       </c>
       <c r="CN14" s="20" t="s">
-        <v>2917</v>
+        <v>2915</v>
       </c>
       <c r="CO14" s="13" t="s">
         <v>2281</v>
       </c>
       <c r="CP14" s="20" t="s">
-        <v>2918</v>
+        <v>2916</v>
       </c>
       <c r="CQ14" s="11" t="s">
         <v>2058</v>
@@ -20529,13 +20523,13 @@
       <c r="CU14" s="68"/>
       <c r="CV14" s="68"/>
       <c r="CZ14" s="12" t="s">
-        <v>2856</v>
+        <v>2854</v>
       </c>
       <c r="DA14" s="73" t="s">
         <v>2498</v>
       </c>
       <c r="DB14" s="12" t="s">
-        <v>2870</v>
+        <v>2868</v>
       </c>
       <c r="DC14" s="12" t="s">
         <v>1791</v>
@@ -20674,34 +20668,34 @@
         <v>1764</v>
       </c>
       <c r="BY15" s="20" t="s">
-        <v>2623</v>
+        <v>2621</v>
       </c>
       <c r="BZ15" s="20" t="s">
-        <v>2639</v>
+        <v>2637</v>
       </c>
       <c r="CA15" s="10" t="s">
-        <v>2850</v>
+        <v>2848</v>
       </c>
       <c r="CB15" s="20" t="s">
-        <v>2646</v>
+        <v>2644</v>
       </c>
       <c r="CC15" s="20" t="s">
-        <v>2849</v>
+        <v>2847</v>
       </c>
       <c r="CG15" s="20" t="s">
         <v>2242</v>
       </c>
       <c r="CH15" s="20" t="s">
-        <v>2575</v>
+        <v>2573</v>
       </c>
       <c r="CI15" s="20" t="s">
-        <v>2579</v>
+        <v>2577</v>
       </c>
       <c r="CJ15" s="14" t="s">
         <v>2527</v>
       </c>
       <c r="CK15" s="20" t="s">
-        <v>2560</v>
+        <v>2558</v>
       </c>
       <c r="CL15" s="20">
         <v>14</v>
@@ -20731,13 +20725,13 @@
       <c r="CU15" s="68"/>
       <c r="CV15" s="68"/>
       <c r="CZ15" s="12" t="s">
-        <v>2857</v>
+        <v>2855</v>
       </c>
       <c r="DA15" s="73" t="s">
         <v>2498</v>
       </c>
       <c r="DB15" s="12" t="s">
-        <v>2871</v>
+        <v>2869</v>
       </c>
       <c r="DC15" s="12" t="s">
         <v>1792</v>
@@ -20755,13 +20749,13 @@
         <v>2334</v>
       </c>
       <c r="DI15" s="12" t="s">
-        <v>2706</v>
+        <v>2704</v>
       </c>
       <c r="DJ15" s="61" t="s">
         <v>2334</v>
       </c>
       <c r="DK15" s="12" t="s">
-        <v>2707</v>
+        <v>2705</v>
       </c>
       <c r="DL15" s="45"/>
       <c r="DO15" s="37" t="s">
@@ -20786,10 +20780,10 @@
       <c r="EE15" s="46"/>
       <c r="EF15" s="46"/>
       <c r="GY15" t="s">
-        <v>2991</v>
+        <v>2989</v>
       </c>
       <c r="GZ15" s="85" t="s">
-        <v>2992</v>
+        <v>2990</v>
       </c>
     </row>
     <row r="16" spans="1:220" x14ac:dyDescent="0.3">
@@ -20873,29 +20867,29 @@
         <v>1763</v>
       </c>
       <c r="BY16" s="20" t="s">
-        <v>2623</v>
+        <v>2621</v>
       </c>
       <c r="BZ16" s="20" t="s">
-        <v>2640</v>
+        <v>2638</v>
       </c>
       <c r="CA16" s="44" t="s">
         <v>2236</v>
       </c>
       <c r="CB16" s="20" t="s">
-        <v>2646</v>
+        <v>2644</v>
       </c>
       <c r="CC16" s="20" t="s">
-        <v>2659</v>
+        <v>2657</v>
       </c>
       <c r="CG16" s="20" t="str">
         <f>_xlfn.CONCAT(CG15,"_error")</f>
         <v>SO4_flux_mmol_m2_d_error</v>
       </c>
       <c r="CH16" s="20" t="s">
-        <v>2575</v>
+        <v>2573</v>
       </c>
       <c r="CI16" s="20" t="s">
-        <v>2826</v>
+        <v>2824</v>
       </c>
       <c r="CJ16" s="14" t="s">
         <v>2270</v>
@@ -20931,10 +20925,10 @@
       <c r="CU16" s="68"/>
       <c r="CV16" s="68"/>
       <c r="CZ16" s="12" t="s">
-        <v>2878</v>
+        <v>2876</v>
       </c>
       <c r="DB16" s="12" t="s">
-        <v>2872</v>
+        <v>2870</v>
       </c>
       <c r="DC16" s="12" t="s">
         <v>1793</v>
@@ -21067,40 +21061,40 @@
         <v>1765</v>
       </c>
       <c r="BY17" s="10" t="s">
-        <v>2623</v>
+        <v>2621</v>
       </c>
       <c r="BZ17" s="20" t="s">
-        <v>2641</v>
+        <v>2639</v>
       </c>
       <c r="CA17" s="44" t="s">
         <v>2237</v>
       </c>
       <c r="CB17" s="20" t="s">
-        <v>2646</v>
+        <v>2644</v>
       </c>
       <c r="CC17" s="20" t="s">
-        <v>2660</v>
+        <v>2658</v>
       </c>
       <c r="CG17" s="20" t="s">
         <v>2243</v>
       </c>
       <c r="CH17" s="20" t="s">
-        <v>2575</v>
+        <v>2573</v>
       </c>
       <c r="CI17" s="20" t="s">
-        <v>2578</v>
+        <v>2576</v>
       </c>
       <c r="CJ17" s="14" t="s">
-        <v>2689</v>
+        <v>2687</v>
       </c>
       <c r="CK17" s="20" t="s">
-        <v>2883</v>
+        <v>2881</v>
       </c>
       <c r="CL17" s="20">
         <v>16</v>
       </c>
       <c r="CM17" s="14" t="s">
-        <v>2923</v>
+        <v>2921</v>
       </c>
       <c r="CN17" s="10" t="s">
         <v>2100</v>
@@ -21139,13 +21133,13 @@
         <v>2334</v>
       </c>
       <c r="DI17" s="12" t="s">
-        <v>2708</v>
+        <v>2706</v>
       </c>
       <c r="DJ17" s="61" t="s">
         <v>2334</v>
       </c>
       <c r="DK17" s="12" t="s">
-        <v>2709</v>
+        <v>2707</v>
       </c>
       <c r="DL17" s="45"/>
       <c r="DO17" s="37" t="s">
@@ -21170,10 +21164,10 @@
       <c r="EE17" s="46"/>
       <c r="EF17" s="46"/>
       <c r="GY17" s="10" t="s">
-        <v>2879</v>
+        <v>2877</v>
       </c>
       <c r="GZ17" s="10" t="s">
-        <v>2879</v>
+        <v>2877</v>
       </c>
     </row>
     <row r="18" spans="2:208" x14ac:dyDescent="0.3">
@@ -21254,10 +21248,10 @@
         <v>1766</v>
       </c>
       <c r="BY18" s="10" t="s">
-        <v>2574</v>
+        <v>2572</v>
       </c>
       <c r="BZ18" s="20" t="s">
-        <v>2642</v>
+        <v>2640</v>
       </c>
       <c r="CA18" s="10"/>
       <c r="CB18" s="10"/>
@@ -21267,22 +21261,22 @@
         <v>PO4_flux_mmol_m2_d_error</v>
       </c>
       <c r="CH18" s="20" t="s">
-        <v>2575</v>
+        <v>2573</v>
       </c>
       <c r="CI18" s="20" t="s">
-        <v>2827</v>
+        <v>2825</v>
       </c>
       <c r="CJ18" s="14" t="s">
-        <v>2885</v>
+        <v>2883</v>
       </c>
       <c r="CK18" s="20" t="s">
-        <v>2886</v>
+        <v>2884</v>
       </c>
       <c r="CL18" s="20">
         <v>17</v>
       </c>
       <c r="CM18" s="14" t="s">
-        <v>2924</v>
+        <v>2922</v>
       </c>
       <c r="CN18" s="10" t="s">
         <v>2139</v>
@@ -21304,13 +21298,13 @@
       <c r="CU18" s="11"/>
       <c r="CV18" s="11"/>
       <c r="DC18" s="12" t="s">
-        <v>2951</v>
+        <v>2949</v>
       </c>
       <c r="DD18" s="84" t="s">
         <v>2320</v>
       </c>
       <c r="DE18" s="84" t="s">
-        <v>2948</v>
+        <v>2946</v>
       </c>
       <c r="DF18" s="12" t="s">
         <v>1805</v>
@@ -21425,10 +21419,10 @@
         <v>1814</v>
       </c>
       <c r="BY19" s="20" t="s">
-        <v>2622</v>
+        <v>2620</v>
       </c>
       <c r="BZ19" s="20" t="s">
-        <v>2643</v>
+        <v>2641</v>
       </c>
       <c r="CA19" s="10"/>
       <c r="CB19" s="10"/>
@@ -21437,22 +21431,22 @@
         <v>2244</v>
       </c>
       <c r="CH19" s="20" t="s">
-        <v>2575</v>
+        <v>2573</v>
       </c>
       <c r="CI19" s="20" t="s">
-        <v>2583</v>
+        <v>2581</v>
       </c>
       <c r="CJ19" s="14" t="s">
+        <v>2880</v>
+      </c>
+      <c r="CK19" s="20" t="s">
         <v>2882</v>
-      </c>
-      <c r="CK19" s="20" t="s">
-        <v>2884</v>
       </c>
       <c r="CL19" s="20">
         <v>18</v>
       </c>
       <c r="CM19" s="14" t="s">
-        <v>2925</v>
+        <v>2923</v>
       </c>
       <c r="CN19" s="10" t="s">
         <v>2260</v>
@@ -21473,13 +21467,13 @@
       <c r="CU19" s="11"/>
       <c r="CV19" s="11"/>
       <c r="DC19" s="12" t="s">
-        <v>2952</v>
+        <v>2950</v>
       </c>
       <c r="DD19" s="84" t="s">
         <v>2320</v>
       </c>
       <c r="DE19" s="84" t="s">
-        <v>2950</v>
+        <v>2948</v>
       </c>
       <c r="DF19" s="12" t="s">
         <v>1806</v>
@@ -21488,13 +21482,13 @@
         <v>2334</v>
       </c>
       <c r="DI19" s="12" t="s">
-        <v>2710</v>
+        <v>2708</v>
       </c>
       <c r="DJ19" s="61" t="s">
         <v>2334</v>
       </c>
       <c r="DK19" s="12" t="s">
-        <v>2711</v>
+        <v>2709</v>
       </c>
       <c r="DL19" s="45"/>
       <c r="DO19" s="37" t="s">
@@ -21591,10 +21585,10 @@
         <v>1815</v>
       </c>
       <c r="BY20" s="20" t="s">
-        <v>2622</v>
+        <v>2620</v>
       </c>
       <c r="BZ20" s="20" t="s">
-        <v>2644</v>
+        <v>2642</v>
       </c>
       <c r="CA20" s="10"/>
       <c r="CB20" s="10"/>
@@ -21604,22 +21598,22 @@
         <v>NO3_flux_mmol_m2_d_error</v>
       </c>
       <c r="CH20" s="20" t="s">
-        <v>2575</v>
+        <v>2573</v>
       </c>
       <c r="CI20" s="20" t="s">
-        <v>2828</v>
+        <v>2826</v>
       </c>
       <c r="CJ20" s="14" t="s">
-        <v>2898</v>
+        <v>2896</v>
       </c>
       <c r="CK20" s="20" t="s">
-        <v>2905</v>
+        <v>2903</v>
       </c>
       <c r="CL20" s="20">
         <v>19</v>
       </c>
       <c r="CM20" s="14" t="s">
-        <v>2926</v>
+        <v>2924</v>
       </c>
       <c r="CQ20" s="11" t="s">
         <v>2423</v>
@@ -21736,10 +21730,10 @@
         <v>1767</v>
       </c>
       <c r="BY21" s="10" t="s">
-        <v>2574</v>
+        <v>2572</v>
       </c>
       <c r="BZ21" s="20" t="s">
-        <v>2645</v>
+        <v>2643</v>
       </c>
       <c r="CA21" s="10"/>
       <c r="CB21" s="10"/>
@@ -21748,19 +21742,19 @@
         <v>2245</v>
       </c>
       <c r="CH21" s="20" t="s">
-        <v>2575</v>
+        <v>2573</v>
       </c>
       <c r="CI21" s="20" t="s">
-        <v>2584</v>
+        <v>2582</v>
       </c>
       <c r="CJ21" s="14" t="s">
+        <v>2951</v>
+      </c>
+      <c r="CK21" s="20" t="s">
         <v>2953</v>
       </c>
-      <c r="CK21" s="20" t="s">
-        <v>2955</v>
-      </c>
       <c r="CM21" s="14" t="s">
-        <v>2927</v>
+        <v>2925</v>
       </c>
       <c r="CQ21" s="11" t="s">
         <v>2427</v>
@@ -21778,13 +21772,13 @@
         <v>2334</v>
       </c>
       <c r="DI21" s="12" t="s">
-        <v>2712</v>
+        <v>2710</v>
       </c>
       <c r="DJ21" s="61" t="s">
         <v>2334</v>
       </c>
       <c r="DK21" s="12" t="s">
-        <v>2713</v>
+        <v>2711</v>
       </c>
       <c r="DO21" s="37" t="s">
         <v>2136</v>
@@ -21856,22 +21850,22 @@
         <v>O2_flux_mmol_m2_d_error</v>
       </c>
       <c r="CH22" s="20" t="s">
-        <v>2575</v>
+        <v>2573</v>
       </c>
       <c r="CI22" s="20" t="s">
-        <v>2829</v>
+        <v>2827</v>
       </c>
       <c r="CJ22" s="14" t="s">
+        <v>2952</v>
+      </c>
+      <c r="CK22" s="20" t="s">
         <v>2954</v>
       </c>
-      <c r="CK22" s="20" t="s">
-        <v>2956</v>
-      </c>
       <c r="CM22" s="14" t="s">
-        <v>2928</v>
+        <v>2926</v>
       </c>
       <c r="CQ22" s="11" t="s">
-        <v>2672</v>
+        <v>2670</v>
       </c>
       <c r="CR22" s="10" t="s">
         <v>2280</v>
@@ -21960,10 +21954,10 @@
       <c r="CB23" s="10"/>
       <c r="CC23" s="10"/>
       <c r="CM23" s="14" t="s">
-        <v>2929</v>
+        <v>2927</v>
       </c>
       <c r="CQ23" s="11" t="s">
-        <v>2673</v>
+        <v>2671</v>
       </c>
       <c r="CR23" s="10" t="s">
         <v>2280</v>
@@ -21984,13 +21978,13 @@
         <v>2334</v>
       </c>
       <c r="DI23" s="12" t="s">
-        <v>2714</v>
+        <v>2712</v>
       </c>
       <c r="DJ23" s="61" t="s">
         <v>2334</v>
       </c>
       <c r="DK23" s="12" t="s">
-        <v>2715</v>
+        <v>2713</v>
       </c>
       <c r="DO23" s="46" t="s">
         <v>2448</v>
@@ -22054,10 +22048,10 @@
       </c>
       <c r="BD24" s="17"/>
       <c r="CM24" s="14" t="s">
-        <v>2930</v>
+        <v>2928</v>
       </c>
       <c r="CQ24" s="11" t="s">
-        <v>2674</v>
+        <v>2672</v>
       </c>
       <c r="CR24" s="10" t="s">
         <v>2280</v>
@@ -22121,7 +22115,7 @@
         <v>657</v>
       </c>
       <c r="Q25" s="18" t="s">
-        <v>2568</v>
+        <v>2566</v>
       </c>
       <c r="AC25" s="6" t="s">
         <v>1413</v>
@@ -22143,10 +22137,10 @@
       </c>
       <c r="BD25" s="17"/>
       <c r="CM25" s="14" t="s">
-        <v>2931</v>
+        <v>2929</v>
       </c>
       <c r="CQ25" s="11" t="s">
-        <v>2675</v>
+        <v>2673</v>
       </c>
       <c r="CR25" s="10" t="s">
         <v>2280</v>
@@ -22164,13 +22158,13 @@
         <v>2334</v>
       </c>
       <c r="DI25" s="12" t="s">
-        <v>2716</v>
+        <v>2714</v>
       </c>
       <c r="DJ25" s="61" t="s">
         <v>2334</v>
       </c>
       <c r="DK25" s="12" t="s">
-        <v>2717</v>
+        <v>2715</v>
       </c>
       <c r="DO25" s="37" t="s">
         <v>2116</v>
@@ -22231,7 +22225,7 @@
       </c>
       <c r="BD26" s="17"/>
       <c r="CM26" s="14" t="s">
-        <v>2932</v>
+        <v>2930</v>
       </c>
       <c r="CQ26" s="11" t="s">
         <v>1768</v>
@@ -22312,7 +22306,7 @@
         <v>1944</v>
       </c>
       <c r="CM27" s="14" t="s">
-        <v>2933</v>
+        <v>2931</v>
       </c>
       <c r="CQ27" s="11" t="s">
         <v>1778</v>
@@ -22330,13 +22324,13 @@
         <v>2430</v>
       </c>
       <c r="DI27" s="12" t="s">
-        <v>2718</v>
+        <v>2716</v>
       </c>
       <c r="DJ27" s="61" t="s">
         <v>2334</v>
       </c>
       <c r="DK27" s="12" t="s">
-        <v>2719</v>
+        <v>2717</v>
       </c>
       <c r="DO27" s="37" t="s">
         <v>2129</v>
@@ -22393,16 +22387,16 @@
         <v>1655</v>
       </c>
       <c r="CM28" s="14" t="s">
-        <v>2934</v>
+        <v>2932</v>
       </c>
       <c r="CQ28" s="11" t="s">
-        <v>2833</v>
+        <v>2831</v>
       </c>
       <c r="CR28" s="11" t="s">
         <v>2280</v>
       </c>
       <c r="CS28" s="11" t="s">
-        <v>2834</v>
+        <v>2832</v>
       </c>
       <c r="CT28" s="11"/>
       <c r="CU28" s="11"/>
@@ -22456,7 +22450,7 @@
         <v>856</v>
       </c>
       <c r="AC29" t="s">
-        <v>2681</v>
+        <v>2679</v>
       </c>
       <c r="AI29" s="6" t="s">
         <v>1964</v>
@@ -22471,15 +22465,11 @@
         <v>1678</v>
       </c>
       <c r="CM29" s="14" t="s">
-        <v>2935</v>
-      </c>
-      <c r="CQ29" s="20" t="s">
-        <v>2538</v>
-      </c>
+        <v>2933</v>
+      </c>
+      <c r="CQ29" s="20"/>
       <c r="CR29" s="14"/>
-      <c r="CS29" s="11" t="s">
-        <v>2539</v>
-      </c>
+      <c r="CS29" s="11"/>
       <c r="CT29" s="14"/>
       <c r="CU29" s="14"/>
       <c r="CV29" s="14"/>
@@ -22487,13 +22477,13 @@
         <v>2431</v>
       </c>
       <c r="DI29" s="12" t="s">
-        <v>2720</v>
+        <v>2718</v>
       </c>
       <c r="DJ29" s="61" t="s">
         <v>2334</v>
       </c>
       <c r="DK29" s="12" t="s">
-        <v>2721</v>
+        <v>2719</v>
       </c>
       <c r="DO29" s="37" t="s">
         <v>2138</v>
@@ -22611,13 +22601,13 @@
         <v>2432</v>
       </c>
       <c r="DI31" s="12" t="s">
-        <v>2722</v>
+        <v>2720</v>
       </c>
       <c r="DJ31" s="61" t="s">
         <v>2334</v>
       </c>
       <c r="DK31" s="12" t="s">
-        <v>2723</v>
+        <v>2721</v>
       </c>
       <c r="DO31" s="37" t="s">
         <v>2534</v>
@@ -22739,13 +22729,13 @@
       <c r="DG33" s="23"/>
       <c r="DH33" s="23"/>
       <c r="DI33" s="12" t="s">
-        <v>2724</v>
+        <v>2722</v>
       </c>
       <c r="DJ33" s="61" t="s">
         <v>2334</v>
       </c>
       <c r="DK33" s="12" t="s">
-        <v>2725</v>
+        <v>2723</v>
       </c>
     </row>
     <row r="34" spans="2:116" x14ac:dyDescent="0.3">
@@ -22854,13 +22844,13 @@
       <c r="DG35" s="23"/>
       <c r="DH35" s="23"/>
       <c r="DI35" s="12" t="s">
-        <v>2726</v>
+        <v>2724</v>
       </c>
       <c r="DJ35" s="61" t="s">
         <v>2334</v>
       </c>
       <c r="DK35" s="12" t="s">
-        <v>2727</v>
+        <v>2725</v>
       </c>
     </row>
     <row r="36" spans="2:116" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -22905,7 +22895,7 @@
       <c r="CU36" s="14"/>
       <c r="CV36" s="14"/>
       <c r="DF36" s="23" t="s">
-        <v>2873</v>
+        <v>2871</v>
       </c>
       <c r="DG36" s="23"/>
       <c r="DH36" s="23"/>
@@ -22962,18 +22952,18 @@
       <c r="CU37" s="14"/>
       <c r="CV37" s="14"/>
       <c r="DF37" s="23" t="s">
-        <v>2874</v>
+        <v>2872</v>
       </c>
       <c r="DG37" s="23"/>
       <c r="DH37" s="23"/>
       <c r="DI37" s="12" t="s">
-        <v>2728</v>
+        <v>2726</v>
       </c>
       <c r="DJ37" s="61" t="s">
         <v>2334</v>
       </c>
       <c r="DK37" s="12" t="s">
-        <v>2729</v>
+        <v>2727</v>
       </c>
     </row>
     <row r="38" spans="2:116" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -23073,13 +23063,13 @@
       <c r="CV39" s="14"/>
       <c r="DF39" s="23"/>
       <c r="DI39" s="12" t="s">
-        <v>2730</v>
+        <v>2728</v>
       </c>
       <c r="DJ39" s="61" t="s">
         <v>2334</v>
       </c>
       <c r="DK39" s="12" t="s">
-        <v>2731</v>
+        <v>2729</v>
       </c>
       <c r="DL39" s="45"/>
     </row>
@@ -23169,13 +23159,13 @@
         <v>1699</v>
       </c>
       <c r="DI41" s="12" t="s">
-        <v>2732</v>
+        <v>2730</v>
       </c>
       <c r="DJ41" s="61" t="s">
         <v>2334</v>
       </c>
       <c r="DK41" s="12" t="s">
-        <v>2733</v>
+        <v>2731</v>
       </c>
       <c r="DL41" s="45"/>
     </row>
@@ -23261,13 +23251,13 @@
         <v>1687</v>
       </c>
       <c r="DI43" s="12" t="s">
-        <v>2734</v>
+        <v>2732</v>
       </c>
       <c r="DJ43" s="61" t="s">
         <v>2334</v>
       </c>
       <c r="DK43" s="12" t="s">
-        <v>2735</v>
+        <v>2733</v>
       </c>
       <c r="DL43" s="45"/>
     </row>
@@ -23356,13 +23346,13 @@
       <c r="DG45" s="23"/>
       <c r="DH45" s="23"/>
       <c r="DI45" s="12" t="s">
-        <v>2736</v>
+        <v>2734</v>
       </c>
       <c r="DJ45" s="61" t="s">
         <v>2334</v>
       </c>
       <c r="DK45" s="12" t="s">
-        <v>2737</v>
+        <v>2735</v>
       </c>
       <c r="DL45" s="45"/>
     </row>
@@ -23449,13 +23439,13 @@
       <c r="DG47" s="23"/>
       <c r="DH47" s="23"/>
       <c r="DI47" s="12" t="s">
-        <v>2738</v>
+        <v>2736</v>
       </c>
       <c r="DJ47" s="61" t="s">
         <v>2334</v>
       </c>
       <c r="DK47" s="12" t="s">
-        <v>2739</v>
+        <v>2737</v>
       </c>
       <c r="DL47" s="45"/>
     </row>
@@ -23541,13 +23531,13 @@
       <c r="DG49" s="23"/>
       <c r="DH49" s="23"/>
       <c r="DI49" s="12" t="s">
-        <v>2740</v>
+        <v>2738</v>
       </c>
       <c r="DJ49" s="61" t="s">
         <v>2334</v>
       </c>
       <c r="DK49" s="12" t="s">
-        <v>2741</v>
+        <v>2739</v>
       </c>
       <c r="DL49" s="45"/>
     </row>
@@ -23635,13 +23625,13 @@
       <c r="DG51" s="23"/>
       <c r="DH51" s="23"/>
       <c r="DI51" s="12" t="s">
-        <v>2742</v>
+        <v>2740</v>
       </c>
       <c r="DJ51" s="61" t="s">
         <v>2334</v>
       </c>
       <c r="DK51" s="12" t="s">
-        <v>2743</v>
+        <v>2741</v>
       </c>
       <c r="DL51" s="45"/>
     </row>
@@ -23728,13 +23718,13 @@
       <c r="DG53" s="23"/>
       <c r="DH53" s="23"/>
       <c r="DI53" s="12" t="s">
-        <v>2744</v>
+        <v>2742</v>
       </c>
       <c r="DJ53" s="61" t="s">
         <v>2334</v>
       </c>
       <c r="DK53" s="12" t="s">
-        <v>2745</v>
+        <v>2743</v>
       </c>
       <c r="DL53" s="45"/>
     </row>
@@ -23818,13 +23808,13 @@
       </c>
       <c r="DF55" s="23"/>
       <c r="DI55" s="12" t="s">
-        <v>2746</v>
+        <v>2744</v>
       </c>
       <c r="DJ55" s="61" t="s">
         <v>2334</v>
       </c>
       <c r="DK55" s="12" t="s">
-        <v>2747</v>
+        <v>2745</v>
       </c>
       <c r="DL55" s="45"/>
     </row>
@@ -23907,13 +23897,13 @@
         <v>1682</v>
       </c>
       <c r="DI57" s="12" t="s">
-        <v>2748</v>
+        <v>2746</v>
       </c>
       <c r="DJ57" s="61" t="s">
         <v>2334</v>
       </c>
       <c r="DK57" s="12" t="s">
-        <v>2749</v>
+        <v>2747</v>
       </c>
       <c r="DL57" s="45"/>
     </row>
@@ -23992,13 +23982,13 @@
         <v>1658</v>
       </c>
       <c r="DI59" s="12" t="s">
-        <v>2750</v>
+        <v>2748</v>
       </c>
       <c r="DJ59" s="61" t="s">
         <v>2334</v>
       </c>
       <c r="DK59" s="12" t="s">
-        <v>2751</v>
+        <v>2749</v>
       </c>
       <c r="DL59" s="45"/>
     </row>
@@ -24074,13 +24064,13 @@
         <v>1673</v>
       </c>
       <c r="DI61" s="12" t="s">
-        <v>2752</v>
+        <v>2750</v>
       </c>
       <c r="DJ61" s="61" t="s">
         <v>2334</v>
       </c>
       <c r="DK61" s="12" t="s">
-        <v>2753</v>
+        <v>2751</v>
       </c>
       <c r="DL61" s="45"/>
     </row>
@@ -24156,13 +24146,13 @@
         <v>1671</v>
       </c>
       <c r="DI63" s="12" t="s">
-        <v>2754</v>
+        <v>2752</v>
       </c>
       <c r="DJ63" s="61" t="s">
         <v>2334</v>
       </c>
       <c r="DK63" s="12" t="s">
-        <v>2755</v>
+        <v>2753</v>
       </c>
       <c r="DL63" s="45"/>
     </row>
@@ -24232,13 +24222,13 @@
         <v>1649</v>
       </c>
       <c r="DI65" s="12" t="s">
-        <v>2756</v>
+        <v>2754</v>
       </c>
       <c r="DJ65" s="61" t="s">
         <v>2334</v>
       </c>
       <c r="DK65" s="12" t="s">
-        <v>2757</v>
+        <v>2755</v>
       </c>
       <c r="DL65" s="45"/>
     </row>
@@ -24308,13 +24298,13 @@
         <v>1674</v>
       </c>
       <c r="DI67" s="12" t="s">
-        <v>2758</v>
+        <v>2756</v>
       </c>
       <c r="DJ67" s="61" t="s">
         <v>2334</v>
       </c>
       <c r="DK67" s="12" t="s">
-        <v>2759</v>
+        <v>2757</v>
       </c>
       <c r="DL67" s="45"/>
     </row>
@@ -24383,13 +24373,13 @@
         <v>1985</v>
       </c>
       <c r="DI69" s="12" t="s">
-        <v>2760</v>
+        <v>2758</v>
       </c>
       <c r="DJ69" s="61" t="s">
         <v>2334</v>
       </c>
       <c r="DK69" s="12" t="s">
-        <v>2761</v>
+        <v>2759</v>
       </c>
       <c r="DL69" s="45"/>
     </row>
@@ -24459,13 +24449,13 @@
         <v>1670</v>
       </c>
       <c r="DI71" s="12" t="s">
-        <v>2762</v>
+        <v>2760</v>
       </c>
       <c r="DJ71" s="61" t="s">
         <v>2334</v>
       </c>
       <c r="DK71" s="12" t="s">
-        <v>2763</v>
+        <v>2761</v>
       </c>
       <c r="DL71" s="45"/>
     </row>
@@ -24535,13 +24525,13 @@
         <v>1696</v>
       </c>
       <c r="DI73" s="12" t="s">
-        <v>2764</v>
+        <v>2762</v>
       </c>
       <c r="DJ73" s="61" t="s">
         <v>2334</v>
       </c>
       <c r="DK73" s="12" t="s">
-        <v>2765</v>
+        <v>2763</v>
       </c>
       <c r="DL73" s="45"/>
     </row>
@@ -24611,13 +24601,13 @@
         <v>1697</v>
       </c>
       <c r="DI75" s="12" t="s">
-        <v>2766</v>
+        <v>2764</v>
       </c>
       <c r="DJ75" s="61" t="s">
         <v>2334</v>
       </c>
       <c r="DK75" s="12" t="s">
-        <v>2767</v>
+        <v>2765</v>
       </c>
       <c r="DL75" s="45"/>
     </row>
@@ -24687,13 +24677,13 @@
         <v>1647</v>
       </c>
       <c r="DI77" s="12" t="s">
-        <v>2768</v>
+        <v>2766</v>
       </c>
       <c r="DJ77" s="61" t="s">
         <v>2334</v>
       </c>
       <c r="DK77" s="12" t="s">
-        <v>2767</v>
+        <v>2765</v>
       </c>
       <c r="DL77" s="45"/>
     </row>
@@ -24763,13 +24753,13 @@
         <v>1648</v>
       </c>
       <c r="DI79" s="12" t="s">
-        <v>2769</v>
+        <v>2767</v>
       </c>
       <c r="DJ79" s="61" t="s">
         <v>2334</v>
       </c>
       <c r="DK79" s="12" t="s">
-        <v>2770</v>
+        <v>2768</v>
       </c>
       <c r="DL79" s="45"/>
     </row>
@@ -24839,13 +24829,13 @@
         <v>1690</v>
       </c>
       <c r="DI81" s="12" t="s">
-        <v>2771</v>
+        <v>2769</v>
       </c>
       <c r="DJ81" s="61" t="s">
         <v>2334</v>
       </c>
       <c r="DK81" s="12" t="s">
-        <v>2770</v>
+        <v>2768</v>
       </c>
       <c r="DL81" s="45"/>
     </row>
@@ -24915,13 +24905,13 @@
         <v>1749</v>
       </c>
       <c r="DI83" s="12" t="s">
-        <v>2772</v>
+        <v>2770</v>
       </c>
       <c r="DJ83" s="61" t="s">
         <v>2334</v>
       </c>
       <c r="DK83" s="12" t="s">
-        <v>2770</v>
+        <v>2768</v>
       </c>
       <c r="DL83" s="45"/>
     </row>
@@ -24990,13 +24980,13 @@
         <v>1656</v>
       </c>
       <c r="DI85" s="12" t="s">
-        <v>2773</v>
+        <v>2771</v>
       </c>
       <c r="DJ85" s="61" t="s">
         <v>2334</v>
       </c>
       <c r="DK85" s="12" t="s">
-        <v>2774</v>
+        <v>2772</v>
       </c>
       <c r="DL85" s="45"/>
     </row>
@@ -25064,13 +25054,13 @@
         <v>1988</v>
       </c>
       <c r="DI87" s="12" t="s">
-        <v>2775</v>
+        <v>2773</v>
       </c>
       <c r="DJ87" s="61" t="s">
         <v>2334</v>
       </c>
       <c r="DK87" s="12" t="s">
-        <v>2776</v>
+        <v>2774</v>
       </c>
       <c r="DL87" s="45"/>
     </row>
@@ -25138,13 +25128,13 @@
         <v>1744</v>
       </c>
       <c r="DI89" s="12" t="s">
-        <v>2777</v>
+        <v>2775</v>
       </c>
       <c r="DJ89" s="61" t="s">
         <v>2334</v>
       </c>
       <c r="DK89" s="12" t="s">
-        <v>2778</v>
+        <v>2776</v>
       </c>
       <c r="DL89" s="45"/>
     </row>
@@ -25212,13 +25202,13 @@
         <v>1989</v>
       </c>
       <c r="DI91" s="12" t="s">
-        <v>2779</v>
+        <v>2777</v>
       </c>
       <c r="DJ91" s="61" t="s">
         <v>2334</v>
       </c>
       <c r="DK91" s="12" t="s">
-        <v>2780</v>
+        <v>2778</v>
       </c>
       <c r="DL91" s="45"/>
     </row>
@@ -25286,13 +25276,13 @@
         <v>1990</v>
       </c>
       <c r="DI93" s="12" t="s">
-        <v>2781</v>
+        <v>2779</v>
       </c>
       <c r="DJ93" s="61" t="s">
         <v>2334</v>
       </c>
       <c r="DK93" s="12" t="s">
-        <v>2782</v>
+        <v>2780</v>
       </c>
       <c r="DL93" s="45"/>
     </row>
@@ -25360,13 +25350,13 @@
         <v>1992</v>
       </c>
       <c r="DI95" s="12" t="s">
-        <v>2783</v>
+        <v>2781</v>
       </c>
       <c r="DJ95" s="61" t="s">
         <v>2334</v>
       </c>
       <c r="DK95" s="12" t="s">
-        <v>2784</v>
+        <v>2782</v>
       </c>
       <c r="DL95" s="45"/>
     </row>
@@ -25434,13 +25424,13 @@
         <v>1993</v>
       </c>
       <c r="DI97" s="12" t="s">
-        <v>2785</v>
+        <v>2783</v>
       </c>
       <c r="DJ97" s="61" t="s">
         <v>2334</v>
       </c>
       <c r="DK97" s="12" t="s">
-        <v>2786</v>
+        <v>2784</v>
       </c>
       <c r="DL97" s="45"/>
     </row>
@@ -25468,7 +25458,7 @@
         <v>1560</v>
       </c>
       <c r="BC98" s="7" t="s">
-        <v>2806</v>
+        <v>2804</v>
       </c>
       <c r="DI98" s="12" t="s">
         <v>2184</v>
@@ -25506,13 +25496,13 @@
       </c>
       <c r="BC99" s="7"/>
       <c r="DI99" s="12" t="s">
-        <v>2787</v>
+        <v>2785</v>
       </c>
       <c r="DJ99" s="61" t="s">
         <v>2334</v>
       </c>
       <c r="DK99" s="12" t="s">
-        <v>2788</v>
+        <v>2786</v>
       </c>
       <c r="DL99" s="45"/>
     </row>
@@ -25574,13 +25564,13 @@
         <v>1562</v>
       </c>
       <c r="DI101" s="12" t="s">
-        <v>2789</v>
+        <v>2787</v>
       </c>
       <c r="DJ101" s="61" t="s">
         <v>2334</v>
       </c>
       <c r="DK101" s="12" t="s">
-        <v>2790</v>
+        <v>2788</v>
       </c>
       <c r="DL101" s="45"/>
     </row>
@@ -25642,13 +25632,13 @@
         <v>1564</v>
       </c>
       <c r="DI103" s="12" t="s">
-        <v>2791</v>
+        <v>2789</v>
       </c>
       <c r="DJ103" s="61" t="s">
         <v>2334</v>
       </c>
       <c r="DK103" s="12" t="s">
-        <v>2792</v>
+        <v>2790</v>
       </c>
       <c r="DL103" s="45"/>
     </row>
@@ -25710,13 +25700,13 @@
         <v>1566</v>
       </c>
       <c r="DI105" s="12" t="s">
-        <v>2793</v>
+        <v>2791</v>
       </c>
       <c r="DJ105" s="61" t="s">
         <v>2334</v>
       </c>
       <c r="DK105" s="12" t="s">
-        <v>2794</v>
+        <v>2792</v>
       </c>
       <c r="DL105" s="45"/>
     </row>
@@ -25778,13 +25768,13 @@
         <v>2011</v>
       </c>
       <c r="DI107" s="12" t="s">
-        <v>2795</v>
+        <v>2793</v>
       </c>
       <c r="DJ107" s="61" t="s">
         <v>2334</v>
       </c>
       <c r="DK107" s="12" t="s">
-        <v>2796</v>
+        <v>2794</v>
       </c>
       <c r="DL107" s="45"/>
     </row>
@@ -25846,13 +25836,13 @@
         <v>1569</v>
       </c>
       <c r="DI109" s="12" t="s">
-        <v>2797</v>
+        <v>2795</v>
       </c>
       <c r="DJ109" s="61" t="s">
         <v>2334</v>
       </c>
       <c r="DK109" s="12" t="s">
-        <v>2798</v>
+        <v>2796</v>
       </c>
       <c r="DL109" s="45"/>
     </row>
@@ -25914,13 +25904,13 @@
         <v>1570</v>
       </c>
       <c r="DI111" s="12" t="s">
-        <v>2799</v>
+        <v>2797</v>
       </c>
       <c r="DJ111" s="61" t="s">
         <v>2334</v>
       </c>
       <c r="DK111" s="12" t="s">
-        <v>2800</v>
+        <v>2798</v>
       </c>
       <c r="DL111" s="45"/>
     </row>
@@ -25982,13 +25972,13 @@
         <v>2013</v>
       </c>
       <c r="DI113" s="12" t="s">
-        <v>2801</v>
+        <v>2799</v>
       </c>
       <c r="DJ113" s="61" t="s">
         <v>2334</v>
       </c>
       <c r="DK113" s="12" t="s">
-        <v>2802</v>
+        <v>2800</v>
       </c>
       <c r="DL113" s="45"/>
     </row>
@@ -26050,13 +26040,13 @@
         <v>1572</v>
       </c>
       <c r="DI115" s="12" t="s">
-        <v>2803</v>
+        <v>2801</v>
       </c>
       <c r="DJ115" s="61" t="s">
         <v>2334</v>
       </c>
       <c r="DK115" s="12" t="s">
-        <v>2804</v>
+        <v>2802</v>
       </c>
       <c r="DL115" s="45"/>
     </row>
@@ -28295,7 +28285,7 @@
       <c r="DL277" s="45"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="Mcatd7Y5thVOYBjly4I5csENk+KJJ2h23IKiVWx9zUm8AA9cQPhjvl1XPQV9gtAqi8w7LMzbopaSaizwttdFRg==" saltValue="93CylD+J8lrbmWSNxRaETA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="F4/6G59ZVuOxlmG+BFCfQvPkU6LHvLGvrt24ZPCG8osbFyUjhNhUQ/JYSPKHjHMHd6FUbQUbs5wEJEXQKS6V8A==" saltValue="Ww5/mQMwKKD3rBaBVhLWXA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="2">
     <mergeCell ref="M27:M28"/>
     <mergeCell ref="M34:M35"/>

</xml_diff>

<commit_message>
Added a column regarding quality of coordinates: whether the coordinates were inferred by georeferencing a map, or if they were provided.
</commit_message>
<xml_diff>
--- a/Excel_templates/MOSAIC_input_excel_file_2022.xlsx
+++ b/Excel_templates/MOSAIC_input_excel_file_2022.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sparadis\Documents\ETH\MOSAIC\MOSAIC_Client\Excel_templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A71EA522-D7C7-4A77-9233-03EF35C924A4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08E4201C-1A05-40ED-A92E-193D681E4F7B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30204" yWindow="10044" windowWidth="40020" windowHeight="22296" tabRatio="694" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30204" yWindow="10044" windowWidth="40020" windowHeight="22296" tabRatio="694" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ARTICLE_AUTHOR" sheetId="3" r:id="rId1"/>
@@ -186,7 +186,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3922" uniqueCount="3008">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3923" uniqueCount="3009">
   <si>
     <t>sample_name</t>
   </si>
@@ -9210,6 +9210,9 @@
   </si>
   <si>
     <t>Mercury</t>
+  </si>
+  <si>
+    <t>Georeferenced coordinates</t>
   </si>
 </sst>
 </file>
@@ -10244,7 +10247,7 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -10334,44 +10337,44 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:O27"/>
+  <dimension ref="A1:P27"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15.69921875" style="29" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22" style="29" customWidth="1"/>
-    <col min="3" max="4" width="10.796875" style="29" customWidth="1"/>
-    <col min="5" max="5" width="13.19921875" style="32" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15" style="33" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15" style="33" customWidth="1"/>
-    <col min="8" max="8" width="28.3984375" style="29" customWidth="1"/>
-    <col min="9" max="9" width="23.296875" style="29" customWidth="1"/>
-    <col min="10" max="10" width="16.8984375" style="29" customWidth="1"/>
-    <col min="11" max="13" width="24.796875" style="29" customWidth="1"/>
-    <col min="14" max="14" width="27.8984375" style="29" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="27.8984375" style="29" customWidth="1"/>
-    <col min="16" max="16" width="10.796875" style="29" customWidth="1"/>
-    <col min="17" max="16384" width="11.19921875" style="29"/>
+    <col min="3" max="5" width="10.796875" style="29" customWidth="1"/>
+    <col min="6" max="6" width="13.19921875" style="32" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15" style="33" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15" style="33" customWidth="1"/>
+    <col min="9" max="9" width="28.3984375" style="29" customWidth="1"/>
+    <col min="10" max="10" width="23.296875" style="29" customWidth="1"/>
+    <col min="11" max="11" width="16.8984375" style="29" customWidth="1"/>
+    <col min="12" max="14" width="24.796875" style="29" customWidth="1"/>
+    <col min="15" max="15" width="27.8984375" style="29" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="27.8984375" style="29" customWidth="1"/>
+    <col min="17" max="17" width="10.796875" style="29" customWidth="1"/>
+    <col min="18" max="16384" width="11.19921875" style="29"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="63" customFormat="1" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:16" s="63" customFormat="1" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A1" s="89" t="s">
         <v>2675</v>
       </c>
       <c r="B1" s="89"/>
       <c r="C1" s="89"/>
       <c r="D1" s="89"/>
-      <c r="E1" s="90" t="s">
+      <c r="E1" s="89"/>
+      <c r="F1" s="90" t="s">
         <v>2815</v>
       </c>
-      <c r="F1" s="90"/>
       <c r="G1" s="90"/>
       <c r="H1" s="90"/>
       <c r="I1" s="90"/>
@@ -10381,8 +10384,9 @@
       <c r="M1" s="90"/>
       <c r="N1" s="90"/>
       <c r="O1" s="90"/>
-    </row>
-    <row r="2" spans="1:15" s="66" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="P1" s="90"/>
+    </row>
+    <row r="2" spans="1:16" s="66" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="62" t="s">
         <v>2565</v>
       </c>
@@ -10395,221 +10399,249 @@
       <c r="D2" s="62" t="s">
         <v>1827</v>
       </c>
-      <c r="E2" s="65" t="s">
+      <c r="E2" s="62" t="s">
+        <v>3008</v>
+      </c>
+      <c r="F2" s="65" t="s">
         <v>1828</v>
       </c>
-      <c r="F2" s="65" t="s">
+      <c r="G2" s="65" t="s">
         <v>1829</v>
       </c>
-      <c r="G2" s="65" t="s">
+      <c r="H2" s="65" t="s">
         <v>2076</v>
       </c>
-      <c r="H2" s="65" t="s">
+      <c r="I2" s="65" t="s">
         <v>2063</v>
       </c>
-      <c r="I2" s="65" t="s">
+      <c r="J2" s="65" t="s">
         <v>2077</v>
       </c>
-      <c r="J2" s="65" t="s">
+      <c r="K2" s="65" t="s">
         <v>2049</v>
       </c>
-      <c r="K2" s="65" t="s">
+      <c r="L2" s="65" t="s">
         <v>1831</v>
       </c>
-      <c r="L2" s="65" t="s">
+      <c r="M2" s="65" t="s">
         <v>1850</v>
       </c>
-      <c r="M2" s="65" t="s">
+      <c r="N2" s="65" t="s">
         <v>1832</v>
       </c>
-      <c r="N2" s="65" t="s">
+      <c r="O2" s="65" t="s">
         <v>1833</v>
       </c>
-      <c r="O2" s="65" t="s">
+      <c r="P2" s="65" t="s">
         <v>1830</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B3" s="41"/>
       <c r="C3" s="41"/>
       <c r="D3" s="41"/>
-      <c r="E3" s="49"/>
-      <c r="F3" s="41"/>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="E3" s="41"/>
+      <c r="F3" s="49"/>
+      <c r="G3" s="41"/>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B4" s="41"/>
       <c r="C4" s="41"/>
       <c r="D4" s="41"/>
-      <c r="E4" s="49"/>
-      <c r="F4" s="41"/>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="E4" s="41"/>
+      <c r="F4" s="49"/>
+      <c r="G4" s="41"/>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B5" s="41"/>
       <c r="C5" s="41"/>
       <c r="D5" s="41"/>
-      <c r="E5" s="49"/>
-      <c r="F5" s="41"/>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="E5" s="41"/>
+      <c r="F5" s="49"/>
+      <c r="G5" s="41"/>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B6" s="41"/>
       <c r="C6" s="41"/>
       <c r="D6" s="41"/>
-      <c r="E6" s="49"/>
-      <c r="F6" s="41"/>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="E6" s="41"/>
+      <c r="F6" s="49"/>
+      <c r="G6" s="41"/>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B7" s="41"/>
       <c r="C7" s="41"/>
       <c r="D7" s="41"/>
-      <c r="E7" s="49"/>
-      <c r="F7" s="41"/>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="E7" s="41"/>
+      <c r="F7" s="49"/>
+      <c r="G7" s="41"/>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B8" s="41"/>
       <c r="C8" s="41"/>
       <c r="D8" s="41"/>
-      <c r="E8" s="49"/>
-      <c r="F8" s="41"/>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="E8" s="41"/>
+      <c r="F8" s="49"/>
+      <c r="G8" s="41"/>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B9" s="41"/>
       <c r="C9" s="41"/>
       <c r="D9" s="41"/>
-      <c r="E9" s="49"/>
-      <c r="F9" s="41"/>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="E9" s="41"/>
+      <c r="F9" s="49"/>
+      <c r="G9" s="41"/>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B10" s="41"/>
       <c r="C10" s="41"/>
       <c r="D10" s="41"/>
-      <c r="E10" s="49"/>
-      <c r="F10" s="41"/>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="E10" s="41"/>
+      <c r="F10" s="49"/>
+      <c r="G10" s="41"/>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B11" s="41"/>
       <c r="C11" s="41"/>
       <c r="D11" s="41"/>
-      <c r="E11" s="49"/>
-      <c r="F11" s="41"/>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="E11" s="41"/>
+      <c r="F11" s="49"/>
+      <c r="G11" s="41"/>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B12" s="41"/>
       <c r="C12" s="41"/>
       <c r="D12" s="41"/>
-      <c r="E12" s="49"/>
-      <c r="F12" s="41"/>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="E12" s="41"/>
+      <c r="F12" s="49"/>
+      <c r="G12" s="41"/>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B13" s="41"/>
       <c r="C13" s="41"/>
       <c r="D13" s="41"/>
-      <c r="E13" s="49"/>
-      <c r="F13" s="41"/>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="E13" s="41"/>
+      <c r="F13" s="49"/>
+      <c r="G13" s="41"/>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B14" s="41"/>
       <c r="C14" s="41"/>
       <c r="D14" s="41"/>
-      <c r="E14" s="49"/>
-      <c r="F14" s="41"/>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="E14" s="41"/>
+      <c r="F14" s="49"/>
+      <c r="G14" s="41"/>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B15" s="41"/>
       <c r="C15" s="41"/>
       <c r="D15" s="41"/>
-      <c r="E15" s="49"/>
-      <c r="F15" s="41"/>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="E15" s="41"/>
+      <c r="F15" s="49"/>
+      <c r="G15" s="41"/>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B16" s="41"/>
       <c r="C16" s="41"/>
       <c r="D16" s="41"/>
-      <c r="E16" s="49"/>
-      <c r="F16" s="41"/>
-    </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="E16" s="41"/>
+      <c r="F16" s="49"/>
+      <c r="G16" s="41"/>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B17" s="41"/>
       <c r="C17" s="41"/>
       <c r="D17" s="41"/>
-      <c r="E17" s="49"/>
-      <c r="F17" s="41"/>
-    </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="E17" s="41"/>
+      <c r="F17" s="49"/>
+      <c r="G17" s="41"/>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B18" s="41"/>
       <c r="C18" s="41"/>
       <c r="D18" s="41"/>
-      <c r="E18" s="49"/>
-      <c r="F18" s="41"/>
-    </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="E18" s="41"/>
+      <c r="F18" s="49"/>
+      <c r="G18" s="41"/>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B19" s="41"/>
       <c r="C19" s="41"/>
       <c r="D19" s="41"/>
-      <c r="E19" s="49"/>
-      <c r="F19" s="41"/>
-    </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="E19" s="41"/>
+      <c r="F19" s="49"/>
+      <c r="G19" s="41"/>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B20" s="41"/>
       <c r="C20" s="41"/>
       <c r="D20" s="41"/>
-      <c r="E20" s="49"/>
-      <c r="F20" s="41"/>
-    </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="E20" s="41"/>
+      <c r="F20" s="49"/>
+      <c r="G20" s="41"/>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B21" s="41"/>
       <c r="C21" s="41"/>
       <c r="D21" s="41"/>
-      <c r="E21" s="49"/>
-      <c r="F21" s="41"/>
-    </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="E21" s="41"/>
+      <c r="F21" s="49"/>
+      <c r="G21" s="41"/>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B22" s="41"/>
       <c r="C22" s="41"/>
       <c r="D22" s="41"/>
-      <c r="E22" s="49"/>
-      <c r="F22" s="41"/>
-    </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="E22" s="41"/>
+      <c r="F22" s="49"/>
+      <c r="G22" s="41"/>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B23" s="41"/>
       <c r="C23" s="41"/>
       <c r="D23" s="41"/>
-      <c r="E23" s="49"/>
-      <c r="F23" s="41"/>
-    </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="E23" s="41"/>
+      <c r="F23" s="49"/>
+      <c r="G23" s="41"/>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B24" s="41"/>
       <c r="C24" s="41"/>
       <c r="D24" s="41"/>
-      <c r="E24" s="49"/>
-      <c r="F24" s="41"/>
-    </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="E24" s="41"/>
+      <c r="F24" s="49"/>
+      <c r="G24" s="41"/>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B25" s="41"/>
       <c r="C25" s="41"/>
       <c r="D25" s="41"/>
-      <c r="E25" s="49"/>
-      <c r="F25" s="41"/>
-    </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="E25" s="41"/>
+      <c r="F25" s="49"/>
+      <c r="G25" s="41"/>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B26" s="41"/>
       <c r="C26" s="41"/>
       <c r="D26" s="41"/>
-      <c r="E26" s="49"/>
-      <c r="F26" s="41"/>
-    </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="E26" s="41"/>
+      <c r="F26" s="49"/>
+      <c r="G26" s="41"/>
+    </row>
+    <row r="27" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B27" s="41"/>
       <c r="C27" s="41"/>
       <c r="D27" s="41"/>
-      <c r="E27" s="49"/>
-      <c r="F27" s="41"/>
+      <c r="E27" s="41"/>
+      <c r="F27" s="49"/>
+      <c r="G27" s="41"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="E1:O1"/>
+    <mergeCell ref="F1:P1"/>
+    <mergeCell ref="A1:E1"/>
   </mergeCells>
-  <conditionalFormatting sqref="B1:B1048576">
+  <conditionalFormatting sqref="B2:B1048576">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="13">
@@ -10621,47 +10653,53 @@
       <formula1>-180</formula1>
       <formula2>180</formula2>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Waer depth should be positive numbers." prompt="Water depth where the core was collected." sqref="F28:F1048576" xr:uid="{00CDF339-1F57-43C3-902E-FF6A4E068910}">
+    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Waer depth should be positive numbers." prompt="Water depth where the core was collected." sqref="G28:G1048576" xr:uid="{00CDF339-1F57-43C3-902E-FF6A4E068910}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="textLength" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Maximum comment length is 200 characters" prompt="Add any additional information of the core" sqref="G3:G1048576" xr:uid="{FF2D52E6-EFBC-4479-B912-8CF305BA6CC6}">
+    <dataValidation type="textLength" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Maximum comment length is 200 characters" prompt="Add any additional information of the core" sqref="H3:H1048576" xr:uid="{FF2D52E6-EFBC-4479-B912-8CF305BA6CC6}">
       <formula1>200</formula1>
     </dataValidation>
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please select geomorphological site if relevant. Choese _unkown if unknown. Otherwise leave blank." prompt="Please select geomorphological site if relevant. Choese _unkown if unknown. Otherwise leave blank." sqref="I3:I1048576" xr:uid="{C409BA21-827A-4726-997B-4DDCEB0E121E}">
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please select geomorphological site if relevant. Choese _unkown if unknown. Otherwise leave blank." prompt="Please select geomorphological site if relevant. Choese _unkown if unknown. Otherwise leave blank." sqref="J3:J1048576" xr:uid="{C409BA21-827A-4726-997B-4DDCEB0E121E}">
       <formula1>geomorphological_site</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Choose the country that the Research Vessel belongs to. If unknown, choose _unknown. If not listed here, check _other." prompt="Choose the country that the Research Vessel belongs to (extracted from Wikipedia, please contact mosaic@ethz.ch for any errors)" sqref="K3:K1048576" xr:uid="{6E72A734-A312-4B86-8990-BB5CA2135DC2}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Choose the country that the Research Vessel belongs to. If unknown, choose _unknown. If not listed here, check _other." prompt="Choose the country that the Research Vessel belongs to (extracted from Wikipedia, please contact mosaic@ethz.ch for any errors)" sqref="L3:L1048576" xr:uid="{6E72A734-A312-4B86-8990-BB5CA2135DC2}">
       <formula1>Research_Vessel_Countries</formula1>
     </dataValidation>
-    <dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Date is not between 1/1/1900 and TODAY" prompt="Add sampling date between 1/1/1900 and TODAY" sqref="E3:E1048576" xr:uid="{7913A979-EC13-4075-870A-D28BCBAC3D30}">
+    <dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Date is not between 1/1/1900 and TODAY" prompt="Add sampling date between 1/1/1900 and TODAY" sqref="F3:F1048576" xr:uid="{7913A979-EC13-4075-870A-D28BCBAC3D30}">
       <formula1>1</formula1>
       <formula2>TODAY()</formula2>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Name of the campaign cruise." sqref="M3:M1048576" xr:uid="{573E733B-B85F-488A-AB24-1BB2993B0FAE}"/>
-    <dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid date" error="Please introduce a date between 1/1/1900 and TODAY." prompt="If known, add the starting date of the cruise. Accepts dates between 1/1/1900 and TODAY." sqref="N3:N1048576" xr:uid="{D9536885-D4AA-431B-A11C-EEFC92030E57}">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Name of the campaign cruise." sqref="N3:N1048576" xr:uid="{573E733B-B85F-488A-AB24-1BB2993B0FAE}"/>
+    <dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid date" error="Please introduce a date between 1/1/1900 and TODAY." prompt="If known, add the starting date of the cruise. Accepts dates between 1/1/1900 and TODAY." sqref="O3:O1048576" xr:uid="{D9536885-D4AA-431B-A11C-EEFC92030E57}">
       <formula1>1</formula1>
       <formula2>TODAY()</formula2>
     </dataValidation>
-    <dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid date" error="Please introduce a date between 1/1/1900 and TODAY." prompt="If known, add the ending date of the cruise. Accepts dates between 1/1/1900 and TODAY." sqref="O3:O1048576" xr:uid="{2F267FE0-8CDD-46BB-9FA7-D775C28F6A0E}">
+    <dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid date" error="Please introduce a date between 1/1/1900 and TODAY." prompt="If known, add the ending date of the cruise. Accepts dates between 1/1/1900 and TODAY." sqref="P3:P1048576" xr:uid="{2F267FE0-8CDD-46BB-9FA7-D775C28F6A0E}">
       <formula1>1</formula1>
       <formula2>TODAY()</formula2>
     </dataValidation>
-    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="If available, specify the length of the core retrieved in cm." sqref="J3:J1048576" xr:uid="{6E15A0C0-8408-4930-8258-97C19A733952}"/>
+    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="If available, specify the length of the core retrieved in cm." sqref="K3:K1048576" xr:uid="{6E15A0C0-8408-4930-8258-97C19A733952}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Name of user who is entering data" sqref="A3:A1048576" xr:uid="{B1508E14-6DD0-4DEF-BE9A-DA048D366864}"/>
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="In order to choose a research vessel, first choose the country it belongs to." sqref="L4:L1048576 L3" xr:uid="{74AEC9A0-D7E8-4D80-8B77-1F64526DD0B8}">
-      <formula1>INDIRECT(K3)</formula1>
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="In order to choose a research vessel, first choose the country it belongs to." sqref="M4:M1048576 M3" xr:uid="{74AEC9A0-D7E8-4D80-8B77-1F64526DD0B8}">
+      <formula1>INDIRECT(L3)</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.70000000000000007" right="0.70000000000000007" top="0.75" bottom="0.75" header="0.30000000000000004" footer="0.30000000000000004"/>
   <pageSetup fitToWidth="0" fitToHeight="0" orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
         <x14:dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please select corer type if relevant. Chosse _unkown if unknown. Otherwise leave blank." prompt="Please select corer type if relevant. Chosse _unkown if unknown. Otherwise leave blank." xr:uid="{89ED9B77-757F-4A56-BFAB-AB1DC0DB17FB}">
           <x14:formula1>
             <xm:f>SET_VARIABLES!$J$2:$J$13</xm:f>
           </x14:formula1>
-          <xm:sqref>H3:H1048576</xm:sqref>
+          <xm:sqref>I3:I1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" prompt="State whether the coordinates were obtained by georeferencing a map, or inferred (TRUE) or whether they were provided in tabular format (FALSE)." xr:uid="{FC9545BB-E799-4EF5-951B-5C2E1E979B37}">
+          <x14:formula1>
+            <xm:f>SET_VARIABLES!$A$2:$A$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>E3:E1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -12133,10 +12171,10 @@
   <dimension ref="A1:CB52"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="3" ySplit="6" topLeftCell="H7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="6" topLeftCell="D7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="N3" sqref="N3"/>
+      <selection pane="bottomRight" activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -14845,7 +14883,7 @@
           <x14:formula1>
             <xm:f>SET_VARIABLES!$A$2:$A$3</xm:f>
           </x14:formula1>
-          <xm:sqref>D7:D1048576</xm:sqref>
+          <xm:sqref>D7 D9:D1048576 D8</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Write the core name or select from the drop-down menu the cores you have in the Workbook._x000a_Make sure that the core name matches with its metadata given in GEOPOINTS_CORES sheet" xr:uid="{E4FFB722-8CB2-4C84-A9DE-29D8614FBFFB}">
           <x14:formula1>
@@ -14870,7 +14908,7 @@
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:HL277"/>
   <sheetViews>
-    <sheetView topLeftCell="CP1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="CQ24" sqref="CQ24"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added "Method details" to core analyses.
</commit_message>
<xml_diff>
--- a/Excel_templates/MOSAIC_input_excel_file_2022.xlsx
+++ b/Excel_templates/MOSAIC_input_excel_file_2022.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sparadis\Documents\ETH\MOSAIC\MOSAIC_Client\Excel_templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08E4201C-1A05-40ED-A92E-193D681E4F7B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED680B39-61C5-4895-80B5-E8A19738F792}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30204" yWindow="10044" windowWidth="40020" windowHeight="22296" tabRatio="694" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30204" yWindow="10044" windowWidth="40020" windowHeight="22296" tabRatio="694" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ARTICLE_AUTHOR" sheetId="3" r:id="rId1"/>
@@ -77,7 +77,7 @@
     <definedName name="K38Et_ng_g">SET_VARIABLES!$HE$2:$HE$4</definedName>
     <definedName name="K38Me_ng_g">SET_VARIABLES!$HF$2:$HF$4</definedName>
     <definedName name="Lebanon">SET_VARIABLES!$AK$2:$AK$4</definedName>
-    <definedName name="MAR_g_cm2_yr">SET_VARIABLES!$GY$2:$GY$17</definedName>
+    <definedName name="MAR_g_cm2_yr">SET_VARIABLES!$GY$2:$GY$19</definedName>
     <definedName name="MAR_model">SET_VARIABLES!$BL$2:$BL$9</definedName>
     <definedName name="MAR_tracer">SET_VARIABLES!$BJ$2:$BJ$12</definedName>
     <definedName name="material_analyzed">SET_VARIABLES!$CM$2:$CM$29</definedName>
@@ -132,7 +132,7 @@
     <definedName name="sample_sedimentation_rate">SET_VARIABLES!$EV$2:$EV$5</definedName>
     <definedName name="Sample_sterols">SET_VARIABLES!$DR$2:$DR$10</definedName>
     <definedName name="sand_">SET_VARIABLES!$FL$2:$FL$4</definedName>
-    <definedName name="SAR_cm_yr">SET_VARIABLES!$GZ$2:$GZ$17</definedName>
+    <definedName name="SAR_cm_yr">SET_VARIABLES!$GZ$2:$GZ$18</definedName>
     <definedName name="SAR_model">SET_VARIABLES!$BK$2:$BK$9</definedName>
     <definedName name="SAR_tracer">SET_VARIABLES!$BJ$2:$BJ$12</definedName>
     <definedName name="silt_">SET_VARIABLES!$FM$2:$FM$4</definedName>
@@ -148,7 +148,7 @@
     <definedName name="total_carbon_">SET_VARIABLES!$FW$2:$FW$4</definedName>
     <definedName name="total_inorganic_carbon_">SET_VARIABLES!$FY$2:$FY$4</definedName>
     <definedName name="total_nitrogen_">SET_VARIABLES!$GC$2:$GC$4</definedName>
-    <definedName name="total_organic_carbon_">SET_VARIABLES!$FG$2:$FG$5</definedName>
+    <definedName name="total_organic_carbon_">SET_VARIABLES!$FG$2:$FG$7</definedName>
     <definedName name="Total_Pb210_Bq_kg">SET_VARIABLES!$GP$2:$GP$4</definedName>
     <definedName name="Turkey">SET_VARIABLES!$AZ$2:$AZ$14</definedName>
     <definedName name="UK38Et">SET_VARIABLES!$HI$2:$HI$4</definedName>
@@ -186,7 +186,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3923" uniqueCount="3009">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3927" uniqueCount="3012">
   <si>
     <t>sample_name</t>
   </si>
@@ -9213,6 +9213,15 @@
   </si>
   <si>
     <t>Georeferenced coordinates</t>
+  </si>
+  <si>
+    <t>manometric</t>
+  </si>
+  <si>
+    <t>pollen</t>
+  </si>
+  <si>
+    <t>Pb-210 unknown</t>
   </si>
 </sst>
 </file>
@@ -9686,7 +9695,7 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="116">
+  <cellXfs count="117">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="13" applyFont="1" applyFill="1" applyAlignment="1"/>
@@ -9818,16 +9827,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="19" fillId="4" borderId="4" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="12" borderId="3" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="14" fontId="21" fillId="12" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="12" borderId="3" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="2" borderId="2" xfId="14" applyFill="1" applyAlignment="1" applyProtection="1">
@@ -10268,15 +10278,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="64" customFormat="1" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="88" t="s">
+      <c r="A1" s="89" t="s">
         <v>2674</v>
       </c>
-      <c r="B1" s="88"/>
-      <c r="C1" s="88"/>
-      <c r="D1" s="88"/>
-      <c r="E1" s="88"/>
-      <c r="F1" s="88"/>
-      <c r="G1" s="88"/>
+      <c r="B1" s="89"/>
+      <c r="C1" s="89"/>
+      <c r="D1" s="89"/>
+      <c r="E1" s="89"/>
+      <c r="F1" s="89"/>
+      <c r="G1" s="89"/>
     </row>
     <row r="2" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="53" t="s">
@@ -10339,7 +10349,7 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:P27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -10365,13 +10375,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" s="63" customFormat="1" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="89" t="s">
+      <c r="A1" s="91" t="s">
         <v>2675</v>
       </c>
-      <c r="B1" s="89"/>
-      <c r="C1" s="89"/>
-      <c r="D1" s="89"/>
-      <c r="E1" s="89"/>
+      <c r="B1" s="91"/>
+      <c r="C1" s="91"/>
+      <c r="D1" s="91"/>
+      <c r="E1" s="91"/>
       <c r="F1" s="90" t="s">
         <v>2815</v>
       </c>
@@ -10710,13 +10720,13 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D8CE71B-0ABD-4CAD-AFB4-025997DA14A6}">
   <sheetPr codeName="Sheet4"/>
-  <dimension ref="A1:AJ43"/>
+  <dimension ref="A1:AJ44"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="2" ySplit="5" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="6" topLeftCell="C7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="G14" sqref="G14"/>
+      <selection pane="bottomRight" activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -10733,37 +10743,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:35" s="55" customFormat="1" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="91" t="s">
+      <c r="A1" s="92" t="s">
         <v>2677</v>
       </c>
-      <c r="B1" s="91"/>
-      <c r="C1" s="91" t="s">
+      <c r="B1" s="92"/>
+      <c r="C1" s="92" t="s">
         <v>2676</v>
       </c>
-      <c r="D1" s="91"/>
-      <c r="E1" s="91"/>
-      <c r="F1" s="91"/>
+      <c r="D1" s="92"/>
+      <c r="E1" s="92"/>
+      <c r="F1" s="92"/>
       <c r="G1" s="55" t="s">
-        <v>2830</v>
+        <v>2221</v>
       </c>
     </row>
     <row r="2" spans="1:35" ht="15.6" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="92" t="s">
+      <c r="A2" s="93" t="s">
         <v>2565</v>
       </c>
-      <c r="B2" s="92" t="s">
+      <c r="B2" s="93" t="s">
         <v>1825</v>
       </c>
-      <c r="C2" s="92" t="s">
+      <c r="C2" s="93" t="s">
         <v>1834</v>
       </c>
-      <c r="D2" s="92" t="s">
+      <c r="D2" s="93" t="s">
         <v>2684</v>
       </c>
-      <c r="E2" s="92" t="s">
+      <c r="E2" s="93" t="s">
         <v>1823</v>
       </c>
-      <c r="F2" s="95" t="s">
+      <c r="F2" s="96" t="s">
         <v>1824</v>
       </c>
       <c r="G2" s="56" t="s">
@@ -10799,12 +10809,12 @@
       <c r="AI2" s="56"/>
     </row>
     <row r="3" spans="1:35" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="93"/>
-      <c r="B3" s="93"/>
-      <c r="C3" s="93"/>
-      <c r="D3" s="93"/>
-      <c r="E3" s="93"/>
-      <c r="F3" s="96"/>
+      <c r="A3" s="94"/>
+      <c r="B3" s="94"/>
+      <c r="C3" s="94"/>
+      <c r="D3" s="94"/>
+      <c r="E3" s="94"/>
+      <c r="F3" s="97"/>
       <c r="G3" s="56"/>
       <c r="H3" s="56"/>
       <c r="I3" s="56"/>
@@ -10841,7 +10851,7 @@
       <c r="C4" s="94"/>
       <c r="D4" s="94"/>
       <c r="E4" s="94"/>
-      <c r="F4" s="96"/>
+      <c r="F4" s="97"/>
       <c r="G4" s="56"/>
       <c r="H4" s="56"/>
       <c r="I4" s="56"/>
@@ -10873,12 +10883,12 @@
       <c r="AI4" s="56"/>
     </row>
     <row r="5" spans="1:35" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="94"/>
-      <c r="B5" s="94"/>
-      <c r="C5" s="94"/>
-      <c r="D5" s="94"/>
-      <c r="E5" s="94"/>
-      <c r="F5" s="96"/>
+      <c r="A5" s="95"/>
+      <c r="B5" s="95"/>
+      <c r="C5" s="95"/>
+      <c r="D5" s="95"/>
+      <c r="E5" s="95"/>
+      <c r="F5" s="97"/>
       <c r="G5" s="56"/>
       <c r="H5" s="56"/>
       <c r="I5" s="56"/>
@@ -10909,36 +10919,42 @@
       <c r="AH5" s="56"/>
       <c r="AI5" s="56"/>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="G6" s="58"/>
-      <c r="H6" s="58"/>
-      <c r="I6" s="58"/>
-      <c r="J6" s="58"/>
-      <c r="K6" s="58"/>
-      <c r="L6" s="58"/>
-      <c r="M6" s="58"/>
-      <c r="N6" s="58"/>
-      <c r="O6" s="58"/>
-      <c r="P6" s="58"/>
-      <c r="Q6" s="58"/>
-      <c r="R6" s="58"/>
-      <c r="S6" s="58"/>
-      <c r="T6" s="58"/>
-      <c r="U6" s="58"/>
-      <c r="V6" s="58"/>
-      <c r="W6" s="58"/>
-      <c r="X6" s="58"/>
-      <c r="Y6" s="58"/>
-      <c r="Z6" s="58"/>
-      <c r="AA6" s="58"/>
-      <c r="AB6" s="58"/>
-      <c r="AC6" s="58"/>
-      <c r="AD6" s="58"/>
-      <c r="AE6" s="58"/>
-      <c r="AF6" s="58"/>
-      <c r="AG6" s="58"/>
-      <c r="AH6" s="58"/>
-      <c r="AI6" s="58"/>
+    <row r="6" spans="1:35" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="95"/>
+      <c r="B6" s="95"/>
+      <c r="C6" s="95"/>
+      <c r="D6" s="95"/>
+      <c r="E6" s="95"/>
+      <c r="F6" s="97"/>
+      <c r="G6" s="56"/>
+      <c r="H6" s="56"/>
+      <c r="I6" s="56"/>
+      <c r="J6" s="56"/>
+      <c r="K6" s="56"/>
+      <c r="L6" s="56"/>
+      <c r="M6" s="56"/>
+      <c r="N6" s="56"/>
+      <c r="O6" s="56"/>
+      <c r="P6" s="56"/>
+      <c r="Q6" s="56"/>
+      <c r="R6" s="56"/>
+      <c r="S6" s="56"/>
+      <c r="T6" s="56"/>
+      <c r="U6" s="56"/>
+      <c r="V6" s="56"/>
+      <c r="W6" s="56"/>
+      <c r="X6" s="56"/>
+      <c r="Y6" s="56"/>
+      <c r="Z6" s="56"/>
+      <c r="AA6" s="56"/>
+      <c r="AB6" s="56"/>
+      <c r="AC6" s="56"/>
+      <c r="AD6" s="56"/>
+      <c r="AE6" s="56"/>
+      <c r="AF6" s="56"/>
+      <c r="AG6" s="56"/>
+      <c r="AH6" s="56"/>
+      <c r="AI6" s="56"/>
     </row>
     <row r="7" spans="1:35" x14ac:dyDescent="0.3">
       <c r="G7" s="58"/>
@@ -12087,35 +12103,67 @@
       <c r="AH43" s="58"/>
       <c r="AI43" s="58"/>
     </row>
+    <row r="44" spans="7:35" x14ac:dyDescent="0.3">
+      <c r="G44" s="58"/>
+      <c r="H44" s="58"/>
+      <c r="I44" s="58"/>
+      <c r="J44" s="58"/>
+      <c r="K44" s="58"/>
+      <c r="L44" s="58"/>
+      <c r="M44" s="58"/>
+      <c r="N44" s="58"/>
+      <c r="O44" s="58"/>
+      <c r="P44" s="58"/>
+      <c r="Q44" s="58"/>
+      <c r="R44" s="58"/>
+      <c r="S44" s="58"/>
+      <c r="T44" s="58"/>
+      <c r="U44" s="58"/>
+      <c r="V44" s="58"/>
+      <c r="W44" s="58"/>
+      <c r="X44" s="58"/>
+      <c r="Y44" s="58"/>
+      <c r="Z44" s="58"/>
+      <c r="AA44" s="58"/>
+      <c r="AB44" s="58"/>
+      <c r="AC44" s="58"/>
+      <c r="AD44" s="58"/>
+      <c r="AE44" s="58"/>
+      <c r="AF44" s="58"/>
+      <c r="AG44" s="58"/>
+      <c r="AH44" s="58"/>
+      <c r="AI44" s="58"/>
+    </row>
   </sheetData>
   <mergeCells count="8">
     <mergeCell ref="C1:F1"/>
     <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A2:A5"/>
-    <mergeCell ref="B2:B5"/>
-    <mergeCell ref="C2:C5"/>
-    <mergeCell ref="D2:D5"/>
-    <mergeCell ref="E2:E5"/>
-    <mergeCell ref="F2:F5"/>
+    <mergeCell ref="A2:A6"/>
+    <mergeCell ref="B2:B6"/>
+    <mergeCell ref="C2:C6"/>
+    <mergeCell ref="D2:D6"/>
+    <mergeCell ref="E2:E6"/>
+    <mergeCell ref="F2:F6"/>
   </mergeCells>
-  <dataValidations xWindow="76" yWindow="363" count="7">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Write the core_name or select from the drop-down menu the cores you have in the Workbook._x000a_Make sure that the core name matches with its metadata given in GEOPOINTS_CORES sheet" sqref="B2:B3" xr:uid="{7D2146A4-D1D6-4E3B-BDAD-27D456B89F1C}"/>
+  <dataValidations xWindow="76" yWindow="363" count="8">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Write the core_name or select from the drop-down menu the cores you have in the Workbook._x000a_Make sure that the core name matches with its metadata given in GEOPOINTS_CORES sheet" sqref="B2:B4" xr:uid="{7D2146A4-D1D6-4E3B-BDAD-27D456B89F1C}"/>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Core analysis category" prompt="Choose from the drop-down list the analysis category the variable belongs to" sqref="G1:AI1" xr:uid="{2CF7E750-B721-48AF-B140-B0C26E790AFE}">
       <formula1>core_analyses_type</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Core analysis" prompt="Choose from the drop-down menu the variable to be added" sqref="G2:AI2" xr:uid="{B0700C72-7D5C-46E0-BFAD-D1DB2660C37D}">
       <formula1>INDIRECT(G$1)</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Name of user who is entering data" sqref="A6:A1048576" xr:uid="{33919C42-5417-487B-BA1B-79EBCC42E970}"/>
-    <dataValidation type="list" allowBlank="1" sqref="G6:AI1048576" xr:uid="{31A6BBB2-02F7-431D-8499-42E40851220A}">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Name of user who is entering data" sqref="A7:A1048576" xr:uid="{33919C42-5417-487B-BA1B-79EBCC42E970}"/>
+    <dataValidation type="list" allowBlank="1" sqref="G7:AI1048576" xr:uid="{31A6BBB2-02F7-431D-8499-42E40851220A}">
       <formula1>INDIRECT(G$2)</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Material analyzed" prompt="Choose from the drop-down menu the material analyzed (i.e. bulk, OC, sand, etc.). If left blank, the default material analyzed (bulk) will be used. " sqref="G4:AI4" xr:uid="{D4905C1B-E491-4C12-B759-9E966D6E43FD}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Material analyzed" prompt="Choose from the drop-down menu the material analyzed (i.e. bulk, OC, sand, etc.). If left blank, the default material analyzed (bulk) will be used. " sqref="G5:AI5" xr:uid="{D4905C1B-E491-4C12-B759-9E966D6E43FD}">
       <formula1>material_analyzed</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Method" prompt="Choose from the drop-down menu the method used to analyze the variable. If unknown, choose _unknown. If the method used is not in the drop-down list, please contact mosaic@erdw.ethz.ch" sqref="G3:AI3" xr:uid="{9B17DCDE-37E9-41D0-98F9-26A0705C15B8}">
       <formula1>INDIRECT(G$2)</formula1>
     </dataValidation>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Method details" prompt="If known, add any additional information about the method used to obtain the variable, such as the model of the analyzer." sqref="G4:AI4" xr:uid="{671D7CD0-13B4-45B2-921A-E5EB66A17497}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -12127,37 +12175,37 @@
           <x14:formula1>
             <xm:f>SET_VARIABLES!$A$2:$A$3</xm:f>
           </x14:formula1>
-          <xm:sqref>C6:C1048576</xm:sqref>
+          <xm:sqref>C7:C1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Write the article name or select from the drop-down menu the articles you have in the Workbook._x000a_Make sure that the article name matches with its metadata given in Article_Author sheet" xr:uid="{8ED4D961-4A65-40A1-8807-CD6F51264743}">
           <x14:formula1>
             <xm:f>ARTICLE_AUTHOR!$B$3:$B$11</xm:f>
           </x14:formula1>
-          <xm:sqref>D6:D1048576</xm:sqref>
+          <xm:sqref>D7:D1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Write the author/contact person of the core, or select from the drop-down menu the authors you have in the Workbook._x000a_Make sure that the author name matches with its metadata given in Article_Author sheet" xr:uid="{C6EA44F1-12DE-43A1-9351-6E8D2CDBD497}">
           <x14:formula1>
             <xm:f>ARTICLE_AUTHOR!$G$3:$G$11</xm:f>
           </x14:formula1>
-          <xm:sqref>F6:F1048576</xm:sqref>
+          <xm:sqref>F7:F1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Write the author/contact person of the core, or select from the drop-down menu the authors you have in the Workbook._x000a_Make sure that the author name matches with its metadata given in Article_Author sheet" xr:uid="{8D3331D8-B31F-4C5A-9DEF-A64F982A0076}">
           <x14:formula1>
             <xm:f>ARTICLE_AUTHOR!$F$3:$F$11</xm:f>
           </x14:formula1>
-          <xm:sqref>E6:E1048576</xm:sqref>
+          <xm:sqref>E7:E1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Write the core name or select from the drop-down menu the cores you have in the Workbook._x000a_Make sure that the core name matches with its metadata given in GEOPOINTS_CORES sheet" xr:uid="{1BC3CC47-CC25-4FD1-B529-1E8DB05AED98}">
           <x14:formula1>
             <xm:f>GEOPOINTS_CORES!$B$3:$B$1048576</xm:f>
           </x14:formula1>
-          <xm:sqref>B6:B1048576</xm:sqref>
+          <xm:sqref>B7:B1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Raw / calculated data" prompt="Specify if the data provided has been extracted directly from the source (i.e. paper) or is calculated using available data. If left blank, default of &quot;raw data&quot; will be used. " xr:uid="{020D4D59-E2D5-48DF-9D12-902C890A1988}">
           <x14:formula1>
             <xm:f>SET_VARIABLES!$BE$2:$BE$3</xm:f>
           </x14:formula1>
-          <xm:sqref>G5:AI5</xm:sqref>
+          <xm:sqref>G6:AI6</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -12170,11 +12218,11 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:CB52"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="3" ySplit="6" topLeftCell="D7" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane xSplit="3" ySplit="6" topLeftCell="F7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="D8" sqref="D8"/>
+      <selection pane="bottomRight" activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -12195,23 +12243,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:80" s="79" customFormat="1" ht="20.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="97" t="s">
+      <c r="A1" s="98" t="s">
         <v>2686</v>
       </c>
-      <c r="B1" s="98"/>
-      <c r="C1" s="99"/>
-      <c r="D1" s="97" t="s">
+      <c r="B1" s="99"/>
+      <c r="C1" s="100"/>
+      <c r="D1" s="98" t="s">
         <v>2676</v>
       </c>
-      <c r="E1" s="98"/>
-      <c r="F1" s="98"/>
-      <c r="G1" s="99"/>
-      <c r="H1" s="100" t="s">
+      <c r="E1" s="99"/>
+      <c r="F1" s="99"/>
+      <c r="G1" s="100"/>
+      <c r="H1" s="101" t="s">
         <v>2678</v>
       </c>
-      <c r="I1" s="101"/>
-      <c r="J1" s="101"/>
-      <c r="K1" s="102"/>
+      <c r="I1" s="102"/>
+      <c r="J1" s="102"/>
+      <c r="K1" s="103"/>
       <c r="L1" s="79" t="s">
         <v>1840</v>
       </c>
@@ -12229,37 +12277,37 @@
       </c>
     </row>
     <row r="2" spans="1:80" s="81" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="103" t="s">
+      <c r="A2" s="104" t="s">
         <v>2565</v>
       </c>
-      <c r="B2" s="106" t="s">
+      <c r="B2" s="107" t="s">
         <v>1825</v>
       </c>
-      <c r="C2" s="109" t="s">
+      <c r="C2" s="110" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="104" t="s">
+      <c r="D2" s="105" t="s">
         <v>1834</v>
       </c>
-      <c r="E2" s="107" t="s">
+      <c r="E2" s="108" t="s">
         <v>2684</v>
       </c>
-      <c r="F2" s="107" t="s">
+      <c r="F2" s="108" t="s">
         <v>1823</v>
       </c>
-      <c r="G2" s="110" t="s">
+      <c r="G2" s="111" t="s">
         <v>1824</v>
       </c>
-      <c r="H2" s="103" t="s">
+      <c r="H2" s="104" t="s">
         <v>1835</v>
       </c>
-      <c r="I2" s="106" t="s">
+      <c r="I2" s="107" t="s">
         <v>1836</v>
       </c>
-      <c r="J2" s="106" t="s">
+      <c r="J2" s="107" t="s">
         <v>1837</v>
       </c>
-      <c r="K2" s="112" t="s">
+      <c r="K2" s="113" t="s">
         <v>1838</v>
       </c>
       <c r="L2" s="80" t="s">
@@ -12343,17 +12391,17 @@
       <c r="CB2" s="80"/>
     </row>
     <row r="3" spans="1:80" s="81" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="104"/>
-      <c r="B3" s="107"/>
-      <c r="C3" s="110"/>
-      <c r="D3" s="104"/>
-      <c r="E3" s="107"/>
-      <c r="F3" s="107"/>
-      <c r="G3" s="110"/>
-      <c r="H3" s="104"/>
-      <c r="I3" s="107"/>
-      <c r="J3" s="107"/>
-      <c r="K3" s="113"/>
+      <c r="A3" s="105"/>
+      <c r="B3" s="108"/>
+      <c r="C3" s="111"/>
+      <c r="D3" s="105"/>
+      <c r="E3" s="108"/>
+      <c r="F3" s="108"/>
+      <c r="G3" s="111"/>
+      <c r="H3" s="105"/>
+      <c r="I3" s="108"/>
+      <c r="J3" s="108"/>
+      <c r="K3" s="114"/>
       <c r="L3" s="80" t="s">
         <v>2934</v>
       </c>
@@ -12427,17 +12475,17 @@
       <c r="CB3" s="80"/>
     </row>
     <row r="4" spans="1:80" s="81" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="104"/>
-      <c r="B4" s="107"/>
-      <c r="C4" s="110"/>
-      <c r="D4" s="104"/>
-      <c r="E4" s="107"/>
-      <c r="F4" s="107"/>
-      <c r="G4" s="110"/>
-      <c r="H4" s="104"/>
-      <c r="I4" s="107"/>
-      <c r="J4" s="107"/>
-      <c r="K4" s="113"/>
+      <c r="A4" s="105"/>
+      <c r="B4" s="108"/>
+      <c r="C4" s="111"/>
+      <c r="D4" s="105"/>
+      <c r="E4" s="108"/>
+      <c r="F4" s="108"/>
+      <c r="G4" s="111"/>
+      <c r="H4" s="105"/>
+      <c r="I4" s="108"/>
+      <c r="J4" s="108"/>
+      <c r="K4" s="114"/>
       <c r="L4" s="80"/>
       <c r="M4" s="80"/>
       <c r="N4" s="80"/>
@@ -12509,17 +12557,17 @@
       <c r="CB4" s="80"/>
     </row>
     <row r="5" spans="1:80" s="81" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="104"/>
-      <c r="B5" s="107"/>
-      <c r="C5" s="110"/>
-      <c r="D5" s="104"/>
-      <c r="E5" s="107"/>
-      <c r="F5" s="107"/>
-      <c r="G5" s="110"/>
-      <c r="H5" s="104"/>
-      <c r="I5" s="107"/>
-      <c r="J5" s="107"/>
-      <c r="K5" s="113"/>
+      <c r="A5" s="105"/>
+      <c r="B5" s="108"/>
+      <c r="C5" s="111"/>
+      <c r="D5" s="105"/>
+      <c r="E5" s="108"/>
+      <c r="F5" s="108"/>
+      <c r="G5" s="111"/>
+      <c r="H5" s="105"/>
+      <c r="I5" s="108"/>
+      <c r="J5" s="108"/>
+      <c r="K5" s="114"/>
       <c r="L5" s="80"/>
       <c r="M5" s="80"/>
       <c r="N5" s="80"/>
@@ -12591,17 +12639,17 @@
       <c r="CB5" s="80"/>
     </row>
     <row r="6" spans="1:80" s="81" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="105"/>
-      <c r="B6" s="108"/>
-      <c r="C6" s="111"/>
-      <c r="D6" s="105"/>
-      <c r="E6" s="108"/>
-      <c r="F6" s="108"/>
-      <c r="G6" s="111"/>
-      <c r="H6" s="105"/>
-      <c r="I6" s="108"/>
-      <c r="J6" s="108"/>
-      <c r="K6" s="114"/>
+      <c r="A6" s="106"/>
+      <c r="B6" s="109"/>
+      <c r="C6" s="112"/>
+      <c r="D6" s="106"/>
+      <c r="E6" s="109"/>
+      <c r="F6" s="109"/>
+      <c r="G6" s="112"/>
+      <c r="H6" s="106"/>
+      <c r="I6" s="109"/>
+      <c r="J6" s="109"/>
+      <c r="K6" s="115"/>
       <c r="L6" s="80"/>
       <c r="M6" s="80"/>
       <c r="N6" s="80"/>
@@ -14908,8 +14956,8 @@
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:HL277"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="CQ24" sqref="CQ24"/>
+    <sheetView topLeftCell="ER1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="GW19" sqref="GW19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -18639,6 +18687,9 @@
       <c r="FE7" s="85" t="s">
         <v>2030</v>
       </c>
+      <c r="FG7" t="s">
+        <v>3009</v>
+      </c>
       <c r="FT7" s="85" t="s">
         <v>3004</v>
       </c>
@@ -19607,8 +19658,8 @@
       <c r="FE10" s="85" t="s">
         <v>2216</v>
       </c>
-      <c r="GY10" t="s">
-        <v>2988</v>
+      <c r="GY10" s="88" t="s">
+        <v>3011</v>
       </c>
       <c r="GZ10" s="85" t="s">
         <v>2988</v>
@@ -19890,7 +19941,7 @@
         <v>2040</v>
       </c>
       <c r="GY11" t="s">
-        <v>2029</v>
+        <v>2988</v>
       </c>
       <c r="GZ11" s="85" t="s">
         <v>2029</v>
@@ -20156,7 +20207,7 @@
         <v>2041</v>
       </c>
       <c r="GY12" t="s">
-        <v>2030</v>
+        <v>2029</v>
       </c>
       <c r="GZ12" s="85" t="s">
         <v>2030</v>
@@ -20400,7 +20451,7 @@
         <v>2031</v>
       </c>
       <c r="GY13" t="s">
-        <v>2031</v>
+        <v>2030</v>
       </c>
       <c r="GZ13" s="85" t="s">
         <v>2031</v>
@@ -20616,7 +20667,7 @@
       <c r="EE14" s="46"/>
       <c r="EF14" s="46"/>
       <c r="GY14" t="s">
-        <v>2036</v>
+        <v>2031</v>
       </c>
       <c r="GZ14" s="85" t="s">
         <v>2036</v>
@@ -20818,7 +20869,7 @@
       <c r="EE15" s="46"/>
       <c r="EF15" s="46"/>
       <c r="GY15" t="s">
-        <v>2989</v>
+        <v>2036</v>
       </c>
       <c r="GZ15" s="85" t="s">
         <v>2990</v>
@@ -21014,8 +21065,8 @@
       <c r="ED16" s="12"/>
       <c r="EE16" s="46"/>
       <c r="EF16" s="46"/>
-      <c r="GY16" s="10" t="s">
-        <v>2259</v>
+      <c r="GY16" t="s">
+        <v>2989</v>
       </c>
       <c r="GZ16" s="10" t="s">
         <v>2259</v>
@@ -21202,7 +21253,7 @@
       <c r="EE17" s="46"/>
       <c r="EF17" s="46"/>
       <c r="GY17" s="10" t="s">
-        <v>2877</v>
+        <v>2259</v>
       </c>
       <c r="GZ17" s="10" t="s">
         <v>2877</v>
@@ -21381,6 +21432,12 @@
       <c r="ED18" s="12"/>
       <c r="EE18" s="46"/>
       <c r="EF18" s="46"/>
+      <c r="GY18" s="10" t="s">
+        <v>2877</v>
+      </c>
+      <c r="GZ18" s="10" t="s">
+        <v>3010</v>
+      </c>
     </row>
     <row r="19" spans="2:208" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
@@ -21550,6 +21607,9 @@
       <c r="ED19" s="12"/>
       <c r="EE19" s="46"/>
       <c r="EF19" s="46"/>
+      <c r="GY19" s="10" t="s">
+        <v>3010</v>
+      </c>
     </row>
     <row r="20" spans="2:208" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
@@ -22321,7 +22381,7 @@
       <c r="L27" t="s">
         <v>228</v>
       </c>
-      <c r="M27" s="115"/>
+      <c r="M27" s="116"/>
       <c r="O27" s="12" t="s">
         <v>822</v>
       </c>
@@ -22402,7 +22462,7 @@
       <c r="L28" t="s">
         <v>235</v>
       </c>
-      <c r="M28" s="115"/>
+      <c r="M28" s="116"/>
       <c r="O28" s="12" t="s">
         <v>1712</v>
       </c>
@@ -22798,7 +22858,7 @@
       <c r="L34" t="s">
         <v>276</v>
       </c>
-      <c r="M34" s="115"/>
+      <c r="M34" s="116"/>
       <c r="O34" s="12" t="s">
         <v>915</v>
       </c>
@@ -22857,7 +22917,7 @@
       <c r="L35" t="s">
         <v>283</v>
       </c>
-      <c r="M35" s="115"/>
+      <c r="M35" s="116"/>
       <c r="O35" s="12" t="s">
         <v>939</v>
       </c>
@@ -28323,7 +28383,6 @@
       <c r="DL277" s="45"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="F4/6G59ZVuOxlmG+BFCfQvPkU6LHvLGvrt24ZPCG8osbFyUjhNhUQ/JYSPKHjHMHd6FUbQUbs5wEJEXQKS6V8A==" saltValue="Ww5/mQMwKKD3rBaBVhLWXA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="2">
     <mergeCell ref="M27:M28"/>
     <mergeCell ref="M34:M35"/>

</xml_diff>

<commit_message>
Locked the VARIABLES sheet
</commit_message>
<xml_diff>
--- a/Excel_templates/MOSAIC_input_excel_file_2022.xlsx
+++ b/Excel_templates/MOSAIC_input_excel_file_2022.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sparadis\Documents\ETH\MOSAIC\MOSAIC_Client\Excel_templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED680B39-61C5-4895-80B5-E8A19738F792}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{178326A2-BFE4-42BB-BE28-E9CBC6CF812B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30204" yWindow="10044" windowWidth="40020" windowHeight="22296" tabRatio="694" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30204" yWindow="10044" windowWidth="40020" windowHeight="22296" tabRatio="694" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ARTICLE_AUTHOR" sheetId="3" r:id="rId1"/>
@@ -10257,7 +10257,7 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -10353,7 +10353,7 @@
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E3" sqref="E3"/>
+      <selection pane="bottomRight" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -10726,7 +10726,7 @@
       <pane xSplit="2" ySplit="6" topLeftCell="C7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="G1" sqref="G1"/>
+      <selection pane="bottomRight" activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -12218,11 +12218,11 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:CB52"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane xSplit="3" ySplit="6" topLeftCell="F7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="L4" sqref="L4"/>
+      <selection pane="bottomRight" activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -28383,6 +28383,7 @@
       <c r="DL277" s="45"/>
     </row>
   </sheetData>
+  <sheetProtection algorithmName="SHA-512" hashValue="Zb7QGKiIC6Wl2lyUtfjLF/D6ZW1H8inEEmfEH0uFndA4q5TvkmjTrzQQmfZOJ+6GvRKbzSPVryI/d8E16CwXwA==" saltValue="a2whRBu5crk7z/7hqsaMHg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="2">
     <mergeCell ref="M27:M28"/>
     <mergeCell ref="M34:M35"/>

</xml_diff>

<commit_message>
Added more methods to SAR and MAR
</commit_message>
<xml_diff>
--- a/Excel_templates/MOSAIC_input_excel_file_2022.xlsx
+++ b/Excel_templates/MOSAIC_input_excel_file_2022.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sparadis\Documents\ETH\MOSAIC\MOSAIC_Client\Excel_templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{178326A2-BFE4-42BB-BE28-E9CBC6CF812B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{8FACFBB9-8918-4CCC-AD2E-8686C6950B48}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30204" yWindow="10044" windowWidth="40020" windowHeight="22296" tabRatio="694" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30204" yWindow="10044" windowWidth="40020" windowHeight="22296" tabRatio="694" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ARTICLE_AUTHOR" sheetId="3" r:id="rId1"/>
@@ -19,8 +19,11 @@
     <sheet name="SAMPLE_ANALYSES" sheetId="7" r:id="rId4"/>
     <sheet name="SET_VARIABLES" sheetId="5" r:id="rId5"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId6"/>
+  </externalReferences>
   <definedNames>
-    <definedName name="Age_14C_ybp">SET_VARIABLES!$GZ$2:$GZ$17</definedName>
+    <definedName name="Age_14C_ybp">SET_VARIABLES!$GZ$2:$GZ$19</definedName>
     <definedName name="Argentina">SET_VARIABLES!$P$2:$P$8</definedName>
     <definedName name="Australia">SET_VARIABLES!$Q$2:$Q$28</definedName>
     <definedName name="Bangladesh">SET_VARIABLES!$R$2:$R$5</definedName>
@@ -77,7 +80,7 @@
     <definedName name="K38Et_ng_g">SET_VARIABLES!$HE$2:$HE$4</definedName>
     <definedName name="K38Me_ng_g">SET_VARIABLES!$HF$2:$HF$4</definedName>
     <definedName name="Lebanon">SET_VARIABLES!$AK$2:$AK$4</definedName>
-    <definedName name="MAR_g_cm2_yr">SET_VARIABLES!$GY$2:$GY$19</definedName>
+    <definedName name="MAR_g_cm2_yr">SET_VARIABLES!$GY$2:$GY$20</definedName>
     <definedName name="MAR_model">SET_VARIABLES!$BL$2:$BL$9</definedName>
     <definedName name="MAR_tracer">SET_VARIABLES!$BJ$2:$BJ$12</definedName>
     <definedName name="material_analyzed">SET_VARIABLES!$CM$2:$CM$29</definedName>
@@ -132,7 +135,7 @@
     <definedName name="sample_sedimentation_rate">SET_VARIABLES!$EV$2:$EV$5</definedName>
     <definedName name="Sample_sterols">SET_VARIABLES!$DR$2:$DR$10</definedName>
     <definedName name="sand_">SET_VARIABLES!$FL$2:$FL$4</definedName>
-    <definedName name="SAR_cm_yr">SET_VARIABLES!$GZ$2:$GZ$18</definedName>
+    <definedName name="SAR_cm_yr">SET_VARIABLES!$GZ$2:$GZ$20</definedName>
     <definedName name="SAR_model">SET_VARIABLES!$BK$2:$BK$9</definedName>
     <definedName name="SAR_tracer">SET_VARIABLES!$BJ$2:$BJ$12</definedName>
     <definedName name="silt_">SET_VARIABLES!$FM$2:$FM$4</definedName>
@@ -186,7 +189,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3927" uniqueCount="3012">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3930" uniqueCount="3011">
   <si>
     <t>sample_name</t>
   </si>
@@ -9219,16 +9222,13 @@
   </si>
   <si>
     <t>pollen</t>
-  </si>
-  <si>
-    <t>Pb-210 unknown</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="23" x14ac:knownFonts="1">
+  <fonts count="25">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -9380,6 +9380,16 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="AdvP70E4"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="TimesNewRoman"/>
     </font>
   </fonts>
   <fills count="14">
@@ -9695,7 +9705,7 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="117">
+  <cellXfs count="120">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="13" applyFont="1" applyFill="1" applyAlignment="1"/>
@@ -9914,6 +9924,11 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="16">
     <cellStyle name="20% - Accent1" xfId="3" builtinId="30" customBuiltin="1"/>
@@ -9955,6 +9970,27 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="ARTICLE_AUTHOR"/>
+      <sheetName val="GEOPOINTS_CORES"/>
+      <sheetName val="CORE_ANALYSES"/>
+      <sheetName val="SAMPLE_ANALYSES"/>
+      <sheetName val="SET_VARIABLES"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="3" refreshError="1"/>
+      <sheetData sheetId="4"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -10257,14 +10293,14 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="A3" sqref="A3:G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
   <cols>
     <col min="1" max="1" width="15.69921875" style="29" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="35.5" style="30" customWidth="1"/>
@@ -10277,7 +10313,7 @@
     <col min="9" max="16384" width="11.19921875" style="29"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="64" customFormat="1" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:8" s="64" customFormat="1" ht="20.399999999999999" thickBot="1">
       <c r="A1" s="89" t="s">
         <v>2674</v>
       </c>
@@ -10288,7 +10324,7 @@
       <c r="F1" s="89"/>
       <c r="G1" s="89"/>
     </row>
-    <row r="2" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" s="27" customFormat="1">
       <c r="A2" s="53" t="s">
         <v>2565</v>
       </c>
@@ -10314,15 +10350,16 @@
         <v>2845</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8">
       <c r="B3" s="28"/>
+      <c r="D3" s="88"/>
       <c r="E3" s="38"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8">
       <c r="B4" s="28"/>
       <c r="E4" s="40"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8">
       <c r="B6" s="28"/>
       <c r="E6" s="38"/>
     </row>
@@ -10333,7 +10370,7 @@
   <dataValidations count="7">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="If published, add title here." sqref="B3:B21" xr:uid="{726928EE-6022-4497-A773-A748CE1158EB}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="If published, add year of publication" sqref="C3:C21" xr:uid="{84FA4110-480C-48A7-BF55-0AFA90817B15}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="If published, add journal where it was published" sqref="D3:D21" xr:uid="{0C9B366E-479D-4C2B-AE48-2C587F10C94E}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="If published, add journal where it was published" sqref="D4:D21" xr:uid="{0C9B366E-479D-4C2B-AE48-2C587F10C94E}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="If available, please add article's DOI to fill in any missing metadata._x000a_Accepts articles that are indexed by Cross-Ref and PANGAEA" sqref="E4:E5 E7:E21" xr:uid="{933007B2-4396-46AD-979F-F8B269E7A170}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="If data is not published, please add here the contact person of the data._x000a_If data is published, this field will be ignored and all the authors will be included during data validation using the article's DOI." sqref="F3:G21" xr:uid="{53038C04-32DF-4B99-BAB1-3AB506AFD923}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Name of user who is entering data" sqref="A3:A1048576" xr:uid="{0ADA87D3-C0C6-4E0D-9F2A-A4CF37A8548E}"/>
@@ -10347,16 +10384,16 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:P27"/>
+  <dimension ref="A1:P15"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
   <cols>
     <col min="1" max="1" width="15.69921875" style="29" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22" style="29" customWidth="1"/>
@@ -10374,7 +10411,7 @@
     <col min="18" max="16384" width="11.19921875" style="29"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="63" customFormat="1" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:16" s="63" customFormat="1" ht="20.399999999999999" thickBot="1">
       <c r="A1" s="91" t="s">
         <v>2675</v>
       </c>
@@ -10396,7 +10433,7 @@
       <c r="O1" s="90"/>
       <c r="P1" s="90"/>
     </row>
-    <row r="2" spans="1:16" s="66" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" s="66" customFormat="1">
       <c r="A2" s="62" t="s">
         <v>2565</v>
       </c>
@@ -10446,15 +10483,18 @@
         <v>1830</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="B3" s="41"/>
-      <c r="C3" s="41"/>
+    <row r="3" spans="1:16">
+      <c r="C3" s="117"/>
       <c r="D3" s="41"/>
       <c r="E3" s="41"/>
       <c r="F3" s="49"/>
-      <c r="G3" s="41"/>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="G3" s="118"/>
+      <c r="J3" s="88"/>
+      <c r="N3" s="119"/>
+      <c r="O3" s="32"/>
+      <c r="P3" s="32"/>
+    </row>
+    <row r="4" spans="1:16">
       <c r="B4" s="41"/>
       <c r="C4" s="41"/>
       <c r="D4" s="41"/>
@@ -10462,7 +10502,7 @@
       <c r="F4" s="49"/>
       <c r="G4" s="41"/>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16">
       <c r="B5" s="41"/>
       <c r="C5" s="41"/>
       <c r="D5" s="41"/>
@@ -10470,7 +10510,7 @@
       <c r="F5" s="49"/>
       <c r="G5" s="41"/>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16">
       <c r="B6" s="41"/>
       <c r="C6" s="41"/>
       <c r="D6" s="41"/>
@@ -10478,7 +10518,7 @@
       <c r="F6" s="49"/>
       <c r="G6" s="41"/>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16">
       <c r="B7" s="41"/>
       <c r="C7" s="41"/>
       <c r="D7" s="41"/>
@@ -10486,7 +10526,7 @@
       <c r="F7" s="49"/>
       <c r="G7" s="41"/>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16">
       <c r="B8" s="41"/>
       <c r="C8" s="41"/>
       <c r="D8" s="41"/>
@@ -10494,7 +10534,7 @@
       <c r="F8" s="49"/>
       <c r="G8" s="41"/>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16">
       <c r="B9" s="41"/>
       <c r="C9" s="41"/>
       <c r="D9" s="41"/>
@@ -10502,7 +10542,7 @@
       <c r="F9" s="49"/>
       <c r="G9" s="41"/>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16">
       <c r="B10" s="41"/>
       <c r="C10" s="41"/>
       <c r="D10" s="41"/>
@@ -10510,7 +10550,7 @@
       <c r="F10" s="49"/>
       <c r="G10" s="41"/>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:16">
       <c r="B11" s="41"/>
       <c r="C11" s="41"/>
       <c r="D11" s="41"/>
@@ -10518,7 +10558,7 @@
       <c r="F11" s="49"/>
       <c r="G11" s="41"/>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:16">
       <c r="B12" s="41"/>
       <c r="C12" s="41"/>
       <c r="D12" s="41"/>
@@ -10526,7 +10566,7 @@
       <c r="F12" s="49"/>
       <c r="G12" s="41"/>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:16">
       <c r="B13" s="41"/>
       <c r="C13" s="41"/>
       <c r="D13" s="41"/>
@@ -10534,7 +10574,7 @@
       <c r="F13" s="49"/>
       <c r="G13" s="41"/>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:16">
       <c r="B14" s="41"/>
       <c r="C14" s="41"/>
       <c r="D14" s="41"/>
@@ -10542,109 +10582,13 @@
       <c r="F14" s="49"/>
       <c r="G14" s="41"/>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:16">
       <c r="B15" s="41"/>
       <c r="C15" s="41"/>
       <c r="D15" s="41"/>
       <c r="E15" s="41"/>
       <c r="F15" s="49"/>
       <c r="G15" s="41"/>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="B16" s="41"/>
-      <c r="C16" s="41"/>
-      <c r="D16" s="41"/>
-      <c r="E16" s="41"/>
-      <c r="F16" s="49"/>
-      <c r="G16" s="41"/>
-    </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B17" s="41"/>
-      <c r="C17" s="41"/>
-      <c r="D17" s="41"/>
-      <c r="E17" s="41"/>
-      <c r="F17" s="49"/>
-      <c r="G17" s="41"/>
-    </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B18" s="41"/>
-      <c r="C18" s="41"/>
-      <c r="D18" s="41"/>
-      <c r="E18" s="41"/>
-      <c r="F18" s="49"/>
-      <c r="G18" s="41"/>
-    </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B19" s="41"/>
-      <c r="C19" s="41"/>
-      <c r="D19" s="41"/>
-      <c r="E19" s="41"/>
-      <c r="F19" s="49"/>
-      <c r="G19" s="41"/>
-    </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B20" s="41"/>
-      <c r="C20" s="41"/>
-      <c r="D20" s="41"/>
-      <c r="E20" s="41"/>
-      <c r="F20" s="49"/>
-      <c r="G20" s="41"/>
-    </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B21" s="41"/>
-      <c r="C21" s="41"/>
-      <c r="D21" s="41"/>
-      <c r="E21" s="41"/>
-      <c r="F21" s="49"/>
-      <c r="G21" s="41"/>
-    </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B22" s="41"/>
-      <c r="C22" s="41"/>
-      <c r="D22" s="41"/>
-      <c r="E22" s="41"/>
-      <c r="F22" s="49"/>
-      <c r="G22" s="41"/>
-    </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B23" s="41"/>
-      <c r="C23" s="41"/>
-      <c r="D23" s="41"/>
-      <c r="E23" s="41"/>
-      <c r="F23" s="49"/>
-      <c r="G23" s="41"/>
-    </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B24" s="41"/>
-      <c r="C24" s="41"/>
-      <c r="D24" s="41"/>
-      <c r="E24" s="41"/>
-      <c r="F24" s="49"/>
-      <c r="G24" s="41"/>
-    </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B25" s="41"/>
-      <c r="C25" s="41"/>
-      <c r="D25" s="41"/>
-      <c r="E25" s="41"/>
-      <c r="F25" s="49"/>
-      <c r="G25" s="41"/>
-    </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B26" s="41"/>
-      <c r="C26" s="41"/>
-      <c r="D26" s="41"/>
-      <c r="E26" s="41"/>
-      <c r="F26" s="49"/>
-      <c r="G26" s="41"/>
-    </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B27" s="41"/>
-      <c r="C27" s="41"/>
-      <c r="D27" s="41"/>
-      <c r="E27" s="41"/>
-      <c r="F27" s="49"/>
-      <c r="G27" s="41"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -10654,23 +10598,24 @@
   <conditionalFormatting sqref="B2:B1048576">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
-  <dataValidations count="13">
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="WGS 84 decimal degrees" sqref="C28:C1048576" xr:uid="{0D6BC13B-7101-4C34-935E-0FF74090A779}">
+  <dataValidations count="14">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="WGS 84 decimal degrees" sqref="C16:C1048576" xr:uid="{0D6BC13B-7101-4C34-935E-0FF74090A779}">
       <formula1>-90</formula1>
       <formula2>90</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="WGS 84 decimal degrees" sqref="D28:D1048576" xr:uid="{4A2A535B-603A-4B6C-9867-3421E068207E}">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="WGS 84 decimal degrees" sqref="D16:D1048576" xr:uid="{4A2A535B-603A-4B6C-9867-3421E068207E}">
       <formula1>-180</formula1>
       <formula2>180</formula2>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Waer depth should be positive numbers." prompt="Water depth where the core was collected." sqref="G28:G1048576" xr:uid="{00CDF339-1F57-43C3-902E-FF6A4E068910}">
+    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Waer depth should be positive numbers." prompt="Water depth where the core was collected." sqref="G16:G1048576" xr:uid="{00CDF339-1F57-43C3-902E-FF6A4E068910}">
       <formula1>0</formula1>
-    </dataValidation>
-    <dataValidation type="textLength" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Maximum comment length is 200 characters" prompt="Add any additional information of the core" sqref="H3:H1048576" xr:uid="{FF2D52E6-EFBC-4479-B912-8CF305BA6CC6}">
-      <formula1>200</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please select geomorphological site if relevant. Choese _unkown if unknown. Otherwise leave blank." prompt="Please select geomorphological site if relevant. Choese _unkown if unknown. Otherwise leave blank." sqref="J3:J1048576" xr:uid="{C409BA21-827A-4726-997B-4DDCEB0E121E}">
       <formula1>geomorphological_site</formula1>
+    </dataValidation>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Name of the campaign cruise." sqref="N4:N1048576" xr:uid="{573E733B-B85F-488A-AB24-1BB2993B0FAE}"/>
+    <dataValidation type="textLength" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Maximum comment length is 200 characters" prompt="Add any additional information of the core" sqref="H3:H1048576" xr:uid="{FF2D52E6-EFBC-4479-B912-8CF305BA6CC6}">
+      <formula1>200</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Choose the country that the Research Vessel belongs to. If unknown, choose _unknown. If not listed here, check _other." prompt="Choose the country that the Research Vessel belongs to (extracted from Wikipedia, please contact mosaic@ethz.ch for any errors)" sqref="L3:L1048576" xr:uid="{6E72A734-A312-4B86-8990-BB5CA2135DC2}">
       <formula1>Research_Vessel_Countries</formula1>
@@ -10679,7 +10624,6 @@
       <formula1>1</formula1>
       <formula2>TODAY()</formula2>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Name of the campaign cruise." sqref="N3:N1048576" xr:uid="{573E733B-B85F-488A-AB24-1BB2993B0FAE}"/>
     <dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid date" error="Please introduce a date between 1/1/1900 and TODAY." prompt="If known, add the starting date of the cruise. Accepts dates between 1/1/1900 and TODAY." sqref="O3:O1048576" xr:uid="{D9536885-D4AA-431B-A11C-EEFC92030E57}">
       <formula1>1</formula1>
       <formula2>TODAY()</formula2>
@@ -10690,20 +10634,29 @@
     </dataValidation>
     <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="If available, specify the length of the core retrieved in cm." sqref="K3:K1048576" xr:uid="{6E15A0C0-8408-4930-8258-97C19A733952}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Name of user who is entering data" sqref="A3:A1048576" xr:uid="{B1508E14-6DD0-4DEF-BE9A-DA048D366864}"/>
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="In order to choose a research vessel, first choose the country it belongs to." sqref="M4:M1048576 M3" xr:uid="{74AEC9A0-D7E8-4D80-8B77-1F64526DD0B8}">
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="In order to choose a research vessel, first choose the country it belongs to." sqref="M3:M1048576" xr:uid="{74AEC9A0-D7E8-4D80-8B77-1F64526DD0B8}">
       <formula1>INDIRECT(L3)</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Write the core name or select from the drop-down menu the cores you have in the Workbook._x000a_Make sure that the core name matches with its metadata given in GEOPOINTS_CORES sheet" sqref="B3" xr:uid="{E17DEF85-BC0F-4D8D-B2CE-51E2C1FE041A}">
+      <formula1>$B$3:$B$1048576</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.70000000000000007" right="0.70000000000000007" top="0.75" bottom="0.75" header="0.30000000000000004" footer="0.30000000000000004"/>
   <pageSetup fitToWidth="0" fitToHeight="0" orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
         <x14:dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please select corer type if relevant. Chosse _unkown if unknown. Otherwise leave blank." prompt="Please select corer type if relevant. Chosse _unkown if unknown. Otherwise leave blank." xr:uid="{89ED9B77-757F-4A56-BFAB-AB1DC0DB17FB}">
           <x14:formula1>
             <xm:f>SET_VARIABLES!$J$2:$J$13</xm:f>
           </x14:formula1>
-          <xm:sqref>I3:I1048576</xm:sqref>
+          <xm:sqref>I4:I1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please select corer type if relevant. Chosse _unkown if unknown. Otherwise leave blank." prompt="Please select corer type if relevant. Chosse _unkown if unknown. Otherwise leave blank." xr:uid="{346EA44C-FE6C-4BA3-B6EC-C552F6E43517}">
+          <x14:formula1>
+            <xm:f>'C:\Users\sparadis\Documents\ETH\MOSAIC\MOSAIC_Server\new_data\[DeGeest_2008.xlsx]SET_VARIABLES'!#REF!</xm:f>
+          </x14:formula1>
+          <xm:sqref>I3</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" prompt="State whether the coordinates were obtained by georeferencing a map, or inferred (TRUE) or whether they were provided in tabular format (FALSE)." xr:uid="{FC9545BB-E799-4EF5-951B-5C2E1E979B37}">
           <x14:formula1>
@@ -10729,7 +10682,7 @@
       <selection pane="bottomRight" activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="15" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="15" defaultRowHeight="15.6"/>
   <cols>
     <col min="1" max="1" width="16" style="29" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.3984375" style="29" bestFit="1" customWidth="1"/>
@@ -10742,7 +10695,7 @@
     <col min="37" max="16384" width="15" style="29"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" s="55" customFormat="1" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:35" s="55" customFormat="1" ht="20.399999999999999" thickBot="1">
       <c r="A1" s="92" t="s">
         <v>2677</v>
       </c>
@@ -10757,7 +10710,7 @@
         <v>2221</v>
       </c>
     </row>
-    <row r="2" spans="1:35" ht="15.6" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:35" ht="15.6" customHeight="1" thickTop="1">
       <c r="A2" s="93" t="s">
         <v>2565</v>
       </c>
@@ -10808,7 +10761,7 @@
       <c r="AH2" s="56"/>
       <c r="AI2" s="56"/>
     </row>
-    <row r="3" spans="1:35" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:35" ht="15.6" customHeight="1">
       <c r="A3" s="94"/>
       <c r="B3" s="94"/>
       <c r="C3" s="94"/>
@@ -10845,7 +10798,7 @@
       <c r="AH3" s="56"/>
       <c r="AI3" s="56"/>
     </row>
-    <row r="4" spans="1:35" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:35" ht="15.6" customHeight="1">
       <c r="A4" s="94"/>
       <c r="B4" s="94"/>
       <c r="C4" s="94"/>
@@ -10882,7 +10835,7 @@
       <c r="AH4" s="56"/>
       <c r="AI4" s="56"/>
     </row>
-    <row r="5" spans="1:35" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:35" ht="15.6" customHeight="1">
       <c r="A5" s="95"/>
       <c r="B5" s="95"/>
       <c r="C5" s="95"/>
@@ -10919,7 +10872,7 @@
       <c r="AH5" s="56"/>
       <c r="AI5" s="56"/>
     </row>
-    <row r="6" spans="1:35" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:35" ht="15.6" customHeight="1">
       <c r="A6" s="95"/>
       <c r="B6" s="95"/>
       <c r="C6" s="95"/>
@@ -10956,7 +10909,7 @@
       <c r="AH6" s="56"/>
       <c r="AI6" s="56"/>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:35">
       <c r="G7" s="58"/>
       <c r="H7" s="58"/>
       <c r="I7" s="58"/>
@@ -10987,7 +10940,7 @@
       <c r="AH7" s="58"/>
       <c r="AI7" s="58"/>
     </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:35">
       <c r="G8" s="58"/>
       <c r="H8" s="58"/>
       <c r="I8" s="58"/>
@@ -11018,7 +10971,7 @@
       <c r="AH8" s="58"/>
       <c r="AI8" s="58"/>
     </row>
-    <row r="9" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:35">
       <c r="G9" s="58"/>
       <c r="H9" s="58"/>
       <c r="I9" s="58"/>
@@ -11049,7 +11002,7 @@
       <c r="AH9" s="58"/>
       <c r="AI9" s="58"/>
     </row>
-    <row r="10" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:35">
       <c r="G10" s="58"/>
       <c r="H10" s="58"/>
       <c r="I10" s="58"/>
@@ -11080,7 +11033,7 @@
       <c r="AH10" s="58"/>
       <c r="AI10" s="58"/>
     </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:35">
       <c r="G11" s="58"/>
       <c r="H11" s="58"/>
       <c r="I11" s="58"/>
@@ -11111,7 +11064,7 @@
       <c r="AH11" s="58"/>
       <c r="AI11" s="58"/>
     </row>
-    <row r="12" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:35">
       <c r="G12" s="58"/>
       <c r="H12" s="58"/>
       <c r="I12" s="58"/>
@@ -11142,7 +11095,7 @@
       <c r="AH12" s="58"/>
       <c r="AI12" s="58"/>
     </row>
-    <row r="13" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:35">
       <c r="G13" s="58"/>
       <c r="H13" s="58"/>
       <c r="I13" s="58"/>
@@ -11173,7 +11126,7 @@
       <c r="AH13" s="58"/>
       <c r="AI13" s="58"/>
     </row>
-    <row r="14" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:35">
       <c r="G14" s="58"/>
       <c r="H14" s="58"/>
       <c r="I14" s="58"/>
@@ -11204,7 +11157,7 @@
       <c r="AH14" s="58"/>
       <c r="AI14" s="58"/>
     </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:35">
       <c r="G15" s="58"/>
       <c r="H15" s="58"/>
       <c r="I15" s="58"/>
@@ -11235,7 +11188,7 @@
       <c r="AH15" s="58"/>
       <c r="AI15" s="58"/>
     </row>
-    <row r="16" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:35">
       <c r="G16" s="58"/>
       <c r="H16" s="58"/>
       <c r="I16" s="58"/>
@@ -11266,7 +11219,7 @@
       <c r="AH16" s="58"/>
       <c r="AI16" s="58"/>
     </row>
-    <row r="17" spans="7:35" x14ac:dyDescent="0.3">
+    <row r="17" spans="7:35">
       <c r="G17" s="58"/>
       <c r="H17" s="58"/>
       <c r="I17" s="58"/>
@@ -11297,7 +11250,7 @@
       <c r="AH17" s="58"/>
       <c r="AI17" s="58"/>
     </row>
-    <row r="18" spans="7:35" x14ac:dyDescent="0.3">
+    <row r="18" spans="7:35">
       <c r="G18" s="58"/>
       <c r="H18" s="58"/>
       <c r="I18" s="58"/>
@@ -11328,7 +11281,7 @@
       <c r="AH18" s="58"/>
       <c r="AI18" s="58"/>
     </row>
-    <row r="19" spans="7:35" x14ac:dyDescent="0.3">
+    <row r="19" spans="7:35">
       <c r="G19" s="58"/>
       <c r="H19" s="58"/>
       <c r="I19" s="58"/>
@@ -11359,7 +11312,7 @@
       <c r="AH19" s="58"/>
       <c r="AI19" s="58"/>
     </row>
-    <row r="20" spans="7:35" x14ac:dyDescent="0.3">
+    <row r="20" spans="7:35">
       <c r="G20" s="58"/>
       <c r="H20" s="58"/>
       <c r="I20" s="58"/>
@@ -11390,7 +11343,7 @@
       <c r="AH20" s="58"/>
       <c r="AI20" s="58"/>
     </row>
-    <row r="21" spans="7:35" x14ac:dyDescent="0.3">
+    <row r="21" spans="7:35">
       <c r="G21" s="58"/>
       <c r="H21" s="58"/>
       <c r="I21" s="58"/>
@@ -11421,7 +11374,7 @@
       <c r="AH21" s="58"/>
       <c r="AI21" s="58"/>
     </row>
-    <row r="22" spans="7:35" x14ac:dyDescent="0.3">
+    <row r="22" spans="7:35">
       <c r="G22" s="58"/>
       <c r="H22" s="58"/>
       <c r="I22" s="58"/>
@@ -11452,7 +11405,7 @@
       <c r="AH22" s="58"/>
       <c r="AI22" s="58"/>
     </row>
-    <row r="23" spans="7:35" x14ac:dyDescent="0.3">
+    <row r="23" spans="7:35">
       <c r="G23" s="58"/>
       <c r="H23" s="58"/>
       <c r="I23" s="58"/>
@@ -11483,7 +11436,7 @@
       <c r="AH23" s="58"/>
       <c r="AI23" s="58"/>
     </row>
-    <row r="24" spans="7:35" x14ac:dyDescent="0.3">
+    <row r="24" spans="7:35">
       <c r="G24" s="58"/>
       <c r="H24" s="58"/>
       <c r="I24" s="58"/>
@@ -11514,7 +11467,7 @@
       <c r="AH24" s="58"/>
       <c r="AI24" s="58"/>
     </row>
-    <row r="25" spans="7:35" x14ac:dyDescent="0.3">
+    <row r="25" spans="7:35">
       <c r="G25" s="58"/>
       <c r="H25" s="58"/>
       <c r="I25" s="58"/>
@@ -11545,7 +11498,7 @@
       <c r="AH25" s="58"/>
       <c r="AI25" s="58"/>
     </row>
-    <row r="26" spans="7:35" x14ac:dyDescent="0.3">
+    <row r="26" spans="7:35">
       <c r="G26" s="58"/>
       <c r="H26" s="58"/>
       <c r="I26" s="58"/>
@@ -11576,7 +11529,7 @@
       <c r="AH26" s="58"/>
       <c r="AI26" s="58"/>
     </row>
-    <row r="27" spans="7:35" x14ac:dyDescent="0.3">
+    <row r="27" spans="7:35">
       <c r="G27" s="58"/>
       <c r="H27" s="58"/>
       <c r="I27" s="58"/>
@@ -11607,7 +11560,7 @@
       <c r="AH27" s="58"/>
       <c r="AI27" s="58"/>
     </row>
-    <row r="28" spans="7:35" x14ac:dyDescent="0.3">
+    <row r="28" spans="7:35">
       <c r="G28" s="58"/>
       <c r="H28" s="58"/>
       <c r="I28" s="58"/>
@@ -11638,7 +11591,7 @@
       <c r="AH28" s="58"/>
       <c r="AI28" s="58"/>
     </row>
-    <row r="29" spans="7:35" x14ac:dyDescent="0.3">
+    <row r="29" spans="7:35">
       <c r="G29" s="58"/>
       <c r="H29" s="58"/>
       <c r="I29" s="58"/>
@@ -11669,7 +11622,7 @@
       <c r="AH29" s="58"/>
       <c r="AI29" s="58"/>
     </row>
-    <row r="30" spans="7:35" x14ac:dyDescent="0.3">
+    <row r="30" spans="7:35">
       <c r="G30" s="58"/>
       <c r="H30" s="58"/>
       <c r="I30" s="58"/>
@@ -11700,7 +11653,7 @@
       <c r="AH30" s="58"/>
       <c r="AI30" s="58"/>
     </row>
-    <row r="31" spans="7:35" x14ac:dyDescent="0.3">
+    <row r="31" spans="7:35">
       <c r="G31" s="58"/>
       <c r="H31" s="58"/>
       <c r="I31" s="58"/>
@@ -11731,7 +11684,7 @@
       <c r="AH31" s="58"/>
       <c r="AI31" s="58"/>
     </row>
-    <row r="32" spans="7:35" x14ac:dyDescent="0.3">
+    <row r="32" spans="7:35">
       <c r="G32" s="58"/>
       <c r="H32" s="58"/>
       <c r="I32" s="58"/>
@@ -11762,7 +11715,7 @@
       <c r="AH32" s="58"/>
       <c r="AI32" s="58"/>
     </row>
-    <row r="33" spans="7:35" x14ac:dyDescent="0.3">
+    <row r="33" spans="7:35">
       <c r="G33" s="58"/>
       <c r="H33" s="58"/>
       <c r="I33" s="58"/>
@@ -11793,7 +11746,7 @@
       <c r="AH33" s="58"/>
       <c r="AI33" s="58"/>
     </row>
-    <row r="34" spans="7:35" x14ac:dyDescent="0.3">
+    <row r="34" spans="7:35">
       <c r="G34" s="58"/>
       <c r="H34" s="58"/>
       <c r="I34" s="58"/>
@@ -11824,7 +11777,7 @@
       <c r="AH34" s="58"/>
       <c r="AI34" s="58"/>
     </row>
-    <row r="35" spans="7:35" x14ac:dyDescent="0.3">
+    <row r="35" spans="7:35">
       <c r="G35" s="58"/>
       <c r="H35" s="58"/>
       <c r="I35" s="58"/>
@@ -11855,7 +11808,7 @@
       <c r="AH35" s="58"/>
       <c r="AI35" s="58"/>
     </row>
-    <row r="36" spans="7:35" x14ac:dyDescent="0.3">
+    <row r="36" spans="7:35">
       <c r="G36" s="58"/>
       <c r="H36" s="58"/>
       <c r="I36" s="58"/>
@@ -11886,7 +11839,7 @@
       <c r="AH36" s="58"/>
       <c r="AI36" s="58"/>
     </row>
-    <row r="37" spans="7:35" x14ac:dyDescent="0.3">
+    <row r="37" spans="7:35">
       <c r="G37" s="58"/>
       <c r="H37" s="58"/>
       <c r="I37" s="58"/>
@@ -11917,7 +11870,7 @@
       <c r="AH37" s="58"/>
       <c r="AI37" s="58"/>
     </row>
-    <row r="38" spans="7:35" x14ac:dyDescent="0.3">
+    <row r="38" spans="7:35">
       <c r="G38" s="58"/>
       <c r="H38" s="58"/>
       <c r="I38" s="58"/>
@@ -11948,7 +11901,7 @@
       <c r="AH38" s="58"/>
       <c r="AI38" s="58"/>
     </row>
-    <row r="39" spans="7:35" x14ac:dyDescent="0.3">
+    <row r="39" spans="7:35">
       <c r="G39" s="58"/>
       <c r="H39" s="58"/>
       <c r="I39" s="58"/>
@@ -11979,7 +11932,7 @@
       <c r="AH39" s="58"/>
       <c r="AI39" s="58"/>
     </row>
-    <row r="40" spans="7:35" x14ac:dyDescent="0.3">
+    <row r="40" spans="7:35">
       <c r="G40" s="58"/>
       <c r="H40" s="58"/>
       <c r="I40" s="58"/>
@@ -12010,7 +11963,7 @@
       <c r="AH40" s="58"/>
       <c r="AI40" s="58"/>
     </row>
-    <row r="41" spans="7:35" x14ac:dyDescent="0.3">
+    <row r="41" spans="7:35">
       <c r="G41" s="58"/>
       <c r="H41" s="58"/>
       <c r="I41" s="58"/>
@@ -12041,7 +11994,7 @@
       <c r="AH41" s="58"/>
       <c r="AI41" s="58"/>
     </row>
-    <row r="42" spans="7:35" x14ac:dyDescent="0.3">
+    <row r="42" spans="7:35">
       <c r="G42" s="58"/>
       <c r="H42" s="58"/>
       <c r="I42" s="58"/>
@@ -12072,7 +12025,7 @@
       <c r="AH42" s="58"/>
       <c r="AI42" s="58"/>
     </row>
-    <row r="43" spans="7:35" x14ac:dyDescent="0.3">
+    <row r="43" spans="7:35">
       <c r="G43" s="58"/>
       <c r="H43" s="58"/>
       <c r="I43" s="58"/>
@@ -12103,7 +12056,7 @@
       <c r="AH43" s="58"/>
       <c r="AI43" s="58"/>
     </row>
-    <row r="44" spans="7:35" x14ac:dyDescent="0.3">
+    <row r="44" spans="7:35">
       <c r="G44" s="58"/>
       <c r="H44" s="58"/>
       <c r="I44" s="58"/>
@@ -12195,17 +12148,17 @@
           </x14:formula1>
           <xm:sqref>E7:E1048576</xm:sqref>
         </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Raw / calculated data" prompt="Specify if the data provided has been extracted directly from the source (i.e. paper) or is calculated using available data. If left blank, default of &quot;raw data&quot; will be used. " xr:uid="{020D4D59-E2D5-48DF-9D12-902C890A1988}">
+          <x14:formula1>
+            <xm:f>SET_VARIABLES!$BE$2:$BE$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>G6:AI6</xm:sqref>
+        </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Write the core name or select from the drop-down menu the cores you have in the Workbook._x000a_Make sure that the core name matches with its metadata given in GEOPOINTS_CORES sheet" xr:uid="{1BC3CC47-CC25-4FD1-B529-1E8DB05AED98}">
           <x14:formula1>
             <xm:f>GEOPOINTS_CORES!$B$3:$B$1048576</xm:f>
           </x14:formula1>
           <xm:sqref>B7:B1048576</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Raw / calculated data" prompt="Specify if the data provided has been extracted directly from the source (i.e. paper) or is calculated using available data. If left blank, default of &quot;raw data&quot; will be used. " xr:uid="{020D4D59-E2D5-48DF-9D12-902C890A1988}">
-          <x14:formula1>
-            <xm:f>SET_VARIABLES!$BE$2:$BE$3</xm:f>
-          </x14:formula1>
-          <xm:sqref>G6:AI6</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -12218,14 +12171,14 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:CB52"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="3" ySplit="6" topLeftCell="F7" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane xSplit="3" ySplit="6" topLeftCell="D7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
       <selection pane="bottomRight" activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="15" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="15" defaultRowHeight="15.6"/>
   <cols>
     <col min="1" max="1" width="17.69921875" style="29" customWidth="1"/>
     <col min="2" max="3" width="15" style="29"/>
@@ -12242,7 +12195,7 @@
     <col min="81" max="16384" width="15" style="29"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:80" s="79" customFormat="1" ht="20.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:80" s="79" customFormat="1" ht="20.399999999999999" customHeight="1" thickBot="1">
       <c r="A1" s="98" t="s">
         <v>2686</v>
       </c>
@@ -12261,7 +12214,7 @@
       <c r="J1" s="102"/>
       <c r="K1" s="103"/>
       <c r="L1" s="79" t="s">
-        <v>1840</v>
+        <v>2951</v>
       </c>
       <c r="M1" s="79" t="s">
         <v>1840</v>
@@ -12276,7 +12229,7 @@
         <v>2951</v>
       </c>
     </row>
-    <row r="2" spans="1:80" s="81" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:80" s="81" customFormat="1">
       <c r="A2" s="104" t="s">
         <v>2565</v>
       </c>
@@ -12311,7 +12264,7 @@
         <v>1838</v>
       </c>
       <c r="L2" s="80" t="s">
-        <v>2052</v>
+        <v>1752</v>
       </c>
       <c r="M2" s="80" t="s">
         <v>2193</v>
@@ -12390,7 +12343,7 @@
       <c r="CA2" s="80"/>
       <c r="CB2" s="80"/>
     </row>
-    <row r="3" spans="1:80" s="81" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:80" s="81" customFormat="1">
       <c r="A3" s="105"/>
       <c r="B3" s="108"/>
       <c r="C3" s="111"/>
@@ -12403,7 +12356,7 @@
       <c r="J3" s="108"/>
       <c r="K3" s="114"/>
       <c r="L3" s="80" t="s">
-        <v>2934</v>
+        <v>2974</v>
       </c>
       <c r="M3" s="80"/>
       <c r="N3" s="80"/>
@@ -12474,7 +12427,7 @@
       <c r="CA3" s="80"/>
       <c r="CB3" s="80"/>
     </row>
-    <row r="4" spans="1:80" s="81" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:80" s="81" customFormat="1">
       <c r="A4" s="105"/>
       <c r="B4" s="108"/>
       <c r="C4" s="111"/>
@@ -12556,7 +12509,7 @@
       <c r="CA4" s="80"/>
       <c r="CB4" s="80"/>
     </row>
-    <row r="5" spans="1:80" s="81" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:80" s="81" customFormat="1">
       <c r="A5" s="105"/>
       <c r="B5" s="108"/>
       <c r="C5" s="111"/>
@@ -12638,7 +12591,7 @@
       <c r="CA5" s="80"/>
       <c r="CB5" s="80"/>
     </row>
-    <row r="6" spans="1:80" s="81" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:80" s="81" customFormat="1" ht="16.2" thickBot="1">
       <c r="A6" s="106"/>
       <c r="B6" s="109"/>
       <c r="C6" s="112"/>
@@ -12720,7 +12673,7 @@
       <c r="CA6" s="80"/>
       <c r="CB6" s="80"/>
     </row>
-    <row r="7" spans="1:80" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:80">
       <c r="H7" s="41"/>
       <c r="I7" s="39"/>
       <c r="L7" s="58"/>
@@ -12793,10 +12746,10 @@
       <c r="CA7" s="58"/>
       <c r="CB7" s="58"/>
     </row>
-    <row r="8" spans="1:80" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:80">
       <c r="H8" s="41"/>
       <c r="I8" s="74"/>
-      <c r="L8" s="59"/>
+      <c r="L8" s="58"/>
       <c r="M8" s="41"/>
       <c r="N8" s="60"/>
       <c r="O8" s="60"/>
@@ -12866,10 +12819,10 @@
       <c r="CA8" s="59"/>
       <c r="CB8" s="59"/>
     </row>
-    <row r="9" spans="1:80" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:80">
       <c r="H9" s="41"/>
       <c r="I9" s="74"/>
-      <c r="L9" s="59"/>
+      <c r="L9" s="58"/>
       <c r="M9" s="41"/>
       <c r="N9" s="60"/>
       <c r="O9" s="60"/>
@@ -12939,10 +12892,10 @@
       <c r="CA9" s="59"/>
       <c r="CB9" s="59"/>
     </row>
-    <row r="10" spans="1:80" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:80">
       <c r="H10" s="41"/>
       <c r="I10" s="74"/>
-      <c r="L10" s="41"/>
+      <c r="L10" s="58"/>
       <c r="M10" s="41"/>
       <c r="N10" s="41"/>
       <c r="O10" s="60"/>
@@ -13012,10 +12965,10 @@
       <c r="CA10" s="59"/>
       <c r="CB10" s="59"/>
     </row>
-    <row r="11" spans="1:80" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:80">
       <c r="H11" s="41"/>
       <c r="I11" s="74"/>
-      <c r="L11" s="59"/>
+      <c r="L11" s="58"/>
       <c r="M11" s="41"/>
       <c r="N11" s="85"/>
       <c r="O11" s="60"/>
@@ -13085,10 +13038,10 @@
       <c r="CA11" s="59"/>
       <c r="CB11" s="59"/>
     </row>
-    <row r="12" spans="1:80" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:80">
       <c r="H12" s="41"/>
       <c r="I12" s="74"/>
-      <c r="L12" s="59"/>
+      <c r="L12" s="58"/>
       <c r="M12" s="41"/>
       <c r="N12" s="60"/>
       <c r="O12" s="60"/>
@@ -13158,10 +13111,10 @@
       <c r="CA12" s="59"/>
       <c r="CB12" s="59"/>
     </row>
-    <row r="13" spans="1:80" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:80">
       <c r="H13" s="41"/>
       <c r="I13" s="74"/>
-      <c r="L13" s="59"/>
+      <c r="L13" s="58"/>
       <c r="M13" s="41"/>
       <c r="N13" s="60"/>
       <c r="O13" s="60"/>
@@ -13231,10 +13184,10 @@
       <c r="CA13" s="59"/>
       <c r="CB13" s="59"/>
     </row>
-    <row r="14" spans="1:80" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:80">
       <c r="H14" s="41"/>
       <c r="I14" s="74"/>
-      <c r="L14" s="59"/>
+      <c r="L14" s="58"/>
       <c r="M14" s="41"/>
       <c r="N14" s="60"/>
       <c r="O14" s="60"/>
@@ -13304,10 +13257,10 @@
       <c r="CA14" s="59"/>
       <c r="CB14" s="59"/>
     </row>
-    <row r="15" spans="1:80" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:80">
       <c r="H15" s="41"/>
       <c r="I15" s="74"/>
-      <c r="L15" s="59"/>
+      <c r="L15" s="58"/>
       <c r="M15" s="41"/>
       <c r="N15" s="60"/>
       <c r="O15" s="60"/>
@@ -13377,10 +13330,10 @@
       <c r="CA15" s="59"/>
       <c r="CB15" s="59"/>
     </row>
-    <row r="16" spans="1:80" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:80">
       <c r="H16" s="41"/>
       <c r="I16" s="74"/>
-      <c r="L16" s="59"/>
+      <c r="L16" s="58"/>
       <c r="M16" s="41"/>
       <c r="N16" s="60"/>
       <c r="O16" s="60"/>
@@ -13450,10 +13403,10 @@
       <c r="CA16" s="59"/>
       <c r="CB16" s="59"/>
     </row>
-    <row r="17" spans="8:80" x14ac:dyDescent="0.3">
+    <row r="17" spans="8:80">
       <c r="H17" s="41"/>
       <c r="I17" s="74"/>
-      <c r="L17" s="59"/>
+      <c r="L17" s="58"/>
       <c r="M17" s="41"/>
       <c r="N17" s="60"/>
       <c r="O17" s="60"/>
@@ -13523,10 +13476,10 @@
       <c r="CA17" s="59"/>
       <c r="CB17" s="59"/>
     </row>
-    <row r="18" spans="8:80" x14ac:dyDescent="0.3">
+    <row r="18" spans="8:80">
       <c r="H18" s="41"/>
       <c r="I18" s="74"/>
-      <c r="L18" s="59"/>
+      <c r="L18" s="58"/>
       <c r="M18" s="41"/>
       <c r="N18" s="60"/>
       <c r="O18" s="60"/>
@@ -13596,10 +13549,10 @@
       <c r="CA18" s="59"/>
       <c r="CB18" s="59"/>
     </row>
-    <row r="19" spans="8:80" x14ac:dyDescent="0.3">
+    <row r="19" spans="8:80">
       <c r="H19" s="41"/>
       <c r="I19" s="74"/>
-      <c r="L19" s="59"/>
+      <c r="L19" s="58"/>
       <c r="M19" s="41"/>
       <c r="N19" s="60"/>
       <c r="O19" s="60"/>
@@ -13669,7 +13622,7 @@
       <c r="CA19" s="59"/>
       <c r="CB19" s="59"/>
     </row>
-    <row r="20" spans="8:80" x14ac:dyDescent="0.3">
+    <row r="20" spans="8:80">
       <c r="H20" s="41"/>
       <c r="I20" s="74"/>
       <c r="L20" s="59"/>
@@ -13742,7 +13695,7 @@
       <c r="CA20" s="59"/>
       <c r="CB20" s="59"/>
     </row>
-    <row r="21" spans="8:80" x14ac:dyDescent="0.3">
+    <row r="21" spans="8:80">
       <c r="H21" s="41"/>
       <c r="I21" s="74"/>
       <c r="L21" s="59"/>
@@ -13815,7 +13768,7 @@
       <c r="CA21" s="59"/>
       <c r="CB21" s="59"/>
     </row>
-    <row r="22" spans="8:80" x14ac:dyDescent="0.3">
+    <row r="22" spans="8:80">
       <c r="H22" s="41"/>
       <c r="I22" s="74"/>
       <c r="L22" s="59"/>
@@ -13888,7 +13841,7 @@
       <c r="CA22" s="59"/>
       <c r="CB22" s="59"/>
     </row>
-    <row r="23" spans="8:80" x14ac:dyDescent="0.3">
+    <row r="23" spans="8:80">
       <c r="H23" s="41"/>
       <c r="I23" s="74"/>
       <c r="L23" s="59"/>
@@ -13961,7 +13914,7 @@
       <c r="CA23" s="59"/>
       <c r="CB23" s="59"/>
     </row>
-    <row r="24" spans="8:80" x14ac:dyDescent="0.3">
+    <row r="24" spans="8:80">
       <c r="H24" s="41"/>
       <c r="I24" s="74"/>
       <c r="L24" s="59"/>
@@ -14034,7 +13987,7 @@
       <c r="CA24" s="59"/>
       <c r="CB24" s="59"/>
     </row>
-    <row r="25" spans="8:80" x14ac:dyDescent="0.3">
+    <row r="25" spans="8:80">
       <c r="H25" s="41"/>
       <c r="I25" s="74"/>
       <c r="L25" s="59"/>
@@ -14107,7 +14060,7 @@
       <c r="CA25" s="59"/>
       <c r="CB25" s="59"/>
     </row>
-    <row r="26" spans="8:80" x14ac:dyDescent="0.3">
+    <row r="26" spans="8:80">
       <c r="H26" s="41"/>
       <c r="I26" s="74"/>
       <c r="L26" s="59"/>
@@ -14180,7 +14133,7 @@
       <c r="CA26" s="59"/>
       <c r="CB26" s="59"/>
     </row>
-    <row r="27" spans="8:80" x14ac:dyDescent="0.3">
+    <row r="27" spans="8:80">
       <c r="H27" s="41"/>
       <c r="I27" s="74"/>
       <c r="L27" s="59"/>
@@ -14253,7 +14206,7 @@
       <c r="CA27" s="59"/>
       <c r="CB27" s="59"/>
     </row>
-    <row r="28" spans="8:80" x14ac:dyDescent="0.3">
+    <row r="28" spans="8:80">
       <c r="H28" s="41"/>
       <c r="I28" s="74"/>
       <c r="L28" s="59"/>
@@ -14326,7 +14279,7 @@
       <c r="CA28" s="59"/>
       <c r="CB28" s="59"/>
     </row>
-    <row r="29" spans="8:80" x14ac:dyDescent="0.3">
+    <row r="29" spans="8:80">
       <c r="H29" s="41"/>
       <c r="I29" s="74"/>
       <c r="L29" s="59"/>
@@ -14399,7 +14352,7 @@
       <c r="CA29" s="59"/>
       <c r="CB29" s="59"/>
     </row>
-    <row r="30" spans="8:80" x14ac:dyDescent="0.3">
+    <row r="30" spans="8:80">
       <c r="H30" s="41"/>
       <c r="I30" s="74"/>
       <c r="L30" s="59"/>
@@ -14472,7 +14425,7 @@
       <c r="CA30" s="59"/>
       <c r="CB30" s="59"/>
     </row>
-    <row r="31" spans="8:80" x14ac:dyDescent="0.3">
+    <row r="31" spans="8:80">
       <c r="H31" s="41"/>
       <c r="I31" s="74"/>
       <c r="L31" s="59"/>
@@ -14545,7 +14498,7 @@
       <c r="CA31" s="59"/>
       <c r="CB31" s="59"/>
     </row>
-    <row r="32" spans="8:80" x14ac:dyDescent="0.3">
+    <row r="32" spans="8:80">
       <c r="H32" s="41"/>
       <c r="I32" s="74"/>
       <c r="L32" s="59"/>
@@ -14618,7 +14571,7 @@
       <c r="CA32" s="59"/>
       <c r="CB32" s="59"/>
     </row>
-    <row r="33" spans="8:80" x14ac:dyDescent="0.3">
+    <row r="33" spans="8:80">
       <c r="H33" s="41"/>
       <c r="I33" s="74"/>
       <c r="L33" s="59"/>
@@ -14691,7 +14644,7 @@
       <c r="CA33" s="59"/>
       <c r="CB33" s="59"/>
     </row>
-    <row r="34" spans="8:80" x14ac:dyDescent="0.3">
+    <row r="34" spans="8:80">
       <c r="H34" s="41"/>
       <c r="I34" s="74"/>
       <c r="L34" s="59"/>
@@ -14764,92 +14717,92 @@
       <c r="CA34" s="59"/>
       <c r="CB34" s="59"/>
     </row>
-    <row r="35" spans="8:80" x14ac:dyDescent="0.3">
+    <row r="35" spans="8:80">
       <c r="H35" s="41"/>
       <c r="I35" s="74"/>
       <c r="M35" s="41"/>
     </row>
-    <row r="36" spans="8:80" x14ac:dyDescent="0.3">
+    <row r="36" spans="8:80">
       <c r="H36" s="41"/>
       <c r="I36" s="74"/>
       <c r="M36" s="41"/>
     </row>
-    <row r="37" spans="8:80" x14ac:dyDescent="0.3">
+    <row r="37" spans="8:80">
       <c r="H37" s="41"/>
       <c r="I37" s="74"/>
       <c r="M37" s="41"/>
     </row>
-    <row r="38" spans="8:80" x14ac:dyDescent="0.3">
+    <row r="38" spans="8:80">
       <c r="H38" s="41"/>
       <c r="I38" s="74"/>
       <c r="M38" s="41"/>
     </row>
-    <row r="39" spans="8:80" x14ac:dyDescent="0.3">
+    <row r="39" spans="8:80">
       <c r="H39" s="41"/>
       <c r="I39" s="74"/>
       <c r="M39" s="41"/>
     </row>
-    <row r="40" spans="8:80" x14ac:dyDescent="0.3">
+    <row r="40" spans="8:80">
       <c r="H40" s="41"/>
       <c r="I40" s="74"/>
       <c r="M40" s="41"/>
     </row>
-    <row r="41" spans="8:80" x14ac:dyDescent="0.3">
+    <row r="41" spans="8:80">
       <c r="H41" s="41"/>
       <c r="I41" s="74"/>
       <c r="M41" s="41"/>
     </row>
-    <row r="42" spans="8:80" x14ac:dyDescent="0.3">
+    <row r="42" spans="8:80">
       <c r="H42" s="41"/>
       <c r="I42" s="74"/>
       <c r="M42" s="41"/>
     </row>
-    <row r="43" spans="8:80" x14ac:dyDescent="0.3">
+    <row r="43" spans="8:80">
       <c r="H43" s="41"/>
       <c r="I43" s="74"/>
       <c r="M43" s="41"/>
     </row>
-    <row r="44" spans="8:80" x14ac:dyDescent="0.3">
+    <row r="44" spans="8:80">
       <c r="H44" s="41"/>
       <c r="I44" s="74"/>
       <c r="M44" s="41"/>
     </row>
-    <row r="45" spans="8:80" x14ac:dyDescent="0.3">
+    <row r="45" spans="8:80">
       <c r="H45" s="41"/>
       <c r="I45" s="74"/>
       <c r="M45" s="41"/>
     </row>
-    <row r="46" spans="8:80" x14ac:dyDescent="0.3">
+    <row r="46" spans="8:80">
       <c r="H46" s="41"/>
       <c r="I46" s="74"/>
       <c r="M46" s="41"/>
     </row>
-    <row r="47" spans="8:80" x14ac:dyDescent="0.3">
+    <row r="47" spans="8:80">
       <c r="H47" s="41"/>
       <c r="I47" s="74"/>
       <c r="M47" s="41"/>
     </row>
-    <row r="48" spans="8:80" x14ac:dyDescent="0.3">
+    <row r="48" spans="8:80">
       <c r="H48" s="41"/>
       <c r="I48" s="74"/>
       <c r="M48" s="41"/>
     </row>
-    <row r="49" spans="8:13" x14ac:dyDescent="0.3">
+    <row r="49" spans="8:13">
       <c r="H49" s="41"/>
       <c r="I49" s="74"/>
       <c r="M49" s="41"/>
     </row>
-    <row r="50" spans="8:13" x14ac:dyDescent="0.3">
+    <row r="50" spans="8:13">
       <c r="H50" s="41"/>
       <c r="I50" s="74"/>
       <c r="M50" s="41"/>
     </row>
-    <row r="51" spans="8:13" x14ac:dyDescent="0.3">
+    <row r="51" spans="8:13">
       <c r="H51" s="41"/>
       <c r="I51" s="74"/>
       <c r="M51" s="41"/>
     </row>
-    <row r="52" spans="8:13" x14ac:dyDescent="0.3">
+    <row r="52" spans="8:13">
       <c r="H52" s="41"/>
       <c r="I52" s="74"/>
       <c r="M52" s="41"/>
@@ -14886,7 +14839,7 @@
     <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Core depth should be positive." prompt="Average sample depth of the sample (i.e. 0.5 cm)" sqref="J7:J1048576" xr:uid="{76CC5D1F-1565-4594-B5AF-8B25948B4A60}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="Q8:Q27 L7 N7:CB7" xr:uid="{6673B6D2-9563-46FC-8335-F6B94E523361}">
+    <dataValidation type="list" allowBlank="1" sqref="Q8:Q27 N7:CB7 L7:L19" xr:uid="{6673B6D2-9563-46FC-8335-F6B94E523361}">
       <formula1>INDIRECT(L$2)</formula1>
     </dataValidation>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Name of user who is entering data" sqref="A7:A1048576" xr:uid="{4BF522A4-2999-4EF9-835E-16C3A98D1BAF}"/>
@@ -14931,19 +14884,19 @@
           <x14:formula1>
             <xm:f>SET_VARIABLES!$A$2:$A$3</xm:f>
           </x14:formula1>
-          <xm:sqref>D7 D9:D1048576 D8</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Write the core name or select from the drop-down menu the cores you have in the Workbook._x000a_Make sure that the core name matches with its metadata given in GEOPOINTS_CORES sheet" xr:uid="{E4FFB722-8CB2-4C84-A9DE-29D8614FBFFB}">
-          <x14:formula1>
-            <xm:f>GEOPOINTS_CORES!$B$3:$B$1048576</xm:f>
-          </x14:formula1>
-          <xm:sqref>B7:B1048576</xm:sqref>
+          <xm:sqref>D7:D1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Raw / calculated data" prompt="Specify if the data provided has been extracted directly from the source (i.e. paper) or is calculated using available data. If left blank, default of &quot;raw data&quot; will be used. " xr:uid="{30C7084F-BEF5-4E01-80B0-5EBF52EBFAA6}">
           <x14:formula1>
             <xm:f>SET_VARIABLES!$BE$2:$BE$3</xm:f>
           </x14:formula1>
           <xm:sqref>L6:CB6</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Write the core name or select from the drop-down menu the cores you have in the Workbook._x000a_Make sure that the core name matches with its metadata given in GEOPOINTS_CORES sheet" xr:uid="{E4FFB722-8CB2-4C84-A9DE-29D8614FBFFB}">
+          <x14:formula1>
+            <xm:f>GEOPOINTS_CORES!$B$3:$B$1048576</xm:f>
+          </x14:formula1>
+          <xm:sqref>B7:B1048576 C7</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -14956,11 +14909,11 @@
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:HL277"/>
   <sheetViews>
-    <sheetView topLeftCell="ER1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="GW19" sqref="GW19"/>
+    <sheetView topLeftCell="GQ1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="GZ14" sqref="GZ14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
   <cols>
     <col min="1" max="10" width="18.19921875" customWidth="1"/>
     <col min="11" max="11" width="18.19921875" style="35" customWidth="1"/>
@@ -15017,9 +14970,10 @@
     <col min="163" max="163" width="21.59765625" bestFit="1" customWidth="1"/>
     <col min="180" max="180" width="13.09765625" bestFit="1" customWidth="1"/>
     <col min="198" max="198" width="17.8984375" bestFit="1" customWidth="1"/>
+    <col min="207" max="208" width="21.3984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:220" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:220" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -15741,7 +15695,7 @@
         <v>2110</v>
       </c>
     </row>
-    <row r="2" spans="1:220" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:220">
       <c r="A2" t="b">
         <v>1</v>
       </c>
@@ -16375,7 +16329,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:220" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:220">
       <c r="A3" t="b">
         <v>0</v>
       </c>
@@ -16936,7 +16890,7 @@
         <v>2028</v>
       </c>
     </row>
-    <row r="4" spans="1:220" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:220">
       <c r="B4" t="s">
         <v>29</v>
       </c>
@@ -17467,7 +17421,7 @@
         <v>2036</v>
       </c>
     </row>
-    <row r="5" spans="1:220" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:220">
       <c r="B5" t="s">
         <v>40</v>
       </c>
@@ -17909,7 +17863,7 @@
         <v>2037</v>
       </c>
     </row>
-    <row r="6" spans="1:220" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:220">
       <c r="B6" t="s">
         <v>52</v>
       </c>
@@ -18321,7 +18275,7 @@
         <v>2038</v>
       </c>
     </row>
-    <row r="7" spans="1:220" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:220">
       <c r="B7" t="s">
         <v>63</v>
       </c>
@@ -18712,7 +18666,7 @@
         <v>2030</v>
       </c>
     </row>
-    <row r="8" spans="1:220" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:220" ht="16.05" customHeight="1">
       <c r="B8" t="s">
         <v>75</v>
       </c>
@@ -19060,7 +19014,7 @@
         <v>2039</v>
       </c>
     </row>
-    <row r="9" spans="1:220" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:220" ht="16.05" customHeight="1">
       <c r="B9" t="s">
         <v>86</v>
       </c>
@@ -19380,7 +19334,7 @@
         <v>2029</v>
       </c>
     </row>
-    <row r="10" spans="1:220" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:220">
       <c r="B10" t="s">
         <v>95</v>
       </c>
@@ -19659,10 +19613,10 @@
         <v>2216</v>
       </c>
       <c r="GY10" s="88" t="s">
-        <v>3011</v>
-      </c>
-      <c r="GZ10" s="85" t="s">
-        <v>2988</v>
+        <v>2028</v>
+      </c>
+      <c r="GZ10" s="88" t="s">
+        <v>2028</v>
       </c>
       <c r="HA10" s="85" t="s">
         <v>2216</v>
@@ -19671,7 +19625,7 @@
         <v>2216</v>
       </c>
     </row>
-    <row r="11" spans="1:220" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:220">
       <c r="B11" t="s">
         <v>104</v>
       </c>
@@ -19944,7 +19898,7 @@
         <v>2988</v>
       </c>
       <c r="GZ11" s="85" t="s">
-        <v>2029</v>
+        <v>2988</v>
       </c>
       <c r="HA11" s="85" t="s">
         <v>2040</v>
@@ -19953,7 +19907,7 @@
         <v>2040</v>
       </c>
     </row>
-    <row r="12" spans="1:220" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:220">
       <c r="B12" t="s">
         <v>113</v>
       </c>
@@ -20206,11 +20160,11 @@
       <c r="FE12" s="85" t="s">
         <v>2041</v>
       </c>
-      <c r="GY12" t="s">
-        <v>2029</v>
-      </c>
-      <c r="GZ12" s="85" t="s">
-        <v>2030</v>
+      <c r="GY12" s="88" t="s">
+        <v>2571</v>
+      </c>
+      <c r="GZ12" s="88" t="s">
+        <v>2571</v>
       </c>
       <c r="HA12" s="85" t="s">
         <v>2041</v>
@@ -20219,7 +20173,7 @@
         <v>2041</v>
       </c>
     </row>
-    <row r="13" spans="1:220" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:220">
       <c r="B13" t="s">
         <v>122</v>
       </c>
@@ -20451,10 +20405,10 @@
         <v>2031</v>
       </c>
       <c r="GY13" t="s">
-        <v>2030</v>
+        <v>2029</v>
       </c>
       <c r="GZ13" s="85" t="s">
-        <v>2031</v>
+        <v>2029</v>
       </c>
       <c r="HA13" s="85" t="s">
         <v>2031</v>
@@ -20463,7 +20417,7 @@
         <v>2031</v>
       </c>
     </row>
-    <row r="14" spans="1:220" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:220">
       <c r="B14" t="s">
         <v>130</v>
       </c>
@@ -20667,13 +20621,13 @@
       <c r="EE14" s="46"/>
       <c r="EF14" s="46"/>
       <c r="GY14" t="s">
-        <v>2031</v>
+        <v>2030</v>
       </c>
       <c r="GZ14" s="85" t="s">
-        <v>2036</v>
-      </c>
-    </row>
-    <row r="15" spans="1:220" x14ac:dyDescent="0.3">
+        <v>2030</v>
+      </c>
+    </row>
+    <row r="15" spans="1:220">
       <c r="B15" t="s">
         <v>138</v>
       </c>
@@ -20869,13 +20823,13 @@
       <c r="EE15" s="46"/>
       <c r="EF15" s="46"/>
       <c r="GY15" t="s">
-        <v>2036</v>
+        <v>2031</v>
       </c>
       <c r="GZ15" s="85" t="s">
-        <v>2990</v>
-      </c>
-    </row>
-    <row r="16" spans="1:220" x14ac:dyDescent="0.3">
+        <v>2031</v>
+      </c>
+    </row>
+    <row r="16" spans="1:220">
       <c r="B16" t="s">
         <v>145</v>
       </c>
@@ -21066,13 +21020,13 @@
       <c r="EE16" s="46"/>
       <c r="EF16" s="46"/>
       <c r="GY16" t="s">
-        <v>2989</v>
-      </c>
-      <c r="GZ16" s="10" t="s">
-        <v>2259</v>
-      </c>
-    </row>
-    <row r="17" spans="2:208" x14ac:dyDescent="0.3">
+        <v>2036</v>
+      </c>
+      <c r="GZ16" s="85" t="s">
+        <v>2036</v>
+      </c>
+    </row>
+    <row r="17" spans="2:208">
       <c r="B17" t="s">
         <v>153</v>
       </c>
@@ -21252,14 +21206,14 @@
       <c r="ED17" s="12"/>
       <c r="EE17" s="46"/>
       <c r="EF17" s="46"/>
-      <c r="GY17" s="10" t="s">
-        <v>2259</v>
-      </c>
-      <c r="GZ17" s="10" t="s">
-        <v>2877</v>
-      </c>
-    </row>
-    <row r="18" spans="2:208" x14ac:dyDescent="0.3">
+      <c r="GY17" t="s">
+        <v>2989</v>
+      </c>
+      <c r="GZ17" s="85" t="s">
+        <v>2990</v>
+      </c>
+    </row>
+    <row r="18" spans="2:208">
       <c r="B18" t="s">
         <v>160</v>
       </c>
@@ -21433,13 +21387,13 @@
       <c r="EE18" s="46"/>
       <c r="EF18" s="46"/>
       <c r="GY18" s="10" t="s">
-        <v>2877</v>
+        <v>2259</v>
       </c>
       <c r="GZ18" s="10" t="s">
-        <v>3010</v>
-      </c>
-    </row>
-    <row r="19" spans="2:208" ht="17.399999999999999" x14ac:dyDescent="0.3">
+        <v>2259</v>
+      </c>
+    </row>
+    <row r="19" spans="2:208" ht="17.399999999999999">
       <c r="B19" t="s">
         <v>167</v>
       </c>
@@ -21608,10 +21562,13 @@
       <c r="EE19" s="46"/>
       <c r="EF19" s="46"/>
       <c r="GY19" s="10" t="s">
-        <v>3010</v>
-      </c>
-    </row>
-    <row r="20" spans="2:208" x14ac:dyDescent="0.3">
+        <v>2877</v>
+      </c>
+      <c r="GZ19" s="10" t="s">
+        <v>2877</v>
+      </c>
+    </row>
+    <row r="20" spans="2:208">
       <c r="B20" t="s">
         <v>174</v>
       </c>
@@ -21760,8 +21717,14 @@
       <c r="ED20" s="12"/>
       <c r="EE20" s="46"/>
       <c r="EF20" s="46"/>
-    </row>
-    <row r="21" spans="2:208" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="GY20" s="10" t="s">
+        <v>3010</v>
+      </c>
+      <c r="GZ20" s="10" t="s">
+        <v>3010</v>
+      </c>
+    </row>
+    <row r="21" spans="2:208" ht="16.8">
       <c r="B21" t="s">
         <v>181</v>
       </c>
@@ -21885,7 +21848,7 @@
         <v>2335</v>
       </c>
     </row>
-    <row r="22" spans="2:208" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:208">
       <c r="B22" t="s">
         <v>188</v>
       </c>
@@ -21996,7 +21959,7 @@
         <v>2335</v>
       </c>
     </row>
-    <row r="23" spans="2:208" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:208">
       <c r="B23" t="s">
         <v>195</v>
       </c>
@@ -22094,7 +22057,7 @@
         <v>2442</v>
       </c>
     </row>
-    <row r="24" spans="2:208" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:208" ht="17.399999999999999">
       <c r="B24" t="s">
         <v>202</v>
       </c>
@@ -22183,7 +22146,7 @@
         <v>2445</v>
       </c>
     </row>
-    <row r="25" spans="2:208" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:208">
       <c r="B25" t="s">
         <v>209</v>
       </c>
@@ -22274,7 +22237,7 @@
         <v>2438</v>
       </c>
     </row>
-    <row r="26" spans="2:208" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:208" ht="16.8">
       <c r="B26" t="s">
         <v>216</v>
       </c>
@@ -22359,7 +22322,7 @@
         <v>2439</v>
       </c>
     </row>
-    <row r="27" spans="2:208" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:208" ht="16.05" customHeight="1">
       <c r="B27" t="s">
         <v>222</v>
       </c>
@@ -22440,7 +22403,7 @@
         <v>2440</v>
       </c>
     </row>
-    <row r="28" spans="2:208" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:208" ht="16.05" customHeight="1">
       <c r="B28" t="s">
         <v>229</v>
       </c>
@@ -22521,7 +22484,7 @@
         <v>2441</v>
       </c>
     </row>
-    <row r="29" spans="2:208" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:208" ht="17.399999999999999">
       <c r="B29" t="s">
         <v>236</v>
       </c>
@@ -22593,7 +22556,7 @@
         <v>2436</v>
       </c>
     </row>
-    <row r="30" spans="2:208" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:208">
       <c r="B30" t="s">
         <v>243</v>
       </c>
@@ -22653,7 +22616,7 @@
         <v>2437</v>
       </c>
     </row>
-    <row r="31" spans="2:208" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:208">
       <c r="B31" t="s">
         <v>249</v>
       </c>
@@ -22714,7 +22677,7 @@
         <v>2537</v>
       </c>
     </row>
-    <row r="32" spans="2:208" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:208" ht="17.399999999999999">
       <c r="B32" t="s">
         <v>256</v>
       </c>
@@ -22777,7 +22740,7 @@
         <v>2536</v>
       </c>
     </row>
-    <row r="33" spans="2:116" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:116" ht="17.399999999999999">
       <c r="B33" t="s">
         <v>263</v>
       </c>
@@ -22836,7 +22799,7 @@
         <v>2723</v>
       </c>
     </row>
-    <row r="34" spans="2:116" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:116">
       <c r="B34" t="s">
         <v>270</v>
       </c>
@@ -22895,7 +22858,7 @@
         <v>2377</v>
       </c>
     </row>
-    <row r="35" spans="2:116" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:116" ht="16.05" customHeight="1">
       <c r="B35" t="s">
         <v>277</v>
       </c>
@@ -22951,7 +22914,7 @@
         <v>2725</v>
       </c>
     </row>
-    <row r="36" spans="2:116" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:116" ht="17.399999999999999">
       <c r="B36" t="s">
         <v>284</v>
       </c>
@@ -23007,7 +22970,7 @@
         <v>2378</v>
       </c>
     </row>
-    <row r="37" spans="2:116" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:116" ht="17.399999999999999">
       <c r="B37" t="s">
         <v>291</v>
       </c>
@@ -23064,7 +23027,7 @@
         <v>2727</v>
       </c>
     </row>
-    <row r="38" spans="2:116" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:116" ht="17.399999999999999">
       <c r="B38" t="s">
         <v>298</v>
       </c>
@@ -23117,7 +23080,7 @@
         <v>2379</v>
       </c>
     </row>
-    <row r="39" spans="2:116" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:116">
       <c r="B39" t="s">
         <v>305</v>
       </c>
@@ -23171,7 +23134,7 @@
       </c>
       <c r="DL39" s="45"/>
     </row>
-    <row r="40" spans="2:116" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:116" ht="17.399999999999999">
       <c r="B40" t="s">
         <v>312</v>
       </c>
@@ -23221,7 +23184,7 @@
       </c>
       <c r="DL40" s="45"/>
     </row>
-    <row r="41" spans="2:116" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:116" ht="17.399999999999999">
       <c r="B41" t="s">
         <v>27</v>
       </c>
@@ -23267,7 +23230,7 @@
       </c>
       <c r="DL41" s="45"/>
     </row>
-    <row r="42" spans="2:116" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:116">
       <c r="B42" t="s">
         <v>325</v>
       </c>
@@ -23313,7 +23276,7 @@
       </c>
       <c r="DL42" s="45"/>
     </row>
-    <row r="43" spans="2:116" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:116" ht="17.399999999999999">
       <c r="B43" t="s">
         <v>332</v>
       </c>
@@ -23359,7 +23322,7 @@
       </c>
       <c r="DL43" s="45"/>
     </row>
-    <row r="44" spans="2:116" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:116" ht="17.399999999999999">
       <c r="B44" t="s">
         <v>339</v>
       </c>
@@ -23408,7 +23371,7 @@
       </c>
       <c r="DL44" s="45"/>
     </row>
-    <row r="45" spans="2:116" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:116" ht="17.399999999999999">
       <c r="B45" t="s">
         <v>346</v>
       </c>
@@ -23454,7 +23417,7 @@
       </c>
       <c r="DL45" s="45"/>
     </row>
-    <row r="46" spans="2:116" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:116">
       <c r="B46" t="s">
         <v>353</v>
       </c>
@@ -23500,7 +23463,7 @@
       </c>
       <c r="DL46" s="45"/>
     </row>
-    <row r="47" spans="2:116" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:116" ht="17.399999999999999">
       <c r="B47" t="s">
         <v>360</v>
       </c>
@@ -23547,7 +23510,7 @@
       </c>
       <c r="DL47" s="45"/>
     </row>
-    <row r="48" spans="2:116" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:116" ht="17.399999999999999">
       <c r="B48" t="s">
         <v>367</v>
       </c>
@@ -23593,7 +23556,7 @@
       </c>
       <c r="DL48" s="45"/>
     </row>
-    <row r="49" spans="2:116" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:116" ht="17.399999999999999">
       <c r="B49" t="s">
         <v>373</v>
       </c>
@@ -23639,7 +23602,7 @@
       </c>
       <c r="DL49" s="45"/>
     </row>
-    <row r="50" spans="2:116" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:116" ht="17.399999999999999">
       <c r="B50" t="s">
         <v>380</v>
       </c>
@@ -23686,7 +23649,7 @@
       </c>
       <c r="DL50" s="45"/>
     </row>
-    <row r="51" spans="2:116" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:116" ht="17.399999999999999">
       <c r="B51" t="s">
         <v>386</v>
       </c>
@@ -23733,7 +23696,7 @@
       </c>
       <c r="DL51" s="45"/>
     </row>
-    <row r="52" spans="2:116" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:116">
       <c r="B52" t="s">
         <v>393</v>
       </c>
@@ -23779,7 +23742,7 @@
       </c>
       <c r="DL52" s="45"/>
     </row>
-    <row r="53" spans="2:116" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:116">
       <c r="B53" t="s">
         <v>400</v>
       </c>
@@ -23826,7 +23789,7 @@
       </c>
       <c r="DL53" s="45"/>
     </row>
-    <row r="54" spans="2:116" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:116" ht="17.399999999999999">
       <c r="B54" t="s">
         <v>407</v>
       </c>
@@ -23871,7 +23834,7 @@
       </c>
       <c r="DL54" s="45"/>
     </row>
-    <row r="55" spans="2:116" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="55" spans="2:116" ht="17.399999999999999">
       <c r="B55" t="s">
         <v>414</v>
       </c>
@@ -23916,7 +23879,7 @@
       </c>
       <c r="DL55" s="45"/>
     </row>
-    <row r="56" spans="2:116" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="56" spans="2:116" ht="17.399999999999999">
       <c r="B56" t="s">
         <v>421</v>
       </c>
@@ -23961,7 +23924,7 @@
       </c>
       <c r="DL56" s="45"/>
     </row>
-    <row r="57" spans="2:116" x14ac:dyDescent="0.3">
+    <row r="57" spans="2:116">
       <c r="B57" t="s">
         <v>428</v>
       </c>
@@ -24005,7 +23968,7 @@
       </c>
       <c r="DL57" s="45"/>
     </row>
-    <row r="58" spans="2:116" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="58" spans="2:116" ht="17.399999999999999">
       <c r="B58" t="s">
         <v>435</v>
       </c>
@@ -24049,7 +24012,7 @@
       </c>
       <c r="DL58" s="45"/>
     </row>
-    <row r="59" spans="2:116" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="59" spans="2:116" ht="17.399999999999999">
       <c r="B59" t="s">
         <v>442</v>
       </c>
@@ -24090,7 +24053,7 @@
       </c>
       <c r="DL59" s="45"/>
     </row>
-    <row r="60" spans="2:116" x14ac:dyDescent="0.3">
+    <row r="60" spans="2:116">
       <c r="B60" t="s">
         <v>448</v>
       </c>
@@ -24131,7 +24094,7 @@
       </c>
       <c r="DL60" s="45"/>
     </row>
-    <row r="61" spans="2:116" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="61" spans="2:116" ht="17.399999999999999">
       <c r="B61" t="s">
         <v>454</v>
       </c>
@@ -24172,7 +24135,7 @@
       </c>
       <c r="DL61" s="45"/>
     </row>
-    <row r="62" spans="2:116" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="62" spans="2:116" ht="17.399999999999999">
       <c r="B62" t="s">
         <v>460</v>
       </c>
@@ -24213,7 +24176,7 @@
       </c>
       <c r="DL62" s="45"/>
     </row>
-    <row r="63" spans="2:116" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="63" spans="2:116" ht="17.399999999999999">
       <c r="B63" t="s">
         <v>466</v>
       </c>
@@ -24254,7 +24217,7 @@
       </c>
       <c r="DL63" s="45"/>
     </row>
-    <row r="64" spans="2:116" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="64" spans="2:116" ht="17.399999999999999">
       <c r="B64" t="s">
         <v>472</v>
       </c>
@@ -24292,7 +24255,7 @@
       </c>
       <c r="DL64" s="45"/>
     </row>
-    <row r="65" spans="2:116" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="65" spans="2:116" ht="17.399999999999999">
       <c r="B65" t="s">
         <v>478</v>
       </c>
@@ -24330,7 +24293,7 @@
       </c>
       <c r="DL65" s="45"/>
     </row>
-    <row r="66" spans="2:116" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="66" spans="2:116" ht="17.399999999999999">
       <c r="B66" t="s">
         <v>484</v>
       </c>
@@ -24368,7 +24331,7 @@
       </c>
       <c r="DL66" s="45"/>
     </row>
-    <row r="67" spans="2:116" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="67" spans="2:116" ht="17.399999999999999">
       <c r="B67" t="s">
         <v>490</v>
       </c>
@@ -24406,7 +24369,7 @@
       </c>
       <c r="DL67" s="45"/>
     </row>
-    <row r="68" spans="2:116" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="68" spans="2:116" ht="17.399999999999999">
       <c r="B68" t="s">
         <v>496</v>
       </c>
@@ -24444,7 +24407,7 @@
       </c>
       <c r="DL68" s="45"/>
     </row>
-    <row r="69" spans="2:116" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="69" spans="2:116" ht="17.399999999999999">
       <c r="B69" t="s">
         <v>502</v>
       </c>
@@ -24481,7 +24444,7 @@
       </c>
       <c r="DL69" s="45"/>
     </row>
-    <row r="70" spans="2:116" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="70" spans="2:116" ht="17.399999999999999">
       <c r="B70" t="s">
         <v>508</v>
       </c>
@@ -24519,7 +24482,7 @@
       </c>
       <c r="DL70" s="45"/>
     </row>
-    <row r="71" spans="2:116" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="71" spans="2:116" ht="17.399999999999999">
       <c r="B71" t="s">
         <v>514</v>
       </c>
@@ -24557,7 +24520,7 @@
       </c>
       <c r="DL71" s="45"/>
     </row>
-    <row r="72" spans="2:116" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="72" spans="2:116" ht="17.399999999999999">
       <c r="B72" t="s">
         <v>520</v>
       </c>
@@ -24595,7 +24558,7 @@
       </c>
       <c r="DL72" s="45"/>
     </row>
-    <row r="73" spans="2:116" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="73" spans="2:116" ht="17.399999999999999">
       <c r="B73" t="s">
         <v>526</v>
       </c>
@@ -24633,7 +24596,7 @@
       </c>
       <c r="DL73" s="45"/>
     </row>
-    <row r="74" spans="2:116" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="74" spans="2:116" ht="17.399999999999999">
       <c r="B74" t="s">
         <v>532</v>
       </c>
@@ -24671,7 +24634,7 @@
       </c>
       <c r="DL74" s="45"/>
     </row>
-    <row r="75" spans="2:116" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="75" spans="2:116" ht="17.399999999999999">
       <c r="B75" t="s">
         <v>538</v>
       </c>
@@ -24709,7 +24672,7 @@
       </c>
       <c r="DL75" s="45"/>
     </row>
-    <row r="76" spans="2:116" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="76" spans="2:116" ht="17.399999999999999">
       <c r="B76" t="s">
         <v>544</v>
       </c>
@@ -24747,7 +24710,7 @@
       </c>
       <c r="DL76" s="45"/>
     </row>
-    <row r="77" spans="2:116" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="77" spans="2:116" ht="17.399999999999999">
       <c r="B77" t="s">
         <v>549</v>
       </c>
@@ -24785,7 +24748,7 @@
       </c>
       <c r="DL77" s="45"/>
     </row>
-    <row r="78" spans="2:116" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="78" spans="2:116" ht="17.399999999999999">
       <c r="B78" t="s">
         <v>555</v>
       </c>
@@ -24823,7 +24786,7 @@
       </c>
       <c r="DL78" s="45"/>
     </row>
-    <row r="79" spans="2:116" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="79" spans="2:116" ht="17.399999999999999">
       <c r="B79" t="s">
         <v>561</v>
       </c>
@@ -24861,7 +24824,7 @@
       </c>
       <c r="DL79" s="45"/>
     </row>
-    <row r="80" spans="2:116" x14ac:dyDescent="0.3">
+    <row r="80" spans="2:116">
       <c r="B80" t="s">
         <v>567</v>
       </c>
@@ -24899,7 +24862,7 @@
       </c>
       <c r="DL80" s="45"/>
     </row>
-    <row r="81" spans="2:116" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="81" spans="2:116" ht="17.399999999999999">
       <c r="B81" t="s">
         <v>573</v>
       </c>
@@ -24937,7 +24900,7 @@
       </c>
       <c r="DL81" s="45"/>
     </row>
-    <row r="82" spans="2:116" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="82" spans="2:116" ht="17.399999999999999">
       <c r="B82" t="s">
         <v>579</v>
       </c>
@@ -24975,7 +24938,7 @@
       </c>
       <c r="DL82" s="45"/>
     </row>
-    <row r="83" spans="2:116" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="83" spans="2:116" ht="17.399999999999999">
       <c r="B83" t="s">
         <v>585</v>
       </c>
@@ -25013,7 +24976,7 @@
       </c>
       <c r="DL83" s="45"/>
     </row>
-    <row r="84" spans="2:116" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="84" spans="2:116" ht="17.399999999999999">
       <c r="B84" t="s">
         <v>591</v>
       </c>
@@ -25051,7 +25014,7 @@
       </c>
       <c r="DL84" s="45"/>
     </row>
-    <row r="85" spans="2:116" x14ac:dyDescent="0.3">
+    <row r="85" spans="2:116">
       <c r="B85" t="s">
         <v>597</v>
       </c>
@@ -25088,7 +25051,7 @@
       </c>
       <c r="DL85" s="45"/>
     </row>
-    <row r="86" spans="2:116" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="86" spans="2:116" ht="17.399999999999999">
       <c r="B86" t="s">
         <v>603</v>
       </c>
@@ -25125,7 +25088,7 @@
       </c>
       <c r="DL86" s="45"/>
     </row>
-    <row r="87" spans="2:116" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="87" spans="2:116" ht="17.399999999999999">
       <c r="B87" t="s">
         <v>609</v>
       </c>
@@ -25162,7 +25125,7 @@
       </c>
       <c r="DL87" s="45"/>
     </row>
-    <row r="88" spans="2:116" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="88" spans="2:116" ht="17.399999999999999">
       <c r="B88" t="s">
         <v>615</v>
       </c>
@@ -25199,7 +25162,7 @@
       </c>
       <c r="DL88" s="45"/>
     </row>
-    <row r="89" spans="2:116" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="89" spans="2:116" ht="17.399999999999999">
       <c r="B89" t="s">
         <v>621</v>
       </c>
@@ -25236,7 +25199,7 @@
       </c>
       <c r="DL89" s="45"/>
     </row>
-    <row r="90" spans="2:116" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="90" spans="2:116" ht="17.399999999999999">
       <c r="B90" t="s">
         <v>627</v>
       </c>
@@ -25273,7 +25236,7 @@
       </c>
       <c r="DL90" s="45"/>
     </row>
-    <row r="91" spans="2:116" x14ac:dyDescent="0.3">
+    <row r="91" spans="2:116">
       <c r="B91" t="s">
         <v>633</v>
       </c>
@@ -25310,7 +25273,7 @@
       </c>
       <c r="DL91" s="45"/>
     </row>
-    <row r="92" spans="2:116" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="92" spans="2:116" ht="17.399999999999999">
       <c r="B92" t="s">
         <v>639</v>
       </c>
@@ -25347,7 +25310,7 @@
       </c>
       <c r="DL92" s="45"/>
     </row>
-    <row r="93" spans="2:116" x14ac:dyDescent="0.3">
+    <row r="93" spans="2:116">
       <c r="B93" t="s">
         <v>645</v>
       </c>
@@ -25384,7 +25347,7 @@
       </c>
       <c r="DL93" s="45"/>
     </row>
-    <row r="94" spans="2:116" x14ac:dyDescent="0.3">
+    <row r="94" spans="2:116">
       <c r="B94" t="s">
         <v>651</v>
       </c>
@@ -25421,7 +25384,7 @@
       </c>
       <c r="DL94" s="45"/>
     </row>
-    <row r="95" spans="2:116" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="95" spans="2:116" ht="17.399999999999999">
       <c r="B95" t="s">
         <v>657</v>
       </c>
@@ -25458,7 +25421,7 @@
       </c>
       <c r="DL95" s="45"/>
     </row>
-    <row r="96" spans="2:116" x14ac:dyDescent="0.3">
+    <row r="96" spans="2:116">
       <c r="B96" t="s">
         <v>663</v>
       </c>
@@ -25495,7 +25458,7 @@
       </c>
       <c r="DL96" s="45"/>
     </row>
-    <row r="97" spans="2:116" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="97" spans="2:116" ht="17.399999999999999">
       <c r="B97" t="s">
         <v>669</v>
       </c>
@@ -25532,7 +25495,7 @@
       </c>
       <c r="DL97" s="45"/>
     </row>
-    <row r="98" spans="2:116" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="98" spans="2:116" ht="17.399999999999999">
       <c r="B98" t="s">
         <v>675</v>
       </c>
@@ -25569,7 +25532,7 @@
       </c>
       <c r="DL98" s="45"/>
     </row>
-    <row r="99" spans="2:116" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="99" spans="2:116" ht="17.399999999999999">
       <c r="B99" t="s">
         <v>681</v>
       </c>
@@ -25604,7 +25567,7 @@
       </c>
       <c r="DL99" s="45"/>
     </row>
-    <row r="100" spans="2:116" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="100" spans="2:116" ht="17.399999999999999">
       <c r="B100" t="s">
         <v>687</v>
       </c>
@@ -25638,7 +25601,7 @@
       </c>
       <c r="DL100" s="45"/>
     </row>
-    <row r="101" spans="2:116" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="101" spans="2:116" ht="17.399999999999999">
       <c r="B101" t="s">
         <v>693</v>
       </c>
@@ -25672,7 +25635,7 @@
       </c>
       <c r="DL101" s="45"/>
     </row>
-    <row r="102" spans="2:116" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="102" spans="2:116" ht="17.399999999999999">
       <c r="B102" t="s">
         <v>699</v>
       </c>
@@ -25706,7 +25669,7 @@
       </c>
       <c r="DL102" s="45"/>
     </row>
-    <row r="103" spans="2:116" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="103" spans="2:116" ht="17.399999999999999">
       <c r="B103" t="s">
         <v>705</v>
       </c>
@@ -25740,7 +25703,7 @@
       </c>
       <c r="DL103" s="45"/>
     </row>
-    <row r="104" spans="2:116" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="104" spans="2:116" ht="17.399999999999999">
       <c r="B104" t="s">
         <v>711</v>
       </c>
@@ -25774,7 +25737,7 @@
       </c>
       <c r="DL104" s="45"/>
     </row>
-    <row r="105" spans="2:116" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="105" spans="2:116" ht="17.399999999999999">
       <c r="B105" t="s">
         <v>717</v>
       </c>
@@ -25808,7 +25771,7 @@
       </c>
       <c r="DL105" s="45"/>
     </row>
-    <row r="106" spans="2:116" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="106" spans="2:116" ht="17.399999999999999">
       <c r="B106" t="s">
         <v>723</v>
       </c>
@@ -25842,7 +25805,7 @@
       </c>
       <c r="DL106" s="45"/>
     </row>
-    <row r="107" spans="2:116" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="107" spans="2:116" ht="17.399999999999999">
       <c r="B107" t="s">
         <v>729</v>
       </c>
@@ -25876,7 +25839,7 @@
       </c>
       <c r="DL107" s="45"/>
     </row>
-    <row r="108" spans="2:116" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="108" spans="2:116" ht="17.399999999999999">
       <c r="B108" t="s">
         <v>734</v>
       </c>
@@ -25910,7 +25873,7 @@
       </c>
       <c r="DL108" s="45"/>
     </row>
-    <row r="109" spans="2:116" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="109" spans="2:116" ht="17.399999999999999">
       <c r="B109" t="s">
         <v>740</v>
       </c>
@@ -25944,7 +25907,7 @@
       </c>
       <c r="DL109" s="45"/>
     </row>
-    <row r="110" spans="2:116" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="110" spans="2:116" ht="17.399999999999999">
       <c r="B110" t="s">
         <v>746</v>
       </c>
@@ -25978,7 +25941,7 @@
       </c>
       <c r="DL110" s="45"/>
     </row>
-    <row r="111" spans="2:116" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="111" spans="2:116" ht="17.399999999999999">
       <c r="B111" t="s">
         <v>752</v>
       </c>
@@ -26012,7 +25975,7 @@
       </c>
       <c r="DL111" s="45"/>
     </row>
-    <row r="112" spans="2:116" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="112" spans="2:116" ht="17.399999999999999">
       <c r="B112" t="s">
         <v>758</v>
       </c>
@@ -26046,7 +26009,7 @@
       </c>
       <c r="DL112" s="45"/>
     </row>
-    <row r="113" spans="2:116" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="113" spans="2:116" ht="17.399999999999999">
       <c r="B113" t="s">
         <v>763</v>
       </c>
@@ -26080,7 +26043,7 @@
       </c>
       <c r="DL113" s="45"/>
     </row>
-    <row r="114" spans="2:116" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="114" spans="2:116" ht="17.399999999999999">
       <c r="B114" t="s">
         <v>769</v>
       </c>
@@ -26114,7 +26077,7 @@
       </c>
       <c r="DL114" s="45"/>
     </row>
-    <row r="115" spans="2:116" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="115" spans="2:116" ht="17.399999999999999">
       <c r="B115" t="s">
         <v>775</v>
       </c>
@@ -26148,7 +26111,7 @@
       </c>
       <c r="DL115" s="45"/>
     </row>
-    <row r="116" spans="2:116" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="116" spans="2:116" ht="17.399999999999999">
       <c r="B116" t="s">
         <v>781</v>
       </c>
@@ -26173,7 +26136,7 @@
       </c>
       <c r="DL116" s="45"/>
     </row>
-    <row r="117" spans="2:116" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="117" spans="2:116" ht="17.399999999999999">
       <c r="B117" t="s">
         <v>787</v>
       </c>
@@ -26198,7 +26161,7 @@
       </c>
       <c r="DL117" s="45"/>
     </row>
-    <row r="118" spans="2:116" x14ac:dyDescent="0.3">
+    <row r="118" spans="2:116">
       <c r="B118" t="s">
         <v>793</v>
       </c>
@@ -26223,7 +26186,7 @@
       </c>
       <c r="DL118" s="45"/>
     </row>
-    <row r="119" spans="2:116" x14ac:dyDescent="0.3">
+    <row r="119" spans="2:116">
       <c r="B119" t="s">
         <v>799</v>
       </c>
@@ -26248,7 +26211,7 @@
       </c>
       <c r="DL119" s="45"/>
     </row>
-    <row r="120" spans="2:116" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="120" spans="2:116" ht="17.399999999999999">
       <c r="B120" t="s">
         <v>805</v>
       </c>
@@ -26273,7 +26236,7 @@
       </c>
       <c r="DL120" s="45"/>
     </row>
-    <row r="121" spans="2:116" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="121" spans="2:116" ht="17.399999999999999">
       <c r="B121" t="s">
         <v>811</v>
       </c>
@@ -26298,7 +26261,7 @@
       </c>
       <c r="DL121" s="45"/>
     </row>
-    <row r="122" spans="2:116" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="122" spans="2:116" ht="17.399999999999999">
       <c r="B122" t="s">
         <v>817</v>
       </c>
@@ -26323,7 +26286,7 @@
       </c>
       <c r="DL122" s="45"/>
     </row>
-    <row r="123" spans="2:116" x14ac:dyDescent="0.3">
+    <row r="123" spans="2:116">
       <c r="B123" t="s">
         <v>822</v>
       </c>
@@ -26348,7 +26311,7 @@
       </c>
       <c r="DL123" s="45"/>
     </row>
-    <row r="124" spans="2:116" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="124" spans="2:116" ht="17.399999999999999">
       <c r="B124" t="s">
         <v>828</v>
       </c>
@@ -26373,7 +26336,7 @@
       </c>
       <c r="DL124" s="45"/>
     </row>
-    <row r="125" spans="2:116" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="125" spans="2:116" ht="17.399999999999999">
       <c r="B125" t="s">
         <v>833</v>
       </c>
@@ -26398,7 +26361,7 @@
       </c>
       <c r="DL125" s="45"/>
     </row>
-    <row r="126" spans="2:116" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="126" spans="2:116" ht="17.399999999999999">
       <c r="B126" t="s">
         <v>427</v>
       </c>
@@ -26423,7 +26386,7 @@
       </c>
       <c r="DL126" s="45"/>
     </row>
-    <row r="127" spans="2:116" x14ac:dyDescent="0.3">
+    <row r="127" spans="2:116">
       <c r="B127" t="s">
         <v>844</v>
       </c>
@@ -26448,7 +26411,7 @@
       </c>
       <c r="DL127" s="45"/>
     </row>
-    <row r="128" spans="2:116" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="128" spans="2:116" ht="17.399999999999999">
       <c r="B128" t="s">
         <v>850</v>
       </c>
@@ -26473,7 +26436,7 @@
       </c>
       <c r="DL128" s="45"/>
     </row>
-    <row r="129" spans="2:116" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="129" spans="2:116" ht="17.399999999999999">
       <c r="B129" t="s">
         <v>856</v>
       </c>
@@ -26498,7 +26461,7 @@
       </c>
       <c r="DL129" s="45"/>
     </row>
-    <row r="130" spans="2:116" x14ac:dyDescent="0.3">
+    <row r="130" spans="2:116">
       <c r="B130" t="s">
         <v>862</v>
       </c>
@@ -26523,7 +26486,7 @@
       </c>
       <c r="DL130" s="45"/>
     </row>
-    <row r="131" spans="2:116" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="131" spans="2:116" ht="17.399999999999999">
       <c r="B131" t="s">
         <v>868</v>
       </c>
@@ -26548,7 +26511,7 @@
       </c>
       <c r="DL131" s="45"/>
     </row>
-    <row r="132" spans="2:116" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="132" spans="2:116" ht="17.399999999999999">
       <c r="B132" t="s">
         <v>874</v>
       </c>
@@ -26573,7 +26536,7 @@
       </c>
       <c r="DL132" s="45"/>
     </row>
-    <row r="133" spans="2:116" x14ac:dyDescent="0.3">
+    <row r="133" spans="2:116">
       <c r="B133" t="s">
         <v>880</v>
       </c>
@@ -26598,7 +26561,7 @@
       </c>
       <c r="DL133" s="45"/>
     </row>
-    <row r="134" spans="2:116" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="134" spans="2:116" ht="17.399999999999999">
       <c r="B134" t="s">
         <v>886</v>
       </c>
@@ -26623,7 +26586,7 @@
       </c>
       <c r="DL134" s="45"/>
     </row>
-    <row r="135" spans="2:116" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="135" spans="2:116" ht="17.399999999999999">
       <c r="B135" t="s">
         <v>722</v>
       </c>
@@ -26645,7 +26608,7 @@
       <c r="M135" s="4"/>
       <c r="DL135" s="45"/>
     </row>
-    <row r="136" spans="2:116" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="136" spans="2:116" ht="17.399999999999999">
       <c r="B136" t="s">
         <v>897</v>
       </c>
@@ -26667,7 +26630,7 @@
       <c r="M136" s="4"/>
       <c r="DL136" s="45"/>
     </row>
-    <row r="137" spans="2:116" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="137" spans="2:116" ht="17.399999999999999">
       <c r="B137" t="s">
         <v>903</v>
       </c>
@@ -26689,7 +26652,7 @@
       <c r="M137" s="4"/>
       <c r="DL137" s="45"/>
     </row>
-    <row r="138" spans="2:116" x14ac:dyDescent="0.3">
+    <row r="138" spans="2:116">
       <c r="B138" t="s">
         <v>909</v>
       </c>
@@ -26711,7 +26674,7 @@
       <c r="M138" s="3"/>
       <c r="DL138" s="45"/>
     </row>
-    <row r="139" spans="2:116" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="139" spans="2:116" ht="17.399999999999999">
       <c r="B139" t="s">
         <v>915</v>
       </c>
@@ -26733,7 +26696,7 @@
       <c r="M139" s="4"/>
       <c r="DL139" s="45"/>
     </row>
-    <row r="140" spans="2:116" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="140" spans="2:116" ht="17.399999999999999">
       <c r="B140" t="s">
         <v>921</v>
       </c>
@@ -26755,7 +26718,7 @@
       <c r="M140" s="4"/>
       <c r="DL140" s="45"/>
     </row>
-    <row r="141" spans="2:116" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="141" spans="2:116" ht="17.399999999999999">
       <c r="B141" t="s">
         <v>927</v>
       </c>
@@ -26777,7 +26740,7 @@
       <c r="M141" s="4"/>
       <c r="DL141" s="45"/>
     </row>
-    <row r="142" spans="2:116" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="142" spans="2:116" ht="17.399999999999999">
       <c r="B142" t="s">
         <v>933</v>
       </c>
@@ -26799,7 +26762,7 @@
       <c r="M142" s="4"/>
       <c r="DL142" s="45"/>
     </row>
-    <row r="143" spans="2:116" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="143" spans="2:116" ht="17.399999999999999">
       <c r="B143" t="s">
         <v>939</v>
       </c>
@@ -26821,7 +26784,7 @@
       <c r="M143" s="4"/>
       <c r="DL143" s="45"/>
     </row>
-    <row r="144" spans="2:116" x14ac:dyDescent="0.3">
+    <row r="144" spans="2:116">
       <c r="B144" t="s">
         <v>945</v>
       </c>
@@ -26839,7 +26802,7 @@
       </c>
       <c r="DL144" s="45"/>
     </row>
-    <row r="145" spans="2:116" x14ac:dyDescent="0.3">
+    <row r="145" spans="2:116">
       <c r="B145" t="s">
         <v>950</v>
       </c>
@@ -26857,7 +26820,7 @@
       </c>
       <c r="DL145" s="45"/>
     </row>
-    <row r="146" spans="2:116" x14ac:dyDescent="0.3">
+    <row r="146" spans="2:116">
       <c r="B146" t="s">
         <v>955</v>
       </c>
@@ -26875,7 +26838,7 @@
       </c>
       <c r="DL146" s="45"/>
     </row>
-    <row r="147" spans="2:116" x14ac:dyDescent="0.3">
+    <row r="147" spans="2:116">
       <c r="B147" t="s">
         <v>960</v>
       </c>
@@ -26893,7 +26856,7 @@
       </c>
       <c r="DL147" s="45"/>
     </row>
-    <row r="148" spans="2:116" x14ac:dyDescent="0.3">
+    <row r="148" spans="2:116">
       <c r="B148" t="s">
         <v>965</v>
       </c>
@@ -26911,7 +26874,7 @@
       </c>
       <c r="DL148" s="45"/>
     </row>
-    <row r="149" spans="2:116" x14ac:dyDescent="0.3">
+    <row r="149" spans="2:116">
       <c r="B149" t="s">
         <v>970</v>
       </c>
@@ -26929,7 +26892,7 @@
       </c>
       <c r="DL149" s="45"/>
     </row>
-    <row r="150" spans="2:116" x14ac:dyDescent="0.3">
+    <row r="150" spans="2:116">
       <c r="B150" t="s">
         <v>975</v>
       </c>
@@ -26947,7 +26910,7 @@
       </c>
       <c r="DL150" s="45"/>
     </row>
-    <row r="151" spans="2:116" x14ac:dyDescent="0.3">
+    <row r="151" spans="2:116">
       <c r="B151" t="s">
         <v>980</v>
       </c>
@@ -26965,7 +26928,7 @@
       </c>
       <c r="DL151" s="45"/>
     </row>
-    <row r="152" spans="2:116" x14ac:dyDescent="0.3">
+    <row r="152" spans="2:116">
       <c r="B152" t="s">
         <v>985</v>
       </c>
@@ -26983,7 +26946,7 @@
       </c>
       <c r="DL152" s="45"/>
     </row>
-    <row r="153" spans="2:116" x14ac:dyDescent="0.3">
+    <row r="153" spans="2:116">
       <c r="B153" t="s">
         <v>990</v>
       </c>
@@ -27001,7 +26964,7 @@
       </c>
       <c r="DL153" s="45"/>
     </row>
-    <row r="154" spans="2:116" x14ac:dyDescent="0.3">
+    <row r="154" spans="2:116">
       <c r="B154" t="s">
         <v>995</v>
       </c>
@@ -27019,7 +26982,7 @@
       </c>
       <c r="DL154" s="45"/>
     </row>
-    <row r="155" spans="2:116" x14ac:dyDescent="0.3">
+    <row r="155" spans="2:116">
       <c r="B155" t="s">
         <v>1000</v>
       </c>
@@ -27034,7 +26997,7 @@
       </c>
       <c r="DL155" s="45"/>
     </row>
-    <row r="156" spans="2:116" x14ac:dyDescent="0.3">
+    <row r="156" spans="2:116">
       <c r="B156" t="s">
         <v>1004</v>
       </c>
@@ -27049,7 +27012,7 @@
       </c>
       <c r="DL156" s="45"/>
     </row>
-    <row r="157" spans="2:116" x14ac:dyDescent="0.3">
+    <row r="157" spans="2:116">
       <c r="B157" t="s">
         <v>1008</v>
       </c>
@@ -27064,7 +27027,7 @@
       </c>
       <c r="DL157" s="45"/>
     </row>
-    <row r="158" spans="2:116" x14ac:dyDescent="0.3">
+    <row r="158" spans="2:116">
       <c r="B158" t="s">
         <v>1012</v>
       </c>
@@ -27079,7 +27042,7 @@
       </c>
       <c r="DL158" s="45"/>
     </row>
-    <row r="159" spans="2:116" x14ac:dyDescent="0.3">
+    <row r="159" spans="2:116">
       <c r="B159" t="s">
         <v>1016</v>
       </c>
@@ -27094,7 +27057,7 @@
       </c>
       <c r="DL159" s="45"/>
     </row>
-    <row r="160" spans="2:116" x14ac:dyDescent="0.3">
+    <row r="160" spans="2:116">
       <c r="B160" t="s">
         <v>1020</v>
       </c>
@@ -27109,7 +27072,7 @@
       </c>
       <c r="DL160" s="45"/>
     </row>
-    <row r="161" spans="2:116" x14ac:dyDescent="0.3">
+    <row r="161" spans="2:116">
       <c r="B161" t="s">
         <v>1024</v>
       </c>
@@ -27124,7 +27087,7 @@
       </c>
       <c r="DL161" s="45"/>
     </row>
-    <row r="162" spans="2:116" x14ac:dyDescent="0.3">
+    <row r="162" spans="2:116">
       <c r="B162" t="s">
         <v>1028</v>
       </c>
@@ -27139,7 +27102,7 @@
       </c>
       <c r="DL162" s="45"/>
     </row>
-    <row r="163" spans="2:116" x14ac:dyDescent="0.3">
+    <row r="163" spans="2:116">
       <c r="B163" t="s">
         <v>1031</v>
       </c>
@@ -27154,7 +27117,7 @@
       </c>
       <c r="DL163" s="45"/>
     </row>
-    <row r="164" spans="2:116" x14ac:dyDescent="0.3">
+    <row r="164" spans="2:116">
       <c r="B164" t="s">
         <v>1035</v>
       </c>
@@ -27169,7 +27132,7 @@
       </c>
       <c r="DL164" s="45"/>
     </row>
-    <row r="165" spans="2:116" x14ac:dyDescent="0.3">
+    <row r="165" spans="2:116">
       <c r="B165" t="s">
         <v>1039</v>
       </c>
@@ -27184,7 +27147,7 @@
       </c>
       <c r="DL165" s="45"/>
     </row>
-    <row r="166" spans="2:116" x14ac:dyDescent="0.3">
+    <row r="166" spans="2:116">
       <c r="B166" t="s">
         <v>1043</v>
       </c>
@@ -27199,7 +27162,7 @@
       </c>
       <c r="DL166" s="45"/>
     </row>
-    <row r="167" spans="2:116" x14ac:dyDescent="0.3">
+    <row r="167" spans="2:116">
       <c r="B167" t="s">
         <v>1047</v>
       </c>
@@ -27214,7 +27177,7 @@
       </c>
       <c r="DL167" s="45"/>
     </row>
-    <row r="168" spans="2:116" x14ac:dyDescent="0.3">
+    <row r="168" spans="2:116">
       <c r="B168" t="s">
         <v>1051</v>
       </c>
@@ -27229,7 +27192,7 @@
       </c>
       <c r="DL168" s="45"/>
     </row>
-    <row r="169" spans="2:116" x14ac:dyDescent="0.3">
+    <row r="169" spans="2:116">
       <c r="B169" t="s">
         <v>1055</v>
       </c>
@@ -27244,7 +27207,7 @@
       </c>
       <c r="DL169" s="45"/>
     </row>
-    <row r="170" spans="2:116" x14ac:dyDescent="0.3">
+    <row r="170" spans="2:116">
       <c r="B170" t="s">
         <v>1059</v>
       </c>
@@ -27259,7 +27222,7 @@
       </c>
       <c r="DL170" s="45"/>
     </row>
-    <row r="171" spans="2:116" x14ac:dyDescent="0.3">
+    <row r="171" spans="2:116">
       <c r="B171" t="s">
         <v>1063</v>
       </c>
@@ -27274,7 +27237,7 @@
       </c>
       <c r="DL171" s="45"/>
     </row>
-    <row r="172" spans="2:116" x14ac:dyDescent="0.3">
+    <row r="172" spans="2:116">
       <c r="B172" t="s">
         <v>1067</v>
       </c>
@@ -27289,7 +27252,7 @@
       </c>
       <c r="DL172" s="45"/>
     </row>
-    <row r="173" spans="2:116" x14ac:dyDescent="0.3">
+    <row r="173" spans="2:116">
       <c r="B173" t="s">
         <v>1071</v>
       </c>
@@ -27304,7 +27267,7 @@
       </c>
       <c r="DL173" s="45"/>
     </row>
-    <row r="174" spans="2:116" x14ac:dyDescent="0.3">
+    <row r="174" spans="2:116">
       <c r="B174" t="s">
         <v>1075</v>
       </c>
@@ -27319,7 +27282,7 @@
       </c>
       <c r="DL174" s="45"/>
     </row>
-    <row r="175" spans="2:116" x14ac:dyDescent="0.3">
+    <row r="175" spans="2:116">
       <c r="B175" t="s">
         <v>1078</v>
       </c>
@@ -27334,7 +27297,7 @@
       </c>
       <c r="DL175" s="45"/>
     </row>
-    <row r="176" spans="2:116" x14ac:dyDescent="0.3">
+    <row r="176" spans="2:116">
       <c r="B176" t="s">
         <v>1082</v>
       </c>
@@ -27349,7 +27312,7 @@
       </c>
       <c r="DL176" s="45"/>
     </row>
-    <row r="177" spans="2:116" x14ac:dyDescent="0.3">
+    <row r="177" spans="2:116">
       <c r="B177" t="s">
         <v>1086</v>
       </c>
@@ -27364,7 +27327,7 @@
       </c>
       <c r="DL177" s="45"/>
     </row>
-    <row r="178" spans="2:116" x14ac:dyDescent="0.3">
+    <row r="178" spans="2:116">
       <c r="B178" t="s">
         <v>1090</v>
       </c>
@@ -27379,7 +27342,7 @@
       </c>
       <c r="DL178" s="45"/>
     </row>
-    <row r="179" spans="2:116" x14ac:dyDescent="0.3">
+    <row r="179" spans="2:116">
       <c r="B179" t="s">
         <v>1094</v>
       </c>
@@ -27394,7 +27357,7 @@
       </c>
       <c r="DL179" s="45"/>
     </row>
-    <row r="180" spans="2:116" x14ac:dyDescent="0.3">
+    <row r="180" spans="2:116">
       <c r="B180" t="s">
         <v>1098</v>
       </c>
@@ -27409,7 +27372,7 @@
       </c>
       <c r="DL180" s="45"/>
     </row>
-    <row r="181" spans="2:116" x14ac:dyDescent="0.3">
+    <row r="181" spans="2:116">
       <c r="B181" t="s">
         <v>1102</v>
       </c>
@@ -27424,7 +27387,7 @@
       </c>
       <c r="DL181" s="45"/>
     </row>
-    <row r="182" spans="2:116" x14ac:dyDescent="0.3">
+    <row r="182" spans="2:116">
       <c r="B182" t="s">
         <v>1106</v>
       </c>
@@ -27439,7 +27402,7 @@
       </c>
       <c r="DL182" s="45"/>
     </row>
-    <row r="183" spans="2:116" x14ac:dyDescent="0.3">
+    <row r="183" spans="2:116">
       <c r="B183" t="s">
         <v>1110</v>
       </c>
@@ -27454,7 +27417,7 @@
       </c>
       <c r="DL183" s="45"/>
     </row>
-    <row r="184" spans="2:116" x14ac:dyDescent="0.3">
+    <row r="184" spans="2:116">
       <c r="B184" t="s">
         <v>1114</v>
       </c>
@@ -27469,7 +27432,7 @@
       </c>
       <c r="DL184" s="45"/>
     </row>
-    <row r="185" spans="2:116" x14ac:dyDescent="0.3">
+    <row r="185" spans="2:116">
       <c r="B185" t="s">
         <v>1117</v>
       </c>
@@ -27484,7 +27447,7 @@
       </c>
       <c r="DL185" s="45"/>
     </row>
-    <row r="186" spans="2:116" x14ac:dyDescent="0.3">
+    <row r="186" spans="2:116">
       <c r="B186" t="s">
         <v>1121</v>
       </c>
@@ -27499,7 +27462,7 @@
       </c>
       <c r="DL186" s="45"/>
     </row>
-    <row r="187" spans="2:116" x14ac:dyDescent="0.3">
+    <row r="187" spans="2:116">
       <c r="B187" t="s">
         <v>1125</v>
       </c>
@@ -27514,7 +27477,7 @@
       </c>
       <c r="DL187" s="45"/>
     </row>
-    <row r="188" spans="2:116" x14ac:dyDescent="0.3">
+    <row r="188" spans="2:116">
       <c r="B188" t="s">
         <v>434</v>
       </c>
@@ -27529,7 +27492,7 @@
       </c>
       <c r="DL188" s="45"/>
     </row>
-    <row r="189" spans="2:116" x14ac:dyDescent="0.3">
+    <row r="189" spans="2:116">
       <c r="B189" t="s">
         <v>1132</v>
       </c>
@@ -27544,7 +27507,7 @@
       </c>
       <c r="DL189" s="45"/>
     </row>
-    <row r="190" spans="2:116" x14ac:dyDescent="0.3">
+    <row r="190" spans="2:116">
       <c r="B190" t="s">
         <v>1135</v>
       </c>
@@ -27559,7 +27522,7 @@
       </c>
       <c r="DL190" s="45"/>
     </row>
-    <row r="191" spans="2:116" x14ac:dyDescent="0.3">
+    <row r="191" spans="2:116">
       <c r="B191" t="s">
         <v>1139</v>
       </c>
@@ -27574,7 +27537,7 @@
       </c>
       <c r="DL191" s="45"/>
     </row>
-    <row r="192" spans="2:116" x14ac:dyDescent="0.3">
+    <row r="192" spans="2:116">
       <c r="B192" t="s">
         <v>1143</v>
       </c>
@@ -27589,7 +27552,7 @@
       </c>
       <c r="DL192" s="45"/>
     </row>
-    <row r="193" spans="2:116" x14ac:dyDescent="0.3">
+    <row r="193" spans="2:116">
       <c r="B193" t="s">
         <v>1147</v>
       </c>
@@ -27604,7 +27567,7 @@
       </c>
       <c r="DL193" s="45"/>
     </row>
-    <row r="194" spans="2:116" x14ac:dyDescent="0.3">
+    <row r="194" spans="2:116">
       <c r="B194" t="s">
         <v>1151</v>
       </c>
@@ -27619,7 +27582,7 @@
       </c>
       <c r="DL194" s="45"/>
     </row>
-    <row r="195" spans="2:116" x14ac:dyDescent="0.3">
+    <row r="195" spans="2:116">
       <c r="B195" t="s">
         <v>1155</v>
       </c>
@@ -27634,7 +27597,7 @@
       </c>
       <c r="DL195" s="45"/>
     </row>
-    <row r="196" spans="2:116" x14ac:dyDescent="0.3">
+    <row r="196" spans="2:116">
       <c r="E196" t="s">
         <v>1159</v>
       </c>
@@ -27646,7 +27609,7 @@
       </c>
       <c r="DL196" s="45"/>
     </row>
-    <row r="197" spans="2:116" x14ac:dyDescent="0.3">
+    <row r="197" spans="2:116">
       <c r="C197">
         <f>LEN(D10)</f>
         <v>47</v>
@@ -27662,7 +27625,7 @@
       </c>
       <c r="DL197" s="45"/>
     </row>
-    <row r="198" spans="2:116" x14ac:dyDescent="0.3">
+    <row r="198" spans="2:116">
       <c r="G198" t="s">
         <v>1165</v>
       </c>
@@ -27671,7 +27634,7 @@
       </c>
       <c r="DL198" s="45"/>
     </row>
-    <row r="199" spans="2:116" x14ac:dyDescent="0.3">
+    <row r="199" spans="2:116">
       <c r="G199" t="s">
         <v>1167</v>
       </c>
@@ -27680,7 +27643,7 @@
       </c>
       <c r="DL199" s="45"/>
     </row>
-    <row r="200" spans="2:116" x14ac:dyDescent="0.3">
+    <row r="200" spans="2:116">
       <c r="G200" t="s">
         <v>1169</v>
       </c>
@@ -27689,7 +27652,7 @@
       </c>
       <c r="DL200" s="45"/>
     </row>
-    <row r="201" spans="2:116" x14ac:dyDescent="0.3">
+    <row r="201" spans="2:116">
       <c r="G201" t="s">
         <v>1171</v>
       </c>
@@ -27698,7 +27661,7 @@
       </c>
       <c r="DL201" s="45"/>
     </row>
-    <row r="202" spans="2:116" x14ac:dyDescent="0.3">
+    <row r="202" spans="2:116">
       <c r="G202" t="s">
         <v>1173</v>
       </c>
@@ -27707,7 +27670,7 @@
       </c>
       <c r="DL202" s="45"/>
     </row>
-    <row r="203" spans="2:116" x14ac:dyDescent="0.3">
+    <row r="203" spans="2:116">
       <c r="G203" t="s">
         <v>1174</v>
       </c>
@@ -27716,7 +27679,7 @@
       </c>
       <c r="DL203" s="45"/>
     </row>
-    <row r="204" spans="2:116" x14ac:dyDescent="0.3">
+    <row r="204" spans="2:116">
       <c r="G204" t="s">
         <v>1176</v>
       </c>
@@ -27725,7 +27688,7 @@
       </c>
       <c r="DL204" s="45"/>
     </row>
-    <row r="205" spans="2:116" x14ac:dyDescent="0.3">
+    <row r="205" spans="2:116">
       <c r="G205" t="s">
         <v>1178</v>
       </c>
@@ -27734,7 +27697,7 @@
       </c>
       <c r="DL205" s="45"/>
     </row>
-    <row r="206" spans="2:116" x14ac:dyDescent="0.3">
+    <row r="206" spans="2:116">
       <c r="G206" t="s">
         <v>1180</v>
       </c>
@@ -27743,7 +27706,7 @@
       </c>
       <c r="DL206" s="45"/>
     </row>
-    <row r="207" spans="2:116" x14ac:dyDescent="0.3">
+    <row r="207" spans="2:116">
       <c r="G207" t="s">
         <v>1182</v>
       </c>
@@ -27752,7 +27715,7 @@
       </c>
       <c r="DL207" s="45"/>
     </row>
-    <row r="208" spans="2:116" x14ac:dyDescent="0.3">
+    <row r="208" spans="2:116">
       <c r="G208" t="s">
         <v>1184</v>
       </c>
@@ -27761,7 +27724,7 @@
       </c>
       <c r="DL208" s="45"/>
     </row>
-    <row r="209" spans="7:116" x14ac:dyDescent="0.3">
+    <row r="209" spans="7:116">
       <c r="G209" t="s">
         <v>1186</v>
       </c>
@@ -27770,7 +27733,7 @@
       </c>
       <c r="DL209" s="45"/>
     </row>
-    <row r="210" spans="7:116" x14ac:dyDescent="0.3">
+    <row r="210" spans="7:116">
       <c r="G210" t="s">
         <v>1188</v>
       </c>
@@ -27779,7 +27742,7 @@
       </c>
       <c r="DL210" s="45"/>
     </row>
-    <row r="211" spans="7:116" x14ac:dyDescent="0.3">
+    <row r="211" spans="7:116">
       <c r="G211" t="s">
         <v>1190</v>
       </c>
@@ -27788,7 +27751,7 @@
       </c>
       <c r="DL211" s="45"/>
     </row>
-    <row r="212" spans="7:116" x14ac:dyDescent="0.3">
+    <row r="212" spans="7:116">
       <c r="G212" t="s">
         <v>1192</v>
       </c>
@@ -27797,7 +27760,7 @@
       </c>
       <c r="DL212" s="45"/>
     </row>
-    <row r="213" spans="7:116" x14ac:dyDescent="0.3">
+    <row r="213" spans="7:116">
       <c r="G213" t="s">
         <v>1194</v>
       </c>
@@ -27806,7 +27769,7 @@
       </c>
       <c r="DL213" s="45"/>
     </row>
-    <row r="214" spans="7:116" x14ac:dyDescent="0.3">
+    <row r="214" spans="7:116">
       <c r="G214" t="s">
         <v>1196</v>
       </c>
@@ -27815,7 +27778,7 @@
       </c>
       <c r="DL214" s="45"/>
     </row>
-    <row r="215" spans="7:116" x14ac:dyDescent="0.3">
+    <row r="215" spans="7:116">
       <c r="G215" t="s">
         <v>1198</v>
       </c>
@@ -27824,7 +27787,7 @@
       </c>
       <c r="DL215" s="45"/>
     </row>
-    <row r="216" spans="7:116" x14ac:dyDescent="0.3">
+    <row r="216" spans="7:116">
       <c r="G216" t="s">
         <v>1200</v>
       </c>
@@ -27833,7 +27796,7 @@
       </c>
       <c r="DL216" s="45"/>
     </row>
-    <row r="217" spans="7:116" x14ac:dyDescent="0.3">
+    <row r="217" spans="7:116">
       <c r="G217" t="s">
         <v>1202</v>
       </c>
@@ -27842,7 +27805,7 @@
       </c>
       <c r="DL217" s="45"/>
     </row>
-    <row r="218" spans="7:116" x14ac:dyDescent="0.3">
+    <row r="218" spans="7:116">
       <c r="G218" t="s">
         <v>1204</v>
       </c>
@@ -27851,7 +27814,7 @@
       </c>
       <c r="DL218" s="45"/>
     </row>
-    <row r="219" spans="7:116" x14ac:dyDescent="0.3">
+    <row r="219" spans="7:116">
       <c r="G219" t="s">
         <v>1206</v>
       </c>
@@ -27860,7 +27823,7 @@
       </c>
       <c r="DL219" s="45"/>
     </row>
-    <row r="220" spans="7:116" x14ac:dyDescent="0.3">
+    <row r="220" spans="7:116">
       <c r="G220" t="s">
         <v>1208</v>
       </c>
@@ -27869,7 +27832,7 @@
       </c>
       <c r="DL220" s="45"/>
     </row>
-    <row r="221" spans="7:116" x14ac:dyDescent="0.3">
+    <row r="221" spans="7:116">
       <c r="G221" t="s">
         <v>1210</v>
       </c>
@@ -27878,7 +27841,7 @@
       </c>
       <c r="DL221" s="45"/>
     </row>
-    <row r="222" spans="7:116" x14ac:dyDescent="0.3">
+    <row r="222" spans="7:116">
       <c r="G222" t="s">
         <v>1212</v>
       </c>
@@ -27887,7 +27850,7 @@
       </c>
       <c r="DL222" s="45"/>
     </row>
-    <row r="223" spans="7:116" x14ac:dyDescent="0.3">
+    <row r="223" spans="7:116">
       <c r="G223" t="s">
         <v>1214</v>
       </c>
@@ -27896,7 +27859,7 @@
       </c>
       <c r="DL223" s="45"/>
     </row>
-    <row r="224" spans="7:116" x14ac:dyDescent="0.3">
+    <row r="224" spans="7:116">
       <c r="G224" t="s">
         <v>1215</v>
       </c>
@@ -27905,7 +27868,7 @@
       </c>
       <c r="DL224" s="45"/>
     </row>
-    <row r="225" spans="7:116" x14ac:dyDescent="0.3">
+    <row r="225" spans="7:116">
       <c r="G225" t="s">
         <v>1217</v>
       </c>
@@ -27914,7 +27877,7 @@
       </c>
       <c r="DL225" s="45"/>
     </row>
-    <row r="226" spans="7:116" x14ac:dyDescent="0.3">
+    <row r="226" spans="7:116">
       <c r="G226" t="s">
         <v>1219</v>
       </c>
@@ -27923,7 +27886,7 @@
       </c>
       <c r="DL226" s="45"/>
     </row>
-    <row r="227" spans="7:116" x14ac:dyDescent="0.3">
+    <row r="227" spans="7:116">
       <c r="G227" t="s">
         <v>1221</v>
       </c>
@@ -27932,7 +27895,7 @@
       </c>
       <c r="DL227" s="45"/>
     </row>
-    <row r="228" spans="7:116" x14ac:dyDescent="0.3">
+    <row r="228" spans="7:116">
       <c r="G228" t="s">
         <v>1223</v>
       </c>
@@ -27941,7 +27904,7 @@
       </c>
       <c r="DL228" s="45"/>
     </row>
-    <row r="229" spans="7:116" x14ac:dyDescent="0.3">
+    <row r="229" spans="7:116">
       <c r="G229" t="s">
         <v>1225</v>
       </c>
@@ -27950,7 +27913,7 @@
       </c>
       <c r="DL229" s="45"/>
     </row>
-    <row r="230" spans="7:116" x14ac:dyDescent="0.3">
+    <row r="230" spans="7:116">
       <c r="G230" t="s">
         <v>1227</v>
       </c>
@@ -27959,7 +27922,7 @@
       </c>
       <c r="DL230" s="45"/>
     </row>
-    <row r="231" spans="7:116" x14ac:dyDescent="0.3">
+    <row r="231" spans="7:116">
       <c r="G231" t="s">
         <v>1229</v>
       </c>
@@ -27968,7 +27931,7 @@
       </c>
       <c r="DL231" s="45"/>
     </row>
-    <row r="232" spans="7:116" x14ac:dyDescent="0.3">
+    <row r="232" spans="7:116">
       <c r="G232" t="s">
         <v>1231</v>
       </c>
@@ -27977,7 +27940,7 @@
       </c>
       <c r="DL232" s="45"/>
     </row>
-    <row r="233" spans="7:116" x14ac:dyDescent="0.3">
+    <row r="233" spans="7:116">
       <c r="G233" t="s">
         <v>1233</v>
       </c>
@@ -27986,7 +27949,7 @@
       </c>
       <c r="DL233" s="45"/>
     </row>
-    <row r="234" spans="7:116" x14ac:dyDescent="0.3">
+    <row r="234" spans="7:116">
       <c r="G234" t="s">
         <v>1235</v>
       </c>
@@ -27995,7 +27958,7 @@
       </c>
       <c r="DL234" s="45"/>
     </row>
-    <row r="235" spans="7:116" x14ac:dyDescent="0.3">
+    <row r="235" spans="7:116">
       <c r="G235" t="s">
         <v>1237</v>
       </c>
@@ -28004,7 +27967,7 @@
       </c>
       <c r="DL235" s="45"/>
     </row>
-    <row r="236" spans="7:116" x14ac:dyDescent="0.3">
+    <row r="236" spans="7:116">
       <c r="G236" t="s">
         <v>1239</v>
       </c>
@@ -28013,7 +27976,7 @@
       </c>
       <c r="DL236" s="45"/>
     </row>
-    <row r="237" spans="7:116" x14ac:dyDescent="0.3">
+    <row r="237" spans="7:116">
       <c r="G237" t="s">
         <v>1241</v>
       </c>
@@ -28022,7 +27985,7 @@
       </c>
       <c r="DL237" s="45"/>
     </row>
-    <row r="238" spans="7:116" x14ac:dyDescent="0.3">
+    <row r="238" spans="7:116">
       <c r="G238" t="s">
         <v>1243</v>
       </c>
@@ -28031,7 +27994,7 @@
       </c>
       <c r="DL238" s="45"/>
     </row>
-    <row r="239" spans="7:116" x14ac:dyDescent="0.3">
+    <row r="239" spans="7:116">
       <c r="G239" t="s">
         <v>1245</v>
       </c>
@@ -28040,7 +28003,7 @@
       </c>
       <c r="DL239" s="45"/>
     </row>
-    <row r="240" spans="7:116" x14ac:dyDescent="0.3">
+    <row r="240" spans="7:116">
       <c r="G240" t="s">
         <v>1247</v>
       </c>
@@ -28049,7 +28012,7 @@
       </c>
       <c r="DL240" s="45"/>
     </row>
-    <row r="241" spans="7:116" x14ac:dyDescent="0.3">
+    <row r="241" spans="7:116">
       <c r="G241" t="s">
         <v>1249</v>
       </c>
@@ -28058,7 +28021,7 @@
       </c>
       <c r="DL241" s="45"/>
     </row>
-    <row r="242" spans="7:116" x14ac:dyDescent="0.3">
+    <row r="242" spans="7:116">
       <c r="G242" t="s">
         <v>1251</v>
       </c>
@@ -28067,7 +28030,7 @@
       </c>
       <c r="DL242" s="45"/>
     </row>
-    <row r="243" spans="7:116" x14ac:dyDescent="0.3">
+    <row r="243" spans="7:116">
       <c r="G243" t="s">
         <v>1253</v>
       </c>
@@ -28076,7 +28039,7 @@
       </c>
       <c r="DL243" s="45"/>
     </row>
-    <row r="244" spans="7:116" x14ac:dyDescent="0.3">
+    <row r="244" spans="7:116">
       <c r="G244" t="s">
         <v>1255</v>
       </c>
@@ -28085,7 +28048,7 @@
       </c>
       <c r="DL244" s="45"/>
     </row>
-    <row r="245" spans="7:116" x14ac:dyDescent="0.3">
+    <row r="245" spans="7:116">
       <c r="G245" t="s">
         <v>1257</v>
       </c>
@@ -28094,7 +28057,7 @@
       </c>
       <c r="DL245" s="45"/>
     </row>
-    <row r="246" spans="7:116" x14ac:dyDescent="0.3">
+    <row r="246" spans="7:116">
       <c r="G246" t="s">
         <v>1258</v>
       </c>
@@ -28103,7 +28066,7 @@
       </c>
       <c r="DL246" s="45"/>
     </row>
-    <row r="247" spans="7:116" x14ac:dyDescent="0.3">
+    <row r="247" spans="7:116">
       <c r="G247" t="s">
         <v>1260</v>
       </c>
@@ -28112,7 +28075,7 @@
       </c>
       <c r="DL247" s="45"/>
     </row>
-    <row r="248" spans="7:116" x14ac:dyDescent="0.3">
+    <row r="248" spans="7:116">
       <c r="G248" t="s">
         <v>1262</v>
       </c>
@@ -28121,7 +28084,7 @@
       </c>
       <c r="DL248" s="45"/>
     </row>
-    <row r="249" spans="7:116" x14ac:dyDescent="0.3">
+    <row r="249" spans="7:116">
       <c r="G249" t="s">
         <v>1264</v>
       </c>
@@ -28130,7 +28093,7 @@
       </c>
       <c r="DL249" s="45"/>
     </row>
-    <row r="250" spans="7:116" x14ac:dyDescent="0.3">
+    <row r="250" spans="7:116">
       <c r="G250" t="s">
         <v>1266</v>
       </c>
@@ -28139,7 +28102,7 @@
       </c>
       <c r="DL250" s="45"/>
     </row>
-    <row r="251" spans="7:116" x14ac:dyDescent="0.3">
+    <row r="251" spans="7:116">
       <c r="G251" t="s">
         <v>1268</v>
       </c>
@@ -28148,7 +28111,7 @@
       </c>
       <c r="DL251" s="45"/>
     </row>
-    <row r="252" spans="7:116" x14ac:dyDescent="0.3">
+    <row r="252" spans="7:116">
       <c r="G252" t="s">
         <v>1270</v>
       </c>
@@ -28157,7 +28120,7 @@
       </c>
       <c r="DL252" s="45"/>
     </row>
-    <row r="253" spans="7:116" x14ac:dyDescent="0.3">
+    <row r="253" spans="7:116">
       <c r="G253" t="s">
         <v>1272</v>
       </c>
@@ -28166,7 +28129,7 @@
       </c>
       <c r="DL253" s="45"/>
     </row>
-    <row r="254" spans="7:116" x14ac:dyDescent="0.3">
+    <row r="254" spans="7:116">
       <c r="G254" t="s">
         <v>1273</v>
       </c>
@@ -28175,7 +28138,7 @@
       </c>
       <c r="DL254" s="45"/>
     </row>
-    <row r="255" spans="7:116" x14ac:dyDescent="0.3">
+    <row r="255" spans="7:116">
       <c r="G255" t="s">
         <v>1275</v>
       </c>
@@ -28184,7 +28147,7 @@
       </c>
       <c r="DL255" s="45"/>
     </row>
-    <row r="256" spans="7:116" x14ac:dyDescent="0.3">
+    <row r="256" spans="7:116">
       <c r="G256" t="s">
         <v>1277</v>
       </c>
@@ -28193,7 +28156,7 @@
       </c>
       <c r="DL256" s="45"/>
     </row>
-    <row r="257" spans="7:116" x14ac:dyDescent="0.3">
+    <row r="257" spans="7:116">
       <c r="G257" t="s">
         <v>1279</v>
       </c>
@@ -28202,7 +28165,7 @@
       </c>
       <c r="DL257" s="45"/>
     </row>
-    <row r="258" spans="7:116" x14ac:dyDescent="0.3">
+    <row r="258" spans="7:116">
       <c r="G258" t="s">
         <v>1281</v>
       </c>
@@ -28211,7 +28174,7 @@
       </c>
       <c r="DL258" s="45"/>
     </row>
-    <row r="259" spans="7:116" x14ac:dyDescent="0.3">
+    <row r="259" spans="7:116">
       <c r="G259" t="s">
         <v>1283</v>
       </c>
@@ -28220,7 +28183,7 @@
       </c>
       <c r="DL259" s="45"/>
     </row>
-    <row r="260" spans="7:116" x14ac:dyDescent="0.3">
+    <row r="260" spans="7:116">
       <c r="G260" t="s">
         <v>1285</v>
       </c>
@@ -28229,7 +28192,7 @@
       </c>
       <c r="DL260" s="45"/>
     </row>
-    <row r="261" spans="7:116" x14ac:dyDescent="0.3">
+    <row r="261" spans="7:116">
       <c r="G261" t="s">
         <v>1287</v>
       </c>
@@ -28238,7 +28201,7 @@
       </c>
       <c r="DL261" s="45"/>
     </row>
-    <row r="262" spans="7:116" x14ac:dyDescent="0.3">
+    <row r="262" spans="7:116">
       <c r="G262" t="s">
         <v>1289</v>
       </c>
@@ -28247,7 +28210,7 @@
       </c>
       <c r="DL262" s="45"/>
     </row>
-    <row r="263" spans="7:116" x14ac:dyDescent="0.3">
+    <row r="263" spans="7:116">
       <c r="G263" t="s">
         <v>1291</v>
       </c>
@@ -28256,7 +28219,7 @@
       </c>
       <c r="DL263" s="45"/>
     </row>
-    <row r="264" spans="7:116" x14ac:dyDescent="0.3">
+    <row r="264" spans="7:116">
       <c r="G264" t="s">
         <v>1293</v>
       </c>
@@ -28265,7 +28228,7 @@
       </c>
       <c r="DL264" s="45"/>
     </row>
-    <row r="265" spans="7:116" x14ac:dyDescent="0.3">
+    <row r="265" spans="7:116">
       <c r="G265" t="s">
         <v>1295</v>
       </c>
@@ -28274,7 +28237,7 @@
       </c>
       <c r="DL265" s="45"/>
     </row>
-    <row r="266" spans="7:116" x14ac:dyDescent="0.3">
+    <row r="266" spans="7:116">
       <c r="G266" t="s">
         <v>1297</v>
       </c>
@@ -28283,7 +28246,7 @@
       </c>
       <c r="DL266" s="45"/>
     </row>
-    <row r="267" spans="7:116" x14ac:dyDescent="0.3">
+    <row r="267" spans="7:116">
       <c r="G267" t="s">
         <v>1299</v>
       </c>
@@ -28292,7 +28255,7 @@
       </c>
       <c r="DL267" s="45"/>
     </row>
-    <row r="268" spans="7:116" x14ac:dyDescent="0.3">
+    <row r="268" spans="7:116">
       <c r="G268" t="s">
         <v>1301</v>
       </c>
@@ -28301,7 +28264,7 @@
       </c>
       <c r="DL268" s="45"/>
     </row>
-    <row r="269" spans="7:116" x14ac:dyDescent="0.3">
+    <row r="269" spans="7:116">
       <c r="G269" t="s">
         <v>1303</v>
       </c>
@@ -28310,7 +28273,7 @@
       </c>
       <c r="DL269" s="45"/>
     </row>
-    <row r="270" spans="7:116" x14ac:dyDescent="0.3">
+    <row r="270" spans="7:116">
       <c r="G270" t="s">
         <v>1305</v>
       </c>
@@ -28319,7 +28282,7 @@
       </c>
       <c r="DL270" s="45"/>
     </row>
-    <row r="271" spans="7:116" x14ac:dyDescent="0.3">
+    <row r="271" spans="7:116">
       <c r="G271" t="s">
         <v>1307</v>
       </c>
@@ -28328,7 +28291,7 @@
       </c>
       <c r="DL271" s="45"/>
     </row>
-    <row r="272" spans="7:116" x14ac:dyDescent="0.3">
+    <row r="272" spans="7:116">
       <c r="G272" t="s">
         <v>1309</v>
       </c>
@@ -28337,7 +28300,7 @@
       </c>
       <c r="DL272" s="45"/>
     </row>
-    <row r="273" spans="7:116" x14ac:dyDescent="0.3">
+    <row r="273" spans="7:116">
       <c r="G273" t="s">
         <v>1311</v>
       </c>
@@ -28346,7 +28309,7 @@
       </c>
       <c r="DL273" s="45"/>
     </row>
-    <row r="274" spans="7:116" x14ac:dyDescent="0.3">
+    <row r="274" spans="7:116">
       <c r="G274" t="s">
         <v>1313</v>
       </c>
@@ -28355,7 +28318,7 @@
       </c>
       <c r="DL274" s="45"/>
     </row>
-    <row r="275" spans="7:116" x14ac:dyDescent="0.3">
+    <row r="275" spans="7:116">
       <c r="G275" t="s">
         <v>1315</v>
       </c>
@@ -28364,7 +28327,7 @@
       </c>
       <c r="DL275" s="45"/>
     </row>
-    <row r="276" spans="7:116" x14ac:dyDescent="0.3">
+    <row r="276" spans="7:116">
       <c r="G276" t="s">
         <v>1316</v>
       </c>
@@ -28373,7 +28336,7 @@
       </c>
       <c r="DL276" s="45"/>
     </row>
-    <row r="277" spans="7:116" x14ac:dyDescent="0.3">
+    <row r="277" spans="7:116">
       <c r="G277" t="s">
         <v>1318</v>
       </c>
@@ -28383,7 +28346,7 @@
       <c r="DL277" s="45"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="Zb7QGKiIC6Wl2lyUtfjLF/D6ZW1H8inEEmfEH0uFndA4q5TvkmjTrzQQmfZOJ+6GvRKbzSPVryI/d8E16CwXwA==" saltValue="a2whRBu5crk7z/7hqsaMHg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="mWqPlp+N+1eI5QZLhNdj52cX2jSAPxyjUBaPAJ9k+tHmErdl8clBXQfn2ID43+7l0pRxqjM4SlKI8pp518drMQ==" saltValue="TGTifRtdnahIelhqRBERSA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="2">
     <mergeCell ref="M27:M28"/>
     <mergeCell ref="M34:M35"/>

</xml_diff>

<commit_message>
Changed default view of the template
</commit_message>
<xml_diff>
--- a/Excel_templates/MOSAIC_input_excel_file_2022.xlsx
+++ b/Excel_templates/MOSAIC_input_excel_file_2022.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sparadis\Documents\ETH\MOSAIC\MOSAIC_Client\Excel_templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8FACFBB9-8918-4CCC-AD2E-8686C6950B48}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47CE022C-3ACC-4BBF-A8F7-77DB1A7F15FE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30204" yWindow="10044" windowWidth="40020" windowHeight="22296" tabRatio="694" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30204" yWindow="10044" windowWidth="40020" windowHeight="22296" tabRatio="694" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ARTICLE_AUTHOR" sheetId="3" r:id="rId1"/>
@@ -10293,11 +10293,11 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A3" sqref="A3:G3"/>
+      <selection pane="bottomRight" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -10390,7 +10390,7 @@
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F3" sqref="F3"/>
+      <selection pane="bottomRight" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -12171,7 +12171,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:CB52"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane xSplit="3" ySplit="6" topLeftCell="D7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
@@ -14910,7 +14910,7 @@
   <dimension ref="A1:HL277"/>
   <sheetViews>
     <sheetView topLeftCell="GQ1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="GZ14" sqref="GZ14"/>
+      <selection activeCell="GZ8" sqref="GZ8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>

</xml_diff>

<commit_message>
Corrected cell of sample_name
</commit_message>
<xml_diff>
--- a/Excel_templates/MOSAIC_input_excel_file_2022.xlsx
+++ b/Excel_templates/MOSAIC_input_excel_file_2022.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sparadis\Documents\ETH\MOSAIC\MOSAIC_Client\Excel_templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DC7C3C1-A5AD-4297-B076-BE30BE07FC44}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F1A0407-BC41-4306-B856-7A6EF44746E2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30204" yWindow="10044" windowWidth="40020" windowHeight="22296" tabRatio="694" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30204" yWindow="10044" windowWidth="40020" windowHeight="22296" tabRatio="694" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ARTICLE_AUTHOR" sheetId="3" r:id="rId1"/>
@@ -10281,7 +10281,7 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -12139,7 +12139,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:CB52"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane xSplit="3" ySplit="6" topLeftCell="D7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
@@ -14864,7 +14864,7 @@
           <x14:formula1>
             <xm:f>GEOPOINTS_CORES!$B$3:$B$1048576</xm:f>
           </x14:formula1>
-          <xm:sqref>B7:B1048576 C7</xm:sqref>
+          <xm:sqref>B7:B1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Eliminated the drop-down in the sample_analyses sheet
</commit_message>
<xml_diff>
--- a/Excel_templates/MOSAIC_input_excel_file_2022.xlsx
+++ b/Excel_templates/MOSAIC_input_excel_file_2022.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sparadis\Documents\ETH\MOSAIC\MOSAIC_Client\Excel_templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F1A0407-BC41-4306-B856-7A6EF44746E2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7610F707-9709-44D6-B37B-34E9ED73D752}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30204" yWindow="10044" windowWidth="40020" windowHeight="22296" tabRatio="694" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30204" yWindow="10044" windowWidth="40020" windowHeight="22296" tabRatio="694" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ARTICLE_AUTHOR" sheetId="3" r:id="rId1"/>
@@ -10281,7 +10281,7 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -12139,7 +12139,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:CB52"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane xSplit="3" ySplit="6" topLeftCell="D7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
@@ -14792,7 +14792,7 @@
     <mergeCell ref="D2:D6"/>
     <mergeCell ref="E2:E6"/>
   </mergeCells>
-  <dataValidations xWindow="389" yWindow="346" count="13">
+  <dataValidations xWindow="389" yWindow="346" count="12">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Write the core_name or select from the drop-down menu the cores you have in the Workbook._x000a_Make sure that the core name matches with its metadata given in GEOPOINTS_CORES sheet" sqref="B2:B4" xr:uid="{6685FF74-A7F2-42C2-901B-99DBBBFECDB4}"/>
     <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Sample analysis category" prompt="Choose from the drop-down list the analysis category the variable belongs to" sqref="L1:CB1" xr:uid="{2372D2F3-EE0C-4296-AC86-BA3569CC20EF}">
       <formula1>Sample_analyses_types</formula1>
@@ -14806,9 +14806,6 @@
     </dataValidation>
     <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Core depth should be positive." prompt="Average sample depth of the sample (i.e. 0.5 cm)" sqref="J7:J1048576" xr:uid="{76CC5D1F-1565-4594-B5AF-8B25948B4A60}">
       <formula1>0</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="Q8:Q27 N7:CB7 L7:L19" xr:uid="{6673B6D2-9563-46FC-8335-F6B94E523361}">
-      <formula1>INDIRECT(L$2)</formula1>
     </dataValidation>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Name of user who is entering data" sqref="A7:A1048576" xr:uid="{4BF522A4-2999-4EF9-835E-16C3A98D1BAF}"/>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Sample analysis" prompt="Choose from the drop-down menu the variable to be added" sqref="L2:CB2" xr:uid="{ADED0455-8DDC-445F-B013-7A6BE4A4748B}">

</xml_diff>

<commit_message>
Added methods for Rock Eval analyses, as well as modified the variable of OI to include the unit, as well.
</commit_message>
<xml_diff>
--- a/Excel_templates/MOSAIC_input_excel_file_2022.xlsx
+++ b/Excel_templates/MOSAIC_input_excel_file_2022.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sparadis\Documents\ETH\MOSAIC\MOSAIC_Client\Excel_templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAD424B3-DD92-404A-9639-D9594D62959D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8E5B34D-AA46-4320-BD7D-F6E37488DB42}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30204" yWindow="10044" windowWidth="40020" windowHeight="22296" tabRatio="694" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30204" yWindow="10044" windowWidth="40020" windowHeight="22296" tabRatio="694" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ARTICLE_AUTHOR" sheetId="3" r:id="rId1"/>
@@ -65,6 +65,7 @@
     <definedName name="Germany">SET_VARIABLES!$AC$2:$AC$29</definedName>
     <definedName name="gravel_">SET_VARIABLES!$EQ$2:$EQ$4</definedName>
     <definedName name="Greece">SET_VARIABLES!$AD$2:$AD$8</definedName>
+    <definedName name="HI_mgHC_OCg">SET_VARIABLES!$GT$2:$GT$3</definedName>
     <definedName name="Iceland">SET_VARIABLES!$AE$2:$AE$5</definedName>
     <definedName name="India">SET_VARIABLES!$AF$2:$AF$25</definedName>
     <definedName name="inorganic_nitrogen_">SET_VARIABLES!$FH$2:$FH$4</definedName>
@@ -93,6 +94,7 @@
     <definedName name="Norway">SET_VARIABLES!$AO$2:$AO$13</definedName>
     <definedName name="OCON_ratio">SET_VARIABLES!$FJ$2:$FJ$4</definedName>
     <definedName name="OCTN_ratio">SET_VARIABLES!$FK$2:$FK$4</definedName>
+    <definedName name="OI_mgCO2_gTOC">SET_VARIABLES!$GU$2:$GU$3</definedName>
     <definedName name="OM_LOI_">SET_VARIABLES!$FD$2:$FD$8</definedName>
     <definedName name="organic_nitrogen_">SET_VARIABLES!$FG$2:$FG$4</definedName>
     <definedName name="P_org_">SET_VARIABLES!$FM$2:$FM$4</definedName>
@@ -110,6 +112,9 @@
     <definedName name="Romania">SET_VARIABLES!$AU$2:$AU$4</definedName>
     <definedName name="Russia">SET_VARIABLES!$AW$2:$AW$134</definedName>
     <definedName name="S_total_">SET_VARIABLES!$FO$2:$FO$4</definedName>
+    <definedName name="S1_mgHC_g">SET_VARIABLES!$GV$2:$GV$3</definedName>
+    <definedName name="S2_mgHC_g">SET_VARIABLES!$GW$2:$GW$3</definedName>
+    <definedName name="S3_mgHC_g">SET_VARIABLES!$GX$2:$GX$3</definedName>
     <definedName name="sample_14C">SET_VARIABLES!$BZ$2:$BZ$9</definedName>
     <definedName name="sample_aliphatic_carbons">SET_VARIABLES!$CU$2:$CU$32</definedName>
     <definedName name="sample_alkenones">SET_VARIABLES!$CR$2:$CR$11</definedName>
@@ -145,6 +150,7 @@
     <definedName name="surface_area_m2_g">SET_VARIABLES!$EZ$2:$EZ$12</definedName>
     <definedName name="Taiwan_Republic_of_China">SET_VARIABLES!$BA$2:$BA$9</definedName>
     <definedName name="Th232_Bq_kg">SET_VARIABLES!$GC$2:$GC$4</definedName>
+    <definedName name="Tmax">SET_VARIABLES!$GS$2:$GS$3</definedName>
     <definedName name="total_carbon_">SET_VARIABLES!$FC$2:$FC$4</definedName>
     <definedName name="total_inorganic_carbon_">SET_VARIABLES!$FE$2:$FE$4</definedName>
     <definedName name="total_nitrogen_">SET_VARIABLES!$FI$2:$FI$4</definedName>
@@ -186,7 +192,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3718" uniqueCount="2910">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3733" uniqueCount="2913">
   <si>
     <t>sample_name</t>
   </si>
@@ -7577,9 +7583,6 @@
     <t>Tmax</t>
   </si>
   <si>
-    <t>OI</t>
-  </si>
-  <si>
     <t>S1_mgHC_g</t>
   </si>
   <si>
@@ -8916,6 +8919,18 @@
   </si>
   <si>
     <t>TOC</t>
+  </si>
+  <si>
+    <t>º Celsius</t>
+  </si>
+  <si>
+    <t>OI_mgCO2_gTOC</t>
+  </si>
+  <si>
+    <t>mg CO2·g TOC-1</t>
+  </si>
+  <si>
+    <t>Oxygen index</t>
   </si>
 </sst>
 </file>
@@ -9949,7 +9964,7 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -9971,7 +9986,7 @@
   <sheetData>
     <row r="1" spans="1:8" s="59" customFormat="1" ht="20.399999999999999" thickBot="1">
       <c r="A1" s="85" t="s">
-        <v>2578</v>
+        <v>2577</v>
       </c>
       <c r="B1" s="85"/>
       <c r="C1" s="85"/>
@@ -9982,10 +9997,10 @@
     </row>
     <row r="2" spans="1:8" s="26" customFormat="1">
       <c r="A2" s="49" t="s">
-        <v>2511</v>
+        <v>2510</v>
       </c>
       <c r="B2" s="49" t="s">
-        <v>2588</v>
+        <v>2587</v>
       </c>
       <c r="C2" s="30" t="s">
         <v>1818</v>
@@ -9994,7 +10009,7 @@
         <v>1819</v>
       </c>
       <c r="E2" s="49" t="s">
-        <v>2589</v>
+        <v>2588</v>
       </c>
       <c r="F2" s="49" t="s">
         <v>1820</v>
@@ -10003,7 +10018,7 @@
         <v>1821</v>
       </c>
       <c r="H2" s="67" t="s">
-        <v>2746</v>
+        <v>2745</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -10069,14 +10084,14 @@
   <sheetData>
     <row r="1" spans="1:16" s="58" customFormat="1" ht="20.399999999999999" thickBot="1">
       <c r="A1" s="87" t="s">
-        <v>2579</v>
+        <v>2578</v>
       </c>
       <c r="B1" s="87"/>
       <c r="C1" s="87"/>
       <c r="D1" s="87"/>
       <c r="E1" s="87"/>
       <c r="F1" s="86" t="s">
-        <v>2717</v>
+        <v>2716</v>
       </c>
       <c r="G1" s="86"/>
       <c r="H1" s="86"/>
@@ -10091,7 +10106,7 @@
     </row>
     <row r="2" spans="1:16" s="61" customFormat="1">
       <c r="A2" s="57" t="s">
-        <v>2511</v>
+        <v>2510</v>
       </c>
       <c r="B2" s="57" t="s">
         <v>1822</v>
@@ -10103,7 +10118,7 @@
         <v>1824</v>
       </c>
       <c r="E2" s="57" t="s">
-        <v>2904</v>
+        <v>2903</v>
       </c>
       <c r="F2" s="60" t="s">
         <v>1825</v>
@@ -10333,11 +10348,11 @@
   <sheetData>
     <row r="1" spans="1:35" s="50" customFormat="1" ht="20.399999999999999" thickBot="1">
       <c r="A1" s="88" t="s">
-        <v>2581</v>
+        <v>2580</v>
       </c>
       <c r="B1" s="88"/>
       <c r="C1" s="88" t="s">
-        <v>2580</v>
+        <v>2579</v>
       </c>
       <c r="D1" s="88"/>
       <c r="E1" s="88"/>
@@ -10348,7 +10363,7 @@
     </row>
     <row r="2" spans="1:35" ht="15.6" customHeight="1" thickTop="1">
       <c r="A2" s="89" t="s">
-        <v>2511</v>
+        <v>2510</v>
       </c>
       <c r="B2" s="89" t="s">
         <v>1822</v>
@@ -10357,7 +10372,7 @@
         <v>1831</v>
       </c>
       <c r="D2" s="89" t="s">
-        <v>2588</v>
+        <v>2587</v>
       </c>
       <c r="E2" s="89" t="s">
         <v>1820</v>
@@ -11810,11 +11825,11 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:CB52"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane xSplit="3" ySplit="6" topLeftCell="D7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="L6" sqref="L6"/>
+      <selection pane="bottomRight" activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15" defaultRowHeight="15.6"/>
@@ -11836,24 +11851,24 @@
   <sheetData>
     <row r="1" spans="1:80" s="74" customFormat="1" ht="20.399999999999999" customHeight="1" thickBot="1">
       <c r="A1" s="94" t="s">
-        <v>2590</v>
+        <v>2589</v>
       </c>
       <c r="B1" s="95"/>
       <c r="C1" s="96"/>
       <c r="D1" s="94" t="s">
-        <v>2580</v>
+        <v>2579</v>
       </c>
       <c r="E1" s="95"/>
       <c r="F1" s="95"/>
       <c r="G1" s="96"/>
       <c r="H1" s="97" t="s">
-        <v>2582</v>
+        <v>2581</v>
       </c>
       <c r="I1" s="98"/>
       <c r="J1" s="98"/>
       <c r="K1" s="99"/>
       <c r="L1" s="74" t="s">
-        <v>2847</v>
+        <v>2472</v>
       </c>
       <c r="M1" s="74" t="s">
         <v>1837</v>
@@ -11862,15 +11877,15 @@
         <v>1838</v>
       </c>
       <c r="O1" s="74" t="s">
-        <v>2792</v>
+        <v>2791</v>
       </c>
       <c r="P1" s="74" t="s">
-        <v>2847</v>
+        <v>2846</v>
       </c>
     </row>
     <row r="2" spans="1:80" s="76" customFormat="1">
       <c r="A2" s="100" t="s">
-        <v>2511</v>
+        <v>2510</v>
       </c>
       <c r="B2" s="103" t="s">
         <v>1822</v>
@@ -11882,7 +11897,7 @@
         <v>1831</v>
       </c>
       <c r="E2" s="104" t="s">
-        <v>2588</v>
+        <v>2587</v>
       </c>
       <c r="F2" s="104" t="s">
         <v>1820</v>
@@ -11903,7 +11918,7 @@
         <v>1835</v>
       </c>
       <c r="L2" s="75" t="s">
-        <v>1752</v>
+        <v>2473</v>
       </c>
       <c r="M2" s="75" t="s">
         <v>2177</v>
@@ -11912,10 +11927,10 @@
         <v>1840</v>
       </c>
       <c r="O2" s="75" t="s">
-        <v>2794</v>
+        <v>2793</v>
       </c>
       <c r="P2" s="75" t="s">
-        <v>2709</v>
+        <v>2708</v>
       </c>
       <c r="Q2" s="75"/>
       <c r="R2" s="75"/>
@@ -11995,7 +12010,7 @@
       <c r="J3" s="104"/>
       <c r="K3" s="110"/>
       <c r="L3" s="75" t="s">
-        <v>2870</v>
+        <v>5</v>
       </c>
       <c r="M3" s="75"/>
       <c r="N3" s="75"/>
@@ -14543,10 +14558,10 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr codeName="Sheet6"/>
-  <dimension ref="A1:GR277"/>
+  <dimension ref="A1:GX277"/>
   <sheetViews>
-    <sheetView topLeftCell="BP1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="BQ19" sqref="BQ19"/>
+    <sheetView topLeftCell="GE1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="GM18" sqref="GM18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -14601,7 +14616,7 @@
     <col min="187" max="188" width="21.3984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:200" s="1" customFormat="1">
+    <row r="1" spans="1:206" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -14771,7 +14786,7 @@
         <v>1143</v>
       </c>
       <c r="BE1" s="1" t="s">
-        <v>2813</v>
+        <v>2812</v>
       </c>
       <c r="BF1" s="15" t="s">
         <v>1848</v>
@@ -14788,7 +14803,7 @@
         <v>core_radionuclide_data_description</v>
       </c>
       <c r="BJ1" s="24" t="s">
-        <v>2732</v>
+        <v>2731</v>
       </c>
       <c r="BK1" s="9" t="str">
         <f>_xlfn.CONCAT(BJ1,"_units")</f>
@@ -14844,7 +14859,7 @@
         <v>sample_composition_description</v>
       </c>
       <c r="BZ1" s="9" t="s">
-        <v>2713</v>
+        <v>2712</v>
       </c>
       <c r="CA1" s="9" t="str">
         <f>_xlfn.CONCAT(BZ1,"_units")</f>
@@ -14954,7 +14969,7 @@
         <v>sample_fatty_acids_description</v>
       </c>
       <c r="DD1" s="9" t="s">
-        <v>2476</v>
+        <v>2475</v>
       </c>
       <c r="DE1" s="9" t="str">
         <f>_xlfn.CONCAT(DD1,"_units")</f>
@@ -14965,7 +14980,7 @@
         <v>sample_amino_acids_description</v>
       </c>
       <c r="DG1" s="9" t="s">
-        <v>2473</v>
+        <v>2472</v>
       </c>
       <c r="DH1" s="9" t="str">
         <f>_xlfn.CONCAT(DG1,"_units")</f>
@@ -14987,7 +15002,7 @@
         <v>sample_pore_water_description</v>
       </c>
       <c r="DM1" s="9" t="s">
-        <v>2591</v>
+        <v>2590</v>
       </c>
       <c r="DN1" s="9" t="str">
         <f>_xlfn.CONCAT(DM1,"_units")</f>
@@ -14998,7 +15013,7 @@
         <v>sample_black_carbon_description</v>
       </c>
       <c r="DP1" s="9" t="s">
-        <v>2776</v>
+        <v>2775</v>
       </c>
       <c r="DQ1" s="9" t="str">
         <f>_xlfn.CONCAT(DP1,"_units")</f>
@@ -15009,7 +15024,7 @@
         <v>sample_mineralogy_description</v>
       </c>
       <c r="DS1" s="9" t="s">
-        <v>2779</v>
+        <v>2778</v>
       </c>
       <c r="DT1" s="9" t="str">
         <f>_xlfn.CONCAT(DS1,"_units")</f>
@@ -15020,7 +15035,7 @@
         <v>sample_dating_description</v>
       </c>
       <c r="DV1" s="9" t="s">
-        <v>2792</v>
+        <v>2791</v>
       </c>
       <c r="DW1" s="9" t="str">
         <f>_xlfn.CONCAT(DV1,"_units")</f>
@@ -15031,7 +15046,7 @@
         <v>sample_neodynium_description</v>
       </c>
       <c r="DY1" s="9" t="s">
-        <v>2797</v>
+        <v>2796</v>
       </c>
       <c r="DZ1" s="9" t="str">
         <f>_xlfn.CONCAT(DY1,"_units")</f>
@@ -15042,7 +15057,7 @@
         <v>sample_strontium_description</v>
       </c>
       <c r="EB1" s="1" t="s">
-        <v>2847</v>
+        <v>2846</v>
       </c>
       <c r="EC1" s="9" t="str">
         <f>_xlfn.CONCAT(EB1,"_units")</f>
@@ -15062,7 +15077,7 @@
         <v>1754</v>
       </c>
       <c r="EH1" s="1" t="s">
-        <v>2848</v>
+        <v>2847</v>
       </c>
       <c r="EI1" s="9" t="str">
         <f>_xlfn.CONCAT(EH1,"_units")</f>
@@ -15076,7 +15091,7 @@
         <v>1753</v>
       </c>
       <c r="EL1" s="80" t="s">
-        <v>2851</v>
+        <v>2850</v>
       </c>
       <c r="EM1" s="1" t="s">
         <v>2048</v>
@@ -15100,10 +15115,10 @@
         <v>1844</v>
       </c>
       <c r="ET1" s="1" t="s">
+        <v>2807</v>
+      </c>
+      <c r="EU1" s="1" t="s">
         <v>2808</v>
-      </c>
-      <c r="EU1" s="1" t="s">
-        <v>2809</v>
       </c>
       <c r="EV1" s="1" t="s">
         <v>1845</v>
@@ -15112,10 +15127,10 @@
         <v>1846</v>
       </c>
       <c r="EX1" s="1" t="s">
-        <v>2748</v>
+        <v>2747</v>
       </c>
       <c r="EY1" s="1" t="s">
-        <v>2811</v>
+        <v>2810</v>
       </c>
       <c r="EZ1" s="1" t="s">
         <v>2058</v>
@@ -15154,16 +15169,16 @@
         <v>2369</v>
       </c>
       <c r="FL1" s="1" t="s">
-        <v>2574</v>
+        <v>2573</v>
       </c>
       <c r="FM1" s="1" t="s">
-        <v>2576</v>
+        <v>2575</v>
       </c>
       <c r="FN1" s="1" t="s">
         <v>1765</v>
       </c>
       <c r="FO1" s="1" t="s">
-        <v>2733</v>
+        <v>2732</v>
       </c>
       <c r="FP1" s="1" t="s">
         <v>1768</v>
@@ -15184,7 +15199,7 @@
         <v>1776</v>
       </c>
       <c r="FV1" s="1" t="s">
-        <v>2735</v>
+        <v>2734</v>
       </c>
       <c r="FW1" s="1" t="s">
         <v>1778</v>
@@ -15208,10 +15223,10 @@
         <v>1790</v>
       </c>
       <c r="GD1" s="1" t="s">
-        <v>2845</v>
+        <v>2844</v>
       </c>
       <c r="GE1" s="1" t="s">
-        <v>2709</v>
+        <v>2708</v>
       </c>
       <c r="GF1" s="1" t="s">
         <v>1752</v>
@@ -15220,7 +15235,7 @@
         <v>1751</v>
       </c>
       <c r="GH1" s="1" t="s">
-        <v>2711</v>
+        <v>2710</v>
       </c>
       <c r="GI1" s="22" t="s">
         <v>2086</v>
@@ -15252,8 +15267,26 @@
       <c r="GR1" s="22" t="s">
         <v>2094</v>
       </c>
-    </row>
-    <row r="2" spans="1:200">
+      <c r="GS1" s="22" t="s">
+        <v>2462</v>
+      </c>
+      <c r="GT1" s="22" t="s">
+        <v>2473</v>
+      </c>
+      <c r="GU1" s="22" t="s">
+        <v>2910</v>
+      </c>
+      <c r="GV1" s="22" t="s">
+        <v>2463</v>
+      </c>
+      <c r="GW1" s="22" t="s">
+        <v>2464</v>
+      </c>
+      <c r="GX1" s="22" t="s">
+        <v>2467</v>
+      </c>
+    </row>
+    <row r="2" spans="1:206">
       <c r="A2" t="b">
         <v>1</v>
       </c>
@@ -15423,7 +15456,7 @@
         <v>5</v>
       </c>
       <c r="BE2" s="72" t="s">
-        <v>2814</v>
+        <v>2813</v>
       </c>
       <c r="BF2" s="16" t="s">
         <v>2182</v>
@@ -15432,28 +15465,28 @@
         <v>1756</v>
       </c>
       <c r="BH2" s="20" t="s">
-        <v>2539</v>
+        <v>2538</v>
       </c>
       <c r="BI2" s="20" t="s">
-        <v>2543</v>
+        <v>2542</v>
       </c>
       <c r="BJ2" s="20" t="s">
         <v>2193</v>
       </c>
       <c r="BK2" s="20" t="s">
-        <v>2563</v>
+        <v>2562</v>
       </c>
       <c r="BL2" s="20" t="s">
-        <v>2567</v>
+        <v>2566</v>
       </c>
       <c r="BM2" s="20" t="s">
         <v>2180</v>
       </c>
       <c r="BN2" s="20" t="s">
-        <v>2518</v>
+        <v>2517</v>
       </c>
       <c r="BO2" s="20" t="s">
-        <v>2520</v>
+        <v>2519</v>
       </c>
       <c r="BP2" s="14" t="s">
         <v>1838</v>
@@ -15465,7 +15498,7 @@
         <v>1</v>
       </c>
       <c r="BS2" s="14" t="s">
-        <v>2741</v>
+        <v>2740</v>
       </c>
       <c r="BT2" s="10" t="s">
         <v>1839</v>
@@ -15492,7 +15525,7 @@
         <v>2264</v>
       </c>
       <c r="CB2" s="25" t="s">
-        <v>2494</v>
+        <v>2493</v>
       </c>
       <c r="CC2" s="25" t="s">
         <v>1766</v>
@@ -15501,10 +15534,10 @@
         <v>2264</v>
       </c>
       <c r="CE2" s="25" t="s">
-        <v>2491</v>
+        <v>2490</v>
       </c>
       <c r="CF2" s="23" t="s">
-        <v>2752</v>
+        <v>2751</v>
       </c>
       <c r="CG2" s="68" t="s">
         <v>2444</v>
@@ -15513,13 +15546,13 @@
         <v>2282</v>
       </c>
       <c r="CI2" s="12" t="s">
-        <v>2735</v>
+        <v>2734</v>
       </c>
       <c r="CJ2" s="66" t="s">
         <v>2266</v>
       </c>
       <c r="CK2" s="66" t="s">
-        <v>2737</v>
+        <v>2736</v>
       </c>
       <c r="CL2" s="12" t="s">
         <v>1792</v>
@@ -15578,58 +15611,60 @@
       <c r="DG2" s="12" t="s">
         <v>2462</v>
       </c>
-      <c r="DH2" s="12"/>
+      <c r="DH2" s="12" t="s">
+        <v>2909</v>
+      </c>
       <c r="DI2" s="12"/>
       <c r="DJ2" s="12" t="s">
+        <v>2498</v>
+      </c>
+      <c r="DK2" s="12" t="s">
         <v>2499</v>
       </c>
-      <c r="DK2" s="12" t="s">
+      <c r="DL2" s="12" t="s">
         <v>2500</v>
       </c>
-      <c r="DL2" s="12" t="s">
-        <v>2501</v>
-      </c>
       <c r="DM2" s="12" t="s">
-        <v>2592</v>
+        <v>2591</v>
       </c>
       <c r="DN2" s="12" t="s">
         <v>2226</v>
       </c>
       <c r="DO2" s="12" t="s">
-        <v>2593</v>
+        <v>2592</v>
       </c>
       <c r="DP2" s="12" t="s">
-        <v>2781</v>
+        <v>2780</v>
       </c>
       <c r="DQ2" s="12" t="s">
         <v>2226</v>
       </c>
       <c r="DR2" s="12" t="s">
-        <v>2785</v>
+        <v>2784</v>
       </c>
       <c r="DS2" s="12" t="s">
         <v>2123</v>
       </c>
       <c r="DT2" s="12" t="s">
-        <v>2790</v>
+        <v>2789</v>
       </c>
       <c r="DU2" s="12" t="s">
         <v>2242</v>
       </c>
       <c r="DV2" s="12" t="s">
-        <v>2793</v>
+        <v>2792</v>
       </c>
       <c r="DW2" s="12" t="s">
-        <v>2795</v>
+        <v>2794</v>
       </c>
       <c r="EB2" s="10" t="s">
-        <v>2709</v>
+        <v>2708</v>
       </c>
       <c r="EC2" s="10" t="s">
-        <v>2529</v>
+        <v>2528</v>
       </c>
       <c r="ED2" s="10" t="s">
-        <v>2533</v>
+        <v>2532</v>
       </c>
       <c r="EE2" s="10" t="s">
         <v>5</v>
@@ -15644,10 +15679,10 @@
         <v>1751</v>
       </c>
       <c r="EI2" s="10" t="s">
-        <v>2518</v>
+        <v>2517</v>
       </c>
       <c r="EJ2" s="10" t="s">
-        <v>2536</v>
+        <v>2535</v>
       </c>
       <c r="EK2" s="10" t="s">
         <v>5</v>
@@ -15826,8 +15861,26 @@
       <c r="GR2" s="10" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:200">
+      <c r="GS2" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="GT2" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="GU2" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="GV2" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="GW2" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="GX2" s="10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:206">
       <c r="A3" t="b">
         <v>0</v>
       </c>
@@ -15856,7 +15909,7 @@
         <v>19</v>
       </c>
       <c r="J3" t="s">
-        <v>2807</v>
+        <v>2806</v>
       </c>
       <c r="K3" s="34" t="s">
         <v>2064</v>
@@ -15997,37 +16050,37 @@
         <v>20</v>
       </c>
       <c r="BE3" s="72" t="s">
-        <v>2815</v>
+        <v>2814</v>
       </c>
       <c r="BF3" s="16" t="s">
-        <v>2732</v>
+        <v>2731</v>
       </c>
       <c r="BG3" s="20" t="s">
         <v>1773</v>
       </c>
       <c r="BH3" s="20" t="s">
-        <v>2539</v>
+        <v>2538</v>
       </c>
       <c r="BI3" s="20" t="s">
-        <v>2544</v>
+        <v>2543</v>
       </c>
       <c r="BJ3" s="20" t="s">
         <v>2176</v>
       </c>
       <c r="BK3" s="20" t="s">
-        <v>2564</v>
+        <v>2563</v>
       </c>
       <c r="BL3" s="20" t="s">
-        <v>2568</v>
+        <v>2567</v>
       </c>
       <c r="BM3" s="20" t="s">
-        <v>2742</v>
+        <v>2741</v>
       </c>
       <c r="BN3" s="20" t="s">
-        <v>2519</v>
+        <v>2518</v>
       </c>
       <c r="BO3" s="20" t="s">
-        <v>2744</v>
+        <v>2743</v>
       </c>
       <c r="BP3" s="14" t="s">
         <v>1837</v>
@@ -16039,7 +16092,7 @@
         <v>2</v>
       </c>
       <c r="BS3" s="14" t="s">
-        <v>2479</v>
+        <v>2478</v>
       </c>
       <c r="BT3" s="10" t="s">
         <v>1840</v>
@@ -16066,7 +16119,7 @@
         <v>2264</v>
       </c>
       <c r="CB3" s="25" t="s">
-        <v>2493</v>
+        <v>2492</v>
       </c>
       <c r="CC3" s="25" t="s">
         <v>1767</v>
@@ -16075,10 +16128,10 @@
         <v>2264</v>
       </c>
       <c r="CE3" s="25" t="s">
-        <v>2492</v>
+        <v>2491</v>
       </c>
       <c r="CF3" s="23" t="s">
-        <v>2753</v>
+        <v>2752</v>
       </c>
       <c r="CG3" s="68" t="s">
         <v>2444</v>
@@ -16087,13 +16140,13 @@
         <v>2283</v>
       </c>
       <c r="CI3" s="12" t="s">
-        <v>2736</v>
+        <v>2735</v>
       </c>
       <c r="CJ3" s="66" t="s">
         <v>2266</v>
       </c>
       <c r="CK3" s="66" t="s">
-        <v>2738</v>
+        <v>2737</v>
       </c>
       <c r="CL3" s="12" t="s">
         <v>1793</v>
@@ -16105,13 +16158,13 @@
         <v>2297</v>
       </c>
       <c r="CO3" s="12" t="s">
-        <v>2596</v>
+        <v>2595</v>
       </c>
       <c r="CP3" s="56" t="s">
         <v>2280</v>
       </c>
       <c r="CQ3" s="12" t="s">
-        <v>2597</v>
+        <v>2596</v>
       </c>
       <c r="CR3" s="12" t="s">
         <v>2087</v>
@@ -16152,57 +16205,57 @@
         <v>2405</v>
       </c>
       <c r="DG3" s="12" t="s">
-        <v>2474</v>
+        <v>2473</v>
       </c>
       <c r="DH3" s="12" t="s">
-        <v>2472</v>
+        <v>2471</v>
       </c>
       <c r="DI3" s="12" t="s">
-        <v>2471</v>
+        <v>2470</v>
       </c>
       <c r="DJ3" s="12" t="s">
+        <v>2505</v>
+      </c>
+      <c r="DK3" s="12" t="s">
         <v>2506</v>
-      </c>
-      <c r="DK3" s="12" t="s">
-        <v>2507</v>
       </c>
       <c r="DL3" s="48"/>
       <c r="DM3" s="12" t="s">
-        <v>2594</v>
+        <v>2593</v>
       </c>
       <c r="DN3" s="12"/>
       <c r="DO3" s="12" t="s">
-        <v>2595</v>
+        <v>2594</v>
       </c>
       <c r="DP3" s="12" t="s">
-        <v>2782</v>
+        <v>2781</v>
       </c>
       <c r="DQ3" t="s">
         <v>2226</v>
       </c>
       <c r="DR3" s="12" t="s">
-        <v>2786</v>
+        <v>2785</v>
       </c>
       <c r="DS3" s="12" t="s">
         <v>2206</v>
       </c>
       <c r="DT3" s="12" t="s">
-        <v>2790</v>
+        <v>2789</v>
       </c>
       <c r="DU3" s="12" t="s">
         <v>2243</v>
       </c>
       <c r="DV3" s="12" t="s">
-        <v>2794</v>
+        <v>2793</v>
       </c>
       <c r="EB3" s="10" t="s">
-        <v>2710</v>
+        <v>2709</v>
       </c>
       <c r="EC3" s="10" t="s">
-        <v>2529</v>
+        <v>2528</v>
       </c>
       <c r="ED3" s="10" t="s">
-        <v>2531</v>
+        <v>2530</v>
       </c>
       <c r="EE3" s="10" t="s">
         <v>2025</v>
@@ -16214,112 +16267,112 @@
         <v>2029</v>
       </c>
       <c r="EH3" s="10" t="s">
-        <v>2711</v>
+        <v>2710</v>
       </c>
       <c r="EI3" s="10" t="s">
-        <v>2535</v>
+        <v>2534</v>
       </c>
       <c r="EJ3" s="10" t="s">
-        <v>2538</v>
+        <v>2537</v>
       </c>
       <c r="EK3" s="10" t="s">
         <v>2025</v>
       </c>
       <c r="EM3" t="s">
-        <v>2830</v>
+        <v>2829</v>
       </c>
       <c r="EN3" t="s">
+        <v>2860</v>
+      </c>
+      <c r="EO3" t="s">
+        <v>2860</v>
+      </c>
+      <c r="EP3" s="79" t="s">
+        <v>2860</v>
+      </c>
+      <c r="EQ3" t="s">
         <v>2861</v>
       </c>
-      <c r="EO3" t="s">
+      <c r="ER3" s="79" t="s">
         <v>2861</v>
       </c>
-      <c r="EP3" s="79" t="s">
+      <c r="ES3" s="79" t="s">
         <v>2861</v>
       </c>
-      <c r="EQ3" t="s">
-        <v>2862</v>
-      </c>
-      <c r="ER3" s="79" t="s">
-        <v>2862</v>
-      </c>
-      <c r="ES3" s="79" t="s">
-        <v>2862</v>
-      </c>
       <c r="ET3" s="79" t="s">
-        <v>2862</v>
+        <v>2861</v>
       </c>
       <c r="EU3" s="79" t="s">
-        <v>2862</v>
+        <v>2861</v>
       </c>
       <c r="EV3" s="79" t="s">
-        <v>2862</v>
+        <v>2861</v>
       </c>
       <c r="EW3" s="79" t="s">
-        <v>2862</v>
+        <v>2861</v>
       </c>
       <c r="EX3" s="79" t="s">
-        <v>2862</v>
+        <v>2861</v>
       </c>
       <c r="EY3" s="79" t="s">
-        <v>2862</v>
+        <v>2861</v>
       </c>
       <c r="EZ3" s="79" t="s">
-        <v>2897</v>
+        <v>2896</v>
       </c>
       <c r="FB3" t="s">
-        <v>2870</v>
+        <v>2869</v>
       </c>
       <c r="FD3" t="s">
-        <v>2864</v>
+        <v>2863</v>
       </c>
       <c r="FE3" t="s">
-        <v>2892</v>
+        <v>2891</v>
       </c>
       <c r="FF3" t="s">
+        <v>2873</v>
+      </c>
+      <c r="FJ3" t="s">
         <v>2874</v>
       </c>
-      <c r="FJ3" t="s">
+      <c r="FK3" s="79" t="s">
+        <v>2874</v>
+      </c>
+      <c r="FO3" t="s">
+        <v>2888</v>
+      </c>
+      <c r="FV3" t="s">
+        <v>2876</v>
+      </c>
+      <c r="FW3" s="79" t="s">
+        <v>2876</v>
+      </c>
+      <c r="FX3" s="79" t="s">
+        <v>2853</v>
+      </c>
+      <c r="FY3" s="79" t="s">
+        <v>2854</v>
+      </c>
+      <c r="FZ3" s="79" t="s">
+        <v>2854</v>
+      </c>
+      <c r="GA3" t="s">
         <v>2875</v>
       </c>
-      <c r="FK3" s="79" t="s">
-        <v>2875</v>
-      </c>
-      <c r="FO3" t="s">
-        <v>2889</v>
-      </c>
-      <c r="FV3" t="s">
-        <v>2877</v>
-      </c>
-      <c r="FW3" s="79" t="s">
-        <v>2877</v>
-      </c>
-      <c r="FX3" s="79" t="s">
-        <v>2854</v>
-      </c>
-      <c r="FY3" s="79" t="s">
-        <v>2855</v>
-      </c>
-      <c r="FZ3" s="79" t="s">
-        <v>2855</v>
-      </c>
-      <c r="GA3" t="s">
-        <v>2876</v>
-      </c>
       <c r="GB3" t="s">
-        <v>2852</v>
+        <v>2851</v>
       </c>
       <c r="GC3" s="79" t="s">
-        <v>2852</v>
+        <v>2851</v>
       </c>
       <c r="GD3" s="79" t="s">
-        <v>2852</v>
+        <v>2851</v>
       </c>
       <c r="GE3" t="s">
-        <v>2870</v>
+        <v>2869</v>
       </c>
       <c r="GF3" s="79" t="s">
-        <v>2870</v>
+        <v>2869</v>
       </c>
       <c r="GG3" s="10" t="s">
         <v>2025</v>
@@ -16328,7 +16381,7 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="4" spans="1:200">
+    <row r="4" spans="1:206">
       <c r="B4" t="s">
         <v>29</v>
       </c>
@@ -16501,34 +16554,34 @@
         <v>2040</v>
       </c>
       <c r="BH4" s="20" t="s">
+        <v>2517</v>
+      </c>
+      <c r="BI4" s="20" t="s">
+        <v>2544</v>
+      </c>
+      <c r="BJ4" s="20" t="s">
+        <v>2746</v>
+      </c>
+      <c r="BK4" s="20" t="s">
+        <v>2564</v>
+      </c>
+      <c r="BL4" s="20" t="s">
+        <v>2568</v>
+      </c>
+      <c r="BM4" s="20" t="s">
+        <v>2742</v>
+      </c>
+      <c r="BN4" s="20" t="s">
         <v>2518</v>
       </c>
-      <c r="BI4" s="20" t="s">
-        <v>2545</v>
-      </c>
-      <c r="BJ4" s="20" t="s">
-        <v>2747</v>
-      </c>
-      <c r="BK4" s="20" t="s">
-        <v>2565</v>
-      </c>
-      <c r="BL4" s="20" t="s">
-        <v>2569</v>
-      </c>
-      <c r="BM4" s="20" t="s">
-        <v>2743</v>
-      </c>
-      <c r="BN4" s="20" t="s">
-        <v>2519</v>
-      </c>
       <c r="BO4" s="20" t="s">
-        <v>2745</v>
+        <v>2744</v>
       </c>
       <c r="BP4" s="14" t="s">
         <v>1836</v>
       </c>
       <c r="BQ4" s="20" t="s">
-        <v>2714</v>
+        <v>2713</v>
       </c>
       <c r="BR4" s="20">
         <v>3</v>
@@ -16559,17 +16612,17 @@
       </c>
       <c r="CA4" s="25"/>
       <c r="CB4" s="25" t="s">
-        <v>2495</v>
+        <v>2494</v>
       </c>
       <c r="CC4" s="25" t="s">
-        <v>2488</v>
+        <v>2487</v>
       </c>
       <c r="CD4" s="25"/>
       <c r="CE4" s="25" t="s">
-        <v>2489</v>
+        <v>2488</v>
       </c>
       <c r="CF4" s="23" t="s">
-        <v>2754</v>
+        <v>2753</v>
       </c>
       <c r="CG4" s="68" t="s">
         <v>2444</v>
@@ -16643,49 +16696,55 @@
         <v>2406</v>
       </c>
       <c r="DG4" s="12" t="s">
-        <v>2463</v>
+        <v>2910</v>
+      </c>
+      <c r="DH4" s="46" t="s">
+        <v>2911</v>
+      </c>
+      <c r="DI4" s="12" t="s">
+        <v>2912</v>
       </c>
       <c r="DJ4" s="12" t="s">
-        <v>2513</v>
+        <v>2512</v>
       </c>
       <c r="DK4" s="48" t="s">
         <v>2264</v>
       </c>
       <c r="DL4" s="48" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="DP4" t="s">
-        <v>2783</v>
+        <v>2782</v>
       </c>
       <c r="DQ4" t="s">
         <v>2226</v>
       </c>
       <c r="DR4" t="s">
-        <v>2787</v>
+        <v>2786</v>
       </c>
       <c r="DS4" t="s">
-        <v>2789</v>
+        <v>2788</v>
       </c>
       <c r="DT4" t="s">
         <v>2228</v>
       </c>
       <c r="DU4" t="s">
-        <v>2791</v>
+        <v>2790</v>
       </c>
       <c r="DV4" t="s">
-        <v>2796</v>
+        <v>2795</v>
       </c>
       <c r="DW4" t="s">
-        <v>2798</v>
+        <v>2797</v>
       </c>
       <c r="EB4" s="10" t="s">
         <v>1752</v>
       </c>
       <c r="EC4" s="10" t="s">
-        <v>2530</v>
+        <v>2529</v>
       </c>
       <c r="ED4" s="10" t="s">
-        <v>2532</v>
+        <v>2531</v>
       </c>
       <c r="EE4" s="10" t="s">
         <v>2026</v>
@@ -16697,100 +16756,100 @@
         <v>2030</v>
       </c>
       <c r="EH4" s="10" t="s">
-        <v>2712</v>
+        <v>2711</v>
       </c>
       <c r="EI4" s="10" t="s">
-        <v>2535</v>
+        <v>2534</v>
       </c>
       <c r="EJ4" s="10" t="s">
-        <v>2537</v>
+        <v>2536</v>
       </c>
       <c r="EK4" s="79" t="s">
         <v>2033</v>
       </c>
       <c r="EM4" t="s">
-        <v>2894</v>
+        <v>2893</v>
       </c>
       <c r="EN4" t="s">
+        <v>2889</v>
+      </c>
+      <c r="EO4" s="79" t="s">
+        <v>2889</v>
+      </c>
+      <c r="EQ4" t="s">
+        <v>2862</v>
+      </c>
+      <c r="ER4" s="79" t="s">
+        <v>2862</v>
+      </c>
+      <c r="ES4" s="79" t="s">
+        <v>2862</v>
+      </c>
+      <c r="ET4" s="79" t="s">
+        <v>2862</v>
+      </c>
+      <c r="EU4" s="79" t="s">
+        <v>2862</v>
+      </c>
+      <c r="EV4" s="79" t="s">
+        <v>2862</v>
+      </c>
+      <c r="EW4" s="79" t="s">
+        <v>2862</v>
+      </c>
+      <c r="EX4" s="79" t="s">
+        <v>2862</v>
+      </c>
+      <c r="EY4" s="79" t="s">
+        <v>2862</v>
+      </c>
+      <c r="EZ4" t="s">
+        <v>2895</v>
+      </c>
+      <c r="FB4" s="79" t="s">
+        <v>2870</v>
+      </c>
+      <c r="FD4" s="79" t="s">
+        <v>2866</v>
+      </c>
+      <c r="FF4" t="s">
         <v>2890</v>
       </c>
-      <c r="EO4" s="79" t="s">
-        <v>2890</v>
-      </c>
-      <c r="EQ4" t="s">
-        <v>2863</v>
-      </c>
-      <c r="ER4" s="79" t="s">
-        <v>2863</v>
-      </c>
-      <c r="ES4" s="79" t="s">
-        <v>2863</v>
-      </c>
-      <c r="ET4" s="79" t="s">
-        <v>2863</v>
-      </c>
-      <c r="EU4" s="79" t="s">
-        <v>2863</v>
-      </c>
-      <c r="EV4" s="79" t="s">
-        <v>2863</v>
-      </c>
-      <c r="EW4" s="79" t="s">
-        <v>2863</v>
-      </c>
-      <c r="EX4" s="79" t="s">
-        <v>2863</v>
-      </c>
-      <c r="EY4" s="79" t="s">
-        <v>2863</v>
-      </c>
-      <c r="EZ4" t="s">
-        <v>2896</v>
-      </c>
-      <c r="FB4" s="79" t="s">
+      <c r="FJ4" t="s">
+        <v>2887</v>
+      </c>
+      <c r="FK4" s="79" t="s">
+        <v>2887</v>
+      </c>
+      <c r="FO4" t="s">
+        <v>2829</v>
+      </c>
+      <c r="FV4" t="s">
+        <v>2852</v>
+      </c>
+      <c r="FW4" s="79" t="s">
+        <v>2852</v>
+      </c>
+      <c r="FY4" s="79" t="s">
+        <v>2855</v>
+      </c>
+      <c r="FZ4" s="79" t="s">
+        <v>2858</v>
+      </c>
+      <c r="GB4" s="79" t="s">
+        <v>2877</v>
+      </c>
+      <c r="GC4" s="79" t="s">
+        <v>2878</v>
+      </c>
+      <c r="GD4" s="79" t="s">
+        <v>2877</v>
+      </c>
+      <c r="GE4" t="s">
         <v>2871</v>
       </c>
-      <c r="FD4" s="79" t="s">
-        <v>2867</v>
-      </c>
-      <c r="FF4" t="s">
-        <v>2891</v>
-      </c>
-      <c r="FJ4" t="s">
-        <v>2888</v>
-      </c>
-      <c r="FK4" s="79" t="s">
-        <v>2888</v>
-      </c>
-      <c r="FO4" t="s">
-        <v>2830</v>
-      </c>
-      <c r="FV4" t="s">
-        <v>2853</v>
-      </c>
-      <c r="FW4" s="79" t="s">
-        <v>2853</v>
-      </c>
-      <c r="FY4" s="79" t="s">
-        <v>2856</v>
-      </c>
-      <c r="FZ4" s="79" t="s">
-        <v>2859</v>
-      </c>
-      <c r="GB4" s="79" t="s">
-        <v>2878</v>
-      </c>
-      <c r="GC4" s="79" t="s">
-        <v>2879</v>
-      </c>
-      <c r="GD4" s="79" t="s">
-        <v>2878</v>
-      </c>
-      <c r="GE4" t="s">
-        <v>2872</v>
-      </c>
       <c r="GF4" s="79" t="s">
-        <v>2872</v>
+        <v>2871</v>
       </c>
       <c r="GG4" s="79" t="s">
         <v>2033</v>
@@ -16799,7 +16858,7 @@
         <v>2033</v>
       </c>
     </row>
-    <row r="5" spans="1:200">
+    <row r="5" spans="1:206">
       <c r="B5" t="s">
         <v>40</v>
       </c>
@@ -16861,7 +16920,7 @@
         <v>1348</v>
       </c>
       <c r="W5" t="s">
-        <v>2584</v>
+        <v>2583</v>
       </c>
       <c r="X5" s="6" t="s">
         <v>1361</v>
@@ -16951,34 +17010,34 @@
         <v>2041</v>
       </c>
       <c r="BH5" s="20" t="s">
-        <v>2541</v>
+        <v>2540</v>
       </c>
       <c r="BI5" s="20" t="s">
-        <v>2546</v>
+        <v>2545</v>
       </c>
       <c r="BJ5" s="20" t="s">
         <v>2125</v>
       </c>
       <c r="BK5" s="20" t="s">
-        <v>2566</v>
+        <v>2565</v>
       </c>
       <c r="BL5" s="20" t="s">
-        <v>2570</v>
+        <v>2569</v>
       </c>
       <c r="BM5" s="20" t="s">
+        <v>2718</v>
+      </c>
+      <c r="BN5" s="20" t="s">
+        <v>2518</v>
+      </c>
+      <c r="BO5" s="20" t="s">
         <v>2719</v>
       </c>
-      <c r="BN5" s="20" t="s">
-        <v>2519</v>
-      </c>
-      <c r="BO5" s="20" t="s">
-        <v>2720</v>
-      </c>
       <c r="BP5" s="14" t="s">
-        <v>2713</v>
+        <v>2712</v>
       </c>
       <c r="BQ5" s="20" t="s">
-        <v>2715</v>
+        <v>2714</v>
       </c>
       <c r="BR5" s="20">
         <v>4</v>
@@ -17009,7 +17068,7 @@
       </c>
       <c r="CA5" s="25"/>
       <c r="CB5" s="25" t="s">
-        <v>2496</v>
+        <v>2495</v>
       </c>
       <c r="CC5" s="25" t="s">
         <v>1770</v>
@@ -17018,10 +17077,10 @@
         <v>2264</v>
       </c>
       <c r="CE5" s="25" t="s">
-        <v>2485</v>
+        <v>2484</v>
       </c>
       <c r="CF5" s="23" t="s">
-        <v>2755</v>
+        <v>2754</v>
       </c>
       <c r="CG5" s="68" t="s">
         <v>2444</v>
@@ -17045,13 +17104,13 @@
         <v>2280</v>
       </c>
       <c r="CO5" s="12" t="s">
-        <v>2598</v>
+        <v>2597</v>
       </c>
       <c r="CP5" s="56" t="s">
         <v>2280</v>
       </c>
       <c r="CQ5" s="12" t="s">
-        <v>2599</v>
+        <v>2598</v>
       </c>
       <c r="CR5" s="35" t="s">
         <v>2089</v>
@@ -17091,40 +17150,40 @@
         <v>2407</v>
       </c>
       <c r="DG5" s="12" t="s">
-        <v>2464</v>
+        <v>2463</v>
       </c>
       <c r="DH5" s="12" t="s">
+        <v>2465</v>
+      </c>
+      <c r="DI5" s="12" t="s">
         <v>2466</v>
       </c>
-      <c r="DI5" s="12" t="s">
-        <v>2467</v>
-      </c>
       <c r="DJ5" s="12" t="s">
-        <v>2514</v>
+        <v>2513</v>
       </c>
       <c r="DK5" s="48" t="s">
         <v>2264</v>
       </c>
       <c r="DL5" s="12" t="s">
-        <v>2509</v>
+        <v>2508</v>
       </c>
       <c r="DP5" t="s">
-        <v>2784</v>
+        <v>2783</v>
       </c>
       <c r="DQ5" t="s">
         <v>2226</v>
       </c>
       <c r="DR5" t="s">
-        <v>2788</v>
+        <v>2787</v>
       </c>
       <c r="EB5" s="10" t="s">
         <v>1774</v>
       </c>
       <c r="EC5" s="10" t="s">
-        <v>2530</v>
+        <v>2529</v>
       </c>
       <c r="ED5" s="10" t="s">
-        <v>2534</v>
+        <v>2533</v>
       </c>
       <c r="EE5" s="10" t="s">
         <v>2181</v>
@@ -17142,34 +17201,34 @@
         <v>2034</v>
       </c>
       <c r="EM5" t="s">
-        <v>2893</v>
+        <v>2892</v>
       </c>
       <c r="EO5" t="s">
-        <v>2902</v>
+        <v>2901</v>
       </c>
       <c r="EZ5" s="79" t="s">
-        <v>2898</v>
+        <v>2897</v>
       </c>
       <c r="FB5" s="79" t="s">
-        <v>2872</v>
+        <v>2871</v>
       </c>
       <c r="FD5" s="79" t="s">
-        <v>2865</v>
+        <v>2864</v>
       </c>
       <c r="FY5" s="79" t="s">
-        <v>2857</v>
+        <v>2856</v>
       </c>
       <c r="FZ5" s="79" t="s">
-        <v>2860</v>
+        <v>2859</v>
       </c>
       <c r="GD5" t="s">
-        <v>2887</v>
+        <v>2886</v>
       </c>
       <c r="GE5" t="s">
-        <v>2871</v>
+        <v>2870</v>
       </c>
       <c r="GF5" s="79" t="s">
-        <v>2871</v>
+        <v>2870</v>
       </c>
       <c r="GG5" s="79" t="s">
         <v>2034</v>
@@ -17178,7 +17237,7 @@
         <v>2034</v>
       </c>
     </row>
-    <row r="6" spans="1:200">
+    <row r="6" spans="1:206">
       <c r="B6" t="s">
         <v>52</v>
       </c>
@@ -17204,7 +17263,7 @@
         <v>59</v>
       </c>
       <c r="J6" t="s">
-        <v>2816</v>
+        <v>2815</v>
       </c>
       <c r="K6" s="34" t="s">
         <v>2067</v>
@@ -17237,7 +17296,7 @@
         <v>1349</v>
       </c>
       <c r="X6" t="s">
-        <v>2585</v>
+        <v>2584</v>
       </c>
       <c r="Y6" s="6" t="s">
         <v>1364</v>
@@ -17323,29 +17382,29 @@
         <v>2042</v>
       </c>
       <c r="BH6" s="20" t="s">
-        <v>2541</v>
+        <v>2540</v>
       </c>
       <c r="BI6" s="20" t="s">
-        <v>2547</v>
+        <v>2546</v>
       </c>
       <c r="BJ6" s="20" t="s">
         <v>2194</v>
       </c>
       <c r="BK6" s="20" t="s">
-        <v>2563</v>
+        <v>2562</v>
       </c>
       <c r="BL6" s="20" t="s">
-        <v>2571</v>
+        <v>2570</v>
       </c>
       <c r="BM6" s="20" t="str">
         <f>_xlfn.CONCAT(BM5,"_error")</f>
         <v>CO2_flux_mmol_m2_d_error</v>
       </c>
       <c r="BN6" s="20" t="s">
-        <v>2519</v>
+        <v>2518</v>
       </c>
       <c r="BO6" s="20" t="s">
-        <v>2721</v>
+        <v>2720</v>
       </c>
       <c r="BP6" s="14" t="s">
         <v>1815</v>
@@ -17384,7 +17443,7 @@
         <v>2265</v>
       </c>
       <c r="CB6" s="25" t="s">
-        <v>2497</v>
+        <v>2496</v>
       </c>
       <c r="CC6" s="25" t="s">
         <v>1771</v>
@@ -17396,7 +17455,7 @@
         <v>2286</v>
       </c>
       <c r="CF6" s="23" t="s">
-        <v>2756</v>
+        <v>2755</v>
       </c>
       <c r="CG6" s="68" t="s">
         <v>2444</v>
@@ -17463,32 +17522,32 @@
         <v>2408</v>
       </c>
       <c r="DG6" s="12" t="s">
+        <v>2464</v>
+      </c>
+      <c r="DH6" s="12" t="s">
         <v>2465</v>
       </c>
-      <c r="DH6" s="12" t="s">
-        <v>2466</v>
-      </c>
       <c r="DI6" s="12" t="s">
-        <v>2469</v>
+        <v>2468</v>
       </c>
       <c r="DJ6" s="12" t="s">
-        <v>2515</v>
+        <v>2514</v>
       </c>
       <c r="DK6" s="48"/>
       <c r="DL6" s="12" t="s">
-        <v>2510</v>
+        <v>2509</v>
       </c>
       <c r="EB6" s="79"/>
       <c r="EC6" s="79"/>
       <c r="ED6" s="79"/>
       <c r="EE6" s="10" t="s">
-        <v>2774</v>
+        <v>2773</v>
       </c>
       <c r="EF6" s="10" t="s">
-        <v>2517</v>
+        <v>2516</v>
       </c>
       <c r="EG6" s="10" t="s">
-        <v>2517</v>
+        <v>2516</v>
       </c>
       <c r="EH6" s="79"/>
       <c r="EI6" s="79"/>
@@ -17497,28 +17556,28 @@
         <v>2035</v>
       </c>
       <c r="EM6" t="s">
-        <v>2891</v>
+        <v>2890</v>
       </c>
       <c r="EO6" t="s">
-        <v>2903</v>
+        <v>2902</v>
       </c>
       <c r="EZ6" s="79" t="s">
-        <v>2899</v>
+        <v>2898</v>
       </c>
       <c r="FB6" t="s">
         <v>2026</v>
       </c>
       <c r="FD6" s="79" t="s">
-        <v>2868</v>
+        <v>2867</v>
       </c>
       <c r="FZ6" t="s">
-        <v>2858</v>
+        <v>2857</v>
       </c>
       <c r="GE6" t="s">
-        <v>2880</v>
+        <v>2879</v>
       </c>
       <c r="GF6" s="79" t="s">
-        <v>2880</v>
+        <v>2879</v>
       </c>
       <c r="GG6" s="79" t="s">
         <v>2035</v>
@@ -17527,7 +17586,7 @@
         <v>2035</v>
       </c>
     </row>
-    <row r="7" spans="1:200">
+    <row r="7" spans="1:206">
       <c r="B7" t="s">
         <v>63</v>
       </c>
@@ -17583,7 +17642,7 @@
         <v>1350</v>
       </c>
       <c r="X7" s="65" t="s">
-        <v>2718</v>
+        <v>2717</v>
       </c>
       <c r="Y7" s="6" t="s">
         <v>1365</v>
@@ -17663,34 +17722,34 @@
         <v>2043</v>
       </c>
       <c r="BH7" s="20" t="s">
-        <v>2540</v>
+        <v>2539</v>
       </c>
       <c r="BI7" s="20" t="s">
-        <v>2548</v>
+        <v>2547</v>
       </c>
       <c r="BJ7" s="20" t="s">
         <v>2195</v>
       </c>
       <c r="BK7" s="20" t="s">
-        <v>2563</v>
+        <v>2562</v>
       </c>
       <c r="BL7" s="20" t="s">
-        <v>2572</v>
+        <v>2571</v>
       </c>
       <c r="BM7" s="20" t="s">
         <v>2185</v>
       </c>
       <c r="BN7" s="20" t="s">
-        <v>2519</v>
+        <v>2518</v>
       </c>
       <c r="BO7" s="20" t="s">
-        <v>2521</v>
+        <v>2520</v>
       </c>
       <c r="BP7" s="14" t="s">
         <v>1816</v>
       </c>
       <c r="BQ7" s="20" t="s">
-        <v>2502</v>
+        <v>2501</v>
       </c>
       <c r="BR7" s="20">
         <v>6</v>
@@ -17723,7 +17782,7 @@
         <v>2265</v>
       </c>
       <c r="CB7" s="25" t="s">
-        <v>2498</v>
+        <v>2497</v>
       </c>
       <c r="CC7" s="20" t="s">
         <v>1776</v>
@@ -17732,10 +17791,10 @@
         <v>2264</v>
       </c>
       <c r="CE7" s="20" t="s">
-        <v>2484</v>
+        <v>2483</v>
       </c>
       <c r="CF7" s="23" t="s">
-        <v>2757</v>
+        <v>2756</v>
       </c>
       <c r="CG7" s="68" t="s">
         <v>2444</v>
@@ -17759,13 +17818,13 @@
         <v>2280</v>
       </c>
       <c r="CO7" s="12" t="s">
-        <v>2600</v>
+        <v>2599</v>
       </c>
       <c r="CP7" s="56" t="s">
         <v>2280</v>
       </c>
       <c r="CQ7" s="12" t="s">
-        <v>2601</v>
+        <v>2600</v>
       </c>
       <c r="CR7" s="35" t="s">
         <v>2091</v>
@@ -17798,22 +17857,22 @@
         <v>2409</v>
       </c>
       <c r="DG7" s="12" t="s">
-        <v>2468</v>
+        <v>2467</v>
       </c>
       <c r="DH7" s="12" t="s">
-        <v>2466</v>
+        <v>2465</v>
       </c>
       <c r="DI7" s="12" t="s">
-        <v>2470</v>
+        <v>2469</v>
       </c>
       <c r="DJ7" s="20" t="s">
         <v>2194</v>
       </c>
       <c r="DK7" s="20" t="s">
-        <v>2563</v>
+        <v>2562</v>
       </c>
       <c r="DL7" s="20" t="s">
-        <v>2835</v>
+        <v>2834</v>
       </c>
       <c r="EB7" s="79"/>
       <c r="EC7" s="79"/>
@@ -17822,10 +17881,10 @@
         <v>2027</v>
       </c>
       <c r="EF7" s="10" t="s">
-        <v>2730</v>
+        <v>2729</v>
       </c>
       <c r="EG7" s="10" t="s">
-        <v>2730</v>
+        <v>2729</v>
       </c>
       <c r="EH7" s="79"/>
       <c r="EI7" s="79"/>
@@ -17834,22 +17893,22 @@
         <v>2027</v>
       </c>
       <c r="EM7" t="s">
-        <v>2905</v>
+        <v>2904</v>
       </c>
       <c r="EZ7" s="79" t="s">
-        <v>2900</v>
+        <v>2899</v>
       </c>
       <c r="FB7" t="s">
         <v>2027</v>
       </c>
       <c r="FD7" s="79" t="s">
-        <v>2866</v>
+        <v>2865</v>
       </c>
       <c r="GE7" s="79" t="s">
-        <v>2881</v>
+        <v>2880</v>
       </c>
       <c r="GF7" s="79" t="s">
-        <v>2881</v>
+        <v>2880</v>
       </c>
       <c r="GG7" s="79" t="s">
         <v>2027</v>
@@ -17858,7 +17917,7 @@
         <v>2027</v>
       </c>
     </row>
-    <row r="8" spans="1:200" ht="16.05" customHeight="1">
+    <row r="8" spans="1:206" ht="16.05" customHeight="1">
       <c r="B8" t="s">
         <v>75</v>
       </c>
@@ -17887,7 +17946,7 @@
         <v>83</v>
       </c>
       <c r="K8" s="70" t="s">
-        <v>2775</v>
+        <v>2774</v>
       </c>
       <c r="L8" t="s">
         <v>84</v>
@@ -17911,7 +17970,7 @@
         <v>1355</v>
       </c>
       <c r="X8" t="s">
-        <v>2586</v>
+        <v>2585</v>
       </c>
       <c r="Z8" s="6" t="s">
         <v>1371</v>
@@ -17949,7 +18008,7 @@
         <v>1968</v>
       </c>
       <c r="AO8" s="6" t="s">
-        <v>2516</v>
+        <v>2515</v>
       </c>
       <c r="AS8" s="6" t="s">
         <v>1913</v>
@@ -17979,29 +18038,29 @@
         <v>2044</v>
       </c>
       <c r="BH8" s="20" t="s">
-        <v>2540</v>
+        <v>2539</v>
       </c>
       <c r="BI8" s="20" t="s">
-        <v>2549</v>
+        <v>2548</v>
       </c>
       <c r="BJ8" s="20" t="s">
         <v>2196</v>
       </c>
       <c r="BK8" s="20" t="s">
-        <v>2563</v>
+        <v>2562</v>
       </c>
       <c r="BL8" s="20" t="s">
-        <v>2573</v>
+        <v>2572</v>
       </c>
       <c r="BM8" s="20" t="str">
         <f>_xlfn.CONCAT(BM7,"_error")</f>
         <v>DIC_flux_mmol_m2_d_error</v>
       </c>
       <c r="BN8" s="20" t="s">
-        <v>2519</v>
+        <v>2518</v>
       </c>
       <c r="BO8" s="20" t="s">
-        <v>2722</v>
+        <v>2721</v>
       </c>
       <c r="BP8" s="14" t="s">
         <v>2128</v>
@@ -18016,7 +18075,7 @@
         <v>2203</v>
       </c>
       <c r="BT8" s="10" t="s">
-        <v>2808</v>
+        <v>2807</v>
       </c>
       <c r="BU8" s="13" t="s">
         <v>2226</v>
@@ -18034,7 +18093,7 @@
         <v>2250</v>
       </c>
       <c r="BZ8" s="12" t="s">
-        <v>2487</v>
+        <v>2486</v>
       </c>
       <c r="CA8" s="12"/>
       <c r="CB8" s="12" t="s">
@@ -18050,7 +18109,7 @@
         <v>2287</v>
       </c>
       <c r="CF8" s="12" t="s">
-        <v>2758</v>
+        <v>2757</v>
       </c>
       <c r="CG8" s="68" t="s">
         <v>2444</v>
@@ -18119,19 +18178,19 @@
         <v>2195</v>
       </c>
       <c r="DK8" s="20" t="s">
-        <v>2563</v>
+        <v>2562</v>
       </c>
       <c r="DL8" s="20" t="s">
-        <v>2836</v>
+        <v>2835</v>
       </c>
       <c r="EE8" s="10" t="s">
         <v>2035</v>
       </c>
       <c r="EF8" s="10" t="s">
-        <v>2731</v>
+        <v>2730</v>
       </c>
       <c r="EG8" s="10" t="s">
-        <v>2731</v>
+        <v>2730</v>
       </c>
       <c r="EH8" s="79"/>
       <c r="EI8" s="79"/>
@@ -18140,19 +18199,19 @@
         <v>2036</v>
       </c>
       <c r="EZ8" s="79" t="s">
-        <v>2901</v>
+        <v>2900</v>
       </c>
       <c r="FB8" t="s">
-        <v>2873</v>
+        <v>2872</v>
       </c>
       <c r="FD8" s="79" t="s">
-        <v>2869</v>
+        <v>2868</v>
       </c>
       <c r="GE8" s="79" t="s">
-        <v>2882</v>
+        <v>2881</v>
       </c>
       <c r="GF8" s="79" t="s">
-        <v>2882</v>
+        <v>2881</v>
       </c>
       <c r="GG8" s="79" t="s">
         <v>2036</v>
@@ -18161,7 +18220,7 @@
         <v>2036</v>
       </c>
     </row>
-    <row r="9" spans="1:200" ht="16.05" customHeight="1">
+    <row r="9" spans="1:206" ht="16.05" customHeight="1">
       <c r="B9" t="s">
         <v>86</v>
       </c>
@@ -18205,7 +18264,7 @@
         <v>1351</v>
       </c>
       <c r="X9" t="s">
-        <v>2587</v>
+        <v>2586</v>
       </c>
       <c r="Z9" s="6" t="s">
         <v>1372</v>
@@ -18270,28 +18329,28 @@
         <v>1757</v>
       </c>
       <c r="BH9" s="20" t="s">
-        <v>2539</v>
+        <v>2538</v>
       </c>
       <c r="BI9" s="20" t="s">
-        <v>2550</v>
+        <v>2549</v>
       </c>
       <c r="BJ9" s="20" t="s">
+        <v>2799</v>
+      </c>
+      <c r="BK9" s="20" t="s">
+        <v>2562</v>
+      </c>
+      <c r="BL9" s="20" t="s">
         <v>2800</v>
-      </c>
-      <c r="BK9" s="20" t="s">
-        <v>2563</v>
-      </c>
-      <c r="BL9" s="20" t="s">
-        <v>2801</v>
       </c>
       <c r="BM9" s="20" t="s">
         <v>2186</v>
       </c>
       <c r="BN9" s="20" t="s">
-        <v>2519</v>
+        <v>2518</v>
       </c>
       <c r="BO9" s="20" t="s">
-        <v>2526</v>
+        <v>2525</v>
       </c>
       <c r="BP9" s="14" t="s">
         <v>2085</v>
@@ -18303,16 +18362,16 @@
         <v>8</v>
       </c>
       <c r="BS9" s="14" t="s">
-        <v>2909</v>
+        <v>2908</v>
       </c>
       <c r="BT9" s="10" t="s">
-        <v>2809</v>
+        <v>2808</v>
       </c>
       <c r="BU9" s="13" t="s">
         <v>2226</v>
       </c>
       <c r="BV9" s="10" t="s">
-        <v>2810</v>
+        <v>2809</v>
       </c>
       <c r="BW9" s="11" t="s">
         <v>2051</v>
@@ -18324,14 +18383,14 @@
         <v>2251</v>
       </c>
       <c r="BZ9" s="12" t="s">
-        <v>2486</v>
+        <v>2485</v>
       </c>
       <c r="CA9" s="12"/>
       <c r="CB9" s="12" t="s">
-        <v>2490</v>
+        <v>2489</v>
       </c>
       <c r="CF9" s="12" t="s">
-        <v>2759</v>
+        <v>2758</v>
       </c>
       <c r="CG9" s="68" t="s">
         <v>2444</v>
@@ -18346,7 +18405,7 @@
         <v>2266</v>
       </c>
       <c r="CK9" s="42" t="s">
-        <v>2843</v>
+        <v>2842</v>
       </c>
       <c r="CL9" s="12" t="s">
         <v>1799</v>
@@ -18355,13 +18414,13 @@
         <v>2280</v>
       </c>
       <c r="CO9" s="12" t="s">
-        <v>2602</v>
+        <v>2601</v>
       </c>
       <c r="CP9" s="56" t="s">
         <v>2280</v>
       </c>
       <c r="CQ9" s="12" t="s">
-        <v>2603</v>
+        <v>2602</v>
       </c>
       <c r="CR9" s="35" t="s">
         <v>2093</v>
@@ -18400,19 +18459,19 @@
         <v>2196</v>
       </c>
       <c r="DK9" s="20" t="s">
-        <v>2563</v>
+        <v>2562</v>
       </c>
       <c r="DL9" s="20" t="s">
-        <v>2837</v>
+        <v>2836</v>
       </c>
       <c r="EE9" s="10" t="s">
         <v>2033</v>
       </c>
       <c r="EF9" s="10" t="s">
-        <v>2834</v>
+        <v>2833</v>
       </c>
       <c r="EG9" s="10" t="s">
-        <v>2833</v>
+        <v>2832</v>
       </c>
       <c r="EH9" s="79"/>
       <c r="EI9" s="79"/>
@@ -18421,13 +18480,13 @@
         <v>2026</v>
       </c>
       <c r="EZ9" t="s">
-        <v>2895</v>
+        <v>2894</v>
       </c>
       <c r="GE9" t="s">
-        <v>2883</v>
+        <v>2882</v>
       </c>
       <c r="GF9" s="79" t="s">
-        <v>2883</v>
+        <v>2882</v>
       </c>
       <c r="GG9" s="79" t="s">
         <v>2026</v>
@@ -18436,7 +18495,7 @@
         <v>2026</v>
       </c>
     </row>
-    <row r="10" spans="1:200">
+    <row r="10" spans="1:206">
       <c r="B10" t="s">
         <v>95</v>
       </c>
@@ -18530,36 +18589,36 @@
         <v>1735</v>
       </c>
       <c r="BC10" s="47" t="s">
-        <v>2475</v>
+        <v>2474</v>
       </c>
       <c r="BD10" s="17"/>
       <c r="BG10" s="20" t="s">
         <v>1772</v>
       </c>
       <c r="BH10" s="20" t="s">
-        <v>2539</v>
+        <v>2538</v>
       </c>
       <c r="BI10" s="20" t="s">
-        <v>2551</v>
+        <v>2550</v>
       </c>
       <c r="BJ10" s="20" t="s">
+        <v>2801</v>
+      </c>
+      <c r="BK10" s="20" t="s">
+        <v>2562</v>
+      </c>
+      <c r="BL10" s="20" t="s">
         <v>2802</v>
-      </c>
-      <c r="BK10" s="20" t="s">
-        <v>2563</v>
-      </c>
-      <c r="BL10" s="20" t="s">
-        <v>2803</v>
       </c>
       <c r="BM10" s="20" t="str">
         <f>_xlfn.CONCAT(BM9,"_error")</f>
         <v>NH4_flux_mmol_m2_d_error</v>
       </c>
       <c r="BN10" s="20" t="s">
-        <v>2519</v>
+        <v>2518</v>
       </c>
       <c r="BO10" s="20" t="s">
-        <v>2723</v>
+        <v>2722</v>
       </c>
       <c r="BP10" s="14" t="s">
         <v>2096</v>
@@ -18571,7 +18630,7 @@
         <v>9</v>
       </c>
       <c r="BS10" s="14" t="s">
-        <v>2477</v>
+        <v>2476</v>
       </c>
       <c r="BT10" s="10" t="s">
         <v>1845</v>
@@ -18595,7 +18654,7 @@
       <c r="CA10" s="63"/>
       <c r="CB10" s="63"/>
       <c r="CF10" s="12" t="s">
-        <v>2760</v>
+        <v>2759</v>
       </c>
       <c r="CG10" s="68" t="s">
         <v>2444</v>
@@ -18655,13 +18714,13 @@
       <c r="DH10" s="12"/>
       <c r="DI10" s="12"/>
       <c r="DJ10" s="20" t="s">
-        <v>2800</v>
+        <v>2799</v>
       </c>
       <c r="DK10" s="20" t="s">
-        <v>2563</v>
+        <v>2562</v>
       </c>
       <c r="DL10" s="20" t="s">
-        <v>2838</v>
+        <v>2837</v>
       </c>
       <c r="EE10" s="10" t="s">
         <v>2028</v>
@@ -18687,7 +18746,7 @@
         <v>2181</v>
       </c>
     </row>
-    <row r="11" spans="1:200">
+    <row r="11" spans="1:206">
       <c r="B11" t="s">
         <v>104</v>
       </c>
@@ -18784,37 +18843,37 @@
       </c>
       <c r="BD11" s="17"/>
       <c r="BG11" s="20" t="s">
-        <v>2542</v>
+        <v>2541</v>
       </c>
       <c r="BH11" s="20" t="s">
-        <v>2518</v>
+        <v>2517</v>
       </c>
       <c r="BI11" s="20" t="s">
-        <v>2552</v>
+        <v>2551</v>
       </c>
       <c r="BJ11" s="20" t="s">
+        <v>2803</v>
+      </c>
+      <c r="BK11" s="20" t="s">
+        <v>2562</v>
+      </c>
+      <c r="BL11" s="20" t="s">
         <v>2804</v>
-      </c>
-      <c r="BK11" s="20" t="s">
-        <v>2563</v>
-      </c>
-      <c r="BL11" s="20" t="s">
-        <v>2805</v>
       </c>
       <c r="BM11" s="20" t="s">
         <v>2187</v>
       </c>
       <c r="BN11" s="20" t="s">
-        <v>2519</v>
+        <v>2518</v>
       </c>
       <c r="BO11" s="20" t="s">
-        <v>2525</v>
+        <v>2524</v>
       </c>
       <c r="BP11" s="14" t="s">
         <v>2395</v>
       </c>
       <c r="BQ11" s="20" t="s">
-        <v>2503</v>
+        <v>2502</v>
       </c>
       <c r="BR11" s="20">
         <v>10</v>
@@ -18844,7 +18903,7 @@
       <c r="CA11" s="63"/>
       <c r="CB11" s="63"/>
       <c r="CF11" s="12" t="s">
-        <v>2761</v>
+        <v>2760</v>
       </c>
       <c r="CG11" s="68" t="s">
         <v>2444</v>
@@ -18868,13 +18927,13 @@
         <v>2280</v>
       </c>
       <c r="CO11" s="12" t="s">
-        <v>2604</v>
+        <v>2603</v>
       </c>
       <c r="CP11" s="56" t="s">
         <v>2280</v>
       </c>
       <c r="CQ11" s="12" t="s">
-        <v>2605</v>
+        <v>2604</v>
       </c>
       <c r="CR11" s="12" t="s">
         <v>2094</v>
@@ -18902,13 +18961,13 @@
       <c r="DH11" s="12"/>
       <c r="DI11" s="12"/>
       <c r="DJ11" s="20" t="s">
-        <v>2802</v>
+        <v>2801</v>
       </c>
       <c r="DK11" s="20" t="s">
-        <v>2563</v>
+        <v>2562</v>
       </c>
       <c r="DL11" s="20" t="s">
-        <v>2839</v>
+        <v>2838</v>
       </c>
       <c r="EE11" s="10" t="s">
         <v>2205</v>
@@ -18919,10 +18978,10 @@
         <v>2037</v>
       </c>
       <c r="GE11" t="s">
-        <v>2884</v>
+        <v>2883</v>
       </c>
       <c r="GF11" s="79" t="s">
-        <v>2884</v>
+        <v>2883</v>
       </c>
       <c r="GG11" s="79" t="s">
         <v>2037</v>
@@ -18931,7 +18990,7 @@
         <v>2037</v>
       </c>
     </row>
-    <row r="12" spans="1:200">
+    <row r="12" spans="1:206">
       <c r="B12" t="s">
         <v>113</v>
       </c>
@@ -18988,7 +19047,7 @@
       </c>
       <c r="AG12" s="17"/>
       <c r="AI12" s="64" t="s">
-        <v>2716</v>
+        <v>2715</v>
       </c>
       <c r="AJ12" s="6" t="s">
         <v>1461</v>
@@ -19028,29 +19087,29 @@
         <v>1758</v>
       </c>
       <c r="BH12" s="20" t="s">
-        <v>2539</v>
+        <v>2538</v>
       </c>
       <c r="BI12" s="20" t="s">
-        <v>2553</v>
+        <v>2552</v>
       </c>
       <c r="BJ12" s="20" t="s">
+        <v>2768</v>
+      </c>
+      <c r="BK12" s="20" t="s">
         <v>2769</v>
       </c>
-      <c r="BK12" s="20" t="s">
+      <c r="BL12" s="20" t="s">
         <v>2770</v>
-      </c>
-      <c r="BL12" s="20" t="s">
-        <v>2771</v>
       </c>
       <c r="BM12" s="20" t="str">
         <f>_xlfn.CONCAT(BM11,"_error")</f>
         <v>Fe_flux_mmol_m2_d_error</v>
       </c>
       <c r="BN12" s="20" t="s">
-        <v>2519</v>
+        <v>2518</v>
       </c>
       <c r="BO12" s="20" t="s">
-        <v>2724</v>
+        <v>2723</v>
       </c>
       <c r="BP12" s="14" t="s">
         <v>2403</v>
@@ -19065,13 +19124,13 @@
         <v>2211</v>
       </c>
       <c r="BT12" s="10" t="s">
-        <v>2739</v>
+        <v>2738</v>
       </c>
       <c r="BU12" s="13" t="s">
         <v>2227</v>
       </c>
       <c r="BV12" s="10" t="s">
-        <v>2740</v>
+        <v>2739</v>
       </c>
       <c r="BW12" s="11" t="s">
         <v>2052</v>
@@ -19086,7 +19145,7 @@
       <c r="CA12" s="63"/>
       <c r="CB12" s="63"/>
       <c r="CF12" s="12" t="s">
-        <v>2762</v>
+        <v>2761</v>
       </c>
       <c r="CG12" s="68" t="s">
         <v>2444</v>
@@ -19137,16 +19196,16 @@
       <c r="DH12" s="12"/>
       <c r="DI12" s="12"/>
       <c r="DJ12" s="20" t="s">
-        <v>2804</v>
+        <v>2803</v>
       </c>
       <c r="DK12" s="20" t="s">
-        <v>2563</v>
+        <v>2562</v>
       </c>
       <c r="DL12" s="20" t="s">
-        <v>2840</v>
+        <v>2839</v>
       </c>
       <c r="EE12" s="10" t="s">
-        <v>2773</v>
+        <v>2772</v>
       </c>
       <c r="EF12" s="10"/>
       <c r="EG12" s="79"/>
@@ -19154,10 +19213,10 @@
         <v>2038</v>
       </c>
       <c r="GE12" s="82" t="s">
-        <v>2517</v>
+        <v>2516</v>
       </c>
       <c r="GF12" s="82" t="s">
-        <v>2517</v>
+        <v>2516</v>
       </c>
       <c r="GG12" s="79" t="s">
         <v>2038</v>
@@ -19166,7 +19225,7 @@
         <v>2038</v>
       </c>
     </row>
-    <row r="13" spans="1:200">
+    <row r="13" spans="1:206">
       <c r="B13" t="s">
         <v>122</v>
       </c>
@@ -19186,7 +19245,7 @@
         <v>127</v>
       </c>
       <c r="J13" t="s">
-        <v>2832</v>
+        <v>2831</v>
       </c>
       <c r="K13" s="34" t="s">
         <v>2073</v>
@@ -19205,7 +19264,7 @@
       </c>
       <c r="U13" s="6"/>
       <c r="V13" s="77" t="s">
-        <v>2831</v>
+        <v>2830</v>
       </c>
       <c r="AB13" s="6" t="s">
         <v>1387</v>
@@ -19258,25 +19317,25 @@
         <v>2039</v>
       </c>
       <c r="BH13" s="20" t="s">
-        <v>2539</v>
+        <v>2538</v>
       </c>
       <c r="BI13" s="20" t="s">
-        <v>2554</v>
+        <v>2553</v>
       </c>
       <c r="BM13" s="20" t="s">
         <v>2188</v>
       </c>
       <c r="BN13" s="20" t="s">
-        <v>2519</v>
+        <v>2518</v>
       </c>
       <c r="BO13" s="20" t="s">
-        <v>2524</v>
+        <v>2523</v>
       </c>
       <c r="BP13" s="14" t="s">
-        <v>2476</v>
+        <v>2475</v>
       </c>
       <c r="BQ13" s="20" t="s">
-        <v>2505</v>
+        <v>2504</v>
       </c>
       <c r="BR13" s="20">
         <v>12</v>
@@ -19285,13 +19344,13 @@
         <v>2212</v>
       </c>
       <c r="BT13" s="10" t="s">
-        <v>2748</v>
+        <v>2747</v>
       </c>
       <c r="BU13" s="13" t="s">
         <v>2227</v>
       </c>
       <c r="BV13" s="10" t="s">
-        <v>2749</v>
+        <v>2748</v>
       </c>
       <c r="BW13" s="11" t="s">
         <v>2053</v>
@@ -19306,7 +19365,7 @@
       <c r="CA13" s="63"/>
       <c r="CB13" s="63"/>
       <c r="CF13" s="12" t="s">
-        <v>2763</v>
+        <v>2762</v>
       </c>
       <c r="CG13" s="68" t="s">
         <v>2444</v>
@@ -19330,13 +19389,13 @@
         <v>2280</v>
       </c>
       <c r="CO13" s="12" t="s">
-        <v>2606</v>
+        <v>2605</v>
       </c>
       <c r="CP13" s="56" t="s">
         <v>2280</v>
       </c>
       <c r="CQ13" s="12" t="s">
-        <v>2607</v>
+        <v>2606</v>
       </c>
       <c r="CU13" s="36" t="s">
         <v>2110</v>
@@ -19354,13 +19413,13 @@
         <v>2415</v>
       </c>
       <c r="DJ13" s="20" t="s">
+        <v>2768</v>
+      </c>
+      <c r="DK13" s="20" t="s">
         <v>2769</v>
       </c>
-      <c r="DK13" s="20" t="s">
-        <v>2770</v>
-      </c>
       <c r="DL13" s="20" t="s">
-        <v>2841</v>
+        <v>2840</v>
       </c>
       <c r="EE13" s="10"/>
       <c r="EF13" s="10"/>
@@ -19381,7 +19440,7 @@
         <v>2028</v>
       </c>
     </row>
-    <row r="14" spans="1:200">
+    <row r="14" spans="1:206">
       <c r="B14" t="s">
         <v>130</v>
       </c>
@@ -19401,7 +19460,7 @@
         <v>135</v>
       </c>
       <c r="K14" s="71" t="s">
-        <v>2806</v>
+        <v>2805</v>
       </c>
       <c r="L14" t="s">
         <v>136</v>
@@ -19417,7 +19476,7 @@
       </c>
       <c r="U14" s="6"/>
       <c r="V14" s="62" t="s">
-        <v>2707</v>
+        <v>2706</v>
       </c>
       <c r="AB14" s="6" t="s">
         <v>1394</v>
@@ -19461,20 +19520,20 @@
         <v>1759</v>
       </c>
       <c r="BH14" s="20" t="s">
-        <v>2518</v>
+        <v>2517</v>
       </c>
       <c r="BI14" s="20" t="s">
-        <v>2555</v>
+        <v>2554</v>
       </c>
       <c r="BM14" s="20" t="str">
         <f>_xlfn.CONCAT(BM13,"_error")</f>
         <v>Mn_flux_mmol_m2_d_error</v>
       </c>
       <c r="BN14" s="20" t="s">
-        <v>2519</v>
+        <v>2518</v>
       </c>
       <c r="BO14" s="20" t="s">
-        <v>2725</v>
+        <v>2724</v>
       </c>
       <c r="BP14" s="14" t="s">
         <v>2124</v>
@@ -19489,13 +19548,13 @@
         <v>2213</v>
       </c>
       <c r="BT14" s="20" t="s">
-        <v>2811</v>
+        <v>2810</v>
       </c>
       <c r="BU14" s="13" t="s">
         <v>2227</v>
       </c>
       <c r="BV14" s="20" t="s">
-        <v>2812</v>
+        <v>2811</v>
       </c>
       <c r="BW14" s="11" t="s">
         <v>2054</v>
@@ -19510,13 +19569,13 @@
       <c r="CA14" s="63"/>
       <c r="CB14" s="63"/>
       <c r="CF14" s="12" t="s">
-        <v>2750</v>
+        <v>2749</v>
       </c>
       <c r="CG14" s="68" t="s">
         <v>2444</v>
       </c>
       <c r="CH14" s="12" t="s">
-        <v>2764</v>
+        <v>2763</v>
       </c>
       <c r="CI14" s="12" t="s">
         <v>1788</v>
@@ -19571,7 +19630,7 @@
         <v>2027</v>
       </c>
     </row>
-    <row r="15" spans="1:200">
+    <row r="15" spans="1:206">
       <c r="B15" t="s">
         <v>138</v>
       </c>
@@ -19644,25 +19703,25 @@
         <v>1761</v>
       </c>
       <c r="BH15" s="20" t="s">
-        <v>2540</v>
+        <v>2539</v>
       </c>
       <c r="BI15" s="20" t="s">
-        <v>2556</v>
+        <v>2555</v>
       </c>
       <c r="BM15" s="20" t="s">
         <v>2189</v>
       </c>
       <c r="BN15" s="20" t="s">
-        <v>2519</v>
+        <v>2518</v>
       </c>
       <c r="BO15" s="20" t="s">
-        <v>2523</v>
+        <v>2522</v>
       </c>
       <c r="BP15" s="14" t="s">
-        <v>2473</v>
+        <v>2472</v>
       </c>
       <c r="BQ15" s="20" t="s">
-        <v>2504</v>
+        <v>2503</v>
       </c>
       <c r="BR15" s="20">
         <v>14</v>
@@ -19692,13 +19751,13 @@
       <c r="CA15" s="63"/>
       <c r="CB15" s="63"/>
       <c r="CF15" s="12" t="s">
-        <v>2751</v>
+        <v>2750</v>
       </c>
       <c r="CG15" s="68" t="s">
         <v>2444</v>
       </c>
       <c r="CH15" s="12" t="s">
-        <v>2765</v>
+        <v>2764</v>
       </c>
       <c r="CI15" s="12" t="s">
         <v>1789</v>
@@ -19716,13 +19775,13 @@
         <v>2280</v>
       </c>
       <c r="CO15" s="12" t="s">
-        <v>2608</v>
+        <v>2607</v>
       </c>
       <c r="CP15" s="56" t="s">
         <v>2280</v>
       </c>
       <c r="CQ15" s="12" t="s">
-        <v>2609</v>
+        <v>2608</v>
       </c>
       <c r="CR15" s="42"/>
       <c r="CU15" s="36" t="s">
@@ -19753,7 +19812,7 @@
         <v>2028</v>
       </c>
     </row>
-    <row r="16" spans="1:200">
+    <row r="16" spans="1:206">
       <c r="B16" t="s">
         <v>145</v>
       </c>
@@ -19797,7 +19856,7 @@
         <v>1406</v>
       </c>
       <c r="AF16" s="47" t="s">
-        <v>2478</v>
+        <v>2477</v>
       </c>
       <c r="AI16" s="6" t="s">
         <v>1445</v>
@@ -19827,20 +19886,20 @@
         <v>1760</v>
       </c>
       <c r="BH16" s="20" t="s">
-        <v>2540</v>
+        <v>2539</v>
       </c>
       <c r="BI16" s="20" t="s">
-        <v>2557</v>
+        <v>2556</v>
       </c>
       <c r="BM16" s="20" t="str">
         <f>_xlfn.CONCAT(BM15,"_error")</f>
         <v>SO4_flux_mmol_m2_d_error</v>
       </c>
       <c r="BN16" s="20" t="s">
-        <v>2519</v>
+        <v>2518</v>
       </c>
       <c r="BO16" s="20" t="s">
-        <v>2726</v>
+        <v>2725</v>
       </c>
       <c r="BP16" s="14" t="s">
         <v>2216</v>
@@ -19876,10 +19935,10 @@
       <c r="CA16" s="63"/>
       <c r="CB16" s="63"/>
       <c r="CF16" s="12" t="s">
-        <v>2772</v>
+        <v>2771</v>
       </c>
       <c r="CH16" s="12" t="s">
-        <v>2766</v>
+        <v>2765</v>
       </c>
       <c r="CI16" s="12" t="s">
         <v>1790</v>
@@ -20005,31 +20064,31 @@
         <v>1762</v>
       </c>
       <c r="BH17" s="10" t="s">
-        <v>2540</v>
+        <v>2539</v>
       </c>
       <c r="BI17" s="20" t="s">
-        <v>2558</v>
+        <v>2557</v>
       </c>
       <c r="BM17" s="20" t="s">
         <v>2190</v>
       </c>
       <c r="BN17" s="20" t="s">
-        <v>2519</v>
+        <v>2518</v>
       </c>
       <c r="BO17" s="20" t="s">
-        <v>2522</v>
+        <v>2521</v>
       </c>
       <c r="BP17" s="14" t="s">
-        <v>2591</v>
+        <v>2590</v>
       </c>
       <c r="BQ17" s="20" t="s">
-        <v>2777</v>
+        <v>2776</v>
       </c>
       <c r="BR17" s="20">
         <v>16</v>
       </c>
       <c r="BS17" s="14" t="s">
-        <v>2817</v>
+        <v>2816</v>
       </c>
       <c r="BT17" s="10" t="s">
         <v>2084</v>
@@ -20068,13 +20127,13 @@
         <v>2280</v>
       </c>
       <c r="CO17" s="12" t="s">
-        <v>2610</v>
+        <v>2609</v>
       </c>
       <c r="CP17" s="56" t="s">
         <v>2280</v>
       </c>
       <c r="CQ17" s="12" t="s">
-        <v>2611</v>
+        <v>2610</v>
       </c>
       <c r="CR17" s="42"/>
       <c r="CU17" s="36" t="s">
@@ -20099,10 +20158,10 @@
       <c r="DK17" s="43"/>
       <c r="DL17" s="43"/>
       <c r="GE17" t="s">
+        <v>2884</v>
+      </c>
+      <c r="GF17" s="79" t="s">
         <v>2885</v>
-      </c>
-      <c r="GF17" s="79" t="s">
-        <v>2886</v>
       </c>
     </row>
     <row r="18" spans="2:188">
@@ -20176,32 +20235,32 @@
         <v>1763</v>
       </c>
       <c r="BH18" s="10" t="s">
-        <v>2518</v>
+        <v>2517</v>
       </c>
       <c r="BI18" s="20" t="s">
-        <v>2559</v>
+        <v>2558</v>
       </c>
       <c r="BM18" s="20" t="str">
         <f>_xlfn.CONCAT(BM17,"_error")</f>
         <v>PO4_flux_mmol_m2_d_error</v>
       </c>
       <c r="BN18" s="20" t="s">
-        <v>2519</v>
+        <v>2518</v>
       </c>
       <c r="BO18" s="20" t="s">
-        <v>2727</v>
+        <v>2726</v>
       </c>
       <c r="BP18" s="14" t="s">
+        <v>2778</v>
+      </c>
+      <c r="BQ18" s="20" t="s">
         <v>2779</v>
-      </c>
-      <c r="BQ18" s="20" t="s">
-        <v>2780</v>
       </c>
       <c r="BR18" s="20">
         <v>17</v>
       </c>
       <c r="BS18" s="14" t="s">
-        <v>2818</v>
+        <v>2817</v>
       </c>
       <c r="BT18" s="10" t="s">
         <v>2123</v>
@@ -20223,13 +20282,13 @@
       <c r="CA18" s="11"/>
       <c r="CB18" s="11"/>
       <c r="CI18" s="12" t="s">
-        <v>2845</v>
+        <v>2844</v>
       </c>
       <c r="CJ18" s="78" t="s">
         <v>2266</v>
       </c>
       <c r="CK18" s="78" t="s">
-        <v>2842</v>
+        <v>2841</v>
       </c>
       <c r="CL18" s="12" t="s">
         <v>1802</v>
@@ -20343,31 +20402,31 @@
         <v>1811</v>
       </c>
       <c r="BH19" s="20" t="s">
-        <v>2539</v>
+        <v>2538</v>
       </c>
       <c r="BI19" s="20" t="s">
-        <v>2560</v>
+        <v>2559</v>
       </c>
       <c r="BM19" s="20" t="s">
         <v>2191</v>
       </c>
       <c r="BN19" s="20" t="s">
-        <v>2519</v>
+        <v>2518</v>
       </c>
       <c r="BO19" s="20" t="s">
-        <v>2527</v>
+        <v>2526</v>
       </c>
       <c r="BP19" s="14" t="s">
-        <v>2776</v>
+        <v>2775</v>
       </c>
       <c r="BQ19" s="20" t="s">
-        <v>2778</v>
+        <v>2777</v>
       </c>
       <c r="BR19" s="20">
         <v>18</v>
       </c>
       <c r="BS19" s="14" t="s">
-        <v>2819</v>
+        <v>2818</v>
       </c>
       <c r="BT19" s="10" t="s">
         <v>2206</v>
@@ -20388,13 +20447,13 @@
       <c r="CA19" s="11"/>
       <c r="CB19" s="11"/>
       <c r="CI19" s="12" t="s">
-        <v>2846</v>
+        <v>2845</v>
       </c>
       <c r="CJ19" s="78" t="s">
         <v>2266</v>
       </c>
       <c r="CK19" s="78" t="s">
-        <v>2844</v>
+        <v>2843</v>
       </c>
       <c r="CL19" s="12" t="s">
         <v>1803</v>
@@ -20403,13 +20462,13 @@
         <v>2280</v>
       </c>
       <c r="CO19" s="12" t="s">
-        <v>2612</v>
+        <v>2611</v>
       </c>
       <c r="CP19" s="56" t="s">
         <v>2280</v>
       </c>
       <c r="CQ19" s="12" t="s">
-        <v>2613</v>
+        <v>2612</v>
       </c>
       <c r="CR19" s="42"/>
       <c r="CU19" s="36" t="s">
@@ -20434,10 +20493,10 @@
       <c r="DK19" s="43"/>
       <c r="DL19" s="43"/>
       <c r="GE19" s="10" t="s">
-        <v>2773</v>
+        <v>2772</v>
       </c>
       <c r="GF19" s="10" t="s">
-        <v>2773</v>
+        <v>2772</v>
       </c>
     </row>
     <row r="20" spans="2:188">
@@ -20505,32 +20564,32 @@
         <v>1812</v>
       </c>
       <c r="BH20" s="20" t="s">
-        <v>2539</v>
+        <v>2538</v>
       </c>
       <c r="BI20" s="20" t="s">
-        <v>2561</v>
+        <v>2560</v>
       </c>
       <c r="BM20" s="20" t="str">
         <f>_xlfn.CONCAT(BM19,"_error")</f>
         <v>NO3_flux_mmol_m2_d_error</v>
       </c>
       <c r="BN20" s="20" t="s">
-        <v>2519</v>
+        <v>2518</v>
       </c>
       <c r="BO20" s="20" t="s">
-        <v>2728</v>
+        <v>2727</v>
       </c>
       <c r="BP20" s="14" t="s">
-        <v>2792</v>
+        <v>2791</v>
       </c>
       <c r="BQ20" s="20" t="s">
-        <v>2799</v>
+        <v>2798</v>
       </c>
       <c r="BR20" s="20">
         <v>19</v>
       </c>
       <c r="BS20" s="14" t="s">
-        <v>2820</v>
+        <v>2819</v>
       </c>
       <c r="BW20" s="11" t="s">
         <v>2369</v>
@@ -20580,10 +20639,10 @@
       <c r="DK20" s="43"/>
       <c r="DL20" s="43"/>
       <c r="GE20" s="10" t="s">
-        <v>2906</v>
+        <v>2905</v>
       </c>
       <c r="GF20" s="10" t="s">
-        <v>2906</v>
+        <v>2905</v>
       </c>
     </row>
     <row r="21" spans="2:188" ht="16.8">
@@ -20646,28 +20705,28 @@
         <v>1764</v>
       </c>
       <c r="BH21" s="10" t="s">
-        <v>2518</v>
+        <v>2517</v>
       </c>
       <c r="BI21" s="20" t="s">
-        <v>2562</v>
+        <v>2561</v>
       </c>
       <c r="BM21" s="20" t="s">
         <v>2192</v>
       </c>
       <c r="BN21" s="20" t="s">
-        <v>2519</v>
+        <v>2518</v>
       </c>
       <c r="BO21" s="20" t="s">
-        <v>2528</v>
+        <v>2527</v>
       </c>
       <c r="BP21" s="14" t="s">
-        <v>2847</v>
+        <v>2846</v>
       </c>
       <c r="BQ21" s="20" t="s">
-        <v>2849</v>
+        <v>2848</v>
       </c>
       <c r="BS21" s="14" t="s">
-        <v>2821</v>
+        <v>2820</v>
       </c>
       <c r="BW21" s="11" t="s">
         <v>2373</v>
@@ -20685,13 +20744,13 @@
         <v>2280</v>
       </c>
       <c r="CO21" s="12" t="s">
-        <v>2614</v>
+        <v>2613</v>
       </c>
       <c r="CP21" s="56" t="s">
         <v>2280</v>
       </c>
       <c r="CQ21" s="12" t="s">
-        <v>2615</v>
+        <v>2614</v>
       </c>
       <c r="CU21" s="36" t="s">
         <v>2120</v>
@@ -20757,22 +20816,22 @@
         <v>O2_flux_mmol_m2_d_error</v>
       </c>
       <c r="BN22" s="20" t="s">
-        <v>2519</v>
+        <v>2518</v>
       </c>
       <c r="BO22" s="20" t="s">
-        <v>2729</v>
+        <v>2728</v>
       </c>
       <c r="BP22" s="14" t="s">
-        <v>2848</v>
+        <v>2847</v>
       </c>
       <c r="BQ22" s="20" t="s">
-        <v>2850</v>
+        <v>2849</v>
       </c>
       <c r="BS22" s="14" t="s">
-        <v>2822</v>
+        <v>2821</v>
       </c>
       <c r="BW22" s="11" t="s">
-        <v>2574</v>
+        <v>2573</v>
       </c>
       <c r="BX22" s="10" t="s">
         <v>2226</v>
@@ -20858,16 +20917,16 @@
       </c>
       <c r="BD23" s="17"/>
       <c r="BP23" s="14" t="s">
+        <v>2906</v>
+      </c>
+      <c r="BQ23" s="20" t="s">
         <v>2907</v>
       </c>
-      <c r="BQ23" s="20" t="s">
-        <v>2908</v>
-      </c>
       <c r="BS23" s="14" t="s">
-        <v>2823</v>
+        <v>2822</v>
       </c>
       <c r="BW23" s="11" t="s">
-        <v>2575</v>
+        <v>2574</v>
       </c>
       <c r="BX23" s="10" t="s">
         <v>2226</v>
@@ -20888,13 +20947,13 @@
         <v>2280</v>
       </c>
       <c r="CO23" s="12" t="s">
-        <v>2616</v>
+        <v>2615</v>
       </c>
       <c r="CP23" s="56" t="s">
         <v>2280</v>
       </c>
       <c r="CQ23" s="12" t="s">
-        <v>2617</v>
+        <v>2616</v>
       </c>
       <c r="CU23" s="43" t="s">
         <v>2394</v>
@@ -20958,10 +21017,10 @@
       </c>
       <c r="BD24" s="17"/>
       <c r="BS24" s="14" t="s">
-        <v>2824</v>
+        <v>2823</v>
       </c>
       <c r="BW24" s="11" t="s">
-        <v>2576</v>
+        <v>2575</v>
       </c>
       <c r="BX24" s="10" t="s">
         <v>2226</v>
@@ -21025,7 +21084,7 @@
         <v>657</v>
       </c>
       <c r="Q25" s="18" t="s">
-        <v>2512</v>
+        <v>2511</v>
       </c>
       <c r="AC25" s="6" t="s">
         <v>1413</v>
@@ -21047,10 +21106,10 @@
       </c>
       <c r="BD25" s="17"/>
       <c r="BS25" s="14" t="s">
-        <v>2825</v>
+        <v>2824</v>
       </c>
       <c r="BW25" s="11" t="s">
-        <v>2577</v>
+        <v>2576</v>
       </c>
       <c r="BX25" s="10" t="s">
         <v>2226</v>
@@ -21068,13 +21127,13 @@
         <v>2280</v>
       </c>
       <c r="CO25" s="12" t="s">
-        <v>2618</v>
+        <v>2617</v>
       </c>
       <c r="CP25" s="56" t="s">
         <v>2280</v>
       </c>
       <c r="CQ25" s="12" t="s">
-        <v>2619</v>
+        <v>2618</v>
       </c>
       <c r="CU25" s="36" t="s">
         <v>2100</v>
@@ -21135,7 +21194,7 @@
       </c>
       <c r="BD26" s="17"/>
       <c r="BS26" s="14" t="s">
-        <v>2826</v>
+        <v>2825</v>
       </c>
       <c r="BW26" s="11" t="s">
         <v>1765</v>
@@ -21216,7 +21275,7 @@
         <v>1941</v>
       </c>
       <c r="BS27" s="14" t="s">
-        <v>2827</v>
+        <v>2826</v>
       </c>
       <c r="BW27" s="11" t="s">
         <v>1775</v>
@@ -21234,13 +21293,13 @@
         <v>2376</v>
       </c>
       <c r="CO27" s="12" t="s">
-        <v>2620</v>
+        <v>2619</v>
       </c>
       <c r="CP27" s="56" t="s">
         <v>2280</v>
       </c>
       <c r="CQ27" s="12" t="s">
-        <v>2621</v>
+        <v>2620</v>
       </c>
       <c r="CU27" s="36" t="s">
         <v>2113</v>
@@ -21297,16 +21356,16 @@
         <v>1655</v>
       </c>
       <c r="BS28" s="14" t="s">
-        <v>2828</v>
+        <v>2827</v>
       </c>
       <c r="BW28" s="11" t="s">
-        <v>2733</v>
+        <v>2732</v>
       </c>
       <c r="BX28" s="11" t="s">
         <v>2226</v>
       </c>
       <c r="BY28" s="11" t="s">
-        <v>2734</v>
+        <v>2733</v>
       </c>
       <c r="BZ28" s="11"/>
       <c r="CA28" s="11"/>
@@ -21360,7 +21419,7 @@
         <v>856</v>
       </c>
       <c r="AC29" t="s">
-        <v>2583</v>
+        <v>2582</v>
       </c>
       <c r="AI29" s="6" t="s">
         <v>1961</v>
@@ -21375,7 +21434,7 @@
         <v>1678</v>
       </c>
       <c r="BS29" s="14" t="s">
-        <v>2829</v>
+        <v>2828</v>
       </c>
       <c r="BW29" s="20"/>
       <c r="BX29" s="14"/>
@@ -21387,13 +21446,13 @@
         <v>2377</v>
       </c>
       <c r="CO29" s="12" t="s">
-        <v>2622</v>
+        <v>2621</v>
       </c>
       <c r="CP29" s="56" t="s">
         <v>2280</v>
       </c>
       <c r="CQ29" s="12" t="s">
-        <v>2623</v>
+        <v>2622</v>
       </c>
       <c r="CU29" s="36" t="s">
         <v>2122</v>
@@ -21511,19 +21570,19 @@
         <v>2378</v>
       </c>
       <c r="CO31" s="12" t="s">
-        <v>2624</v>
+        <v>2623</v>
       </c>
       <c r="CP31" s="56" t="s">
         <v>2280</v>
       </c>
       <c r="CQ31" s="12" t="s">
-        <v>2625</v>
+        <v>2624</v>
       </c>
       <c r="CU31" s="36" t="s">
-        <v>2480</v>
+        <v>2479</v>
       </c>
       <c r="CW31" s="42" t="s">
-        <v>2483</v>
+        <v>2482</v>
       </c>
     </row>
     <row r="32" spans="2:188" ht="17.399999999999999">
@@ -21583,10 +21642,10 @@
         <v>2322</v>
       </c>
       <c r="CU32" t="s">
+        <v>2480</v>
+      </c>
+      <c r="CW32" s="42" t="s">
         <v>2481</v>
-      </c>
-      <c r="CW32" s="42" t="s">
-        <v>2482</v>
       </c>
     </row>
     <row r="33" spans="2:96" ht="17.399999999999999">
@@ -21639,13 +21698,13 @@
       <c r="CM33" s="23"/>
       <c r="CN33" s="23"/>
       <c r="CO33" s="12" t="s">
-        <v>2626</v>
+        <v>2625</v>
       </c>
       <c r="CP33" s="56" t="s">
         <v>2280</v>
       </c>
       <c r="CQ33" s="12" t="s">
-        <v>2627</v>
+        <v>2626</v>
       </c>
     </row>
     <row r="34" spans="2:96">
@@ -21754,13 +21813,13 @@
       <c r="CM35" s="23"/>
       <c r="CN35" s="23"/>
       <c r="CO35" s="12" t="s">
-        <v>2628</v>
+        <v>2627</v>
       </c>
       <c r="CP35" s="56" t="s">
         <v>2280</v>
       </c>
       <c r="CQ35" s="12" t="s">
-        <v>2629</v>
+        <v>2628</v>
       </c>
     </row>
     <row r="36" spans="2:96" ht="17.399999999999999">
@@ -21805,7 +21864,7 @@
       <c r="CA36" s="14"/>
       <c r="CB36" s="14"/>
       <c r="CL36" s="23" t="s">
-        <v>2767</v>
+        <v>2766</v>
       </c>
       <c r="CM36" s="23"/>
       <c r="CN36" s="23"/>
@@ -21862,18 +21921,18 @@
       <c r="CA37" s="14"/>
       <c r="CB37" s="14"/>
       <c r="CL37" s="23" t="s">
-        <v>2768</v>
+        <v>2767</v>
       </c>
       <c r="CM37" s="23"/>
       <c r="CN37" s="23"/>
       <c r="CO37" s="12" t="s">
-        <v>2630</v>
+        <v>2629</v>
       </c>
       <c r="CP37" s="56" t="s">
         <v>2280</v>
       </c>
       <c r="CQ37" s="12" t="s">
-        <v>2631</v>
+        <v>2630</v>
       </c>
     </row>
     <row r="38" spans="2:96" ht="17.399999999999999">
@@ -21973,13 +22032,13 @@
       <c r="CB39" s="14"/>
       <c r="CL39" s="23"/>
       <c r="CO39" s="12" t="s">
-        <v>2632</v>
+        <v>2631</v>
       </c>
       <c r="CP39" s="56" t="s">
         <v>2280</v>
       </c>
       <c r="CQ39" s="12" t="s">
-        <v>2633</v>
+        <v>2632</v>
       </c>
       <c r="CR39" s="42"/>
     </row>
@@ -22069,13 +22128,13 @@
         <v>1699</v>
       </c>
       <c r="CO41" s="12" t="s">
-        <v>2634</v>
+        <v>2633</v>
       </c>
       <c r="CP41" s="56" t="s">
         <v>2280</v>
       </c>
       <c r="CQ41" s="12" t="s">
-        <v>2635</v>
+        <v>2634</v>
       </c>
       <c r="CR41" s="42"/>
     </row>
@@ -22161,13 +22220,13 @@
         <v>1687</v>
       </c>
       <c r="CO43" s="12" t="s">
-        <v>2636</v>
+        <v>2635</v>
       </c>
       <c r="CP43" s="56" t="s">
         <v>2280</v>
       </c>
       <c r="CQ43" s="12" t="s">
-        <v>2637</v>
+        <v>2636</v>
       </c>
       <c r="CR43" s="42"/>
     </row>
@@ -22256,13 +22315,13 @@
       <c r="CM45" s="23"/>
       <c r="CN45" s="23"/>
       <c r="CO45" s="12" t="s">
-        <v>2638</v>
+        <v>2637</v>
       </c>
       <c r="CP45" s="56" t="s">
         <v>2280</v>
       </c>
       <c r="CQ45" s="12" t="s">
-        <v>2639</v>
+        <v>2638</v>
       </c>
       <c r="CR45" s="42"/>
     </row>
@@ -22349,13 +22408,13 @@
       <c r="CM47" s="23"/>
       <c r="CN47" s="23"/>
       <c r="CO47" s="12" t="s">
-        <v>2640</v>
+        <v>2639</v>
       </c>
       <c r="CP47" s="56" t="s">
         <v>2280</v>
       </c>
       <c r="CQ47" s="12" t="s">
-        <v>2641</v>
+        <v>2640</v>
       </c>
       <c r="CR47" s="42"/>
     </row>
@@ -22441,13 +22500,13 @@
       <c r="CM49" s="23"/>
       <c r="CN49" s="23"/>
       <c r="CO49" s="12" t="s">
-        <v>2642</v>
+        <v>2641</v>
       </c>
       <c r="CP49" s="56" t="s">
         <v>2280</v>
       </c>
       <c r="CQ49" s="12" t="s">
-        <v>2643</v>
+        <v>2642</v>
       </c>
       <c r="CR49" s="42"/>
     </row>
@@ -22535,13 +22594,13 @@
       <c r="CM51" s="23"/>
       <c r="CN51" s="23"/>
       <c r="CO51" s="12" t="s">
-        <v>2644</v>
+        <v>2643</v>
       </c>
       <c r="CP51" s="56" t="s">
         <v>2280</v>
       </c>
       <c r="CQ51" s="12" t="s">
-        <v>2645</v>
+        <v>2644</v>
       </c>
       <c r="CR51" s="42"/>
     </row>
@@ -22628,13 +22687,13 @@
       <c r="CM53" s="23"/>
       <c r="CN53" s="23"/>
       <c r="CO53" s="12" t="s">
-        <v>2646</v>
+        <v>2645</v>
       </c>
       <c r="CP53" s="56" t="s">
         <v>2280</v>
       </c>
       <c r="CQ53" s="12" t="s">
-        <v>2647</v>
+        <v>2646</v>
       </c>
       <c r="CR53" s="42"/>
     </row>
@@ -22718,13 +22777,13 @@
       </c>
       <c r="CL55" s="23"/>
       <c r="CO55" s="12" t="s">
-        <v>2648</v>
+        <v>2647</v>
       </c>
       <c r="CP55" s="56" t="s">
         <v>2280</v>
       </c>
       <c r="CQ55" s="12" t="s">
-        <v>2649</v>
+        <v>2648</v>
       </c>
       <c r="CR55" s="42"/>
     </row>
@@ -22807,13 +22866,13 @@
         <v>1682</v>
       </c>
       <c r="CO57" s="12" t="s">
-        <v>2650</v>
+        <v>2649</v>
       </c>
       <c r="CP57" s="56" t="s">
         <v>2280</v>
       </c>
       <c r="CQ57" s="12" t="s">
-        <v>2651</v>
+        <v>2650</v>
       </c>
       <c r="CR57" s="42"/>
     </row>
@@ -22892,13 +22951,13 @@
         <v>1658</v>
       </c>
       <c r="CO59" s="12" t="s">
-        <v>2652</v>
+        <v>2651</v>
       </c>
       <c r="CP59" s="56" t="s">
         <v>2280</v>
       </c>
       <c r="CQ59" s="12" t="s">
-        <v>2653</v>
+        <v>2652</v>
       </c>
       <c r="CR59" s="42"/>
     </row>
@@ -22974,13 +23033,13 @@
         <v>1673</v>
       </c>
       <c r="CO61" s="12" t="s">
-        <v>2654</v>
+        <v>2653</v>
       </c>
       <c r="CP61" s="56" t="s">
         <v>2280</v>
       </c>
       <c r="CQ61" s="12" t="s">
-        <v>2655</v>
+        <v>2654</v>
       </c>
       <c r="CR61" s="42"/>
     </row>
@@ -23056,13 +23115,13 @@
         <v>1671</v>
       </c>
       <c r="CO63" s="12" t="s">
-        <v>2656</v>
+        <v>2655</v>
       </c>
       <c r="CP63" s="56" t="s">
         <v>2280</v>
       </c>
       <c r="CQ63" s="12" t="s">
-        <v>2657</v>
+        <v>2656</v>
       </c>
       <c r="CR63" s="42"/>
     </row>
@@ -23132,13 +23191,13 @@
         <v>1649</v>
       </c>
       <c r="CO65" s="12" t="s">
-        <v>2658</v>
+        <v>2657</v>
       </c>
       <c r="CP65" s="56" t="s">
         <v>2280</v>
       </c>
       <c r="CQ65" s="12" t="s">
-        <v>2659</v>
+        <v>2658</v>
       </c>
       <c r="CR65" s="42"/>
     </row>
@@ -23208,13 +23267,13 @@
         <v>1674</v>
       </c>
       <c r="CO67" s="12" t="s">
-        <v>2660</v>
+        <v>2659</v>
       </c>
       <c r="CP67" s="56" t="s">
         <v>2280</v>
       </c>
       <c r="CQ67" s="12" t="s">
-        <v>2661</v>
+        <v>2660</v>
       </c>
       <c r="CR67" s="42"/>
     </row>
@@ -23283,13 +23342,13 @@
         <v>1982</v>
       </c>
       <c r="CO69" s="12" t="s">
-        <v>2662</v>
+        <v>2661</v>
       </c>
       <c r="CP69" s="56" t="s">
         <v>2280</v>
       </c>
       <c r="CQ69" s="12" t="s">
-        <v>2663</v>
+        <v>2662</v>
       </c>
       <c r="CR69" s="42"/>
     </row>
@@ -23359,13 +23418,13 @@
         <v>1670</v>
       </c>
       <c r="CO71" s="12" t="s">
-        <v>2664</v>
+        <v>2663</v>
       </c>
       <c r="CP71" s="56" t="s">
         <v>2280</v>
       </c>
       <c r="CQ71" s="12" t="s">
-        <v>2665</v>
+        <v>2664</v>
       </c>
       <c r="CR71" s="42"/>
     </row>
@@ -23435,13 +23494,13 @@
         <v>1696</v>
       </c>
       <c r="CO73" s="12" t="s">
-        <v>2666</v>
+        <v>2665</v>
       </c>
       <c r="CP73" s="56" t="s">
         <v>2280</v>
       </c>
       <c r="CQ73" s="12" t="s">
-        <v>2667</v>
+        <v>2666</v>
       </c>
       <c r="CR73" s="42"/>
     </row>
@@ -23511,13 +23570,13 @@
         <v>1697</v>
       </c>
       <c r="CO75" s="12" t="s">
-        <v>2668</v>
+        <v>2667</v>
       </c>
       <c r="CP75" s="56" t="s">
         <v>2280</v>
       </c>
       <c r="CQ75" s="12" t="s">
-        <v>2669</v>
+        <v>2668</v>
       </c>
       <c r="CR75" s="42"/>
     </row>
@@ -23587,13 +23646,13 @@
         <v>1647</v>
       </c>
       <c r="CO77" s="12" t="s">
-        <v>2670</v>
+        <v>2669</v>
       </c>
       <c r="CP77" s="56" t="s">
         <v>2280</v>
       </c>
       <c r="CQ77" s="12" t="s">
-        <v>2669</v>
+        <v>2668</v>
       </c>
       <c r="CR77" s="42"/>
     </row>
@@ -23663,13 +23722,13 @@
         <v>1648</v>
       </c>
       <c r="CO79" s="12" t="s">
-        <v>2671</v>
+        <v>2670</v>
       </c>
       <c r="CP79" s="56" t="s">
         <v>2280</v>
       </c>
       <c r="CQ79" s="12" t="s">
-        <v>2672</v>
+        <v>2671</v>
       </c>
       <c r="CR79" s="42"/>
     </row>
@@ -23739,13 +23798,13 @@
         <v>1690</v>
       </c>
       <c r="CO81" s="12" t="s">
-        <v>2673</v>
+        <v>2672</v>
       </c>
       <c r="CP81" s="56" t="s">
         <v>2280</v>
       </c>
       <c r="CQ81" s="12" t="s">
-        <v>2672</v>
+        <v>2671</v>
       </c>
       <c r="CR81" s="42"/>
     </row>
@@ -23815,13 +23874,13 @@
         <v>1749</v>
       </c>
       <c r="CO83" s="12" t="s">
-        <v>2674</v>
+        <v>2673</v>
       </c>
       <c r="CP83" s="56" t="s">
         <v>2280</v>
       </c>
       <c r="CQ83" s="12" t="s">
-        <v>2672</v>
+        <v>2671</v>
       </c>
       <c r="CR83" s="42"/>
     </row>
@@ -23890,13 +23949,13 @@
         <v>1656</v>
       </c>
       <c r="CO85" s="12" t="s">
-        <v>2675</v>
+        <v>2674</v>
       </c>
       <c r="CP85" s="56" t="s">
         <v>2280</v>
       </c>
       <c r="CQ85" s="12" t="s">
-        <v>2676</v>
+        <v>2675</v>
       </c>
       <c r="CR85" s="42"/>
     </row>
@@ -23964,13 +24023,13 @@
         <v>1985</v>
       </c>
       <c r="CO87" s="12" t="s">
-        <v>2677</v>
+        <v>2676</v>
       </c>
       <c r="CP87" s="56" t="s">
         <v>2280</v>
       </c>
       <c r="CQ87" s="12" t="s">
-        <v>2678</v>
+        <v>2677</v>
       </c>
       <c r="CR87" s="42"/>
     </row>
@@ -24038,13 +24097,13 @@
         <v>1744</v>
       </c>
       <c r="CO89" s="12" t="s">
-        <v>2679</v>
+        <v>2678</v>
       </c>
       <c r="CP89" s="56" t="s">
         <v>2280</v>
       </c>
       <c r="CQ89" s="12" t="s">
-        <v>2680</v>
+        <v>2679</v>
       </c>
       <c r="CR89" s="42"/>
     </row>
@@ -24112,13 +24171,13 @@
         <v>1986</v>
       </c>
       <c r="CO91" s="12" t="s">
-        <v>2681</v>
+        <v>2680</v>
       </c>
       <c r="CP91" s="56" t="s">
         <v>2280</v>
       </c>
       <c r="CQ91" s="12" t="s">
-        <v>2682</v>
+        <v>2681</v>
       </c>
       <c r="CR91" s="42"/>
     </row>
@@ -24186,13 +24245,13 @@
         <v>1987</v>
       </c>
       <c r="CO93" s="12" t="s">
-        <v>2683</v>
+        <v>2682</v>
       </c>
       <c r="CP93" s="56" t="s">
         <v>2280</v>
       </c>
       <c r="CQ93" s="12" t="s">
-        <v>2684</v>
+        <v>2683</v>
       </c>
       <c r="CR93" s="42"/>
     </row>
@@ -24260,13 +24319,13 @@
         <v>1989</v>
       </c>
       <c r="CO95" s="12" t="s">
-        <v>2685</v>
+        <v>2684</v>
       </c>
       <c r="CP95" s="56" t="s">
         <v>2280</v>
       </c>
       <c r="CQ95" s="12" t="s">
-        <v>2686</v>
+        <v>2685</v>
       </c>
       <c r="CR95" s="42"/>
     </row>
@@ -24334,13 +24393,13 @@
         <v>1990</v>
       </c>
       <c r="CO97" s="12" t="s">
-        <v>2687</v>
+        <v>2686</v>
       </c>
       <c r="CP97" s="56" t="s">
         <v>2280</v>
       </c>
       <c r="CQ97" s="12" t="s">
-        <v>2688</v>
+        <v>2687</v>
       </c>
       <c r="CR97" s="42"/>
     </row>
@@ -24368,7 +24427,7 @@
         <v>1560</v>
       </c>
       <c r="BC98" s="7" t="s">
-        <v>2708</v>
+        <v>2707</v>
       </c>
       <c r="CO98" s="12" t="s">
         <v>2168</v>
@@ -24406,13 +24465,13 @@
       </c>
       <c r="BC99" s="7"/>
       <c r="CO99" s="12" t="s">
-        <v>2689</v>
+        <v>2688</v>
       </c>
       <c r="CP99" s="56" t="s">
         <v>2280</v>
       </c>
       <c r="CQ99" s="12" t="s">
-        <v>2690</v>
+        <v>2689</v>
       </c>
       <c r="CR99" s="42"/>
     </row>
@@ -24474,13 +24533,13 @@
         <v>1562</v>
       </c>
       <c r="CO101" s="12" t="s">
-        <v>2691</v>
+        <v>2690</v>
       </c>
       <c r="CP101" s="56" t="s">
         <v>2280</v>
       </c>
       <c r="CQ101" s="12" t="s">
-        <v>2692</v>
+        <v>2691</v>
       </c>
       <c r="CR101" s="42"/>
     </row>
@@ -24542,13 +24601,13 @@
         <v>1564</v>
       </c>
       <c r="CO103" s="12" t="s">
-        <v>2693</v>
+        <v>2692</v>
       </c>
       <c r="CP103" s="56" t="s">
         <v>2280</v>
       </c>
       <c r="CQ103" s="12" t="s">
-        <v>2694</v>
+        <v>2693</v>
       </c>
       <c r="CR103" s="42"/>
     </row>
@@ -24610,13 +24669,13 @@
         <v>1566</v>
       </c>
       <c r="CO105" s="12" t="s">
-        <v>2695</v>
+        <v>2694</v>
       </c>
       <c r="CP105" s="56" t="s">
         <v>2280</v>
       </c>
       <c r="CQ105" s="12" t="s">
-        <v>2696</v>
+        <v>2695</v>
       </c>
       <c r="CR105" s="42"/>
     </row>
@@ -24678,13 +24737,13 @@
         <v>2008</v>
       </c>
       <c r="CO107" s="12" t="s">
-        <v>2697</v>
+        <v>2696</v>
       </c>
       <c r="CP107" s="56" t="s">
         <v>2280</v>
       </c>
       <c r="CQ107" s="12" t="s">
-        <v>2698</v>
+        <v>2697</v>
       </c>
       <c r="CR107" s="42"/>
     </row>
@@ -24746,13 +24805,13 @@
         <v>1569</v>
       </c>
       <c r="CO109" s="12" t="s">
-        <v>2699</v>
+        <v>2698</v>
       </c>
       <c r="CP109" s="56" t="s">
         <v>2280</v>
       </c>
       <c r="CQ109" s="12" t="s">
-        <v>2700</v>
+        <v>2699</v>
       </c>
       <c r="CR109" s="42"/>
     </row>
@@ -24814,13 +24873,13 @@
         <v>1570</v>
       </c>
       <c r="CO111" s="12" t="s">
-        <v>2701</v>
+        <v>2700</v>
       </c>
       <c r="CP111" s="56" t="s">
         <v>2280</v>
       </c>
       <c r="CQ111" s="12" t="s">
-        <v>2702</v>
+        <v>2701</v>
       </c>
       <c r="CR111" s="42"/>
     </row>
@@ -24882,13 +24941,13 @@
         <v>2010</v>
       </c>
       <c r="CO113" s="12" t="s">
-        <v>2703</v>
+        <v>2702</v>
       </c>
       <c r="CP113" s="56" t="s">
         <v>2280</v>
       </c>
       <c r="CQ113" s="12" t="s">
-        <v>2704</v>
+        <v>2703</v>
       </c>
       <c r="CR113" s="42"/>
     </row>
@@ -24950,13 +25009,13 @@
         <v>1572</v>
       </c>
       <c r="CO115" s="12" t="s">
-        <v>2705</v>
+        <v>2704</v>
       </c>
       <c r="CP115" s="56" t="s">
         <v>2280</v>
       </c>
       <c r="CQ115" s="12" t="s">
-        <v>2706</v>
+        <v>2705</v>
       </c>
       <c r="CR115" s="42"/>
     </row>
@@ -27195,7 +27254,7 @@
       <c r="CR277" s="42"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="56VpJFlsCUD1jco12mk1zESojs9cfiGy6+5iKH9uHy7/MUErMXsbvVbH+WGzvIvCwYP78FQndyXwUvsA+bjWzg==" saltValue="NbD8jnfYohH4RciOSIpiaA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="Nui/WFCkAiM0/CddZH2BeeUckAlyyX+waYESgZQHD7xExq5G73EzJ3ahN5CGEk6uA54E7XlFhpXYP2dxa/xdDA==" saltValue="BSqL34JuvMRNPmhdLprQJQ==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="2">
     <mergeCell ref="M27:M28"/>
     <mergeCell ref="M34:M35"/>

</xml_diff>

<commit_message>
Added sample_dating drop-down menu
</commit_message>
<xml_diff>
--- a/Excel_templates/MOSAIC_input_excel_file_2022.xlsx
+++ b/Excel_templates/MOSAIC_input_excel_file_2022.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sparadis\Documents\ETH\MOSAIC\MOSAIC_Client\Excel_templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8E5B34D-AA46-4320-BD7D-F6E37488DB42}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{227AE783-FB6A-439A-B7DA-7324C301B1BC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30204" yWindow="10044" windowWidth="40020" windowHeight="22296" tabRatio="694" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30204" yWindow="10044" windowWidth="40020" windowHeight="22296" tabRatio="694" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ARTICLE_AUTHOR" sheetId="3" r:id="rId1"/>
@@ -49,7 +49,7 @@
     <definedName name="core_sedimentation_rate">SET_VARIABLES!#REF!</definedName>
     <definedName name="Cs137_Bq_kg">SET_VARIABLES!$FX$2:$FX$4</definedName>
     <definedName name="cumulative_dry_mass_g_cm2">SET_VARIABLES!$FA$2:$FA$4</definedName>
-    <definedName name="dating_year">SET_VARIABLES!$FB$2:$FB$8</definedName>
+    <definedName name="dating_year">SET_VARIABLES!$FB$2:$FB$9</definedName>
     <definedName name="Delta_13C">SET_VARIABLES!$FS$2:$FS$4</definedName>
     <definedName name="Delta_14C">SET_VARIABLES!$FP$2:$FP$4</definedName>
     <definedName name="Delta_15N">SET_VARIABLES!$FU$2:$FU$4</definedName>
@@ -124,6 +124,7 @@
     <definedName name="sample_biomarkers_CuO_grouped">SET_VARIABLES!$CL$2:$CL$37</definedName>
     <definedName name="sample_black_carbon">SET_VARIABLES!$DM$2:$DM$5</definedName>
     <definedName name="Sample_composition">SET_VARIABLES!$BW$2:$BW$29</definedName>
+    <definedName name="sample_dating">SET_VARIABLES!$DS$2:$DS$3</definedName>
     <definedName name="sample_fatty_acids">SET_VARIABLES!$DA$2:$DA$6</definedName>
     <definedName name="Sample_isotopes">SET_VARIABLES!$CC$2:$CC$16</definedName>
     <definedName name="sample_macronutrients">SET_VARIABLES!$CF$2:$CF$16</definedName>
@@ -192,7 +193,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3733" uniqueCount="2913">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3732" uniqueCount="2911">
   <si>
     <t>sample_name</t>
   </si>
@@ -8558,13 +8559,7 @@
     <t>Concentration of smectite or montmorillonite in the sediment sample</t>
   </si>
   <si>
-    <t>dating_method</t>
-  </si>
-  <si>
     <t>calendar year</t>
-  </si>
-  <si>
-    <t>Dating method used to obtain the age of the sample section</t>
   </si>
   <si>
     <t>sample_neodynium</t>
@@ -9404,7 +9399,7 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="113">
+  <cellXfs count="114">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="13" applyFont="1" applyFill="1" applyAlignment="1"/>
@@ -9535,6 +9530,7 @@
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="4" borderId="4" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
@@ -9964,7 +9960,7 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -9985,15 +9981,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="59" customFormat="1" ht="20.399999999999999" thickBot="1">
-      <c r="A1" s="85" t="s">
+      <c r="A1" s="86" t="s">
         <v>2577</v>
       </c>
-      <c r="B1" s="85"/>
-      <c r="C1" s="85"/>
-      <c r="D1" s="85"/>
-      <c r="E1" s="85"/>
-      <c r="F1" s="85"/>
-      <c r="G1" s="85"/>
+      <c r="B1" s="86"/>
+      <c r="C1" s="86"/>
+      <c r="D1" s="86"/>
+      <c r="E1" s="86"/>
+      <c r="F1" s="86"/>
+      <c r="G1" s="86"/>
     </row>
     <row r="2" spans="1:8" s="26" customFormat="1">
       <c r="A2" s="49" t="s">
@@ -10083,26 +10079,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" s="58" customFormat="1" ht="20.399999999999999" thickBot="1">
-      <c r="A1" s="87" t="s">
+      <c r="A1" s="88" t="s">
         <v>2578</v>
       </c>
-      <c r="B1" s="87"/>
-      <c r="C1" s="87"/>
-      <c r="D1" s="87"/>
-      <c r="E1" s="87"/>
-      <c r="F1" s="86" t="s">
+      <c r="B1" s="88"/>
+      <c r="C1" s="88"/>
+      <c r="D1" s="88"/>
+      <c r="E1" s="88"/>
+      <c r="F1" s="87" t="s">
         <v>2716</v>
       </c>
-      <c r="G1" s="86"/>
-      <c r="H1" s="86"/>
-      <c r="I1" s="86"/>
-      <c r="J1" s="86"/>
-      <c r="K1" s="86"/>
-      <c r="L1" s="86"/>
-      <c r="M1" s="86"/>
-      <c r="N1" s="86"/>
-      <c r="O1" s="86"/>
-      <c r="P1" s="86"/>
+      <c r="G1" s="87"/>
+      <c r="H1" s="87"/>
+      <c r="I1" s="87"/>
+      <c r="J1" s="87"/>
+      <c r="K1" s="87"/>
+      <c r="L1" s="87"/>
+      <c r="M1" s="87"/>
+      <c r="N1" s="87"/>
+      <c r="O1" s="87"/>
+      <c r="P1" s="87"/>
     </row>
     <row r="2" spans="1:16" s="61" customFormat="1">
       <c r="A2" s="57" t="s">
@@ -10118,7 +10114,7 @@
         <v>1824</v>
       </c>
       <c r="E2" s="57" t="s">
-        <v>2903</v>
+        <v>2901</v>
       </c>
       <c r="F2" s="60" t="s">
         <v>1825</v>
@@ -10347,37 +10343,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:35" s="50" customFormat="1" ht="20.399999999999999" thickBot="1">
-      <c r="A1" s="88" t="s">
+      <c r="A1" s="89" t="s">
         <v>2580</v>
       </c>
-      <c r="B1" s="88"/>
-      <c r="C1" s="88" t="s">
+      <c r="B1" s="89"/>
+      <c r="C1" s="89" t="s">
         <v>2579</v>
       </c>
-      <c r="D1" s="88"/>
-      <c r="E1" s="88"/>
-      <c r="F1" s="88"/>
+      <c r="D1" s="89"/>
+      <c r="E1" s="89"/>
+      <c r="F1" s="89"/>
       <c r="G1" s="50" t="s">
         <v>2183</v>
       </c>
     </row>
     <row r="2" spans="1:35" ht="15.6" customHeight="1" thickTop="1">
-      <c r="A2" s="89" t="s">
+      <c r="A2" s="90" t="s">
         <v>2510</v>
       </c>
-      <c r="B2" s="89" t="s">
+      <c r="B2" s="90" t="s">
         <v>1822</v>
       </c>
-      <c r="C2" s="89" t="s">
+      <c r="C2" s="90" t="s">
         <v>1831</v>
       </c>
-      <c r="D2" s="89" t="s">
+      <c r="D2" s="90" t="s">
         <v>2587</v>
       </c>
-      <c r="E2" s="89" t="s">
+      <c r="E2" s="90" t="s">
         <v>1820</v>
       </c>
-      <c r="F2" s="92" t="s">
+      <c r="F2" s="93" t="s">
         <v>1821</v>
       </c>
       <c r="G2" s="51" t="s">
@@ -10413,12 +10409,12 @@
       <c r="AI2" s="51"/>
     </row>
     <row r="3" spans="1:35" ht="15.6" customHeight="1">
-      <c r="A3" s="90"/>
-      <c r="B3" s="90"/>
-      <c r="C3" s="90"/>
-      <c r="D3" s="90"/>
-      <c r="E3" s="90"/>
-      <c r="F3" s="93"/>
+      <c r="A3" s="91"/>
+      <c r="B3" s="91"/>
+      <c r="C3" s="91"/>
+      <c r="D3" s="91"/>
+      <c r="E3" s="91"/>
+      <c r="F3" s="94"/>
       <c r="G3" s="51"/>
       <c r="H3" s="51"/>
       <c r="I3" s="51"/>
@@ -10450,12 +10446,12 @@
       <c r="AI3" s="51"/>
     </row>
     <row r="4" spans="1:35" ht="15.6" customHeight="1">
-      <c r="A4" s="90"/>
-      <c r="B4" s="90"/>
-      <c r="C4" s="90"/>
-      <c r="D4" s="90"/>
-      <c r="E4" s="90"/>
-      <c r="F4" s="93"/>
+      <c r="A4" s="91"/>
+      <c r="B4" s="91"/>
+      <c r="C4" s="91"/>
+      <c r="D4" s="91"/>
+      <c r="E4" s="91"/>
+      <c r="F4" s="94"/>
       <c r="G4" s="51"/>
       <c r="H4" s="51"/>
       <c r="I4" s="51"/>
@@ -10487,12 +10483,12 @@
       <c r="AI4" s="51"/>
     </row>
     <row r="5" spans="1:35" ht="15.6" customHeight="1">
-      <c r="A5" s="91"/>
-      <c r="B5" s="91"/>
-      <c r="C5" s="91"/>
-      <c r="D5" s="91"/>
-      <c r="E5" s="91"/>
-      <c r="F5" s="93"/>
+      <c r="A5" s="92"/>
+      <c r="B5" s="92"/>
+      <c r="C5" s="92"/>
+      <c r="D5" s="92"/>
+      <c r="E5" s="92"/>
+      <c r="F5" s="94"/>
       <c r="G5" s="51"/>
       <c r="H5" s="51"/>
       <c r="I5" s="51"/>
@@ -10524,12 +10520,12 @@
       <c r="AI5" s="51"/>
     </row>
     <row r="6" spans="1:35" ht="15.6" customHeight="1">
-      <c r="A6" s="91"/>
-      <c r="B6" s="91"/>
-      <c r="C6" s="91"/>
-      <c r="D6" s="91"/>
-      <c r="E6" s="91"/>
-      <c r="F6" s="93"/>
+      <c r="A6" s="92"/>
+      <c r="B6" s="92"/>
+      <c r="C6" s="92"/>
+      <c r="D6" s="92"/>
+      <c r="E6" s="92"/>
+      <c r="F6" s="94"/>
       <c r="G6" s="51"/>
       <c r="H6" s="51"/>
       <c r="I6" s="51"/>
@@ -11825,11 +11821,11 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:CB52"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane xSplit="3" ySplit="6" topLeftCell="D7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="A7" sqref="A7"/>
+      <selection pane="bottomRight" activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15" defaultRowHeight="15.6"/>
@@ -11850,25 +11846,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:80" s="74" customFormat="1" ht="20.399999999999999" customHeight="1" thickBot="1">
-      <c r="A1" s="94" t="s">
+      <c r="A1" s="95" t="s">
         <v>2589</v>
       </c>
-      <c r="B1" s="95"/>
-      <c r="C1" s="96"/>
-      <c r="D1" s="94" t="s">
+      <c r="B1" s="96"/>
+      <c r="C1" s="97"/>
+      <c r="D1" s="95" t="s">
         <v>2579</v>
       </c>
-      <c r="E1" s="95"/>
-      <c r="F1" s="95"/>
-      <c r="G1" s="96"/>
-      <c r="H1" s="97" t="s">
+      <c r="E1" s="96"/>
+      <c r="F1" s="96"/>
+      <c r="G1" s="97"/>
+      <c r="H1" s="98" t="s">
         <v>2581</v>
       </c>
-      <c r="I1" s="98"/>
-      <c r="J1" s="98"/>
-      <c r="K1" s="99"/>
+      <c r="I1" s="99"/>
+      <c r="J1" s="99"/>
+      <c r="K1" s="100"/>
       <c r="L1" s="74" t="s">
-        <v>2472</v>
+        <v>2778</v>
       </c>
       <c r="M1" s="74" t="s">
         <v>1837</v>
@@ -11877,57 +11873,57 @@
         <v>1838</v>
       </c>
       <c r="O1" s="74" t="s">
-        <v>2791</v>
+        <v>2789</v>
       </c>
       <c r="P1" s="74" t="s">
-        <v>2846</v>
+        <v>2844</v>
       </c>
     </row>
     <row r="2" spans="1:80" s="76" customFormat="1">
-      <c r="A2" s="100" t="s">
+      <c r="A2" s="101" t="s">
         <v>2510</v>
       </c>
-      <c r="B2" s="103" t="s">
+      <c r="B2" s="104" t="s">
         <v>1822</v>
       </c>
-      <c r="C2" s="106" t="s">
+      <c r="C2" s="107" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="101" t="s">
+      <c r="D2" s="102" t="s">
         <v>1831</v>
       </c>
-      <c r="E2" s="104" t="s">
+      <c r="E2" s="105" t="s">
         <v>2587</v>
       </c>
-      <c r="F2" s="104" t="s">
+      <c r="F2" s="105" t="s">
         <v>1820</v>
       </c>
-      <c r="G2" s="107" t="s">
+      <c r="G2" s="108" t="s">
         <v>1821</v>
       </c>
-      <c r="H2" s="100" t="s">
+      <c r="H2" s="101" t="s">
         <v>1832</v>
       </c>
-      <c r="I2" s="103" t="s">
+      <c r="I2" s="104" t="s">
         <v>1833</v>
       </c>
-      <c r="J2" s="103" t="s">
+      <c r="J2" s="104" t="s">
         <v>1834</v>
       </c>
-      <c r="K2" s="109" t="s">
+      <c r="K2" s="110" t="s">
         <v>1835</v>
       </c>
       <c r="L2" s="75" t="s">
-        <v>2473</v>
+        <v>2123</v>
       </c>
       <c r="M2" s="75" t="s">
-        <v>2177</v>
+        <v>1</v>
       </c>
       <c r="N2" s="75" t="s">
         <v>1840</v>
       </c>
       <c r="O2" s="75" t="s">
-        <v>2793</v>
+        <v>2791</v>
       </c>
       <c r="P2" s="75" t="s">
         <v>2708</v>
@@ -11997,22 +11993,24 @@
       <c r="CA2" s="75"/>
       <c r="CB2" s="75"/>
     </row>
-    <row r="3" spans="1:80" s="76" customFormat="1">
-      <c r="A3" s="101"/>
-      <c r="B3" s="104"/>
-      <c r="C3" s="107"/>
-      <c r="D3" s="101"/>
-      <c r="E3" s="104"/>
-      <c r="F3" s="104"/>
-      <c r="G3" s="107"/>
-      <c r="H3" s="101"/>
-      <c r="I3" s="104"/>
-      <c r="J3" s="104"/>
-      <c r="K3" s="110"/>
+    <row r="3" spans="1:80" s="76" customFormat="1" ht="31.2">
+      <c r="A3" s="102"/>
+      <c r="B3" s="105"/>
+      <c r="C3" s="108"/>
+      <c r="D3" s="102"/>
+      <c r="E3" s="105"/>
+      <c r="F3" s="105"/>
+      <c r="G3" s="108"/>
+      <c r="H3" s="102"/>
+      <c r="I3" s="105"/>
+      <c r="J3" s="105"/>
+      <c r="K3" s="111"/>
       <c r="L3" s="75" t="s">
-        <v>5</v>
-      </c>
-      <c r="M3" s="75"/>
+        <v>2867</v>
+      </c>
+      <c r="M3" s="75" t="s">
+        <v>2871</v>
+      </c>
       <c r="N3" s="75"/>
       <c r="O3" s="75"/>
       <c r="P3" s="75"/>
@@ -12082,17 +12080,17 @@
       <c r="CB3" s="75"/>
     </row>
     <row r="4" spans="1:80" s="76" customFormat="1">
-      <c r="A4" s="101"/>
-      <c r="B4" s="104"/>
-      <c r="C4" s="107"/>
-      <c r="D4" s="101"/>
-      <c r="E4" s="104"/>
-      <c r="F4" s="104"/>
-      <c r="G4" s="107"/>
-      <c r="H4" s="101"/>
-      <c r="I4" s="104"/>
-      <c r="J4" s="104"/>
-      <c r="K4" s="110"/>
+      <c r="A4" s="102"/>
+      <c r="B4" s="105"/>
+      <c r="C4" s="108"/>
+      <c r="D4" s="102"/>
+      <c r="E4" s="105"/>
+      <c r="F4" s="105"/>
+      <c r="G4" s="108"/>
+      <c r="H4" s="102"/>
+      <c r="I4" s="105"/>
+      <c r="J4" s="105"/>
+      <c r="K4" s="111"/>
       <c r="L4" s="75"/>
       <c r="M4" s="75"/>
       <c r="N4" s="75"/>
@@ -12164,17 +12162,17 @@
       <c r="CB4" s="75"/>
     </row>
     <row r="5" spans="1:80" s="76" customFormat="1">
-      <c r="A5" s="101"/>
-      <c r="B5" s="104"/>
-      <c r="C5" s="107"/>
-      <c r="D5" s="101"/>
-      <c r="E5" s="104"/>
-      <c r="F5" s="104"/>
-      <c r="G5" s="107"/>
-      <c r="H5" s="101"/>
-      <c r="I5" s="104"/>
-      <c r="J5" s="104"/>
-      <c r="K5" s="110"/>
+      <c r="A5" s="102"/>
+      <c r="B5" s="105"/>
+      <c r="C5" s="108"/>
+      <c r="D5" s="102"/>
+      <c r="E5" s="105"/>
+      <c r="F5" s="105"/>
+      <c r="G5" s="108"/>
+      <c r="H5" s="102"/>
+      <c r="I5" s="105"/>
+      <c r="J5" s="105"/>
+      <c r="K5" s="111"/>
       <c r="L5" s="75"/>
       <c r="M5" s="75"/>
       <c r="N5" s="75"/>
@@ -12246,17 +12244,17 @@
       <c r="CB5" s="75"/>
     </row>
     <row r="6" spans="1:80" s="76" customFormat="1" ht="16.2" thickBot="1">
-      <c r="A6" s="102"/>
-      <c r="B6" s="105"/>
-      <c r="C6" s="108"/>
-      <c r="D6" s="102"/>
-      <c r="E6" s="105"/>
-      <c r="F6" s="105"/>
-      <c r="G6" s="108"/>
-      <c r="H6" s="102"/>
-      <c r="I6" s="105"/>
-      <c r="J6" s="105"/>
-      <c r="K6" s="111"/>
+      <c r="A6" s="103"/>
+      <c r="B6" s="106"/>
+      <c r="C6" s="109"/>
+      <c r="D6" s="103"/>
+      <c r="E6" s="106"/>
+      <c r="F6" s="106"/>
+      <c r="G6" s="109"/>
+      <c r="H6" s="103"/>
+      <c r="I6" s="106"/>
+      <c r="J6" s="106"/>
+      <c r="K6" s="112"/>
       <c r="L6" s="75"/>
       <c r="M6" s="75"/>
       <c r="N6" s="75"/>
@@ -14558,10 +14556,10 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr codeName="Sheet6"/>
-  <dimension ref="A1:GX277"/>
+  <dimension ref="A1:GZ277"/>
   <sheetViews>
-    <sheetView topLeftCell="GE1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="GM18" sqref="GM18"/>
+    <sheetView topLeftCell="EQ1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="FA21" sqref="FA21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -14616,7 +14614,7 @@
     <col min="187" max="188" width="21.3984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:206" s="1" customFormat="1">
+    <row r="1" spans="1:208" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -14786,7 +14784,7 @@
         <v>1143</v>
       </c>
       <c r="BE1" s="1" t="s">
-        <v>2812</v>
+        <v>2810</v>
       </c>
       <c r="BF1" s="15" t="s">
         <v>1848</v>
@@ -15035,7 +15033,7 @@
         <v>sample_dating_description</v>
       </c>
       <c r="DV1" s="9" t="s">
-        <v>2791</v>
+        <v>2789</v>
       </c>
       <c r="DW1" s="9" t="str">
         <f>_xlfn.CONCAT(DV1,"_units")</f>
@@ -15046,7 +15044,7 @@
         <v>sample_neodynium_description</v>
       </c>
       <c r="DY1" s="9" t="s">
-        <v>2796</v>
+        <v>2794</v>
       </c>
       <c r="DZ1" s="9" t="str">
         <f>_xlfn.CONCAT(DY1,"_units")</f>
@@ -15057,7 +15055,7 @@
         <v>sample_strontium_description</v>
       </c>
       <c r="EB1" s="1" t="s">
-        <v>2846</v>
+        <v>2844</v>
       </c>
       <c r="EC1" s="9" t="str">
         <f>_xlfn.CONCAT(EB1,"_units")</f>
@@ -15077,7 +15075,7 @@
         <v>1754</v>
       </c>
       <c r="EH1" s="1" t="s">
-        <v>2847</v>
+        <v>2845</v>
       </c>
       <c r="EI1" s="9" t="str">
         <f>_xlfn.CONCAT(EH1,"_units")</f>
@@ -15091,7 +15089,7 @@
         <v>1753</v>
       </c>
       <c r="EL1" s="80" t="s">
-        <v>2850</v>
+        <v>2848</v>
       </c>
       <c r="EM1" s="1" t="s">
         <v>2048</v>
@@ -15115,10 +15113,10 @@
         <v>1844</v>
       </c>
       <c r="ET1" s="1" t="s">
-        <v>2807</v>
+        <v>2805</v>
       </c>
       <c r="EU1" s="1" t="s">
-        <v>2808</v>
+        <v>2806</v>
       </c>
       <c r="EV1" s="1" t="s">
         <v>1845</v>
@@ -15130,7 +15128,7 @@
         <v>2747</v>
       </c>
       <c r="EY1" s="1" t="s">
-        <v>2810</v>
+        <v>2808</v>
       </c>
       <c r="EZ1" s="1" t="s">
         <v>2058</v>
@@ -15223,7 +15221,7 @@
         <v>1790</v>
       </c>
       <c r="GD1" s="1" t="s">
-        <v>2844</v>
+        <v>2842</v>
       </c>
       <c r="GE1" s="1" t="s">
         <v>2708</v>
@@ -15274,7 +15272,7 @@
         <v>2473</v>
       </c>
       <c r="GU1" s="22" t="s">
-        <v>2910</v>
+        <v>2908</v>
       </c>
       <c r="GV1" s="22" t="s">
         <v>2463</v>
@@ -15285,8 +15283,10 @@
       <c r="GX1" s="22" t="s">
         <v>2467</v>
       </c>
-    </row>
-    <row r="2" spans="1:206">
+      <c r="GY1" s="22"/>
+      <c r="GZ1" s="22"/>
+    </row>
+    <row r="2" spans="1:208">
       <c r="A2" t="b">
         <v>1</v>
       </c>
@@ -15456,7 +15456,7 @@
         <v>5</v>
       </c>
       <c r="BE2" s="72" t="s">
-        <v>2813</v>
+        <v>2811</v>
       </c>
       <c r="BF2" s="16" t="s">
         <v>2182</v>
@@ -15612,7 +15612,7 @@
         <v>2462</v>
       </c>
       <c r="DH2" s="12" t="s">
-        <v>2909</v>
+        <v>2907</v>
       </c>
       <c r="DI2" s="12"/>
       <c r="DJ2" s="12" t="s">
@@ -15646,16 +15646,16 @@
         <v>2123</v>
       </c>
       <c r="DT2" s="12" t="s">
-        <v>2789</v>
+        <v>2788</v>
       </c>
       <c r="DU2" s="12" t="s">
         <v>2242</v>
       </c>
       <c r="DV2" s="12" t="s">
+        <v>2790</v>
+      </c>
+      <c r="DW2" s="12" t="s">
         <v>2792</v>
-      </c>
-      <c r="DW2" s="12" t="s">
-        <v>2794</v>
       </c>
       <c r="EB2" s="10" t="s">
         <v>2708</v>
@@ -15879,8 +15879,9 @@
       <c r="GX2" s="10" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:206">
+      <c r="GY2" s="10"/>
+    </row>
+    <row r="3" spans="1:208">
       <c r="A3" t="b">
         <v>0</v>
       </c>
@@ -15909,7 +15910,7 @@
         <v>19</v>
       </c>
       <c r="J3" t="s">
-        <v>2806</v>
+        <v>2804</v>
       </c>
       <c r="K3" s="34" t="s">
         <v>2064</v>
@@ -16050,7 +16051,7 @@
         <v>20</v>
       </c>
       <c r="BE3" s="72" t="s">
-        <v>2814</v>
+        <v>2812</v>
       </c>
       <c r="BF3" s="16" t="s">
         <v>2731</v>
@@ -16240,13 +16241,13 @@
         <v>2206</v>
       </c>
       <c r="DT3" s="12" t="s">
-        <v>2789</v>
+        <v>2788</v>
       </c>
       <c r="DU3" s="12" t="s">
         <v>2243</v>
       </c>
       <c r="DV3" s="12" t="s">
-        <v>2793</v>
+        <v>2791</v>
       </c>
       <c r="EB3" s="10" t="s">
         <v>2709</v>
@@ -16279,100 +16280,100 @@
         <v>2025</v>
       </c>
       <c r="EM3" t="s">
-        <v>2829</v>
+        <v>2827</v>
       </c>
       <c r="EN3" t="s">
-        <v>2860</v>
+        <v>2858</v>
       </c>
       <c r="EO3" t="s">
-        <v>2860</v>
+        <v>2858</v>
       </c>
       <c r="EP3" s="79" t="s">
-        <v>2860</v>
+        <v>2858</v>
       </c>
       <c r="EQ3" t="s">
+        <v>2859</v>
+      </c>
+      <c r="ER3" s="79" t="s">
+        <v>2859</v>
+      </c>
+      <c r="ES3" s="79" t="s">
+        <v>2859</v>
+      </c>
+      <c r="ET3" s="79" t="s">
+        <v>2859</v>
+      </c>
+      <c r="EU3" s="79" t="s">
+        <v>2859</v>
+      </c>
+      <c r="EV3" s="79" t="s">
+        <v>2859</v>
+      </c>
+      <c r="EW3" s="79" t="s">
+        <v>2859</v>
+      </c>
+      <c r="EX3" s="79" t="s">
+        <v>2859</v>
+      </c>
+      <c r="EY3" s="79" t="s">
+        <v>2859</v>
+      </c>
+      <c r="EZ3" s="79" t="s">
+        <v>2894</v>
+      </c>
+      <c r="FB3" t="s">
+        <v>2867</v>
+      </c>
+      <c r="FD3" t="s">
         <v>2861</v>
       </c>
-      <c r="ER3" s="79" t="s">
-        <v>2861</v>
-      </c>
-      <c r="ES3" s="79" t="s">
-        <v>2861</v>
-      </c>
-      <c r="ET3" s="79" t="s">
-        <v>2861</v>
-      </c>
-      <c r="EU3" s="79" t="s">
-        <v>2861</v>
-      </c>
-      <c r="EV3" s="79" t="s">
-        <v>2861</v>
-      </c>
-      <c r="EW3" s="79" t="s">
-        <v>2861</v>
-      </c>
-      <c r="EX3" s="79" t="s">
-        <v>2861</v>
-      </c>
-      <c r="EY3" s="79" t="s">
-        <v>2861</v>
-      </c>
-      <c r="EZ3" s="79" t="s">
-        <v>2896</v>
-      </c>
-      <c r="FB3" t="s">
-        <v>2869</v>
-      </c>
-      <c r="FD3" t="s">
-        <v>2863</v>
-      </c>
       <c r="FE3" t="s">
-        <v>2891</v>
+        <v>2889</v>
       </c>
       <c r="FF3" t="s">
+        <v>2871</v>
+      </c>
+      <c r="FJ3" t="s">
+        <v>2872</v>
+      </c>
+      <c r="FK3" s="79" t="s">
+        <v>2872</v>
+      </c>
+      <c r="FO3" t="s">
+        <v>2886</v>
+      </c>
+      <c r="FV3" t="s">
+        <v>2874</v>
+      </c>
+      <c r="FW3" s="79" t="s">
+        <v>2874</v>
+      </c>
+      <c r="FX3" s="79" t="s">
+        <v>2851</v>
+      </c>
+      <c r="FY3" s="79" t="s">
+        <v>2852</v>
+      </c>
+      <c r="FZ3" s="79" t="s">
+        <v>2852</v>
+      </c>
+      <c r="GA3" t="s">
         <v>2873</v>
       </c>
-      <c r="FJ3" t="s">
-        <v>2874</v>
-      </c>
-      <c r="FK3" s="79" t="s">
-        <v>2874</v>
-      </c>
-      <c r="FO3" t="s">
-        <v>2888</v>
-      </c>
-      <c r="FV3" t="s">
-        <v>2876</v>
-      </c>
-      <c r="FW3" s="79" t="s">
-        <v>2876</v>
-      </c>
-      <c r="FX3" s="79" t="s">
-        <v>2853</v>
-      </c>
-      <c r="FY3" s="79" t="s">
-        <v>2854</v>
-      </c>
-      <c r="FZ3" s="79" t="s">
-        <v>2854</v>
-      </c>
-      <c r="GA3" t="s">
-        <v>2875</v>
-      </c>
       <c r="GB3" t="s">
-        <v>2851</v>
+        <v>2849</v>
       </c>
       <c r="GC3" s="79" t="s">
-        <v>2851</v>
+        <v>2849</v>
       </c>
       <c r="GD3" s="79" t="s">
-        <v>2851</v>
+        <v>2849</v>
       </c>
       <c r="GE3" t="s">
-        <v>2869</v>
+        <v>2867</v>
       </c>
       <c r="GF3" s="79" t="s">
-        <v>2869</v>
+        <v>2867</v>
       </c>
       <c r="GG3" s="10" t="s">
         <v>2025</v>
@@ -16380,8 +16381,9 @@
       <c r="GH3" s="10" t="s">
         <v>2025</v>
       </c>
-    </row>
-    <row r="4" spans="1:206">
+      <c r="GY3" s="10"/>
+    </row>
+    <row r="4" spans="1:208">
       <c r="B4" t="s">
         <v>29</v>
       </c>
@@ -16696,13 +16698,13 @@
         <v>2406</v>
       </c>
       <c r="DG4" s="12" t="s">
+        <v>2908</v>
+      </c>
+      <c r="DH4" s="46" t="s">
+        <v>2909</v>
+      </c>
+      <c r="DI4" s="12" t="s">
         <v>2910</v>
-      </c>
-      <c r="DH4" s="46" t="s">
-        <v>2911</v>
-      </c>
-      <c r="DI4" s="12" t="s">
-        <v>2912</v>
       </c>
       <c r="DJ4" s="12" t="s">
         <v>2512</v>
@@ -16722,20 +16724,11 @@
       <c r="DR4" t="s">
         <v>2786</v>
       </c>
-      <c r="DS4" t="s">
-        <v>2788</v>
-      </c>
-      <c r="DT4" t="s">
-        <v>2228</v>
-      </c>
-      <c r="DU4" t="s">
-        <v>2790</v>
-      </c>
       <c r="DV4" t="s">
+        <v>2793</v>
+      </c>
+      <c r="DW4" t="s">
         <v>2795</v>
-      </c>
-      <c r="DW4" t="s">
-        <v>2797</v>
       </c>
       <c r="EB4" s="10" t="s">
         <v>1752</v>
@@ -16768,88 +16761,88 @@
         <v>2033</v>
       </c>
       <c r="EM4" t="s">
+        <v>2891</v>
+      </c>
+      <c r="EN4" t="s">
+        <v>2887</v>
+      </c>
+      <c r="EO4" s="79" t="s">
+        <v>2887</v>
+      </c>
+      <c r="EQ4" t="s">
+        <v>2860</v>
+      </c>
+      <c r="ER4" s="79" t="s">
+        <v>2860</v>
+      </c>
+      <c r="ES4" s="79" t="s">
+        <v>2860</v>
+      </c>
+      <c r="ET4" s="79" t="s">
+        <v>2860</v>
+      </c>
+      <c r="EU4" s="79" t="s">
+        <v>2860</v>
+      </c>
+      <c r="EV4" s="79" t="s">
+        <v>2860</v>
+      </c>
+      <c r="EW4" s="79" t="s">
+        <v>2860</v>
+      </c>
+      <c r="EX4" s="79" t="s">
+        <v>2860</v>
+      </c>
+      <c r="EY4" s="79" t="s">
+        <v>2860</v>
+      </c>
+      <c r="EZ4" t="s">
         <v>2893</v>
       </c>
-      <c r="EN4" t="s">
-        <v>2889</v>
-      </c>
-      <c r="EO4" s="79" t="s">
-        <v>2889</v>
-      </c>
-      <c r="EQ4" t="s">
-        <v>2862</v>
-      </c>
-      <c r="ER4" s="79" t="s">
-        <v>2862</v>
-      </c>
-      <c r="ES4" s="79" t="s">
-        <v>2862</v>
-      </c>
-      <c r="ET4" s="79" t="s">
-        <v>2862</v>
-      </c>
-      <c r="EU4" s="79" t="s">
-        <v>2862</v>
-      </c>
-      <c r="EV4" s="79" t="s">
-        <v>2862</v>
-      </c>
-      <c r="EW4" s="79" t="s">
-        <v>2862</v>
-      </c>
-      <c r="EX4" s="79" t="s">
-        <v>2862</v>
-      </c>
-      <c r="EY4" s="79" t="s">
-        <v>2862</v>
-      </c>
-      <c r="EZ4" t="s">
-        <v>2895</v>
-      </c>
       <c r="FB4" s="79" t="s">
-        <v>2870</v>
+        <v>2868</v>
       </c>
       <c r="FD4" s="79" t="s">
-        <v>2866</v>
+        <v>2864</v>
       </c>
       <c r="FF4" t="s">
-        <v>2890</v>
+        <v>2888</v>
       </c>
       <c r="FJ4" t="s">
-        <v>2887</v>
+        <v>2885</v>
       </c>
       <c r="FK4" s="79" t="s">
-        <v>2887</v>
+        <v>2885</v>
       </c>
       <c r="FO4" t="s">
-        <v>2829</v>
+        <v>2827</v>
       </c>
       <c r="FV4" t="s">
-        <v>2852</v>
+        <v>2850</v>
       </c>
       <c r="FW4" s="79" t="s">
-        <v>2852</v>
+        <v>2850</v>
       </c>
       <c r="FY4" s="79" t="s">
-        <v>2855</v>
+        <v>2853</v>
       </c>
       <c r="FZ4" s="79" t="s">
-        <v>2858</v>
+        <v>2856</v>
       </c>
       <c r="GB4" s="79" t="s">
-        <v>2877</v>
+        <v>2875</v>
       </c>
       <c r="GC4" s="79" t="s">
-        <v>2878</v>
+        <v>2876</v>
       </c>
       <c r="GD4" s="79" t="s">
-        <v>2877</v>
+        <v>2875</v>
       </c>
       <c r="GE4" t="s">
-        <v>2871</v>
+        <v>2869</v>
       </c>
       <c r="GF4" s="79" t="s">
-        <v>2871</v>
+        <v>2869</v>
       </c>
       <c r="GG4" s="79" t="s">
         <v>2033</v>
@@ -16858,7 +16851,7 @@
         <v>2033</v>
       </c>
     </row>
-    <row r="5" spans="1:206">
+    <row r="5" spans="1:208">
       <c r="B5" t="s">
         <v>40</v>
       </c>
@@ -17201,34 +17194,34 @@
         <v>2034</v>
       </c>
       <c r="EM5" t="s">
-        <v>2892</v>
+        <v>2890</v>
       </c>
       <c r="EO5" t="s">
-        <v>2901</v>
+        <v>2899</v>
       </c>
       <c r="EZ5" s="79" t="s">
-        <v>2897</v>
+        <v>2895</v>
       </c>
       <c r="FB5" s="79" t="s">
-        <v>2871</v>
+        <v>2869</v>
       </c>
       <c r="FD5" s="79" t="s">
-        <v>2864</v>
+        <v>2862</v>
       </c>
       <c r="FY5" s="79" t="s">
-        <v>2856</v>
+        <v>2854</v>
       </c>
       <c r="FZ5" s="79" t="s">
-        <v>2859</v>
+        <v>2857</v>
       </c>
       <c r="GD5" t="s">
-        <v>2886</v>
+        <v>2884</v>
       </c>
       <c r="GE5" t="s">
-        <v>2870</v>
+        <v>2868</v>
       </c>
       <c r="GF5" s="79" t="s">
-        <v>2870</v>
+        <v>2868</v>
       </c>
       <c r="GG5" s="79" t="s">
         <v>2034</v>
@@ -17237,7 +17230,7 @@
         <v>2034</v>
       </c>
     </row>
-    <row r="6" spans="1:206">
+    <row r="6" spans="1:208">
       <c r="B6" t="s">
         <v>52</v>
       </c>
@@ -17263,7 +17256,7 @@
         <v>59</v>
       </c>
       <c r="J6" t="s">
-        <v>2815</v>
+        <v>2813</v>
       </c>
       <c r="K6" s="34" t="s">
         <v>2067</v>
@@ -17556,28 +17549,28 @@
         <v>2035</v>
       </c>
       <c r="EM6" t="s">
-        <v>2890</v>
+        <v>2888</v>
       </c>
       <c r="EO6" t="s">
-        <v>2902</v>
+        <v>2900</v>
       </c>
       <c r="EZ6" s="79" t="s">
-        <v>2898</v>
+        <v>2896</v>
       </c>
       <c r="FB6" t="s">
         <v>2026</v>
       </c>
       <c r="FD6" s="79" t="s">
-        <v>2867</v>
+        <v>2865</v>
       </c>
       <c r="FZ6" t="s">
-        <v>2857</v>
+        <v>2855</v>
       </c>
       <c r="GE6" t="s">
-        <v>2879</v>
+        <v>2877</v>
       </c>
       <c r="GF6" s="79" t="s">
-        <v>2879</v>
+        <v>2877</v>
       </c>
       <c r="GG6" s="79" t="s">
         <v>2035</v>
@@ -17586,7 +17579,7 @@
         <v>2035</v>
       </c>
     </row>
-    <row r="7" spans="1:206">
+    <row r="7" spans="1:208">
       <c r="B7" t="s">
         <v>63</v>
       </c>
@@ -17872,7 +17865,7 @@
         <v>2562</v>
       </c>
       <c r="DL7" s="20" t="s">
-        <v>2834</v>
+        <v>2832</v>
       </c>
       <c r="EB7" s="79"/>
       <c r="EC7" s="79"/>
@@ -17893,22 +17886,22 @@
         <v>2027</v>
       </c>
       <c r="EM7" t="s">
-        <v>2904</v>
+        <v>2902</v>
       </c>
       <c r="EZ7" s="79" t="s">
-        <v>2899</v>
+        <v>2897</v>
       </c>
       <c r="FB7" t="s">
         <v>2027</v>
       </c>
       <c r="FD7" s="79" t="s">
-        <v>2865</v>
+        <v>2863</v>
       </c>
       <c r="GE7" s="79" t="s">
-        <v>2880</v>
+        <v>2878</v>
       </c>
       <c r="GF7" s="79" t="s">
-        <v>2880</v>
+        <v>2878</v>
       </c>
       <c r="GG7" s="79" t="s">
         <v>2027</v>
@@ -17917,7 +17910,7 @@
         <v>2027</v>
       </c>
     </row>
-    <row r="8" spans="1:206" ht="16.05" customHeight="1">
+    <row r="8" spans="1:208" ht="16.05" customHeight="1">
       <c r="B8" t="s">
         <v>75</v>
       </c>
@@ -18075,7 +18068,7 @@
         <v>2203</v>
       </c>
       <c r="BT8" s="10" t="s">
-        <v>2807</v>
+        <v>2805</v>
       </c>
       <c r="BU8" s="13" t="s">
         <v>2226</v>
@@ -18181,7 +18174,7 @@
         <v>2562</v>
       </c>
       <c r="DL8" s="20" t="s">
-        <v>2835</v>
+        <v>2833</v>
       </c>
       <c r="EE8" s="10" t="s">
         <v>2035</v>
@@ -18199,19 +18192,19 @@
         <v>2036</v>
       </c>
       <c r="EZ8" s="79" t="s">
-        <v>2900</v>
-      </c>
-      <c r="FB8" t="s">
-        <v>2872</v>
+        <v>2898</v>
+      </c>
+      <c r="FB8" s="85" t="s">
+        <v>2903</v>
       </c>
       <c r="FD8" s="79" t="s">
-        <v>2868</v>
+        <v>2866</v>
       </c>
       <c r="GE8" s="79" t="s">
-        <v>2881</v>
+        <v>2879</v>
       </c>
       <c r="GF8" s="79" t="s">
-        <v>2881</v>
+        <v>2879</v>
       </c>
       <c r="GG8" s="79" t="s">
         <v>2036</v>
@@ -18220,7 +18213,7 @@
         <v>2036</v>
       </c>
     </row>
-    <row r="9" spans="1:206" ht="16.05" customHeight="1">
+    <row r="9" spans="1:208" ht="16.05" customHeight="1">
       <c r="B9" t="s">
         <v>86</v>
       </c>
@@ -18335,13 +18328,13 @@
         <v>2549</v>
       </c>
       <c r="BJ9" s="20" t="s">
-        <v>2799</v>
+        <v>2797</v>
       </c>
       <c r="BK9" s="20" t="s">
         <v>2562</v>
       </c>
       <c r="BL9" s="20" t="s">
-        <v>2800</v>
+        <v>2798</v>
       </c>
       <c r="BM9" s="20" t="s">
         <v>2186</v>
@@ -18362,16 +18355,16 @@
         <v>8</v>
       </c>
       <c r="BS9" s="14" t="s">
-        <v>2908</v>
+        <v>2906</v>
       </c>
       <c r="BT9" s="10" t="s">
-        <v>2808</v>
+        <v>2806</v>
       </c>
       <c r="BU9" s="13" t="s">
         <v>2226</v>
       </c>
       <c r="BV9" s="10" t="s">
-        <v>2809</v>
+        <v>2807</v>
       </c>
       <c r="BW9" s="11" t="s">
         <v>2051</v>
@@ -18405,7 +18398,7 @@
         <v>2266</v>
       </c>
       <c r="CK9" s="42" t="s">
-        <v>2842</v>
+        <v>2840</v>
       </c>
       <c r="CL9" s="12" t="s">
         <v>1799</v>
@@ -18462,16 +18455,16 @@
         <v>2562</v>
       </c>
       <c r="DL9" s="20" t="s">
-        <v>2836</v>
+        <v>2834</v>
       </c>
       <c r="EE9" s="10" t="s">
         <v>2033</v>
       </c>
       <c r="EF9" s="10" t="s">
-        <v>2833</v>
+        <v>2831</v>
       </c>
       <c r="EG9" s="10" t="s">
-        <v>2832</v>
+        <v>2830</v>
       </c>
       <c r="EH9" s="79"/>
       <c r="EI9" s="79"/>
@@ -18480,13 +18473,16 @@
         <v>2026</v>
       </c>
       <c r="EZ9" t="s">
-        <v>2894</v>
+        <v>2892</v>
+      </c>
+      <c r="FB9" t="s">
+        <v>2870</v>
       </c>
       <c r="GE9" t="s">
-        <v>2882</v>
+        <v>2880</v>
       </c>
       <c r="GF9" s="79" t="s">
-        <v>2882</v>
+        <v>2880</v>
       </c>
       <c r="GG9" s="79" t="s">
         <v>2026</v>
@@ -18495,7 +18491,7 @@
         <v>2026</v>
       </c>
     </row>
-    <row r="10" spans="1:206">
+    <row r="10" spans="1:208">
       <c r="B10" t="s">
         <v>95</v>
       </c>
@@ -18602,13 +18598,13 @@
         <v>2550</v>
       </c>
       <c r="BJ10" s="20" t="s">
-        <v>2801</v>
+        <v>2799</v>
       </c>
       <c r="BK10" s="20" t="s">
         <v>2562</v>
       </c>
       <c r="BL10" s="20" t="s">
-        <v>2802</v>
+        <v>2800</v>
       </c>
       <c r="BM10" s="20" t="str">
         <f>_xlfn.CONCAT(BM9,"_error")</f>
@@ -18714,13 +18710,13 @@
       <c r="DH10" s="12"/>
       <c r="DI10" s="12"/>
       <c r="DJ10" s="20" t="s">
-        <v>2799</v>
+        <v>2797</v>
       </c>
       <c r="DK10" s="20" t="s">
         <v>2562</v>
       </c>
       <c r="DL10" s="20" t="s">
-        <v>2837</v>
+        <v>2835</v>
       </c>
       <c r="EE10" s="10" t="s">
         <v>2028</v>
@@ -18746,7 +18742,7 @@
         <v>2181</v>
       </c>
     </row>
-    <row r="11" spans="1:206">
+    <row r="11" spans="1:208">
       <c r="B11" t="s">
         <v>104</v>
       </c>
@@ -18852,13 +18848,13 @@
         <v>2551</v>
       </c>
       <c r="BJ11" s="20" t="s">
-        <v>2803</v>
+        <v>2801</v>
       </c>
       <c r="BK11" s="20" t="s">
         <v>2562</v>
       </c>
       <c r="BL11" s="20" t="s">
-        <v>2804</v>
+        <v>2802</v>
       </c>
       <c r="BM11" s="20" t="s">
         <v>2187</v>
@@ -18961,13 +18957,13 @@
       <c r="DH11" s="12"/>
       <c r="DI11" s="12"/>
       <c r="DJ11" s="20" t="s">
-        <v>2801</v>
+        <v>2799</v>
       </c>
       <c r="DK11" s="20" t="s">
         <v>2562</v>
       </c>
       <c r="DL11" s="20" t="s">
-        <v>2838</v>
+        <v>2836</v>
       </c>
       <c r="EE11" s="10" t="s">
         <v>2205</v>
@@ -18978,10 +18974,10 @@
         <v>2037</v>
       </c>
       <c r="GE11" t="s">
-        <v>2883</v>
+        <v>2881</v>
       </c>
       <c r="GF11" s="79" t="s">
-        <v>2883</v>
+        <v>2881</v>
       </c>
       <c r="GG11" s="79" t="s">
         <v>2037</v>
@@ -18990,7 +18986,7 @@
         <v>2037</v>
       </c>
     </row>
-    <row r="12" spans="1:206">
+    <row r="12" spans="1:208">
       <c r="B12" t="s">
         <v>113</v>
       </c>
@@ -19196,13 +19192,13 @@
       <c r="DH12" s="12"/>
       <c r="DI12" s="12"/>
       <c r="DJ12" s="20" t="s">
-        <v>2803</v>
+        <v>2801</v>
       </c>
       <c r="DK12" s="20" t="s">
         <v>2562</v>
       </c>
       <c r="DL12" s="20" t="s">
-        <v>2839</v>
+        <v>2837</v>
       </c>
       <c r="EE12" s="10" t="s">
         <v>2772</v>
@@ -19225,7 +19221,7 @@
         <v>2038</v>
       </c>
     </row>
-    <row r="13" spans="1:206">
+    <row r="13" spans="1:208">
       <c r="B13" t="s">
         <v>122</v>
       </c>
@@ -19245,7 +19241,7 @@
         <v>127</v>
       </c>
       <c r="J13" t="s">
-        <v>2831</v>
+        <v>2829</v>
       </c>
       <c r="K13" s="34" t="s">
         <v>2073</v>
@@ -19264,7 +19260,7 @@
       </c>
       <c r="U13" s="6"/>
       <c r="V13" s="77" t="s">
-        <v>2830</v>
+        <v>2828</v>
       </c>
       <c r="AB13" s="6" t="s">
         <v>1387</v>
@@ -19419,7 +19415,7 @@
         <v>2769</v>
       </c>
       <c r="DL13" s="20" t="s">
-        <v>2840</v>
+        <v>2838</v>
       </c>
       <c r="EE13" s="10"/>
       <c r="EF13" s="10"/>
@@ -19440,7 +19436,7 @@
         <v>2028</v>
       </c>
     </row>
-    <row r="14" spans="1:206">
+    <row r="14" spans="1:208">
       <c r="B14" t="s">
         <v>130</v>
       </c>
@@ -19460,7 +19456,7 @@
         <v>135</v>
       </c>
       <c r="K14" s="71" t="s">
-        <v>2805</v>
+        <v>2803</v>
       </c>
       <c r="L14" t="s">
         <v>136</v>
@@ -19548,13 +19544,13 @@
         <v>2213</v>
       </c>
       <c r="BT14" s="20" t="s">
-        <v>2810</v>
+        <v>2808</v>
       </c>
       <c r="BU14" s="13" t="s">
         <v>2227</v>
       </c>
       <c r="BV14" s="20" t="s">
-        <v>2811</v>
+        <v>2809</v>
       </c>
       <c r="BW14" s="11" t="s">
         <v>2054</v>
@@ -19630,7 +19626,7 @@
         <v>2027</v>
       </c>
     </row>
-    <row r="15" spans="1:206">
+    <row r="15" spans="1:208">
       <c r="B15" t="s">
         <v>138</v>
       </c>
@@ -19812,7 +19808,7 @@
         <v>2028</v>
       </c>
     </row>
-    <row r="16" spans="1:206">
+    <row r="16" spans="1:208">
       <c r="B16" t="s">
         <v>145</v>
       </c>
@@ -20088,7 +20084,7 @@
         <v>16</v>
       </c>
       <c r="BS17" s="14" t="s">
-        <v>2816</v>
+        <v>2814</v>
       </c>
       <c r="BT17" s="10" t="s">
         <v>2084</v>
@@ -20158,10 +20154,10 @@
       <c r="DK17" s="43"/>
       <c r="DL17" s="43"/>
       <c r="GE17" t="s">
-        <v>2884</v>
+        <v>2882</v>
       </c>
       <c r="GF17" s="79" t="s">
-        <v>2885</v>
+        <v>2883</v>
       </c>
     </row>
     <row r="18" spans="2:188">
@@ -20260,7 +20256,7 @@
         <v>17</v>
       </c>
       <c r="BS18" s="14" t="s">
-        <v>2817</v>
+        <v>2815</v>
       </c>
       <c r="BT18" s="10" t="s">
         <v>2123</v>
@@ -20282,13 +20278,13 @@
       <c r="CA18" s="11"/>
       <c r="CB18" s="11"/>
       <c r="CI18" s="12" t="s">
-        <v>2844</v>
+        <v>2842</v>
       </c>
       <c r="CJ18" s="78" t="s">
         <v>2266</v>
       </c>
       <c r="CK18" s="78" t="s">
-        <v>2841</v>
+        <v>2839</v>
       </c>
       <c r="CL18" s="12" t="s">
         <v>1802</v>
@@ -20426,7 +20422,7 @@
         <v>18</v>
       </c>
       <c r="BS19" s="14" t="s">
-        <v>2818</v>
+        <v>2816</v>
       </c>
       <c r="BT19" s="10" t="s">
         <v>2206</v>
@@ -20447,13 +20443,13 @@
       <c r="CA19" s="11"/>
       <c r="CB19" s="11"/>
       <c r="CI19" s="12" t="s">
-        <v>2845</v>
+        <v>2843</v>
       </c>
       <c r="CJ19" s="78" t="s">
         <v>2266</v>
       </c>
       <c r="CK19" s="78" t="s">
-        <v>2843</v>
+        <v>2841</v>
       </c>
       <c r="CL19" s="12" t="s">
         <v>1803</v>
@@ -20580,16 +20576,16 @@
         <v>2727</v>
       </c>
       <c r="BP20" s="14" t="s">
-        <v>2791</v>
+        <v>2789</v>
       </c>
       <c r="BQ20" s="20" t="s">
-        <v>2798</v>
+        <v>2796</v>
       </c>
       <c r="BR20" s="20">
         <v>19</v>
       </c>
       <c r="BS20" s="14" t="s">
-        <v>2819</v>
+        <v>2817</v>
       </c>
       <c r="BW20" s="11" t="s">
         <v>2369</v>
@@ -20639,10 +20635,10 @@
       <c r="DK20" s="43"/>
       <c r="DL20" s="43"/>
       <c r="GE20" s="10" t="s">
-        <v>2905</v>
+        <v>2903</v>
       </c>
       <c r="GF20" s="10" t="s">
-        <v>2905</v>
+        <v>2903</v>
       </c>
     </row>
     <row r="21" spans="2:188" ht="16.8">
@@ -20720,13 +20716,13 @@
         <v>2527</v>
       </c>
       <c r="BP21" s="14" t="s">
+        <v>2844</v>
+      </c>
+      <c r="BQ21" s="20" t="s">
         <v>2846</v>
       </c>
-      <c r="BQ21" s="20" t="s">
-        <v>2848</v>
-      </c>
       <c r="BS21" s="14" t="s">
-        <v>2820</v>
+        <v>2818</v>
       </c>
       <c r="BW21" s="11" t="s">
         <v>2373</v>
@@ -20822,13 +20818,13 @@
         <v>2728</v>
       </c>
       <c r="BP22" s="14" t="s">
+        <v>2845</v>
+      </c>
+      <c r="BQ22" s="20" t="s">
         <v>2847</v>
       </c>
-      <c r="BQ22" s="20" t="s">
-        <v>2849</v>
-      </c>
       <c r="BS22" s="14" t="s">
-        <v>2821</v>
+        <v>2819</v>
       </c>
       <c r="BW22" s="11" t="s">
         <v>2573</v>
@@ -20917,13 +20913,13 @@
       </c>
       <c r="BD23" s="17"/>
       <c r="BP23" s="14" t="s">
-        <v>2906</v>
+        <v>2904</v>
       </c>
       <c r="BQ23" s="20" t="s">
-        <v>2907</v>
+        <v>2905</v>
       </c>
       <c r="BS23" s="14" t="s">
-        <v>2822</v>
+        <v>2820</v>
       </c>
       <c r="BW23" s="11" t="s">
         <v>2574</v>
@@ -21017,7 +21013,7 @@
       </c>
       <c r="BD24" s="17"/>
       <c r="BS24" s="14" t="s">
-        <v>2823</v>
+        <v>2821</v>
       </c>
       <c r="BW24" s="11" t="s">
         <v>2575</v>
@@ -21106,7 +21102,7 @@
       </c>
       <c r="BD25" s="17"/>
       <c r="BS25" s="14" t="s">
-        <v>2824</v>
+        <v>2822</v>
       </c>
       <c r="BW25" s="11" t="s">
         <v>2576</v>
@@ -21194,7 +21190,7 @@
       </c>
       <c r="BD26" s="17"/>
       <c r="BS26" s="14" t="s">
-        <v>2825</v>
+        <v>2823</v>
       </c>
       <c r="BW26" s="11" t="s">
         <v>1765</v>
@@ -21252,7 +21248,7 @@
       <c r="L27" t="s">
         <v>228</v>
       </c>
-      <c r="M27" s="112"/>
+      <c r="M27" s="113"/>
       <c r="O27" s="12" t="s">
         <v>822</v>
       </c>
@@ -21275,7 +21271,7 @@
         <v>1941</v>
       </c>
       <c r="BS27" s="14" t="s">
-        <v>2826</v>
+        <v>2824</v>
       </c>
       <c r="BW27" s="11" t="s">
         <v>1775</v>
@@ -21333,7 +21329,7 @@
       <c r="L28" t="s">
         <v>235</v>
       </c>
-      <c r="M28" s="112"/>
+      <c r="M28" s="113"/>
       <c r="O28" s="12" t="s">
         <v>1712</v>
       </c>
@@ -21356,7 +21352,7 @@
         <v>1655</v>
       </c>
       <c r="BS28" s="14" t="s">
-        <v>2827</v>
+        <v>2825</v>
       </c>
       <c r="BW28" s="11" t="s">
         <v>2732</v>
@@ -21434,7 +21430,7 @@
         <v>1678</v>
       </c>
       <c r="BS29" s="14" t="s">
-        <v>2828</v>
+        <v>2826</v>
       </c>
       <c r="BW29" s="20"/>
       <c r="BX29" s="14"/>
@@ -21729,7 +21725,7 @@
       <c r="L34" t="s">
         <v>276</v>
       </c>
-      <c r="M34" s="112"/>
+      <c r="M34" s="113"/>
       <c r="O34" s="12" t="s">
         <v>915</v>
       </c>
@@ -21788,7 +21784,7 @@
       <c r="L35" t="s">
         <v>283</v>
       </c>
-      <c r="M35" s="112"/>
+      <c r="M35" s="113"/>
       <c r="O35" s="12" t="s">
         <v>939</v>
       </c>
@@ -27254,7 +27250,7 @@
       <c r="CR277" s="42"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="Nui/WFCkAiM0/CddZH2BeeUckAlyyX+waYESgZQHD7xExq5G73EzJ3ahN5CGEk6uA54E7XlFhpXYP2dxa/xdDA==" saltValue="BSqL34JuvMRNPmhdLprQJQ==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="NE97licGlkyxTUWiqo5EY0YSTyeAmE/76uPT7IrmiCEPuI2W7BZOB0wTQXAmMQcp7JL0WVplWv20C8IKGTthkg==" saltValue="6gGNCFzucn1D7guxsrSnsQ==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="2">
     <mergeCell ref="M27:M28"/>
     <mergeCell ref="M34:M35"/>

</xml_diff>

<commit_message>
Eliminated sample_dating from sample_sediment_properties
</commit_message>
<xml_diff>
--- a/Excel_templates/MOSAIC_input_excel_file_2022.xlsx
+++ b/Excel_templates/MOSAIC_input_excel_file_2022.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sparadis\Documents\ETH\MOSAIC\MOSAIC_Client\Excel_templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{227AE783-FB6A-439A-B7DA-7324C301B1BC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{702D8C62-DECE-4D9E-99B3-39196A326CEC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="30204" yWindow="10044" windowWidth="40020" windowHeight="22296" tabRatio="694" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -193,7 +193,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3732" uniqueCount="2911">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3726" uniqueCount="2911">
   <si>
     <t>sample_name</t>
   </si>
@@ -11825,7 +11825,7 @@
       <pane xSplit="3" ySplit="6" topLeftCell="D7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="L10" sqref="L10"/>
+      <selection pane="bottomRight" activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15" defaultRowHeight="15.6"/>
@@ -14558,8 +14558,8 @@
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:GZ277"/>
   <sheetViews>
-    <sheetView topLeftCell="EQ1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="FA21" sqref="FA21"/>
+    <sheetView topLeftCell="BS1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="BT14" sqref="BT14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -20258,15 +20258,6 @@
       <c r="BS18" s="14" t="s">
         <v>2815</v>
       </c>
-      <c r="BT18" s="10" t="s">
-        <v>2123</v>
-      </c>
-      <c r="BU18" s="10" t="s">
-        <v>1818</v>
-      </c>
-      <c r="BV18" s="10" t="s">
-        <v>2242</v>
-      </c>
       <c r="BW18" s="11" t="s">
         <v>2368</v>
       </c>
@@ -20423,15 +20414,6 @@
       </c>
       <c r="BS19" s="14" t="s">
         <v>2816</v>
-      </c>
-      <c r="BT19" s="10" t="s">
-        <v>2206</v>
-      </c>
-      <c r="BU19" s="10" t="s">
-        <v>1818</v>
-      </c>
-      <c r="BV19" s="10" t="s">
-        <v>2243</v>
       </c>
       <c r="BW19" s="11" t="s">
         <v>2370</v>
@@ -27250,7 +27232,6 @@
       <c r="CR277" s="42"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="NE97licGlkyxTUWiqo5EY0YSTyeAmE/76uPT7IrmiCEPuI2W7BZOB0wTQXAmMQcp7JL0WVplWv20C8IKGTthkg==" saltValue="6gGNCFzucn1D7guxsrSnsQ==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="2">
     <mergeCell ref="M27:M28"/>
     <mergeCell ref="M34:M35"/>

</xml_diff>

<commit_message>
Changed Neodynium_detrital to Neodynium epsilon, and instead added a material_analyzed of detrital and leached
</commit_message>
<xml_diff>
--- a/Excel_templates/MOSAIC_input_excel_file_2022.xlsx
+++ b/Excel_templates/MOSAIC_input_excel_file_2022.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sparadis\Documents\ETH\MOSAIC\MOSAIC_Client\Excel_templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{702D8C62-DECE-4D9E-99B3-39196A326CEC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAA44C3C-AEAD-4938-B53B-7121451E0B1D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="30204" yWindow="10044" windowWidth="40020" windowHeight="22296" tabRatio="694" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,6 +20,7 @@
     <sheet name="SET_VARIABLES" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
+    <definedName name="_143Nd_144Nd">SET_VARIABLES!$GZ$2:$GZ$3</definedName>
     <definedName name="Age_14C_ybp">SET_VARIABLES!$GF$2:$GF$19</definedName>
     <definedName name="Argentina">SET_VARIABLES!$P$2:$P$8</definedName>
     <definedName name="Australia">SET_VARIABLES!$Q$2:$Q$28</definedName>
@@ -81,14 +82,14 @@
     <definedName name="MAR_g_cm2_yr">SET_VARIABLES!$GE$2:$GE$20</definedName>
     <definedName name="MAR_model">SET_VARIABLES!#REF!</definedName>
     <definedName name="MAR_tracer">SET_VARIABLES!#REF!</definedName>
-    <definedName name="material_analyzed">SET_VARIABLES!$BS$2:$BS$29</definedName>
+    <definedName name="material_analyzed">SET_VARIABLES!$BS$2:$BS$31</definedName>
     <definedName name="Mauritania">SET_VARIABLES!$AL$2:$AL$7</definedName>
     <definedName name="mean_grain_size_microm">SET_VARIABLES!$EW$2:$EW$4</definedName>
     <definedName name="median_grain_size_microm">SET_VARIABLES!$EX$2:$EX$4</definedName>
-    <definedName name="Mixing_rate_cm2_yr">SET_VARIABLES!$GH$2:$GH$13</definedName>
-    <definedName name="Mixing_rate_tracer">SET_VARIABLES!#REF!</definedName>
+    <definedName name="Mixing_rate_cm2_yr">SET_VARIABLES!$GH$2:$GH$14</definedName>
     <definedName name="mode_grain_size_microm">SET_VARIABLES!$EY$2:$EY$4</definedName>
     <definedName name="mud_silt_clay_">SET_VARIABLES!$EV$2:$EV$4</definedName>
+    <definedName name="Nd_epsilon">SET_VARIABLES!$HA$2:$HA$3</definedName>
     <definedName name="Netherlands">SET_VARIABLES!$AM$2:$AM$13</definedName>
     <definedName name="New_Zealand">SET_VARIABLES!$AN$2:$AN$13</definedName>
     <definedName name="Norway">SET_VARIABLES!$AO$2:$AO$13</definedName>
@@ -154,6 +155,7 @@
     <definedName name="Tmax">SET_VARIABLES!$GS$2:$GS$3</definedName>
     <definedName name="total_carbon_">SET_VARIABLES!$FC$2:$FC$4</definedName>
     <definedName name="total_inorganic_carbon_">SET_VARIABLES!$FE$2:$FE$4</definedName>
+    <definedName name="total_Nd_ppm">SET_VARIABLES!$GY$2:$GY$3</definedName>
     <definedName name="total_nitrogen_">SET_VARIABLES!$FI$2:$FI$4</definedName>
     <definedName name="total_organic_carbon_">SET_VARIABLES!$EM$2:$EM$7</definedName>
     <definedName name="Total_Pb210_Bq_kg">SET_VARIABLES!$FV$2:$FV$4</definedName>
@@ -193,7 +195,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3726" uniqueCount="2911">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3738" uniqueCount="2915">
   <si>
     <t>sample_name</t>
   </si>
@@ -8574,9 +8576,6 @@
     <t>ppm</t>
   </si>
   <si>
-    <t>Nd_detrital</t>
-  </si>
-  <si>
     <t>sample_strontium</t>
   </si>
   <si>
@@ -8926,6 +8925,21 @@
   </si>
   <si>
     <t>Oxygen index</t>
+  </si>
+  <si>
+    <t>OMEXDIA</t>
+  </si>
+  <si>
+    <t>Nd_epsilon</t>
+  </si>
+  <si>
+    <t>detrital</t>
+  </si>
+  <si>
+    <t>leached</t>
+  </si>
+  <si>
+    <t>Mass spect.</t>
   </si>
 </sst>
 </file>
@@ -10114,7 +10128,7 @@
         <v>1824</v>
       </c>
       <c r="E2" s="57" t="s">
-        <v>2901</v>
+        <v>2900</v>
       </c>
       <c r="F2" s="60" t="s">
         <v>1825</v>
@@ -11825,7 +11839,7 @@
       <pane xSplit="3" ySplit="6" topLeftCell="D7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="N2" sqref="N2"/>
+      <selection pane="bottomRight" activeCell="O5" sqref="O5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15" defaultRowHeight="15.6"/>
@@ -11876,10 +11890,10 @@
         <v>2789</v>
       </c>
       <c r="P1" s="74" t="s">
-        <v>2844</v>
-      </c>
-    </row>
-    <row r="2" spans="1:80" s="76" customFormat="1">
+        <v>1815</v>
+      </c>
+    </row>
+    <row r="2" spans="1:80" s="76" customFormat="1" ht="31.2">
       <c r="A2" s="101" t="s">
         <v>2510</v>
       </c>
@@ -11923,10 +11937,10 @@
         <v>1840</v>
       </c>
       <c r="O2" s="75" t="s">
-        <v>2791</v>
+        <v>2911</v>
       </c>
       <c r="P2" s="75" t="s">
-        <v>2708</v>
+        <v>2710</v>
       </c>
       <c r="Q2" s="75"/>
       <c r="R2" s="75"/>
@@ -12006,10 +12020,10 @@
       <c r="J3" s="105"/>
       <c r="K3" s="111"/>
       <c r="L3" s="75" t="s">
-        <v>2867</v>
+        <v>2866</v>
       </c>
       <c r="M3" s="75" t="s">
-        <v>2871</v>
+        <v>2870</v>
       </c>
       <c r="N3" s="75"/>
       <c r="O3" s="75"/>
@@ -14556,10 +14570,10 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr codeName="Sheet6"/>
-  <dimension ref="A1:GZ277"/>
+  <dimension ref="A1:HA277"/>
   <sheetViews>
-    <sheetView topLeftCell="BS1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="BT14" sqref="BT14"/>
+    <sheetView topLeftCell="GF1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="GP14" sqref="GP14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -14614,7 +14628,7 @@
     <col min="187" max="188" width="21.3984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:208" s="1" customFormat="1">
+    <row r="1" spans="1:209" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -14784,7 +14798,7 @@
         <v>1143</v>
       </c>
       <c r="BE1" s="1" t="s">
-        <v>2810</v>
+        <v>2809</v>
       </c>
       <c r="BF1" s="15" t="s">
         <v>1848</v>
@@ -15044,7 +15058,7 @@
         <v>sample_neodynium_description</v>
       </c>
       <c r="DY1" s="9" t="s">
-        <v>2794</v>
+        <v>2793</v>
       </c>
       <c r="DZ1" s="9" t="str">
         <f>_xlfn.CONCAT(DY1,"_units")</f>
@@ -15055,7 +15069,7 @@
         <v>sample_strontium_description</v>
       </c>
       <c r="EB1" s="1" t="s">
-        <v>2844</v>
+        <v>2843</v>
       </c>
       <c r="EC1" s="9" t="str">
         <f>_xlfn.CONCAT(EB1,"_units")</f>
@@ -15075,7 +15089,7 @@
         <v>1754</v>
       </c>
       <c r="EH1" s="1" t="s">
-        <v>2845</v>
+        <v>2844</v>
       </c>
       <c r="EI1" s="9" t="str">
         <f>_xlfn.CONCAT(EH1,"_units")</f>
@@ -15089,7 +15103,7 @@
         <v>1753</v>
       </c>
       <c r="EL1" s="80" t="s">
-        <v>2848</v>
+        <v>2847</v>
       </c>
       <c r="EM1" s="1" t="s">
         <v>2048</v>
@@ -15113,10 +15127,10 @@
         <v>1844</v>
       </c>
       <c r="ET1" s="1" t="s">
+        <v>2804</v>
+      </c>
+      <c r="EU1" s="1" t="s">
         <v>2805</v>
-      </c>
-      <c r="EU1" s="1" t="s">
-        <v>2806</v>
       </c>
       <c r="EV1" s="1" t="s">
         <v>1845</v>
@@ -15128,7 +15142,7 @@
         <v>2747</v>
       </c>
       <c r="EY1" s="1" t="s">
-        <v>2808</v>
+        <v>2807</v>
       </c>
       <c r="EZ1" s="1" t="s">
         <v>2058</v>
@@ -15221,7 +15235,7 @@
         <v>1790</v>
       </c>
       <c r="GD1" s="1" t="s">
-        <v>2842</v>
+        <v>2841</v>
       </c>
       <c r="GE1" s="1" t="s">
         <v>2708</v>
@@ -15272,7 +15286,7 @@
         <v>2473</v>
       </c>
       <c r="GU1" s="22" t="s">
-        <v>2908</v>
+        <v>2907</v>
       </c>
       <c r="GV1" s="22" t="s">
         <v>2463</v>
@@ -15283,10 +15297,17 @@
       <c r="GX1" s="22" t="s">
         <v>2467</v>
       </c>
-      <c r="GY1" s="22"/>
-      <c r="GZ1" s="22"/>
-    </row>
-    <row r="2" spans="1:208">
+      <c r="GY1" s="22" t="s">
+        <v>2790</v>
+      </c>
+      <c r="GZ1" s="22" t="s">
+        <v>2791</v>
+      </c>
+      <c r="HA1" s="22" t="s">
+        <v>2911</v>
+      </c>
+    </row>
+    <row r="2" spans="1:209">
       <c r="A2" t="b">
         <v>1</v>
       </c>
@@ -15456,7 +15477,7 @@
         <v>5</v>
       </c>
       <c r="BE2" s="72" t="s">
-        <v>2811</v>
+        <v>2810</v>
       </c>
       <c r="BF2" s="16" t="s">
         <v>2182</v>
@@ -15612,7 +15633,7 @@
         <v>2462</v>
       </c>
       <c r="DH2" s="12" t="s">
-        <v>2907</v>
+        <v>2906</v>
       </c>
       <c r="DI2" s="12"/>
       <c r="DJ2" s="12" t="s">
@@ -15879,9 +15900,17 @@
       <c r="GX2" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="GY2" s="10"/>
-    </row>
-    <row r="3" spans="1:208">
+      <c r="GY2" s="10" t="s">
+        <v>2914</v>
+      </c>
+      <c r="GZ2" s="10" t="s">
+        <v>2914</v>
+      </c>
+      <c r="HA2" s="10" t="s">
+        <v>2914</v>
+      </c>
+    </row>
+    <row r="3" spans="1:209">
       <c r="A3" t="b">
         <v>0</v>
       </c>
@@ -15910,7 +15939,7 @@
         <v>19</v>
       </c>
       <c r="J3" t="s">
-        <v>2804</v>
+        <v>2803</v>
       </c>
       <c r="K3" s="34" t="s">
         <v>2064</v>
@@ -16051,7 +16080,7 @@
         <v>20</v>
       </c>
       <c r="BE3" s="72" t="s">
-        <v>2812</v>
+        <v>2811</v>
       </c>
       <c r="BF3" s="16" t="s">
         <v>2731</v>
@@ -16280,100 +16309,100 @@
         <v>2025</v>
       </c>
       <c r="EM3" t="s">
-        <v>2827</v>
+        <v>2826</v>
       </c>
       <c r="EN3" t="s">
+        <v>2857</v>
+      </c>
+      <c r="EO3" t="s">
+        <v>2857</v>
+      </c>
+      <c r="EP3" s="79" t="s">
+        <v>2857</v>
+      </c>
+      <c r="EQ3" t="s">
         <v>2858</v>
       </c>
-      <c r="EO3" t="s">
+      <c r="ER3" s="79" t="s">
         <v>2858</v>
       </c>
-      <c r="EP3" s="79" t="s">
+      <c r="ES3" s="79" t="s">
         <v>2858</v>
       </c>
-      <c r="EQ3" t="s">
-        <v>2859</v>
-      </c>
-      <c r="ER3" s="79" t="s">
-        <v>2859</v>
-      </c>
-      <c r="ES3" s="79" t="s">
-        <v>2859</v>
-      </c>
       <c r="ET3" s="79" t="s">
-        <v>2859</v>
+        <v>2858</v>
       </c>
       <c r="EU3" s="79" t="s">
-        <v>2859</v>
+        <v>2858</v>
       </c>
       <c r="EV3" s="79" t="s">
-        <v>2859</v>
+        <v>2858</v>
       </c>
       <c r="EW3" s="79" t="s">
-        <v>2859</v>
+        <v>2858</v>
       </c>
       <c r="EX3" s="79" t="s">
-        <v>2859</v>
+        <v>2858</v>
       </c>
       <c r="EY3" s="79" t="s">
-        <v>2859</v>
+        <v>2858</v>
       </c>
       <c r="EZ3" s="79" t="s">
-        <v>2894</v>
+        <v>2893</v>
       </c>
       <c r="FB3" t="s">
-        <v>2867</v>
+        <v>2866</v>
       </c>
       <c r="FD3" t="s">
-        <v>2861</v>
+        <v>2860</v>
       </c>
       <c r="FE3" t="s">
-        <v>2889</v>
+        <v>2888</v>
       </c>
       <c r="FF3" t="s">
+        <v>2870</v>
+      </c>
+      <c r="FJ3" t="s">
         <v>2871</v>
       </c>
-      <c r="FJ3" t="s">
+      <c r="FK3" s="79" t="s">
+        <v>2871</v>
+      </c>
+      <c r="FO3" t="s">
+        <v>2885</v>
+      </c>
+      <c r="FV3" t="s">
+        <v>2873</v>
+      </c>
+      <c r="FW3" s="79" t="s">
+        <v>2873</v>
+      </c>
+      <c r="FX3" s="79" t="s">
+        <v>2850</v>
+      </c>
+      <c r="FY3" s="79" t="s">
+        <v>2851</v>
+      </c>
+      <c r="FZ3" s="79" t="s">
+        <v>2851</v>
+      </c>
+      <c r="GA3" t="s">
         <v>2872</v>
       </c>
-      <c r="FK3" s="79" t="s">
-        <v>2872</v>
-      </c>
-      <c r="FO3" t="s">
-        <v>2886</v>
-      </c>
-      <c r="FV3" t="s">
-        <v>2874</v>
-      </c>
-      <c r="FW3" s="79" t="s">
-        <v>2874</v>
-      </c>
-      <c r="FX3" s="79" t="s">
-        <v>2851</v>
-      </c>
-      <c r="FY3" s="79" t="s">
-        <v>2852</v>
-      </c>
-      <c r="FZ3" s="79" t="s">
-        <v>2852</v>
-      </c>
-      <c r="GA3" t="s">
-        <v>2873</v>
-      </c>
       <c r="GB3" t="s">
-        <v>2849</v>
+        <v>2848</v>
       </c>
       <c r="GC3" s="79" t="s">
-        <v>2849</v>
+        <v>2848</v>
       </c>
       <c r="GD3" s="79" t="s">
-        <v>2849</v>
+        <v>2848</v>
       </c>
       <c r="GE3" t="s">
-        <v>2867</v>
+        <v>2866</v>
       </c>
       <c r="GF3" s="79" t="s">
-        <v>2867</v>
+        <v>2866</v>
       </c>
       <c r="GG3" s="10" t="s">
         <v>2025</v>
@@ -16381,9 +16410,17 @@
       <c r="GH3" s="10" t="s">
         <v>2025</v>
       </c>
-      <c r="GY3" s="10"/>
-    </row>
-    <row r="4" spans="1:208">
+      <c r="GY3" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="GZ3" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="HA3" s="10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:209">
       <c r="B4" t="s">
         <v>29</v>
       </c>
@@ -16698,13 +16735,13 @@
         <v>2406</v>
       </c>
       <c r="DG4" s="12" t="s">
+        <v>2907</v>
+      </c>
+      <c r="DH4" s="46" t="s">
         <v>2908</v>
       </c>
-      <c r="DH4" s="46" t="s">
+      <c r="DI4" s="12" t="s">
         <v>2909</v>
-      </c>
-      <c r="DI4" s="12" t="s">
-        <v>2910</v>
       </c>
       <c r="DJ4" s="12" t="s">
         <v>2512</v>
@@ -16725,10 +16762,10 @@
         <v>2786</v>
       </c>
       <c r="DV4" t="s">
-        <v>2793</v>
+        <v>2911</v>
       </c>
       <c r="DW4" t="s">
-        <v>2795</v>
+        <v>2794</v>
       </c>
       <c r="EB4" s="10" t="s">
         <v>1752</v>
@@ -16761,88 +16798,88 @@
         <v>2033</v>
       </c>
       <c r="EM4" t="s">
-        <v>2891</v>
+        <v>2890</v>
       </c>
       <c r="EN4" t="s">
+        <v>2886</v>
+      </c>
+      <c r="EO4" s="79" t="s">
+        <v>2886</v>
+      </c>
+      <c r="EQ4" t="s">
+        <v>2859</v>
+      </c>
+      <c r="ER4" s="79" t="s">
+        <v>2859</v>
+      </c>
+      <c r="ES4" s="79" t="s">
+        <v>2859</v>
+      </c>
+      <c r="ET4" s="79" t="s">
+        <v>2859</v>
+      </c>
+      <c r="EU4" s="79" t="s">
+        <v>2859</v>
+      </c>
+      <c r="EV4" s="79" t="s">
+        <v>2859</v>
+      </c>
+      <c r="EW4" s="79" t="s">
+        <v>2859</v>
+      </c>
+      <c r="EX4" s="79" t="s">
+        <v>2859</v>
+      </c>
+      <c r="EY4" s="79" t="s">
+        <v>2859</v>
+      </c>
+      <c r="EZ4" t="s">
+        <v>2892</v>
+      </c>
+      <c r="FB4" s="79" t="s">
+        <v>2867</v>
+      </c>
+      <c r="FD4" s="79" t="s">
+        <v>2863</v>
+      </c>
+      <c r="FF4" t="s">
         <v>2887</v>
       </c>
-      <c r="EO4" s="79" t="s">
-        <v>2887</v>
-      </c>
-      <c r="EQ4" t="s">
-        <v>2860</v>
-      </c>
-      <c r="ER4" s="79" t="s">
-        <v>2860</v>
-      </c>
-      <c r="ES4" s="79" t="s">
-        <v>2860</v>
-      </c>
-      <c r="ET4" s="79" t="s">
-        <v>2860</v>
-      </c>
-      <c r="EU4" s="79" t="s">
-        <v>2860</v>
-      </c>
-      <c r="EV4" s="79" t="s">
-        <v>2860</v>
-      </c>
-      <c r="EW4" s="79" t="s">
-        <v>2860</v>
-      </c>
-      <c r="EX4" s="79" t="s">
-        <v>2860</v>
-      </c>
-      <c r="EY4" s="79" t="s">
-        <v>2860</v>
-      </c>
-      <c r="EZ4" t="s">
-        <v>2893</v>
-      </c>
-      <c r="FB4" s="79" t="s">
+      <c r="FJ4" t="s">
+        <v>2884</v>
+      </c>
+      <c r="FK4" s="79" t="s">
+        <v>2884</v>
+      </c>
+      <c r="FO4" t="s">
+        <v>2826</v>
+      </c>
+      <c r="FV4" t="s">
+        <v>2849</v>
+      </c>
+      <c r="FW4" s="79" t="s">
+        <v>2849</v>
+      </c>
+      <c r="FY4" s="79" t="s">
+        <v>2852</v>
+      </c>
+      <c r="FZ4" s="79" t="s">
+        <v>2855</v>
+      </c>
+      <c r="GB4" s="79" t="s">
+        <v>2874</v>
+      </c>
+      <c r="GC4" s="79" t="s">
+        <v>2875</v>
+      </c>
+      <c r="GD4" s="79" t="s">
+        <v>2874</v>
+      </c>
+      <c r="GE4" t="s">
         <v>2868</v>
       </c>
-      <c r="FD4" s="79" t="s">
-        <v>2864</v>
-      </c>
-      <c r="FF4" t="s">
-        <v>2888</v>
-      </c>
-      <c r="FJ4" t="s">
-        <v>2885</v>
-      </c>
-      <c r="FK4" s="79" t="s">
-        <v>2885</v>
-      </c>
-      <c r="FO4" t="s">
-        <v>2827</v>
-      </c>
-      <c r="FV4" t="s">
-        <v>2850</v>
-      </c>
-      <c r="FW4" s="79" t="s">
-        <v>2850</v>
-      </c>
-      <c r="FY4" s="79" t="s">
-        <v>2853</v>
-      </c>
-      <c r="FZ4" s="79" t="s">
-        <v>2856</v>
-      </c>
-      <c r="GB4" s="79" t="s">
-        <v>2875</v>
-      </c>
-      <c r="GC4" s="79" t="s">
-        <v>2876</v>
-      </c>
-      <c r="GD4" s="79" t="s">
-        <v>2875</v>
-      </c>
-      <c r="GE4" t="s">
-        <v>2869</v>
-      </c>
       <c r="GF4" s="79" t="s">
-        <v>2869</v>
+        <v>2868</v>
       </c>
       <c r="GG4" s="79" t="s">
         <v>2033</v>
@@ -16851,7 +16888,7 @@
         <v>2033</v>
       </c>
     </row>
-    <row r="5" spans="1:208">
+    <row r="5" spans="1:209">
       <c r="B5" t="s">
         <v>40</v>
       </c>
@@ -17194,34 +17231,34 @@
         <v>2034</v>
       </c>
       <c r="EM5" t="s">
-        <v>2890</v>
+        <v>2889</v>
       </c>
       <c r="EO5" t="s">
-        <v>2899</v>
+        <v>2898</v>
       </c>
       <c r="EZ5" s="79" t="s">
-        <v>2895</v>
+        <v>2894</v>
       </c>
       <c r="FB5" s="79" t="s">
-        <v>2869</v>
+        <v>2868</v>
       </c>
       <c r="FD5" s="79" t="s">
-        <v>2862</v>
+        <v>2861</v>
       </c>
       <c r="FY5" s="79" t="s">
-        <v>2854</v>
+        <v>2853</v>
       </c>
       <c r="FZ5" s="79" t="s">
-        <v>2857</v>
+        <v>2856</v>
       </c>
       <c r="GD5" t="s">
-        <v>2884</v>
+        <v>2883</v>
       </c>
       <c r="GE5" t="s">
-        <v>2868</v>
+        <v>2867</v>
       </c>
       <c r="GF5" s="79" t="s">
-        <v>2868</v>
+        <v>2867</v>
       </c>
       <c r="GG5" s="79" t="s">
         <v>2034</v>
@@ -17230,7 +17267,7 @@
         <v>2034</v>
       </c>
     </row>
-    <row r="6" spans="1:208">
+    <row r="6" spans="1:209">
       <c r="B6" t="s">
         <v>52</v>
       </c>
@@ -17256,7 +17293,7 @@
         <v>59</v>
       </c>
       <c r="J6" t="s">
-        <v>2813</v>
+        <v>2812</v>
       </c>
       <c r="K6" s="34" t="s">
         <v>2067</v>
@@ -17549,28 +17586,28 @@
         <v>2035</v>
       </c>
       <c r="EM6" t="s">
-        <v>2888</v>
+        <v>2887</v>
       </c>
       <c r="EO6" t="s">
-        <v>2900</v>
+        <v>2899</v>
       </c>
       <c r="EZ6" s="79" t="s">
-        <v>2896</v>
+        <v>2895</v>
       </c>
       <c r="FB6" t="s">
         <v>2026</v>
       </c>
       <c r="FD6" s="79" t="s">
-        <v>2865</v>
+        <v>2864</v>
       </c>
       <c r="FZ6" t="s">
-        <v>2855</v>
+        <v>2854</v>
       </c>
       <c r="GE6" t="s">
-        <v>2877</v>
+        <v>2876</v>
       </c>
       <c r="GF6" s="79" t="s">
-        <v>2877</v>
+        <v>2876</v>
       </c>
       <c r="GG6" s="79" t="s">
         <v>2035</v>
@@ -17579,7 +17616,7 @@
         <v>2035</v>
       </c>
     </row>
-    <row r="7" spans="1:208">
+    <row r="7" spans="1:209">
       <c r="B7" t="s">
         <v>63</v>
       </c>
@@ -17865,7 +17902,7 @@
         <v>2562</v>
       </c>
       <c r="DL7" s="20" t="s">
-        <v>2832</v>
+        <v>2831</v>
       </c>
       <c r="EB7" s="79"/>
       <c r="EC7" s="79"/>
@@ -17886,22 +17923,22 @@
         <v>2027</v>
       </c>
       <c r="EM7" t="s">
-        <v>2902</v>
+        <v>2901</v>
       </c>
       <c r="EZ7" s="79" t="s">
-        <v>2897</v>
+        <v>2896</v>
       </c>
       <c r="FB7" t="s">
         <v>2027</v>
       </c>
       <c r="FD7" s="79" t="s">
-        <v>2863</v>
+        <v>2862</v>
       </c>
       <c r="GE7" s="79" t="s">
-        <v>2878</v>
+        <v>2877</v>
       </c>
       <c r="GF7" s="79" t="s">
-        <v>2878</v>
+        <v>2877</v>
       </c>
       <c r="GG7" s="79" t="s">
         <v>2027</v>
@@ -17910,7 +17947,7 @@
         <v>2027</v>
       </c>
     </row>
-    <row r="8" spans="1:208" ht="16.05" customHeight="1">
+    <row r="8" spans="1:209" ht="16.05" customHeight="1">
       <c r="B8" t="s">
         <v>75</v>
       </c>
@@ -18068,7 +18105,7 @@
         <v>2203</v>
       </c>
       <c r="BT8" s="10" t="s">
-        <v>2805</v>
+        <v>2804</v>
       </c>
       <c r="BU8" s="13" t="s">
         <v>2226</v>
@@ -18174,7 +18211,7 @@
         <v>2562</v>
       </c>
       <c r="DL8" s="20" t="s">
-        <v>2833</v>
+        <v>2832</v>
       </c>
       <c r="EE8" s="10" t="s">
         <v>2035</v>
@@ -18192,19 +18229,19 @@
         <v>2036</v>
       </c>
       <c r="EZ8" s="79" t="s">
-        <v>2898</v>
+        <v>2897</v>
       </c>
       <c r="FB8" s="85" t="s">
-        <v>2903</v>
+        <v>2902</v>
       </c>
       <c r="FD8" s="79" t="s">
-        <v>2866</v>
+        <v>2865</v>
       </c>
       <c r="GE8" s="79" t="s">
-        <v>2879</v>
+        <v>2878</v>
       </c>
       <c r="GF8" s="79" t="s">
-        <v>2879</v>
+        <v>2878</v>
       </c>
       <c r="GG8" s="79" t="s">
         <v>2036</v>
@@ -18213,7 +18250,7 @@
         <v>2036</v>
       </c>
     </row>
-    <row r="9" spans="1:208" ht="16.05" customHeight="1">
+    <row r="9" spans="1:209" ht="16.05" customHeight="1">
       <c r="B9" t="s">
         <v>86</v>
       </c>
@@ -18328,13 +18365,13 @@
         <v>2549</v>
       </c>
       <c r="BJ9" s="20" t="s">
-        <v>2797</v>
+        <v>2796</v>
       </c>
       <c r="BK9" s="20" t="s">
         <v>2562</v>
       </c>
       <c r="BL9" s="20" t="s">
-        <v>2798</v>
+        <v>2797</v>
       </c>
       <c r="BM9" s="20" t="s">
         <v>2186</v>
@@ -18355,16 +18392,16 @@
         <v>8</v>
       </c>
       <c r="BS9" s="14" t="s">
-        <v>2906</v>
+        <v>2905</v>
       </c>
       <c r="BT9" s="10" t="s">
-        <v>2806</v>
+        <v>2805</v>
       </c>
       <c r="BU9" s="13" t="s">
         <v>2226</v>
       </c>
       <c r="BV9" s="10" t="s">
-        <v>2807</v>
+        <v>2806</v>
       </c>
       <c r="BW9" s="11" t="s">
         <v>2051</v>
@@ -18398,7 +18435,7 @@
         <v>2266</v>
       </c>
       <c r="CK9" s="42" t="s">
-        <v>2840</v>
+        <v>2839</v>
       </c>
       <c r="CL9" s="12" t="s">
         <v>1799</v>
@@ -18455,16 +18492,16 @@
         <v>2562</v>
       </c>
       <c r="DL9" s="20" t="s">
-        <v>2834</v>
+        <v>2833</v>
       </c>
       <c r="EE9" s="10" t="s">
         <v>2033</v>
       </c>
       <c r="EF9" s="10" t="s">
-        <v>2831</v>
+        <v>2830</v>
       </c>
       <c r="EG9" s="10" t="s">
-        <v>2830</v>
+        <v>2829</v>
       </c>
       <c r="EH9" s="79"/>
       <c r="EI9" s="79"/>
@@ -18473,16 +18510,16 @@
         <v>2026</v>
       </c>
       <c r="EZ9" t="s">
-        <v>2892</v>
+        <v>2891</v>
       </c>
       <c r="FB9" t="s">
-        <v>2870</v>
+        <v>2869</v>
       </c>
       <c r="GE9" t="s">
-        <v>2880</v>
+        <v>2879</v>
       </c>
       <c r="GF9" s="79" t="s">
-        <v>2880</v>
+        <v>2879</v>
       </c>
       <c r="GG9" s="79" t="s">
         <v>2026</v>
@@ -18491,7 +18528,7 @@
         <v>2026</v>
       </c>
     </row>
-    <row r="10" spans="1:208">
+    <row r="10" spans="1:209">
       <c r="B10" t="s">
         <v>95</v>
       </c>
@@ -18598,13 +18635,13 @@
         <v>2550</v>
       </c>
       <c r="BJ10" s="20" t="s">
-        <v>2799</v>
+        <v>2798</v>
       </c>
       <c r="BK10" s="20" t="s">
         <v>2562</v>
       </c>
       <c r="BL10" s="20" t="s">
-        <v>2800</v>
+        <v>2799</v>
       </c>
       <c r="BM10" s="20" t="str">
         <f>_xlfn.CONCAT(BM9,"_error")</f>
@@ -18710,13 +18747,13 @@
       <c r="DH10" s="12"/>
       <c r="DI10" s="12"/>
       <c r="DJ10" s="20" t="s">
-        <v>2797</v>
+        <v>2796</v>
       </c>
       <c r="DK10" s="20" t="s">
         <v>2562</v>
       </c>
       <c r="DL10" s="20" t="s">
-        <v>2835</v>
+        <v>2834</v>
       </c>
       <c r="EE10" s="10" t="s">
         <v>2028</v>
@@ -18742,7 +18779,7 @@
         <v>2181</v>
       </c>
     </row>
-    <row r="11" spans="1:208">
+    <row r="11" spans="1:209">
       <c r="B11" t="s">
         <v>104</v>
       </c>
@@ -18848,13 +18885,13 @@
         <v>2551</v>
       </c>
       <c r="BJ11" s="20" t="s">
-        <v>2801</v>
+        <v>2800</v>
       </c>
       <c r="BK11" s="20" t="s">
         <v>2562</v>
       </c>
       <c r="BL11" s="20" t="s">
-        <v>2802</v>
+        <v>2801</v>
       </c>
       <c r="BM11" s="20" t="s">
         <v>2187</v>
@@ -18957,13 +18994,13 @@
       <c r="DH11" s="12"/>
       <c r="DI11" s="12"/>
       <c r="DJ11" s="20" t="s">
-        <v>2799</v>
+        <v>2798</v>
       </c>
       <c r="DK11" s="20" t="s">
         <v>2562</v>
       </c>
       <c r="DL11" s="20" t="s">
-        <v>2836</v>
+        <v>2835</v>
       </c>
       <c r="EE11" s="10" t="s">
         <v>2205</v>
@@ -18974,10 +19011,10 @@
         <v>2037</v>
       </c>
       <c r="GE11" t="s">
-        <v>2881</v>
+        <v>2880</v>
       </c>
       <c r="GF11" s="79" t="s">
-        <v>2881</v>
+        <v>2880</v>
       </c>
       <c r="GG11" s="79" t="s">
         <v>2037</v>
@@ -18986,7 +19023,7 @@
         <v>2037</v>
       </c>
     </row>
-    <row r="12" spans="1:208">
+    <row r="12" spans="1:209">
       <c r="B12" t="s">
         <v>113</v>
       </c>
@@ -19192,13 +19229,13 @@
       <c r="DH12" s="12"/>
       <c r="DI12" s="12"/>
       <c r="DJ12" s="20" t="s">
-        <v>2801</v>
+        <v>2800</v>
       </c>
       <c r="DK12" s="20" t="s">
         <v>2562</v>
       </c>
       <c r="DL12" s="20" t="s">
-        <v>2837</v>
+        <v>2836</v>
       </c>
       <c r="EE12" s="10" t="s">
         <v>2772</v>
@@ -19221,7 +19258,7 @@
         <v>2038</v>
       </c>
     </row>
-    <row r="13" spans="1:208">
+    <row r="13" spans="1:209">
       <c r="B13" t="s">
         <v>122</v>
       </c>
@@ -19241,7 +19278,7 @@
         <v>127</v>
       </c>
       <c r="J13" t="s">
-        <v>2829</v>
+        <v>2828</v>
       </c>
       <c r="K13" s="34" t="s">
         <v>2073</v>
@@ -19260,7 +19297,7 @@
       </c>
       <c r="U13" s="6"/>
       <c r="V13" s="77" t="s">
-        <v>2828</v>
+        <v>2827</v>
       </c>
       <c r="AB13" s="6" t="s">
         <v>1387</v>
@@ -19415,7 +19452,7 @@
         <v>2769</v>
       </c>
       <c r="DL13" s="20" t="s">
-        <v>2838</v>
+        <v>2837</v>
       </c>
       <c r="EE13" s="10"/>
       <c r="EF13" s="10"/>
@@ -19436,7 +19473,7 @@
         <v>2028</v>
       </c>
     </row>
-    <row r="14" spans="1:208">
+    <row r="14" spans="1:209">
       <c r="B14" t="s">
         <v>130</v>
       </c>
@@ -19456,7 +19493,7 @@
         <v>135</v>
       </c>
       <c r="K14" s="71" t="s">
-        <v>2803</v>
+        <v>2802</v>
       </c>
       <c r="L14" t="s">
         <v>136</v>
@@ -19544,13 +19581,13 @@
         <v>2213</v>
       </c>
       <c r="BT14" s="20" t="s">
-        <v>2808</v>
+        <v>2807</v>
       </c>
       <c r="BU14" s="13" t="s">
         <v>2227</v>
       </c>
       <c r="BV14" s="20" t="s">
-        <v>2809</v>
+        <v>2808</v>
       </c>
       <c r="BW14" s="11" t="s">
         <v>2054</v>
@@ -19625,8 +19662,11 @@
       <c r="GF14" s="79" t="s">
         <v>2027</v>
       </c>
-    </row>
-    <row r="15" spans="1:208">
+      <c r="GH14" t="s">
+        <v>2910</v>
+      </c>
+    </row>
+    <row r="15" spans="1:209">
       <c r="B15" t="s">
         <v>138</v>
       </c>
@@ -19808,7 +19848,7 @@
         <v>2028</v>
       </c>
     </row>
-    <row r="16" spans="1:208">
+    <row r="16" spans="1:209">
       <c r="B16" t="s">
         <v>145</v>
       </c>
@@ -20084,7 +20124,7 @@
         <v>16</v>
       </c>
       <c r="BS17" s="14" t="s">
-        <v>2814</v>
+        <v>2813</v>
       </c>
       <c r="BT17" s="10" t="s">
         <v>2084</v>
@@ -20154,10 +20194,10 @@
       <c r="DK17" s="43"/>
       <c r="DL17" s="43"/>
       <c r="GE17" t="s">
+        <v>2881</v>
+      </c>
+      <c r="GF17" s="79" t="s">
         <v>2882</v>
-      </c>
-      <c r="GF17" s="79" t="s">
-        <v>2883</v>
       </c>
     </row>
     <row r="18" spans="2:188">
@@ -20256,7 +20296,7 @@
         <v>17</v>
       </c>
       <c r="BS18" s="14" t="s">
-        <v>2815</v>
+        <v>2912</v>
       </c>
       <c r="BW18" s="11" t="s">
         <v>2368</v>
@@ -20269,13 +20309,13 @@
       <c r="CA18" s="11"/>
       <c r="CB18" s="11"/>
       <c r="CI18" s="12" t="s">
-        <v>2842</v>
+        <v>2841</v>
       </c>
       <c r="CJ18" s="78" t="s">
         <v>2266</v>
       </c>
       <c r="CK18" s="78" t="s">
-        <v>2839</v>
+        <v>2838</v>
       </c>
       <c r="CL18" s="12" t="s">
         <v>1802</v>
@@ -20413,7 +20453,7 @@
         <v>18</v>
       </c>
       <c r="BS19" s="14" t="s">
-        <v>2816</v>
+        <v>2913</v>
       </c>
       <c r="BW19" s="11" t="s">
         <v>2370</v>
@@ -20425,13 +20465,13 @@
       <c r="CA19" s="11"/>
       <c r="CB19" s="11"/>
       <c r="CI19" s="12" t="s">
-        <v>2843</v>
+        <v>2842</v>
       </c>
       <c r="CJ19" s="78" t="s">
         <v>2266</v>
       </c>
       <c r="CK19" s="78" t="s">
-        <v>2841</v>
+        <v>2840</v>
       </c>
       <c r="CL19" s="12" t="s">
         <v>1803</v>
@@ -20561,13 +20601,13 @@
         <v>2789</v>
       </c>
       <c r="BQ20" s="20" t="s">
-        <v>2796</v>
+        <v>2795</v>
       </c>
       <c r="BR20" s="20">
         <v>19</v>
       </c>
       <c r="BS20" s="14" t="s">
-        <v>2817</v>
+        <v>2814</v>
       </c>
       <c r="BW20" s="11" t="s">
         <v>2369</v>
@@ -20617,10 +20657,10 @@
       <c r="DK20" s="43"/>
       <c r="DL20" s="43"/>
       <c r="GE20" s="10" t="s">
-        <v>2903</v>
+        <v>2902</v>
       </c>
       <c r="GF20" s="10" t="s">
-        <v>2903</v>
+        <v>2902</v>
       </c>
     </row>
     <row r="21" spans="2:188" ht="16.8">
@@ -20698,13 +20738,13 @@
         <v>2527</v>
       </c>
       <c r="BP21" s="14" t="s">
-        <v>2844</v>
+        <v>2843</v>
       </c>
       <c r="BQ21" s="20" t="s">
-        <v>2846</v>
+        <v>2845</v>
       </c>
       <c r="BS21" s="14" t="s">
-        <v>2818</v>
+        <v>2815</v>
       </c>
       <c r="BW21" s="11" t="s">
         <v>2373</v>
@@ -20800,13 +20840,13 @@
         <v>2728</v>
       </c>
       <c r="BP22" s="14" t="s">
-        <v>2845</v>
+        <v>2844</v>
       </c>
       <c r="BQ22" s="20" t="s">
-        <v>2847</v>
+        <v>2846</v>
       </c>
       <c r="BS22" s="14" t="s">
-        <v>2819</v>
+        <v>2816</v>
       </c>
       <c r="BW22" s="11" t="s">
         <v>2573</v>
@@ -20895,13 +20935,13 @@
       </c>
       <c r="BD23" s="17"/>
       <c r="BP23" s="14" t="s">
+        <v>2903</v>
+      </c>
+      <c r="BQ23" s="20" t="s">
         <v>2904</v>
       </c>
-      <c r="BQ23" s="20" t="s">
-        <v>2905</v>
-      </c>
       <c r="BS23" s="14" t="s">
-        <v>2820</v>
+        <v>2817</v>
       </c>
       <c r="BW23" s="11" t="s">
         <v>2574</v>
@@ -20995,7 +21035,7 @@
       </c>
       <c r="BD24" s="17"/>
       <c r="BS24" s="14" t="s">
-        <v>2821</v>
+        <v>2818</v>
       </c>
       <c r="BW24" s="11" t="s">
         <v>2575</v>
@@ -21084,7 +21124,7 @@
       </c>
       <c r="BD25" s="17"/>
       <c r="BS25" s="14" t="s">
-        <v>2822</v>
+        <v>2819</v>
       </c>
       <c r="BW25" s="11" t="s">
         <v>2576</v>
@@ -21172,7 +21212,7 @@
       </c>
       <c r="BD26" s="17"/>
       <c r="BS26" s="14" t="s">
-        <v>2823</v>
+        <v>2820</v>
       </c>
       <c r="BW26" s="11" t="s">
         <v>1765</v>
@@ -21253,7 +21293,7 @@
         <v>1941</v>
       </c>
       <c r="BS27" s="14" t="s">
-        <v>2824</v>
+        <v>2821</v>
       </c>
       <c r="BW27" s="11" t="s">
         <v>1775</v>
@@ -21334,7 +21374,7 @@
         <v>1655</v>
       </c>
       <c r="BS28" s="14" t="s">
-        <v>2825</v>
+        <v>2822</v>
       </c>
       <c r="BW28" s="11" t="s">
         <v>2732</v>
@@ -21412,7 +21452,7 @@
         <v>1678</v>
       </c>
       <c r="BS29" s="14" t="s">
-        <v>2826</v>
+        <v>2823</v>
       </c>
       <c r="BW29" s="20"/>
       <c r="BX29" s="14"/>
@@ -21477,6 +21517,9 @@
       <c r="BC30" s="6" t="s">
         <v>1679</v>
       </c>
+      <c r="BS30" s="14" t="s">
+        <v>2824</v>
+      </c>
       <c r="BW30" s="14"/>
       <c r="BX30" s="14"/>
       <c r="BY30" s="14"/>
@@ -21537,6 +21580,9 @@
       </c>
       <c r="BC31" s="6" t="s">
         <v>1677</v>
+      </c>
+      <c r="BS31" s="14" t="s">
+        <v>2825</v>
       </c>
       <c r="BW31" s="14"/>
       <c r="BX31" s="14"/>
@@ -27232,6 +27278,7 @@
       <c r="CR277" s="42"/>
     </row>
   </sheetData>
+  <sheetProtection algorithmName="SHA-512" hashValue="3XX+/3s4rJIBJDTVCYLw0fNZauFUWCslks+LT4Sr0dEiohOsA3vGHkUvFgnzhkAfFIKqf0fYwVKHSvxLahk7Gg==" saltValue="TUnFDCPoM9+Z4g2t00k2dg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="2">
     <mergeCell ref="M27:M28"/>
     <mergeCell ref="M34:M35"/>

</xml_diff>

<commit_message>
Modified the column header of "georeferenced coordinates" to non-capitalized
</commit_message>
<xml_diff>
--- a/Excel_templates/MOSAIC_input_excel_file_2022.xlsx
+++ b/Excel_templates/MOSAIC_input_excel_file_2022.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sparadis\Documents\ETH\MOSAIC\MOSAIC_Client\Excel_templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAA44C3C-AEAD-4938-B53B-7121451E0B1D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6730288B-F4CF-4CD6-A66F-B7E18BCA2D57}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30204" yWindow="10044" windowWidth="40020" windowHeight="22296" tabRatio="694" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30204" yWindow="10044" windowWidth="40020" windowHeight="22296" tabRatio="694" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ARTICLE_AUTHOR" sheetId="3" r:id="rId1"/>
@@ -107,7 +107,7 @@
     <definedName name="porosity">SET_VARIABLES!$EO$2:$EO$6</definedName>
     <definedName name="Portugal">SET_VARIABLES!$AT$4:$AT$14</definedName>
     <definedName name="Ra224_Bq_kg">SET_VARIABLES!$GD$2:$GD$5</definedName>
-    <definedName name="Ra226_Bq_kg">SET_VARIABLES!$FY$2:$FY$5</definedName>
+    <definedName name="Ra226_Bq_kg">SET_VARIABLES!$FY$2:$FY$6</definedName>
     <definedName name="Republic_of_Korea">SET_VARIABLES!$AV$2:$AV$6</definedName>
     <definedName name="Research_Vessel_Countries">SET_VARIABLES!$O$2:$O$44</definedName>
     <definedName name="Romania">SET_VARIABLES!$AU$2:$AU$4</definedName>
@@ -195,7 +195,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3738" uniqueCount="2915">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3739" uniqueCount="2916">
   <si>
     <t>sample_name</t>
   </si>
@@ -8897,9 +8897,6 @@
     <t>Mercury</t>
   </si>
   <si>
-    <t>Georeferenced coordinates</t>
-  </si>
-  <si>
     <t>manometric</t>
   </si>
   <si>
@@ -8940,6 +8937,12 @@
   </si>
   <si>
     <t>Mass spect.</t>
+  </si>
+  <si>
+    <t>LSC</t>
+  </si>
+  <si>
+    <t>georeferenced coordinates</t>
   </si>
 </sst>
 </file>
@@ -9974,11 +9977,11 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -10067,7 +10070,7 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:P15"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -10128,7 +10131,7 @@
         <v>1824</v>
       </c>
       <c r="E2" s="57" t="s">
-        <v>2900</v>
+        <v>2915</v>
       </c>
       <c r="F2" s="60" t="s">
         <v>1825</v>
@@ -11937,7 +11940,7 @@
         <v>1840</v>
       </c>
       <c r="O2" s="75" t="s">
-        <v>2911</v>
+        <v>2910</v>
       </c>
       <c r="P2" s="75" t="s">
         <v>2710</v>
@@ -14572,8 +14575,8 @@
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:HA277"/>
   <sheetViews>
-    <sheetView topLeftCell="GF1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="GP14" sqref="GP14"/>
+    <sheetView topLeftCell="FQ1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="FZ17" sqref="FZ17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -15286,7 +15289,7 @@
         <v>2473</v>
       </c>
       <c r="GU1" s="22" t="s">
-        <v>2907</v>
+        <v>2906</v>
       </c>
       <c r="GV1" s="22" t="s">
         <v>2463</v>
@@ -15304,7 +15307,7 @@
         <v>2791</v>
       </c>
       <c r="HA1" s="22" t="s">
-        <v>2911</v>
+        <v>2910</v>
       </c>
     </row>
     <row r="2" spans="1:209">
@@ -15633,7 +15636,7 @@
         <v>2462</v>
       </c>
       <c r="DH2" s="12" t="s">
-        <v>2906</v>
+        <v>2905</v>
       </c>
       <c r="DI2" s="12"/>
       <c r="DJ2" s="12" t="s">
@@ -15901,13 +15904,13 @@
         <v>5</v>
       </c>
       <c r="GY2" s="10" t="s">
-        <v>2914</v>
+        <v>2913</v>
       </c>
       <c r="GZ2" s="10" t="s">
-        <v>2914</v>
+        <v>2913</v>
       </c>
       <c r="HA2" s="10" t="s">
-        <v>2914</v>
+        <v>2913</v>
       </c>
     </row>
     <row r="3" spans="1:209">
@@ -16735,13 +16738,13 @@
         <v>2406</v>
       </c>
       <c r="DG4" s="12" t="s">
+        <v>2906</v>
+      </c>
+      <c r="DH4" s="46" t="s">
         <v>2907</v>
       </c>
-      <c r="DH4" s="46" t="s">
+      <c r="DI4" s="12" t="s">
         <v>2908</v>
-      </c>
-      <c r="DI4" s="12" t="s">
-        <v>2909</v>
       </c>
       <c r="DJ4" s="12" t="s">
         <v>2512</v>
@@ -16762,7 +16765,7 @@
         <v>2786</v>
       </c>
       <c r="DV4" t="s">
-        <v>2911</v>
+        <v>2910</v>
       </c>
       <c r="DW4" t="s">
         <v>2794</v>
@@ -17600,6 +17603,9 @@
       <c r="FD6" s="79" t="s">
         <v>2864</v>
       </c>
+      <c r="FY6" t="s">
+        <v>2914</v>
+      </c>
       <c r="FZ6" t="s">
         <v>2854</v>
       </c>
@@ -17923,7 +17929,7 @@
         <v>2027</v>
       </c>
       <c r="EM7" t="s">
-        <v>2901</v>
+        <v>2900</v>
       </c>
       <c r="EZ7" s="79" t="s">
         <v>2896</v>
@@ -18232,7 +18238,7 @@
         <v>2897</v>
       </c>
       <c r="FB8" s="85" t="s">
-        <v>2902</v>
+        <v>2901</v>
       </c>
       <c r="FD8" s="79" t="s">
         <v>2865</v>
@@ -18392,7 +18398,7 @@
         <v>8</v>
       </c>
       <c r="BS9" s="14" t="s">
-        <v>2905</v>
+        <v>2904</v>
       </c>
       <c r="BT9" s="10" t="s">
         <v>2805</v>
@@ -19663,7 +19669,7 @@
         <v>2027</v>
       </c>
       <c r="GH14" t="s">
-        <v>2910</v>
+        <v>2909</v>
       </c>
     </row>
     <row r="15" spans="1:209">
@@ -20296,7 +20302,7 @@
         <v>17</v>
       </c>
       <c r="BS18" s="14" t="s">
-        <v>2912</v>
+        <v>2911</v>
       </c>
       <c r="BW18" s="11" t="s">
         <v>2368</v>
@@ -20453,7 +20459,7 @@
         <v>18</v>
       </c>
       <c r="BS19" s="14" t="s">
-        <v>2913</v>
+        <v>2912</v>
       </c>
       <c r="BW19" s="11" t="s">
         <v>2370</v>
@@ -20657,10 +20663,10 @@
       <c r="DK20" s="43"/>
       <c r="DL20" s="43"/>
       <c r="GE20" s="10" t="s">
-        <v>2902</v>
+        <v>2901</v>
       </c>
       <c r="GF20" s="10" t="s">
-        <v>2902</v>
+        <v>2901</v>
       </c>
     </row>
     <row r="21" spans="2:188" ht="16.8">
@@ -20935,10 +20941,10 @@
       </c>
       <c r="BD23" s="17"/>
       <c r="BP23" s="14" t="s">
+        <v>2902</v>
+      </c>
+      <c r="BQ23" s="20" t="s">
         <v>2903</v>
-      </c>
-      <c r="BQ23" s="20" t="s">
-        <v>2904</v>
       </c>
       <c r="BS23" s="14" t="s">
         <v>2817</v>
@@ -27278,7 +27284,7 @@
       <c r="CR277" s="42"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="3XX+/3s4rJIBJDTVCYLw0fNZauFUWCslks+LT4Sr0dEiohOsA3vGHkUvFgnzhkAfFIKqf0fYwVKHSvxLahk7Gg==" saltValue="TUnFDCPoM9+Z4g2t00k2dg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="AMZCrMs69nSm9O/05DTsgjJuLM1GiMwf/Fs2/F3EKTpWTai7Xpu9vWxu0/MRfCxo4udsypiKCQgGDle1UioXPQ==" saltValue="MyLIjiD4CiwlmFGszxWiIw==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="2">
     <mergeCell ref="M27:M28"/>
     <mergeCell ref="M34:M35"/>

</xml_diff>

<commit_message>
Modified the column header of "georeferenced coordinates" to "georeferenced_coordinates" (no space)
</commit_message>
<xml_diff>
--- a/Excel_templates/MOSAIC_input_excel_file_2022.xlsx
+++ b/Excel_templates/MOSAIC_input_excel_file_2022.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sparadis\Documents\ETH\MOSAIC\MOSAIC_Client\Excel_templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6730288B-F4CF-4CD6-A66F-B7E18BCA2D57}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{815373EA-590C-4E87-A88E-504E9BE6FE1E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30204" yWindow="10044" windowWidth="40020" windowHeight="22296" tabRatio="694" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30204" yWindow="10044" windowWidth="40020" windowHeight="22296" tabRatio="694" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ARTICLE_AUTHOR" sheetId="3" r:id="rId1"/>
@@ -8942,7 +8942,7 @@
     <t>LSC</t>
   </si>
   <si>
-    <t>georeferenced coordinates</t>
+    <t>georeferenced_coordinates</t>
   </si>
 </sst>
 </file>
@@ -9977,7 +9977,7 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -10070,7 +10070,7 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:P15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>

</xml_diff>

<commit_message>
Added pore_water to material_analyzed
</commit_message>
<xml_diff>
--- a/Excel_templates/MOSAIC_input_excel_file_2022.xlsx
+++ b/Excel_templates/MOSAIC_input_excel_file_2022.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sparadis\Documents\ETH\MOSAIC\MOSAIC_Client\Excel_templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAC0A304-8572-4910-AEAC-1EAAD06009A3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9F934F2-4D37-4063-80F6-8CC5968A0691}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="30204" yWindow="10044" windowWidth="40020" windowHeight="22296" tabRatio="694" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -82,7 +82,7 @@
     <definedName name="MAR_g_cm2_yr">SET_VARIABLES!$GE$2:$GE$20</definedName>
     <definedName name="MAR_model">SET_VARIABLES!#REF!</definedName>
     <definedName name="MAR_tracer">SET_VARIABLES!#REF!</definedName>
-    <definedName name="material_analyzed">SET_VARIABLES!$BS$2:$BS$31</definedName>
+    <definedName name="material_analyzed">SET_VARIABLES!$BS$2:$BS$32</definedName>
     <definedName name="Mauritania">SET_VARIABLES!$AL$2:$AL$7</definedName>
     <definedName name="mean_grain_size_microm">SET_VARIABLES!$EW$2:$EW$4</definedName>
     <definedName name="median_grain_size_microm">SET_VARIABLES!$EX$2:$EX$4</definedName>
@@ -195,7 +195,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3740" uniqueCount="2916">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3741" uniqueCount="2917">
   <si>
     <t>sample_name</t>
   </si>
@@ -8943,6 +8943,9 @@
   </si>
   <si>
     <t>georeferenced_coordinates</t>
+  </si>
+  <si>
+    <t>pore_water</t>
   </si>
 </sst>
 </file>
@@ -9539,6 +9542,23 @@
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="4" borderId="4" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
@@ -9625,23 +9645,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="16">
     <cellStyle name="20% - Accent1" xfId="3" builtinId="30" customBuiltin="1"/>
@@ -10006,15 +10009,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="57" customFormat="1" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="82" t="s">
+      <c r="A1" s="88" t="s">
         <v>2577</v>
       </c>
-      <c r="B1" s="82"/>
-      <c r="C1" s="82"/>
-      <c r="D1" s="82"/>
-      <c r="E1" s="82"/>
-      <c r="F1" s="82"/>
-      <c r="G1" s="82"/>
+      <c r="B1" s="88"/>
+      <c r="C1" s="88"/>
+      <c r="D1" s="88"/>
+      <c r="E1" s="88"/>
+      <c r="F1" s="88"/>
+      <c r="G1" s="88"/>
     </row>
     <row r="2" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="47" t="s">
@@ -10087,43 +10090,43 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.69921875" style="110" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22" style="110" customWidth="1"/>
-    <col min="3" max="5" width="10.796875" style="110" customWidth="1"/>
-    <col min="6" max="6" width="13.19921875" style="112" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15" style="114" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15" style="114" customWidth="1"/>
-    <col min="9" max="9" width="28.3984375" style="110" customWidth="1"/>
-    <col min="10" max="10" width="23.296875" style="110" customWidth="1"/>
-    <col min="11" max="11" width="16.8984375" style="110" customWidth="1"/>
-    <col min="12" max="14" width="24.796875" style="110" customWidth="1"/>
-    <col min="15" max="15" width="27.8984375" style="110" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="27.8984375" style="110" customWidth="1"/>
-    <col min="17" max="17" width="10.796875" style="110" customWidth="1"/>
-    <col min="18" max="16384" width="11.19921875" style="110"/>
+    <col min="1" max="1" width="15.69921875" style="82" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22" style="82" customWidth="1"/>
+    <col min="3" max="5" width="10.796875" style="82" customWidth="1"/>
+    <col min="6" max="6" width="13.19921875" style="84" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15" style="86" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15" style="86" customWidth="1"/>
+    <col min="9" max="9" width="28.3984375" style="82" customWidth="1"/>
+    <col min="10" max="10" width="23.296875" style="82" customWidth="1"/>
+    <col min="11" max="11" width="16.8984375" style="82" customWidth="1"/>
+    <col min="12" max="14" width="24.796875" style="82" customWidth="1"/>
+    <col min="15" max="15" width="27.8984375" style="82" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="27.8984375" style="82" customWidth="1"/>
+    <col min="17" max="17" width="10.796875" style="82" customWidth="1"/>
+    <col min="18" max="16384" width="11.19921875" style="82"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" s="56" customFormat="1" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="84" t="s">
+      <c r="A1" s="90" t="s">
         <v>2578</v>
       </c>
-      <c r="B1" s="84"/>
-      <c r="C1" s="84"/>
-      <c r="D1" s="84"/>
-      <c r="E1" s="84"/>
-      <c r="F1" s="83" t="s">
+      <c r="B1" s="90"/>
+      <c r="C1" s="90"/>
+      <c r="D1" s="90"/>
+      <c r="E1" s="90"/>
+      <c r="F1" s="89" t="s">
         <v>2716</v>
       </c>
-      <c r="G1" s="83"/>
-      <c r="H1" s="83"/>
-      <c r="I1" s="83"/>
-      <c r="J1" s="83"/>
-      <c r="K1" s="83"/>
-      <c r="L1" s="83"/>
-      <c r="M1" s="83"/>
-      <c r="N1" s="83"/>
-      <c r="O1" s="83"/>
-      <c r="P1" s="83"/>
+      <c r="G1" s="89"/>
+      <c r="H1" s="89"/>
+      <c r="I1" s="89"/>
+      <c r="J1" s="89"/>
+      <c r="K1" s="89"/>
+      <c r="L1" s="89"/>
+      <c r="M1" s="89"/>
+      <c r="N1" s="89"/>
+      <c r="O1" s="89"/>
+      <c r="P1" s="89"/>
     </row>
     <row r="2" spans="1:16" s="59" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="55" t="s">
@@ -10176,97 +10179,97 @@
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="C3" s="111"/>
-      <c r="D3" s="111"/>
-      <c r="E3" s="111"/>
-      <c r="G3" s="113"/>
-      <c r="N3" s="115"/>
-      <c r="O3" s="112"/>
-      <c r="P3" s="112"/>
+      <c r="C3" s="83"/>
+      <c r="D3" s="83"/>
+      <c r="E3" s="83"/>
+      <c r="G3" s="85"/>
+      <c r="N3" s="87"/>
+      <c r="O3" s="84"/>
+      <c r="P3" s="84"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="B4" s="111"/>
-      <c r="C4" s="111"/>
-      <c r="D4" s="111"/>
-      <c r="E4" s="111"/>
-      <c r="G4" s="111"/>
+      <c r="B4" s="83"/>
+      <c r="C4" s="83"/>
+      <c r="D4" s="83"/>
+      <c r="E4" s="83"/>
+      <c r="G4" s="83"/>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="B5" s="111"/>
-      <c r="C5" s="111"/>
-      <c r="D5" s="111"/>
-      <c r="E5" s="111"/>
-      <c r="G5" s="111"/>
+      <c r="B5" s="83"/>
+      <c r="C5" s="83"/>
+      <c r="D5" s="83"/>
+      <c r="E5" s="83"/>
+      <c r="G5" s="83"/>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="B6" s="111"/>
-      <c r="C6" s="111"/>
-      <c r="D6" s="111"/>
-      <c r="E6" s="111"/>
-      <c r="G6" s="111"/>
+      <c r="B6" s="83"/>
+      <c r="C6" s="83"/>
+      <c r="D6" s="83"/>
+      <c r="E6" s="83"/>
+      <c r="G6" s="83"/>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="B7" s="111"/>
-      <c r="C7" s="111"/>
-      <c r="D7" s="111"/>
-      <c r="E7" s="111"/>
-      <c r="G7" s="111"/>
+      <c r="B7" s="83"/>
+      <c r="C7" s="83"/>
+      <c r="D7" s="83"/>
+      <c r="E7" s="83"/>
+      <c r="G7" s="83"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="B8" s="111"/>
-      <c r="C8" s="111"/>
-      <c r="D8" s="111"/>
-      <c r="E8" s="111"/>
-      <c r="G8" s="111"/>
+      <c r="B8" s="83"/>
+      <c r="C8" s="83"/>
+      <c r="D8" s="83"/>
+      <c r="E8" s="83"/>
+      <c r="G8" s="83"/>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="B9" s="111"/>
-      <c r="C9" s="111"/>
-      <c r="D9" s="111"/>
-      <c r="E9" s="111"/>
-      <c r="G9" s="111"/>
+      <c r="B9" s="83"/>
+      <c r="C9" s="83"/>
+      <c r="D9" s="83"/>
+      <c r="E9" s="83"/>
+      <c r="G9" s="83"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="B10" s="111"/>
-      <c r="C10" s="111"/>
-      <c r="D10" s="111"/>
-      <c r="E10" s="111"/>
-      <c r="G10" s="111"/>
+      <c r="B10" s="83"/>
+      <c r="C10" s="83"/>
+      <c r="D10" s="83"/>
+      <c r="E10" s="83"/>
+      <c r="G10" s="83"/>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="B11" s="111"/>
-      <c r="C11" s="111"/>
-      <c r="D11" s="111"/>
-      <c r="E11" s="111"/>
-      <c r="G11" s="111"/>
+      <c r="B11" s="83"/>
+      <c r="C11" s="83"/>
+      <c r="D11" s="83"/>
+      <c r="E11" s="83"/>
+      <c r="G11" s="83"/>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="B12" s="111"/>
-      <c r="C12" s="111"/>
-      <c r="D12" s="111"/>
-      <c r="E12" s="111"/>
-      <c r="G12" s="111"/>
+      <c r="B12" s="83"/>
+      <c r="C12" s="83"/>
+      <c r="D12" s="83"/>
+      <c r="E12" s="83"/>
+      <c r="G12" s="83"/>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="B13" s="111"/>
-      <c r="C13" s="111"/>
-      <c r="D13" s="111"/>
-      <c r="E13" s="111"/>
-      <c r="G13" s="111"/>
+      <c r="B13" s="83"/>
+      <c r="C13" s="83"/>
+      <c r="D13" s="83"/>
+      <c r="E13" s="83"/>
+      <c r="G13" s="83"/>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="B14" s="111"/>
-      <c r="C14" s="111"/>
-      <c r="D14" s="111"/>
-      <c r="E14" s="111"/>
-      <c r="G14" s="111"/>
+      <c r="B14" s="83"/>
+      <c r="C14" s="83"/>
+      <c r="D14" s="83"/>
+      <c r="E14" s="83"/>
+      <c r="G14" s="83"/>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="B15" s="111"/>
-      <c r="C15" s="111"/>
-      <c r="D15" s="111"/>
-      <c r="E15" s="111"/>
-      <c r="G15" s="111"/>
+      <c r="B15" s="83"/>
+      <c r="C15" s="83"/>
+      <c r="D15" s="83"/>
+      <c r="E15" s="83"/>
+      <c r="G15" s="83"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -10368,37 +10371,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:35" s="48" customFormat="1" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="85" t="s">
+      <c r="A1" s="91" t="s">
         <v>2580</v>
       </c>
-      <c r="B1" s="85"/>
-      <c r="C1" s="85" t="s">
+      <c r="B1" s="91"/>
+      <c r="C1" s="91" t="s">
         <v>2579</v>
       </c>
-      <c r="D1" s="85"/>
-      <c r="E1" s="85"/>
-      <c r="F1" s="85"/>
+      <c r="D1" s="91"/>
+      <c r="E1" s="91"/>
+      <c r="F1" s="91"/>
       <c r="G1" s="48" t="s">
         <v>2183</v>
       </c>
     </row>
     <row r="2" spans="1:35" ht="15.6" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="86" t="s">
+      <c r="A2" s="92" t="s">
         <v>2510</v>
       </c>
-      <c r="B2" s="86" t="s">
+      <c r="B2" s="92" t="s">
         <v>1822</v>
       </c>
-      <c r="C2" s="86" t="s">
+      <c r="C2" s="92" t="s">
         <v>1831</v>
       </c>
-      <c r="D2" s="86" t="s">
+      <c r="D2" s="92" t="s">
         <v>2587</v>
       </c>
-      <c r="E2" s="86" t="s">
+      <c r="E2" s="92" t="s">
         <v>1820</v>
       </c>
-      <c r="F2" s="89" t="s">
+      <c r="F2" s="95" t="s">
         <v>1821</v>
       </c>
       <c r="G2" s="49" t="s">
@@ -10434,12 +10437,12 @@
       <c r="AI2" s="49"/>
     </row>
     <row r="3" spans="1:35" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="87"/>
-      <c r="B3" s="87"/>
-      <c r="C3" s="87"/>
-      <c r="D3" s="87"/>
-      <c r="E3" s="87"/>
-      <c r="F3" s="90"/>
+      <c r="A3" s="93"/>
+      <c r="B3" s="93"/>
+      <c r="C3" s="93"/>
+      <c r="D3" s="93"/>
+      <c r="E3" s="93"/>
+      <c r="F3" s="96"/>
       <c r="G3" s="49"/>
       <c r="H3" s="49"/>
       <c r="I3" s="49"/>
@@ -10471,12 +10474,12 @@
       <c r="AI3" s="49"/>
     </row>
     <row r="4" spans="1:35" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="87"/>
-      <c r="B4" s="87"/>
-      <c r="C4" s="87"/>
-      <c r="D4" s="87"/>
-      <c r="E4" s="87"/>
-      <c r="F4" s="90"/>
+      <c r="A4" s="93"/>
+      <c r="B4" s="93"/>
+      <c r="C4" s="93"/>
+      <c r="D4" s="93"/>
+      <c r="E4" s="93"/>
+      <c r="F4" s="96"/>
       <c r="G4" s="49"/>
       <c r="H4" s="49"/>
       <c r="I4" s="49"/>
@@ -10508,12 +10511,12 @@
       <c r="AI4" s="49"/>
     </row>
     <row r="5" spans="1:35" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="88"/>
-      <c r="B5" s="88"/>
-      <c r="C5" s="88"/>
-      <c r="D5" s="88"/>
-      <c r="E5" s="88"/>
-      <c r="F5" s="90"/>
+      <c r="A5" s="94"/>
+      <c r="B5" s="94"/>
+      <c r="C5" s="94"/>
+      <c r="D5" s="94"/>
+      <c r="E5" s="94"/>
+      <c r="F5" s="96"/>
       <c r="G5" s="49"/>
       <c r="H5" s="49"/>
       <c r="I5" s="49"/>
@@ -10545,12 +10548,12 @@
       <c r="AI5" s="49"/>
     </row>
     <row r="6" spans="1:35" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="88"/>
-      <c r="B6" s="88"/>
-      <c r="C6" s="88"/>
-      <c r="D6" s="88"/>
-      <c r="E6" s="88"/>
-      <c r="F6" s="90"/>
+      <c r="A6" s="94"/>
+      <c r="B6" s="94"/>
+      <c r="C6" s="94"/>
+      <c r="D6" s="94"/>
+      <c r="E6" s="94"/>
+      <c r="F6" s="96"/>
       <c r="G6" s="49"/>
       <c r="H6" s="49"/>
       <c r="I6" s="49"/>
@@ -11847,10 +11850,10 @@
   <dimension ref="A1:CB52"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="3" ySplit="6" topLeftCell="D7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="6" topLeftCell="H7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="H12" sqref="H12"/>
+      <selection pane="bottomRight" activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -11871,25 +11874,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:80" s="72" customFormat="1" ht="20.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="91" t="s">
+      <c r="A1" s="97" t="s">
         <v>2589</v>
       </c>
-      <c r="B1" s="92"/>
-      <c r="C1" s="93"/>
-      <c r="D1" s="91" t="s">
+      <c r="B1" s="98"/>
+      <c r="C1" s="99"/>
+      <c r="D1" s="97" t="s">
         <v>2579</v>
       </c>
-      <c r="E1" s="92"/>
-      <c r="F1" s="92"/>
-      <c r="G1" s="93"/>
-      <c r="H1" s="94" t="s">
+      <c r="E1" s="98"/>
+      <c r="F1" s="98"/>
+      <c r="G1" s="99"/>
+      <c r="H1" s="100" t="s">
         <v>2581</v>
       </c>
-      <c r="I1" s="95"/>
-      <c r="J1" s="95"/>
-      <c r="K1" s="96"/>
+      <c r="I1" s="101"/>
+      <c r="J1" s="101"/>
+      <c r="K1" s="102"/>
       <c r="L1" s="72" t="s">
-        <v>2778</v>
+        <v>1837</v>
       </c>
       <c r="M1" s="72" t="s">
         <v>1837</v>
@@ -11905,44 +11908,44 @@
       </c>
     </row>
     <row r="2" spans="1:80" s="74" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A2" s="97" t="s">
+      <c r="A2" s="103" t="s">
         <v>2510</v>
       </c>
-      <c r="B2" s="100" t="s">
+      <c r="B2" s="106" t="s">
         <v>1822</v>
       </c>
-      <c r="C2" s="103" t="s">
+      <c r="C2" s="109" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="98" t="s">
+      <c r="D2" s="104" t="s">
         <v>1831</v>
       </c>
-      <c r="E2" s="101" t="s">
+      <c r="E2" s="107" t="s">
         <v>2587</v>
       </c>
-      <c r="F2" s="101" t="s">
+      <c r="F2" s="107" t="s">
         <v>1820</v>
       </c>
-      <c r="G2" s="104" t="s">
+      <c r="G2" s="110" t="s">
         <v>1821</v>
       </c>
-      <c r="H2" s="97" t="s">
+      <c r="H2" s="103" t="s">
         <v>1832</v>
       </c>
-      <c r="I2" s="100" t="s">
+      <c r="I2" s="106" t="s">
         <v>1833</v>
       </c>
-      <c r="J2" s="100" t="s">
+      <c r="J2" s="106" t="s">
         <v>1834</v>
       </c>
-      <c r="K2" s="106" t="s">
+      <c r="K2" s="112" t="s">
         <v>1835</v>
       </c>
       <c r="L2" s="73" t="s">
-        <v>2123</v>
+        <v>2048</v>
       </c>
       <c r="M2" s="73" t="s">
-        <v>2048</v>
+        <v>1</v>
       </c>
       <c r="N2" s="73" t="s">
         <v>1840</v>
@@ -12019,19 +12022,19 @@
       <c r="CB2" s="73"/>
     </row>
     <row r="3" spans="1:80" s="74" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A3" s="98"/>
-      <c r="B3" s="101"/>
-      <c r="C3" s="104"/>
-      <c r="D3" s="98"/>
-      <c r="E3" s="101"/>
-      <c r="F3" s="101"/>
-      <c r="G3" s="104"/>
-      <c r="H3" s="98"/>
-      <c r="I3" s="101"/>
-      <c r="J3" s="101"/>
-      <c r="K3" s="107"/>
+      <c r="A3" s="104"/>
+      <c r="B3" s="107"/>
+      <c r="C3" s="110"/>
+      <c r="D3" s="104"/>
+      <c r="E3" s="107"/>
+      <c r="F3" s="107"/>
+      <c r="G3" s="110"/>
+      <c r="H3" s="104"/>
+      <c r="I3" s="107"/>
+      <c r="J3" s="107"/>
+      <c r="K3" s="113"/>
       <c r="L3" s="73" t="s">
-        <v>2866</v>
+        <v>2826</v>
       </c>
       <c r="M3" s="73" t="s">
         <v>2870</v>
@@ -12105,17 +12108,17 @@
       <c r="CB3" s="73"/>
     </row>
     <row r="4" spans="1:80" s="74" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="98"/>
-      <c r="B4" s="101"/>
-      <c r="C4" s="104"/>
-      <c r="D4" s="98"/>
-      <c r="E4" s="101"/>
-      <c r="F4" s="101"/>
-      <c r="G4" s="104"/>
-      <c r="H4" s="98"/>
-      <c r="I4" s="101"/>
-      <c r="J4" s="101"/>
-      <c r="K4" s="107"/>
+      <c r="A4" s="104"/>
+      <c r="B4" s="107"/>
+      <c r="C4" s="110"/>
+      <c r="D4" s="104"/>
+      <c r="E4" s="107"/>
+      <c r="F4" s="107"/>
+      <c r="G4" s="110"/>
+      <c r="H4" s="104"/>
+      <c r="I4" s="107"/>
+      <c r="J4" s="107"/>
+      <c r="K4" s="113"/>
       <c r="L4" s="73"/>
       <c r="M4" s="73"/>
       <c r="N4" s="73"/>
@@ -12187,17 +12190,17 @@
       <c r="CB4" s="73"/>
     </row>
     <row r="5" spans="1:80" s="74" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="98"/>
-      <c r="B5" s="101"/>
-      <c r="C5" s="104"/>
-      <c r="D5" s="98"/>
-      <c r="E5" s="101"/>
-      <c r="F5" s="101"/>
-      <c r="G5" s="104"/>
-      <c r="H5" s="98"/>
-      <c r="I5" s="101"/>
-      <c r="J5" s="101"/>
-      <c r="K5" s="107"/>
+      <c r="A5" s="104"/>
+      <c r="B5" s="107"/>
+      <c r="C5" s="110"/>
+      <c r="D5" s="104"/>
+      <c r="E5" s="107"/>
+      <c r="F5" s="107"/>
+      <c r="G5" s="110"/>
+      <c r="H5" s="104"/>
+      <c r="I5" s="107"/>
+      <c r="J5" s="107"/>
+      <c r="K5" s="113"/>
       <c r="L5" s="73"/>
       <c r="M5" s="73"/>
       <c r="N5" s="73"/>
@@ -12269,17 +12272,17 @@
       <c r="CB5" s="73"/>
     </row>
     <row r="6" spans="1:80" s="74" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="99"/>
-      <c r="B6" s="102"/>
-      <c r="C6" s="105"/>
-      <c r="D6" s="99"/>
-      <c r="E6" s="102"/>
-      <c r="F6" s="102"/>
-      <c r="G6" s="105"/>
-      <c r="H6" s="99"/>
-      <c r="I6" s="102"/>
-      <c r="J6" s="102"/>
-      <c r="K6" s="108"/>
+      <c r="A6" s="105"/>
+      <c r="B6" s="108"/>
+      <c r="C6" s="111"/>
+      <c r="D6" s="105"/>
+      <c r="E6" s="108"/>
+      <c r="F6" s="108"/>
+      <c r="G6" s="111"/>
+      <c r="H6" s="105"/>
+      <c r="I6" s="108"/>
+      <c r="J6" s="108"/>
+      <c r="K6" s="114"/>
       <c r="L6" s="73"/>
       <c r="M6" s="73"/>
       <c r="N6" s="73"/>
@@ -14583,8 +14586,8 @@
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:HA277"/>
   <sheetViews>
-    <sheetView topLeftCell="EX1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="FK4" sqref="FK4"/>
+    <sheetView topLeftCell="BQ1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="BS11" sqref="BS11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -18929,7 +18932,7 @@
         <v>10</v>
       </c>
       <c r="BS11" s="14" t="s">
-        <v>2205</v>
+        <v>2916</v>
       </c>
       <c r="BT11" s="10" t="s">
         <v>1846</v>
@@ -19171,7 +19174,7 @@
         <v>11</v>
       </c>
       <c r="BS12" s="14" t="s">
-        <v>2211</v>
+        <v>2205</v>
       </c>
       <c r="BT12" s="10" t="s">
         <v>2738</v>
@@ -19391,7 +19394,7 @@
         <v>12</v>
       </c>
       <c r="BS13" s="14" t="s">
-        <v>2212</v>
+        <v>2211</v>
       </c>
       <c r="BT13" s="10" t="s">
         <v>2747</v>
@@ -19595,7 +19598,7 @@
         <v>13</v>
       </c>
       <c r="BS14" s="14" t="s">
-        <v>2213</v>
+        <v>2212</v>
       </c>
       <c r="BT14" s="20" t="s">
         <v>2807</v>
@@ -19780,7 +19783,7 @@
         <v>14</v>
       </c>
       <c r="BS15" s="14" t="s">
-        <v>2214</v>
+        <v>2213</v>
       </c>
       <c r="BT15" s="10" t="s">
         <v>2058</v>
@@ -19964,7 +19967,7 @@
         <v>15</v>
       </c>
       <c r="BS16" s="14" t="s">
-        <v>2215</v>
+        <v>2214</v>
       </c>
       <c r="BT16" s="10" t="s">
         <v>2374</v>
@@ -20141,7 +20144,7 @@
         <v>16</v>
       </c>
       <c r="BS17" s="14" t="s">
-        <v>2813</v>
+        <v>2215</v>
       </c>
       <c r="BT17" s="10" t="s">
         <v>2084</v>
@@ -20313,7 +20316,7 @@
         <v>17</v>
       </c>
       <c r="BS18" s="14" t="s">
-        <v>2911</v>
+        <v>2813</v>
       </c>
       <c r="BW18" s="11" t="s">
         <v>2368</v>
@@ -20470,7 +20473,7 @@
         <v>18</v>
       </c>
       <c r="BS19" s="14" t="s">
-        <v>2912</v>
+        <v>2911</v>
       </c>
       <c r="BW19" s="11" t="s">
         <v>2370</v>
@@ -20624,7 +20627,7 @@
         <v>19</v>
       </c>
       <c r="BS20" s="14" t="s">
-        <v>2814</v>
+        <v>2912</v>
       </c>
       <c r="BW20" s="11" t="s">
         <v>2369</v>
@@ -20761,7 +20764,7 @@
         <v>2845</v>
       </c>
       <c r="BS21" s="14" t="s">
-        <v>2815</v>
+        <v>2814</v>
       </c>
       <c r="BW21" s="11" t="s">
         <v>2373</v>
@@ -20863,7 +20866,7 @@
         <v>2846</v>
       </c>
       <c r="BS22" s="14" t="s">
-        <v>2816</v>
+        <v>2815</v>
       </c>
       <c r="BW22" s="11" t="s">
         <v>2573</v>
@@ -20958,7 +20961,7 @@
         <v>2903</v>
       </c>
       <c r="BS23" s="14" t="s">
-        <v>2817</v>
+        <v>2816</v>
       </c>
       <c r="BW23" s="11" t="s">
         <v>2574</v>
@@ -21052,7 +21055,7 @@
       </c>
       <c r="BD24" s="17"/>
       <c r="BS24" s="14" t="s">
-        <v>2818</v>
+        <v>2817</v>
       </c>
       <c r="BW24" s="11" t="s">
         <v>2575</v>
@@ -21141,7 +21144,7 @@
       </c>
       <c r="BD25" s="17"/>
       <c r="BS25" s="14" t="s">
-        <v>2819</v>
+        <v>2818</v>
       </c>
       <c r="BW25" s="11" t="s">
         <v>2576</v>
@@ -21229,7 +21232,7 @@
       </c>
       <c r="BD26" s="17"/>
       <c r="BS26" s="14" t="s">
-        <v>2820</v>
+        <v>2819</v>
       </c>
       <c r="BW26" s="11" t="s">
         <v>1765</v>
@@ -21287,7 +21290,7 @@
       <c r="L27" t="s">
         <v>228</v>
       </c>
-      <c r="M27" s="109"/>
+      <c r="M27" s="115"/>
       <c r="O27" s="12" t="s">
         <v>822</v>
       </c>
@@ -21310,7 +21313,7 @@
         <v>1941</v>
       </c>
       <c r="BS27" s="14" t="s">
-        <v>2821</v>
+        <v>2820</v>
       </c>
       <c r="BW27" s="11" t="s">
         <v>1775</v>
@@ -21368,7 +21371,7 @@
       <c r="L28" t="s">
         <v>235</v>
       </c>
-      <c r="M28" s="109"/>
+      <c r="M28" s="115"/>
       <c r="O28" s="12" t="s">
         <v>1712</v>
       </c>
@@ -21391,7 +21394,7 @@
         <v>1655</v>
       </c>
       <c r="BS28" s="14" t="s">
-        <v>2822</v>
+        <v>2821</v>
       </c>
       <c r="BW28" s="11" t="s">
         <v>2732</v>
@@ -21469,7 +21472,7 @@
         <v>1678</v>
       </c>
       <c r="BS29" s="14" t="s">
-        <v>2823</v>
+        <v>2822</v>
       </c>
       <c r="BW29" s="20"/>
       <c r="BX29" s="14"/>
@@ -21535,7 +21538,7 @@
         <v>1679</v>
       </c>
       <c r="BS30" s="14" t="s">
-        <v>2824</v>
+        <v>2823</v>
       </c>
       <c r="BW30" s="14"/>
       <c r="BX30" s="14"/>
@@ -21599,7 +21602,7 @@
         <v>1677</v>
       </c>
       <c r="BS31" s="14" t="s">
-        <v>2825</v>
+        <v>2824</v>
       </c>
       <c r="BW31" s="14"/>
       <c r="BX31" s="14"/>
@@ -21661,6 +21664,9 @@
       </c>
       <c r="BC32" s="6" t="s">
         <v>1676</v>
+      </c>
+      <c r="BS32" s="14" t="s">
+        <v>2825</v>
       </c>
       <c r="BW32" s="14"/>
       <c r="BX32" s="14"/>
@@ -21770,7 +21776,7 @@
       <c r="L34" t="s">
         <v>276</v>
       </c>
-      <c r="M34" s="109"/>
+      <c r="M34" s="115"/>
       <c r="O34" s="12" t="s">
         <v>915</v>
       </c>
@@ -21829,7 +21835,7 @@
       <c r="L35" t="s">
         <v>283</v>
       </c>
-      <c r="M35" s="109"/>
+      <c r="M35" s="115"/>
       <c r="O35" s="12" t="s">
         <v>939</v>
       </c>
@@ -27295,7 +27301,7 @@
       <c r="CR277" s="40"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="Vwi+bMJVmN0LoXu3ewZ9K2qe258qMTvdF2s0qn41LN5y21MB06S8uU4iWT+jk0nhgJGc5dbtcqIqlRgkg29XPw==" saltValue="m67BHG1uDzitN3kKjLx5XA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="RF7S/6YfteRJsE8MuGcEnXcFz/Vo0IImoUJLAmiiKClLOgnD0s1HnbgcnAjLP7SGF4zdG2XgGecYkESjhbvZJg==" saltValue="JA2tovrn9pQBceYEs0vUiQ==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="2">
     <mergeCell ref="M27:M28"/>
     <mergeCell ref="M34:M35"/>

</xml_diff>

<commit_message>
Added columns with separate year, month, day
</commit_message>
<xml_diff>
--- a/Excel_templates/MOSAIC_input_excel_file_2022.xlsx
+++ b/Excel_templates/MOSAIC_input_excel_file_2022.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20386"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20387"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sparadis\Documents\ETH\MOSAIC\MOSAIC_Client\Excel_templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9F934F2-4D37-4063-80F6-8CC5968A0691}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24F13571-CCAD-434B-BAC8-B1D9AC02E09F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30204" yWindow="10044" windowWidth="40020" windowHeight="22296" tabRatio="694" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30204" yWindow="10044" windowWidth="40020" windowHeight="22296" tabRatio="694" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ARTICLE_AUTHOR" sheetId="3" r:id="rId1"/>
@@ -195,7 +195,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3741" uniqueCount="2917">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3744" uniqueCount="2920">
   <si>
     <t>sample_name</t>
   </si>
@@ -8946,6 +8946,15 @@
   </si>
   <si>
     <t>pore_water</t>
+  </si>
+  <si>
+    <t>sampling_year</t>
+  </si>
+  <si>
+    <t>sampling_month</t>
+  </si>
+  <si>
+    <t>sampling_day</t>
   </si>
 </sst>
 </file>
@@ -9988,7 +9997,7 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -10079,13 +10088,13 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:P15"/>
+  <dimension ref="A1:S15"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -10094,19 +10103,22 @@
     <col min="2" max="2" width="22" style="82" customWidth="1"/>
     <col min="3" max="5" width="10.796875" style="82" customWidth="1"/>
     <col min="6" max="6" width="13.19921875" style="84" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15" style="86" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15" style="86" customWidth="1"/>
-    <col min="9" max="9" width="28.3984375" style="82" customWidth="1"/>
-    <col min="10" max="10" width="23.296875" style="82" customWidth="1"/>
-    <col min="11" max="11" width="16.8984375" style="82" customWidth="1"/>
-    <col min="12" max="14" width="24.796875" style="82" customWidth="1"/>
-    <col min="15" max="15" width="27.8984375" style="82" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="27.8984375" style="82" customWidth="1"/>
-    <col min="17" max="17" width="10.796875" style="82" customWidth="1"/>
-    <col min="18" max="16384" width="11.19921875" style="82"/>
+    <col min="7" max="7" width="13.19921875" style="84" customWidth="1"/>
+    <col min="8" max="8" width="15.5" style="84" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.19921875" style="84" customWidth="1"/>
+    <col min="10" max="10" width="15" style="86" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15" style="86" customWidth="1"/>
+    <col min="12" max="12" width="28.3984375" style="82" customWidth="1"/>
+    <col min="13" max="13" width="23.296875" style="82" customWidth="1"/>
+    <col min="14" max="14" width="16.8984375" style="82" customWidth="1"/>
+    <col min="15" max="17" width="24.796875" style="82" customWidth="1"/>
+    <col min="18" max="18" width="27.8984375" style="82" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="27.8984375" style="82" customWidth="1"/>
+    <col min="20" max="20" width="10.796875" style="82" customWidth="1"/>
+    <col min="21" max="16384" width="11.19921875" style="82"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="56" customFormat="1" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:19" s="56" customFormat="1" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A1" s="90" t="s">
         <v>2578</v>
       </c>
@@ -10127,8 +10139,11 @@
       <c r="N1" s="89"/>
       <c r="O1" s="89"/>
       <c r="P1" s="89"/>
-    </row>
-    <row r="2" spans="1:16" s="59" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="Q1" s="89"/>
+      <c r="R1" s="89"/>
+      <c r="S1" s="89"/>
+    </row>
+    <row r="2" spans="1:19" s="59" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="55" t="s">
         <v>2510</v>
       </c>
@@ -10148,132 +10163,141 @@
         <v>1825</v>
       </c>
       <c r="G2" s="58" t="s">
+        <v>2917</v>
+      </c>
+      <c r="H2" s="58" t="s">
+        <v>2918</v>
+      </c>
+      <c r="I2" s="58" t="s">
+        <v>2919</v>
+      </c>
+      <c r="J2" s="58" t="s">
         <v>1826</v>
       </c>
-      <c r="H2" s="58" t="s">
+      <c r="K2" s="58" t="s">
         <v>2060</v>
       </c>
-      <c r="I2" s="58" t="s">
+      <c r="L2" s="58" t="s">
         <v>2059</v>
       </c>
-      <c r="J2" s="58" t="s">
+      <c r="M2" s="58" t="s">
         <v>2061</v>
       </c>
-      <c r="K2" s="58" t="s">
+      <c r="N2" s="58" t="s">
         <v>2045</v>
       </c>
-      <c r="L2" s="58" t="s">
+      <c r="O2" s="58" t="s">
         <v>1828</v>
       </c>
-      <c r="M2" s="58" t="s">
+      <c r="P2" s="58" t="s">
         <v>1847</v>
       </c>
-      <c r="N2" s="58" t="s">
+      <c r="Q2" s="58" t="s">
         <v>1829</v>
       </c>
-      <c r="O2" s="58" t="s">
+      <c r="R2" s="58" t="s">
         <v>1830</v>
       </c>
-      <c r="P2" s="58" t="s">
+      <c r="S2" s="58" t="s">
         <v>1827</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="C3" s="83"/>
       <c r="D3" s="83"/>
       <c r="E3" s="83"/>
-      <c r="G3" s="85"/>
-      <c r="N3" s="87"/>
-      <c r="O3" s="84"/>
-      <c r="P3" s="84"/>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="J3" s="85"/>
+      <c r="Q3" s="87"/>
+      <c r="R3" s="84"/>
+      <c r="S3" s="84"/>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B4" s="83"/>
       <c r="C4" s="83"/>
       <c r="D4" s="83"/>
       <c r="E4" s="83"/>
-      <c r="G4" s="83"/>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="J4" s="83"/>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B5" s="83"/>
       <c r="C5" s="83"/>
       <c r="D5" s="83"/>
       <c r="E5" s="83"/>
-      <c r="G5" s="83"/>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="J5" s="83"/>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B6" s="83"/>
       <c r="C6" s="83"/>
       <c r="D6" s="83"/>
       <c r="E6" s="83"/>
-      <c r="G6" s="83"/>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="J6" s="83"/>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B7" s="83"/>
       <c r="C7" s="83"/>
       <c r="D7" s="83"/>
       <c r="E7" s="83"/>
-      <c r="G7" s="83"/>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="J7" s="83"/>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B8" s="83"/>
       <c r="C8" s="83"/>
       <c r="D8" s="83"/>
       <c r="E8" s="83"/>
-      <c r="G8" s="83"/>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="J8" s="83"/>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B9" s="83"/>
       <c r="C9" s="83"/>
       <c r="D9" s="83"/>
       <c r="E9" s="83"/>
-      <c r="G9" s="83"/>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="J9" s="83"/>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B10" s="83"/>
       <c r="C10" s="83"/>
       <c r="D10" s="83"/>
       <c r="E10" s="83"/>
-      <c r="G10" s="83"/>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="J10" s="83"/>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B11" s="83"/>
       <c r="C11" s="83"/>
       <c r="D11" s="83"/>
       <c r="E11" s="83"/>
-      <c r="G11" s="83"/>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="J11" s="83"/>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B12" s="83"/>
       <c r="C12" s="83"/>
       <c r="D12" s="83"/>
       <c r="E12" s="83"/>
-      <c r="G12" s="83"/>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="J12" s="83"/>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B13" s="83"/>
       <c r="C13" s="83"/>
       <c r="D13" s="83"/>
       <c r="E13" s="83"/>
-      <c r="G13" s="83"/>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="J13" s="83"/>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B14" s="83"/>
       <c r="C14" s="83"/>
       <c r="D14" s="83"/>
       <c r="E14" s="83"/>
-      <c r="G14" s="83"/>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="J14" s="83"/>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B15" s="83"/>
       <c r="C15" s="83"/>
       <c r="D15" s="83"/>
       <c r="E15" s="83"/>
-      <c r="G15" s="83"/>
+      <c r="J15" s="83"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="F1:P1"/>
+    <mergeCell ref="F1:S1"/>
     <mergeCell ref="A1:E1"/>
   </mergeCells>
   <conditionalFormatting sqref="B2:B1048576">
@@ -10288,35 +10312,35 @@
       <formula1>-180</formula1>
       <formula2>180</formula2>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Waer depth should be positive numbers." prompt="Water depth where the core was collected." sqref="G16:G1048576" xr:uid="{00CDF339-1F57-43C3-902E-FF6A4E068910}">
+    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Waer depth should be positive numbers." prompt="Water depth where the core was collected." sqref="J16:J1048576" xr:uid="{00CDF339-1F57-43C3-902E-FF6A4E068910}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please select geomorphological site if relevant. Choese _unkown if unknown. Otherwise leave blank." prompt="Please select geomorphological site if relevant. Choese _unkown if unknown. Otherwise leave blank." sqref="J3:J1048576" xr:uid="{C409BA21-827A-4726-997B-4DDCEB0E121E}">
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please select geomorphological site if relevant. Choese _unkown if unknown. Otherwise leave blank." prompt="Please select geomorphological site if relevant. Choese _unkown if unknown. Otherwise leave blank." sqref="M3:M1048576" xr:uid="{C409BA21-827A-4726-997B-4DDCEB0E121E}">
       <formula1>geomorphological_site</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Name of the campaign cruise." sqref="N4:N1048576" xr:uid="{573E733B-B85F-488A-AB24-1BB2993B0FAE}"/>
-    <dataValidation type="textLength" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Maximum comment length is 200 characters" prompt="Add any additional information of the core" sqref="H3:H1048576" xr:uid="{FF2D52E6-EFBC-4479-B912-8CF305BA6CC6}">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Name of the campaign cruise." sqref="Q4:Q1048576" xr:uid="{573E733B-B85F-488A-AB24-1BB2993B0FAE}"/>
+    <dataValidation type="textLength" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Maximum comment length is 200 characters" prompt="Add any additional information of the core" sqref="K3:K1048576" xr:uid="{FF2D52E6-EFBC-4479-B912-8CF305BA6CC6}">
       <formula1>200</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Choose the country that the Research Vessel belongs to. If unknown, choose _unknown. If not listed here, check _other." prompt="Choose the country that the Research Vessel belongs to (extracted from Wikipedia, please contact mosaic@ethz.ch for any errors)" sqref="L3:L1048576" xr:uid="{6E72A734-A312-4B86-8990-BB5CA2135DC2}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Choose the country that the Research Vessel belongs to. If unknown, choose _unknown. If not listed here, check _other." prompt="Choose the country that the Research Vessel belongs to (extracted from Wikipedia, please contact mosaic@ethz.ch for any errors)" sqref="O3:O1048576" xr:uid="{6E72A734-A312-4B86-8990-BB5CA2135DC2}">
       <formula1>Research_Vessel_Countries</formula1>
     </dataValidation>
-    <dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Date is not between 1/1/1900 and TODAY" prompt="Add sampling date between 1/1/1900 and TODAY" sqref="F3:F1048576" xr:uid="{7913A979-EC13-4075-870A-D28BCBAC3D30}">
+    <dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Date is not between 1/1/1900 and TODAY" prompt="Add sampling date between 1/1/1900 and TODAY" sqref="F3:I1048576" xr:uid="{7913A979-EC13-4075-870A-D28BCBAC3D30}">
       <formula1>1</formula1>
       <formula2>TODAY()</formula2>
     </dataValidation>
-    <dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid date" error="Please introduce a date between 1/1/1900 and TODAY." prompt="If known, add the starting date of the cruise. Accepts dates between 1/1/1900 and TODAY." sqref="O3:O1048576" xr:uid="{D9536885-D4AA-431B-A11C-EEFC92030E57}">
+    <dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid date" error="Please introduce a date between 1/1/1900 and TODAY." prompt="If known, add the starting date of the cruise. Accepts dates between 1/1/1900 and TODAY." sqref="R3:R1048576" xr:uid="{D9536885-D4AA-431B-A11C-EEFC92030E57}">
       <formula1>1</formula1>
       <formula2>TODAY()</formula2>
     </dataValidation>
-    <dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid date" error="Please introduce a date between 1/1/1900 and TODAY." prompt="If known, add the ending date of the cruise. Accepts dates between 1/1/1900 and TODAY." sqref="P3:P1048576" xr:uid="{2F267FE0-8CDD-46BB-9FA7-D775C28F6A0E}">
+    <dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid date" error="Please introduce a date between 1/1/1900 and TODAY." prompt="If known, add the ending date of the cruise. Accepts dates between 1/1/1900 and TODAY." sqref="S3:S1048576" xr:uid="{2F267FE0-8CDD-46BB-9FA7-D775C28F6A0E}">
       <formula1>1</formula1>
       <formula2>TODAY()</formula2>
     </dataValidation>
-    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="If available, specify the length of the core retrieved in cm." sqref="K3:K1048576" xr:uid="{6E15A0C0-8408-4930-8258-97C19A733952}"/>
+    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="If available, specify the length of the core retrieved in cm." sqref="N3:N1048576" xr:uid="{6E15A0C0-8408-4930-8258-97C19A733952}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Name of user who is entering data" sqref="A3:A1048576" xr:uid="{B1508E14-6DD0-4DEF-BE9A-DA048D366864}"/>
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="In order to choose a research vessel, first choose the country it belongs to." sqref="M3:M1048576" xr:uid="{74AEC9A0-D7E8-4D80-8B77-1F64526DD0B8}">
-      <formula1>INDIRECT(L3)</formula1>
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="In order to choose a research vessel, first choose the country it belongs to." sqref="P3:P1048576" xr:uid="{74AEC9A0-D7E8-4D80-8B77-1F64526DD0B8}">
+      <formula1>INDIRECT(O3)</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Write the core name or select from the drop-down menu the cores you have in the Workbook._x000a_Make sure that the core name matches with its metadata given in GEOPOINTS_CORES sheet" sqref="B3" xr:uid="{E17DEF85-BC0F-4D8D-B2CE-51E2C1FE041A}">
       <formula1>$B$3:$B$1048576</formula1>
@@ -10331,7 +10355,7 @@
           <x14:formula1>
             <xm:f>SET_VARIABLES!$J$2:$J$13</xm:f>
           </x14:formula1>
-          <xm:sqref>I3:I1048576</xm:sqref>
+          <xm:sqref>L3:L1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" prompt="State whether the coordinates were obtained by georeferencing a map, or inferred (TRUE) or whether they were provided in tabular format (FALSE)." xr:uid="{FC9545BB-E799-4EF5-951B-5C2E1E979B37}">
           <x14:formula1>

</xml_diff>

<commit_message>
Modified number format of columns year, month, day
</commit_message>
<xml_diff>
--- a/Excel_templates/MOSAIC_input_excel_file_2022.xlsx
+++ b/Excel_templates/MOSAIC_input_excel_file_2022.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sparadis\Documents\ETH\MOSAIC\MOSAIC_Client\Excel_templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24F13571-CCAD-434B-BAC8-B1D9AC02E09F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2406CBD4-ACC3-4BF4-8081-BDE3F8398713}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30204" yWindow="10044" windowWidth="40020" windowHeight="22296" tabRatio="694" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30204" yWindow="10044" windowWidth="40020" windowHeight="22296" tabRatio="694" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ARTICLE_AUTHOR" sheetId="3" r:id="rId1"/>
@@ -9430,7 +9430,7 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="116">
+  <cellXfs count="117">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="13" applyFont="1" applyFill="1" applyAlignment="1"/>
@@ -9654,6 +9654,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="2" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="16">
     <cellStyle name="20% - Accent1" xfId="3" builtinId="30" customBuiltin="1"/>
@@ -9997,7 +10000,7 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -10090,11 +10093,11 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:S15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I7" sqref="I7"/>
+      <selection pane="bottomRight" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -10103,9 +10106,9 @@
     <col min="2" max="2" width="22" style="82" customWidth="1"/>
     <col min="3" max="5" width="10.796875" style="82" customWidth="1"/>
     <col min="6" max="6" width="13.19921875" style="84" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.19921875" style="84" customWidth="1"/>
-    <col min="8" max="8" width="15.5" style="84" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.19921875" style="84" customWidth="1"/>
+    <col min="7" max="7" width="13.19921875" style="116" customWidth="1"/>
+    <col min="8" max="8" width="15.5" style="116" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.19921875" style="116" customWidth="1"/>
     <col min="10" max="10" width="15" style="86" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="15" style="86" customWidth="1"/>
     <col min="12" max="12" width="28.3984375" style="82" customWidth="1"/>

</xml_diff>

<commit_message>
Added new grain size fractions into material_analyzed
</commit_message>
<xml_diff>
--- a/Excel_templates/MOSAIC_input_excel_file_2022.xlsx
+++ b/Excel_templates/MOSAIC_input_excel_file_2022.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sparadis\Documents\ETH\MOSAIC\MOSAIC_Client\Excel_templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3B3FCAA-A8BE-4FA3-9286-914012568C8B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBE7BE3F-69C0-4B2A-9527-8A0487B702E7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="30204" yWindow="10044" windowWidth="40020" windowHeight="22296" tabRatio="694" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -93,7 +93,7 @@
     <definedName name="MAR_g_cm2_yr">SET_VARIABLES!$GH$2:$GH$20</definedName>
     <definedName name="MAR_model">SET_VARIABLES!#REF!</definedName>
     <definedName name="MAR_tracer">SET_VARIABLES!#REF!</definedName>
-    <definedName name="material_analyzed">SET_VARIABLES!$BS$2:$BS$78</definedName>
+    <definedName name="material_analyzed">SET_VARIABLES!$BS$2:$BS$82</definedName>
     <definedName name="Mauritania">SET_VARIABLES!$AL$2:$AL$7</definedName>
     <definedName name="mean_grain_size_microm">SET_VARIABLES!$EZ$2:$EZ$5</definedName>
     <definedName name="median_grain_size_microm">SET_VARIABLES!$FA$2:$FA$5</definedName>
@@ -211,7 +211,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4106" uniqueCount="3031">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4110" uniqueCount="3035">
   <si>
     <t>sample_name</t>
   </si>
@@ -9304,6 +9304,18 @@
   </si>
   <si>
     <t>C26-C28_alc</t>
+  </si>
+  <si>
+    <t>&gt;0.063 mm</t>
+  </si>
+  <si>
+    <t>&lt;0.002 mm</t>
+  </si>
+  <si>
+    <t>0.010-0.063 mm</t>
+  </si>
+  <si>
+    <t>0.002-0.010 mm</t>
   </si>
 </sst>
 </file>
@@ -15093,8 +15105,8 @@
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:IB277"/>
   <sheetViews>
-    <sheetView topLeftCell="BQ1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="BQ30" sqref="BQ30"/>
+    <sheetView topLeftCell="BQ4" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="BQ33" sqref="BQ33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -22157,7 +22169,7 @@
         <v>2813</v>
       </c>
       <c r="BS22" s="14" t="s">
-        <v>2786</v>
+        <v>3031</v>
       </c>
       <c r="BW22" s="11" t="s">
         <v>2541</v>
@@ -22260,7 +22272,7 @@
         <v>2814</v>
       </c>
       <c r="BS23" s="14" t="s">
-        <v>2787</v>
+        <v>2786</v>
       </c>
       <c r="BW23" s="11" t="s">
         <v>2542</v>
@@ -22364,7 +22376,7 @@
         <v>2871</v>
       </c>
       <c r="BS24" s="14" t="s">
-        <v>2788</v>
+        <v>2787</v>
       </c>
       <c r="BW24" s="11" t="s">
         <v>2543</v>
@@ -22460,7 +22472,7 @@
       </c>
       <c r="BD25" s="17"/>
       <c r="BS25" s="14" t="s">
-        <v>2789</v>
+        <v>2788</v>
       </c>
       <c r="BW25" s="11" t="s">
         <v>2544</v>
@@ -22552,7 +22564,7 @@
       </c>
       <c r="BD26" s="17"/>
       <c r="BS26" s="14" t="s">
-        <v>2790</v>
+        <v>2789</v>
       </c>
       <c r="BW26" s="11" t="s">
         <v>1765</v>
@@ -22638,7 +22650,7 @@
         <v>1941</v>
       </c>
       <c r="BS27" s="14" t="s">
-        <v>2791</v>
+        <v>2790</v>
       </c>
       <c r="BW27" s="11" t="s">
         <v>1775</v>
@@ -22723,7 +22735,7 @@
         <v>1655</v>
       </c>
       <c r="BS28" s="14" t="s">
-        <v>2792</v>
+        <v>2791</v>
       </c>
       <c r="BW28" s="11" t="s">
         <v>2700</v>
@@ -22802,7 +22814,7 @@
         <v>1678</v>
       </c>
       <c r="BS29" s="14" t="s">
-        <v>2793</v>
+        <v>3033</v>
       </c>
       <c r="BW29" s="20"/>
       <c r="BX29" s="14"/>
@@ -22872,7 +22884,7 @@
         <v>1679</v>
       </c>
       <c r="BS30" s="14" t="s">
-        <v>3000</v>
+        <v>3034</v>
       </c>
       <c r="BW30" s="14"/>
       <c r="BX30" s="14"/>
@@ -22940,7 +22952,7 @@
         <v>1677</v>
       </c>
       <c r="BS31" s="14" t="s">
-        <v>2999</v>
+        <v>2792</v>
       </c>
       <c r="BW31" s="14"/>
       <c r="BX31" s="14"/>
@@ -23011,7 +23023,7 @@
         <v>1676</v>
       </c>
       <c r="BS32" s="14" t="s">
-        <v>2998</v>
+        <v>3032</v>
       </c>
       <c r="BW32" s="14"/>
       <c r="BX32" s="14"/>
@@ -23077,7 +23089,7 @@
         <v>1666</v>
       </c>
       <c r="BS33" s="14" t="s">
-        <v>2997</v>
+        <v>2793</v>
       </c>
       <c r="BW33" s="14"/>
       <c r="BX33" s="14"/>
@@ -23139,7 +23151,7 @@
         <v>1683</v>
       </c>
       <c r="BS34" s="14" t="s">
-        <v>2996</v>
+        <v>3000</v>
       </c>
       <c r="BW34" s="14"/>
       <c r="BX34" s="14"/>
@@ -23201,7 +23213,7 @@
         <v>1675</v>
       </c>
       <c r="BS35" s="14" t="s">
-        <v>3003</v>
+        <v>2999</v>
       </c>
       <c r="BW35" s="14"/>
       <c r="BX35" s="14"/>
@@ -23260,7 +23272,7 @@
         <v>1680</v>
       </c>
       <c r="BS36" s="14" t="s">
-        <v>2995</v>
+        <v>2998</v>
       </c>
       <c r="BW36" s="14"/>
       <c r="BX36" s="14"/>
@@ -23320,7 +23332,7 @@
         <v>1681</v>
       </c>
       <c r="BS37" s="14" t="s">
-        <v>3004</v>
+        <v>2997</v>
       </c>
       <c r="BW37" s="14"/>
       <c r="BX37" s="14"/>
@@ -23380,7 +23392,7 @@
         <v>1651</v>
       </c>
       <c r="BS38" s="14" t="s">
-        <v>3001</v>
+        <v>2996</v>
       </c>
       <c r="BW38" s="14"/>
       <c r="BX38" s="14"/>
@@ -23436,7 +23448,7 @@
         <v>1663</v>
       </c>
       <c r="BS39" s="14" t="s">
-        <v>3005</v>
+        <v>3003</v>
       </c>
       <c r="BW39" s="14"/>
       <c r="BX39" s="14"/>
@@ -23492,7 +23504,7 @@
         <v>1688</v>
       </c>
       <c r="BS40" s="14" t="s">
-        <v>2930</v>
+        <v>2995</v>
       </c>
       <c r="BW40" s="14"/>
       <c r="BX40" s="14"/>
@@ -23545,7 +23557,7 @@
         <v>1699</v>
       </c>
       <c r="BS41" s="14" t="s">
-        <v>3006</v>
+        <v>3004</v>
       </c>
       <c r="CO41" s="12" t="s">
         <v>2601</v>
@@ -23594,7 +23606,7 @@
         <v>1659</v>
       </c>
       <c r="BS42" s="14" t="s">
-        <v>2931</v>
+        <v>3001</v>
       </c>
       <c r="CO42" s="12" t="s">
         <v>2118</v>
@@ -23643,7 +23655,7 @@
         <v>1687</v>
       </c>
       <c r="BS43" s="14" t="s">
-        <v>3007</v>
+        <v>3005</v>
       </c>
       <c r="CO43" s="12" t="s">
         <v>2603</v>
@@ -23693,7 +23705,7 @@
         <v>1664</v>
       </c>
       <c r="BS44" s="14" t="s">
-        <v>2932</v>
+        <v>2930</v>
       </c>
       <c r="CM44" s="23"/>
       <c r="CN44" s="23"/>
@@ -23742,7 +23754,7 @@
         <v>1691</v>
       </c>
       <c r="BS45" s="14" t="s">
-        <v>3008</v>
+        <v>3006</v>
       </c>
       <c r="CM45" s="23"/>
       <c r="CN45" s="23"/>
@@ -23791,7 +23803,7 @@
         <v>1692</v>
       </c>
       <c r="BS46" s="14" t="s">
-        <v>2933</v>
+        <v>2931</v>
       </c>
       <c r="CM46" s="23"/>
       <c r="CN46" s="23"/>
@@ -23840,7 +23852,7 @@
         <v>1693</v>
       </c>
       <c r="BS47" s="14" t="s">
-        <v>3009</v>
+        <v>3007</v>
       </c>
       <c r="CL47" s="23"/>
       <c r="CM47" s="23"/>
@@ -23889,7 +23901,7 @@
         <v>1672</v>
       </c>
       <c r="BS48" s="14" t="s">
-        <v>3002</v>
+        <v>2932</v>
       </c>
       <c r="CL48" s="23"/>
       <c r="CM48" s="23"/>
@@ -23938,7 +23950,7 @@
         <v>1667</v>
       </c>
       <c r="BS49" s="14" t="s">
-        <v>2934</v>
+        <v>3008</v>
       </c>
       <c r="CL49" s="23"/>
       <c r="CM49" s="23"/>
@@ -23988,7 +24000,7 @@
         <v>2105</v>
       </c>
       <c r="BS50" s="14" t="s">
-        <v>2935</v>
+        <v>2933</v>
       </c>
       <c r="CL50" s="23"/>
       <c r="CM50" s="23"/>
@@ -24038,7 +24050,7 @@
         <v>1689</v>
       </c>
       <c r="BS51" s="14" t="s">
-        <v>3010</v>
+        <v>3009</v>
       </c>
       <c r="CL51" s="23"/>
       <c r="CM51" s="23"/>
@@ -24087,7 +24099,7 @@
         <v>1668</v>
       </c>
       <c r="BS52" s="14" t="s">
-        <v>3011</v>
+        <v>3002</v>
       </c>
       <c r="CL52" s="23"/>
       <c r="CM52" s="23"/>
@@ -24137,7 +24149,7 @@
         <v>1685</v>
       </c>
       <c r="BS53" s="14" t="s">
-        <v>3012</v>
+        <v>2934</v>
       </c>
       <c r="CL53" s="23"/>
       <c r="CM53" s="23"/>
@@ -24187,7 +24199,7 @@
         <v>1657</v>
       </c>
       <c r="BS54" s="14" t="s">
-        <v>3013</v>
+        <v>2935</v>
       </c>
       <c r="CL54" s="23"/>
       <c r="CO54" s="12" t="s">
@@ -24235,7 +24247,7 @@
         <v>1654</v>
       </c>
       <c r="BS55" s="14" t="s">
-        <v>3014</v>
+        <v>3010</v>
       </c>
       <c r="CL55" s="23"/>
       <c r="CO55" s="12" t="s">
@@ -24283,7 +24295,7 @@
         <v>2104</v>
       </c>
       <c r="BS56" s="14" t="s">
-        <v>3015</v>
+        <v>3011</v>
       </c>
       <c r="CL56" s="23"/>
       <c r="CO56" s="12" t="s">
@@ -24331,7 +24343,7 @@
         <v>1682</v>
       </c>
       <c r="BS57" s="14" t="s">
-        <v>3016</v>
+        <v>3012</v>
       </c>
       <c r="CO57" s="12" t="s">
         <v>2617</v>
@@ -24378,7 +24390,7 @@
         <v>1980</v>
       </c>
       <c r="BS58" s="14" t="s">
-        <v>3017</v>
+        <v>3013</v>
       </c>
       <c r="CO58" s="12" t="s">
         <v>2126</v>
@@ -24422,7 +24434,7 @@
         <v>1658</v>
       </c>
       <c r="BS59" s="14" t="s">
-        <v>3018</v>
+        <v>3014</v>
       </c>
       <c r="CO59" s="12" t="s">
         <v>2619</v>
@@ -24466,7 +24478,7 @@
         <v>1981</v>
       </c>
       <c r="BS60" s="14" t="s">
-        <v>3019</v>
+        <v>3015</v>
       </c>
       <c r="CO60" s="12" t="s">
         <v>2127</v>
@@ -24510,7 +24522,7 @@
         <v>1673</v>
       </c>
       <c r="BS61" s="14" t="s">
-        <v>3020</v>
+        <v>3016</v>
       </c>
       <c r="CO61" s="12" t="s">
         <v>2621</v>
@@ -24554,7 +24566,7 @@
         <v>1686</v>
       </c>
       <c r="BS62" s="14" t="s">
-        <v>3021</v>
+        <v>3017</v>
       </c>
       <c r="CO62" s="12" t="s">
         <v>2128</v>
@@ -24598,7 +24610,7 @@
         <v>1671</v>
       </c>
       <c r="BS63" s="14" t="s">
-        <v>3022</v>
+        <v>3018</v>
       </c>
       <c r="CO63" s="12" t="s">
         <v>2623</v>
@@ -24639,7 +24651,7 @@
         <v>1700</v>
       </c>
       <c r="BS64" s="14" t="s">
-        <v>3023</v>
+        <v>3019</v>
       </c>
       <c r="CO64" s="23" t="s">
         <v>2129</v>
@@ -24680,7 +24692,7 @@
         <v>1649</v>
       </c>
       <c r="BS65" s="14" t="s">
-        <v>3024</v>
+        <v>3020</v>
       </c>
       <c r="CO65" s="12" t="s">
         <v>2625</v>
@@ -24721,7 +24733,7 @@
         <v>1669</v>
       </c>
       <c r="BS66" s="14" t="s">
-        <v>3025</v>
+        <v>3021</v>
       </c>
       <c r="CO66" s="23" t="s">
         <v>2130</v>
@@ -24762,7 +24774,7 @@
         <v>1674</v>
       </c>
       <c r="BS67" s="14" t="s">
-        <v>3026</v>
+        <v>3022</v>
       </c>
       <c r="CO67" s="12" t="s">
         <v>2627</v>
@@ -24803,7 +24815,7 @@
         <v>1652</v>
       </c>
       <c r="BS68" s="14" t="s">
-        <v>3027</v>
+        <v>3023</v>
       </c>
       <c r="CO68" s="23" t="s">
         <v>2131</v>
@@ -24843,7 +24855,7 @@
         <v>1982</v>
       </c>
       <c r="BS69" s="14" t="s">
-        <v>3028</v>
+        <v>3024</v>
       </c>
       <c r="CO69" s="12" t="s">
         <v>2629</v>
@@ -24884,7 +24896,7 @@
         <v>1695</v>
       </c>
       <c r="BS70" s="14" t="s">
-        <v>3029</v>
+        <v>3025</v>
       </c>
       <c r="CO70" s="23" t="s">
         <v>2132</v>
@@ -24925,7 +24937,7 @@
         <v>1670</v>
       </c>
       <c r="BS71" s="14" t="s">
-        <v>2975</v>
+        <v>3026</v>
       </c>
       <c r="CO71" s="12" t="s">
         <v>2631</v>
@@ -24966,7 +24978,7 @@
         <v>1665</v>
       </c>
       <c r="BS72" s="14" t="s">
-        <v>2972</v>
+        <v>3027</v>
       </c>
       <c r="CO72" s="23" t="s">
         <v>2133</v>
@@ -25007,7 +25019,7 @@
         <v>1696</v>
       </c>
       <c r="BS73" s="14" t="s">
-        <v>2973</v>
+        <v>3028</v>
       </c>
       <c r="CO73" s="12" t="s">
         <v>2633</v>
@@ -25048,7 +25060,7 @@
         <v>1684</v>
       </c>
       <c r="BS74" s="14" t="s">
-        <v>2974</v>
+        <v>3029</v>
       </c>
       <c r="CO74" s="23" t="s">
         <v>2134</v>
@@ -25130,7 +25142,7 @@
         <v>1983</v>
       </c>
       <c r="BS76" s="14" t="s">
-        <v>2976</v>
+        <v>2972</v>
       </c>
       <c r="CO76" s="23" t="s">
         <v>2135</v>
@@ -25171,7 +25183,7 @@
         <v>1647</v>
       </c>
       <c r="BS77" s="14" t="s">
-        <v>2977</v>
+        <v>2973</v>
       </c>
       <c r="CO77" s="12" t="s">
         <v>2637</v>
@@ -25212,7 +25224,7 @@
         <v>1698</v>
       </c>
       <c r="BS78" s="14" t="s">
-        <v>3030</v>
+        <v>2974</v>
       </c>
       <c r="CO78" s="23" t="s">
         <v>2136</v>
@@ -25252,6 +25264,9 @@
       <c r="BC79" s="6" t="s">
         <v>1648</v>
       </c>
+      <c r="BS79" s="14" t="s">
+        <v>2975</v>
+      </c>
       <c r="CO79" s="12" t="s">
         <v>2638</v>
       </c>
@@ -25290,6 +25305,9 @@
       <c r="BC80" s="6" t="s">
         <v>1694</v>
       </c>
+      <c r="BS80" s="14" t="s">
+        <v>2976</v>
+      </c>
       <c r="CO80" s="23" t="s">
         <v>2137</v>
       </c>
@@ -25328,6 +25346,9 @@
       <c r="BC81" s="6" t="s">
         <v>1690</v>
       </c>
+      <c r="BS81" s="14" t="s">
+        <v>2977</v>
+      </c>
       <c r="CO81" s="12" t="s">
         <v>2640</v>
       </c>
@@ -25366,6 +25387,9 @@
       <c r="BC82" s="6" t="s">
         <v>1747</v>
       </c>
+      <c r="BS82" s="14" t="s">
+        <v>3030</v>
+      </c>
       <c r="CO82" s="23" t="s">
         <v>2138</v>
       </c>
@@ -28785,7 +28809,7 @@
       <c r="CR277" s="40"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="ONDJ1Sh7WWO160GDsLAl6Cx5XxBugrcJ2PYT9zh+ZdlI4CuwrKnZhYEEMzhU16PSrwBkUoQqawnuHsIx/elCZw==" saltValue="Xjlca8GWbjJsR4AVPmd0Kw==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="SJsOPiQdwxD9NKH5nLKHUBguqQpxHkgQoQAlGaLS0BXPoJdOt0P3Dja2v73+LDp8b9Ucd3GckKTY3195UTpnJA==" saltValue="Oyli968zt4pi2YH1j/UcuA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="2">
     <mergeCell ref="M27:M28"/>
     <mergeCell ref="M34:M35"/>

</xml_diff>

<commit_message>
Added new research vessels
</commit_message>
<xml_diff>
--- a/Excel_templates/MOSAIC_input_excel_file_2022.xlsx
+++ b/Excel_templates/MOSAIC_input_excel_file_2022.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20391"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20393"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sparadis\Documents\ETH\MOSAIC\MOSAIC_Client\Excel_templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0310B55C-D97D-41EA-8B0D-1C1C709340A1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3796063-9DE9-43B1-8447-4E968061B392}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="30204" yWindow="10044" windowWidth="40020" windowHeight="22296" tabRatio="694" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -126,7 +126,7 @@
     <definedName name="Republic_of_Korea">SET_VARIABLES!$AW$2:$AW$6</definedName>
     <definedName name="Research_Vessel_Countries">SET_VARIABLES!$O$2:$O$45</definedName>
     <definedName name="Romania">SET_VARIABLES!$AV$2:$AV$4</definedName>
-    <definedName name="Russia">SET_VARIABLES!$AX$2:$AX$134</definedName>
+    <definedName name="Russia">SET_VARIABLES!$AX$2:$AX$146</definedName>
     <definedName name="S_total_">SET_VARIABLES!$FS$2:$FS$4</definedName>
     <definedName name="S1_mgHC_g">SET_VARIABLES!$GZ$2:$GZ$3</definedName>
     <definedName name="S2_mgHC_g">SET_VARIABLES!$HA$2:$HA$3</definedName>
@@ -211,7 +211,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4115" uniqueCount="3038">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4127" uniqueCount="3050">
   <si>
     <t>sample_name</t>
   </si>
@@ -9325,6 +9325,42 @@
   </si>
   <si>
     <t>RV Aaron</t>
+  </si>
+  <si>
+    <t>RV Gigiga</t>
+  </si>
+  <si>
+    <t>RV Kolonist</t>
+  </si>
+  <si>
+    <t>RV Belogorsk</t>
+  </si>
+  <si>
+    <t>RV Mudiug</t>
+  </si>
+  <si>
+    <t>RV Muinac</t>
+  </si>
+  <si>
+    <t>RV Ob</t>
+  </si>
+  <si>
+    <t>RV Ostashkovo</t>
+  </si>
+  <si>
+    <t>RV Petr Lebedev</t>
+  </si>
+  <si>
+    <t>RV Professor Mesyatsev</t>
+  </si>
+  <si>
+    <t>RV Polyus</t>
+  </si>
+  <si>
+    <t>RV Sevastopole</t>
+  </si>
+  <si>
+    <t>RV Vityaz (II)</t>
   </si>
 </sst>
 </file>
@@ -9800,7 +9836,7 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="122">
+  <cellXfs count="123">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="13" applyFont="1" applyFill="1" applyAlignment="1"/>
@@ -9944,6 +9980,7 @@
     <xf numFmtId="1" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="4" borderId="4" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -10396,15 +10433,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="57" customFormat="1" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="94" t="s">
+      <c r="A1" s="95" t="s">
         <v>2545</v>
       </c>
-      <c r="B1" s="94"/>
-      <c r="C1" s="94"/>
-      <c r="D1" s="94"/>
-      <c r="E1" s="94"/>
-      <c r="F1" s="94"/>
-      <c r="G1" s="94"/>
+      <c r="B1" s="95"/>
+      <c r="C1" s="95"/>
+      <c r="D1" s="95"/>
+      <c r="E1" s="95"/>
+      <c r="F1" s="95"/>
+      <c r="G1" s="95"/>
     </row>
     <row r="2" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="47" t="s">
@@ -10497,29 +10534,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="56" customFormat="1" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="96" t="s">
+      <c r="A1" s="97" t="s">
         <v>2546</v>
       </c>
-      <c r="B1" s="96"/>
-      <c r="C1" s="96"/>
-      <c r="D1" s="96"/>
-      <c r="E1" s="96"/>
-      <c r="F1" s="95" t="s">
+      <c r="B1" s="97"/>
+      <c r="C1" s="97"/>
+      <c r="D1" s="97"/>
+      <c r="E1" s="97"/>
+      <c r="F1" s="96" t="s">
         <v>2684</v>
       </c>
-      <c r="G1" s="95"/>
-      <c r="H1" s="95"/>
-      <c r="I1" s="95"/>
-      <c r="J1" s="95"/>
-      <c r="K1" s="95"/>
-      <c r="L1" s="95"/>
-      <c r="M1" s="95"/>
-      <c r="N1" s="95"/>
-      <c r="O1" s="95"/>
-      <c r="P1" s="95"/>
-      <c r="Q1" s="95"/>
-      <c r="R1" s="95"/>
-      <c r="S1" s="95"/>
+      <c r="G1" s="96"/>
+      <c r="H1" s="96"/>
+      <c r="I1" s="96"/>
+      <c r="J1" s="96"/>
+      <c r="K1" s="96"/>
+      <c r="L1" s="96"/>
+      <c r="M1" s="96"/>
+      <c r="N1" s="96"/>
+      <c r="O1" s="96"/>
+      <c r="P1" s="96"/>
+      <c r="Q1" s="96"/>
+      <c r="R1" s="96"/>
+      <c r="S1" s="96"/>
     </row>
     <row r="2" spans="1:19" s="59" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="55" t="s">
@@ -10785,37 +10822,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:35" s="48" customFormat="1" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="97" t="s">
+      <c r="A1" s="98" t="s">
         <v>2548</v>
       </c>
-      <c r="B1" s="97"/>
-      <c r="C1" s="97" t="s">
+      <c r="B1" s="98"/>
+      <c r="C1" s="98" t="s">
         <v>2547</v>
       </c>
-      <c r="D1" s="97"/>
-      <c r="E1" s="97"/>
-      <c r="F1" s="97"/>
+      <c r="D1" s="98"/>
+      <c r="E1" s="98"/>
+      <c r="F1" s="98"/>
       <c r="G1" s="48" t="s">
         <v>2161</v>
       </c>
     </row>
     <row r="2" spans="1:35" ht="15.6" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="98" t="s">
+      <c r="A2" s="99" t="s">
         <v>2478</v>
       </c>
-      <c r="B2" s="98" t="s">
+      <c r="B2" s="99" t="s">
         <v>1822</v>
       </c>
-      <c r="C2" s="98" t="s">
+      <c r="C2" s="99" t="s">
         <v>1831</v>
       </c>
-      <c r="D2" s="98" t="s">
+      <c r="D2" s="99" t="s">
         <v>2555</v>
       </c>
-      <c r="E2" s="98" t="s">
+      <c r="E2" s="99" t="s">
         <v>1820</v>
       </c>
-      <c r="F2" s="101" t="s">
+      <c r="F2" s="102" t="s">
         <v>1821</v>
       </c>
       <c r="G2" s="49" t="s">
@@ -10851,12 +10888,12 @@
       <c r="AI2" s="49"/>
     </row>
     <row r="3" spans="1:35" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="99"/>
-      <c r="B3" s="99"/>
-      <c r="C3" s="99"/>
-      <c r="D3" s="99"/>
-      <c r="E3" s="99"/>
-      <c r="F3" s="102"/>
+      <c r="A3" s="100"/>
+      <c r="B3" s="100"/>
+      <c r="C3" s="100"/>
+      <c r="D3" s="100"/>
+      <c r="E3" s="100"/>
+      <c r="F3" s="103"/>
       <c r="G3" s="49"/>
       <c r="H3" s="49"/>
       <c r="I3" s="49"/>
@@ -10888,12 +10925,12 @@
       <c r="AI3" s="49"/>
     </row>
     <row r="4" spans="1:35" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="99"/>
-      <c r="B4" s="99"/>
-      <c r="C4" s="99"/>
-      <c r="D4" s="99"/>
-      <c r="E4" s="99"/>
-      <c r="F4" s="102"/>
+      <c r="A4" s="100"/>
+      <c r="B4" s="100"/>
+      <c r="C4" s="100"/>
+      <c r="D4" s="100"/>
+      <c r="E4" s="100"/>
+      <c r="F4" s="103"/>
       <c r="G4" s="49"/>
       <c r="H4" s="49"/>
       <c r="I4" s="49"/>
@@ -10925,12 +10962,12 @@
       <c r="AI4" s="49"/>
     </row>
     <row r="5" spans="1:35" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="100"/>
-      <c r="B5" s="100"/>
-      <c r="C5" s="100"/>
-      <c r="D5" s="100"/>
-      <c r="E5" s="100"/>
-      <c r="F5" s="102"/>
+      <c r="A5" s="101"/>
+      <c r="B5" s="101"/>
+      <c r="C5" s="101"/>
+      <c r="D5" s="101"/>
+      <c r="E5" s="101"/>
+      <c r="F5" s="103"/>
       <c r="G5" s="49"/>
       <c r="H5" s="49"/>
       <c r="I5" s="49"/>
@@ -10962,12 +10999,12 @@
       <c r="AI5" s="49"/>
     </row>
     <row r="6" spans="1:35" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="100"/>
-      <c r="B6" s="100"/>
-      <c r="C6" s="100"/>
-      <c r="D6" s="100"/>
-      <c r="E6" s="100"/>
-      <c r="F6" s="102"/>
+      <c r="A6" s="101"/>
+      <c r="B6" s="101"/>
+      <c r="C6" s="101"/>
+      <c r="D6" s="101"/>
+      <c r="E6" s="101"/>
+      <c r="F6" s="103"/>
       <c r="G6" s="49"/>
       <c r="H6" s="49"/>
       <c r="I6" s="49"/>
@@ -12289,23 +12326,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:80" s="72" customFormat="1" ht="20.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="103" t="s">
+      <c r="A1" s="104" t="s">
         <v>2557</v>
       </c>
-      <c r="B1" s="104"/>
-      <c r="C1" s="105"/>
-      <c r="D1" s="103" t="s">
+      <c r="B1" s="105"/>
+      <c r="C1" s="106"/>
+      <c r="D1" s="104" t="s">
         <v>2547</v>
       </c>
-      <c r="E1" s="104"/>
-      <c r="F1" s="104"/>
-      <c r="G1" s="105"/>
-      <c r="H1" s="106" t="s">
+      <c r="E1" s="105"/>
+      <c r="F1" s="105"/>
+      <c r="G1" s="106"/>
+      <c r="H1" s="107" t="s">
         <v>2549</v>
       </c>
-      <c r="I1" s="107"/>
-      <c r="J1" s="107"/>
-      <c r="K1" s="108"/>
+      <c r="I1" s="108"/>
+      <c r="J1" s="108"/>
+      <c r="K1" s="109"/>
       <c r="L1" s="72" t="s">
         <v>1837</v>
       </c>
@@ -12368,37 +12405,37 @@
       </c>
     </row>
     <row r="2" spans="1:80" s="74" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="109" t="s">
+      <c r="A2" s="110" t="s">
         <v>2478</v>
       </c>
-      <c r="B2" s="112" t="s">
+      <c r="B2" s="113" t="s">
         <v>1822</v>
       </c>
-      <c r="C2" s="115" t="s">
+      <c r="C2" s="116" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="110" t="s">
+      <c r="D2" s="111" t="s">
         <v>1831</v>
       </c>
-      <c r="E2" s="113" t="s">
+      <c r="E2" s="114" t="s">
         <v>2555</v>
       </c>
-      <c r="F2" s="113" t="s">
+      <c r="F2" s="114" t="s">
         <v>1820</v>
       </c>
-      <c r="G2" s="116" t="s">
+      <c r="G2" s="117" t="s">
         <v>1821</v>
       </c>
-      <c r="H2" s="109" t="s">
+      <c r="H2" s="110" t="s">
         <v>1832</v>
       </c>
-      <c r="I2" s="112" t="s">
+      <c r="I2" s="113" t="s">
         <v>1833</v>
       </c>
-      <c r="J2" s="112" t="s">
+      <c r="J2" s="113" t="s">
         <v>1834</v>
       </c>
-      <c r="K2" s="118" t="s">
+      <c r="K2" s="119" t="s">
         <v>1835</v>
       </c>
       <c r="L2" s="73" t="s">
@@ -12512,17 +12549,17 @@
       <c r="CB2" s="73"/>
     </row>
     <row r="3" spans="1:80" s="74" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A3" s="110"/>
-      <c r="B3" s="113"/>
-      <c r="C3" s="116"/>
-      <c r="D3" s="110"/>
-      <c r="E3" s="113"/>
-      <c r="F3" s="113"/>
-      <c r="G3" s="116"/>
-      <c r="H3" s="110"/>
-      <c r="I3" s="113"/>
-      <c r="J3" s="113"/>
-      <c r="K3" s="119"/>
+      <c r="A3" s="111"/>
+      <c r="B3" s="114"/>
+      <c r="C3" s="117"/>
+      <c r="D3" s="111"/>
+      <c r="E3" s="114"/>
+      <c r="F3" s="114"/>
+      <c r="G3" s="117"/>
+      <c r="H3" s="111"/>
+      <c r="I3" s="114"/>
+      <c r="J3" s="114"/>
+      <c r="K3" s="120"/>
       <c r="L3" s="73" t="s">
         <v>2793</v>
       </c>
@@ -12632,17 +12669,17 @@
       <c r="CB3" s="73"/>
     </row>
     <row r="4" spans="1:80" s="74" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="110"/>
-      <c r="B4" s="113"/>
-      <c r="C4" s="116"/>
-      <c r="D4" s="110"/>
-      <c r="E4" s="113"/>
-      <c r="F4" s="113"/>
-      <c r="G4" s="116"/>
-      <c r="H4" s="110"/>
-      <c r="I4" s="113"/>
-      <c r="J4" s="113"/>
-      <c r="K4" s="119"/>
+      <c r="A4" s="111"/>
+      <c r="B4" s="114"/>
+      <c r="C4" s="117"/>
+      <c r="D4" s="111"/>
+      <c r="E4" s="114"/>
+      <c r="F4" s="114"/>
+      <c r="G4" s="117"/>
+      <c r="H4" s="111"/>
+      <c r="I4" s="114"/>
+      <c r="J4" s="114"/>
+      <c r="K4" s="120"/>
       <c r="L4" s="73"/>
       <c r="M4" s="73"/>
       <c r="N4" s="73"/>
@@ -12720,17 +12757,17 @@
       <c r="CB4" s="73"/>
     </row>
     <row r="5" spans="1:80" s="74" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="110"/>
-      <c r="B5" s="113"/>
-      <c r="C5" s="116"/>
-      <c r="D5" s="110"/>
-      <c r="E5" s="113"/>
-      <c r="F5" s="113"/>
-      <c r="G5" s="116"/>
-      <c r="H5" s="110"/>
-      <c r="I5" s="113"/>
-      <c r="J5" s="113"/>
-      <c r="K5" s="119"/>
+      <c r="A5" s="111"/>
+      <c r="B5" s="114"/>
+      <c r="C5" s="117"/>
+      <c r="D5" s="111"/>
+      <c r="E5" s="114"/>
+      <c r="F5" s="114"/>
+      <c r="G5" s="117"/>
+      <c r="H5" s="111"/>
+      <c r="I5" s="114"/>
+      <c r="J5" s="114"/>
+      <c r="K5" s="120"/>
       <c r="L5" s="73"/>
       <c r="M5" s="73"/>
       <c r="N5" s="73"/>
@@ -12802,17 +12839,17 @@
       <c r="CB5" s="73"/>
     </row>
     <row r="6" spans="1:80" s="74" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="111"/>
-      <c r="B6" s="114"/>
-      <c r="C6" s="117"/>
-      <c r="D6" s="111"/>
-      <c r="E6" s="114"/>
-      <c r="F6" s="114"/>
-      <c r="G6" s="117"/>
-      <c r="H6" s="111"/>
-      <c r="I6" s="114"/>
-      <c r="J6" s="114"/>
-      <c r="K6" s="120"/>
+      <c r="A6" s="112"/>
+      <c r="B6" s="115"/>
+      <c r="C6" s="118"/>
+      <c r="D6" s="112"/>
+      <c r="E6" s="115"/>
+      <c r="F6" s="115"/>
+      <c r="G6" s="118"/>
+      <c r="H6" s="112"/>
+      <c r="I6" s="115"/>
+      <c r="J6" s="115"/>
+      <c r="K6" s="121"/>
       <c r="L6" s="73"/>
       <c r="M6" s="73"/>
       <c r="N6" s="73"/>
@@ -15115,8 +15152,8 @@
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:IC277"/>
   <sheetViews>
-    <sheetView topLeftCell="AE1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="AK5" sqref="AK5"/>
+    <sheetView topLeftCell="AK124" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="AX133" sqref="AX133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -22651,7 +22688,7 @@
       <c r="L27" t="s">
         <v>228</v>
       </c>
-      <c r="M27" s="121"/>
+      <c r="M27" s="122"/>
       <c r="O27" s="12" t="s">
         <v>746</v>
       </c>
@@ -22736,7 +22773,7 @@
       <c r="L28" t="s">
         <v>235</v>
       </c>
-      <c r="M28" s="121"/>
+      <c r="M28" s="122"/>
       <c r="O28" s="12" t="s">
         <v>822</v>
       </c>
@@ -23161,7 +23198,7 @@
       <c r="L34" t="s">
         <v>276</v>
       </c>
-      <c r="M34" s="121"/>
+      <c r="M34" s="122"/>
       <c r="O34" s="12" t="s">
         <v>909</v>
       </c>
@@ -23223,7 +23260,7 @@
       <c r="L35" t="s">
         <v>283</v>
       </c>
-      <c r="M35" s="121"/>
+      <c r="M35" s="122"/>
       <c r="O35" s="12" t="s">
         <v>915</v>
       </c>
@@ -23518,8 +23555,8 @@
       <c r="O40" s="12" t="s">
         <v>1035</v>
       </c>
-      <c r="AX40" s="6" t="s">
-        <v>1863</v>
+      <c r="AX40" s="94" t="s">
+        <v>3040</v>
       </c>
       <c r="BC40" s="6" t="s">
         <v>1625</v>
@@ -23572,7 +23609,7 @@
         <v>1094</v>
       </c>
       <c r="AX41" s="6" t="s">
-        <v>1864</v>
+        <v>1863</v>
       </c>
       <c r="BC41" s="6" t="s">
         <v>1626</v>
@@ -23621,7 +23658,7 @@
         <v>1734</v>
       </c>
       <c r="AX42" s="6" t="s">
-        <v>1865</v>
+        <v>1864</v>
       </c>
       <c r="BC42" s="6" t="s">
         <v>1617</v>
@@ -23670,7 +23707,7 @@
         <v>1720</v>
       </c>
       <c r="AX43" s="6" t="s">
-        <v>1536</v>
+        <v>1865</v>
       </c>
       <c r="BC43" s="6" t="s">
         <v>1613</v>
@@ -23720,7 +23757,7 @@
       </c>
       <c r="P44" s="6"/>
       <c r="AX44" s="6" t="s">
-        <v>1537</v>
+        <v>1536</v>
       </c>
       <c r="BC44" s="6" t="s">
         <v>1636</v>
@@ -23772,7 +23809,7 @@
       </c>
       <c r="P45" s="6"/>
       <c r="AX45" s="6" t="s">
-        <v>1866</v>
+        <v>1537</v>
       </c>
       <c r="BC45" s="6" t="s">
         <v>1637</v>
@@ -23821,7 +23858,7 @@
       <c r="M46" s="3"/>
       <c r="P46" s="6"/>
       <c r="AX46" s="6" t="s">
-        <v>1538</v>
+        <v>1866</v>
       </c>
       <c r="BC46" s="6" t="s">
         <v>1638</v>
@@ -23870,7 +23907,7 @@
       <c r="M47" s="4"/>
       <c r="P47" s="6"/>
       <c r="AX47" s="6" t="s">
-        <v>1867</v>
+        <v>1538</v>
       </c>
       <c r="BC47" s="6" t="s">
         <v>1920</v>
@@ -23919,7 +23956,7 @@
       </c>
       <c r="M48" s="4"/>
       <c r="AX48" s="6" t="s">
-        <v>1868</v>
+        <v>1867</v>
       </c>
       <c r="BC48" s="6" t="s">
         <v>1639</v>
@@ -23968,7 +24005,7 @@
       </c>
       <c r="M49" s="4"/>
       <c r="AX49" s="6" t="s">
-        <v>1869</v>
+        <v>1868</v>
       </c>
       <c r="BC49" s="6" t="s">
         <v>1628</v>
@@ -24018,7 +24055,7 @@
       <c r="M50" s="4"/>
       <c r="P50" s="6"/>
       <c r="AX50" s="6" t="s">
-        <v>1539</v>
+        <v>1869</v>
       </c>
       <c r="BC50" s="6" t="s">
         <v>1615</v>
@@ -24068,7 +24105,7 @@
       <c r="M51" s="4"/>
       <c r="P51" s="6"/>
       <c r="AX51" s="6" t="s">
-        <v>1870</v>
+        <v>1539</v>
       </c>
       <c r="BC51" s="6" t="s">
         <v>1616</v>
@@ -24117,7 +24154,7 @@
       </c>
       <c r="M52" s="3"/>
       <c r="AX52" s="6" t="s">
-        <v>1871</v>
+        <v>1870</v>
       </c>
       <c r="BC52" s="6" t="s">
         <v>1632</v>
@@ -24167,7 +24204,7 @@
       <c r="M53" s="3"/>
       <c r="P53" s="6"/>
       <c r="AX53" s="6" t="s">
-        <v>1540</v>
+        <v>1871</v>
       </c>
       <c r="BC53" s="6" t="s">
         <v>1610</v>
@@ -24217,7 +24254,7 @@
       <c r="M54" s="4"/>
       <c r="P54" s="6"/>
       <c r="AX54" s="6" t="s">
-        <v>1541</v>
+        <v>1540</v>
       </c>
       <c r="BC54" s="6" t="s">
         <v>1921</v>
@@ -24265,7 +24302,7 @@
       <c r="M55" s="4"/>
       <c r="P55" s="6"/>
       <c r="AX55" s="6" t="s">
-        <v>1542</v>
+        <v>1541</v>
       </c>
       <c r="BC55" s="6" t="s">
         <v>1629</v>
@@ -24313,7 +24350,7 @@
       <c r="M56" s="4"/>
       <c r="P56" s="6"/>
       <c r="AX56" s="6" t="s">
-        <v>1543</v>
+        <v>1542</v>
       </c>
       <c r="BC56" s="6" t="s">
         <v>1644</v>
@@ -24361,7 +24398,7 @@
       <c r="M57" s="3"/>
       <c r="P57" s="6"/>
       <c r="AX57" s="6" t="s">
-        <v>1517</v>
+        <v>1543</v>
       </c>
       <c r="BC57" s="6" t="s">
         <v>1922</v>
@@ -24408,7 +24445,7 @@
       <c r="M58" s="4"/>
       <c r="P58" s="6"/>
       <c r="AX58" s="6" t="s">
-        <v>1544</v>
+        <v>1517</v>
       </c>
       <c r="BC58" s="6" t="s">
         <v>1923</v>
@@ -24452,7 +24489,7 @@
       <c r="M59" s="4"/>
       <c r="P59" s="6"/>
       <c r="AX59" s="6" t="s">
-        <v>1872</v>
+        <v>1544</v>
       </c>
       <c r="BC59" s="6" t="s">
         <v>1630</v>
@@ -24496,7 +24533,7 @@
       <c r="M60" s="3"/>
       <c r="P60" s="6"/>
       <c r="AX60" s="6" t="s">
-        <v>1873</v>
+        <v>1872</v>
       </c>
       <c r="BC60" s="6" t="s">
         <v>1640</v>
@@ -24540,7 +24577,7 @@
       <c r="M61" s="4"/>
       <c r="P61" s="6"/>
       <c r="AX61" s="6" t="s">
-        <v>1874</v>
+        <v>1873</v>
       </c>
       <c r="BC61" s="6" t="s">
         <v>1633</v>
@@ -24583,8 +24620,8 @@
       </c>
       <c r="M62" s="4"/>
       <c r="P62" s="6"/>
-      <c r="AX62" s="6" t="s">
-        <v>1875</v>
+      <c r="AX62" s="94" t="s">
+        <v>3038</v>
       </c>
       <c r="BC62" s="6" t="s">
         <v>1634</v>
@@ -24628,7 +24665,7 @@
       <c r="M63" s="4"/>
       <c r="P63" s="6"/>
       <c r="AX63" s="6" t="s">
-        <v>1545</v>
+        <v>1874</v>
       </c>
       <c r="BC63" s="6" t="s">
         <v>1627</v>
@@ -24672,7 +24709,7 @@
       <c r="M64" s="4"/>
       <c r="P64" s="6"/>
       <c r="AX64" s="6" t="s">
-        <v>1876</v>
+        <v>1875</v>
       </c>
       <c r="BD64" s="6" t="s">
         <v>1700</v>
@@ -24713,7 +24750,7 @@
       <c r="M65" s="4"/>
       <c r="P65" s="6"/>
       <c r="AX65" s="6" t="s">
-        <v>1877</v>
+        <v>1545</v>
       </c>
       <c r="BD65" s="6" t="s">
         <v>1649</v>
@@ -24754,7 +24791,7 @@
       <c r="M66" s="4"/>
       <c r="P66" s="6"/>
       <c r="AX66" s="6" t="s">
-        <v>1878</v>
+        <v>1876</v>
       </c>
       <c r="BD66" s="6" t="s">
         <v>1669</v>
@@ -24795,7 +24832,7 @@
       <c r="M67" s="4"/>
       <c r="P67" s="6"/>
       <c r="AX67" s="6" t="s">
-        <v>1546</v>
+        <v>1877</v>
       </c>
       <c r="BD67" s="6" t="s">
         <v>1674</v>
@@ -24836,7 +24873,7 @@
       <c r="M68" s="4"/>
       <c r="P68" s="6"/>
       <c r="AX68" s="6" t="s">
-        <v>1547</v>
+        <v>1878</v>
       </c>
       <c r="BD68" s="6" t="s">
         <v>1652</v>
@@ -24876,7 +24913,7 @@
       </c>
       <c r="M69" s="4"/>
       <c r="AX69" s="6" t="s">
-        <v>1548</v>
+        <v>1546</v>
       </c>
       <c r="BD69" s="6" t="s">
         <v>1982</v>
@@ -24917,7 +24954,7 @@
       <c r="M70" s="4"/>
       <c r="P70" s="6"/>
       <c r="AX70" s="6" t="s">
-        <v>1549</v>
+        <v>1547</v>
       </c>
       <c r="BD70" s="6" t="s">
         <v>1695</v>
@@ -24958,7 +24995,7 @@
       <c r="M71" s="4"/>
       <c r="P71" s="6"/>
       <c r="AX71" s="6" t="s">
-        <v>1550</v>
+        <v>1548</v>
       </c>
       <c r="BD71" s="6" t="s">
         <v>1670</v>
@@ -24999,7 +25036,7 @@
       <c r="M72" s="4"/>
       <c r="P72" s="6"/>
       <c r="AX72" s="6" t="s">
-        <v>1519</v>
+        <v>1549</v>
       </c>
       <c r="BD72" s="6" t="s">
         <v>1665</v>
@@ -25040,7 +25077,7 @@
       <c r="M73" s="4"/>
       <c r="P73" s="6"/>
       <c r="AX73" s="6" t="s">
-        <v>1551</v>
+        <v>1550</v>
       </c>
       <c r="BD73" s="6" t="s">
         <v>1696</v>
@@ -25081,7 +25118,7 @@
       <c r="M74" s="4"/>
       <c r="P74" s="6"/>
       <c r="AX74" s="6" t="s">
-        <v>1879</v>
+        <v>1519</v>
       </c>
       <c r="BD74" s="6" t="s">
         <v>1684</v>
@@ -25122,7 +25159,7 @@
       <c r="M75" s="4"/>
       <c r="P75" s="6"/>
       <c r="AX75" s="6" t="s">
-        <v>1880</v>
+        <v>1551</v>
       </c>
       <c r="BD75" s="6" t="s">
         <v>1697</v>
@@ -25162,8 +25199,8 @@
       </c>
       <c r="M76" s="4"/>
       <c r="P76" s="6"/>
-      <c r="AX76" s="6" t="s">
-        <v>1881</v>
+      <c r="AX76" s="94" t="s">
+        <v>3039</v>
       </c>
       <c r="BD76" s="6" t="s">
         <v>1983</v>
@@ -25204,7 +25241,7 @@
       <c r="M77" s="4"/>
       <c r="P77" s="6"/>
       <c r="AX77" s="6" t="s">
-        <v>1997</v>
+        <v>1879</v>
       </c>
       <c r="BD77" s="6" t="s">
         <v>1647</v>
@@ -25245,7 +25282,7 @@
       <c r="M78" s="4"/>
       <c r="P78" s="6"/>
       <c r="AX78" s="6" t="s">
-        <v>1998</v>
+        <v>1880</v>
       </c>
       <c r="BD78" s="6" t="s">
         <v>1698</v>
@@ -25286,7 +25323,7 @@
       <c r="M79" s="4"/>
       <c r="P79" s="6"/>
       <c r="AX79" s="6" t="s">
-        <v>1552</v>
+        <v>1881</v>
       </c>
       <c r="BD79" s="6" t="s">
         <v>1648</v>
@@ -25327,7 +25364,7 @@
       <c r="M80" s="3"/>
       <c r="P80" s="6"/>
       <c r="AX80" s="6" t="s">
-        <v>1999</v>
+        <v>1997</v>
       </c>
       <c r="BD80" s="6" t="s">
         <v>1694</v>
@@ -25368,7 +25405,7 @@
       <c r="M81" s="4"/>
       <c r="P81" s="6"/>
       <c r="AX81" s="6" t="s">
-        <v>1883</v>
+        <v>1998</v>
       </c>
       <c r="BD81" s="6" t="s">
         <v>1690</v>
@@ -25409,7 +25446,7 @@
       <c r="M82" s="4"/>
       <c r="P82" s="6"/>
       <c r="AX82" s="6" t="s">
-        <v>1553</v>
+        <v>1552</v>
       </c>
       <c r="BD82" s="6" t="s">
         <v>1747</v>
@@ -25450,7 +25487,7 @@
       <c r="M83" s="4"/>
       <c r="P83" s="6"/>
       <c r="AX83" s="6" t="s">
-        <v>1884</v>
+        <v>1999</v>
       </c>
       <c r="BD83" s="6" t="s">
         <v>1749</v>
@@ -25488,7 +25525,7 @@
       <c r="M84" s="4"/>
       <c r="P84" s="6"/>
       <c r="AX84" s="6" t="s">
-        <v>2000</v>
+        <v>1883</v>
       </c>
       <c r="BD84" s="6" t="s">
         <v>1984</v>
@@ -25525,7 +25562,7 @@
       </c>
       <c r="M85" s="3"/>
       <c r="AX85" s="6" t="s">
-        <v>2001</v>
+        <v>1553</v>
       </c>
       <c r="BD85" s="6" t="s">
         <v>1656</v>
@@ -25561,8 +25598,8 @@
         <v>608</v>
       </c>
       <c r="M86" s="4"/>
-      <c r="AX86" s="6" t="s">
-        <v>2002</v>
+      <c r="AX86" s="94" t="s">
+        <v>3041</v>
       </c>
       <c r="BD86" s="6" t="s">
         <v>1748</v>
@@ -25598,8 +25635,8 @@
         <v>614</v>
       </c>
       <c r="M87" s="4"/>
-      <c r="AX87" s="6" t="s">
-        <v>2003</v>
+      <c r="AX87" s="94" t="s">
+        <v>3042</v>
       </c>
       <c r="BD87" s="6" t="s">
         <v>1985</v>
@@ -25636,7 +25673,7 @@
       </c>
       <c r="M88" s="4"/>
       <c r="AX88" s="6" t="s">
-        <v>2004</v>
+        <v>1884</v>
       </c>
       <c r="BD88" s="6" t="s">
         <v>1750</v>
@@ -25673,7 +25710,7 @@
       </c>
       <c r="M89" s="4"/>
       <c r="AX89" s="6" t="s">
-        <v>1554</v>
+        <v>2000</v>
       </c>
       <c r="BD89" s="6" t="s">
         <v>1744</v>
@@ -25709,8 +25746,8 @@
         <v>632</v>
       </c>
       <c r="M90" s="4"/>
-      <c r="AX90" s="6" t="s">
-        <v>1885</v>
+      <c r="AX90" s="94" t="s">
+        <v>3043</v>
       </c>
       <c r="BD90" s="6" t="s">
         <v>1745</v>
@@ -25747,7 +25784,7 @@
       </c>
       <c r="M91" s="3"/>
       <c r="AX91" s="6" t="s">
-        <v>2005</v>
+        <v>2001</v>
       </c>
       <c r="BD91" s="6" t="s">
         <v>1986</v>
@@ -25784,7 +25821,7 @@
       </c>
       <c r="M92" s="4"/>
       <c r="AX92" s="6" t="s">
-        <v>1555</v>
+        <v>2002</v>
       </c>
       <c r="BD92" s="6" t="s">
         <v>1746</v>
@@ -25820,8 +25857,8 @@
         <v>650</v>
       </c>
       <c r="M93" s="3"/>
-      <c r="AX93" s="6" t="s">
-        <v>2006</v>
+      <c r="AX93" s="94" t="s">
+        <v>3044</v>
       </c>
       <c r="BD93" s="6" t="s">
         <v>1987</v>
@@ -25858,7 +25895,7 @@
       </c>
       <c r="M94" s="3"/>
       <c r="AX94" s="6" t="s">
-        <v>1556</v>
+        <v>2003</v>
       </c>
       <c r="BD94" s="6" t="s">
         <v>1988</v>
@@ -25895,7 +25932,7 @@
       </c>
       <c r="M95" s="4"/>
       <c r="AX95" s="6" t="s">
-        <v>1557</v>
+        <v>2004</v>
       </c>
       <c r="BD95" s="6" t="s">
         <v>1989</v>
@@ -25932,7 +25969,7 @@
       </c>
       <c r="M96" s="3"/>
       <c r="AX96" s="6" t="s">
-        <v>1558</v>
+        <v>1554</v>
       </c>
       <c r="BD96" s="6" t="s">
         <v>1660</v>
@@ -25969,7 +26006,7 @@
       </c>
       <c r="M97" s="4"/>
       <c r="AX97" s="6" t="s">
-        <v>1559</v>
+        <v>1885</v>
       </c>
       <c r="BD97" s="6" t="s">
         <v>1990</v>
@@ -26005,8 +26042,8 @@
         <v>680</v>
       </c>
       <c r="M98" s="4"/>
-      <c r="AX98" s="6" t="s">
-        <v>1560</v>
+      <c r="AX98" s="94" t="s">
+        <v>3047</v>
       </c>
       <c r="BD98" s="7" t="s">
         <v>2675</v>
@@ -26043,7 +26080,7 @@
       </c>
       <c r="M99" s="4"/>
       <c r="AX99" s="6" t="s">
-        <v>1561</v>
+        <v>2005</v>
       </c>
       <c r="BD99" s="7"/>
       <c r="CP99" s="12" t="s">
@@ -26078,7 +26115,7 @@
       </c>
       <c r="M100" s="4"/>
       <c r="AX100" s="6" t="s">
-        <v>2007</v>
+        <v>1555</v>
       </c>
       <c r="CP100" s="12" t="s">
         <v>2147</v>
@@ -26112,7 +26149,7 @@
       </c>
       <c r="M101" s="4"/>
       <c r="AX101" s="6" t="s">
-        <v>1562</v>
+        <v>2006</v>
       </c>
       <c r="CP101" s="12" t="s">
         <v>2658</v>
@@ -26146,7 +26183,7 @@
       </c>
       <c r="M102" s="4"/>
       <c r="AX102" s="6" t="s">
-        <v>1563</v>
+        <v>1556</v>
       </c>
       <c r="CP102" s="12" t="s">
         <v>2148</v>
@@ -26180,7 +26217,7 @@
       </c>
       <c r="M103" s="4"/>
       <c r="AX103" s="6" t="s">
-        <v>1564</v>
+        <v>1557</v>
       </c>
       <c r="CP103" s="12" t="s">
         <v>2660</v>
@@ -26214,7 +26251,7 @@
       </c>
       <c r="M104" s="4"/>
       <c r="AX104" s="6" t="s">
-        <v>1565</v>
+        <v>1558</v>
       </c>
       <c r="CP104" s="12" t="s">
         <v>2149</v>
@@ -26248,7 +26285,7 @@
       </c>
       <c r="M105" s="4"/>
       <c r="AX105" s="6" t="s">
-        <v>1566</v>
+        <v>1559</v>
       </c>
       <c r="CP105" s="12" t="s">
         <v>2662</v>
@@ -26282,7 +26319,7 @@
       </c>
       <c r="M106" s="4"/>
       <c r="AX106" s="6" t="s">
-        <v>1567</v>
+        <v>1560</v>
       </c>
       <c r="CP106" s="12" t="s">
         <v>2298</v>
@@ -26316,7 +26353,7 @@
       </c>
       <c r="M107" s="4"/>
       <c r="AX107" s="6" t="s">
-        <v>2008</v>
+        <v>1561</v>
       </c>
       <c r="CP107" s="12" t="s">
         <v>2664</v>
@@ -26349,8 +26386,8 @@
         <v>739</v>
       </c>
       <c r="M108" s="4"/>
-      <c r="AX108" s="6" t="s">
-        <v>1568</v>
+      <c r="AX108" s="94" t="s">
+        <v>3046</v>
       </c>
       <c r="CP108" s="12" t="s">
         <v>2150</v>
@@ -26384,7 +26421,7 @@
       </c>
       <c r="M109" s="4"/>
       <c r="AX109" s="6" t="s">
-        <v>1569</v>
+        <v>2007</v>
       </c>
       <c r="CP109" s="12" t="s">
         <v>2666</v>
@@ -26418,7 +26455,7 @@
       </c>
       <c r="M110" s="4"/>
       <c r="AX110" s="6" t="s">
-        <v>2009</v>
+        <v>1562</v>
       </c>
       <c r="CP110" s="12" t="s">
         <v>2299</v>
@@ -26452,7 +26489,7 @@
       </c>
       <c r="M111" s="4"/>
       <c r="AX111" s="6" t="s">
-        <v>1570</v>
+        <v>1563</v>
       </c>
       <c r="CP111" s="12" t="s">
         <v>2668</v>
@@ -26486,7 +26523,7 @@
       </c>
       <c r="M112" s="4"/>
       <c r="AX112" s="6" t="s">
-        <v>1571</v>
+        <v>1564</v>
       </c>
       <c r="CP112" s="12" t="s">
         <v>2300</v>
@@ -26520,7 +26557,7 @@
       </c>
       <c r="M113" s="4"/>
       <c r="AX113" s="6" t="s">
-        <v>2010</v>
+        <v>1565</v>
       </c>
       <c r="CP113" s="12" t="s">
         <v>2670</v>
@@ -26554,7 +26591,7 @@
       </c>
       <c r="M114" s="4"/>
       <c r="AX114" s="6" t="s">
-        <v>2011</v>
+        <v>1566</v>
       </c>
       <c r="CP114" s="12" t="s">
         <v>2151</v>
@@ -26588,7 +26625,7 @@
       </c>
       <c r="M115" s="4"/>
       <c r="AX115" s="6" t="s">
-        <v>1572</v>
+        <v>1567</v>
       </c>
       <c r="CP115" s="12" t="s">
         <v>2672</v>
@@ -26622,7 +26659,7 @@
       </c>
       <c r="M116" s="4"/>
       <c r="AX116" s="6" t="s">
-        <v>2012</v>
+        <v>2008</v>
       </c>
       <c r="CS116" s="40"/>
     </row>
@@ -26647,7 +26684,7 @@
       </c>
       <c r="M117" s="4"/>
       <c r="AX117" s="6" t="s">
-        <v>1573</v>
+        <v>1568</v>
       </c>
       <c r="CS117" s="40"/>
     </row>
@@ -26671,8 +26708,8 @@
         <v>798</v>
       </c>
       <c r="M118" s="3"/>
-      <c r="AX118" s="6" t="s">
-        <v>2013</v>
+      <c r="AX118" s="94" t="s">
+        <v>3045</v>
       </c>
       <c r="CS118" s="40"/>
     </row>
@@ -26697,7 +26734,7 @@
       </c>
       <c r="M119" s="3"/>
       <c r="AX119" s="6" t="s">
-        <v>2014</v>
+        <v>1569</v>
       </c>
       <c r="CS119" s="40"/>
     </row>
@@ -26722,7 +26759,7 @@
       </c>
       <c r="M120" s="4"/>
       <c r="AX120" s="6" t="s">
-        <v>2015</v>
+        <v>2009</v>
       </c>
       <c r="CS120" s="40"/>
     </row>
@@ -26747,7 +26784,7 @@
       </c>
       <c r="M121" s="4"/>
       <c r="AX121" s="6" t="s">
-        <v>1574</v>
+        <v>1570</v>
       </c>
       <c r="CS121" s="40"/>
     </row>
@@ -26772,7 +26809,7 @@
       </c>
       <c r="M122" s="4"/>
       <c r="AX122" s="6" t="s">
-        <v>1991</v>
+        <v>1571</v>
       </c>
       <c r="CS122" s="40"/>
     </row>
@@ -26796,8 +26833,8 @@
         <v>827</v>
       </c>
       <c r="M123" s="3"/>
-      <c r="AX123" s="6" t="s">
-        <v>1882</v>
+      <c r="AX123" s="94" t="s">
+        <v>3048</v>
       </c>
       <c r="CS123" s="40"/>
     </row>
@@ -26822,7 +26859,7 @@
       </c>
       <c r="M124" s="4"/>
       <c r="AX124" s="6" t="s">
-        <v>1575</v>
+        <v>2010</v>
       </c>
       <c r="CS124" s="40"/>
     </row>
@@ -26847,7 +26884,7 @@
       </c>
       <c r="M125" s="4"/>
       <c r="AX125" s="6" t="s">
-        <v>1996</v>
+        <v>2011</v>
       </c>
       <c r="CS125" s="40"/>
     </row>
@@ -26872,7 +26909,7 @@
       </c>
       <c r="M126" s="4"/>
       <c r="AX126" s="6" t="s">
-        <v>1995</v>
+        <v>1572</v>
       </c>
       <c r="CS126" s="40"/>
     </row>
@@ -26897,7 +26934,7 @@
       </c>
       <c r="M127" s="3"/>
       <c r="AX127" s="6" t="s">
-        <v>1576</v>
+        <v>2012</v>
       </c>
       <c r="CS127" s="40"/>
     </row>
@@ -26922,7 +26959,7 @@
       </c>
       <c r="M128" s="4"/>
       <c r="AX128" s="6" t="s">
-        <v>1398</v>
+        <v>1573</v>
       </c>
       <c r="CS128" s="40"/>
     </row>
@@ -26946,8 +26983,8 @@
         <v>861</v>
       </c>
       <c r="M129" s="4"/>
-      <c r="AX129" s="39" t="s">
-        <v>2157</v>
+      <c r="AX129" s="6" t="s">
+        <v>2013</v>
       </c>
       <c r="CS129" s="40"/>
     </row>
@@ -26972,7 +27009,7 @@
       </c>
       <c r="M130" s="3"/>
       <c r="AX130" s="6" t="s">
-        <v>1992</v>
+        <v>2014</v>
       </c>
       <c r="CS130" s="40"/>
     </row>
@@ -26997,7 +27034,7 @@
       </c>
       <c r="M131" s="4"/>
       <c r="AX131" s="6" t="s">
-        <v>1994</v>
+        <v>2015</v>
       </c>
       <c r="CS131" s="40"/>
     </row>
@@ -27022,7 +27059,7 @@
       </c>
       <c r="M132" s="4"/>
       <c r="AX132" s="6" t="s">
-        <v>1577</v>
+        <v>1574</v>
       </c>
       <c r="CS132" s="40"/>
     </row>
@@ -27046,8 +27083,8 @@
         <v>885</v>
       </c>
       <c r="M133" s="3"/>
-      <c r="AX133" s="6" t="s">
-        <v>1578</v>
+      <c r="AX133" s="94" t="s">
+        <v>3049</v>
       </c>
       <c r="CS133" s="40"/>
     </row>
@@ -27072,7 +27109,7 @@
       </c>
       <c r="M134" s="4"/>
       <c r="AX134" s="6" t="s">
-        <v>1993</v>
+        <v>1991</v>
       </c>
       <c r="CS134" s="40"/>
     </row>
@@ -27096,6 +27133,9 @@
         <v>896</v>
       </c>
       <c r="M135" s="4"/>
+      <c r="AX135" s="6" t="s">
+        <v>1882</v>
+      </c>
       <c r="CS135" s="40"/>
     </row>
     <row r="136" spans="2:97" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -27118,6 +27158,9 @@
         <v>902</v>
       </c>
       <c r="M136" s="4"/>
+      <c r="AX136" s="6" t="s">
+        <v>1575</v>
+      </c>
       <c r="CS136" s="40"/>
     </row>
     <row r="137" spans="2:97" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -27140,6 +27183,9 @@
         <v>908</v>
       </c>
       <c r="M137" s="4"/>
+      <c r="AX137" s="6" t="s">
+        <v>1996</v>
+      </c>
       <c r="CS137" s="40"/>
     </row>
     <row r="138" spans="2:97" x14ac:dyDescent="0.3">
@@ -27162,6 +27208,9 @@
         <v>914</v>
       </c>
       <c r="M138" s="3"/>
+      <c r="AX138" s="6" t="s">
+        <v>1995</v>
+      </c>
       <c r="CS138" s="40"/>
     </row>
     <row r="139" spans="2:97" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -27184,6 +27233,9 @@
         <v>920</v>
       </c>
       <c r="M139" s="4"/>
+      <c r="AX139" s="6" t="s">
+        <v>1576</v>
+      </c>
       <c r="CS139" s="40"/>
     </row>
     <row r="140" spans="2:97" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -27206,6 +27258,9 @@
         <v>926</v>
       </c>
       <c r="M140" s="4"/>
+      <c r="AX140" s="6" t="s">
+        <v>1398</v>
+      </c>
       <c r="CS140" s="40"/>
     </row>
     <row r="141" spans="2:97" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -27228,6 +27283,9 @@
         <v>932</v>
       </c>
       <c r="M141" s="4"/>
+      <c r="AX141" s="39" t="s">
+        <v>2157</v>
+      </c>
       <c r="CS141" s="40"/>
     </row>
     <row r="142" spans="2:97" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -27250,6 +27308,9 @@
         <v>938</v>
       </c>
       <c r="M142" s="4"/>
+      <c r="AX142" s="6" t="s">
+        <v>1992</v>
+      </c>
       <c r="CS142" s="40"/>
     </row>
     <row r="143" spans="2:97" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -27272,6 +27333,9 @@
         <v>944</v>
       </c>
       <c r="M143" s="4"/>
+      <c r="AX143" s="6" t="s">
+        <v>1994</v>
+      </c>
       <c r="CS143" s="40"/>
     </row>
     <row r="144" spans="2:97" x14ac:dyDescent="0.3">
@@ -27290,6 +27354,9 @@
       <c r="H144" t="s">
         <v>949</v>
       </c>
+      <c r="AX144" s="6" t="s">
+        <v>1577</v>
+      </c>
       <c r="CS144" s="40"/>
     </row>
     <row r="145" spans="2:97" x14ac:dyDescent="0.3">
@@ -27308,6 +27375,9 @@
       <c r="H145" t="s">
         <v>954</v>
       </c>
+      <c r="AX145" s="6" t="s">
+        <v>1578</v>
+      </c>
       <c r="CS145" s="40"/>
     </row>
     <row r="146" spans="2:97" x14ac:dyDescent="0.3">
@@ -27325,6 +27395,9 @@
       </c>
       <c r="H146" t="s">
         <v>959</v>
+      </c>
+      <c r="AX146" s="6" t="s">
+        <v>1993</v>
       </c>
       <c r="CS146" s="40"/>
     </row>
@@ -28836,7 +28909,7 @@
       <c r="CS277" s="40"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="l8XLfF/Enq7Cr/WDkixgZHvDmvGd4Us6dBeJkqyY1BsI3RDU4ixSx6K+KUKpkZVC2YCKy30xAauu2ydDMrR5Ww==" saltValue="9KZhV0eAboNH4tT0xVCMiQ==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="ReLuXiCIzrYRqmaP2jDysp01Zx9gpOUw/dn0RvJcXcm4J4PW5d7cb2O4iZNZC0SXSTTCndFImQ4YfBam9XEKcw==" saltValue="ACYHVy7WShbC5GkNGwql2Q==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="2">
     <mergeCell ref="M27:M28"/>
     <mergeCell ref="M34:M35"/>

</xml_diff>

<commit_message>
Modified "raw data" to "reported data"
</commit_message>
<xml_diff>
--- a/Excel_templates/MOSAIC_input_excel_file_2022.xlsx
+++ b/Excel_templates/MOSAIC_input_excel_file_2022.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20393"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20394"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sparadis\Documents\ETH\MOSAIC\MOSAIC_Client\Excel_templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3796063-9DE9-43B1-8447-4E968061B392}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BED7ED62-A88F-4851-90FC-E287F95B89FA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30204" yWindow="10044" windowWidth="40020" windowHeight="22296" tabRatio="694" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30204" yWindow="10044" windowWidth="40020" windowHeight="22296" tabRatio="694" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ARTICLE_AUTHOR" sheetId="3" r:id="rId1"/>
@@ -10412,7 +10412,7 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -12300,11 +12300,11 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:CB52"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane xSplit="3" ySplit="6" topLeftCell="D7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="A7" sqref="A7"/>
+      <selection pane="bottomRight" activeCell="L6" sqref="L6:CB6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -15129,7 +15129,7 @@
           </x14:formula1>
           <xm:sqref>D7:D1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Raw / calculated data" prompt="Specify if the data provided has been extracted directly from the source (i.e. paper) or is calculated using available data. If left blank, default of &quot;raw data&quot; will be used. " xr:uid="{30C7084F-BEF5-4E01-80B0-5EBF52EBFAA6}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Reported / calculated data" prompt="Specify if the data provided has been extracted directly from the source (i.e. paper) or is calculated using available data. If left blank, default of &quot;reported data&quot; will be used. " xr:uid="{30C7084F-BEF5-4E01-80B0-5EBF52EBFAA6}">
           <x14:formula1>
             <xm:f>SET_VARIABLES!$BF$2:$BF$3</xm:f>
           </x14:formula1>

</xml_diff>

<commit_message>
Modified "raw data" to "reported data" in the drop-down menu.
</commit_message>
<xml_diff>
--- a/Excel_templates/MOSAIC_input_excel_file_2022.xlsx
+++ b/Excel_templates/MOSAIC_input_excel_file_2022.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sparadis\Documents\ETH\MOSAIC\MOSAIC_Client\Excel_templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BED7ED62-A88F-4851-90FC-E287F95B89FA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{999EF069-EC65-4261-8929-97D3FD3B96F6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30204" yWindow="10044" windowWidth="40020" windowHeight="22296" tabRatio="694" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30204" yWindow="10044" windowWidth="40020" windowHeight="22296" tabRatio="694" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ARTICLE_AUTHOR" sheetId="3" r:id="rId1"/>
@@ -8547,9 +8547,6 @@
     <t>Data_source</t>
   </si>
   <si>
-    <t>Raw_data</t>
-  </si>
-  <si>
     <t>Calculated_data</t>
   </si>
   <si>
@@ -9361,6 +9358,9 @@
   </si>
   <si>
     <t>RV Vityaz (II)</t>
+  </si>
+  <si>
+    <t>Reported_data</t>
   </si>
 </sst>
 </file>
@@ -9836,7 +9836,7 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="123">
+  <cellXfs count="124">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="13" applyFont="1" applyFill="1" applyAlignment="1"/>
@@ -10069,6 +10069,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="12" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="16">
     <cellStyle name="20% - Accent1" xfId="3" builtinId="30" customBuiltin="1"/>
@@ -10412,7 +10415,7 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -10472,7 +10475,7 @@
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B3" s="27"/>
       <c r="D3" s="92"/>
-      <c r="E3" s="35"/>
+      <c r="E3" s="123"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B4" s="27"/>
@@ -10572,19 +10575,19 @@
         <v>1824</v>
       </c>
       <c r="E2" s="55" t="s">
-        <v>2882</v>
+        <v>2881</v>
       </c>
       <c r="F2" s="58" t="s">
         <v>1825</v>
       </c>
       <c r="G2" s="58" t="s">
+        <v>2883</v>
+      </c>
+      <c r="H2" s="58" t="s">
         <v>2884</v>
       </c>
-      <c r="H2" s="58" t="s">
+      <c r="I2" s="58" t="s">
         <v>2885</v>
-      </c>
-      <c r="I2" s="58" t="s">
-        <v>2886</v>
       </c>
       <c r="J2" s="58" t="s">
         <v>1826</v>
@@ -12300,11 +12303,11 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:CB52"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane xSplit="3" ySplit="6" topLeftCell="D7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="L6" sqref="L6:CB6"/>
+      <selection pane="bottomRight" activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -12353,55 +12356,55 @@
         <v>2680</v>
       </c>
       <c r="O1" s="72" t="s">
-        <v>2966</v>
+        <v>2965</v>
       </c>
       <c r="P1" s="72" t="s">
-        <v>2966</v>
+        <v>2965</v>
       </c>
       <c r="Q1" s="72" t="s">
-        <v>2966</v>
+        <v>2965</v>
       </c>
       <c r="R1" s="72" t="s">
-        <v>2966</v>
+        <v>2965</v>
       </c>
       <c r="S1" s="72" t="s">
-        <v>2966</v>
+        <v>2965</v>
       </c>
       <c r="T1" s="72" t="s">
-        <v>2966</v>
+        <v>2965</v>
       </c>
       <c r="U1" s="72" t="s">
-        <v>2966</v>
+        <v>2965</v>
       </c>
       <c r="V1" s="72" t="s">
-        <v>2966</v>
+        <v>2965</v>
       </c>
       <c r="W1" s="72" t="s">
-        <v>2966</v>
+        <v>2965</v>
       </c>
       <c r="X1" s="72" t="s">
-        <v>2966</v>
+        <v>2965</v>
       </c>
       <c r="Y1" s="72" t="s">
-        <v>2966</v>
+        <v>2965</v>
       </c>
       <c r="Z1" s="72" t="s">
-        <v>2966</v>
+        <v>2965</v>
       </c>
       <c r="AA1" s="72" t="s">
-        <v>2966</v>
+        <v>2965</v>
       </c>
       <c r="AB1" s="72" t="s">
-        <v>2966</v>
+        <v>2965</v>
       </c>
       <c r="AC1" s="72" t="s">
-        <v>2966</v>
+        <v>2965</v>
       </c>
       <c r="AD1" s="72" t="s">
-        <v>2966</v>
+        <v>2965</v>
       </c>
       <c r="AE1" s="72" t="s">
-        <v>2966</v>
+        <v>2965</v>
       </c>
     </row>
     <row r="2" spans="1:80" s="74" customFormat="1" x14ac:dyDescent="0.3">
@@ -12448,55 +12451,55 @@
         <v>1768</v>
       </c>
       <c r="O2" s="73" t="s">
+        <v>2977</v>
+      </c>
+      <c r="P2" s="73" t="s">
         <v>2978</v>
       </c>
-      <c r="P2" s="73" t="s">
+      <c r="Q2" s="73" t="s">
         <v>2979</v>
       </c>
-      <c r="Q2" s="73" t="s">
+      <c r="R2" s="73" t="s">
         <v>2980</v>
       </c>
-      <c r="R2" s="73" t="s">
+      <c r="S2" s="73" t="s">
         <v>2981</v>
       </c>
-      <c r="S2" s="73" t="s">
+      <c r="T2" s="73" t="s">
         <v>2982</v>
       </c>
-      <c r="T2" s="73" t="s">
+      <c r="U2" s="73" t="s">
         <v>2983</v>
       </c>
-      <c r="U2" s="73" t="s">
+      <c r="V2" s="73" t="s">
         <v>2984</v>
       </c>
-      <c r="V2" s="73" t="s">
+      <c r="W2" s="73" t="s">
         <v>2985</v>
       </c>
-      <c r="W2" s="73" t="s">
+      <c r="X2" s="73" t="s">
         <v>2986</v>
       </c>
-      <c r="X2" s="73" t="s">
+      <c r="Y2" s="73" t="s">
         <v>2987</v>
       </c>
-      <c r="Y2" s="73" t="s">
+      <c r="Z2" s="73" t="s">
         <v>2988</v>
       </c>
-      <c r="Z2" s="73" t="s">
+      <c r="AA2" s="73" t="s">
         <v>2989</v>
       </c>
-      <c r="AA2" s="73" t="s">
+      <c r="AB2" s="73" t="s">
         <v>2990</v>
       </c>
-      <c r="AB2" s="73" t="s">
-        <v>2991</v>
-      </c>
       <c r="AC2" s="73" t="s">
-        <v>2967</v>
+        <v>2966</v>
       </c>
       <c r="AD2" s="73" t="s">
-        <v>2967</v>
+        <v>2966</v>
       </c>
       <c r="AE2" s="73" t="s">
-        <v>2970</v>
+        <v>2969</v>
       </c>
       <c r="AF2" s="73"/>
       <c r="AG2" s="73"/>
@@ -12561,62 +12564,62 @@
       <c r="J3" s="114"/>
       <c r="K3" s="120"/>
       <c r="L3" s="73" t="s">
-        <v>2793</v>
+        <v>2792</v>
       </c>
       <c r="M3" s="73" t="s">
-        <v>2825</v>
+        <v>2824</v>
       </c>
       <c r="N3" s="73"/>
       <c r="O3" s="73" t="s">
-        <v>2894</v>
+        <v>2893</v>
       </c>
       <c r="P3" s="73" t="s">
-        <v>2894</v>
+        <v>2893</v>
       </c>
       <c r="Q3" s="73" t="s">
-        <v>2894</v>
+        <v>2893</v>
       </c>
       <c r="R3" s="73" t="s">
-        <v>2894</v>
+        <v>2893</v>
       </c>
       <c r="S3" s="73" t="s">
-        <v>2894</v>
+        <v>2893</v>
       </c>
       <c r="T3" s="73" t="s">
-        <v>2894</v>
+        <v>2893</v>
       </c>
       <c r="U3" s="73" t="s">
-        <v>2894</v>
+        <v>2893</v>
       </c>
       <c r="V3" s="73" t="s">
-        <v>2894</v>
+        <v>2893</v>
       </c>
       <c r="W3" s="73" t="s">
-        <v>2894</v>
+        <v>2893</v>
       </c>
       <c r="X3" s="73" t="s">
-        <v>2894</v>
+        <v>2893</v>
       </c>
       <c r="Y3" s="73" t="s">
-        <v>2894</v>
+        <v>2893</v>
       </c>
       <c r="Z3" s="73" t="s">
-        <v>2894</v>
+        <v>2893</v>
       </c>
       <c r="AA3" s="73" t="s">
-        <v>2894</v>
+        <v>2893</v>
       </c>
       <c r="AB3" s="73" t="s">
-        <v>2894</v>
+        <v>2893</v>
       </c>
       <c r="AC3" s="73" t="s">
-        <v>2894</v>
+        <v>2893</v>
       </c>
       <c r="AD3" s="73" t="s">
-        <v>2894</v>
+        <v>2893</v>
       </c>
       <c r="AE3" s="73" t="s">
-        <v>2894</v>
+        <v>2893</v>
       </c>
       <c r="AF3" s="73"/>
       <c r="AG3" s="73"/>
@@ -12698,13 +12701,13 @@
       <c r="AA4" s="73"/>
       <c r="AB4" s="73"/>
       <c r="AC4" s="73" t="s">
-        <v>2993</v>
+        <v>2992</v>
       </c>
       <c r="AD4" s="73" t="s">
-        <v>2925</v>
+        <v>2924</v>
       </c>
       <c r="AE4" s="73" t="s">
-        <v>2944</v>
+        <v>2943</v>
       </c>
       <c r="AF4" s="73"/>
       <c r="AG4" s="73"/>
@@ -15152,8 +15155,8 @@
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:IC277"/>
   <sheetViews>
-    <sheetView topLeftCell="AK124" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="AX133" sqref="AX133"/>
+    <sheetView topLeftCell="BA1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="BF3" sqref="BF3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -15323,7 +15326,7 @@
         <v>603</v>
       </c>
       <c r="AK1" s="1" t="s">
-        <v>3035</v>
+        <v>3034</v>
       </c>
       <c r="AL1" s="1" t="s">
         <v>657</v>
@@ -15536,7 +15539,7 @@
         <v>sample_alkenones_description</v>
       </c>
       <c r="CV1" s="1" t="s">
-        <v>2890</v>
+        <v>2889</v>
       </c>
       <c r="CW1" s="9" t="str">
         <f>_xlfn.CONCAT(CV1,"_units")</f>
@@ -15657,7 +15660,7 @@
         <v>sample_strontium_description</v>
       </c>
       <c r="EC1" s="1" t="s">
-        <v>2810</v>
+        <v>2809</v>
       </c>
       <c r="ED1" s="9" t="str">
         <f>_xlfn.CONCAT(EC1,"_units")</f>
@@ -15677,7 +15680,7 @@
         <v>1754</v>
       </c>
       <c r="EI1" s="1" t="s">
-        <v>2811</v>
+        <v>2810</v>
       </c>
       <c r="EJ1" s="9" t="str">
         <f>_xlfn.CONCAT(EI1,"_units")</f>
@@ -15691,7 +15694,7 @@
         <v>1753</v>
       </c>
       <c r="EM1" s="9" t="s">
-        <v>2966</v>
+        <v>2965</v>
       </c>
       <c r="EN1" s="9" t="str">
         <f>_xlfn.CONCAT(EM1,"_units")</f>
@@ -15702,7 +15705,7 @@
         <v>sample_alcohols_description</v>
       </c>
       <c r="EP1" s="78" t="s">
-        <v>2814</v>
+        <v>2813</v>
       </c>
       <c r="EQ1" s="1" t="s">
         <v>2048</v>
@@ -15834,7 +15837,7 @@
         <v>1790</v>
       </c>
       <c r="GH1" s="1" t="s">
-        <v>2808</v>
+        <v>2807</v>
       </c>
       <c r="GI1" s="1" t="s">
         <v>2676</v>
@@ -15885,7 +15888,7 @@
         <v>2443</v>
       </c>
       <c r="GY1" s="22" t="s">
-        <v>2873</v>
+        <v>2872</v>
       </c>
       <c r="GZ1" s="22" t="s">
         <v>2433</v>
@@ -15903,79 +15906,79 @@
         <v>2759</v>
       </c>
       <c r="HE1" s="22" t="s">
-        <v>2877</v>
+        <v>2876</v>
       </c>
       <c r="HF1" s="1" t="s">
         <v>2364</v>
       </c>
       <c r="HG1" s="1" t="s">
+        <v>2890</v>
+      </c>
+      <c r="HH1" s="1" t="s">
         <v>2891</v>
       </c>
-      <c r="HH1" s="1" t="s">
+      <c r="HI1" s="1" t="s">
         <v>2892</v>
       </c>
-      <c r="HI1" s="1" t="s">
-        <v>2893</v>
-      </c>
       <c r="HJ1" s="1" t="s">
+        <v>2899</v>
+      </c>
+      <c r="HK1" s="1" t="s">
         <v>2900</v>
       </c>
-      <c r="HK1" s="1" t="s">
-        <v>2901</v>
-      </c>
       <c r="HL1" s="1" t="s">
-        <v>2992</v>
+        <v>2991</v>
       </c>
       <c r="HM1" s="1" t="s">
-        <v>2967</v>
+        <v>2966</v>
       </c>
       <c r="HN1" s="1" t="s">
-        <v>2970</v>
+        <v>2969</v>
       </c>
       <c r="HO1" s="1" t="s">
+        <v>2976</v>
+      </c>
+      <c r="HP1" s="1" t="s">
         <v>2977</v>
       </c>
-      <c r="HP1" s="1" t="s">
+      <c r="HQ1" s="1" t="s">
         <v>2978</v>
       </c>
-      <c r="HQ1" s="1" t="s">
+      <c r="HR1" s="1" t="s">
         <v>2979</v>
       </c>
-      <c r="HR1" s="1" t="s">
+      <c r="HS1" s="1" t="s">
         <v>2980</v>
       </c>
-      <c r="HS1" s="1" t="s">
+      <c r="HT1" s="1" t="s">
         <v>2981</v>
       </c>
-      <c r="HT1" s="1" t="s">
+      <c r="HU1" s="1" t="s">
         <v>2982</v>
       </c>
-      <c r="HU1" s="1" t="s">
+      <c r="HV1" s="1" t="s">
         <v>2983</v>
       </c>
-      <c r="HV1" s="1" t="s">
+      <c r="HW1" s="1" t="s">
         <v>2984</v>
       </c>
-      <c r="HW1" s="1" t="s">
+      <c r="HX1" s="1" t="s">
         <v>2985</v>
       </c>
-      <c r="HX1" s="1" t="s">
+      <c r="HY1" s="1" t="s">
         <v>2986</v>
       </c>
-      <c r="HY1" s="1" t="s">
+      <c r="HZ1" s="1" t="s">
         <v>2987</v>
       </c>
-      <c r="HZ1" s="1" t="s">
+      <c r="IA1" s="1" t="s">
         <v>2988</v>
       </c>
-      <c r="IA1" s="1" t="s">
+      <c r="IB1" s="1" t="s">
         <v>2989</v>
       </c>
-      <c r="IB1" s="1" t="s">
+      <c r="IC1" s="1" t="s">
         <v>2990</v>
-      </c>
-      <c r="IC1" s="1" t="s">
-        <v>2991</v>
       </c>
     </row>
     <row r="2" spans="1:237" x14ac:dyDescent="0.3">
@@ -16151,7 +16154,7 @@
         <v>5</v>
       </c>
       <c r="BF2" s="70" t="s">
-        <v>2778</v>
+        <v>3049</v>
       </c>
       <c r="BG2" s="16" t="s">
         <v>2160</v>
@@ -16310,7 +16313,7 @@
         <v>2432</v>
       </c>
       <c r="DI2" s="12" t="s">
-        <v>2872</v>
+        <v>2871</v>
       </c>
       <c r="DJ2" s="12"/>
       <c r="DK2" s="12" t="s">
@@ -16386,7 +16389,7 @@
         <v>5</v>
       </c>
       <c r="EM2" s="10" t="s">
-        <v>2967</v>
+        <v>2966</v>
       </c>
       <c r="EN2" s="90" t="s">
         <v>2253</v>
@@ -16587,85 +16590,85 @@
         <v>5</v>
       </c>
       <c r="HC2" s="10" t="s">
-        <v>2880</v>
+        <v>2879</v>
       </c>
       <c r="HD2" s="10" t="s">
-        <v>2880</v>
+        <v>2879</v>
       </c>
       <c r="HE2" s="10" t="s">
-        <v>2880</v>
+        <v>2879</v>
       </c>
       <c r="HF2" s="10" t="s">
-        <v>2894</v>
+        <v>2893</v>
       </c>
       <c r="HG2" s="10" t="s">
-        <v>2894</v>
+        <v>2893</v>
       </c>
       <c r="HH2" s="10" t="s">
-        <v>2894</v>
+        <v>2893</v>
       </c>
       <c r="HI2" s="10" t="s">
-        <v>2894</v>
+        <v>2893</v>
       </c>
       <c r="HJ2" s="10" t="s">
-        <v>2928</v>
+        <v>2927</v>
       </c>
       <c r="HK2" s="10" t="s">
-        <v>2922</v>
+        <v>2921</v>
       </c>
       <c r="HL2" s="10" t="s">
-        <v>2922</v>
+        <v>2921</v>
       </c>
       <c r="HM2" s="10" t="s">
-        <v>2894</v>
+        <v>2893</v>
       </c>
       <c r="HN2" s="10" t="s">
-        <v>2894</v>
+        <v>2893</v>
       </c>
       <c r="HO2" s="10" t="s">
-        <v>2894</v>
+        <v>2893</v>
       </c>
       <c r="HP2" s="10" t="s">
-        <v>2894</v>
+        <v>2893</v>
       </c>
       <c r="HQ2" s="10" t="s">
-        <v>2894</v>
+        <v>2893</v>
       </c>
       <c r="HR2" s="10" t="s">
-        <v>2894</v>
+        <v>2893</v>
       </c>
       <c r="HS2" s="10" t="s">
-        <v>2894</v>
+        <v>2893</v>
       </c>
       <c r="HT2" s="10" t="s">
-        <v>2894</v>
+        <v>2893</v>
       </c>
       <c r="HU2" s="10" t="s">
-        <v>2894</v>
+        <v>2893</v>
       </c>
       <c r="HV2" s="10" t="s">
-        <v>2894</v>
+        <v>2893</v>
       </c>
       <c r="HW2" s="10" t="s">
-        <v>2894</v>
+        <v>2893</v>
       </c>
       <c r="HX2" s="10" t="s">
-        <v>2894</v>
+        <v>2893</v>
       </c>
       <c r="HY2" s="10" t="s">
-        <v>2894</v>
+        <v>2893</v>
       </c>
       <c r="HZ2" s="10" t="s">
-        <v>2894</v>
+        <v>2893</v>
       </c>
       <c r="IA2" s="10" t="s">
-        <v>2894</v>
+        <v>2893</v>
       </c>
       <c r="IB2" s="10" t="s">
-        <v>2894</v>
+        <v>2893</v>
       </c>
       <c r="IC2" s="10" t="s">
-        <v>2894</v>
+        <v>2893</v>
       </c>
     </row>
     <row r="3" spans="1:237" x14ac:dyDescent="0.3">
@@ -16778,7 +16781,7 @@
         <v>20</v>
       </c>
       <c r="AK3" s="93" t="s">
-        <v>3036</v>
+        <v>3035</v>
       </c>
       <c r="AL3" s="7" t="s">
         <v>20</v>
@@ -16841,7 +16844,7 @@
         <v>20</v>
       </c>
       <c r="BF3" s="70" t="s">
-        <v>2779</v>
+        <v>2778</v>
       </c>
       <c r="BG3" s="16" t="s">
         <v>2699</v>
@@ -16965,10 +16968,10 @@
       </c>
       <c r="CU3" s="12"/>
       <c r="CV3" s="34" t="s">
-        <v>2891</v>
+        <v>2890</v>
       </c>
       <c r="CX3" s="40" t="s">
-        <v>2888</v>
+        <v>2887</v>
       </c>
       <c r="CY3" s="12" t="s">
         <v>2415</v>
@@ -17070,113 +17073,113 @@
         <v>2025</v>
       </c>
       <c r="EM3" s="10" t="s">
-        <v>2970</v>
+        <v>2969</v>
       </c>
       <c r="EN3" s="10"/>
       <c r="EO3" s="90" t="s">
-        <v>2888</v>
+        <v>2887</v>
       </c>
       <c r="EQ3" t="s">
-        <v>2793</v>
+        <v>2792</v>
       </c>
       <c r="ER3" t="s">
+        <v>2823</v>
+      </c>
+      <c r="ES3" t="s">
+        <v>2823</v>
+      </c>
+      <c r="ET3" s="77" t="s">
+        <v>2823</v>
+      </c>
+      <c r="EU3" t="s">
         <v>2824</v>
       </c>
-      <c r="ES3" t="s">
+      <c r="EV3" s="77" t="s">
         <v>2824</v>
       </c>
-      <c r="ET3" s="77" t="s">
+      <c r="EW3" s="77" t="s">
         <v>2824</v>
       </c>
-      <c r="EU3" t="s">
-        <v>2825</v>
-      </c>
-      <c r="EV3" s="77" t="s">
-        <v>2825</v>
-      </c>
-      <c r="EW3" s="77" t="s">
-        <v>2825</v>
-      </c>
       <c r="EX3" s="77" t="s">
-        <v>2825</v>
+        <v>2824</v>
       </c>
       <c r="EY3" s="77" t="s">
-        <v>2825</v>
+        <v>2824</v>
       </c>
       <c r="EZ3" s="77" t="s">
-        <v>2825</v>
+        <v>2824</v>
       </c>
       <c r="FA3" s="77" t="s">
-        <v>2825</v>
+        <v>2824</v>
       </c>
       <c r="FB3" s="77" t="s">
-        <v>2825</v>
+        <v>2824</v>
       </c>
       <c r="FC3" s="77" t="s">
-        <v>2825</v>
+        <v>2824</v>
       </c>
       <c r="FD3" s="77" t="s">
-        <v>2860</v>
+        <v>2859</v>
       </c>
       <c r="FF3" t="s">
-        <v>2833</v>
+        <v>2832</v>
       </c>
       <c r="FG3" s="89" t="s">
-        <v>2793</v>
+        <v>2792</v>
       </c>
       <c r="FH3" t="s">
-        <v>2827</v>
+        <v>2826</v>
       </c>
       <c r="FI3" t="s">
-        <v>2855</v>
+        <v>2854</v>
       </c>
       <c r="FJ3" t="s">
+        <v>2836</v>
+      </c>
+      <c r="FM3" t="s">
+        <v>2792</v>
+      </c>
+      <c r="FN3" t="s">
         <v>2837</v>
       </c>
-      <c r="FM3" t="s">
-        <v>2793</v>
-      </c>
-      <c r="FN3" t="s">
+      <c r="FO3" s="77" t="s">
+        <v>2837</v>
+      </c>
+      <c r="FS3" t="s">
+        <v>2851</v>
+      </c>
+      <c r="FZ3" t="s">
+        <v>2839</v>
+      </c>
+      <c r="GA3" s="77" t="s">
+        <v>2839</v>
+      </c>
+      <c r="GB3" s="77" t="s">
+        <v>2816</v>
+      </c>
+      <c r="GC3" s="77" t="s">
+        <v>2817</v>
+      </c>
+      <c r="GD3" s="77" t="s">
+        <v>2817</v>
+      </c>
+      <c r="GE3" t="s">
         <v>2838</v>
       </c>
-      <c r="FO3" s="77" t="s">
-        <v>2838</v>
-      </c>
-      <c r="FS3" t="s">
-        <v>2852</v>
-      </c>
-      <c r="FZ3" t="s">
-        <v>2840</v>
-      </c>
-      <c r="GA3" s="77" t="s">
-        <v>2840</v>
-      </c>
-      <c r="GB3" s="77" t="s">
-        <v>2817</v>
-      </c>
-      <c r="GC3" s="77" t="s">
-        <v>2818</v>
-      </c>
-      <c r="GD3" s="77" t="s">
-        <v>2818</v>
-      </c>
-      <c r="GE3" t="s">
-        <v>2839</v>
-      </c>
       <c r="GF3" t="s">
-        <v>2815</v>
+        <v>2814</v>
       </c>
       <c r="GG3" s="77" t="s">
-        <v>2815</v>
+        <v>2814</v>
       </c>
       <c r="GH3" s="77" t="s">
-        <v>2815</v>
+        <v>2814</v>
       </c>
       <c r="GI3" t="s">
-        <v>2833</v>
+        <v>2832</v>
       </c>
       <c r="GJ3" s="77" t="s">
-        <v>2833</v>
+        <v>2832</v>
       </c>
       <c r="GK3" s="10" t="s">
         <v>2025</v>
@@ -17194,76 +17197,76 @@
         <v>5</v>
       </c>
       <c r="HF3" s="10" t="s">
-        <v>2895</v>
+        <v>2894</v>
       </c>
       <c r="HG3" s="10" t="s">
-        <v>2895</v>
+        <v>2894</v>
       </c>
       <c r="HH3" s="10" t="s">
-        <v>2895</v>
+        <v>2894</v>
       </c>
       <c r="HI3" s="10" t="s">
-        <v>2895</v>
+        <v>2894</v>
       </c>
       <c r="HJ3" s="10" t="s">
-        <v>2927</v>
+        <v>2926</v>
       </c>
       <c r="HK3" s="10" t="s">
-        <v>2923</v>
+        <v>2922</v>
       </c>
       <c r="HL3" s="10" t="s">
-        <v>2923</v>
+        <v>2922</v>
       </c>
       <c r="HM3" s="10" t="s">
-        <v>2895</v>
+        <v>2894</v>
       </c>
       <c r="HN3" s="10" t="s">
-        <v>2895</v>
+        <v>2894</v>
       </c>
       <c r="HO3" s="10" t="s">
-        <v>2895</v>
+        <v>2894</v>
       </c>
       <c r="HP3" s="10" t="s">
-        <v>2895</v>
+        <v>2894</v>
       </c>
       <c r="HQ3" s="10" t="s">
-        <v>2895</v>
+        <v>2894</v>
       </c>
       <c r="HR3" s="10" t="s">
-        <v>2895</v>
+        <v>2894</v>
       </c>
       <c r="HS3" s="10" t="s">
-        <v>2895</v>
+        <v>2894</v>
       </c>
       <c r="HT3" s="10" t="s">
-        <v>2895</v>
+        <v>2894</v>
       </c>
       <c r="HU3" s="10" t="s">
-        <v>2895</v>
+        <v>2894</v>
       </c>
       <c r="HV3" s="10" t="s">
-        <v>2895</v>
+        <v>2894</v>
       </c>
       <c r="HW3" s="10" t="s">
-        <v>2895</v>
+        <v>2894</v>
       </c>
       <c r="HX3" s="10" t="s">
-        <v>2895</v>
+        <v>2894</v>
       </c>
       <c r="HY3" s="10" t="s">
-        <v>2895</v>
+        <v>2894</v>
       </c>
       <c r="HZ3" s="10" t="s">
-        <v>2895</v>
+        <v>2894</v>
       </c>
       <c r="IA3" s="10" t="s">
-        <v>2895</v>
+        <v>2894</v>
       </c>
       <c r="IB3" s="10" t="s">
-        <v>2895</v>
+        <v>2894</v>
       </c>
       <c r="IC3" s="10" t="s">
-        <v>2895</v>
+        <v>2894</v>
       </c>
     </row>
     <row r="4" spans="1:237" x14ac:dyDescent="0.3">
@@ -17373,7 +17376,7 @@
         <v>1709</v>
       </c>
       <c r="AK4" s="93" t="s">
-        <v>3037</v>
+        <v>3036</v>
       </c>
       <c r="AL4" t="s">
         <v>1468</v>
@@ -17475,7 +17478,7 @@
         <v>3</v>
       </c>
       <c r="BT4" s="14" t="s">
-        <v>2871</v>
+        <v>2870</v>
       </c>
       <c r="BU4" s="10" t="s">
         <v>1841</v>
@@ -17553,7 +17556,7 @@
       </c>
       <c r="CU4" s="12"/>
       <c r="CV4" s="34" t="s">
-        <v>2892</v>
+        <v>2891</v>
       </c>
       <c r="CX4" s="40" t="s">
         <v>2450</v>
@@ -17584,13 +17587,13 @@
         <v>2376</v>
       </c>
       <c r="DH4" s="12" t="s">
+        <v>2872</v>
+      </c>
+      <c r="DI4" s="44" t="s">
         <v>2873</v>
       </c>
-      <c r="DI4" s="44" t="s">
+      <c r="DJ4" s="12" t="s">
         <v>2874</v>
-      </c>
-      <c r="DJ4" s="12" t="s">
-        <v>2875</v>
       </c>
       <c r="DK4" s="12" t="s">
         <v>2480</v>
@@ -17611,7 +17614,7 @@
         <v>2754</v>
       </c>
       <c r="DW4" t="s">
-        <v>2877</v>
+        <v>2876</v>
       </c>
       <c r="DX4" t="s">
         <v>2762</v>
@@ -17647,94 +17650,94 @@
         <v>2033</v>
       </c>
       <c r="EM4" s="90" t="s">
-        <v>2977</v>
+        <v>2976</v>
       </c>
       <c r="EN4" s="90" t="s">
         <v>2253</v>
       </c>
       <c r="EQ4" t="s">
-        <v>2857</v>
+        <v>2856</v>
       </c>
       <c r="ER4" t="s">
+        <v>2852</v>
+      </c>
+      <c r="ES4" s="77" t="s">
+        <v>2852</v>
+      </c>
+      <c r="EU4" s="89" t="s">
+        <v>2917</v>
+      </c>
+      <c r="EV4" s="89" t="s">
+        <v>2917</v>
+      </c>
+      <c r="EW4" s="89" t="s">
+        <v>2917</v>
+      </c>
+      <c r="EX4" s="89" t="s">
+        <v>2917</v>
+      </c>
+      <c r="EY4" s="89" t="s">
+        <v>2917</v>
+      </c>
+      <c r="EZ4" s="89" t="s">
+        <v>2917</v>
+      </c>
+      <c r="FA4" s="89" t="s">
+        <v>2917</v>
+      </c>
+      <c r="FB4" s="89" t="s">
+        <v>2917</v>
+      </c>
+      <c r="FC4" s="89" t="s">
+        <v>2917</v>
+      </c>
+      <c r="FD4" t="s">
+        <v>2858</v>
+      </c>
+      <c r="FF4" s="77" t="s">
+        <v>2833</v>
+      </c>
+      <c r="FH4" s="77" t="s">
+        <v>2829</v>
+      </c>
+      <c r="FJ4" t="s">
         <v>2853</v>
       </c>
-      <c r="ES4" s="77" t="s">
-        <v>2853</v>
-      </c>
-      <c r="EU4" s="89" t="s">
-        <v>2918</v>
-      </c>
-      <c r="EV4" s="89" t="s">
-        <v>2918</v>
-      </c>
-      <c r="EW4" s="89" t="s">
-        <v>2918</v>
-      </c>
-      <c r="EX4" s="89" t="s">
-        <v>2918</v>
-      </c>
-      <c r="EY4" s="89" t="s">
-        <v>2918</v>
-      </c>
-      <c r="EZ4" s="89" t="s">
-        <v>2918</v>
-      </c>
-      <c r="FA4" s="89" t="s">
-        <v>2918</v>
-      </c>
-      <c r="FB4" s="89" t="s">
-        <v>2918</v>
-      </c>
-      <c r="FC4" s="89" t="s">
-        <v>2918</v>
-      </c>
-      <c r="FD4" t="s">
-        <v>2859</v>
-      </c>
-      <c r="FF4" s="77" t="s">
+      <c r="FN4" t="s">
+        <v>2850</v>
+      </c>
+      <c r="FO4" s="77" t="s">
+        <v>2850</v>
+      </c>
+      <c r="FS4" t="s">
+        <v>2792</v>
+      </c>
+      <c r="FZ4" t="s">
+        <v>2815</v>
+      </c>
+      <c r="GA4" s="77" t="s">
+        <v>2815</v>
+      </c>
+      <c r="GC4" s="77" t="s">
+        <v>2818</v>
+      </c>
+      <c r="GD4" s="77" t="s">
+        <v>2821</v>
+      </c>
+      <c r="GF4" s="77" t="s">
+        <v>2840</v>
+      </c>
+      <c r="GG4" s="77" t="s">
+        <v>2841</v>
+      </c>
+      <c r="GH4" s="77" t="s">
+        <v>2840</v>
+      </c>
+      <c r="GI4" t="s">
         <v>2834</v>
       </c>
-      <c r="FH4" s="77" t="s">
-        <v>2830</v>
-      </c>
-      <c r="FJ4" t="s">
-        <v>2854</v>
-      </c>
-      <c r="FN4" t="s">
-        <v>2851</v>
-      </c>
-      <c r="FO4" s="77" t="s">
-        <v>2851</v>
-      </c>
-      <c r="FS4" t="s">
-        <v>2793</v>
-      </c>
-      <c r="FZ4" t="s">
-        <v>2816</v>
-      </c>
-      <c r="GA4" s="77" t="s">
-        <v>2816</v>
-      </c>
-      <c r="GC4" s="77" t="s">
-        <v>2819</v>
-      </c>
-      <c r="GD4" s="77" t="s">
-        <v>2822</v>
-      </c>
-      <c r="GF4" s="77" t="s">
-        <v>2841</v>
-      </c>
-      <c r="GG4" s="77" t="s">
-        <v>2842</v>
-      </c>
-      <c r="GH4" s="77" t="s">
-        <v>2841</v>
-      </c>
-      <c r="GI4" t="s">
-        <v>2835</v>
-      </c>
       <c r="GJ4" s="77" t="s">
-        <v>2835</v>
+        <v>2834</v>
       </c>
       <c r="GK4" s="77" t="s">
         <v>2033</v>
@@ -17743,76 +17746,76 @@
         <v>2033</v>
       </c>
       <c r="HF4" t="s">
-        <v>2896</v>
+        <v>2895</v>
       </c>
       <c r="HG4" s="88" t="s">
-        <v>2896</v>
+        <v>2895</v>
       </c>
       <c r="HH4" s="88" t="s">
-        <v>2896</v>
+        <v>2895</v>
       </c>
       <c r="HI4" s="88" t="s">
-        <v>2896</v>
+        <v>2895</v>
       </c>
       <c r="HJ4" s="10" t="s">
-        <v>2919</v>
+        <v>2918</v>
       </c>
       <c r="HK4" t="s">
-        <v>2924</v>
+        <v>2923</v>
       </c>
       <c r="HL4" s="90" t="s">
-        <v>2924</v>
+        <v>2923</v>
       </c>
       <c r="HM4" s="90" t="s">
-        <v>2896</v>
+        <v>2895</v>
       </c>
       <c r="HN4" s="90" t="s">
-        <v>2896</v>
+        <v>2895</v>
       </c>
       <c r="HO4" s="90" t="s">
-        <v>2896</v>
+        <v>2895</v>
       </c>
       <c r="HP4" s="90" t="s">
-        <v>2896</v>
+        <v>2895</v>
       </c>
       <c r="HQ4" s="90" t="s">
-        <v>2896</v>
+        <v>2895</v>
       </c>
       <c r="HR4" s="90" t="s">
-        <v>2896</v>
+        <v>2895</v>
       </c>
       <c r="HS4" s="90" t="s">
-        <v>2896</v>
+        <v>2895</v>
       </c>
       <c r="HT4" s="90" t="s">
-        <v>2896</v>
+        <v>2895</v>
       </c>
       <c r="HU4" s="90" t="s">
-        <v>2896</v>
+        <v>2895</v>
       </c>
       <c r="HV4" s="90" t="s">
-        <v>2896</v>
+        <v>2895</v>
       </c>
       <c r="HW4" s="90" t="s">
-        <v>2896</v>
+        <v>2895</v>
       </c>
       <c r="HX4" s="90" t="s">
-        <v>2896</v>
+        <v>2895</v>
       </c>
       <c r="HY4" s="90" t="s">
-        <v>2896</v>
+        <v>2895</v>
       </c>
       <c r="HZ4" s="90" t="s">
-        <v>2896</v>
+        <v>2895</v>
       </c>
       <c r="IA4" s="90" t="s">
-        <v>2896</v>
+        <v>2895</v>
       </c>
       <c r="IB4" s="90" t="s">
-        <v>2896</v>
+        <v>2895</v>
       </c>
       <c r="IC4" s="90" t="s">
-        <v>2896</v>
+        <v>2895</v>
       </c>
     </row>
     <row r="5" spans="1:237" x14ac:dyDescent="0.3">
@@ -18000,7 +18003,7 @@
         <v>4</v>
       </c>
       <c r="BT5" s="14" t="s">
-        <v>2889</v>
+        <v>2888</v>
       </c>
       <c r="BU5" s="13" t="s">
         <v>1842</v>
@@ -18076,7 +18079,7 @@
         <v>2253</v>
       </c>
       <c r="CV5" t="s">
-        <v>2893</v>
+        <v>2892</v>
       </c>
       <c r="CX5" s="40" t="s">
         <v>2449</v>
@@ -18158,67 +18161,67 @@
         <v>2034</v>
       </c>
       <c r="EM5" s="90" t="s">
-        <v>2978</v>
+        <v>2977</v>
       </c>
       <c r="EN5" s="90" t="s">
         <v>2253</v>
       </c>
       <c r="EQ5" t="s">
-        <v>2856</v>
+        <v>2855</v>
       </c>
       <c r="ES5" t="s">
-        <v>2865</v>
+        <v>2864</v>
       </c>
       <c r="EU5" t="s">
-        <v>2826</v>
+        <v>2825</v>
       </c>
       <c r="EV5" s="77" t="s">
-        <v>2826</v>
+        <v>2825</v>
       </c>
       <c r="EW5" s="77" t="s">
-        <v>2826</v>
+        <v>2825</v>
       </c>
       <c r="EX5" s="77" t="s">
-        <v>2826</v>
+        <v>2825</v>
       </c>
       <c r="EY5" s="77" t="s">
-        <v>2826</v>
+        <v>2825</v>
       </c>
       <c r="EZ5" s="77" t="s">
-        <v>2826</v>
+        <v>2825</v>
       </c>
       <c r="FA5" s="77" t="s">
-        <v>2826</v>
+        <v>2825</v>
       </c>
       <c r="FB5" s="77" t="s">
-        <v>2826</v>
+        <v>2825</v>
       </c>
       <c r="FC5" s="77" t="s">
-        <v>2826</v>
+        <v>2825</v>
       </c>
       <c r="FD5" s="77" t="s">
-        <v>2861</v>
+        <v>2860</v>
       </c>
       <c r="FF5" s="77" t="s">
-        <v>2835</v>
+        <v>2834</v>
       </c>
       <c r="FH5" s="77" t="s">
-        <v>2828</v>
+        <v>2827</v>
       </c>
       <c r="GC5" s="77" t="s">
-        <v>2820</v>
+        <v>2819</v>
       </c>
       <c r="GD5" s="77" t="s">
-        <v>2823</v>
+        <v>2822</v>
       </c>
       <c r="GH5" t="s">
-        <v>2850</v>
+        <v>2849</v>
       </c>
       <c r="GI5" t="s">
-        <v>2834</v>
+        <v>2833</v>
       </c>
       <c r="GJ5" s="77" t="s">
-        <v>2834</v>
+        <v>2833</v>
       </c>
       <c r="GK5" s="77" t="s">
         <v>2034</v>
@@ -18227,76 +18230,76 @@
         <v>2034</v>
       </c>
       <c r="HF5" t="s">
-        <v>2897</v>
+        <v>2896</v>
       </c>
       <c r="HG5" s="88" t="s">
-        <v>2897</v>
+        <v>2896</v>
       </c>
       <c r="HH5" s="88" t="s">
-        <v>2897</v>
+        <v>2896</v>
       </c>
       <c r="HI5" s="88" t="s">
-        <v>2897</v>
+        <v>2896</v>
       </c>
       <c r="HJ5" s="10" t="s">
-        <v>2921</v>
+        <v>2920</v>
       </c>
       <c r="HK5" t="s">
-        <v>2925</v>
+        <v>2924</v>
       </c>
       <c r="HL5" s="90" t="s">
-        <v>2925</v>
+        <v>2924</v>
       </c>
       <c r="HM5" s="90" t="s">
-        <v>2897</v>
+        <v>2896</v>
       </c>
       <c r="HN5" s="90" t="s">
-        <v>2897</v>
+        <v>2896</v>
       </c>
       <c r="HO5" s="90" t="s">
-        <v>2897</v>
+        <v>2896</v>
       </c>
       <c r="HP5" s="90" t="s">
-        <v>2897</v>
+        <v>2896</v>
       </c>
       <c r="HQ5" s="90" t="s">
-        <v>2897</v>
+        <v>2896</v>
       </c>
       <c r="HR5" s="90" t="s">
-        <v>2897</v>
+        <v>2896</v>
       </c>
       <c r="HS5" s="90" t="s">
-        <v>2897</v>
+        <v>2896</v>
       </c>
       <c r="HT5" s="90" t="s">
-        <v>2897</v>
+        <v>2896</v>
       </c>
       <c r="HU5" s="90" t="s">
-        <v>2897</v>
+        <v>2896</v>
       </c>
       <c r="HV5" s="90" t="s">
-        <v>2897</v>
+        <v>2896</v>
       </c>
       <c r="HW5" s="90" t="s">
-        <v>2897</v>
+        <v>2896</v>
       </c>
       <c r="HX5" s="90" t="s">
-        <v>2897</v>
+        <v>2896</v>
       </c>
       <c r="HY5" s="90" t="s">
-        <v>2897</v>
+        <v>2896</v>
       </c>
       <c r="HZ5" s="90" t="s">
-        <v>2897</v>
+        <v>2896</v>
       </c>
       <c r="IA5" s="90" t="s">
-        <v>2897</v>
+        <v>2896</v>
       </c>
       <c r="IB5" s="90" t="s">
-        <v>2897</v>
+        <v>2896</v>
       </c>
       <c r="IC5" s="90" t="s">
-        <v>2897</v>
+        <v>2896</v>
       </c>
     </row>
     <row r="6" spans="1:237" x14ac:dyDescent="0.3">
@@ -18325,7 +18328,7 @@
         <v>59</v>
       </c>
       <c r="J6" t="s">
-        <v>3034</v>
+        <v>3033</v>
       </c>
       <c r="K6" s="32" t="s">
         <v>2067</v>
@@ -18619,37 +18622,37 @@
         <v>2035</v>
       </c>
       <c r="EM6" s="90" t="s">
-        <v>2979</v>
+        <v>2978</v>
       </c>
       <c r="EN6" s="90" t="s">
         <v>2253</v>
       </c>
       <c r="EQ6" t="s">
-        <v>2854</v>
+        <v>2853</v>
       </c>
       <c r="ES6" t="s">
-        <v>2866</v>
+        <v>2865</v>
       </c>
       <c r="FD6" s="77" t="s">
-        <v>2862</v>
+        <v>2861</v>
       </c>
       <c r="FF6" t="s">
         <v>2026</v>
       </c>
       <c r="FH6" s="77" t="s">
-        <v>2831</v>
+        <v>2830</v>
       </c>
       <c r="GC6" t="s">
-        <v>2881</v>
+        <v>2880</v>
       </c>
       <c r="GD6" t="s">
-        <v>2821</v>
+        <v>2820</v>
       </c>
       <c r="GI6" t="s">
-        <v>2843</v>
+        <v>2842</v>
       </c>
       <c r="GJ6" s="77" t="s">
-        <v>2843</v>
+        <v>2842</v>
       </c>
       <c r="GK6" s="77" t="s">
         <v>2035</v>
@@ -18658,76 +18661,76 @@
         <v>2035</v>
       </c>
       <c r="HF6" t="s">
-        <v>2898</v>
+        <v>2897</v>
       </c>
       <c r="HG6" s="88" t="s">
-        <v>2898</v>
+        <v>2897</v>
       </c>
       <c r="HH6" s="88" t="s">
-        <v>2898</v>
+        <v>2897</v>
       </c>
       <c r="HI6" s="88" t="s">
-        <v>2898</v>
+        <v>2897</v>
       </c>
       <c r="HJ6" t="s">
-        <v>2920</v>
+        <v>2919</v>
       </c>
       <c r="HK6" t="s">
-        <v>2926</v>
+        <v>2925</v>
       </c>
       <c r="HL6" s="90" t="s">
-        <v>2926</v>
+        <v>2925</v>
       </c>
       <c r="HM6" s="90" t="s">
-        <v>2898</v>
+        <v>2897</v>
       </c>
       <c r="HN6" s="90" t="s">
-        <v>2898</v>
+        <v>2897</v>
       </c>
       <c r="HO6" s="90" t="s">
-        <v>2898</v>
+        <v>2897</v>
       </c>
       <c r="HP6" s="90" t="s">
-        <v>2898</v>
+        <v>2897</v>
       </c>
       <c r="HQ6" s="90" t="s">
-        <v>2898</v>
+        <v>2897</v>
       </c>
       <c r="HR6" s="90" t="s">
-        <v>2898</v>
+        <v>2897</v>
       </c>
       <c r="HS6" s="90" t="s">
-        <v>2898</v>
+        <v>2897</v>
       </c>
       <c r="HT6" s="90" t="s">
-        <v>2898</v>
+        <v>2897</v>
       </c>
       <c r="HU6" s="90" t="s">
-        <v>2898</v>
+        <v>2897</v>
       </c>
       <c r="HV6" s="90" t="s">
-        <v>2898</v>
+        <v>2897</v>
       </c>
       <c r="HW6" s="90" t="s">
-        <v>2898</v>
+        <v>2897</v>
       </c>
       <c r="HX6" s="90" t="s">
-        <v>2898</v>
+        <v>2897</v>
       </c>
       <c r="HY6" s="90" t="s">
-        <v>2898</v>
+        <v>2897</v>
       </c>
       <c r="HZ6" s="90" t="s">
-        <v>2898</v>
+        <v>2897</v>
       </c>
       <c r="IA6" s="90" t="s">
-        <v>2898</v>
+        <v>2897</v>
       </c>
       <c r="IB6" s="90" t="s">
-        <v>2898</v>
+        <v>2897</v>
       </c>
       <c r="IC6" s="90" t="s">
-        <v>2898</v>
+        <v>2897</v>
       </c>
     </row>
     <row r="7" spans="1:237" x14ac:dyDescent="0.3">
@@ -18899,7 +18902,7 @@
         <v>6</v>
       </c>
       <c r="BT7" s="14" t="s">
-        <v>2883</v>
+        <v>2882</v>
       </c>
       <c r="BU7" s="10" t="s">
         <v>1844</v>
@@ -18992,13 +18995,13 @@
         <v>2370</v>
       </c>
       <c r="DB7" s="12" t="s">
-        <v>2914</v>
+        <v>2913</v>
       </c>
       <c r="DC7" s="12" t="s">
         <v>2200</v>
       </c>
       <c r="DD7" s="12" t="s">
-        <v>2917</v>
+        <v>2916</v>
       </c>
       <c r="DE7" s="12" t="s">
         <v>2399</v>
@@ -19025,7 +19028,7 @@
         <v>2530</v>
       </c>
       <c r="DM7" s="20" t="s">
-        <v>2798</v>
+        <v>2797</v>
       </c>
       <c r="EC7" s="77"/>
       <c r="ED7" s="77"/>
@@ -19046,28 +19049,28 @@
         <v>2027</v>
       </c>
       <c r="EM7" s="90" t="s">
-        <v>2980</v>
+        <v>2979</v>
       </c>
       <c r="EN7" s="90" t="s">
         <v>2253</v>
       </c>
       <c r="EQ7" t="s">
-        <v>2867</v>
+        <v>2866</v>
       </c>
       <c r="FD7" s="77" t="s">
-        <v>2863</v>
+        <v>2862</v>
       </c>
       <c r="FF7" t="s">
         <v>2027</v>
       </c>
       <c r="FH7" s="77" t="s">
-        <v>2829</v>
+        <v>2828</v>
       </c>
       <c r="GI7" s="77" t="s">
-        <v>2844</v>
+        <v>2843</v>
       </c>
       <c r="GJ7" s="77" t="s">
-        <v>2844</v>
+        <v>2843</v>
       </c>
       <c r="GK7" s="77" t="s">
         <v>2027</v>
@@ -19091,10 +19094,10 @@
         <v>5</v>
       </c>
       <c r="HK7" s="90" t="s">
-        <v>2944</v>
+        <v>2943</v>
       </c>
       <c r="HL7" s="90" t="s">
-        <v>2944</v>
+        <v>2943</v>
       </c>
       <c r="HM7" s="90" t="s">
         <v>5</v>
@@ -19394,13 +19397,13 @@
         <v>2371</v>
       </c>
       <c r="DB8" s="12" t="s">
-        <v>2915</v>
+        <v>2914</v>
       </c>
       <c r="DC8" s="12" t="s">
         <v>2200</v>
       </c>
       <c r="DD8" s="12" t="s">
-        <v>2916</v>
+        <v>2915</v>
       </c>
       <c r="DE8" s="12" t="s">
         <v>2400</v>
@@ -19421,7 +19424,7 @@
         <v>2530</v>
       </c>
       <c r="DM8" s="20" t="s">
-        <v>2799</v>
+        <v>2798</v>
       </c>
       <c r="EF8" s="10" t="s">
         <v>2035</v>
@@ -19439,25 +19442,25 @@
         <v>2036</v>
       </c>
       <c r="EM8" s="90" t="s">
-        <v>2981</v>
+        <v>2980</v>
       </c>
       <c r="EN8" s="90" t="s">
         <v>2253</v>
       </c>
       <c r="FD8" s="77" t="s">
-        <v>2864</v>
+        <v>2863</v>
       </c>
       <c r="FF8" s="81" t="s">
-        <v>2868</v>
+        <v>2867</v>
       </c>
       <c r="FH8" s="77" t="s">
-        <v>2832</v>
+        <v>2831</v>
       </c>
       <c r="GI8" s="77" t="s">
-        <v>2845</v>
+        <v>2844</v>
       </c>
       <c r="GJ8" s="77" t="s">
-        <v>2845</v>
+        <v>2844</v>
       </c>
       <c r="GK8" s="77" t="s">
         <v>2036</v>
@@ -19657,7 +19660,7 @@
         <v>2238</v>
       </c>
       <c r="CL9" s="40" t="s">
-        <v>2806</v>
+        <v>2805</v>
       </c>
       <c r="CM9" s="12" t="s">
         <v>1799</v>
@@ -19696,7 +19699,7 @@
         <v>2372</v>
       </c>
       <c r="DB9" s="12" t="s">
-        <v>2902</v>
+        <v>2901</v>
       </c>
       <c r="DC9" s="88" t="s">
         <v>2253</v>
@@ -19721,16 +19724,16 @@
         <v>2530</v>
       </c>
       <c r="DM9" s="20" t="s">
-        <v>2800</v>
+        <v>2799</v>
       </c>
       <c r="EF9" s="10" t="s">
         <v>2033</v>
       </c>
       <c r="EG9" s="10" t="s">
-        <v>2797</v>
+        <v>2796</v>
       </c>
       <c r="EH9" s="10" t="s">
-        <v>2796</v>
+        <v>2795</v>
       </c>
       <c r="EI9" s="77"/>
       <c r="EJ9" s="77"/>
@@ -19739,22 +19742,22 @@
         <v>2026</v>
       </c>
       <c r="EM9" s="90" t="s">
-        <v>2982</v>
+        <v>2981</v>
       </c>
       <c r="EN9" s="90" t="s">
         <v>2253</v>
       </c>
       <c r="FD9" t="s">
-        <v>2858</v>
+        <v>2857</v>
       </c>
       <c r="FF9" t="s">
-        <v>2836</v>
+        <v>2835</v>
       </c>
       <c r="GI9" t="s">
-        <v>2846</v>
+        <v>2845</v>
       </c>
       <c r="GJ9" s="77" t="s">
-        <v>2846</v>
+        <v>2845</v>
       </c>
       <c r="GK9" s="77" t="s">
         <v>2026</v>
@@ -19890,10 +19893,10 @@
         <v>2690</v>
       </c>
       <c r="BQ10" s="14" t="s">
-        <v>2890</v>
+        <v>2889</v>
       </c>
       <c r="BR10" s="20" t="s">
-        <v>2899</v>
+        <v>2898</v>
       </c>
       <c r="BS10" s="20">
         <v>9</v>
@@ -19971,7 +19974,7 @@
       <c r="CY10" s="12"/>
       <c r="DA10" s="12"/>
       <c r="DB10" s="12" t="s">
-        <v>2935</v>
+        <v>2934</v>
       </c>
       <c r="DC10" s="90" t="s">
         <v>2253</v>
@@ -19996,7 +19999,7 @@
         <v>2530</v>
       </c>
       <c r="DM10" s="20" t="s">
-        <v>2801</v>
+        <v>2800</v>
       </c>
       <c r="EF10" s="10" t="s">
         <v>2028</v>
@@ -20010,7 +20013,7 @@
         <v>2159</v>
       </c>
       <c r="EM10" s="90" t="s">
-        <v>2983</v>
+        <v>2982</v>
       </c>
       <c r="EN10" s="90" t="s">
         <v>2253</v>
@@ -20234,7 +20237,7 @@
         <v>2354</v>
       </c>
       <c r="DB11" s="20" t="s">
-        <v>2903</v>
+        <v>2902</v>
       </c>
       <c r="DC11" s="90" t="s">
         <v>2253</v>
@@ -20259,7 +20262,7 @@
         <v>2530</v>
       </c>
       <c r="DM11" s="20" t="s">
-        <v>2802</v>
+        <v>2801</v>
       </c>
       <c r="EF11" s="10" t="s">
         <v>2178</v>
@@ -20270,16 +20273,16 @@
         <v>2037</v>
       </c>
       <c r="EM11" s="90" t="s">
-        <v>2984</v>
+        <v>2983</v>
       </c>
       <c r="EN11" s="90" t="s">
         <v>2253</v>
       </c>
       <c r="GI11" t="s">
-        <v>2847</v>
+        <v>2846</v>
       </c>
       <c r="GJ11" s="77" t="s">
-        <v>2847</v>
+        <v>2846</v>
       </c>
       <c r="GK11" s="77" t="s">
         <v>2037</v>
@@ -20413,7 +20416,7 @@
         <v>2373</v>
       </c>
       <c r="BR12" s="20" t="s">
-        <v>2969</v>
+        <v>2968</v>
       </c>
       <c r="BS12" s="20">
         <v>11</v>
@@ -20476,14 +20479,14 @@
         <v>2275</v>
       </c>
       <c r="CV12" s="90" t="s">
-        <v>2945</v>
+        <v>2944</v>
       </c>
       <c r="CW12" s="90" t="s">
         <v>2253</v>
       </c>
       <c r="CX12" s="88"/>
       <c r="DB12" s="20" t="s">
-        <v>2936</v>
+        <v>2935</v>
       </c>
       <c r="DC12" s="90" t="s">
         <v>2253</v>
@@ -20508,7 +20511,7 @@
         <v>2530</v>
       </c>
       <c r="DM12" s="20" t="s">
-        <v>2803</v>
+        <v>2802</v>
       </c>
       <c r="EF12" s="10" t="s">
         <v>2740</v>
@@ -20519,7 +20522,7 @@
         <v>2038</v>
       </c>
       <c r="EM12" s="90" t="s">
-        <v>2985</v>
+        <v>2984</v>
       </c>
       <c r="EN12" s="90" t="s">
         <v>2253</v>
@@ -20557,7 +20560,7 @@
         <v>127</v>
       </c>
       <c r="J13" t="s">
-        <v>2795</v>
+        <v>2794</v>
       </c>
       <c r="K13" s="32" t="s">
         <v>2073</v>
@@ -20576,7 +20579,7 @@
       </c>
       <c r="U13" s="6"/>
       <c r="V13" s="75" t="s">
-        <v>2794</v>
+        <v>2793</v>
       </c>
       <c r="AB13" s="6" t="s">
         <v>1387</v>
@@ -20710,14 +20713,14 @@
         <v>2574</v>
       </c>
       <c r="CV13" s="90" t="s">
-        <v>2956</v>
+        <v>2955</v>
       </c>
       <c r="CW13" s="90" t="s">
         <v>2253</v>
       </c>
       <c r="CX13" s="88"/>
       <c r="DB13" s="12" t="s">
-        <v>2904</v>
+        <v>2903</v>
       </c>
       <c r="DC13" s="90" t="s">
         <v>2253</v>
@@ -20739,7 +20742,7 @@
         <v>2737</v>
       </c>
       <c r="DM13" s="20" t="s">
-        <v>2804</v>
+        <v>2803</v>
       </c>
       <c r="EF13" s="10"/>
       <c r="EG13" s="10"/>
@@ -20748,7 +20751,7 @@
         <v>2028</v>
       </c>
       <c r="EM13" s="90" t="s">
-        <v>2986</v>
+        <v>2985</v>
       </c>
       <c r="EN13" s="90" t="s">
         <v>2253</v>
@@ -20871,7 +20874,7 @@
         <v>13</v>
       </c>
       <c r="BT14" s="14" t="s">
-        <v>2780</v>
+        <v>2779</v>
       </c>
       <c r="BU14" s="20" t="s">
         <v>2775</v>
@@ -20929,14 +20932,14 @@
       </c>
       <c r="CS14" s="40"/>
       <c r="CV14" s="90" t="s">
-        <v>2946</v>
+        <v>2945</v>
       </c>
       <c r="CW14" s="90" t="s">
         <v>2253</v>
       </c>
       <c r="CX14" s="88"/>
       <c r="DB14" s="12" t="s">
-        <v>2937</v>
+        <v>2936</v>
       </c>
       <c r="DC14" s="90" t="s">
         <v>2253</v>
@@ -20958,7 +20961,7 @@
       <c r="DL14" s="41"/>
       <c r="DM14" s="41"/>
       <c r="EM14" s="90" t="s">
-        <v>2987</v>
+        <v>2986</v>
       </c>
       <c r="EN14" s="90" t="s">
         <v>2253</v>
@@ -20970,7 +20973,7 @@
         <v>2027</v>
       </c>
       <c r="GL14" t="s">
-        <v>2876</v>
+        <v>2875</v>
       </c>
     </row>
     <row r="15" spans="1:237" x14ac:dyDescent="0.3">
@@ -21061,16 +21064,16 @@
         <v>2490</v>
       </c>
       <c r="BQ15" s="14" t="s">
-        <v>2966</v>
+        <v>2965</v>
       </c>
       <c r="BR15" s="20" t="s">
-        <v>2968</v>
+        <v>2967</v>
       </c>
       <c r="BS15" s="20">
         <v>14</v>
       </c>
       <c r="BT15" s="14" t="s">
-        <v>2878</v>
+        <v>2877</v>
       </c>
       <c r="BU15" s="10" t="s">
         <v>2058</v>
@@ -21128,14 +21131,14 @@
       </c>
       <c r="CS15" s="40"/>
       <c r="CV15" s="90" t="s">
-        <v>2957</v>
+        <v>2956</v>
       </c>
       <c r="CW15" s="90" t="s">
         <v>2253</v>
       </c>
       <c r="CX15" s="88"/>
       <c r="DB15" s="20" t="s">
-        <v>2905</v>
+        <v>2904</v>
       </c>
       <c r="DC15" s="90" t="s">
         <v>2253</v>
@@ -21157,7 +21160,7 @@
       <c r="DL15" s="41"/>
       <c r="DM15" s="41"/>
       <c r="EM15" s="90" t="s">
-        <v>2988</v>
+        <v>2987</v>
       </c>
       <c r="EN15" s="90" t="s">
         <v>2253</v>
@@ -21268,7 +21271,7 @@
         <v>15</v>
       </c>
       <c r="BT16" s="14" t="s">
-        <v>2879</v>
+        <v>2878</v>
       </c>
       <c r="BU16" s="10" t="s">
         <v>2346</v>
@@ -21323,14 +21326,14 @@
       </c>
       <c r="CS16" s="40"/>
       <c r="CV16" s="90" t="s">
-        <v>2947</v>
+        <v>2946</v>
       </c>
       <c r="CW16" s="90" t="s">
         <v>2253</v>
       </c>
       <c r="CX16" s="88"/>
       <c r="DB16" s="20" t="s">
-        <v>2938</v>
+        <v>2937</v>
       </c>
       <c r="DC16" s="90" t="s">
         <v>2253</v>
@@ -21352,7 +21355,7 @@
       <c r="DL16" s="41"/>
       <c r="DM16" s="41"/>
       <c r="EM16" s="90" t="s">
-        <v>2989</v>
+        <v>2988</v>
       </c>
       <c r="EN16" s="90" t="s">
         <v>2253</v>
@@ -21459,7 +21462,7 @@
         <v>16</v>
       </c>
       <c r="BT17" s="14" t="s">
-        <v>2887</v>
+        <v>2886</v>
       </c>
       <c r="BU17" s="10" t="s">
         <v>2084</v>
@@ -21508,14 +21511,14 @@
       </c>
       <c r="CS17" s="40"/>
       <c r="CV17" s="90" t="s">
-        <v>2958</v>
+        <v>2957</v>
       </c>
       <c r="CW17" s="90" t="s">
         <v>2253</v>
       </c>
       <c r="CX17" s="88"/>
       <c r="DB17" s="12" t="s">
-        <v>2906</v>
+        <v>2905</v>
       </c>
       <c r="DC17" s="90" t="s">
         <v>2253</v>
@@ -21536,16 +21539,16 @@
       <c r="DL17" s="41"/>
       <c r="DM17" s="41"/>
       <c r="EM17" s="90" t="s">
-        <v>2990</v>
+        <v>2989</v>
       </c>
       <c r="EN17" s="90" t="s">
         <v>2253</v>
       </c>
       <c r="GI17" t="s">
+        <v>2847</v>
+      </c>
+      <c r="GJ17" s="77" t="s">
         <v>2848</v>
-      </c>
-      <c r="GJ17" s="77" t="s">
-        <v>2849</v>
       </c>
     </row>
     <row r="18" spans="2:192" x14ac:dyDescent="0.3">
@@ -21644,7 +21647,7 @@
         <v>17</v>
       </c>
       <c r="BT18" s="14" t="s">
-        <v>2781</v>
+        <v>2780</v>
       </c>
       <c r="BX18" s="11" t="s">
         <v>2340</v>
@@ -21657,13 +21660,13 @@
       <c r="CB18" s="11"/>
       <c r="CC18" s="11"/>
       <c r="CJ18" s="12" t="s">
-        <v>2808</v>
+        <v>2807</v>
       </c>
       <c r="CK18" s="76" t="s">
         <v>2238</v>
       </c>
       <c r="CL18" s="76" t="s">
-        <v>2805</v>
+        <v>2804</v>
       </c>
       <c r="CM18" s="12" t="s">
         <v>1802</v>
@@ -21682,14 +21685,14 @@
       </c>
       <c r="CS18" s="40"/>
       <c r="CV18" s="90" t="s">
-        <v>2948</v>
+        <v>2947</v>
       </c>
       <c r="CW18" s="90" t="s">
         <v>2253</v>
       </c>
       <c r="CX18" s="88"/>
       <c r="DB18" s="12" t="s">
-        <v>2939</v>
+        <v>2938</v>
       </c>
       <c r="DC18" s="90" t="s">
         <v>2253</v>
@@ -21711,7 +21714,7 @@
       <c r="DL18" s="41"/>
       <c r="DM18" s="41"/>
       <c r="EM18" s="90" t="s">
-        <v>2991</v>
+        <v>2990</v>
       </c>
       <c r="EN18" s="90" t="s">
         <v>2253</v>
@@ -21815,7 +21818,7 @@
         <v>18</v>
       </c>
       <c r="BT19" s="14" t="s">
-        <v>2782</v>
+        <v>2781</v>
       </c>
       <c r="BX19" s="11" t="s">
         <v>2342</v>
@@ -21827,13 +21830,13 @@
       <c r="CB19" s="11"/>
       <c r="CC19" s="11"/>
       <c r="CJ19" s="12" t="s">
-        <v>2809</v>
+        <v>2808</v>
       </c>
       <c r="CK19" s="76" t="s">
         <v>2238</v>
       </c>
       <c r="CL19" s="76" t="s">
-        <v>2807</v>
+        <v>2806</v>
       </c>
       <c r="CM19" s="12" t="s">
         <v>1803</v>
@@ -21852,14 +21855,14 @@
       </c>
       <c r="CS19" s="40"/>
       <c r="CV19" s="90" t="s">
-        <v>2959</v>
+        <v>2958</v>
       </c>
       <c r="CW19" s="90" t="s">
         <v>2253</v>
       </c>
       <c r="CX19" s="88"/>
       <c r="DB19" s="20" t="s">
-        <v>2907</v>
+        <v>2906</v>
       </c>
       <c r="DC19" s="90" t="s">
         <v>2253</v>
@@ -21976,7 +21979,7 @@
         <v>19</v>
       </c>
       <c r="BT20" s="14" t="s">
-        <v>2783</v>
+        <v>2782</v>
       </c>
       <c r="BX20" s="11" t="s">
         <v>2341</v>
@@ -22005,14 +22008,14 @@
       </c>
       <c r="CS20" s="40"/>
       <c r="CV20" s="90" t="s">
-        <v>2949</v>
+        <v>2948</v>
       </c>
       <c r="CW20" s="90" t="s">
         <v>2253</v>
       </c>
       <c r="CX20" s="88"/>
       <c r="DB20" s="20" t="s">
-        <v>2940</v>
+        <v>2939</v>
       </c>
       <c r="DC20" s="90" t="s">
         <v>2253</v>
@@ -22034,10 +22037,10 @@
       <c r="DL20" s="41"/>
       <c r="DM20" s="41"/>
       <c r="GI20" s="10" t="s">
-        <v>2868</v>
+        <v>2867</v>
       </c>
       <c r="GJ20" s="10" t="s">
-        <v>2868</v>
+        <v>2867</v>
       </c>
     </row>
     <row r="21" spans="2:192" ht="16.8" x14ac:dyDescent="0.3">
@@ -22121,7 +22124,7 @@
         <v>2763</v>
       </c>
       <c r="BT21" s="14" t="s">
-        <v>2784</v>
+        <v>2783</v>
       </c>
       <c r="BX21" s="11" t="s">
         <v>2345</v>
@@ -22148,14 +22151,14 @@
         <v>2582</v>
       </c>
       <c r="CV21" s="90" t="s">
-        <v>2960</v>
+        <v>2959</v>
       </c>
       <c r="CW21" s="90" t="s">
         <v>2253</v>
       </c>
       <c r="CX21" s="88"/>
       <c r="DB21" s="12" t="s">
-        <v>2908</v>
+        <v>2907</v>
       </c>
       <c r="DC21" s="90" t="s">
         <v>2253</v>
@@ -22224,13 +22227,13 @@
         <v>2696</v>
       </c>
       <c r="BQ22" s="14" t="s">
-        <v>2810</v>
+        <v>2809</v>
       </c>
       <c r="BR22" s="20" t="s">
-        <v>2812</v>
+        <v>2811</v>
       </c>
       <c r="BT22" s="14" t="s">
-        <v>3030</v>
+        <v>3029</v>
       </c>
       <c r="BX22" s="11" t="s">
         <v>2541</v>
@@ -22260,14 +22263,14 @@
         <v>2281</v>
       </c>
       <c r="CV22" s="90" t="s">
-        <v>2950</v>
+        <v>2949</v>
       </c>
       <c r="CW22" s="90" t="s">
         <v>2253</v>
       </c>
       <c r="CX22" s="88"/>
       <c r="DB22" s="12" t="s">
-        <v>2941</v>
+        <v>2940</v>
       </c>
       <c r="DC22" s="90" t="s">
         <v>2253</v>
@@ -22327,13 +22330,13 @@
       </c>
       <c r="BE23" s="17"/>
       <c r="BQ23" s="14" t="s">
-        <v>2811</v>
+        <v>2810</v>
       </c>
       <c r="BR23" s="20" t="s">
-        <v>2813</v>
+        <v>2812</v>
       </c>
       <c r="BT23" s="14" t="s">
-        <v>2785</v>
+        <v>2784</v>
       </c>
       <c r="BX23" s="11" t="s">
         <v>2542</v>
@@ -22366,14 +22369,14 @@
         <v>2584</v>
       </c>
       <c r="CV23" s="90" t="s">
-        <v>2961</v>
+        <v>2960</v>
       </c>
       <c r="CW23" s="90" t="s">
         <v>2253</v>
       </c>
       <c r="CX23" s="88"/>
       <c r="DB23" s="20" t="s">
-        <v>2909</v>
+        <v>2908</v>
       </c>
       <c r="DC23" s="90" t="s">
         <v>2253</v>
@@ -22431,13 +22434,13 @@
       </c>
       <c r="BE24" s="17"/>
       <c r="BQ24" s="14" t="s">
+        <v>2868</v>
+      </c>
+      <c r="BR24" s="20" t="s">
         <v>2869</v>
       </c>
-      <c r="BR24" s="20" t="s">
-        <v>2870</v>
-      </c>
       <c r="BT24" s="14" t="s">
-        <v>2786</v>
+        <v>2785</v>
       </c>
       <c r="BX24" s="11" t="s">
         <v>2543</v>
@@ -22467,14 +22470,14 @@
         <v>2290</v>
       </c>
       <c r="CV24" s="90" t="s">
-        <v>2951</v>
+        <v>2950</v>
       </c>
       <c r="CW24" s="90" t="s">
         <v>2253</v>
       </c>
       <c r="CX24" s="88"/>
       <c r="DB24" s="20" t="s">
-        <v>2942</v>
+        <v>2941</v>
       </c>
       <c r="DC24" s="90" t="s">
         <v>2253</v>
@@ -22508,7 +22511,7 @@
       </c>
       <c r="M25" s="3"/>
       <c r="O25" s="12" t="s">
-        <v>3035</v>
+        <v>3034</v>
       </c>
       <c r="Q25" s="18" t="s">
         <v>2479</v>
@@ -22533,7 +22536,7 @@
       </c>
       <c r="BE25" s="17"/>
       <c r="BT25" s="14" t="s">
-        <v>2787</v>
+        <v>2786</v>
       </c>
       <c r="BX25" s="11" t="s">
         <v>2544</v>
@@ -22563,14 +22566,14 @@
         <v>2586</v>
       </c>
       <c r="CV25" s="90" t="s">
-        <v>2962</v>
+        <v>2961</v>
       </c>
       <c r="CW25" s="90" t="s">
         <v>2253</v>
       </c>
       <c r="CX25" s="88"/>
       <c r="DB25" s="12" t="s">
-        <v>2910</v>
+        <v>2909</v>
       </c>
       <c r="DC25" s="90" t="s">
         <v>2253</v>
@@ -22625,7 +22628,7 @@
       </c>
       <c r="BE26" s="17"/>
       <c r="BT26" s="14" t="s">
-        <v>2788</v>
+        <v>2787</v>
       </c>
       <c r="BX26" s="11" t="s">
         <v>1765</v>
@@ -22652,14 +22655,14 @@
         <v>2291</v>
       </c>
       <c r="CV26" s="90" t="s">
-        <v>2952</v>
+        <v>2951</v>
       </c>
       <c r="CW26" s="90" t="s">
         <v>2253</v>
       </c>
       <c r="CX26" s="88"/>
       <c r="DB26" s="12" t="s">
-        <v>2943</v>
+        <v>2942</v>
       </c>
       <c r="DC26" s="90" t="s">
         <v>2253</v>
@@ -22711,7 +22714,7 @@
         <v>1941</v>
       </c>
       <c r="BT27" s="14" t="s">
-        <v>2789</v>
+        <v>2788</v>
       </c>
       <c r="BX27" s="11" t="s">
         <v>1775</v>
@@ -22738,14 +22741,14 @@
         <v>2588</v>
       </c>
       <c r="CV27" s="90" t="s">
-        <v>2963</v>
+        <v>2962</v>
       </c>
       <c r="CW27" s="90" t="s">
         <v>2253</v>
       </c>
       <c r="CX27" s="88"/>
       <c r="DB27" s="20" t="s">
-        <v>2911</v>
+        <v>2910</v>
       </c>
       <c r="DC27" s="90" t="s">
         <v>2253</v>
@@ -22796,7 +22799,7 @@
         <v>1655</v>
       </c>
       <c r="BT28" s="14" t="s">
-        <v>2790</v>
+        <v>2789</v>
       </c>
       <c r="BX28" s="11" t="s">
         <v>2700</v>
@@ -22823,7 +22826,7 @@
         <v>2292</v>
       </c>
       <c r="CV28" s="90" t="s">
-        <v>2953</v>
+        <v>2952</v>
       </c>
       <c r="CW28" s="90" t="s">
         <v>2253</v>
@@ -22875,7 +22878,7 @@
         <v>1678</v>
       </c>
       <c r="BT29" s="14" t="s">
-        <v>3032</v>
+        <v>3031</v>
       </c>
       <c r="BX29" s="20"/>
       <c r="BY29" s="14"/>
@@ -22896,14 +22899,14 @@
         <v>2590</v>
       </c>
       <c r="CV29" s="90" t="s">
-        <v>2964</v>
+        <v>2963</v>
       </c>
       <c r="CW29" s="90" t="s">
         <v>2253</v>
       </c>
       <c r="CX29" s="88"/>
       <c r="DB29" s="12" t="s">
-        <v>2912</v>
+        <v>2911</v>
       </c>
       <c r="DC29" s="88" t="s">
         <v>2253</v>
@@ -22945,7 +22948,7 @@
         <v>1679</v>
       </c>
       <c r="BT30" s="14" t="s">
-        <v>3033</v>
+        <v>3032</v>
       </c>
       <c r="BX30" s="14"/>
       <c r="BY30" s="14"/>
@@ -22966,7 +22969,7 @@
         <v>2293</v>
       </c>
       <c r="CV30" s="90" t="s">
-        <v>2954</v>
+        <v>2953</v>
       </c>
       <c r="CW30" s="90" t="s">
         <v>2253</v>
@@ -23013,7 +23016,7 @@
         <v>1677</v>
       </c>
       <c r="BT31" s="14" t="s">
-        <v>2791</v>
+        <v>2790</v>
       </c>
       <c r="BX31" s="14"/>
       <c r="BY31" s="14"/>
@@ -23034,14 +23037,14 @@
         <v>2592</v>
       </c>
       <c r="CV31" s="90" t="s">
-        <v>2965</v>
+        <v>2964</v>
       </c>
       <c r="CW31" s="90" t="s">
         <v>2253</v>
       </c>
       <c r="CX31" s="88"/>
       <c r="DB31" s="20" t="s">
-        <v>2913</v>
+        <v>2912</v>
       </c>
       <c r="DC31" s="88" t="s">
         <v>2253</v>
@@ -23084,7 +23087,7 @@
         <v>1676</v>
       </c>
       <c r="BT32" s="14" t="s">
-        <v>3031</v>
+        <v>3030</v>
       </c>
       <c r="BX32" s="14"/>
       <c r="BY32" s="14"/>
@@ -23107,7 +23110,7 @@
         <v>2294</v>
       </c>
       <c r="CV32" s="90" t="s">
-        <v>2955</v>
+        <v>2954</v>
       </c>
       <c r="CW32" s="90" t="s">
         <v>2253</v>
@@ -23150,7 +23153,7 @@
         <v>1666</v>
       </c>
       <c r="BT33" s="14" t="s">
-        <v>2792</v>
+        <v>2791</v>
       </c>
       <c r="BX33" s="14"/>
       <c r="BY33" s="14"/>
@@ -23212,7 +23215,7 @@
         <v>1683</v>
       </c>
       <c r="BT34" s="14" t="s">
-        <v>2999</v>
+        <v>2998</v>
       </c>
       <c r="BX34" s="14"/>
       <c r="BY34" s="14"/>
@@ -23274,7 +23277,7 @@
         <v>1675</v>
       </c>
       <c r="BT35" s="14" t="s">
-        <v>2998</v>
+        <v>2997</v>
       </c>
       <c r="BX35" s="14"/>
       <c r="BY35" s="14"/>
@@ -23333,7 +23336,7 @@
         <v>1680</v>
       </c>
       <c r="BT36" s="14" t="s">
-        <v>2997</v>
+        <v>2996</v>
       </c>
       <c r="BX36" s="14"/>
       <c r="BY36" s="14"/>
@@ -23393,7 +23396,7 @@
         <v>1681</v>
       </c>
       <c r="BT37" s="14" t="s">
-        <v>2996</v>
+        <v>2995</v>
       </c>
       <c r="BX37" s="14"/>
       <c r="BY37" s="14"/>
@@ -23453,7 +23456,7 @@
         <v>1651</v>
       </c>
       <c r="BT38" s="14" t="s">
-        <v>2995</v>
+        <v>2994</v>
       </c>
       <c r="BX38" s="14"/>
       <c r="BY38" s="14"/>
@@ -23509,7 +23512,7 @@
         <v>1663</v>
       </c>
       <c r="BT39" s="14" t="s">
-        <v>3002</v>
+        <v>3001</v>
       </c>
       <c r="BX39" s="14"/>
       <c r="BY39" s="14"/>
@@ -23556,7 +23559,7 @@
         <v>1035</v>
       </c>
       <c r="AX40" s="94" t="s">
-        <v>3040</v>
+        <v>3039</v>
       </c>
       <c r="BC40" s="6" t="s">
         <v>1625</v>
@@ -23565,7 +23568,7 @@
         <v>1688</v>
       </c>
       <c r="BT40" s="14" t="s">
-        <v>2994</v>
+        <v>2993</v>
       </c>
       <c r="BX40" s="14"/>
       <c r="BY40" s="14"/>
@@ -23618,7 +23621,7 @@
         <v>1699</v>
       </c>
       <c r="BT41" s="14" t="s">
-        <v>3003</v>
+        <v>3002</v>
       </c>
       <c r="CP41" s="12" t="s">
         <v>2601</v>
@@ -23667,7 +23670,7 @@
         <v>1659</v>
       </c>
       <c r="BT42" s="14" t="s">
-        <v>3000</v>
+        <v>2999</v>
       </c>
       <c r="CP42" s="12" t="s">
         <v>2118</v>
@@ -23716,7 +23719,7 @@
         <v>1687</v>
       </c>
       <c r="BT43" s="14" t="s">
-        <v>3004</v>
+        <v>3003</v>
       </c>
       <c r="CP43" s="12" t="s">
         <v>2603</v>
@@ -23766,7 +23769,7 @@
         <v>1664</v>
       </c>
       <c r="BT44" s="14" t="s">
-        <v>2929</v>
+        <v>2928</v>
       </c>
       <c r="CN44" s="23"/>
       <c r="CO44" s="23"/>
@@ -23818,7 +23821,7 @@
         <v>1691</v>
       </c>
       <c r="BT45" s="14" t="s">
-        <v>3005</v>
+        <v>3004</v>
       </c>
       <c r="CN45" s="23"/>
       <c r="CO45" s="23"/>
@@ -23867,7 +23870,7 @@
         <v>1692</v>
       </c>
       <c r="BT46" s="14" t="s">
-        <v>2930</v>
+        <v>2929</v>
       </c>
       <c r="CN46" s="23"/>
       <c r="CO46" s="23"/>
@@ -23916,7 +23919,7 @@
         <v>1693</v>
       </c>
       <c r="BT47" s="14" t="s">
-        <v>3006</v>
+        <v>3005</v>
       </c>
       <c r="CM47" s="23"/>
       <c r="CN47" s="23"/>
@@ -23965,7 +23968,7 @@
         <v>1672</v>
       </c>
       <c r="BT48" s="14" t="s">
-        <v>2931</v>
+        <v>2930</v>
       </c>
       <c r="CM48" s="23"/>
       <c r="CN48" s="23"/>
@@ -24014,7 +24017,7 @@
         <v>1667</v>
       </c>
       <c r="BT49" s="14" t="s">
-        <v>3007</v>
+        <v>3006</v>
       </c>
       <c r="CM49" s="23"/>
       <c r="CN49" s="23"/>
@@ -24064,7 +24067,7 @@
         <v>2105</v>
       </c>
       <c r="BT50" s="14" t="s">
-        <v>2932</v>
+        <v>2931</v>
       </c>
       <c r="CM50" s="23"/>
       <c r="CN50" s="23"/>
@@ -24114,7 +24117,7 @@
         <v>1689</v>
       </c>
       <c r="BT51" s="14" t="s">
-        <v>3008</v>
+        <v>3007</v>
       </c>
       <c r="CM51" s="23"/>
       <c r="CN51" s="23"/>
@@ -24163,7 +24166,7 @@
         <v>1668</v>
       </c>
       <c r="BT52" s="14" t="s">
-        <v>3001</v>
+        <v>3000</v>
       </c>
       <c r="CM52" s="23"/>
       <c r="CN52" s="23"/>
@@ -24213,7 +24216,7 @@
         <v>1685</v>
       </c>
       <c r="BT53" s="14" t="s">
-        <v>2933</v>
+        <v>2932</v>
       </c>
       <c r="CM53" s="23"/>
       <c r="CN53" s="23"/>
@@ -24263,7 +24266,7 @@
         <v>1657</v>
       </c>
       <c r="BT54" s="14" t="s">
-        <v>2934</v>
+        <v>2933</v>
       </c>
       <c r="CM54" s="23"/>
       <c r="CP54" s="12" t="s">
@@ -24311,7 +24314,7 @@
         <v>1654</v>
       </c>
       <c r="BT55" s="14" t="s">
-        <v>3009</v>
+        <v>3008</v>
       </c>
       <c r="CM55" s="23"/>
       <c r="CP55" s="12" t="s">
@@ -24359,7 +24362,7 @@
         <v>2104</v>
       </c>
       <c r="BT56" s="14" t="s">
-        <v>3010</v>
+        <v>3009</v>
       </c>
       <c r="CM56" s="23"/>
       <c r="CP56" s="12" t="s">
@@ -24407,7 +24410,7 @@
         <v>1682</v>
       </c>
       <c r="BT57" s="14" t="s">
-        <v>3011</v>
+        <v>3010</v>
       </c>
       <c r="CP57" s="12" t="s">
         <v>2617</v>
@@ -24454,7 +24457,7 @@
         <v>1980</v>
       </c>
       <c r="BT58" s="14" t="s">
-        <v>3012</v>
+        <v>3011</v>
       </c>
       <c r="CP58" s="12" t="s">
         <v>2126</v>
@@ -24498,7 +24501,7 @@
         <v>1658</v>
       </c>
       <c r="BT59" s="14" t="s">
-        <v>3013</v>
+        <v>3012</v>
       </c>
       <c r="CP59" s="12" t="s">
         <v>2619</v>
@@ -24542,7 +24545,7 @@
         <v>1981</v>
       </c>
       <c r="BT60" s="14" t="s">
-        <v>3014</v>
+        <v>3013</v>
       </c>
       <c r="CP60" s="12" t="s">
         <v>2127</v>
@@ -24586,7 +24589,7 @@
         <v>1673</v>
       </c>
       <c r="BT61" s="14" t="s">
-        <v>3015</v>
+        <v>3014</v>
       </c>
       <c r="CP61" s="12" t="s">
         <v>2621</v>
@@ -24621,7 +24624,7 @@
       <c r="M62" s="4"/>
       <c r="P62" s="6"/>
       <c r="AX62" s="94" t="s">
-        <v>3038</v>
+        <v>3037</v>
       </c>
       <c r="BC62" s="6" t="s">
         <v>1634</v>
@@ -24630,7 +24633,7 @@
         <v>1686</v>
       </c>
       <c r="BT62" s="14" t="s">
-        <v>3016</v>
+        <v>3015</v>
       </c>
       <c r="CP62" s="12" t="s">
         <v>2128</v>
@@ -24674,7 +24677,7 @@
         <v>1671</v>
       </c>
       <c r="BT63" s="14" t="s">
-        <v>3017</v>
+        <v>3016</v>
       </c>
       <c r="CP63" s="12" t="s">
         <v>2623</v>
@@ -24715,7 +24718,7 @@
         <v>1700</v>
       </c>
       <c r="BT64" s="14" t="s">
-        <v>3018</v>
+        <v>3017</v>
       </c>
       <c r="CP64" s="23" t="s">
         <v>2129</v>
@@ -24756,7 +24759,7 @@
         <v>1649</v>
       </c>
       <c r="BT65" s="14" t="s">
-        <v>3019</v>
+        <v>3018</v>
       </c>
       <c r="CP65" s="12" t="s">
         <v>2625</v>
@@ -24797,7 +24800,7 @@
         <v>1669</v>
       </c>
       <c r="BT66" s="14" t="s">
-        <v>3020</v>
+        <v>3019</v>
       </c>
       <c r="CP66" s="23" t="s">
         <v>2130</v>
@@ -24838,7 +24841,7 @@
         <v>1674</v>
       </c>
       <c r="BT67" s="14" t="s">
-        <v>3021</v>
+        <v>3020</v>
       </c>
       <c r="CP67" s="12" t="s">
         <v>2627</v>
@@ -24879,7 +24882,7 @@
         <v>1652</v>
       </c>
       <c r="BT68" s="14" t="s">
-        <v>3022</v>
+        <v>3021</v>
       </c>
       <c r="CP68" s="23" t="s">
         <v>2131</v>
@@ -24919,7 +24922,7 @@
         <v>1982</v>
       </c>
       <c r="BT69" s="14" t="s">
-        <v>3023</v>
+        <v>3022</v>
       </c>
       <c r="CP69" s="12" t="s">
         <v>2629</v>
@@ -24960,7 +24963,7 @@
         <v>1695</v>
       </c>
       <c r="BT70" s="14" t="s">
-        <v>3024</v>
+        <v>3023</v>
       </c>
       <c r="CP70" s="23" t="s">
         <v>2132</v>
@@ -25001,7 +25004,7 @@
         <v>1670</v>
       </c>
       <c r="BT71" s="14" t="s">
-        <v>3025</v>
+        <v>3024</v>
       </c>
       <c r="CP71" s="12" t="s">
         <v>2631</v>
@@ -25042,7 +25045,7 @@
         <v>1665</v>
       </c>
       <c r="BT72" s="14" t="s">
-        <v>3026</v>
+        <v>3025</v>
       </c>
       <c r="CP72" s="23" t="s">
         <v>2133</v>
@@ -25083,7 +25086,7 @@
         <v>1696</v>
       </c>
       <c r="BT73" s="14" t="s">
-        <v>3027</v>
+        <v>3026</v>
       </c>
       <c r="CP73" s="12" t="s">
         <v>2633</v>
@@ -25124,7 +25127,7 @@
         <v>1684</v>
       </c>
       <c r="BT74" s="14" t="s">
-        <v>3028</v>
+        <v>3027</v>
       </c>
       <c r="CP74" s="23" t="s">
         <v>2134</v>
@@ -25165,7 +25168,7 @@
         <v>1697</v>
       </c>
       <c r="BT75" s="14" t="s">
-        <v>2974</v>
+        <v>2973</v>
       </c>
       <c r="CP75" s="12" t="s">
         <v>2635</v>
@@ -25200,13 +25203,13 @@
       <c r="M76" s="4"/>
       <c r="P76" s="6"/>
       <c r="AX76" s="94" t="s">
-        <v>3039</v>
+        <v>3038</v>
       </c>
       <c r="BD76" s="6" t="s">
         <v>1983</v>
       </c>
       <c r="BT76" s="14" t="s">
-        <v>2971</v>
+        <v>2970</v>
       </c>
       <c r="CP76" s="23" t="s">
         <v>2135</v>
@@ -25247,7 +25250,7 @@
         <v>1647</v>
       </c>
       <c r="BT77" s="14" t="s">
-        <v>2972</v>
+        <v>2971</v>
       </c>
       <c r="CP77" s="12" t="s">
         <v>2637</v>
@@ -25288,7 +25291,7 @@
         <v>1698</v>
       </c>
       <c r="BT78" s="14" t="s">
-        <v>2973</v>
+        <v>2972</v>
       </c>
       <c r="CP78" s="23" t="s">
         <v>2136</v>
@@ -25329,7 +25332,7 @@
         <v>1648</v>
       </c>
       <c r="BT79" s="14" t="s">
-        <v>2974</v>
+        <v>2973</v>
       </c>
       <c r="CP79" s="12" t="s">
         <v>2638</v>
@@ -25370,7 +25373,7 @@
         <v>1694</v>
       </c>
       <c r="BT80" s="14" t="s">
-        <v>2975</v>
+        <v>2974</v>
       </c>
       <c r="CP80" s="23" t="s">
         <v>2137</v>
@@ -25411,7 +25414,7 @@
         <v>1690</v>
       </c>
       <c r="BT81" s="14" t="s">
-        <v>2976</v>
+        <v>2975</v>
       </c>
       <c r="CP81" s="12" t="s">
         <v>2640</v>
@@ -25452,7 +25455,7 @@
         <v>1747</v>
       </c>
       <c r="BT82" s="14" t="s">
-        <v>3029</v>
+        <v>3028</v>
       </c>
       <c r="CP82" s="23" t="s">
         <v>2138</v>
@@ -25599,7 +25602,7 @@
       </c>
       <c r="M86" s="4"/>
       <c r="AX86" s="94" t="s">
-        <v>3041</v>
+        <v>3040</v>
       </c>
       <c r="BD86" s="6" t="s">
         <v>1748</v>
@@ -25636,7 +25639,7 @@
       </c>
       <c r="M87" s="4"/>
       <c r="AX87" s="94" t="s">
-        <v>3042</v>
+        <v>3041</v>
       </c>
       <c r="BD87" s="6" t="s">
         <v>1985</v>
@@ -25747,7 +25750,7 @@
       </c>
       <c r="M90" s="4"/>
       <c r="AX90" s="94" t="s">
-        <v>3043</v>
+        <v>3042</v>
       </c>
       <c r="BD90" s="6" t="s">
         <v>1745</v>
@@ -25858,7 +25861,7 @@
       </c>
       <c r="M93" s="3"/>
       <c r="AX93" s="94" t="s">
-        <v>3044</v>
+        <v>3043</v>
       </c>
       <c r="BD93" s="6" t="s">
         <v>1987</v>
@@ -26043,7 +26046,7 @@
       </c>
       <c r="M98" s="4"/>
       <c r="AX98" s="94" t="s">
-        <v>3047</v>
+        <v>3046</v>
       </c>
       <c r="BD98" s="7" t="s">
         <v>2675</v>
@@ -26387,7 +26390,7 @@
       </c>
       <c r="M108" s="4"/>
       <c r="AX108" s="94" t="s">
-        <v>3046</v>
+        <v>3045</v>
       </c>
       <c r="CP108" s="12" t="s">
         <v>2150</v>
@@ -26709,7 +26712,7 @@
       </c>
       <c r="M118" s="3"/>
       <c r="AX118" s="94" t="s">
-        <v>3045</v>
+        <v>3044</v>
       </c>
       <c r="CS118" s="40"/>
     </row>
@@ -26834,7 +26837,7 @@
       </c>
       <c r="M123" s="3"/>
       <c r="AX123" s="94" t="s">
-        <v>3048</v>
+        <v>3047</v>
       </c>
       <c r="CS123" s="40"/>
     </row>
@@ -27084,7 +27087,7 @@
       </c>
       <c r="M133" s="3"/>
       <c r="AX133" s="94" t="s">
-        <v>3049</v>
+        <v>3048</v>
       </c>
       <c r="CS133" s="40"/>
     </row>
@@ -28909,7 +28912,7 @@
       <c r="CS277" s="40"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="ReLuXiCIzrYRqmaP2jDysp01Zx9gpOUw/dn0RvJcXcm4J4PW5d7cb2O4iZNZC0SXSTTCndFImQ4YfBam9XEKcw==" saltValue="ACYHVy7WShbC5GkNGwql2Q==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="zIICaV1ZMZOZvaDRsZmOiK1HohbYKuu5KryAP4BgjVrPXVxpGbPekllZzXWp5E5DBe+aopjRjlWsauD9ViD8zQ==" saltValue="eVhZYkrn9dRtdFQXNw9EZg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="2">
     <mergeCell ref="M27:M28"/>
     <mergeCell ref="M34:M35"/>

</xml_diff>

<commit_message>
Added new grain size fractions to "material_analyzed"
</commit_message>
<xml_diff>
--- a/Excel_templates/MOSAIC_input_excel_file_2022.xlsx
+++ b/Excel_templates/MOSAIC_input_excel_file_2022.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sparadis\Documents\ETH\MOSAIC\MOSAIC_Client\Excel_templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63552C0A-2F67-4955-B005-B6B3344C92DF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BECFC844-E768-4752-88CD-C38899C7B1F4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30204" yWindow="10044" windowWidth="40020" windowHeight="22296" tabRatio="694" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30204" yWindow="10044" windowWidth="40020" windowHeight="22296" tabRatio="694" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ARTICLE_AUTHOR" sheetId="3" r:id="rId1"/>
@@ -93,7 +93,7 @@
     <definedName name="MAR_g_cm2_yr">SET_VARIABLES!$GJ$2:$GJ$20</definedName>
     <definedName name="MAR_model">SET_VARIABLES!#REF!</definedName>
     <definedName name="MAR_tracer">SET_VARIABLES!#REF!</definedName>
-    <definedName name="material_analyzed">SET_VARIABLES!$BU$2:$BU$82</definedName>
+    <definedName name="material_analyzed">SET_VARIABLES!$BU$2:$BU$90</definedName>
     <definedName name="Mauritania">SET_VARIABLES!$AN$2:$AN$7</definedName>
     <definedName name="mean_grain_size_microm">SET_VARIABLES!$FB$2:$FB$5</definedName>
     <definedName name="median_grain_size_microm">SET_VARIABLES!$FC$2:$FC$5</definedName>
@@ -187,7 +187,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4122" uniqueCount="3050">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4130" uniqueCount="3058">
   <si>
     <t>sample_name</t>
   </si>
@@ -9337,6 +9337,30 @@
   </si>
   <si>
     <t>single corer (Niemisto, NIOZ, Kajak corer)</t>
+  </si>
+  <si>
+    <t>0.156-0.5 mm</t>
+  </si>
+  <si>
+    <t>0.05-0.156 mm</t>
+  </si>
+  <si>
+    <t>0.026-0.05 mm</t>
+  </si>
+  <si>
+    <t>0.011-0.026 mm</t>
+  </si>
+  <si>
+    <t>0.005-0.011 mm</t>
+  </si>
+  <si>
+    <t>0.002-0.005 mm</t>
+  </si>
+  <si>
+    <t>0.0008-0.002 mm</t>
+  </si>
+  <si>
+    <t>&lt;0.0005 mm</t>
   </si>
 </sst>
 </file>
@@ -10341,8 +10365,8 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C30" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="A3" sqref="A3"/>
@@ -10730,11 +10754,11 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:CB52"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane xSplit="3" ySplit="6" topLeftCell="D7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="L6" sqref="L6"/>
+      <selection pane="bottomRight" activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -13582,8 +13606,8 @@
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:ID277"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+    <sheetView topLeftCell="BR13" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="BU41" sqref="BU41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -20977,7 +21001,7 @@
       </c>
       <c r="BF25" s="17"/>
       <c r="BU25" s="14" t="s">
-        <v>2784</v>
+        <v>3050</v>
       </c>
       <c r="BY25" s="11" t="s">
         <v>2543</v>
@@ -21069,7 +21093,7 @@
       </c>
       <c r="BF26" s="17"/>
       <c r="BU26" s="14" t="s">
-        <v>2785</v>
+        <v>2784</v>
       </c>
       <c r="BY26" s="11" t="s">
         <v>1765</v>
@@ -21155,7 +21179,7 @@
         <v>1941</v>
       </c>
       <c r="BU27" s="14" t="s">
-        <v>2786</v>
+        <v>2785</v>
       </c>
       <c r="BY27" s="11" t="s">
         <v>1775</v>
@@ -21240,7 +21264,7 @@
         <v>1655</v>
       </c>
       <c r="BU28" s="14" t="s">
-        <v>2787</v>
+        <v>3051</v>
       </c>
       <c r="BY28" s="11" t="s">
         <v>2698</v>
@@ -21319,7 +21343,7 @@
         <v>1678</v>
       </c>
       <c r="BU29" s="14" t="s">
-        <v>3028</v>
+        <v>2786</v>
       </c>
       <c r="BY29" s="20"/>
       <c r="BZ29" s="14"/>
@@ -21389,7 +21413,7 @@
         <v>1679</v>
       </c>
       <c r="BU30" s="14" t="s">
-        <v>3029</v>
+        <v>3052</v>
       </c>
       <c r="BY30" s="14"/>
       <c r="BZ30" s="14"/>
@@ -21457,7 +21481,7 @@
         <v>1677</v>
       </c>
       <c r="BU31" s="14" t="s">
-        <v>2788</v>
+        <v>2787</v>
       </c>
       <c r="BY31" s="14"/>
       <c r="BZ31" s="14"/>
@@ -21528,7 +21552,7 @@
         <v>1676</v>
       </c>
       <c r="BU32" s="14" t="s">
-        <v>3027</v>
+        <v>3053</v>
       </c>
       <c r="BY32" s="14"/>
       <c r="BZ32" s="14"/>
@@ -21594,7 +21618,7 @@
         <v>1666</v>
       </c>
       <c r="BU33" s="14" t="s">
-        <v>2789</v>
+        <v>3028</v>
       </c>
       <c r="BY33" s="14"/>
       <c r="BZ33" s="14"/>
@@ -21656,7 +21680,7 @@
         <v>1683</v>
       </c>
       <c r="BU34" s="14" t="s">
-        <v>2995</v>
+        <v>3054</v>
       </c>
       <c r="BY34" s="14"/>
       <c r="BZ34" s="14"/>
@@ -21718,7 +21742,7 @@
         <v>1675</v>
       </c>
       <c r="BU35" s="14" t="s">
-        <v>2994</v>
+        <v>3029</v>
       </c>
       <c r="BY35" s="14"/>
       <c r="BZ35" s="14"/>
@@ -21777,7 +21801,7 @@
         <v>1680</v>
       </c>
       <c r="BU36" s="14" t="s">
-        <v>2993</v>
+        <v>3055</v>
       </c>
       <c r="BY36" s="14"/>
       <c r="BZ36" s="14"/>
@@ -21837,7 +21861,7 @@
         <v>1681</v>
       </c>
       <c r="BU37" s="14" t="s">
-        <v>2992</v>
+        <v>3056</v>
       </c>
       <c r="BY37" s="14"/>
       <c r="BZ37" s="14"/>
@@ -21897,7 +21921,7 @@
         <v>1651</v>
       </c>
       <c r="BU38" s="14" t="s">
-        <v>2991</v>
+        <v>2788</v>
       </c>
       <c r="BY38" s="14"/>
       <c r="BZ38" s="14"/>
@@ -21953,7 +21977,7 @@
         <v>1663</v>
       </c>
       <c r="BU39" s="14" t="s">
-        <v>2998</v>
+        <v>3027</v>
       </c>
       <c r="BY39" s="14"/>
       <c r="BZ39" s="14"/>
@@ -22009,7 +22033,7 @@
         <v>1688</v>
       </c>
       <c r="BU40" s="14" t="s">
-        <v>2990</v>
+        <v>3057</v>
       </c>
       <c r="BY40" s="14"/>
       <c r="BZ40" s="14"/>
@@ -22062,7 +22086,7 @@
         <v>1699</v>
       </c>
       <c r="BU41" s="14" t="s">
-        <v>2999</v>
+        <v>2789</v>
       </c>
       <c r="CQ41" s="12" t="s">
         <v>2599</v>
@@ -22111,7 +22135,7 @@
         <v>1659</v>
       </c>
       <c r="BU42" s="14" t="s">
-        <v>2996</v>
+        <v>2995</v>
       </c>
       <c r="CQ42" s="12" t="s">
         <v>2118</v>
@@ -22160,7 +22184,7 @@
         <v>1687</v>
       </c>
       <c r="BU43" s="14" t="s">
-        <v>3000</v>
+        <v>2994</v>
       </c>
       <c r="CQ43" s="12" t="s">
         <v>2601</v>
@@ -22210,7 +22234,7 @@
         <v>1664</v>
       </c>
       <c r="BU44" s="14" t="s">
-        <v>2925</v>
+        <v>2993</v>
       </c>
       <c r="CO44" s="23"/>
       <c r="CP44" s="23"/>
@@ -22262,7 +22286,7 @@
         <v>1691</v>
       </c>
       <c r="BU45" s="14" t="s">
-        <v>3001</v>
+        <v>2992</v>
       </c>
       <c r="CO45" s="23"/>
       <c r="CP45" s="23"/>
@@ -22314,7 +22338,7 @@
         <v>1692</v>
       </c>
       <c r="BU46" s="14" t="s">
-        <v>2926</v>
+        <v>2991</v>
       </c>
       <c r="CO46" s="23"/>
       <c r="CP46" s="23"/>
@@ -22363,7 +22387,7 @@
         <v>1693</v>
       </c>
       <c r="BU47" s="14" t="s">
-        <v>3002</v>
+        <v>2998</v>
       </c>
       <c r="CN47" s="23"/>
       <c r="CO47" s="23"/>
@@ -22412,7 +22436,7 @@
         <v>1672</v>
       </c>
       <c r="BU48" s="14" t="s">
-        <v>2927</v>
+        <v>2990</v>
       </c>
       <c r="CN48" s="23"/>
       <c r="CO48" s="23"/>
@@ -22461,7 +22485,7 @@
         <v>1667</v>
       </c>
       <c r="BU49" s="14" t="s">
-        <v>3003</v>
+        <v>2999</v>
       </c>
       <c r="CN49" s="23"/>
       <c r="CO49" s="23"/>
@@ -22511,7 +22535,7 @@
         <v>2105</v>
       </c>
       <c r="BU50" s="14" t="s">
-        <v>2928</v>
+        <v>2996</v>
       </c>
       <c r="CN50" s="23"/>
       <c r="CO50" s="23"/>
@@ -22561,7 +22585,7 @@
         <v>1689</v>
       </c>
       <c r="BU51" s="14" t="s">
-        <v>3004</v>
+        <v>3000</v>
       </c>
       <c r="CN51" s="23"/>
       <c r="CO51" s="23"/>
@@ -22610,7 +22634,7 @@
         <v>1668</v>
       </c>
       <c r="BU52" s="14" t="s">
-        <v>2997</v>
+        <v>2925</v>
       </c>
       <c r="CN52" s="23"/>
       <c r="CO52" s="23"/>
@@ -22660,7 +22684,7 @@
         <v>1685</v>
       </c>
       <c r="BU53" s="14" t="s">
-        <v>2929</v>
+        <v>3001</v>
       </c>
       <c r="CN53" s="23"/>
       <c r="CO53" s="23"/>
@@ -22710,7 +22734,7 @@
         <v>1657</v>
       </c>
       <c r="BU54" s="14" t="s">
-        <v>2930</v>
+        <v>2926</v>
       </c>
       <c r="CN54" s="23"/>
       <c r="CQ54" s="12" t="s">
@@ -22758,7 +22782,7 @@
         <v>1654</v>
       </c>
       <c r="BU55" s="14" t="s">
-        <v>3005</v>
+        <v>3002</v>
       </c>
       <c r="CN55" s="23"/>
       <c r="CQ55" s="12" t="s">
@@ -22806,7 +22830,7 @@
         <v>2104</v>
       </c>
       <c r="BU56" s="14" t="s">
-        <v>3006</v>
+        <v>2927</v>
       </c>
       <c r="CN56" s="23"/>
       <c r="CQ56" s="12" t="s">
@@ -22854,7 +22878,7 @@
         <v>1682</v>
       </c>
       <c r="BU57" s="14" t="s">
-        <v>3007</v>
+        <v>3003</v>
       </c>
       <c r="CQ57" s="12" t="s">
         <v>2615</v>
@@ -22901,7 +22925,7 @@
         <v>1980</v>
       </c>
       <c r="BU58" s="14" t="s">
-        <v>3008</v>
+        <v>2928</v>
       </c>
       <c r="CQ58" s="12" t="s">
         <v>2126</v>
@@ -22945,7 +22969,7 @@
         <v>1658</v>
       </c>
       <c r="BU59" s="14" t="s">
-        <v>3009</v>
+        <v>3004</v>
       </c>
       <c r="CQ59" s="12" t="s">
         <v>2617</v>
@@ -22989,7 +23013,7 @@
         <v>1981</v>
       </c>
       <c r="BU60" s="14" t="s">
-        <v>3010</v>
+        <v>2997</v>
       </c>
       <c r="CQ60" s="12" t="s">
         <v>2127</v>
@@ -23033,7 +23057,7 @@
         <v>1673</v>
       </c>
       <c r="BU61" s="14" t="s">
-        <v>3011</v>
+        <v>2929</v>
       </c>
       <c r="CQ61" s="12" t="s">
         <v>2619</v>
@@ -23077,7 +23101,7 @@
         <v>1686</v>
       </c>
       <c r="BU62" s="14" t="s">
-        <v>3012</v>
+        <v>2930</v>
       </c>
       <c r="CQ62" s="12" t="s">
         <v>2128</v>
@@ -23121,7 +23145,7 @@
         <v>1671</v>
       </c>
       <c r="BU63" s="14" t="s">
-        <v>3013</v>
+        <v>3005</v>
       </c>
       <c r="CQ63" s="12" t="s">
         <v>2621</v>
@@ -23162,7 +23186,7 @@
         <v>1700</v>
       </c>
       <c r="BU64" s="14" t="s">
-        <v>3014</v>
+        <v>3006</v>
       </c>
       <c r="CQ64" s="23" t="s">
         <v>2129</v>
@@ -23203,7 +23227,7 @@
         <v>1649</v>
       </c>
       <c r="BU65" s="14" t="s">
-        <v>3015</v>
+        <v>3007</v>
       </c>
       <c r="CQ65" s="12" t="s">
         <v>2623</v>
@@ -23244,7 +23268,7 @@
         <v>1669</v>
       </c>
       <c r="BU66" s="14" t="s">
-        <v>3016</v>
+        <v>3008</v>
       </c>
       <c r="CQ66" s="23" t="s">
         <v>2130</v>
@@ -23285,7 +23309,7 @@
         <v>1674</v>
       </c>
       <c r="BU67" s="14" t="s">
-        <v>3017</v>
+        <v>3009</v>
       </c>
       <c r="CQ67" s="12" t="s">
         <v>2625</v>
@@ -23326,7 +23350,7 @@
         <v>1652</v>
       </c>
       <c r="BU68" s="14" t="s">
-        <v>3018</v>
+        <v>3010</v>
       </c>
       <c r="CQ68" s="23" t="s">
         <v>2131</v>
@@ -23366,7 +23390,7 @@
         <v>1982</v>
       </c>
       <c r="BU69" s="14" t="s">
-        <v>3019</v>
+        <v>3011</v>
       </c>
       <c r="CQ69" s="12" t="s">
         <v>2627</v>
@@ -23407,7 +23431,7 @@
         <v>1695</v>
       </c>
       <c r="BU70" s="14" t="s">
-        <v>3020</v>
+        <v>3012</v>
       </c>
       <c r="CQ70" s="23" t="s">
         <v>2132</v>
@@ -23448,7 +23472,7 @@
         <v>1670</v>
       </c>
       <c r="BU71" s="14" t="s">
-        <v>3021</v>
+        <v>3013</v>
       </c>
       <c r="CQ71" s="12" t="s">
         <v>2629</v>
@@ -23489,7 +23513,7 @@
         <v>1665</v>
       </c>
       <c r="BU72" s="14" t="s">
-        <v>3022</v>
+        <v>3014</v>
       </c>
       <c r="CQ72" s="23" t="s">
         <v>2133</v>
@@ -23530,7 +23554,7 @@
         <v>1696</v>
       </c>
       <c r="BU73" s="14" t="s">
-        <v>3023</v>
+        <v>3015</v>
       </c>
       <c r="CQ73" s="12" t="s">
         <v>2631</v>
@@ -23571,7 +23595,7 @@
         <v>1684</v>
       </c>
       <c r="BU74" s="14" t="s">
-        <v>3024</v>
+        <v>3016</v>
       </c>
       <c r="CQ74" s="23" t="s">
         <v>2134</v>
@@ -23612,7 +23636,7 @@
         <v>1697</v>
       </c>
       <c r="BU75" s="14" t="s">
-        <v>2970</v>
+        <v>3017</v>
       </c>
       <c r="CQ75" s="12" t="s">
         <v>2633</v>
@@ -23653,7 +23677,7 @@
         <v>1983</v>
       </c>
       <c r="BU76" s="14" t="s">
-        <v>2967</v>
+        <v>3018</v>
       </c>
       <c r="CQ76" s="23" t="s">
         <v>2135</v>
@@ -23694,7 +23718,7 @@
         <v>1647</v>
       </c>
       <c r="BU77" s="14" t="s">
-        <v>2968</v>
+        <v>3019</v>
       </c>
       <c r="CQ77" s="12" t="s">
         <v>2635</v>
@@ -23735,7 +23759,7 @@
         <v>1698</v>
       </c>
       <c r="BU78" s="14" t="s">
-        <v>2969</v>
+        <v>3020</v>
       </c>
       <c r="CQ78" s="23" t="s">
         <v>2136</v>
@@ -23776,7 +23800,7 @@
         <v>1648</v>
       </c>
       <c r="BU79" s="14" t="s">
-        <v>2970</v>
+        <v>3021</v>
       </c>
       <c r="CQ79" s="12" t="s">
         <v>2636</v>
@@ -23817,7 +23841,7 @@
         <v>1694</v>
       </c>
       <c r="BU80" s="14" t="s">
-        <v>2971</v>
+        <v>3022</v>
       </c>
       <c r="CQ80" s="23" t="s">
         <v>2137</v>
@@ -23858,7 +23882,7 @@
         <v>1690</v>
       </c>
       <c r="BU81" s="14" t="s">
-        <v>2972</v>
+        <v>3023</v>
       </c>
       <c r="CQ81" s="12" t="s">
         <v>2638</v>
@@ -23899,7 +23923,7 @@
         <v>1747</v>
       </c>
       <c r="BU82" s="14" t="s">
-        <v>3025</v>
+        <v>3024</v>
       </c>
       <c r="CQ82" s="23" t="s">
         <v>2138</v>
@@ -23939,6 +23963,9 @@
       <c r="BE83" s="6" t="s">
         <v>1749</v>
       </c>
+      <c r="BU83" s="14" t="s">
+        <v>2970</v>
+      </c>
       <c r="CQ83" s="12" t="s">
         <v>2639</v>
       </c>
@@ -23977,6 +24004,9 @@
       <c r="BE84" s="6" t="s">
         <v>1984</v>
       </c>
+      <c r="BU84" s="14" t="s">
+        <v>2967</v>
+      </c>
       <c r="CQ84" s="23" t="s">
         <v>2139</v>
       </c>
@@ -24014,6 +24044,9 @@
       <c r="BE85" s="6" t="s">
         <v>1656</v>
       </c>
+      <c r="BU85" s="14" t="s">
+        <v>2968</v>
+      </c>
       <c r="CQ85" s="12" t="s">
         <v>2640</v>
       </c>
@@ -24051,6 +24084,9 @@
       <c r="BE86" s="6" t="s">
         <v>1748</v>
       </c>
+      <c r="BU86" s="14" t="s">
+        <v>2969</v>
+      </c>
       <c r="CQ86" s="23" t="s">
         <v>2140</v>
       </c>
@@ -24088,6 +24124,9 @@
       <c r="BE87" s="6" t="s">
         <v>1985</v>
       </c>
+      <c r="BU87" s="14" t="s">
+        <v>2970</v>
+      </c>
       <c r="CQ87" s="12" t="s">
         <v>2642</v>
       </c>
@@ -24125,6 +24164,9 @@
       <c r="BE88" s="6" t="s">
         <v>1750</v>
       </c>
+      <c r="BU88" s="14" t="s">
+        <v>2971</v>
+      </c>
       <c r="CQ88" s="23" t="s">
         <v>2141</v>
       </c>
@@ -24162,6 +24204,9 @@
       <c r="BE89" s="6" t="s">
         <v>1744</v>
       </c>
+      <c r="BU89" s="14" t="s">
+        <v>2972</v>
+      </c>
       <c r="CQ89" s="12" t="s">
         <v>2644</v>
       </c>
@@ -24198,6 +24243,9 @@
       </c>
       <c r="BE90" s="6" t="s">
         <v>1745</v>
+      </c>
+      <c r="BU90" s="14" t="s">
+        <v>3025</v>
       </c>
       <c r="CQ90" s="23" t="s">
         <v>2142</v>
@@ -27356,7 +27404,7 @@
       <c r="CT277" s="40"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="idxTFXldcr+BeibAFZGI6cPVFJj52DuMnv1RvRdHdzwioV3aP6qSSP0gJUxxWyC90DFHLhY0OrKJurVY6qKTKg==" saltValue="6IN8dJ8X1F3U4y5sQBjvpg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="u3ikDjYQU5ICeZdTr2QlsS0wtjnly2LQhwV3I6lBzoEekxL5FaX7pyoJjX9dZkVARsXJXarPS9Dx/Oxd1V4jlg==" saltValue="jOYq+wIxxaq8oX4NVrPIIg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="2">
     <mergeCell ref="M27:M28"/>
     <mergeCell ref="M34:M35"/>

</xml_diff>

<commit_message>
Modified the pop-up comment of sample_exclusivity_clause
</commit_message>
<xml_diff>
--- a/Excel_templates/MOSAIC_input_excel_file_2022.xlsx
+++ b/Excel_templates/MOSAIC_input_excel_file_2022.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sparadis\Documents\ETH\MOSAIC\MOSAIC_Client\Excel_templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BECFC844-E768-4752-88CD-C38899C7B1F4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D4B5B6A-7F7C-4A2A-B2D3-5A28C7F811BD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30204" yWindow="10044" windowWidth="40020" windowHeight="22296" tabRatio="694" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30204" yWindow="10044" windowWidth="40020" windowHeight="22296" tabRatio="694" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ARTICLE_AUTHOR" sheetId="3" r:id="rId1"/>
@@ -10365,7 +10365,7 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -10754,11 +10754,11 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:CB52"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane xSplit="3" ySplit="6" topLeftCell="D7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="A7" sqref="A7"/>
+      <selection pane="bottomRight" activeCell="D2" sqref="D2:D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -13530,7 +13530,6 @@
     <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Sample analysis category" prompt="Choose from the drop-down list the analysis category the variable belongs to" sqref="L1:CB1" xr:uid="{2372D2F3-EE0C-4296-AC86-BA3569CC20EF}">
       <formula1>Sample_analyses_types</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Specify if the following analyses are open or private (i.e. published or unpublished)" sqref="D2:D4" xr:uid="{2D0E370F-3B05-4238-897F-C6B71BB62191}"/>
     <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Depth should be positive." prompt="Core depth of the upper limit of the sample (i.e. 0 cm)" sqref="H7:H1048576" xr:uid="{BE1F0784-49D8-4BCD-8064-3F609B2CEBBB}">
       <formula1>0</formula1>
     </dataValidation>
@@ -13553,6 +13552,7 @@
     <dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" promptTitle="Method details" prompt="If known, add any additional information about the method used to obtain the variable, such as the model of the analyzer. For certain biomarkers, we encourage you to add information from the drop-down list (if relevant)." sqref="L4:CB4" xr:uid="{A2878DFE-8081-4751-8EA1-1B0E764D61E4}">
       <formula1>IF(L1="sample_alkanes",INDIRECT("alkane_ranges"),IF(L1="sample_fatty_acids",INDIRECT("fa_ranges"),IF(L1="sample_alcohols",INDIRECT("alcohol_ranges"),INDIRECT("no_method_details"))))</formula1>
     </dataValidation>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Specify if the following analyses are for exclusive use (TRUE) or public (FALSE). For instance, if the data is published, it should be set to FALSE (publically accessible)." sqref="D2:D6" xr:uid="{9A380B36-1978-4D96-8689-777E66C2E25E}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Added >1.6 g/cm3 to material analyzed
</commit_message>
<xml_diff>
--- a/Excel_templates/MOSAIC_input_excel_file_2022.xlsx
+++ b/Excel_templates/MOSAIC_input_excel_file_2022.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20395"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20399"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sparadis\Documents\ETH\MOSAIC\MOSAIC_Client\Excel_templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D4B5B6A-7F7C-4A2A-B2D3-5A28C7F811BD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0E1DAC4-19B7-4595-8408-9170B496BB9E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30204" yWindow="10044" windowWidth="40020" windowHeight="22296" tabRatio="694" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30204" yWindow="10044" windowWidth="40020" windowHeight="22296" tabRatio="694" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ARTICLE_AUTHOR" sheetId="3" r:id="rId1"/>
@@ -93,7 +93,7 @@
     <definedName name="MAR_g_cm2_yr">SET_VARIABLES!$GJ$2:$GJ$20</definedName>
     <definedName name="MAR_model">SET_VARIABLES!#REF!</definedName>
     <definedName name="MAR_tracer">SET_VARIABLES!#REF!</definedName>
-    <definedName name="material_analyzed">SET_VARIABLES!$BU$2:$BU$90</definedName>
+    <definedName name="material_analyzed">SET_VARIABLES!$BU$2:$BU$91</definedName>
     <definedName name="Mauritania">SET_VARIABLES!$AN$2:$AN$7</definedName>
     <definedName name="mean_grain_size_microm">SET_VARIABLES!$FB$2:$FB$5</definedName>
     <definedName name="median_grain_size_microm">SET_VARIABLES!$FC$2:$FC$5</definedName>
@@ -187,7 +187,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4130" uniqueCount="3058">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4131" uniqueCount="3059">
   <si>
     <t>sample_name</t>
   </si>
@@ -9361,6 +9361,9 @@
   </si>
   <si>
     <t>&lt;0.0005 mm</t>
+  </si>
+  <si>
+    <t>&gt;1.6 g/cm3</t>
   </si>
 </sst>
 </file>
@@ -10365,7 +10368,7 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -10459,7 +10462,7 @@
   <dimension ref="A1:S15"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="G3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="A3" sqref="A3"/>
@@ -10754,11 +10757,11 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:CB52"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane xSplit="3" ySplit="6" topLeftCell="D7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="D2" sqref="D2:D6"/>
+      <selection pane="bottomRight" activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -13607,7 +13610,7 @@
   <dimension ref="A1:ID277"/>
   <sheetViews>
     <sheetView topLeftCell="BR13" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="BU41" sqref="BU41"/>
+      <selection activeCell="BU23" sqref="BU23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -20698,7 +20701,7 @@
         <v>2808</v>
       </c>
       <c r="BU22" s="14" t="s">
-        <v>3026</v>
+        <v>3058</v>
       </c>
       <c r="BY22" s="11" t="s">
         <v>2540</v>
@@ -20801,7 +20804,7 @@
         <v>2809</v>
       </c>
       <c r="BU23" s="14" t="s">
-        <v>2782</v>
+        <v>3026</v>
       </c>
       <c r="BY23" s="11" t="s">
         <v>2541</v>
@@ -20905,7 +20908,7 @@
         <v>2866</v>
       </c>
       <c r="BU24" s="14" t="s">
-        <v>2783</v>
+        <v>2782</v>
       </c>
       <c r="BY24" s="11" t="s">
         <v>2542</v>
@@ -21001,7 +21004,7 @@
       </c>
       <c r="BF25" s="17"/>
       <c r="BU25" s="14" t="s">
-        <v>3050</v>
+        <v>2783</v>
       </c>
       <c r="BY25" s="11" t="s">
         <v>2543</v>
@@ -21093,7 +21096,7 @@
       </c>
       <c r="BF26" s="17"/>
       <c r="BU26" s="14" t="s">
-        <v>2784</v>
+        <v>3050</v>
       </c>
       <c r="BY26" s="11" t="s">
         <v>1765</v>
@@ -21179,7 +21182,7 @@
         <v>1941</v>
       </c>
       <c r="BU27" s="14" t="s">
-        <v>2785</v>
+        <v>2784</v>
       </c>
       <c r="BY27" s="11" t="s">
         <v>1775</v>
@@ -21264,7 +21267,7 @@
         <v>1655</v>
       </c>
       <c r="BU28" s="14" t="s">
-        <v>3051</v>
+        <v>2785</v>
       </c>
       <c r="BY28" s="11" t="s">
         <v>2698</v>
@@ -21343,7 +21346,7 @@
         <v>1678</v>
       </c>
       <c r="BU29" s="14" t="s">
-        <v>2786</v>
+        <v>3051</v>
       </c>
       <c r="BY29" s="20"/>
       <c r="BZ29" s="14"/>
@@ -21413,7 +21416,7 @@
         <v>1679</v>
       </c>
       <c r="BU30" s="14" t="s">
-        <v>3052</v>
+        <v>2786</v>
       </c>
       <c r="BY30" s="14"/>
       <c r="BZ30" s="14"/>
@@ -21481,7 +21484,7 @@
         <v>1677</v>
       </c>
       <c r="BU31" s="14" t="s">
-        <v>2787</v>
+        <v>3052</v>
       </c>
       <c r="BY31" s="14"/>
       <c r="BZ31" s="14"/>
@@ -21552,7 +21555,7 @@
         <v>1676</v>
       </c>
       <c r="BU32" s="14" t="s">
-        <v>3053</v>
+        <v>2787</v>
       </c>
       <c r="BY32" s="14"/>
       <c r="BZ32" s="14"/>
@@ -21618,7 +21621,7 @@
         <v>1666</v>
       </c>
       <c r="BU33" s="14" t="s">
-        <v>3028</v>
+        <v>3053</v>
       </c>
       <c r="BY33" s="14"/>
       <c r="BZ33" s="14"/>
@@ -21680,7 +21683,7 @@
         <v>1683</v>
       </c>
       <c r="BU34" s="14" t="s">
-        <v>3054</v>
+        <v>3028</v>
       </c>
       <c r="BY34" s="14"/>
       <c r="BZ34" s="14"/>
@@ -21742,7 +21745,7 @@
         <v>1675</v>
       </c>
       <c r="BU35" s="14" t="s">
-        <v>3029</v>
+        <v>3054</v>
       </c>
       <c r="BY35" s="14"/>
       <c r="BZ35" s="14"/>
@@ -21801,7 +21804,7 @@
         <v>1680</v>
       </c>
       <c r="BU36" s="14" t="s">
-        <v>3055</v>
+        <v>3029</v>
       </c>
       <c r="BY36" s="14"/>
       <c r="BZ36" s="14"/>
@@ -21861,7 +21864,7 @@
         <v>1681</v>
       </c>
       <c r="BU37" s="14" t="s">
-        <v>3056</v>
+        <v>3055</v>
       </c>
       <c r="BY37" s="14"/>
       <c r="BZ37" s="14"/>
@@ -21921,7 +21924,7 @@
         <v>1651</v>
       </c>
       <c r="BU38" s="14" t="s">
-        <v>2788</v>
+        <v>3056</v>
       </c>
       <c r="BY38" s="14"/>
       <c r="BZ38" s="14"/>
@@ -21977,7 +21980,7 @@
         <v>1663</v>
       </c>
       <c r="BU39" s="14" t="s">
-        <v>3027</v>
+        <v>2788</v>
       </c>
       <c r="BY39" s="14"/>
       <c r="BZ39" s="14"/>
@@ -22033,7 +22036,7 @@
         <v>1688</v>
       </c>
       <c r="BU40" s="14" t="s">
-        <v>3057</v>
+        <v>3027</v>
       </c>
       <c r="BY40" s="14"/>
       <c r="BZ40" s="14"/>
@@ -22086,7 +22089,7 @@
         <v>1699</v>
       </c>
       <c r="BU41" s="14" t="s">
-        <v>2789</v>
+        <v>3057</v>
       </c>
       <c r="CQ41" s="12" t="s">
         <v>2599</v>
@@ -22135,7 +22138,7 @@
         <v>1659</v>
       </c>
       <c r="BU42" s="14" t="s">
-        <v>2995</v>
+        <v>2789</v>
       </c>
       <c r="CQ42" s="12" t="s">
         <v>2118</v>
@@ -22184,7 +22187,7 @@
         <v>1687</v>
       </c>
       <c r="BU43" s="14" t="s">
-        <v>2994</v>
+        <v>2995</v>
       </c>
       <c r="CQ43" s="12" t="s">
         <v>2601</v>
@@ -22234,7 +22237,7 @@
         <v>1664</v>
       </c>
       <c r="BU44" s="14" t="s">
-        <v>2993</v>
+        <v>2994</v>
       </c>
       <c r="CO44" s="23"/>
       <c r="CP44" s="23"/>
@@ -22286,7 +22289,7 @@
         <v>1691</v>
       </c>
       <c r="BU45" s="14" t="s">
-        <v>2992</v>
+        <v>2993</v>
       </c>
       <c r="CO45" s="23"/>
       <c r="CP45" s="23"/>
@@ -22338,7 +22341,7 @@
         <v>1692</v>
       </c>
       <c r="BU46" s="14" t="s">
-        <v>2991</v>
+        <v>2992</v>
       </c>
       <c r="CO46" s="23"/>
       <c r="CP46" s="23"/>
@@ -22387,7 +22390,7 @@
         <v>1693</v>
       </c>
       <c r="BU47" s="14" t="s">
-        <v>2998</v>
+        <v>2991</v>
       </c>
       <c r="CN47" s="23"/>
       <c r="CO47" s="23"/>
@@ -22436,7 +22439,7 @@
         <v>1672</v>
       </c>
       <c r="BU48" s="14" t="s">
-        <v>2990</v>
+        <v>2998</v>
       </c>
       <c r="CN48" s="23"/>
       <c r="CO48" s="23"/>
@@ -22485,7 +22488,7 @@
         <v>1667</v>
       </c>
       <c r="BU49" s="14" t="s">
-        <v>2999</v>
+        <v>2990</v>
       </c>
       <c r="CN49" s="23"/>
       <c r="CO49" s="23"/>
@@ -22535,7 +22538,7 @@
         <v>2105</v>
       </c>
       <c r="BU50" s="14" t="s">
-        <v>2996</v>
+        <v>2999</v>
       </c>
       <c r="CN50" s="23"/>
       <c r="CO50" s="23"/>
@@ -22585,7 +22588,7 @@
         <v>1689</v>
       </c>
       <c r="BU51" s="14" t="s">
-        <v>3000</v>
+        <v>2996</v>
       </c>
       <c r="CN51" s="23"/>
       <c r="CO51" s="23"/>
@@ -22634,7 +22637,7 @@
         <v>1668</v>
       </c>
       <c r="BU52" s="14" t="s">
-        <v>2925</v>
+        <v>3000</v>
       </c>
       <c r="CN52" s="23"/>
       <c r="CO52" s="23"/>
@@ -22684,7 +22687,7 @@
         <v>1685</v>
       </c>
       <c r="BU53" s="14" t="s">
-        <v>3001</v>
+        <v>2925</v>
       </c>
       <c r="CN53" s="23"/>
       <c r="CO53" s="23"/>
@@ -22734,7 +22737,7 @@
         <v>1657</v>
       </c>
       <c r="BU54" s="14" t="s">
-        <v>2926</v>
+        <v>3001</v>
       </c>
       <c r="CN54" s="23"/>
       <c r="CQ54" s="12" t="s">
@@ -22782,7 +22785,7 @@
         <v>1654</v>
       </c>
       <c r="BU55" s="14" t="s">
-        <v>3002</v>
+        <v>2926</v>
       </c>
       <c r="CN55" s="23"/>
       <c r="CQ55" s="12" t="s">
@@ -22830,7 +22833,7 @@
         <v>2104</v>
       </c>
       <c r="BU56" s="14" t="s">
-        <v>2927</v>
+        <v>3002</v>
       </c>
       <c r="CN56" s="23"/>
       <c r="CQ56" s="12" t="s">
@@ -22878,7 +22881,7 @@
         <v>1682</v>
       </c>
       <c r="BU57" s="14" t="s">
-        <v>3003</v>
+        <v>2927</v>
       </c>
       <c r="CQ57" s="12" t="s">
         <v>2615</v>
@@ -22925,7 +22928,7 @@
         <v>1980</v>
       </c>
       <c r="BU58" s="14" t="s">
-        <v>2928</v>
+        <v>3003</v>
       </c>
       <c r="CQ58" s="12" t="s">
         <v>2126</v>
@@ -22969,7 +22972,7 @@
         <v>1658</v>
       </c>
       <c r="BU59" s="14" t="s">
-        <v>3004</v>
+        <v>2928</v>
       </c>
       <c r="CQ59" s="12" t="s">
         <v>2617</v>
@@ -23013,7 +23016,7 @@
         <v>1981</v>
       </c>
       <c r="BU60" s="14" t="s">
-        <v>2997</v>
+        <v>3004</v>
       </c>
       <c r="CQ60" s="12" t="s">
         <v>2127</v>
@@ -23057,7 +23060,7 @@
         <v>1673</v>
       </c>
       <c r="BU61" s="14" t="s">
-        <v>2929</v>
+        <v>2997</v>
       </c>
       <c r="CQ61" s="12" t="s">
         <v>2619</v>
@@ -23101,7 +23104,7 @@
         <v>1686</v>
       </c>
       <c r="BU62" s="14" t="s">
-        <v>2930</v>
+        <v>2929</v>
       </c>
       <c r="CQ62" s="12" t="s">
         <v>2128</v>
@@ -23145,7 +23148,7 @@
         <v>1671</v>
       </c>
       <c r="BU63" s="14" t="s">
-        <v>3005</v>
+        <v>2930</v>
       </c>
       <c r="CQ63" s="12" t="s">
         <v>2621</v>
@@ -23186,7 +23189,7 @@
         <v>1700</v>
       </c>
       <c r="BU64" s="14" t="s">
-        <v>3006</v>
+        <v>3005</v>
       </c>
       <c r="CQ64" s="23" t="s">
         <v>2129</v>
@@ -23227,7 +23230,7 @@
         <v>1649</v>
       </c>
       <c r="BU65" s="14" t="s">
-        <v>3007</v>
+        <v>3006</v>
       </c>
       <c r="CQ65" s="12" t="s">
         <v>2623</v>
@@ -23268,7 +23271,7 @@
         <v>1669</v>
       </c>
       <c r="BU66" s="14" t="s">
-        <v>3008</v>
+        <v>3007</v>
       </c>
       <c r="CQ66" s="23" t="s">
         <v>2130</v>
@@ -23309,7 +23312,7 @@
         <v>1674</v>
       </c>
       <c r="BU67" s="14" t="s">
-        <v>3009</v>
+        <v>3008</v>
       </c>
       <c r="CQ67" s="12" t="s">
         <v>2625</v>
@@ -23350,7 +23353,7 @@
         <v>1652</v>
       </c>
       <c r="BU68" s="14" t="s">
-        <v>3010</v>
+        <v>3009</v>
       </c>
       <c r="CQ68" s="23" t="s">
         <v>2131</v>
@@ -23390,7 +23393,7 @@
         <v>1982</v>
       </c>
       <c r="BU69" s="14" t="s">
-        <v>3011</v>
+        <v>3010</v>
       </c>
       <c r="CQ69" s="12" t="s">
         <v>2627</v>
@@ -23431,7 +23434,7 @@
         <v>1695</v>
       </c>
       <c r="BU70" s="14" t="s">
-        <v>3012</v>
+        <v>3011</v>
       </c>
       <c r="CQ70" s="23" t="s">
         <v>2132</v>
@@ -23472,7 +23475,7 @@
         <v>1670</v>
       </c>
       <c r="BU71" s="14" t="s">
-        <v>3013</v>
+        <v>3012</v>
       </c>
       <c r="CQ71" s="12" t="s">
         <v>2629</v>
@@ -23513,7 +23516,7 @@
         <v>1665</v>
       </c>
       <c r="BU72" s="14" t="s">
-        <v>3014</v>
+        <v>3013</v>
       </c>
       <c r="CQ72" s="23" t="s">
         <v>2133</v>
@@ -23554,7 +23557,7 @@
         <v>1696</v>
       </c>
       <c r="BU73" s="14" t="s">
-        <v>3015</v>
+        <v>3014</v>
       </c>
       <c r="CQ73" s="12" t="s">
         <v>2631</v>
@@ -23595,7 +23598,7 @@
         <v>1684</v>
       </c>
       <c r="BU74" s="14" t="s">
-        <v>3016</v>
+        <v>3015</v>
       </c>
       <c r="CQ74" s="23" t="s">
         <v>2134</v>
@@ -23636,7 +23639,7 @@
         <v>1697</v>
       </c>
       <c r="BU75" s="14" t="s">
-        <v>3017</v>
+        <v>3016</v>
       </c>
       <c r="CQ75" s="12" t="s">
         <v>2633</v>
@@ -23677,7 +23680,7 @@
         <v>1983</v>
       </c>
       <c r="BU76" s="14" t="s">
-        <v>3018</v>
+        <v>3017</v>
       </c>
       <c r="CQ76" s="23" t="s">
         <v>2135</v>
@@ -23718,7 +23721,7 @@
         <v>1647</v>
       </c>
       <c r="BU77" s="14" t="s">
-        <v>3019</v>
+        <v>3018</v>
       </c>
       <c r="CQ77" s="12" t="s">
         <v>2635</v>
@@ -23759,7 +23762,7 @@
         <v>1698</v>
       </c>
       <c r="BU78" s="14" t="s">
-        <v>3020</v>
+        <v>3019</v>
       </c>
       <c r="CQ78" s="23" t="s">
         <v>2136</v>
@@ -23800,7 +23803,7 @@
         <v>1648</v>
       </c>
       <c r="BU79" s="14" t="s">
-        <v>3021</v>
+        <v>3020</v>
       </c>
       <c r="CQ79" s="12" t="s">
         <v>2636</v>
@@ -23841,7 +23844,7 @@
         <v>1694</v>
       </c>
       <c r="BU80" s="14" t="s">
-        <v>3022</v>
+        <v>3021</v>
       </c>
       <c r="CQ80" s="23" t="s">
         <v>2137</v>
@@ -23882,7 +23885,7 @@
         <v>1690</v>
       </c>
       <c r="BU81" s="14" t="s">
-        <v>3023</v>
+        <v>3022</v>
       </c>
       <c r="CQ81" s="12" t="s">
         <v>2638</v>
@@ -23923,7 +23926,7 @@
         <v>1747</v>
       </c>
       <c r="BU82" s="14" t="s">
-        <v>3024</v>
+        <v>3023</v>
       </c>
       <c r="CQ82" s="23" t="s">
         <v>2138</v>
@@ -23964,7 +23967,7 @@
         <v>1749</v>
       </c>
       <c r="BU83" s="14" t="s">
-        <v>2970</v>
+        <v>3024</v>
       </c>
       <c r="CQ83" s="12" t="s">
         <v>2639</v>
@@ -24005,7 +24008,7 @@
         <v>1984</v>
       </c>
       <c r="BU84" s="14" t="s">
-        <v>2967</v>
+        <v>2970</v>
       </c>
       <c r="CQ84" s="23" t="s">
         <v>2139</v>
@@ -24045,7 +24048,7 @@
         <v>1656</v>
       </c>
       <c r="BU85" s="14" t="s">
-        <v>2968</v>
+        <v>2967</v>
       </c>
       <c r="CQ85" s="12" t="s">
         <v>2640</v>
@@ -24085,7 +24088,7 @@
         <v>1748</v>
       </c>
       <c r="BU86" s="14" t="s">
-        <v>2969</v>
+        <v>2968</v>
       </c>
       <c r="CQ86" s="23" t="s">
         <v>2140</v>
@@ -24125,7 +24128,7 @@
         <v>1985</v>
       </c>
       <c r="BU87" s="14" t="s">
-        <v>2970</v>
+        <v>2969</v>
       </c>
       <c r="CQ87" s="12" t="s">
         <v>2642</v>
@@ -24165,7 +24168,7 @@
         <v>1750</v>
       </c>
       <c r="BU88" s="14" t="s">
-        <v>2971</v>
+        <v>2970</v>
       </c>
       <c r="CQ88" s="23" t="s">
         <v>2141</v>
@@ -24205,7 +24208,7 @@
         <v>1744</v>
       </c>
       <c r="BU89" s="14" t="s">
-        <v>2972</v>
+        <v>2971</v>
       </c>
       <c r="CQ89" s="12" t="s">
         <v>2644</v>
@@ -24245,7 +24248,7 @@
         <v>1745</v>
       </c>
       <c r="BU90" s="14" t="s">
-        <v>3025</v>
+        <v>2972</v>
       </c>
       <c r="CQ90" s="23" t="s">
         <v>2142</v>
@@ -24283,6 +24286,9 @@
       </c>
       <c r="BE91" s="6" t="s">
         <v>1986</v>
+      </c>
+      <c r="BU91" s="14" t="s">
+        <v>3025</v>
       </c>
       <c r="CQ91" s="12" t="s">
         <v>2646</v>
@@ -27404,7 +27410,7 @@
       <c r="CT277" s="40"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="u3ikDjYQU5ICeZdTr2QlsS0wtjnly2LQhwV3I6lBzoEekxL5FaX7pyoJjX9dZkVARsXJXarPS9Dx/Oxd1V4jlg==" saltValue="jOYq+wIxxaq8oX4NVrPIIg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="6Sfl9EgLRjysEMhemw5uhffLwoTMdjLhAtWghqYgi0lBueT+EEGzrvy6v1jNB67XpfzG2VCUd9qHEe3daUPR0g==" saltValue="71y8oTq+aa7bfOoeKLjyCg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="2">
     <mergeCell ref="M27:M28"/>
     <mergeCell ref="M34:M35"/>

</xml_diff>